<commit_message>
Add traceability between USgenerated and prompt used
</commit_message>
<xml_diff>
--- a/refair-server/datasets/few shot dataset/FSDataset.xlsx
+++ b/refair-server/datasets/few shot dataset/FSDataset.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\morel\Desktop\Refair\ReFair-App\refair-server\datasets\few shot dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{204CE33E-88A1-494D-A291-B60BEC871D7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35EE34A9-5330-42A1-9575-011CE9DDA2FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{80773445-FB61-4F04-A882-1600FD96C55A}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="70">
   <si>
     <t>Domain cluster</t>
   </si>
@@ -240,6 +240,12 @@
   </si>
   <si>
     <t>As a literature researcher, I want to employ word embedding algorithms to identify and analyze shifts in literary themes and motifs across different periods and genres, uncovering evolutionary patterns in the use of language within the literary canon.</t>
+  </si>
+  <si>
+    <t>Prompt used</t>
+  </si>
+  <si>
+    <t>Domain_FSPrompt</t>
   </si>
 </sst>
 </file>
@@ -300,11 +306,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -639,10 +648,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8DF0B04-8323-4309-B759-D1CDDA1FBB0E}">
-  <dimension ref="A1:E41"/>
+  <dimension ref="A1:F41"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" topLeftCell="A17" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E36" sqref="E36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -650,27 +659,31 @@
     <col min="1" max="3" width="26" style="1" customWidth="1"/>
     <col min="4" max="4" width="26" style="2" customWidth="1"/>
     <col min="5" max="5" width="255.6640625" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.88671875" style="1"/>
+    <col min="6" max="6" width="26.5546875" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="4" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1" s="4" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
@@ -686,8 +699,11 @@
       <c r="E2" s="1" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F2" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
@@ -703,8 +719,11 @@
       <c r="E3" s="1" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F3" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>4</v>
       </c>
@@ -720,8 +739,11 @@
       <c r="E4" s="1" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F4" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>4</v>
       </c>
@@ -737,8 +759,11 @@
       <c r="E5" s="1" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F5" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>4</v>
       </c>
@@ -754,8 +779,11 @@
       <c r="E6" s="1" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F6" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>4</v>
       </c>
@@ -771,8 +799,11 @@
       <c r="E7" s="1" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F7" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>4</v>
       </c>
@@ -788,8 +819,11 @@
       <c r="E8" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F8" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>4</v>
       </c>
@@ -805,8 +839,11 @@
       <c r="E9" s="1" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F9" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>4</v>
       </c>
@@ -822,8 +859,11 @@
       <c r="E10" s="1" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F10" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>4</v>
       </c>
@@ -839,8 +879,11 @@
       <c r="E11" s="1" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F11" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>4</v>
       </c>
@@ -856,8 +899,11 @@
       <c r="E12" s="1" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F12" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>4</v>
       </c>
@@ -873,8 +919,11 @@
       <c r="E13" s="1" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F13" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>4</v>
       </c>
@@ -890,8 +939,11 @@
       <c r="E14" s="1" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F14" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>4</v>
       </c>
@@ -907,8 +959,11 @@
       <c r="E15" s="1" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F15" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>4</v>
       </c>
@@ -924,8 +979,11 @@
       <c r="E16" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F16" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>4</v>
       </c>
@@ -941,8 +999,11 @@
       <c r="E17" s="1" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F17" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>4</v>
       </c>
@@ -958,8 +1019,11 @@
       <c r="E18" s="1" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F18" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>4</v>
       </c>
@@ -975,8 +1039,11 @@
       <c r="E19" s="1" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F19" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>4</v>
       </c>
@@ -992,8 +1059,11 @@
       <c r="E20" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F20" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>4</v>
       </c>
@@ -1009,8 +1079,11 @@
       <c r="E21" s="1" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F21" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>4</v>
       </c>
@@ -1026,8 +1099,11 @@
       <c r="E22" s="1" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F22" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>4</v>
       </c>
@@ -1043,8 +1119,11 @@
       <c r="E23" s="1" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F23" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>4</v>
       </c>
@@ -1060,8 +1139,11 @@
       <c r="E24" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F24" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>4</v>
       </c>
@@ -1077,8 +1159,11 @@
       <c r="E25" s="1" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F25" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>4</v>
       </c>
@@ -1094,8 +1179,11 @@
       <c r="E26" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F26" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>4</v>
       </c>
@@ -1111,8 +1199,11 @@
       <c r="E27" s="1" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F27" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>4</v>
       </c>
@@ -1128,8 +1219,11 @@
       <c r="E28" s="1" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F28" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>4</v>
       </c>
@@ -1145,8 +1239,11 @@
       <c r="E29" s="1" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F29" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>4</v>
       </c>
@@ -1162,8 +1259,11 @@
       <c r="E30" s="1" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F30" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
         <v>4</v>
       </c>
@@ -1179,8 +1279,11 @@
       <c r="E31" s="1" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F31" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
         <v>4</v>
       </c>
@@ -1196,8 +1299,11 @@
       <c r="E32" s="1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F32" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
         <v>4</v>
       </c>
@@ -1213,8 +1319,11 @@
       <c r="E33" s="1" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F33" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
         <v>4</v>
       </c>
@@ -1230,8 +1339,11 @@
       <c r="E34" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F34" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
         <v>4</v>
       </c>
@@ -1247,8 +1359,11 @@
       <c r="E35" s="1" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F35" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
         <v>4</v>
       </c>
@@ -1264,8 +1379,11 @@
       <c r="E36" s="1" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F36" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
         <v>4</v>
       </c>
@@ -1281,8 +1399,11 @@
       <c r="E37" s="1" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F37" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
         <v>4</v>
       </c>
@@ -1298,8 +1419,11 @@
       <c r="E38" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F38" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
         <v>4</v>
       </c>
@@ -1315,8 +1439,11 @@
       <c r="E39" s="1" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F39" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
         <v>4</v>
       </c>
@@ -1332,8 +1459,11 @@
       <c r="E40" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F40" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
         <v>4</v>
       </c>
@@ -1348,6 +1478,9 @@
       </c>
       <c r="E41" s="1" t="s">
         <v>67</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>69</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add US related to Law domain
</commit_message>
<xml_diff>
--- a/refair-server/datasets/few shot dataset/FSDataset.xlsx
+++ b/refair-server/datasets/few shot dataset/FSDataset.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\morel\Desktop\Refair\ReFair-App\refair-server\datasets\few shot dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{963F4CA1-6CC7-4DD3-95E6-BD645D33B997}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E63F4E66-D898-4B15-9CFC-5D297CFD5D0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{80773445-FB61-4F04-A882-1600FD96C55A}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="406" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="506" uniqueCount="134">
   <si>
     <t>Domain cluster</t>
   </si>
@@ -375,13 +375,76 @@
   </si>
   <si>
     <t>As a political scientist, I want to use word embedding models to analyze historical texts and speeches by political leaders, tracing the evolution of political ideologies and rhetoric over time to understand the shaping of political narratives and public discourse.</t>
+  </si>
+  <si>
+    <t>Law</t>
+  </si>
+  <si>
+    <t>As a legal researcher, I want to apply adversarial learning techniques to identify potential vulnerabilities in legal text classifiers, so that I can enhance the robustness of legal document analysis systems against adversarial attacks.</t>
+  </si>
+  <si>
+    <t>As a lawyer, I want to utilize convolutional neural networks to analyze the sentiment and context of legal texts in public opinion, providing insights into public perceptions that could influence case strategy and client counseling.</t>
+  </si>
+  <si>
+    <t>As a legal researcher, I want to develop a conversational agent powered by natural language processing to provide legal advice and guidance to clients, enhancing access to legal information and services.</t>
+  </si>
+  <si>
+    <t>As a legal researcher, I want to develop decision tree models to classify legal documents based on case types and legal issues, enabling automated document sorting and categorization for law firms.</t>
+  </si>
+  <si>
+    <t>As a legal researcher, I want to implement document classification algorithms to categorize legal documents based on case types (e.g., civil, criminal, administrative) for efficient document management and retrieval in law firms.</t>
+  </si>
+  <si>
+    <t>As a lawyer, I aim to implement entity extraction algorithms to extract crucial information such as court decisions, judges' names, and legal citations from judicial opinions, supporting comprehensive case law analysis and citation tracking.</t>
+  </si>
+  <si>
+    <t>As a legal researcher, I want to implement feature selection techniques to identify discriminatory factors in legal decision-making processes, helping to mitigate bias and promote fairness in legal judgments.</t>
+  </si>
+  <si>
+    <t>As a legal researcher, I want to address class imbalance in legal datasets related to case outcomes (e.g., favorable vs. unfavorable judgments) using techniques like oversampling or undersampling, to improve the accuracy of predictive models used in legal prediction tasks.</t>
+  </si>
+  <si>
+    <t>As a lawyer, I aim to leverage keyword extraction methods to automatically tag and organize legal contracts based on important clauses and terms, supporting contract management and review processes in law firms.</t>
+  </si>
+  <si>
+    <t>As a lawyer, I aim to implement k-nearest neighbor models to identify similar historical cases with favorable outcomes for strategic case preparation and argumentation, enhancing the likelihood of success in litigation.</t>
+  </si>
+  <si>
+    <t>As a legal researcher, I want to develop a multi-label classification system to categorize legal documents according to multiple relevant legal topics (e.g., contracts, intellectual property, torts), enhancing the organization and retrieval of legal information.</t>
+  </si>
+  <si>
+    <t>As a legal researcher, I want to develop a neural network model to predict court case outcomes based on various legal factors such as case type, jurisdiction, and historical precedents, providing insights into potential case strategies and outcomes.</t>
+  </si>
+  <si>
+    <t>As a legal researcher, I want to use a random forest algorithm to classify legal documents into different categories such as case types (e.g., civil, criminal, administrative), improving the efficiency of document management systems in law firms.</t>
+  </si>
+  <si>
+    <t>As a legal researcher, I want to develop semantic similarity models to compare legal texts such as contracts and agreements, identifying similarities in language and clauses to support contract analysis and negotiation processes.</t>
+  </si>
+  <si>
+    <t>As a lawyer, I aim to utilize sentiment analysis to assess the sentiment expressed in legal documents such as complaints and motions, helping to understand emotional tones and implications for case strategy.</t>
+  </si>
+  <si>
+    <t>As a legal researcher, I want to develop speech to text models to transcribe courtroom proceedings and depositions accurately, enabling efficient documentation and retrieval of legal transcripts for case preparation.</t>
+  </si>
+  <si>
+    <t>As a legal researcher, I want to develop a text categorization system to classify legal documents into different practice areas (e.g., corporate law, family law, intellectual property), facilitating efficient document retrieval and management in law firms.</t>
+  </si>
+  <si>
+    <t>As a legal researcher, I want to apply unsupervised clustering techniques to group similar legal cases based on factual similarities and legal issues, enabling clustering of case law for comparative legal analysis and precedent identification.</t>
+  </si>
+  <si>
+    <t>As a legal researcher, I want to implement voice recognition algorithms to transcribe interviews and witness testimonies, enabling thorough analysis and documentation of legal evidence and statements.</t>
+  </si>
+  <si>
+    <t>As a legal researcher, I want to apply word embedding models to automate the extraction of key legal concepts and trends from large volumes of legislative texts and regulatory documents, aiding in regulatory compliance analysis and policy research.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -407,11 +470,6 @@
       <color rgb="FFFFFFFF"/>
       <name val="Arial"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="4">
@@ -453,7 +511,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -463,6 +520,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -797,16 +855,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8DF0B04-8323-4309-B759-D1CDDA1FBB0E}">
-  <dimension ref="A1:F81"/>
+  <dimension ref="A1:F101"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="3" width="26" style="1" customWidth="1"/>
-    <col min="4" max="4" width="26" style="6" customWidth="1"/>
+    <col min="4" max="4" width="26" style="5" customWidth="1"/>
     <col min="5" max="5" width="255.6640625" style="1" customWidth="1"/>
     <col min="6" max="6" width="26.5546875" style="1" customWidth="1"/>
     <col min="7" max="16384" width="8.88671875" style="1"/>
@@ -822,7 +880,7 @@
       <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="3" t="s">
@@ -833,800 +891,800 @@
       </c>
     </row>
     <row r="2" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="B2" s="4">
-        <v>4</v>
-      </c>
-      <c r="C2" s="4" t="s">
+      <c r="A2" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="B2" s="7">
+        <v>4</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="B3" s="7">
+        <v>4</v>
+      </c>
+      <c r="C3" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D3" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="F2" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="B3" s="4">
-        <v>4</v>
-      </c>
-      <c r="C3" s="4" t="s">
+      <c r="F3" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="B4" s="7">
+        <v>4</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="B5" s="7">
+        <v>4</v>
+      </c>
+      <c r="C5" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D5" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E5" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="F3" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="B4" s="4">
-        <v>4</v>
-      </c>
-      <c r="C4" s="4" t="s">
+      <c r="F5" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="B6" s="7">
+        <v>4</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="B7" s="7">
+        <v>4</v>
+      </c>
+      <c r="C7" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D7" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E7" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="F4" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="B5" s="4">
-        <v>4</v>
-      </c>
-      <c r="C5" s="4" t="s">
+      <c r="F7" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="B8" s="7">
+        <v>4</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="B9" s="7">
+        <v>4</v>
+      </c>
+      <c r="C9" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D9" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="E9" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="F5" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="B6" s="4">
-        <v>4</v>
-      </c>
-      <c r="C6" s="4" t="s">
+      <c r="F9" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="B10" s="7">
+        <v>4</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="B11" s="7">
+        <v>4</v>
+      </c>
+      <c r="C11" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="D11" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="E11" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="F6" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="B7" s="4">
-        <v>4</v>
-      </c>
-      <c r="C7" s="4" t="s">
+      <c r="F11" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="B12" s="7">
+        <v>4</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="B13" s="7">
+        <v>4</v>
+      </c>
+      <c r="C13" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="D13" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="E13" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="F7" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="B8" s="4">
-        <v>4</v>
-      </c>
-      <c r="C8" s="4" t="s">
+      <c r="F13" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="B14" s="7">
+        <v>4</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="B15" s="7">
+        <v>4</v>
+      </c>
+      <c r="C15" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="D15" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="E15" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="F8" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="B9" s="4">
-        <v>4</v>
-      </c>
-      <c r="C9" s="4" t="s">
+      <c r="F15" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="B16" s="7">
+        <v>4</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="B17" s="7">
+        <v>4</v>
+      </c>
+      <c r="C17" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="D9" s="5" t="s">
+      <c r="D17" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="E17" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="F9" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="B10" s="4">
-        <v>4</v>
-      </c>
-      <c r="C10" s="4" t="s">
+      <c r="F17" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="B18" s="7">
+        <v>4</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="B19" s="7">
+        <v>4</v>
+      </c>
+      <c r="C19" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="D10" s="5" t="s">
+      <c r="D19" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="E19" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="F10" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="B11" s="4">
-        <v>4</v>
-      </c>
-      <c r="C11" s="4" t="s">
+      <c r="F19" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="B20" s="7">
+        <v>4</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="B21" s="7">
+        <v>4</v>
+      </c>
+      <c r="C21" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="D11" s="5" t="s">
+      <c r="D21" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="E21" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="F11" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="B12" s="4">
-        <v>4</v>
-      </c>
-      <c r="C12" s="4" t="s">
+      <c r="F21" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="B22" s="7">
+        <v>4</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="B23" s="7">
+        <v>4</v>
+      </c>
+      <c r="C23" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="D12" s="5" t="s">
+      <c r="D23" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="E12" s="1" t="s">
+      <c r="E23" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="F12" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="B13" s="4">
-        <v>4</v>
-      </c>
-      <c r="C13" s="4" t="s">
+      <c r="F23" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="B24" s="7">
+        <v>4</v>
+      </c>
+      <c r="C24" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="B25" s="7">
+        <v>4</v>
+      </c>
+      <c r="C25" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="D13" s="5" t="s">
+      <c r="D25" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="E13" s="1" t="s">
+      <c r="E25" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="F13" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="B14" s="4">
-        <v>4</v>
-      </c>
-      <c r="C14" s="4" t="s">
+      <c r="F25" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="B26" s="7">
+        <v>4</v>
+      </c>
+      <c r="C26" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="B27" s="7">
+        <v>4</v>
+      </c>
+      <c r="C27" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="D14" s="5" t="s">
+      <c r="D27" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="E14" s="1" t="s">
+      <c r="E27" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="F14" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="B15" s="4">
-        <v>4</v>
-      </c>
-      <c r="C15" s="4" t="s">
+      <c r="F27" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="B28" s="7">
+        <v>4</v>
+      </c>
+      <c r="C28" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="B29" s="7">
+        <v>4</v>
+      </c>
+      <c r="C29" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="D15" s="5" t="s">
+      <c r="D29" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="E15" s="1" t="s">
+      <c r="E29" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="F15" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="B16" s="4">
-        <v>4</v>
-      </c>
-      <c r="C16" s="4" t="s">
+      <c r="F29" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="B30" s="7">
+        <v>4</v>
+      </c>
+      <c r="C30" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="D30" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="B31" s="7">
+        <v>4</v>
+      </c>
+      <c r="C31" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="D16" s="5" t="s">
+      <c r="D31" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="E16" s="1" t="s">
+      <c r="E31" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="F16" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="B17" s="4">
-        <v>4</v>
-      </c>
-      <c r="C17" s="4" t="s">
+      <c r="F31" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="B32" s="7">
+        <v>4</v>
+      </c>
+      <c r="C32" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="D32" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="B33" s="7">
+        <v>4</v>
+      </c>
+      <c r="C33" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="D17" s="5" t="s">
+      <c r="D33" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="E17" s="1" t="s">
+      <c r="E33" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="F17" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="B18" s="4">
-        <v>4</v>
-      </c>
-      <c r="C18" s="4" t="s">
+      <c r="F33" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="B34" s="7">
+        <v>4</v>
+      </c>
+      <c r="C34" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="D34" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="B35" s="7">
+        <v>4</v>
+      </c>
+      <c r="C35" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="D18" s="5" t="s">
+      <c r="D35" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="E18" s="7" t="s">
+      <c r="E35" s="6" t="s">
         <v>109</v>
       </c>
-      <c r="F18" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="B19" s="4">
-        <v>4</v>
-      </c>
-      <c r="C19" s="4" t="s">
+      <c r="F35" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="B36" s="7">
+        <v>4</v>
+      </c>
+      <c r="C36" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="D36" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="B37" s="7">
+        <v>4</v>
+      </c>
+      <c r="C37" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="D19" s="5" t="s">
+      <c r="D37" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="E19" s="1" t="s">
+      <c r="E37" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="F19" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="B20" s="4">
-        <v>4</v>
-      </c>
-      <c r="C20" s="4" t="s">
+      <c r="F37" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="B38" s="7">
+        <v>4</v>
+      </c>
+      <c r="C38" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="D38" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="B39" s="7">
+        <v>4</v>
+      </c>
+      <c r="C39" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="D20" s="5" t="s">
+      <c r="D39" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E20" s="1" t="s">
+      <c r="E39" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="F20" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="B21" s="4">
-        <v>4</v>
-      </c>
-      <c r="C21" s="4" t="s">
+      <c r="F39" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="B40" s="7">
+        <v>4</v>
+      </c>
+      <c r="C40" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="D40" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="F40" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="B41" s="7">
+        <v>4</v>
+      </c>
+      <c r="C41" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="D21" s="5" t="s">
+      <c r="D41" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="E21" s="1" t="s">
+      <c r="E41" s="1" t="s">
         <v>112</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B22" s="2">
-        <v>5</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D22" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B23" s="2">
-        <v>5</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="D23" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="F23" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B24" s="2">
-        <v>5</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D24" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="F24" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B25" s="2">
-        <v>5</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="D25" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="F25" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B26" s="2">
-        <v>5</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D26" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="E26" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="F26" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B27" s="2">
-        <v>5</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="D27" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="E27" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="F27" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B28" s="2">
-        <v>5</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D28" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="E28" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F28" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B29" s="2">
-        <v>5</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="D29" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="E29" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="F29" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B30" s="2">
-        <v>5</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D30" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="E30" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="F30" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B31" s="2">
-        <v>5</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="D31" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="E31" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="F31" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B32" s="2">
-        <v>5</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D32" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="E32" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="F32" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B33" s="2">
-        <v>5</v>
-      </c>
-      <c r="C33" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="D33" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="E33" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="F33" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B34" s="2">
-        <v>5</v>
-      </c>
-      <c r="C34" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D34" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="E34" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="F34" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B35" s="2">
-        <v>5</v>
-      </c>
-      <c r="C35" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="D35" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="E35" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="F35" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B36" s="2">
-        <v>5</v>
-      </c>
-      <c r="C36" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D36" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="E36" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F36" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B37" s="2">
-        <v>5</v>
-      </c>
-      <c r="C37" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="D37" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="E37" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="F37" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B38" s="2">
-        <v>5</v>
-      </c>
-      <c r="C38" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D38" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="E38" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="F38" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B39" s="2">
-        <v>5</v>
-      </c>
-      <c r="C39" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="D39" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="E39" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="F39" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B40" s="2">
-        <v>5</v>
-      </c>
-      <c r="C40" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D40" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="E40" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F40" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B41" s="2">
-        <v>5</v>
-      </c>
-      <c r="C41" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="D41" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="E41" s="1" t="s">
-        <v>57</v>
       </c>
       <c r="F41" s="1" t="s">
         <v>69</v>
@@ -1642,11 +1700,11 @@
       <c r="C42" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D42" s="6" t="s">
-        <v>40</v>
+      <c r="D42" s="5" t="s">
+        <v>28</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="F42" s="1" t="s">
         <v>69</v>
@@ -1662,11 +1720,11 @@
       <c r="C43" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="D43" s="6" t="s">
-        <v>40</v>
+      <c r="D43" s="5" t="s">
+        <v>28</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="F43" s="1" t="s">
         <v>69</v>
@@ -1682,11 +1740,11 @@
       <c r="C44" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D44" s="6" t="s">
-        <v>18</v>
+      <c r="D44" s="5" t="s">
+        <v>43</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>17</v>
+        <v>42</v>
       </c>
       <c r="F44" s="1" t="s">
         <v>69</v>
@@ -1702,11 +1760,11 @@
       <c r="C45" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="D45" s="6" t="s">
-        <v>18</v>
+      <c r="D45" s="5" t="s">
+        <v>43</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
       <c r="F45" s="1" t="s">
         <v>69</v>
@@ -1722,11 +1780,11 @@
       <c r="C46" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D46" s="6" t="s">
-        <v>20</v>
+      <c r="D46" s="5" t="s">
+        <v>30</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="F46" s="1" t="s">
         <v>69</v>
@@ -1742,11 +1800,11 @@
       <c r="C47" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="D47" s="6" t="s">
-        <v>20</v>
+      <c r="D47" s="5" t="s">
+        <v>30</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="F47" s="1" t="s">
         <v>69</v>
@@ -1762,11 +1820,11 @@
       <c r="C48" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D48" s="6" t="s">
-        <v>22</v>
+      <c r="D48" s="5" t="s">
+        <v>13</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="F48" s="1" t="s">
         <v>69</v>
@@ -1782,11 +1840,11 @@
       <c r="C49" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="D49" s="6" t="s">
-        <v>22</v>
+      <c r="D49" s="5" t="s">
+        <v>13</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="F49" s="1" t="s">
         <v>69</v>
@@ -1802,11 +1860,11 @@
       <c r="C50" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D50" s="6" t="s">
-        <v>38</v>
+      <c r="D50" s="5" t="s">
+        <v>46</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="F50" s="1" t="s">
         <v>69</v>
@@ -1822,11 +1880,11 @@
       <c r="C51" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="D51" s="6" t="s">
-        <v>38</v>
+      <c r="D51" s="5" t="s">
+        <v>46</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>64</v>
+        <v>53</v>
       </c>
       <c r="F51" s="1" t="s">
         <v>69</v>
@@ -1842,11 +1900,11 @@
       <c r="C52" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D52" s="6" t="s">
-        <v>24</v>
+      <c r="D52" s="5" t="s">
+        <v>33</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="F52" s="1" t="s">
         <v>69</v>
@@ -1862,11 +1920,11 @@
       <c r="C53" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="D53" s="6" t="s">
-        <v>24</v>
+      <c r="D53" s="5" t="s">
+        <v>33</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="F53" s="1" t="s">
         <v>69</v>
@@ -1882,11 +1940,11 @@
       <c r="C54" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D54" s="6" t="s">
-        <v>26</v>
+      <c r="D54" s="5" t="s">
+        <v>36</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="F54" s="1" t="s">
         <v>69</v>
@@ -1902,11 +1960,11 @@
       <c r="C55" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="D55" s="6" t="s">
-        <v>26</v>
+      <c r="D55" s="5" t="s">
+        <v>36</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="F55" s="1" t="s">
         <v>69</v>
@@ -1922,11 +1980,11 @@
       <c r="C56" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D56" s="6" t="s">
-        <v>31</v>
+      <c r="D56" s="5" t="s">
+        <v>14</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>44</v>
+        <v>12</v>
       </c>
       <c r="F56" s="1" t="s">
         <v>69</v>
@@ -1942,11 +2000,11 @@
       <c r="C57" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="D57" s="6" t="s">
-        <v>31</v>
+      <c r="D57" s="5" t="s">
+        <v>14</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="F57" s="1" t="s">
         <v>69</v>
@@ -1962,11 +2020,11 @@
       <c r="C58" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D58" s="6" t="s">
-        <v>7</v>
+      <c r="D58" s="5" t="s">
+        <v>34</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>6</v>
+        <v>41</v>
       </c>
       <c r="F58" s="1" t="s">
         <v>69</v>
@@ -1982,11 +2040,11 @@
       <c r="C59" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="D59" s="6" t="s">
-        <v>7</v>
+      <c r="D59" s="5" t="s">
+        <v>34</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
       <c r="F59" s="1" t="s">
         <v>69</v>
@@ -2002,11 +2060,11 @@
       <c r="C60" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D60" s="6" t="s">
-        <v>9</v>
+      <c r="D60" s="5" t="s">
+        <v>16</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="F60" s="1" t="s">
         <v>69</v>
@@ -2022,11 +2080,11 @@
       <c r="C61" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="D61" s="6" t="s">
-        <v>9</v>
+      <c r="D61" s="5" t="s">
+        <v>16</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="F61" s="1" t="s">
         <v>69</v>
@@ -2040,13 +2098,13 @@
         <v>5</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="D62" s="6" t="s">
-        <v>28</v>
+        <v>5</v>
+      </c>
+      <c r="D62" s="5" t="s">
+        <v>40</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>71</v>
+        <v>39</v>
       </c>
       <c r="F62" s="1" t="s">
         <v>69</v>
@@ -2060,13 +2118,13 @@
         <v>5</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="D63" s="6" t="s">
-        <v>43</v>
+        <v>47</v>
+      </c>
+      <c r="D63" s="5" t="s">
+        <v>40</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>72</v>
+        <v>58</v>
       </c>
       <c r="F63" s="1" t="s">
         <v>69</v>
@@ -2080,13 +2138,13 @@
         <v>5</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="D64" s="6" t="s">
-        <v>30</v>
+        <v>5</v>
+      </c>
+      <c r="D64" s="5" t="s">
+        <v>18</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>73</v>
+        <v>17</v>
       </c>
       <c r="F64" s="1" t="s">
         <v>69</v>
@@ -2100,13 +2158,13 @@
         <v>5</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="D65" s="6" t="s">
-        <v>13</v>
+        <v>47</v>
+      </c>
+      <c r="D65" s="5" t="s">
+        <v>18</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>74</v>
+        <v>59</v>
       </c>
       <c r="F65" s="1" t="s">
         <v>69</v>
@@ -2120,13 +2178,13 @@
         <v>5</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="D66" s="6" t="s">
-        <v>46</v>
+        <v>5</v>
+      </c>
+      <c r="D66" s="5" t="s">
+        <v>20</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>75</v>
+        <v>19</v>
       </c>
       <c r="F66" s="1" t="s">
         <v>69</v>
@@ -2140,13 +2198,13 @@
         <v>5</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="D67" s="6" t="s">
-        <v>33</v>
+        <v>47</v>
+      </c>
+      <c r="D67" s="5" t="s">
+        <v>20</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>76</v>
+        <v>60</v>
       </c>
       <c r="F67" s="1" t="s">
         <v>69</v>
@@ -2160,13 +2218,13 @@
         <v>5</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="D68" s="6" t="s">
-        <v>36</v>
+        <v>5</v>
+      </c>
+      <c r="D68" s="5" t="s">
+        <v>22</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>77</v>
+        <v>21</v>
       </c>
       <c r="F68" s="1" t="s">
         <v>69</v>
@@ -2180,13 +2238,13 @@
         <v>5</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="D69" s="6" t="s">
-        <v>14</v>
+        <v>47</v>
+      </c>
+      <c r="D69" s="5" t="s">
+        <v>22</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>78</v>
+        <v>61</v>
       </c>
       <c r="F69" s="1" t="s">
         <v>69</v>
@@ -2200,13 +2258,13 @@
         <v>5</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="D70" s="6" t="s">
-        <v>34</v>
+        <v>5</v>
+      </c>
+      <c r="D70" s="5" t="s">
+        <v>38</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>79</v>
+        <v>37</v>
       </c>
       <c r="F70" s="1" t="s">
         <v>69</v>
@@ -2220,13 +2278,13 @@
         <v>5</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="D71" s="6" t="s">
-        <v>16</v>
+        <v>47</v>
+      </c>
+      <c r="D71" s="5" t="s">
+        <v>38</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>80</v>
+        <v>64</v>
       </c>
       <c r="F71" s="1" t="s">
         <v>69</v>
@@ -2240,13 +2298,13 @@
         <v>5</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="D72" s="6" t="s">
-        <v>40</v>
+        <v>5</v>
+      </c>
+      <c r="D72" s="5" t="s">
+        <v>24</v>
       </c>
       <c r="E72" s="1" t="s">
-        <v>82</v>
+        <v>23</v>
       </c>
       <c r="F72" s="1" t="s">
         <v>69</v>
@@ -2260,13 +2318,13 @@
         <v>5</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="D73" s="6" t="s">
-        <v>18</v>
+        <v>47</v>
+      </c>
+      <c r="D73" s="5" t="s">
+        <v>24</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>81</v>
+        <v>62</v>
       </c>
       <c r="F73" s="1" t="s">
         <v>69</v>
@@ -2280,13 +2338,13 @@
         <v>5</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="D74" s="6" t="s">
-        <v>20</v>
+        <v>5</v>
+      </c>
+      <c r="D74" s="5" t="s">
+        <v>26</v>
       </c>
       <c r="E74" s="1" t="s">
-        <v>83</v>
+        <v>25</v>
       </c>
       <c r="F74" s="1" t="s">
         <v>69</v>
@@ -2300,13 +2358,13 @@
         <v>5</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="D75" s="6" t="s">
-        <v>22</v>
+        <v>47</v>
+      </c>
+      <c r="D75" s="5" t="s">
+        <v>26</v>
       </c>
       <c r="E75" s="1" t="s">
-        <v>84</v>
+        <v>63</v>
       </c>
       <c r="F75" s="1" t="s">
         <v>69</v>
@@ -2320,13 +2378,13 @@
         <v>5</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="D76" s="6" t="s">
-        <v>38</v>
+        <v>5</v>
+      </c>
+      <c r="D76" s="5" t="s">
+        <v>31</v>
       </c>
       <c r="E76" s="1" t="s">
-        <v>85</v>
+        <v>44</v>
       </c>
       <c r="F76" s="1" t="s">
         <v>69</v>
@@ -2340,13 +2398,13 @@
         <v>5</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="D77" s="6" t="s">
-        <v>24</v>
+        <v>47</v>
+      </c>
+      <c r="D77" s="5" t="s">
+        <v>31</v>
       </c>
       <c r="E77" s="1" t="s">
-        <v>86</v>
+        <v>65</v>
       </c>
       <c r="F77" s="1" t="s">
         <v>69</v>
@@ -2360,13 +2418,13 @@
         <v>5</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="D78" s="6" t="s">
-        <v>26</v>
+        <v>5</v>
+      </c>
+      <c r="D78" s="5" t="s">
+        <v>7</v>
       </c>
       <c r="E78" s="1" t="s">
-        <v>87</v>
+        <v>6</v>
       </c>
       <c r="F78" s="1" t="s">
         <v>69</v>
@@ -2380,13 +2438,13 @@
         <v>5</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="D79" s="6" t="s">
-        <v>31</v>
+        <v>47</v>
+      </c>
+      <c r="D79" s="5" t="s">
+        <v>7</v>
       </c>
       <c r="E79" s="1" t="s">
-        <v>88</v>
+        <v>66</v>
       </c>
       <c r="F79" s="1" t="s">
         <v>69</v>
@@ -2400,13 +2458,13 @@
         <v>5</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="D80" s="6" t="s">
-        <v>7</v>
+        <v>5</v>
+      </c>
+      <c r="D80" s="5" t="s">
+        <v>9</v>
       </c>
       <c r="E80" s="1" t="s">
-        <v>89</v>
+        <v>8</v>
       </c>
       <c r="F80" s="1" t="s">
         <v>69</v>
@@ -2420,21 +2478,421 @@
         <v>5</v>
       </c>
       <c r="C81" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D81" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E81" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F81" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A82" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B82" s="2">
+        <v>5</v>
+      </c>
+      <c r="C82" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="D81" s="6" t="s">
+      <c r="D82" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E82" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="F82" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A83" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B83" s="2">
+        <v>5</v>
+      </c>
+      <c r="C83" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D83" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="E83" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="F83" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A84" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B84" s="2">
+        <v>5</v>
+      </c>
+      <c r="C84" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D84" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="E84" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="F84" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A85" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B85" s="2">
+        <v>5</v>
+      </c>
+      <c r="C85" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D85" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E85" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="F85" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A86" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B86" s="2">
+        <v>5</v>
+      </c>
+      <c r="C86" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D86" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="E86" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="F86" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A87" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B87" s="2">
+        <v>5</v>
+      </c>
+      <c r="C87" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D87" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="E87" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="F87" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A88" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B88" s="2">
+        <v>5</v>
+      </c>
+      <c r="C88" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D88" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="E88" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="F88" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A89" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B89" s="2">
+        <v>5</v>
+      </c>
+      <c r="C89" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D89" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E89" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="F89" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A90" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B90" s="2">
+        <v>5</v>
+      </c>
+      <c r="C90" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D90" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E90" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="F90" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A91" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B91" s="2">
+        <v>5</v>
+      </c>
+      <c r="C91" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D91" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E91" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="F91" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A92" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B92" s="2">
+        <v>5</v>
+      </c>
+      <c r="C92" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D92" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="E92" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="F92" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A93" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B93" s="2">
+        <v>5</v>
+      </c>
+      <c r="C93" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D93" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E93" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="F93" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A94" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B94" s="2">
+        <v>5</v>
+      </c>
+      <c r="C94" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D94" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E94" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="F94" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A95" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B95" s="2">
+        <v>5</v>
+      </c>
+      <c r="C95" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D95" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E95" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="F95" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A96" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B96" s="2">
+        <v>5</v>
+      </c>
+      <c r="C96" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D96" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="E96" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="F96" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A97" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B97" s="2">
+        <v>5</v>
+      </c>
+      <c r="C97" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D97" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E97" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="F97" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A98" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B98" s="2">
+        <v>5</v>
+      </c>
+      <c r="C98" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D98" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E98" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="F98" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A99" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B99" s="2">
+        <v>5</v>
+      </c>
+      <c r="C99" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D99" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="E99" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="F99" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A100" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B100" s="2">
+        <v>5</v>
+      </c>
+      <c r="C100" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D100" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E100" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="F100" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A101" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B101" s="2">
+        <v>5</v>
+      </c>
+      <c r="C101" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D101" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="E81" s="1" t="s">
+      <c r="E101" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="F81" s="1" t="s">
+      <c r="F101" s="1" t="s">
         <v>69</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A22:E61">
-    <sortCondition ref="D24:D61"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A42:E81">
+    <sortCondition ref="D44:D81"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Add US related to Information Systems domain
</commit_message>
<xml_diff>
--- a/refair-server/datasets/few shot dataset/FSDataset.xlsx
+++ b/refair-server/datasets/few shot dataset/FSDataset.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\morel\Desktop\Refair\ReFair-App\refair-server\datasets\few shot dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E63F4E66-D898-4B15-9CFC-5D297CFD5D0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9D1C4FE-242D-462A-AD80-1E121E26918A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{80773445-FB61-4F04-A882-1600FD96C55A}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="506" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="606" uniqueCount="156">
   <si>
     <t>Domain cluster</t>
   </si>
@@ -438,13 +438,79 @@
   </si>
   <si>
     <t>As a legal researcher, I want to apply word embedding models to automate the extraction of key legal concepts and trends from large volumes of legislative texts and regulatory documents, aiding in regulatory compliance analysis and policy research.</t>
+  </si>
+  <si>
+    <t>Information Systems &amp; News</t>
+  </si>
+  <si>
+    <t>Information Systems</t>
+  </si>
+  <si>
+    <t>As an information systems analyst, I want to apply adversarial learning techniques to enhance cybersecurity measures, specifically to detect and mitigate advanced persistent threats (APTs), in order to safeguard sensitive organizational data and maintain operational continuity.</t>
+  </si>
+  <si>
+    <t>As an IT professional, I want to integrate CNNs into video surveillance systems for real-time object detection and tracking, enhancing security monitoring capabilities and ensuring prompt response to potential security incidents.</t>
+  </si>
+  <si>
+    <t>As an information systems manager, I want to integrate a conversational agent into our knowledge management system to facilitate collaborative problem-solving among team members, fostering innovation and knowledge sharing within our organization</t>
+  </si>
+  <si>
+    <t>As an information systems analyst, I want to employ decision trees to optimize resource allocation in IT infrastructure management, ensuring efficient use of hardware and software resources based on workload and performance metrics.</t>
+  </si>
+  <si>
+    <t>As an information systems analyst, I want to develop document classification algorithms to categorize technical documentation based on product features and specifications, improving accessibility and usability for engineering teams.</t>
+  </si>
+  <si>
+    <t>As an IT professional, I want to develop entity extraction capabilities to parse and extract relevant information from customer emails and support tickets, enabling automated routing and efficient resolution of customer inquiries.</t>
+  </si>
+  <si>
+    <t>As an IT professional, I want to implement feature selection methods in network traffic analysis to identify and prioritize key network parameters affecting performance and security, optimizing resource allocation and enhancing cybersecurity measures.</t>
+  </si>
+  <si>
+    <t>As an information systems manager, I want to implement solutions for imbalanced datasets in healthcare data analysis to improve disease prediction models and early diagnosis capabilities, enhancing patient care and healthcare outcomes.</t>
+  </si>
+  <si>
+    <t>As an information systems analyst, I aim to implement keyword extraction algorithms to analyze technical documents and extract essential terms related to software specifications, facilitating effective documentation and knowledge management within our IT department.</t>
+  </si>
+  <si>
+    <t>As an information systems analyst, I aim to deploy k-Nearest Neighbor models to classify customer support tickets based on similarity to resolved cases, automating ticket routing and improving efficiency in resolving customer inquiries.</t>
+  </si>
+  <si>
+    <t>As an IT professional, I want to deploy multi-label classification models in content moderation systems to classify social media posts into multiple categories such as hate speech, misinformation, and spam, ensuring a safer online environment.</t>
+  </si>
+  <si>
+    <t>As an information systems analyst, I aim to develop a neural network-based recommendation system that suggests personalized news articles to readers based on their browsing history and preferences, enhancing user engagement and retention on our news platform.</t>
+  </si>
+  <si>
+    <t>As an information systems manager, I aim to integrate random forest models into our healthcare analytics system to predict patient outcomes based on medical history and treatment data, supporting personalized healthcare delivery and improving patient care.</t>
+  </si>
+  <si>
+    <t>As an information systems analyst, I aim to develop a semantic similarity model to automatically match job descriptions with candidate resumes, streamlining the recruitment process and improving efficiency in talent acquisition.</t>
+  </si>
+  <si>
+    <t>As an IT professional, I want to integrate sentiment analysis algorithms into our product review system to automatically classify customer sentiments (positive, negative, neutral), providing actionable insights for product improvement and marketing strategies.</t>
+  </si>
+  <si>
+    <t>As an information systems analyst, I aim to develop a speech to text application for converting recorded meetings and discussions into text format, facilitating easier documentation and knowledge sharing within our organization.</t>
+  </si>
+  <si>
+    <t>As an information systems analyst, I aim to implement text categorization algorithms to automatically classify incoming emails and support tickets based on their topics and urgency, improving response times and customer satisfaction.</t>
+  </si>
+  <si>
+    <t>As an IT professional, I want to implement unsupervised clustering models to analyze user behavior patterns on our website, segmenting users into clusters based on their browsing habits to personalize user experiences and optimize website navigation.</t>
+  </si>
+  <si>
+    <t>As an information systems analyst, I aim to integrate voice recognition technology into our customer service platform to enable hands-free interaction for users, improving accessibility and user satisfaction.</t>
+  </si>
+  <si>
+    <t>As an information systems analyst, I aim to implement word embedding models to map technical documentation and software manuals into a semantic space, facilitating better search and retrieval capabilities for our engineering team.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -471,8 +537,13 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -491,6 +562,12 @@
         <bgColor rgb="FFE6B8AF"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCFE2F3"/>
+        <bgColor rgb="FFCFE2F3"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -504,7 +581,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -521,6 +598,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -855,10 +933,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8DF0B04-8323-4309-B759-D1CDDA1FBB0E}">
-  <dimension ref="A1:F101"/>
+  <dimension ref="A1:F121"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -891,400 +969,400 @@
       </c>
     </row>
     <row r="2" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="B2" s="7">
-        <v>4</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="D2" s="4" t="s">
+      <c r="A2" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="B2" s="8">
+        <v>3</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="D2" s="5" t="s">
         <v>28</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>114</v>
+        <v>136</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="3" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="B3" s="7">
-        <v>4</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>28</v>
+      <c r="A3" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="B3" s="8">
+        <v>3</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>43</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>93</v>
+        <v>137</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="4" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="B4" s="7">
-        <v>4</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>43</v>
+      <c r="A4" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="B4" s="8">
+        <v>3</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>30</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>115</v>
+        <v>138</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="5" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="B5" s="7">
-        <v>4</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>43</v>
+      <c r="A5" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="B5" s="8">
+        <v>3</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>13</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>94</v>
+        <v>139</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="6" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="B6" s="7">
-        <v>4</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>30</v>
+      <c r="A6" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="B6" s="8">
+        <v>3</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>46</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>116</v>
+        <v>140</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="7" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="B7" s="7">
-        <v>4</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>30</v>
+      <c r="A7" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="B7" s="8">
+        <v>3</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>33</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>95</v>
+        <v>141</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="8" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="B8" s="7">
-        <v>4</v>
-      </c>
-      <c r="C8" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>13</v>
+      <c r="A8" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="B8" s="8">
+        <v>3</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>36</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>117</v>
+        <v>142</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="9" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="B9" s="7">
-        <v>4</v>
-      </c>
-      <c r="C9" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>13</v>
+      <c r="A9" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="B9" s="8">
+        <v>3</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>14</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>96</v>
+        <v>143</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="10" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="B10" s="7">
-        <v>4</v>
-      </c>
-      <c r="C10" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>46</v>
+      <c r="A10" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="B10" s="8">
+        <v>3</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>34</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>118</v>
+        <v>144</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="11" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="B11" s="7">
-        <v>4</v>
-      </c>
-      <c r="C11" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>46</v>
+      <c r="A11" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="B11" s="8">
+        <v>3</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>16</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>97</v>
+        <v>145</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="12" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="B12" s="7">
-        <v>4</v>
-      </c>
-      <c r="C12" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>33</v>
+      <c r="A12" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="B12" s="8">
+        <v>3</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>40</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>119</v>
+        <v>146</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="13" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="B13" s="7">
-        <v>4</v>
-      </c>
-      <c r="C13" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>33</v>
+      <c r="A13" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="B13" s="8">
+        <v>3</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>18</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>98</v>
+        <v>147</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="14" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="B14" s="7">
-        <v>4</v>
-      </c>
-      <c r="C14" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>36</v>
+      <c r="A14" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="B14" s="8">
+        <v>3</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>20</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>120</v>
+        <v>148</v>
       </c>
       <c r="F14" s="1" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="15" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="B15" s="7">
-        <v>4</v>
-      </c>
-      <c r="C15" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="D15" s="4" t="s">
-        <v>36</v>
+      <c r="A15" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="B15" s="8">
+        <v>3</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>22</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>99</v>
+        <v>149</v>
       </c>
       <c r="F15" s="1" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="16" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="B16" s="7">
-        <v>4</v>
-      </c>
-      <c r="C16" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="D16" s="4" t="s">
-        <v>14</v>
+      <c r="A16" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="B16" s="8">
+        <v>3</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>38</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>121</v>
+        <v>150</v>
       </c>
       <c r="F16" s="1" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="17" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="B17" s="7">
-        <v>4</v>
-      </c>
-      <c r="C17" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="D17" s="4" t="s">
-        <v>14</v>
+      <c r="A17" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="B17" s="8">
+        <v>3</v>
+      </c>
+      <c r="C17" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>24</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>100</v>
+        <v>151</v>
       </c>
       <c r="F17" s="1" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="18" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="B18" s="7">
-        <v>4</v>
-      </c>
-      <c r="C18" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="D18" s="4" t="s">
-        <v>34</v>
+      <c r="A18" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="B18" s="8">
+        <v>3</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>26</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>122</v>
+        <v>152</v>
       </c>
       <c r="F18" s="1" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="19" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="B19" s="7">
-        <v>4</v>
-      </c>
-      <c r="C19" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="D19" s="4" t="s">
-        <v>34</v>
+      <c r="A19" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="B19" s="8">
+        <v>3</v>
+      </c>
+      <c r="C19" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>31</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>101</v>
+        <v>153</v>
       </c>
       <c r="F19" s="1" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="20" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="B20" s="7">
-        <v>4</v>
-      </c>
-      <c r="C20" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="D20" s="4" t="s">
-        <v>16</v>
+      <c r="A20" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="B20" s="8">
+        <v>3</v>
+      </c>
+      <c r="C20" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>7</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>123</v>
+        <v>154</v>
       </c>
       <c r="F20" s="1" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="21" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="B21" s="7">
-        <v>4</v>
-      </c>
-      <c r="C21" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="D21" s="4" t="s">
-        <v>16</v>
+      <c r="A21" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="B21" s="8">
+        <v>3</v>
+      </c>
+      <c r="C21" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>9</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>102</v>
+        <v>155</v>
       </c>
       <c r="F21" s="1" t="s">
         <v>69</v>
@@ -1301,10 +1379,10 @@
         <v>113</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>124</v>
+        <v>114</v>
       </c>
       <c r="F22" s="1" t="s">
         <v>69</v>
@@ -1321,10 +1399,10 @@
         <v>92</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>103</v>
+        <v>93</v>
       </c>
       <c r="F23" s="1" t="s">
         <v>69</v>
@@ -1341,10 +1419,10 @@
         <v>113</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>18</v>
+        <v>43</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>125</v>
+        <v>115</v>
       </c>
       <c r="F24" s="1" t="s">
         <v>69</v>
@@ -1361,10 +1439,10 @@
         <v>92</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>18</v>
+        <v>43</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>104</v>
+        <v>94</v>
       </c>
       <c r="F25" s="1" t="s">
         <v>69</v>
@@ -1381,10 +1459,10 @@
         <v>113</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
       <c r="F26" s="1" t="s">
         <v>69</v>
@@ -1401,10 +1479,10 @@
         <v>92</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>105</v>
+        <v>95</v>
       </c>
       <c r="F27" s="1" t="s">
         <v>69</v>
@@ -1421,10 +1499,10 @@
         <v>113</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>127</v>
+        <v>117</v>
       </c>
       <c r="F28" s="1" t="s">
         <v>69</v>
@@ -1441,10 +1519,10 @@
         <v>92</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="F29" s="1" t="s">
         <v>69</v>
@@ -1461,10 +1539,10 @@
         <v>113</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>128</v>
+        <v>118</v>
       </c>
       <c r="F30" s="1" t="s">
         <v>69</v>
@@ -1481,10 +1559,10 @@
         <v>92</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>107</v>
+        <v>97</v>
       </c>
       <c r="F31" s="1" t="s">
         <v>69</v>
@@ -1501,10 +1579,10 @@
         <v>113</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
       <c r="F32" s="1" t="s">
         <v>69</v>
@@ -1521,10 +1599,10 @@
         <v>92</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="F33" s="1" t="s">
         <v>69</v>
@@ -1541,10 +1619,10 @@
         <v>113</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>26</v>
+        <v>36</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="F34" s="1" t="s">
         <v>69</v>
@@ -1561,10 +1639,10 @@
         <v>92</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="E35" s="6" t="s">
-        <v>109</v>
+        <v>36</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>99</v>
       </c>
       <c r="F35" s="1" t="s">
         <v>69</v>
@@ -1581,10 +1659,10 @@
         <v>113</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>31</v>
+        <v>14</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>131</v>
+        <v>121</v>
       </c>
       <c r="F36" s="1" t="s">
         <v>69</v>
@@ -1601,10 +1679,10 @@
         <v>92</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>31</v>
+        <v>14</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="F37" s="1" t="s">
         <v>69</v>
@@ -1621,10 +1699,10 @@
         <v>113</v>
       </c>
       <c r="D38" s="4" t="s">
-        <v>7</v>
+        <v>34</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>132</v>
+        <v>122</v>
       </c>
       <c r="F38" s="1" t="s">
         <v>69</v>
@@ -1641,10 +1719,10 @@
         <v>92</v>
       </c>
       <c r="D39" s="4" t="s">
-        <v>7</v>
+        <v>34</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
       <c r="F39" s="1" t="s">
         <v>69</v>
@@ -1661,10 +1739,10 @@
         <v>113</v>
       </c>
       <c r="D40" s="4" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>133</v>
+        <v>123</v>
       </c>
       <c r="F40" s="1" t="s">
         <v>69</v>
@@ -1681,410 +1759,410 @@
         <v>92</v>
       </c>
       <c r="D41" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="B42" s="7">
+        <v>4</v>
+      </c>
+      <c r="C42" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="D42" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="B43" s="7">
+        <v>4</v>
+      </c>
+      <c r="C43" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="D43" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="F43" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="B44" s="7">
+        <v>4</v>
+      </c>
+      <c r="C44" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="D44" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="F44" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="B45" s="7">
+        <v>4</v>
+      </c>
+      <c r="C45" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="D45" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="F45" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="B46" s="7">
+        <v>4</v>
+      </c>
+      <c r="C46" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="D46" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="F46" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="B47" s="7">
+        <v>4</v>
+      </c>
+      <c r="C47" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="D47" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="F47" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="B48" s="7">
+        <v>4</v>
+      </c>
+      <c r="C48" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="D48" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="F48" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="B49" s="7">
+        <v>4</v>
+      </c>
+      <c r="C49" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="D49" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="F49" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="B50" s="7">
+        <v>4</v>
+      </c>
+      <c r="C50" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="D50" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="F50" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="B51" s="7">
+        <v>4</v>
+      </c>
+      <c r="C51" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="D51" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="E51" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="F51" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="B52" s="7">
+        <v>4</v>
+      </c>
+      <c r="C52" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="D52" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E52" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="F52" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="B53" s="7">
+        <v>4</v>
+      </c>
+      <c r="C53" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="D53" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E53" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="F53" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="B54" s="7">
+        <v>4</v>
+      </c>
+      <c r="C54" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="D54" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="E54" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="F54" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="B55" s="7">
+        <v>4</v>
+      </c>
+      <c r="C55" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="D55" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="E55" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="F55" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="B56" s="7">
+        <v>4</v>
+      </c>
+      <c r="C56" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="D56" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="E56" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="F56" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="B57" s="7">
+        <v>4</v>
+      </c>
+      <c r="C57" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="D57" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="E57" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="F57" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="B58" s="7">
+        <v>4</v>
+      </c>
+      <c r="C58" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="D58" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E58" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="F58" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="B59" s="7">
+        <v>4</v>
+      </c>
+      <c r="C59" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="D59" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E59" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="F59" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="B60" s="7">
+        <v>4</v>
+      </c>
+      <c r="C60" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="D60" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="E41" s="1" t="s">
+      <c r="E60" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="F60" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="B61" s="7">
+        <v>4</v>
+      </c>
+      <c r="C61" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="D61" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E61" s="1" t="s">
         <v>112</v>
-      </c>
-      <c r="F41" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A42" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B42" s="2">
-        <v>5</v>
-      </c>
-      <c r="C42" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D42" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E42" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="F42" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A43" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B43" s="2">
-        <v>5</v>
-      </c>
-      <c r="C43" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="D43" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E43" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="F43" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A44" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B44" s="2">
-        <v>5</v>
-      </c>
-      <c r="C44" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D44" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="E44" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="F44" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A45" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B45" s="2">
-        <v>5</v>
-      </c>
-      <c r="C45" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="D45" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="E45" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="F45" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A46" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B46" s="2">
-        <v>5</v>
-      </c>
-      <c r="C46" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D46" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="E46" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="F46" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A47" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B47" s="2">
-        <v>5</v>
-      </c>
-      <c r="C47" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="D47" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="E47" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="F47" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A48" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B48" s="2">
-        <v>5</v>
-      </c>
-      <c r="C48" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D48" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="E48" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F48" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A49" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B49" s="2">
-        <v>5</v>
-      </c>
-      <c r="C49" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="D49" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="E49" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="F49" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A50" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B50" s="2">
-        <v>5</v>
-      </c>
-      <c r="C50" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D50" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="E50" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="F50" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A51" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B51" s="2">
-        <v>5</v>
-      </c>
-      <c r="C51" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="D51" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="E51" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="F51" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A52" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B52" s="2">
-        <v>5</v>
-      </c>
-      <c r="C52" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D52" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="E52" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="F52" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A53" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B53" s="2">
-        <v>5</v>
-      </c>
-      <c r="C53" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="D53" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="E53" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="F53" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A54" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B54" s="2">
-        <v>5</v>
-      </c>
-      <c r="C54" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D54" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="E54" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="F54" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A55" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B55" s="2">
-        <v>5</v>
-      </c>
-      <c r="C55" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="D55" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="E55" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="F55" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A56" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B56" s="2">
-        <v>5</v>
-      </c>
-      <c r="C56" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D56" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="E56" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F56" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A57" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B57" s="2">
-        <v>5</v>
-      </c>
-      <c r="C57" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="D57" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="E57" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="F57" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A58" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B58" s="2">
-        <v>5</v>
-      </c>
-      <c r="C58" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D58" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="E58" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="F58" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A59" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B59" s="2">
-        <v>5</v>
-      </c>
-      <c r="C59" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="D59" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="E59" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="F59" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A60" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B60" s="2">
-        <v>5</v>
-      </c>
-      <c r="C60" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D60" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="E60" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F60" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A61" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B61" s="2">
-        <v>5</v>
-      </c>
-      <c r="C61" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="D61" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="E61" s="1" t="s">
-        <v>57</v>
       </c>
       <c r="F61" s="1" t="s">
         <v>69</v>
@@ -2101,10 +2179,10 @@
         <v>5</v>
       </c>
       <c r="D62" s="5" t="s">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="F62" s="1" t="s">
         <v>69</v>
@@ -2121,10 +2199,10 @@
         <v>47</v>
       </c>
       <c r="D63" s="5" t="s">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="F63" s="1" t="s">
         <v>69</v>
@@ -2141,10 +2219,10 @@
         <v>5</v>
       </c>
       <c r="D64" s="5" t="s">
-        <v>18</v>
+        <v>43</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>17</v>
+        <v>42</v>
       </c>
       <c r="F64" s="1" t="s">
         <v>69</v>
@@ -2161,10 +2239,10 @@
         <v>47</v>
       </c>
       <c r="D65" s="5" t="s">
-        <v>18</v>
+        <v>43</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
       <c r="F65" s="1" t="s">
         <v>69</v>
@@ -2181,10 +2259,10 @@
         <v>5</v>
       </c>
       <c r="D66" s="5" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="F66" s="1" t="s">
         <v>69</v>
@@ -2201,10 +2279,10 @@
         <v>47</v>
       </c>
       <c r="D67" s="5" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="F67" s="1" t="s">
         <v>69</v>
@@ -2221,10 +2299,10 @@
         <v>5</v>
       </c>
       <c r="D68" s="5" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="F68" s="1" t="s">
         <v>69</v>
@@ -2241,10 +2319,10 @@
         <v>47</v>
       </c>
       <c r="D69" s="5" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="F69" s="1" t="s">
         <v>69</v>
@@ -2261,10 +2339,10 @@
         <v>5</v>
       </c>
       <c r="D70" s="5" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="F70" s="1" t="s">
         <v>69</v>
@@ -2281,10 +2359,10 @@
         <v>47</v>
       </c>
       <c r="D71" s="5" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>64</v>
+        <v>53</v>
       </c>
       <c r="F71" s="1" t="s">
         <v>69</v>
@@ -2301,10 +2379,10 @@
         <v>5</v>
       </c>
       <c r="D72" s="5" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="E72" s="1" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="F72" s="1" t="s">
         <v>69</v>
@@ -2321,10 +2399,10 @@
         <v>47</v>
       </c>
       <c r="D73" s="5" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="F73" s="1" t="s">
         <v>69</v>
@@ -2341,10 +2419,10 @@
         <v>5</v>
       </c>
       <c r="D74" s="5" t="s">
-        <v>26</v>
+        <v>36</v>
       </c>
       <c r="E74" s="1" t="s">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="F74" s="1" t="s">
         <v>69</v>
@@ -2361,10 +2439,10 @@
         <v>47</v>
       </c>
       <c r="D75" s="5" t="s">
-        <v>26</v>
+        <v>36</v>
       </c>
       <c r="E75" s="1" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="F75" s="1" t="s">
         <v>69</v>
@@ -2381,10 +2459,10 @@
         <v>5</v>
       </c>
       <c r="D76" s="5" t="s">
-        <v>31</v>
+        <v>14</v>
       </c>
       <c r="E76" s="1" t="s">
-        <v>44</v>
+        <v>12</v>
       </c>
       <c r="F76" s="1" t="s">
         <v>69</v>
@@ -2401,10 +2479,10 @@
         <v>47</v>
       </c>
       <c r="D77" s="5" t="s">
-        <v>31</v>
+        <v>14</v>
       </c>
       <c r="E77" s="1" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="F77" s="1" t="s">
         <v>69</v>
@@ -2421,10 +2499,10 @@
         <v>5</v>
       </c>
       <c r="D78" s="5" t="s">
-        <v>7</v>
+        <v>34</v>
       </c>
       <c r="E78" s="1" t="s">
-        <v>6</v>
+        <v>41</v>
       </c>
       <c r="F78" s="1" t="s">
         <v>69</v>
@@ -2441,10 +2519,10 @@
         <v>47</v>
       </c>
       <c r="D79" s="5" t="s">
-        <v>7</v>
+        <v>34</v>
       </c>
       <c r="E79" s="1" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
       <c r="F79" s="1" t="s">
         <v>69</v>
@@ -2461,10 +2539,10 @@
         <v>5</v>
       </c>
       <c r="D80" s="5" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="E80" s="1" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="F80" s="1" t="s">
         <v>69</v>
@@ -2481,10 +2559,10 @@
         <v>47</v>
       </c>
       <c r="D81" s="5" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="E81" s="1" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="F81" s="1" t="s">
         <v>69</v>
@@ -2498,13 +2576,13 @@
         <v>5</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>70</v>
+        <v>5</v>
       </c>
       <c r="D82" s="5" t="s">
-        <v>28</v>
+        <v>40</v>
       </c>
       <c r="E82" s="1" t="s">
-        <v>71</v>
+        <v>39</v>
       </c>
       <c r="F82" s="1" t="s">
         <v>69</v>
@@ -2518,13 +2596,13 @@
         <v>5</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>70</v>
+        <v>47</v>
       </c>
       <c r="D83" s="5" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="E83" s="1" t="s">
-        <v>72</v>
+        <v>58</v>
       </c>
       <c r="F83" s="1" t="s">
         <v>69</v>
@@ -2538,13 +2616,13 @@
         <v>5</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>70</v>
+        <v>5</v>
       </c>
       <c r="D84" s="5" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="E84" s="1" t="s">
-        <v>73</v>
+        <v>17</v>
       </c>
       <c r="F84" s="1" t="s">
         <v>69</v>
@@ -2558,13 +2636,13 @@
         <v>5</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>70</v>
+        <v>47</v>
       </c>
       <c r="D85" s="5" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="E85" s="1" t="s">
-        <v>74</v>
+        <v>59</v>
       </c>
       <c r="F85" s="1" t="s">
         <v>69</v>
@@ -2578,13 +2656,13 @@
         <v>5</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>70</v>
+        <v>5</v>
       </c>
       <c r="D86" s="5" t="s">
-        <v>46</v>
+        <v>20</v>
       </c>
       <c r="E86" s="1" t="s">
-        <v>75</v>
+        <v>19</v>
       </c>
       <c r="F86" s="1" t="s">
         <v>69</v>
@@ -2598,13 +2676,13 @@
         <v>5</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>70</v>
+        <v>47</v>
       </c>
       <c r="D87" s="5" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
       <c r="E87" s="1" t="s">
-        <v>76</v>
+        <v>60</v>
       </c>
       <c r="F87" s="1" t="s">
         <v>69</v>
@@ -2618,13 +2696,13 @@
         <v>5</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>70</v>
+        <v>5</v>
       </c>
       <c r="D88" s="5" t="s">
-        <v>36</v>
+        <v>22</v>
       </c>
       <c r="E88" s="1" t="s">
-        <v>77</v>
+        <v>21</v>
       </c>
       <c r="F88" s="1" t="s">
         <v>69</v>
@@ -2638,13 +2716,13 @@
         <v>5</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>70</v>
+        <v>47</v>
       </c>
       <c r="D89" s="5" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="E89" s="1" t="s">
-        <v>78</v>
+        <v>61</v>
       </c>
       <c r="F89" s="1" t="s">
         <v>69</v>
@@ -2658,13 +2736,13 @@
         <v>5</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>70</v>
+        <v>5</v>
       </c>
       <c r="D90" s="5" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="E90" s="1" t="s">
-        <v>79</v>
+        <v>37</v>
       </c>
       <c r="F90" s="1" t="s">
         <v>69</v>
@@ -2678,13 +2756,13 @@
         <v>5</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>70</v>
+        <v>47</v>
       </c>
       <c r="D91" s="5" t="s">
-        <v>16</v>
+        <v>38</v>
       </c>
       <c r="E91" s="1" t="s">
-        <v>80</v>
+        <v>64</v>
       </c>
       <c r="F91" s="1" t="s">
         <v>69</v>
@@ -2698,13 +2776,13 @@
         <v>5</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>70</v>
+        <v>5</v>
       </c>
       <c r="D92" s="5" t="s">
-        <v>40</v>
+        <v>24</v>
       </c>
       <c r="E92" s="1" t="s">
-        <v>82</v>
+        <v>23</v>
       </c>
       <c r="F92" s="1" t="s">
         <v>69</v>
@@ -2718,13 +2796,13 @@
         <v>5</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>70</v>
+        <v>47</v>
       </c>
       <c r="D93" s="5" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="E93" s="1" t="s">
-        <v>81</v>
+        <v>62</v>
       </c>
       <c r="F93" s="1" t="s">
         <v>69</v>
@@ -2738,13 +2816,13 @@
         <v>5</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>70</v>
+        <v>5</v>
       </c>
       <c r="D94" s="5" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="E94" s="1" t="s">
-        <v>83</v>
+        <v>25</v>
       </c>
       <c r="F94" s="1" t="s">
         <v>69</v>
@@ -2758,13 +2836,13 @@
         <v>5</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>70</v>
+        <v>47</v>
       </c>
       <c r="D95" s="5" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="E95" s="1" t="s">
-        <v>84</v>
+        <v>63</v>
       </c>
       <c r="F95" s="1" t="s">
         <v>69</v>
@@ -2778,13 +2856,13 @@
         <v>5</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>70</v>
+        <v>5</v>
       </c>
       <c r="D96" s="5" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="E96" s="1" t="s">
-        <v>85</v>
+        <v>44</v>
       </c>
       <c r="F96" s="1" t="s">
         <v>69</v>
@@ -2798,13 +2876,13 @@
         <v>5</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>70</v>
+        <v>47</v>
       </c>
       <c r="D97" s="5" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="E97" s="1" t="s">
-        <v>86</v>
+        <v>65</v>
       </c>
       <c r="F97" s="1" t="s">
         <v>69</v>
@@ -2818,13 +2896,13 @@
         <v>5</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>70</v>
+        <v>5</v>
       </c>
       <c r="D98" s="5" t="s">
-        <v>26</v>
+        <v>7</v>
       </c>
       <c r="E98" s="1" t="s">
-        <v>87</v>
+        <v>6</v>
       </c>
       <c r="F98" s="1" t="s">
         <v>69</v>
@@ -2838,13 +2916,13 @@
         <v>5</v>
       </c>
       <c r="C99" s="2" t="s">
-        <v>70</v>
+        <v>47</v>
       </c>
       <c r="D99" s="5" t="s">
-        <v>31</v>
+        <v>7</v>
       </c>
       <c r="E99" s="1" t="s">
-        <v>88</v>
+        <v>66</v>
       </c>
       <c r="F99" s="1" t="s">
         <v>69</v>
@@ -2858,13 +2936,13 @@
         <v>5</v>
       </c>
       <c r="C100" s="2" t="s">
-        <v>70</v>
+        <v>5</v>
       </c>
       <c r="D100" s="5" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="E100" s="1" t="s">
-        <v>89</v>
+        <v>8</v>
       </c>
       <c r="F100" s="1" t="s">
         <v>69</v>
@@ -2878,21 +2956,421 @@
         <v>5</v>
       </c>
       <c r="C101" s="2" t="s">
-        <v>70</v>
+        <v>47</v>
       </c>
       <c r="D101" s="5" t="s">
         <v>9</v>
       </c>
       <c r="E101" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F101" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A102" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B102" s="2">
+        <v>5</v>
+      </c>
+      <c r="C102" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D102" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E102" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="F102" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A103" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B103" s="2">
+        <v>5</v>
+      </c>
+      <c r="C103" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D103" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="E103" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="F103" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A104" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B104" s="2">
+        <v>5</v>
+      </c>
+      <c r="C104" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D104" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="E104" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="F104" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A105" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B105" s="2">
+        <v>5</v>
+      </c>
+      <c r="C105" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D105" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E105" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="F105" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A106" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B106" s="2">
+        <v>5</v>
+      </c>
+      <c r="C106" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D106" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="E106" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="F106" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A107" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B107" s="2">
+        <v>5</v>
+      </c>
+      <c r="C107" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D107" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="E107" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="F107" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A108" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B108" s="2">
+        <v>5</v>
+      </c>
+      <c r="C108" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D108" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="E108" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="F108" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A109" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B109" s="2">
+        <v>5</v>
+      </c>
+      <c r="C109" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D109" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E109" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="F109" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A110" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B110" s="2">
+        <v>5</v>
+      </c>
+      <c r="C110" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D110" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E110" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="F110" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A111" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B111" s="2">
+        <v>5</v>
+      </c>
+      <c r="C111" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D111" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E111" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="F111" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A112" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B112" s="2">
+        <v>5</v>
+      </c>
+      <c r="C112" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D112" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="E112" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="F112" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A113" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B113" s="2">
+        <v>5</v>
+      </c>
+      <c r="C113" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D113" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E113" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="F113" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A114" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B114" s="2">
+        <v>5</v>
+      </c>
+      <c r="C114" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D114" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E114" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="F114" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A115" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B115" s="2">
+        <v>5</v>
+      </c>
+      <c r="C115" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D115" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E115" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="F115" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A116" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B116" s="2">
+        <v>5</v>
+      </c>
+      <c r="C116" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D116" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="E116" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="F116" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A117" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B117" s="2">
+        <v>5</v>
+      </c>
+      <c r="C117" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D117" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E117" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="F117" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A118" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B118" s="2">
+        <v>5</v>
+      </c>
+      <c r="C118" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D118" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E118" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="F118" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A119" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B119" s="2">
+        <v>5</v>
+      </c>
+      <c r="C119" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D119" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="E119" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="F119" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A120" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B120" s="2">
+        <v>5</v>
+      </c>
+      <c r="C120" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D120" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E120" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="F120" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A121" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B121" s="2">
+        <v>5</v>
+      </c>
+      <c r="C121" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D121" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E121" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="F101" s="1" t="s">
+      <c r="F121" s="1" t="s">
         <v>69</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A42:E81">
-    <sortCondition ref="D44:D81"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A62:E101">
+    <sortCondition ref="D64:D101"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Add US related to News domain & fix order of Linguistics domain
</commit_message>
<xml_diff>
--- a/refair-server/datasets/few shot dataset/FSDataset.xlsx
+++ b/refair-server/datasets/few shot dataset/FSDataset.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\morel\Desktop\Refair\ReFair-App\refair-server\datasets\few shot dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9D1C4FE-242D-462A-AD80-1E121E26918A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4C6B2FC-0718-4391-B56F-A6954D62325F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{80773445-FB61-4F04-A882-1600FD96C55A}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="606" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="706" uniqueCount="177">
   <si>
     <t>Domain cluster</t>
   </si>
@@ -504,6 +504,69 @@
   </si>
   <si>
     <t>As an information systems analyst, I aim to implement word embedding models to map technical documentation and software manuals into a semantic space, facilitating better search and retrieval capabilities for our engineering team.</t>
+  </si>
+  <si>
+    <t>News</t>
+  </si>
+  <si>
+    <t>As a journalist, I want to employ adversarial learning models to identify malicious attempts to manipulate public opinion through comment sections and social media interactions on news articles.</t>
+  </si>
+  <si>
+    <t>As a news organization, I want to deploy CNN models to classify and categorize news images based on content and relevance, improving the visual storytelling capabilities of our news platform.</t>
+  </si>
+  <si>
+    <t>As a news editor, I want to implement a conversational agent that can conduct interviews with newsmakers and automatically generate summaries or transcripts, accelerating the news reporting process and enhancing coverage depth.</t>
+  </si>
+  <si>
+    <t>As a journalist, I want to use decision tree models to classify news articles into relevant categories such as politics, sports, and entertainment, optimizing content organization for our news website.</t>
+  </si>
+  <si>
+    <t>As a news editor, I want to implement document classification algorithms to automatically categorize incoming news articles into sections such as politics, business, sports, and entertainment, facilitating efficient content management and navigation for our readers.</t>
+  </si>
+  <si>
+    <t>As a journalist, I want to utilize entity extraction models to automatically identify and extract named entities such as people, organizations, and locations mentioned in news articles, enhancing the accuracy and comprehensiveness of our reporting.</t>
+  </si>
+  <si>
+    <t>As a journalist, I want to apply feature selection algorithms to prioritize and extract key information from multimedia elements (images, videos) accompanying news articles, enhancing the visual storytelling impact of our news reports.</t>
+  </si>
+  <si>
+    <t>As a news organization, I want to develop strategies to handle imbalanced datasets in news article classification tasks, ensuring that minority topics or less-covered issues receive adequate representation and visibility.</t>
+  </si>
+  <si>
+    <t>As a news editor, I want to integrate keyword extraction capabilities into our editorial workflow to automatically suggest relevant hashtags for social media promotion of news articles, enhancing visibility and engagement across digital platforms.</t>
+  </si>
+  <si>
+    <t>As a journalist, I want to apply k-nearest neighbor techniques to identify and connect related news stories across different languages or regions, enabling cross-linguistic or international news coverage on our global news platform.</t>
+  </si>
+  <si>
+    <t>As a news editor, I want to implement multi-label classification models to categorize news articles into multiple relevant topics such as politics, economy, and environment, ensuring comprehensive coverage and indexing for our readers.</t>
+  </si>
+  <si>
+    <t>As a news organization, I want to deploy neural network architectures for natural language processing tasks such as summarizing news articles or generating concise headlines, improving content readability and user engagement.</t>
+  </si>
+  <si>
+    <t>As a news editor, I want to utilize random forest algorithms to classify news articles into different categories such as politics, sports, and entertainment based on a combination of textual features and metadata, improving content organization and navigation on our news platform.</t>
+  </si>
+  <si>
+    <t>As a news editor, I want to implement semantic similarity algorithms to automatically detect and merge duplicate or highly similar news articles in our content management system, optimizing resource allocation and improving content quality.</t>
+  </si>
+  <si>
+    <t>As a journalist, I want to apply sentiment analysis to social media comments on news stories so that I can understand public opinion and incorporate it into my reporting.</t>
+  </si>
+  <si>
+    <t>As a journalist, I want to use speech-to-text technology to transcribe interviews and press conferences so that I can quickly produce accurate written content without manual transcription.</t>
+  </si>
+  <si>
+    <t>As a news editor, I want to integrate text categorization tools into our editorial workflow to ensure that breaking news stories are quickly and accurately categorized, allowing for timely and relevant news delivery to our audience.</t>
+  </si>
+  <si>
+    <t>As a journalist, I want to apply unsupervised clustering techniques to identify emerging trends and hot topics in the news so that I can stay ahead of the curve and provide timely coverage.</t>
+  </si>
+  <si>
+    <t>As a journalist, I want to use voice recognition technology to transcribe interviews and press conferences so that I can quickly and accurately produce written articles from spoken content.</t>
+  </si>
+  <si>
+    <t>As a news editor, I want to use word embedding techniques to analyze the semantic similarity between different news articles, allowing me to group related stories and provide comprehensive coverage on our platform.</t>
   </si>
 </sst>
 </file>
@@ -581,7 +644,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -599,6 +662,7 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -933,10 +997,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8DF0B04-8323-4309-B759-D1CDDA1FBB0E}">
-  <dimension ref="A1:F121"/>
+  <dimension ref="A1:F141"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+    <sheetView tabSelected="1" topLeftCell="A130" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2:F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -996,13 +1060,13 @@
         <v>3</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>135</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>43</v>
+        <v>156</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>28</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>137</v>
+        <v>157</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>69</v>
@@ -1019,10 +1083,10 @@
         <v>135</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>69</v>
@@ -1036,13 +1100,13 @@
         <v>3</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>135</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>13</v>
+        <v>156</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>43</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>139</v>
+        <v>158</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>69</v>
@@ -1059,10 +1123,10 @@
         <v>135</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>46</v>
+        <v>30</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>69</v>
@@ -1076,13 +1140,13 @@
         <v>3</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>135</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>33</v>
+        <v>156</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>30</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>141</v>
+        <v>159</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>69</v>
@@ -1099,10 +1163,10 @@
         <v>135</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>36</v>
+        <v>13</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>69</v>
@@ -1116,13 +1180,13 @@
         <v>3</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>135</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>14</v>
+        <v>156</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>13</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>143</v>
+        <v>160</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>69</v>
@@ -1139,10 +1203,10 @@
         <v>135</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>34</v>
+        <v>46</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>69</v>
@@ -1156,13 +1220,13 @@
         <v>3</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>135</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>16</v>
+        <v>156</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>46</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>145</v>
+        <v>161</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>69</v>
@@ -1179,10 +1243,10 @@
         <v>135</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>69</v>
@@ -1196,13 +1260,13 @@
         <v>3</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>135</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>18</v>
+        <v>156</v>
+      </c>
+      <c r="D13" s="9" t="s">
+        <v>33</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>147</v>
+        <v>162</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>69</v>
@@ -1219,10 +1283,10 @@
         <v>135</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>20</v>
+        <v>36</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="F14" s="1" t="s">
         <v>69</v>
@@ -1236,13 +1300,13 @@
         <v>3</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>135</v>
-      </c>
-      <c r="D15" s="5" t="s">
-        <v>22</v>
+        <v>156</v>
+      </c>
+      <c r="D15" s="9" t="s">
+        <v>36</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>149</v>
+        <v>163</v>
       </c>
       <c r="F15" s="1" t="s">
         <v>69</v>
@@ -1259,10 +1323,10 @@
         <v>135</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>38</v>
+        <v>14</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="F16" s="1" t="s">
         <v>69</v>
@@ -1276,13 +1340,13 @@
         <v>3</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>135</v>
-      </c>
-      <c r="D17" s="5" t="s">
-        <v>24</v>
+        <v>156</v>
+      </c>
+      <c r="D17" s="9" t="s">
+        <v>14</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>151</v>
+        <v>164</v>
       </c>
       <c r="F17" s="1" t="s">
         <v>69</v>
@@ -1299,10 +1363,10 @@
         <v>135</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>152</v>
+        <v>144</v>
       </c>
       <c r="F18" s="1" t="s">
         <v>69</v>
@@ -1316,13 +1380,13 @@
         <v>3</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>135</v>
-      </c>
-      <c r="D19" s="5" t="s">
-        <v>31</v>
+        <v>156</v>
+      </c>
+      <c r="D19" s="9" t="s">
+        <v>34</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>153</v>
+        <v>165</v>
       </c>
       <c r="F19" s="1" t="s">
         <v>69</v>
@@ -1339,10 +1403,10 @@
         <v>135</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="F20" s="1" t="s">
         <v>69</v>
@@ -1356,413 +1420,413 @@
         <v>3</v>
       </c>
       <c r="C21" s="8" t="s">
+        <v>156</v>
+      </c>
+      <c r="D21" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="B22" s="8">
+        <v>3</v>
+      </c>
+      <c r="C22" s="8" t="s">
         <v>135</v>
       </c>
-      <c r="D21" s="5" t="s">
+      <c r="D22" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="B23" s="8">
+        <v>3</v>
+      </c>
+      <c r="C23" s="8" t="s">
+        <v>156</v>
+      </c>
+      <c r="D23" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="B24" s="8">
+        <v>3</v>
+      </c>
+      <c r="C24" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="B25" s="8">
+        <v>3</v>
+      </c>
+      <c r="C25" s="8" t="s">
+        <v>156</v>
+      </c>
+      <c r="D25" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="B26" s="8">
+        <v>3</v>
+      </c>
+      <c r="C26" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="B27" s="8">
+        <v>3</v>
+      </c>
+      <c r="C27" s="8" t="s">
+        <v>156</v>
+      </c>
+      <c r="D27" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="B28" s="8">
+        <v>3</v>
+      </c>
+      <c r="C28" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="D28" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="B29" s="8">
+        <v>3</v>
+      </c>
+      <c r="C29" s="8" t="s">
+        <v>156</v>
+      </c>
+      <c r="D29" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="B30" s="8">
+        <v>3</v>
+      </c>
+      <c r="C30" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="D30" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="B31" s="8">
+        <v>3</v>
+      </c>
+      <c r="C31" s="8" t="s">
+        <v>156</v>
+      </c>
+      <c r="D31" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="B32" s="8">
+        <v>3</v>
+      </c>
+      <c r="C32" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="D32" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="B33" s="8">
+        <v>3</v>
+      </c>
+      <c r="C33" s="8" t="s">
+        <v>156</v>
+      </c>
+      <c r="D33" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="B34" s="8">
+        <v>3</v>
+      </c>
+      <c r="C34" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="D34" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="B35" s="8">
+        <v>3</v>
+      </c>
+      <c r="C35" s="8" t="s">
+        <v>156</v>
+      </c>
+      <c r="D35" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="B36" s="8">
+        <v>3</v>
+      </c>
+      <c r="C36" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="D36" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="B37" s="8">
+        <v>3</v>
+      </c>
+      <c r="C37" s="8" t="s">
+        <v>156</v>
+      </c>
+      <c r="D37" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="B38" s="8">
+        <v>3</v>
+      </c>
+      <c r="C38" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="D38" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="B39" s="8">
+        <v>3</v>
+      </c>
+      <c r="C39" s="8" t="s">
+        <v>156</v>
+      </c>
+      <c r="D39" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="F39" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="B40" s="8">
+        <v>3</v>
+      </c>
+      <c r="C40" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="D40" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="E21" s="1" t="s">
+      <c r="E40" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="F21" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="B22" s="7">
-        <v>4</v>
-      </c>
-      <c r="C22" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="D22" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="B23" s="7">
-        <v>4</v>
-      </c>
-      <c r="C23" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="D23" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="F23" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="B24" s="7">
-        <v>4</v>
-      </c>
-      <c r="C24" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="D24" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="F24" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="B25" s="7">
-        <v>4</v>
-      </c>
-      <c r="C25" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="D25" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="F25" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="B26" s="7">
-        <v>4</v>
-      </c>
-      <c r="C26" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="D26" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="E26" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="F26" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="B27" s="7">
-        <v>4</v>
-      </c>
-      <c r="C27" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="D27" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="E27" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="F27" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="B28" s="7">
-        <v>4</v>
-      </c>
-      <c r="C28" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="D28" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E28" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="F28" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="B29" s="7">
-        <v>4</v>
-      </c>
-      <c r="C29" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="D29" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E29" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="F29" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="B30" s="7">
-        <v>4</v>
-      </c>
-      <c r="C30" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="D30" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="E30" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="F30" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="B31" s="7">
-        <v>4</v>
-      </c>
-      <c r="C31" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="D31" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="E31" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="F31" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="B32" s="7">
-        <v>4</v>
-      </c>
-      <c r="C32" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="D32" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="E32" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="F32" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="B33" s="7">
-        <v>4</v>
-      </c>
-      <c r="C33" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="D33" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="E33" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="F33" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="B34" s="7">
-        <v>4</v>
-      </c>
-      <c r="C34" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="D34" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="E34" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="F34" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="B35" s="7">
-        <v>4</v>
-      </c>
-      <c r="C35" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="D35" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="E35" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="F35" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="B36" s="7">
-        <v>4</v>
-      </c>
-      <c r="C36" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="D36" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="E36" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="F36" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="B37" s="7">
-        <v>4</v>
-      </c>
-      <c r="C37" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="D37" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="E37" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="F37" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="B38" s="7">
-        <v>4</v>
-      </c>
-      <c r="C38" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="D38" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="E38" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="F38" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="B39" s="7">
-        <v>4</v>
-      </c>
-      <c r="C39" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="D39" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="E39" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="F39" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="B40" s="7">
-        <v>4</v>
-      </c>
-      <c r="C40" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="D40" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="E40" s="1" t="s">
-        <v>123</v>
-      </c>
       <c r="F40" s="1" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="41" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="B41" s="7">
-        <v>4</v>
-      </c>
-      <c r="C41" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="D41" s="4" t="s">
-        <v>16</v>
+      <c r="A41" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="B41" s="8">
+        <v>3</v>
+      </c>
+      <c r="C41" s="8" t="s">
+        <v>156</v>
+      </c>
+      <c r="D41" s="9" t="s">
+        <v>9</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>102</v>
+        <v>176</v>
       </c>
       <c r="F41" s="1" t="s">
         <v>69</v>
@@ -1779,10 +1843,10 @@
         <v>113</v>
       </c>
       <c r="D42" s="4" t="s">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>124</v>
+        <v>114</v>
       </c>
       <c r="F42" s="1" t="s">
         <v>69</v>
@@ -1799,10 +1863,10 @@
         <v>92</v>
       </c>
       <c r="D43" s="4" t="s">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>103</v>
+        <v>93</v>
       </c>
       <c r="F43" s="1" t="s">
         <v>69</v>
@@ -1819,10 +1883,10 @@
         <v>113</v>
       </c>
       <c r="D44" s="4" t="s">
-        <v>18</v>
+        <v>43</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>125</v>
+        <v>115</v>
       </c>
       <c r="F44" s="1" t="s">
         <v>69</v>
@@ -1839,10 +1903,10 @@
         <v>92</v>
       </c>
       <c r="D45" s="4" t="s">
-        <v>18</v>
+        <v>43</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>104</v>
+        <v>94</v>
       </c>
       <c r="F45" s="1" t="s">
         <v>69</v>
@@ -1859,10 +1923,10 @@
         <v>113</v>
       </c>
       <c r="D46" s="4" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
       <c r="F46" s="1" t="s">
         <v>69</v>
@@ -1879,10 +1943,10 @@
         <v>92</v>
       </c>
       <c r="D47" s="4" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>105</v>
+        <v>95</v>
       </c>
       <c r="F47" s="1" t="s">
         <v>69</v>
@@ -1899,10 +1963,10 @@
         <v>113</v>
       </c>
       <c r="D48" s="4" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>127</v>
+        <v>117</v>
       </c>
       <c r="F48" s="1" t="s">
         <v>69</v>
@@ -1919,10 +1983,10 @@
         <v>92</v>
       </c>
       <c r="D49" s="4" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="F49" s="1" t="s">
         <v>69</v>
@@ -1939,10 +2003,10 @@
         <v>113</v>
       </c>
       <c r="D50" s="4" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>128</v>
+        <v>118</v>
       </c>
       <c r="F50" s="1" t="s">
         <v>69</v>
@@ -1959,10 +2023,10 @@
         <v>92</v>
       </c>
       <c r="D51" s="4" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>107</v>
+        <v>97</v>
       </c>
       <c r="F51" s="1" t="s">
         <v>69</v>
@@ -1979,10 +2043,10 @@
         <v>113</v>
       </c>
       <c r="D52" s="4" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
       <c r="F52" s="1" t="s">
         <v>69</v>
@@ -1999,10 +2063,10 @@
         <v>92</v>
       </c>
       <c r="D53" s="4" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="F53" s="1" t="s">
         <v>69</v>
@@ -2019,10 +2083,10 @@
         <v>113</v>
       </c>
       <c r="D54" s="4" t="s">
-        <v>26</v>
+        <v>36</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="F54" s="1" t="s">
         <v>69</v>
@@ -2039,10 +2103,10 @@
         <v>92</v>
       </c>
       <c r="D55" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="E55" s="6" t="s">
-        <v>109</v>
+        <v>36</v>
+      </c>
+      <c r="E55" s="1" t="s">
+        <v>99</v>
       </c>
       <c r="F55" s="1" t="s">
         <v>69</v>
@@ -2059,10 +2123,10 @@
         <v>113</v>
       </c>
       <c r="D56" s="4" t="s">
-        <v>31</v>
+        <v>14</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>131</v>
+        <v>121</v>
       </c>
       <c r="F56" s="1" t="s">
         <v>69</v>
@@ -2079,10 +2143,10 @@
         <v>92</v>
       </c>
       <c r="D57" s="4" t="s">
-        <v>31</v>
+        <v>14</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="F57" s="1" t="s">
         <v>69</v>
@@ -2099,10 +2163,10 @@
         <v>113</v>
       </c>
       <c r="D58" s="4" t="s">
-        <v>7</v>
+        <v>34</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>132</v>
+        <v>122</v>
       </c>
       <c r="F58" s="1" t="s">
         <v>69</v>
@@ -2119,10 +2183,10 @@
         <v>92</v>
       </c>
       <c r="D59" s="4" t="s">
-        <v>7</v>
+        <v>34</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
       <c r="F59" s="1" t="s">
         <v>69</v>
@@ -2139,10 +2203,10 @@
         <v>113</v>
       </c>
       <c r="D60" s="4" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>133</v>
+        <v>123</v>
       </c>
       <c r="F60" s="1" t="s">
         <v>69</v>
@@ -2159,410 +2223,410 @@
         <v>92</v>
       </c>
       <c r="D61" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E61" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="F61" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="B62" s="7">
+        <v>4</v>
+      </c>
+      <c r="C62" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="D62" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="E62" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="F62" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="B63" s="7">
+        <v>4</v>
+      </c>
+      <c r="C63" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="D63" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="E63" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="F63" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="B64" s="7">
+        <v>4</v>
+      </c>
+      <c r="C64" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="D64" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E64" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="F64" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="B65" s="7">
+        <v>4</v>
+      </c>
+      <c r="C65" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="D65" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E65" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="F65" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="B66" s="7">
+        <v>4</v>
+      </c>
+      <c r="C66" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="D66" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E66" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="F66" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A67" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="B67" s="7">
+        <v>4</v>
+      </c>
+      <c r="C67" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="D67" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E67" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="F67" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A68" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="B68" s="7">
+        <v>4</v>
+      </c>
+      <c r="C68" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="D68" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E68" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="F68" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="B69" s="7">
+        <v>4</v>
+      </c>
+      <c r="C69" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="D69" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E69" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="F69" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A70" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="B70" s="7">
+        <v>4</v>
+      </c>
+      <c r="C70" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="D70" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="E70" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="F70" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A71" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="B71" s="7">
+        <v>4</v>
+      </c>
+      <c r="C71" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="D71" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="E71" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="F71" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A72" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="B72" s="7">
+        <v>4</v>
+      </c>
+      <c r="C72" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="D72" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E72" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="F72" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A73" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="B73" s="7">
+        <v>4</v>
+      </c>
+      <c r="C73" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="D73" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E73" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="F73" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A74" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="B74" s="7">
+        <v>4</v>
+      </c>
+      <c r="C74" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="D74" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="E74" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="F74" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A75" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="B75" s="7">
+        <v>4</v>
+      </c>
+      <c r="C75" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="D75" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="E75" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="F75" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A76" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="B76" s="7">
+        <v>4</v>
+      </c>
+      <c r="C76" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="D76" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="E76" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="F76" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A77" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="B77" s="7">
+        <v>4</v>
+      </c>
+      <c r="C77" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="D77" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="E77" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="F77" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A78" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="B78" s="7">
+        <v>4</v>
+      </c>
+      <c r="C78" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="D78" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E78" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="F78" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A79" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="B79" s="7">
+        <v>4</v>
+      </c>
+      <c r="C79" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="D79" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E79" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="F79" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A80" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="B80" s="7">
+        <v>4</v>
+      </c>
+      <c r="C80" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="D80" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="E61" s="1" t="s">
+      <c r="E80" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="F80" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A81" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="B81" s="7">
+        <v>4</v>
+      </c>
+      <c r="C81" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="D81" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E81" s="1" t="s">
         <v>112</v>
-      </c>
-      <c r="F61" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A62" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B62" s="2">
-        <v>5</v>
-      </c>
-      <c r="C62" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D62" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E62" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="F62" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A63" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B63" s="2">
-        <v>5</v>
-      </c>
-      <c r="C63" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="D63" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E63" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="F63" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A64" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B64" s="2">
-        <v>5</v>
-      </c>
-      <c r="C64" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D64" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="E64" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="F64" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A65" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B65" s="2">
-        <v>5</v>
-      </c>
-      <c r="C65" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="D65" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="E65" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="F65" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A66" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B66" s="2">
-        <v>5</v>
-      </c>
-      <c r="C66" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D66" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="E66" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="F66" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A67" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B67" s="2">
-        <v>5</v>
-      </c>
-      <c r="C67" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="D67" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="E67" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="F67" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A68" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B68" s="2">
-        <v>5</v>
-      </c>
-      <c r="C68" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D68" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="E68" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F68" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A69" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B69" s="2">
-        <v>5</v>
-      </c>
-      <c r="C69" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="D69" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="E69" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="F69" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A70" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B70" s="2">
-        <v>5</v>
-      </c>
-      <c r="C70" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D70" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="E70" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="F70" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A71" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B71" s="2">
-        <v>5</v>
-      </c>
-      <c r="C71" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="D71" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="E71" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="F71" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A72" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B72" s="2">
-        <v>5</v>
-      </c>
-      <c r="C72" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D72" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="E72" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="F72" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A73" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B73" s="2">
-        <v>5</v>
-      </c>
-      <c r="C73" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="D73" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="E73" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="F73" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A74" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B74" s="2">
-        <v>5</v>
-      </c>
-      <c r="C74" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D74" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="E74" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="F74" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A75" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B75" s="2">
-        <v>5</v>
-      </c>
-      <c r="C75" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="D75" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="E75" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="F75" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A76" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B76" s="2">
-        <v>5</v>
-      </c>
-      <c r="C76" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D76" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="E76" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F76" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A77" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B77" s="2">
-        <v>5</v>
-      </c>
-      <c r="C77" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="D77" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="E77" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="F77" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A78" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B78" s="2">
-        <v>5</v>
-      </c>
-      <c r="C78" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D78" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="E78" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="F78" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A79" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B79" s="2">
-        <v>5</v>
-      </c>
-      <c r="C79" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="D79" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="E79" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="F79" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A80" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B80" s="2">
-        <v>5</v>
-      </c>
-      <c r="C80" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D80" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="E80" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F80" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A81" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B81" s="2">
-        <v>5</v>
-      </c>
-      <c r="C81" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="D81" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="E81" s="1" t="s">
-        <v>57</v>
       </c>
       <c r="F81" s="1" t="s">
         <v>69</v>
@@ -2579,10 +2643,10 @@
         <v>5</v>
       </c>
       <c r="D82" s="5" t="s">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="E82" s="1" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="F82" s="1" t="s">
         <v>69</v>
@@ -2599,10 +2663,10 @@
         <v>47</v>
       </c>
       <c r="D83" s="5" t="s">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="E83" s="1" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="F83" s="1" t="s">
         <v>69</v>
@@ -2616,13 +2680,13 @@
         <v>5</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>5</v>
+        <v>70</v>
       </c>
       <c r="D84" s="5" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="E84" s="1" t="s">
-        <v>17</v>
+        <v>71</v>
       </c>
       <c r="F84" s="1" t="s">
         <v>69</v>
@@ -2636,13 +2700,13 @@
         <v>5</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>47</v>
+        <v>5</v>
       </c>
       <c r="D85" s="5" t="s">
-        <v>18</v>
+        <v>43</v>
       </c>
       <c r="E85" s="1" t="s">
-        <v>59</v>
+        <v>42</v>
       </c>
       <c r="F85" s="1" t="s">
         <v>69</v>
@@ -2656,13 +2720,13 @@
         <v>5</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>5</v>
+        <v>47</v>
       </c>
       <c r="D86" s="5" t="s">
-        <v>20</v>
+        <v>43</v>
       </c>
       <c r="E86" s="1" t="s">
-        <v>19</v>
+        <v>48</v>
       </c>
       <c r="F86" s="1" t="s">
         <v>69</v>
@@ -2676,13 +2740,13 @@
         <v>5</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>47</v>
+        <v>70</v>
       </c>
       <c r="D87" s="5" t="s">
-        <v>20</v>
+        <v>43</v>
       </c>
       <c r="E87" s="1" t="s">
-        <v>60</v>
+        <v>72</v>
       </c>
       <c r="F87" s="1" t="s">
         <v>69</v>
@@ -2699,10 +2763,10 @@
         <v>5</v>
       </c>
       <c r="D88" s="5" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="E88" s="1" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="F88" s="1" t="s">
         <v>69</v>
@@ -2719,10 +2783,10 @@
         <v>47</v>
       </c>
       <c r="D89" s="5" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="E89" s="1" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="F89" s="1" t="s">
         <v>69</v>
@@ -2736,13 +2800,13 @@
         <v>5</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>5</v>
+        <v>70</v>
       </c>
       <c r="D90" s="5" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="E90" s="1" t="s">
-        <v>37</v>
+        <v>73</v>
       </c>
       <c r="F90" s="1" t="s">
         <v>69</v>
@@ -2756,13 +2820,13 @@
         <v>5</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>47</v>
+        <v>5</v>
       </c>
       <c r="D91" s="5" t="s">
-        <v>38</v>
+        <v>13</v>
       </c>
       <c r="E91" s="1" t="s">
-        <v>64</v>
+        <v>11</v>
       </c>
       <c r="F91" s="1" t="s">
         <v>69</v>
@@ -2776,13 +2840,13 @@
         <v>5</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>5</v>
+        <v>47</v>
       </c>
       <c r="D92" s="5" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="E92" s="1" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
       <c r="F92" s="1" t="s">
         <v>69</v>
@@ -2796,13 +2860,13 @@
         <v>5</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>47</v>
+        <v>70</v>
       </c>
       <c r="D93" s="5" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="E93" s="1" t="s">
-        <v>62</v>
+        <v>74</v>
       </c>
       <c r="F93" s="1" t="s">
         <v>69</v>
@@ -2819,10 +2883,10 @@
         <v>5</v>
       </c>
       <c r="D94" s="5" t="s">
-        <v>26</v>
+        <v>46</v>
       </c>
       <c r="E94" s="1" t="s">
-        <v>25</v>
+        <v>45</v>
       </c>
       <c r="F94" s="1" t="s">
         <v>69</v>
@@ -2839,10 +2903,10 @@
         <v>47</v>
       </c>
       <c r="D95" s="5" t="s">
-        <v>26</v>
+        <v>46</v>
       </c>
       <c r="E95" s="1" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="F95" s="1" t="s">
         <v>69</v>
@@ -2856,13 +2920,13 @@
         <v>5</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>5</v>
+        <v>70</v>
       </c>
       <c r="D96" s="5" t="s">
-        <v>31</v>
+        <v>46</v>
       </c>
       <c r="E96" s="1" t="s">
-        <v>44</v>
+        <v>75</v>
       </c>
       <c r="F96" s="1" t="s">
         <v>69</v>
@@ -2876,13 +2940,13 @@
         <v>5</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>47</v>
+        <v>5</v>
       </c>
       <c r="D97" s="5" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="E97" s="1" t="s">
-        <v>65</v>
+        <v>32</v>
       </c>
       <c r="F97" s="1" t="s">
         <v>69</v>
@@ -2896,13 +2960,13 @@
         <v>5</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>5</v>
+        <v>47</v>
       </c>
       <c r="D98" s="5" t="s">
-        <v>7</v>
+        <v>33</v>
       </c>
       <c r="E98" s="1" t="s">
-        <v>6</v>
+        <v>52</v>
       </c>
       <c r="F98" s="1" t="s">
         <v>69</v>
@@ -2916,13 +2980,13 @@
         <v>5</v>
       </c>
       <c r="C99" s="2" t="s">
-        <v>47</v>
+        <v>70</v>
       </c>
       <c r="D99" s="5" t="s">
-        <v>7</v>
+        <v>33</v>
       </c>
       <c r="E99" s="1" t="s">
-        <v>66</v>
+        <v>76</v>
       </c>
       <c r="F99" s="1" t="s">
         <v>69</v>
@@ -2939,10 +3003,10 @@
         <v>5</v>
       </c>
       <c r="D100" s="5" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
       <c r="E100" s="1" t="s">
-        <v>8</v>
+        <v>35</v>
       </c>
       <c r="F100" s="1" t="s">
         <v>69</v>
@@ -2959,10 +3023,10 @@
         <v>47</v>
       </c>
       <c r="D101" s="5" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
       <c r="E101" s="1" t="s">
-        <v>67</v>
+        <v>54</v>
       </c>
       <c r="F101" s="1" t="s">
         <v>69</v>
@@ -2979,10 +3043,10 @@
         <v>70</v>
       </c>
       <c r="D102" s="5" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="E102" s="1" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="F102" s="1" t="s">
         <v>69</v>
@@ -2996,13 +3060,13 @@
         <v>5</v>
       </c>
       <c r="C103" s="2" t="s">
-        <v>70</v>
+        <v>5</v>
       </c>
       <c r="D103" s="5" t="s">
-        <v>43</v>
+        <v>14</v>
       </c>
       <c r="E103" s="1" t="s">
-        <v>72</v>
+        <v>12</v>
       </c>
       <c r="F103" s="1" t="s">
         <v>69</v>
@@ -3016,13 +3080,13 @@
         <v>5</v>
       </c>
       <c r="C104" s="2" t="s">
-        <v>70</v>
+        <v>47</v>
       </c>
       <c r="D104" s="5" t="s">
-        <v>30</v>
+        <v>14</v>
       </c>
       <c r="E104" s="1" t="s">
-        <v>73</v>
+        <v>55</v>
       </c>
       <c r="F104" s="1" t="s">
         <v>69</v>
@@ -3039,10 +3103,10 @@
         <v>70</v>
       </c>
       <c r="D105" s="5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E105" s="1" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="F105" s="1" t="s">
         <v>69</v>
@@ -3056,13 +3120,13 @@
         <v>5</v>
       </c>
       <c r="C106" s="2" t="s">
-        <v>70</v>
+        <v>5</v>
       </c>
       <c r="D106" s="5" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="E106" s="1" t="s">
-        <v>75</v>
+        <v>41</v>
       </c>
       <c r="F106" s="1" t="s">
         <v>69</v>
@@ -3076,13 +3140,13 @@
         <v>5</v>
       </c>
       <c r="C107" s="2" t="s">
-        <v>70</v>
+        <v>47</v>
       </c>
       <c r="D107" s="5" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E107" s="1" t="s">
-        <v>76</v>
+        <v>56</v>
       </c>
       <c r="F107" s="1" t="s">
         <v>69</v>
@@ -3099,10 +3163,10 @@
         <v>70</v>
       </c>
       <c r="D108" s="5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E108" s="1" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="F108" s="1" t="s">
         <v>69</v>
@@ -3116,13 +3180,13 @@
         <v>5</v>
       </c>
       <c r="C109" s="2" t="s">
-        <v>70</v>
+        <v>5</v>
       </c>
       <c r="D109" s="5" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E109" s="1" t="s">
-        <v>78</v>
+        <v>15</v>
       </c>
       <c r="F109" s="1" t="s">
         <v>69</v>
@@ -3136,13 +3200,13 @@
         <v>5</v>
       </c>
       <c r="C110" s="2" t="s">
-        <v>70</v>
+        <v>47</v>
       </c>
       <c r="D110" s="5" t="s">
-        <v>34</v>
+        <v>16</v>
       </c>
       <c r="E110" s="1" t="s">
-        <v>79</v>
+        <v>57</v>
       </c>
       <c r="F110" s="1" t="s">
         <v>69</v>
@@ -3176,13 +3240,13 @@
         <v>5</v>
       </c>
       <c r="C112" s="2" t="s">
-        <v>70</v>
+        <v>5</v>
       </c>
       <c r="D112" s="5" t="s">
         <v>40</v>
       </c>
       <c r="E112" s="1" t="s">
-        <v>82</v>
+        <v>39</v>
       </c>
       <c r="F112" s="1" t="s">
         <v>69</v>
@@ -3196,13 +3260,13 @@
         <v>5</v>
       </c>
       <c r="C113" s="2" t="s">
-        <v>70</v>
+        <v>47</v>
       </c>
       <c r="D113" s="5" t="s">
-        <v>18</v>
+        <v>40</v>
       </c>
       <c r="E113" s="1" t="s">
-        <v>81</v>
+        <v>58</v>
       </c>
       <c r="F113" s="1" t="s">
         <v>69</v>
@@ -3219,10 +3283,10 @@
         <v>70</v>
       </c>
       <c r="D114" s="5" t="s">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="E114" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F114" s="1" t="s">
         <v>69</v>
@@ -3236,13 +3300,13 @@
         <v>5</v>
       </c>
       <c r="C115" s="2" t="s">
-        <v>70</v>
+        <v>5</v>
       </c>
       <c r="D115" s="5" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="E115" s="1" t="s">
-        <v>84</v>
+        <v>17</v>
       </c>
       <c r="F115" s="1" t="s">
         <v>69</v>
@@ -3256,13 +3320,13 @@
         <v>5</v>
       </c>
       <c r="C116" s="2" t="s">
-        <v>70</v>
+        <v>47</v>
       </c>
       <c r="D116" s="5" t="s">
-        <v>38</v>
+        <v>18</v>
       </c>
       <c r="E116" s="1" t="s">
-        <v>85</v>
+        <v>59</v>
       </c>
       <c r="F116" s="1" t="s">
         <v>69</v>
@@ -3279,10 +3343,10 @@
         <v>70</v>
       </c>
       <c r="D117" s="5" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="E117" s="1" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="F117" s="1" t="s">
         <v>69</v>
@@ -3296,13 +3360,13 @@
         <v>5</v>
       </c>
       <c r="C118" s="2" t="s">
-        <v>70</v>
+        <v>5</v>
       </c>
       <c r="D118" s="5" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="E118" s="1" t="s">
-        <v>87</v>
+        <v>19</v>
       </c>
       <c r="F118" s="1" t="s">
         <v>69</v>
@@ -3316,13 +3380,13 @@
         <v>5</v>
       </c>
       <c r="C119" s="2" t="s">
-        <v>70</v>
+        <v>47</v>
       </c>
       <c r="D119" s="5" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="E119" s="1" t="s">
-        <v>88</v>
+        <v>60</v>
       </c>
       <c r="F119" s="1" t="s">
         <v>69</v>
@@ -3339,10 +3403,10 @@
         <v>70</v>
       </c>
       <c r="D120" s="5" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="E120" s="1" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="F120" s="1" t="s">
         <v>69</v>
@@ -3356,21 +3420,421 @@
         <v>5</v>
       </c>
       <c r="C121" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D121" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E121" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F121" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A122" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B122" s="2">
+        <v>5</v>
+      </c>
+      <c r="C122" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D122" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E122" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="F122" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A123" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B123" s="2">
+        <v>5</v>
+      </c>
+      <c r="C123" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="D121" s="5" t="s">
+      <c r="D123" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E123" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="F123" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A124" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B124" s="2">
+        <v>5</v>
+      </c>
+      <c r="C124" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D124" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="E124" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F124" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A125" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B125" s="2">
+        <v>5</v>
+      </c>
+      <c r="C125" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D125" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="E125" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="F125" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="126" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A126" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B126" s="2">
+        <v>5</v>
+      </c>
+      <c r="C126" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D126" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="E126" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="F126" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="127" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A127" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B127" s="2">
+        <v>5</v>
+      </c>
+      <c r="C127" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D127" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E127" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F127" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="128" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A128" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B128" s="2">
+        <v>5</v>
+      </c>
+      <c r="C128" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D128" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E128" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="F128" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="129" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A129" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B129" s="2">
+        <v>5</v>
+      </c>
+      <c r="C129" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D129" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E129" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="F129" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="130" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A130" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B130" s="2">
+        <v>5</v>
+      </c>
+      <c r="C130" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D130" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E130" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F130" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="131" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A131" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B131" s="2">
+        <v>5</v>
+      </c>
+      <c r="C131" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D131" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E131" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="F131" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="132" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A132" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B132" s="2">
+        <v>5</v>
+      </c>
+      <c r="C132" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D132" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E132" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="F132" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="133" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A133" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B133" s="2">
+        <v>5</v>
+      </c>
+      <c r="C133" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D133" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="E133" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F133" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="134" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A134" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B134" s="2">
+        <v>5</v>
+      </c>
+      <c r="C134" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D134" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="E134" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="F134" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="135" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A135" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B135" s="2">
+        <v>5</v>
+      </c>
+      <c r="C135" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D135" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="E135" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="F135" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="136" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A136" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B136" s="2">
+        <v>5</v>
+      </c>
+      <c r="C136" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D136" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E136" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F136" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="137" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A137" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B137" s="2">
+        <v>5</v>
+      </c>
+      <c r="C137" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D137" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E137" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F137" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="138" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A138" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B138" s="2">
+        <v>5</v>
+      </c>
+      <c r="C138" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D138" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E138" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="F138" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="139" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A139" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B139" s="2">
+        <v>5</v>
+      </c>
+      <c r="C139" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D139" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="E121" s="1" t="s">
+      <c r="E139" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F139" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="140" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A140" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B140" s="2">
+        <v>5</v>
+      </c>
+      <c r="C140" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D140" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E140" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F140" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="141" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A141" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B141" s="2">
+        <v>5</v>
+      </c>
+      <c r="C141" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D141" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E141" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="F121" s="1" t="s">
+      <c r="F141" s="1" t="s">
         <v>69</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A62:E101">
-    <sortCondition ref="D64:D101"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A82:E121">
+    <sortCondition ref="D84:D121"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Add US related to Finance & Marketing domain
</commit_message>
<xml_diff>
--- a/refair-server/datasets/few shot dataset/FSDataset.xlsx
+++ b/refair-server/datasets/few shot dataset/FSDataset.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\morel\Desktop\Refair\ReFair-App\refair-server\datasets\few shot dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4C6B2FC-0718-4391-B56F-A6954D62325F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B859DB2D-0B7B-4DE6-A75C-D15ADA85659F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{80773445-FB61-4F04-A882-1600FD96C55A}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="706" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="806" uniqueCount="199">
   <si>
     <t>Domain cluster</t>
   </si>
@@ -567,6 +567,72 @@
   </si>
   <si>
     <t>As a news editor, I want to use word embedding techniques to analyze the semantic similarity between different news articles, allowing me to group related stories and provide comprehensive coverage on our platform.</t>
+  </si>
+  <si>
+    <t>Economy &amp; Marketing</t>
+  </si>
+  <si>
+    <t>Finance &amp; Marketing</t>
+  </si>
+  <si>
+    <t>As a financial institution, I want to apply adversarial learning techniques to detect and mitigate fraudulent transactions in real-time, so that I can protect our customers' financial assets more effectively.</t>
+  </si>
+  <si>
+    <t>As a financial institution, I want to utilize CNNs to analyze time-series financial data and predict short-term market trends with higher accuracy, enabling us to optimize our investment strategies.</t>
+  </si>
+  <si>
+    <t>As a financial institution, I want to integrate a conversational agent into our mobile banking app to guide users through complex financial processes such as loan applications and investment portfolio management, simplifying the user experience and increasing adoption rates.</t>
+  </si>
+  <si>
+    <t>As a financial analyst, I want to develop a decision tree model to predict stock price movements based on historical market data and economic indicators, assisting investors in making informed trading decisions.</t>
+  </si>
+  <si>
+    <t>As a financial institution, I want to use document classification algorithms to automatically categorize and prioritize incoming financial reports and statements, enabling faster decision-making and compliance monitoring.</t>
+  </si>
+  <si>
+    <t>As a financial institution, I want to implement entity extraction models to automatically identify and extract key financial entities (e.g., company names, stock symbols, monetary amounts) from news articles and financial reports, enhancing our market analysis and investment strategies.</t>
+  </si>
+  <si>
+    <t>As a financial institution, I want to employ feature selection techniques to identify the most relevant financial indicators (such as volatility, liquidity ratios) from a large dataset for predicting stock prices, improving the accuracy of our investment models.</t>
+  </si>
+  <si>
+    <t>As a financial institution, I want to address imbalanced datasets in fraud detection by employing ensemble learning techniques like AdaBoost to enhance the detection of fraudulent transactions while minimizing false alarms.</t>
+  </si>
+  <si>
+    <t>As a financial institution, I want to implement keyword extraction algorithms to analyze customer reviews and identify recurring themes and concerns related to our financial products, enabling us to prioritize areas for improvement.</t>
+  </si>
+  <si>
+    <t>As a financial analyst, I want to implement KNN algorithms to classify stocks based on historical trading patterns and market indicators, helping investors identify similar stocks for portfolio diversification strategies.</t>
+  </si>
+  <si>
+    <t>As a financial institution, I want to develop multi-label classification models to categorize financial products based on risk levels, return potential, and investment duration, providing comprehensive recommendations to clients.</t>
+  </si>
+  <si>
+    <t>As a financial analyst, I want to build a neural network model to predict stock prices based on historical market data and economic indicators, providing accurate forecasts to guide investment decisions.</t>
+  </si>
+  <si>
+    <t>As a financial institution, I want to develop a random forest-based recommendation system for personalized financial products, suggesting suitable investment options based on customer profiles and financial goals.</t>
+  </si>
+  <si>
+    <t>As a financial institution, I want to apply semantic similarity algorithms to compare legal documents such as contracts and agreements, ensuring consistency and accuracy in regulatory compliance across different jurisdictions.</t>
+  </si>
+  <si>
+    <t>As a marketer, I want to use sentiment analysis to monitor customer sentiment towards our brand and products on social media platforms, identifying opportunities to enhance customer experience and address negative feedback promptly.</t>
+  </si>
+  <si>
+    <t>As a financial institution, I want to deploy speech to text systems for automated transcription of customer service calls and inquiries, improving efficiency in resolving customer issues and enhancing service quality.</t>
+  </si>
+  <si>
+    <t>As a financial analyst, I want to develop text categorization models to classify research papers and articles into relevant financial topics such as macroeconomics, stock analysis, and industry trends, supporting comprehensive market analysis.</t>
+  </si>
+  <si>
+    <t>As a marketer, I want to use unsupervised clustering techniques to group social media followers based on engagement behaviors and interests, optimizing social media marketing campaigns to increase brand awareness and customer engagement.</t>
+  </si>
+  <si>
+    <t>As a financial analyst, I want to develop voice recognition systems to transcribe and analyze financial podcasts and interviews with industry experts, extracting key insights and market predictions for investors.</t>
+  </si>
+  <si>
+    <t>As a marketer, I want to apply word embedding techniques to analyze customer reviews and social media comments about our products, identifying key product features and sentiments that influence consumer preferences and purchasing decisions.</t>
   </si>
 </sst>
 </file>
@@ -606,7 +672,7 @@
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -631,6 +697,12 @@
         <bgColor rgb="FFCFE2F3"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FFFFFF00"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -644,7 +716,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -663,6 +735,7 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -997,10 +1070,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8DF0B04-8323-4309-B759-D1CDDA1FBB0E}">
-  <dimension ref="A1:F141"/>
+  <dimension ref="A1:F161"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A130" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:F21"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1033,400 +1106,400 @@
       </c>
     </row>
     <row r="2" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
-        <v>134</v>
-      </c>
-      <c r="B2" s="8">
-        <v>3</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>135</v>
-      </c>
-      <c r="D2" s="5" t="s">
+      <c r="A2" s="10" t="s">
+        <v>177</v>
+      </c>
+      <c r="B2" s="10">
+        <v>2</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>178</v>
+      </c>
+      <c r="D2" s="9" t="s">
         <v>28</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>136</v>
+        <v>179</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="3" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
-        <v>134</v>
-      </c>
-      <c r="B3" s="8">
-        <v>3</v>
-      </c>
-      <c r="C3" s="8" t="s">
-        <v>156</v>
+      <c r="A3" s="10" t="s">
+        <v>177</v>
+      </c>
+      <c r="B3" s="10">
+        <v>2</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>178</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>157</v>
+        <v>180</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="4" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="8" t="s">
-        <v>134</v>
-      </c>
-      <c r="B4" s="8">
-        <v>3</v>
-      </c>
-      <c r="C4" s="8" t="s">
-        <v>135</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>43</v>
+      <c r="A4" s="10" t="s">
+        <v>177</v>
+      </c>
+      <c r="B4" s="10">
+        <v>2</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>178</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>30</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>137</v>
+        <v>181</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="5" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="8" t="s">
-        <v>134</v>
-      </c>
-      <c r="B5" s="8">
-        <v>3</v>
-      </c>
-      <c r="C5" s="8" t="s">
-        <v>156</v>
+      <c r="A5" s="10" t="s">
+        <v>177</v>
+      </c>
+      <c r="B5" s="10">
+        <v>2</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>178</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>43</v>
+        <v>13</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>158</v>
+        <v>182</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="6" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="8" t="s">
-        <v>134</v>
-      </c>
-      <c r="B6" s="8">
-        <v>3</v>
-      </c>
-      <c r="C6" s="8" t="s">
-        <v>135</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>30</v>
+      <c r="A6" s="10" t="s">
+        <v>177</v>
+      </c>
+      <c r="B6" s="10">
+        <v>2</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>178</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>46</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>138</v>
+        <v>183</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="7" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="8" t="s">
-        <v>134</v>
-      </c>
-      <c r="B7" s="8">
-        <v>3</v>
-      </c>
-      <c r="C7" s="8" t="s">
-        <v>156</v>
+      <c r="A7" s="10" t="s">
+        <v>177</v>
+      </c>
+      <c r="B7" s="10">
+        <v>2</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>178</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>159</v>
+        <v>184</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="8" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="8" t="s">
-        <v>134</v>
-      </c>
-      <c r="B8" s="8">
-        <v>3</v>
-      </c>
-      <c r="C8" s="8" t="s">
-        <v>135</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>13</v>
+      <c r="A8" s="10" t="s">
+        <v>177</v>
+      </c>
+      <c r="B8" s="10">
+        <v>2</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>178</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>36</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>139</v>
+        <v>185</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="9" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="8" t="s">
-        <v>134</v>
-      </c>
-      <c r="B9" s="8">
-        <v>3</v>
-      </c>
-      <c r="C9" s="8" t="s">
-        <v>156</v>
+      <c r="A9" s="10" t="s">
+        <v>177</v>
+      </c>
+      <c r="B9" s="10">
+        <v>2</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>178</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>160</v>
+        <v>186</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="10" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="8" t="s">
-        <v>134</v>
-      </c>
-      <c r="B10" s="8">
-        <v>3</v>
-      </c>
-      <c r="C10" s="8" t="s">
-        <v>135</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>46</v>
+      <c r="A10" s="10" t="s">
+        <v>177</v>
+      </c>
+      <c r="B10" s="10">
+        <v>2</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>178</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>34</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>140</v>
+        <v>187</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="11" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="8" t="s">
-        <v>134</v>
-      </c>
-      <c r="B11" s="8">
-        <v>3</v>
-      </c>
-      <c r="C11" s="8" t="s">
-        <v>156</v>
+      <c r="A11" s="10" t="s">
+        <v>177</v>
+      </c>
+      <c r="B11" s="10">
+        <v>2</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>178</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>46</v>
+        <v>16</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>161</v>
+        <v>188</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="12" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="8" t="s">
-        <v>134</v>
-      </c>
-      <c r="B12" s="8">
-        <v>3</v>
-      </c>
-      <c r="C12" s="8" t="s">
-        <v>135</v>
-      </c>
-      <c r="D12" s="5" t="s">
-        <v>33</v>
+      <c r="A12" s="10" t="s">
+        <v>177</v>
+      </c>
+      <c r="B12" s="10">
+        <v>2</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>178</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>40</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>141</v>
+        <v>189</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="13" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="8" t="s">
-        <v>134</v>
-      </c>
-      <c r="B13" s="8">
-        <v>3</v>
-      </c>
-      <c r="C13" s="8" t="s">
-        <v>156</v>
+      <c r="A13" s="10" t="s">
+        <v>177</v>
+      </c>
+      <c r="B13" s="10">
+        <v>2</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>178</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>33</v>
+        <v>18</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>162</v>
+        <v>190</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="14" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="8" t="s">
-        <v>134</v>
-      </c>
-      <c r="B14" s="8">
-        <v>3</v>
-      </c>
-      <c r="C14" s="8" t="s">
-        <v>135</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>36</v>
+      <c r="A14" s="10" t="s">
+        <v>177</v>
+      </c>
+      <c r="B14" s="10">
+        <v>2</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>178</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>20</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>142</v>
+        <v>191</v>
       </c>
       <c r="F14" s="1" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="15" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="8" t="s">
-        <v>134</v>
-      </c>
-      <c r="B15" s="8">
-        <v>3</v>
-      </c>
-      <c r="C15" s="8" t="s">
-        <v>156</v>
+      <c r="A15" s="10" t="s">
+        <v>177</v>
+      </c>
+      <c r="B15" s="10">
+        <v>2</v>
+      </c>
+      <c r="C15" s="10" t="s">
+        <v>178</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>36</v>
+        <v>22</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>163</v>
+        <v>192</v>
       </c>
       <c r="F15" s="1" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="16" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="8" t="s">
-        <v>134</v>
-      </c>
-      <c r="B16" s="8">
-        <v>3</v>
-      </c>
-      <c r="C16" s="8" t="s">
-        <v>135</v>
-      </c>
-      <c r="D16" s="5" t="s">
-        <v>14</v>
+      <c r="A16" s="10" t="s">
+        <v>177</v>
+      </c>
+      <c r="B16" s="10">
+        <v>2</v>
+      </c>
+      <c r="C16" s="10" t="s">
+        <v>178</v>
+      </c>
+      <c r="D16" s="9" t="s">
+        <v>38</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>143</v>
+        <v>193</v>
       </c>
       <c r="F16" s="1" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="17" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="8" t="s">
-        <v>134</v>
-      </c>
-      <c r="B17" s="8">
-        <v>3</v>
-      </c>
-      <c r="C17" s="8" t="s">
-        <v>156</v>
+      <c r="A17" s="10" t="s">
+        <v>177</v>
+      </c>
+      <c r="B17" s="10">
+        <v>2</v>
+      </c>
+      <c r="C17" s="10" t="s">
+        <v>178</v>
       </c>
       <c r="D17" s="9" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>164</v>
+        <v>194</v>
       </c>
       <c r="F17" s="1" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="18" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="8" t="s">
-        <v>134</v>
-      </c>
-      <c r="B18" s="8">
-        <v>3</v>
-      </c>
-      <c r="C18" s="8" t="s">
-        <v>135</v>
-      </c>
-      <c r="D18" s="5" t="s">
-        <v>34</v>
+      <c r="A18" s="10" t="s">
+        <v>177</v>
+      </c>
+      <c r="B18" s="10">
+        <v>2</v>
+      </c>
+      <c r="C18" s="10" t="s">
+        <v>178</v>
+      </c>
+      <c r="D18" s="9" t="s">
+        <v>26</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>144</v>
+        <v>195</v>
       </c>
       <c r="F18" s="1" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="19" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="8" t="s">
-        <v>134</v>
-      </c>
-      <c r="B19" s="8">
-        <v>3</v>
-      </c>
-      <c r="C19" s="8" t="s">
-        <v>156</v>
+      <c r="A19" s="10" t="s">
+        <v>177</v>
+      </c>
+      <c r="B19" s="10">
+        <v>2</v>
+      </c>
+      <c r="C19" s="10" t="s">
+        <v>178</v>
       </c>
       <c r="D19" s="9" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>165</v>
+        <v>196</v>
       </c>
       <c r="F19" s="1" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="20" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="8" t="s">
-        <v>134</v>
-      </c>
-      <c r="B20" s="8">
-        <v>3</v>
-      </c>
-      <c r="C20" s="8" t="s">
-        <v>135</v>
-      </c>
-      <c r="D20" s="5" t="s">
-        <v>16</v>
+      <c r="A20" s="10" t="s">
+        <v>177</v>
+      </c>
+      <c r="B20" s="10">
+        <v>2</v>
+      </c>
+      <c r="C20" s="10" t="s">
+        <v>178</v>
+      </c>
+      <c r="D20" s="9" t="s">
+        <v>7</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>145</v>
+        <v>197</v>
       </c>
       <c r="F20" s="1" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="21" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="8" t="s">
-        <v>134</v>
-      </c>
-      <c r="B21" s="8">
-        <v>3</v>
-      </c>
-      <c r="C21" s="8" t="s">
-        <v>156</v>
+      <c r="A21" s="10" t="s">
+        <v>177</v>
+      </c>
+      <c r="B21" s="10">
+        <v>2</v>
+      </c>
+      <c r="C21" s="10" t="s">
+        <v>178</v>
       </c>
       <c r="D21" s="9" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>166</v>
+        <v>198</v>
       </c>
       <c r="F21" s="1" t="s">
         <v>69</v>
@@ -1443,10 +1516,10 @@
         <v>135</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>146</v>
+        <v>136</v>
       </c>
       <c r="F22" s="1" t="s">
         <v>69</v>
@@ -1463,10 +1536,10 @@
         <v>156</v>
       </c>
       <c r="D23" s="9" t="s">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>167</v>
+        <v>157</v>
       </c>
       <c r="F23" s="1" t="s">
         <v>69</v>
@@ -1483,10 +1556,10 @@
         <v>135</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>18</v>
+        <v>43</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>147</v>
+        <v>137</v>
       </c>
       <c r="F24" s="1" t="s">
         <v>69</v>
@@ -1503,10 +1576,10 @@
         <v>156</v>
       </c>
       <c r="D25" s="9" t="s">
-        <v>18</v>
+        <v>43</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>168</v>
+        <v>158</v>
       </c>
       <c r="F25" s="1" t="s">
         <v>69</v>
@@ -1523,10 +1596,10 @@
         <v>135</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>148</v>
+        <v>138</v>
       </c>
       <c r="F26" s="1" t="s">
         <v>69</v>
@@ -1543,10 +1616,10 @@
         <v>156</v>
       </c>
       <c r="D27" s="9" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>169</v>
+        <v>159</v>
       </c>
       <c r="F27" s="1" t="s">
         <v>69</v>
@@ -1563,10 +1636,10 @@
         <v>135</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>149</v>
+        <v>139</v>
       </c>
       <c r="F28" s="1" t="s">
         <v>69</v>
@@ -1583,10 +1656,10 @@
         <v>156</v>
       </c>
       <c r="D29" s="9" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>170</v>
+        <v>160</v>
       </c>
       <c r="F29" s="1" t="s">
         <v>69</v>
@@ -1603,10 +1676,10 @@
         <v>135</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>150</v>
+        <v>140</v>
       </c>
       <c r="F30" s="1" t="s">
         <v>69</v>
@@ -1623,10 +1696,10 @@
         <v>156</v>
       </c>
       <c r="D31" s="9" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>171</v>
+        <v>161</v>
       </c>
       <c r="F31" s="1" t="s">
         <v>69</v>
@@ -1643,10 +1716,10 @@
         <v>135</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>151</v>
+        <v>141</v>
       </c>
       <c r="F32" s="1" t="s">
         <v>69</v>
@@ -1663,10 +1736,10 @@
         <v>156</v>
       </c>
       <c r="D33" s="9" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>172</v>
+        <v>162</v>
       </c>
       <c r="F33" s="1" t="s">
         <v>69</v>
@@ -1683,10 +1756,10 @@
         <v>135</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>26</v>
+        <v>36</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>152</v>
+        <v>142</v>
       </c>
       <c r="F34" s="1" t="s">
         <v>69</v>
@@ -1703,10 +1776,10 @@
         <v>156</v>
       </c>
       <c r="D35" s="9" t="s">
-        <v>26</v>
+        <v>36</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>173</v>
+        <v>163</v>
       </c>
       <c r="F35" s="1" t="s">
         <v>69</v>
@@ -1723,10 +1796,10 @@
         <v>135</v>
       </c>
       <c r="D36" s="5" t="s">
-        <v>31</v>
+        <v>14</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>153</v>
+        <v>143</v>
       </c>
       <c r="F36" s="1" t="s">
         <v>69</v>
@@ -1743,10 +1816,10 @@
         <v>156</v>
       </c>
       <c r="D37" s="9" t="s">
-        <v>31</v>
+        <v>14</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>174</v>
+        <v>164</v>
       </c>
       <c r="F37" s="1" t="s">
         <v>69</v>
@@ -1763,10 +1836,10 @@
         <v>135</v>
       </c>
       <c r="D38" s="5" t="s">
-        <v>7</v>
+        <v>34</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>154</v>
+        <v>144</v>
       </c>
       <c r="F38" s="1" t="s">
         <v>69</v>
@@ -1783,10 +1856,10 @@
         <v>156</v>
       </c>
       <c r="D39" s="9" t="s">
-        <v>7</v>
+        <v>34</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>175</v>
+        <v>165</v>
       </c>
       <c r="F39" s="1" t="s">
         <v>69</v>
@@ -1803,10 +1876,10 @@
         <v>135</v>
       </c>
       <c r="D40" s="5" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>155</v>
+        <v>145</v>
       </c>
       <c r="F40" s="1" t="s">
         <v>69</v>
@@ -1823,410 +1896,410 @@
         <v>156</v>
       </c>
       <c r="D41" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="B42" s="8">
+        <v>3</v>
+      </c>
+      <c r="C42" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="D42" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="B43" s="8">
+        <v>3</v>
+      </c>
+      <c r="C43" s="8" t="s">
+        <v>156</v>
+      </c>
+      <c r="D43" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="F43" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="B44" s="8">
+        <v>3</v>
+      </c>
+      <c r="C44" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="D44" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="F44" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="B45" s="8">
+        <v>3</v>
+      </c>
+      <c r="C45" s="8" t="s">
+        <v>156</v>
+      </c>
+      <c r="D45" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="F45" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="B46" s="8">
+        <v>3</v>
+      </c>
+      <c r="C46" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="D46" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="F46" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="B47" s="8">
+        <v>3</v>
+      </c>
+      <c r="C47" s="8" t="s">
+        <v>156</v>
+      </c>
+      <c r="D47" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="F47" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="B48" s="8">
+        <v>3</v>
+      </c>
+      <c r="C48" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="D48" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="F48" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="B49" s="8">
+        <v>3</v>
+      </c>
+      <c r="C49" s="8" t="s">
+        <v>156</v>
+      </c>
+      <c r="D49" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="F49" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="B50" s="8">
+        <v>3</v>
+      </c>
+      <c r="C50" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="D50" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="F50" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="B51" s="8">
+        <v>3</v>
+      </c>
+      <c r="C51" s="8" t="s">
+        <v>156</v>
+      </c>
+      <c r="D51" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="E51" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="F51" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="B52" s="8">
+        <v>3</v>
+      </c>
+      <c r="C52" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="D52" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E52" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="F52" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="B53" s="8">
+        <v>3</v>
+      </c>
+      <c r="C53" s="8" t="s">
+        <v>156</v>
+      </c>
+      <c r="D53" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="E53" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="F53" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="B54" s="8">
+        <v>3</v>
+      </c>
+      <c r="C54" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="D54" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E54" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="F54" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="B55" s="8">
+        <v>3</v>
+      </c>
+      <c r="C55" s="8" t="s">
+        <v>156</v>
+      </c>
+      <c r="D55" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="E55" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="F55" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="B56" s="8">
+        <v>3</v>
+      </c>
+      <c r="C56" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="D56" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="E56" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="F56" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="B57" s="8">
+        <v>3</v>
+      </c>
+      <c r="C57" s="8" t="s">
+        <v>156</v>
+      </c>
+      <c r="D57" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="E57" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="F57" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="B58" s="8">
+        <v>3</v>
+      </c>
+      <c r="C58" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="D58" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E58" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="F58" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="B59" s="8">
+        <v>3</v>
+      </c>
+      <c r="C59" s="8" t="s">
+        <v>156</v>
+      </c>
+      <c r="D59" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="E59" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="F59" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="B60" s="8">
+        <v>3</v>
+      </c>
+      <c r="C60" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="D60" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="E41" s="1" t="s">
+      <c r="E60" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="F60" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="B61" s="8">
+        <v>3</v>
+      </c>
+      <c r="C61" s="8" t="s">
+        <v>156</v>
+      </c>
+      <c r="D61" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E61" s="1" t="s">
         <v>176</v>
-      </c>
-      <c r="F41" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="B42" s="7">
-        <v>4</v>
-      </c>
-      <c r="C42" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="D42" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="E42" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="F42" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="B43" s="7">
-        <v>4</v>
-      </c>
-      <c r="C43" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="D43" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="E43" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="F43" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="B44" s="7">
-        <v>4</v>
-      </c>
-      <c r="C44" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="D44" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="E44" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="F44" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="B45" s="7">
-        <v>4</v>
-      </c>
-      <c r="C45" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="D45" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="E45" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="F45" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="B46" s="7">
-        <v>4</v>
-      </c>
-      <c r="C46" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="D46" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="E46" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="F46" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="B47" s="7">
-        <v>4</v>
-      </c>
-      <c r="C47" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="D47" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="E47" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="F47" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="B48" s="7">
-        <v>4</v>
-      </c>
-      <c r="C48" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="D48" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E48" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="F48" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="B49" s="7">
-        <v>4</v>
-      </c>
-      <c r="C49" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="D49" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E49" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="F49" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="B50" s="7">
-        <v>4</v>
-      </c>
-      <c r="C50" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="D50" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="E50" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="F50" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="B51" s="7">
-        <v>4</v>
-      </c>
-      <c r="C51" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="D51" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="E51" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="F51" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="B52" s="7">
-        <v>4</v>
-      </c>
-      <c r="C52" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="D52" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="E52" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="F52" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="B53" s="7">
-        <v>4</v>
-      </c>
-      <c r="C53" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="D53" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="E53" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="F53" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="B54" s="7">
-        <v>4</v>
-      </c>
-      <c r="C54" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="D54" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="E54" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="F54" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="B55" s="7">
-        <v>4</v>
-      </c>
-      <c r="C55" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="D55" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="E55" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="F55" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="B56" s="7">
-        <v>4</v>
-      </c>
-      <c r="C56" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="D56" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="E56" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="F56" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="B57" s="7">
-        <v>4</v>
-      </c>
-      <c r="C57" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="D57" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="E57" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="F57" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="B58" s="7">
-        <v>4</v>
-      </c>
-      <c r="C58" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="D58" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="E58" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="F58" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="B59" s="7">
-        <v>4</v>
-      </c>
-      <c r="C59" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="D59" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="E59" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="F59" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="B60" s="7">
-        <v>4</v>
-      </c>
-      <c r="C60" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="D60" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="E60" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="F60" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="B61" s="7">
-        <v>4</v>
-      </c>
-      <c r="C61" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="D61" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="E61" s="1" t="s">
-        <v>102</v>
       </c>
       <c r="F61" s="1" t="s">
         <v>69</v>
@@ -2243,10 +2316,10 @@
         <v>113</v>
       </c>
       <c r="D62" s="4" t="s">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>124</v>
+        <v>114</v>
       </c>
       <c r="F62" s="1" t="s">
         <v>69</v>
@@ -2263,10 +2336,10 @@
         <v>92</v>
       </c>
       <c r="D63" s="4" t="s">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>103</v>
+        <v>93</v>
       </c>
       <c r="F63" s="1" t="s">
         <v>69</v>
@@ -2283,10 +2356,10 @@
         <v>113</v>
       </c>
       <c r="D64" s="4" t="s">
-        <v>18</v>
+        <v>43</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>125</v>
+        <v>115</v>
       </c>
       <c r="F64" s="1" t="s">
         <v>69</v>
@@ -2303,10 +2376,10 @@
         <v>92</v>
       </c>
       <c r="D65" s="4" t="s">
-        <v>18</v>
+        <v>43</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>104</v>
+        <v>94</v>
       </c>
       <c r="F65" s="1" t="s">
         <v>69</v>
@@ -2323,10 +2396,10 @@
         <v>113</v>
       </c>
       <c r="D66" s="4" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
       <c r="F66" s="1" t="s">
         <v>69</v>
@@ -2343,10 +2416,10 @@
         <v>92</v>
       </c>
       <c r="D67" s="4" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>105</v>
+        <v>95</v>
       </c>
       <c r="F67" s="1" t="s">
         <v>69</v>
@@ -2363,10 +2436,10 @@
         <v>113</v>
       </c>
       <c r="D68" s="4" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>127</v>
+        <v>117</v>
       </c>
       <c r="F68" s="1" t="s">
         <v>69</v>
@@ -2383,10 +2456,10 @@
         <v>92</v>
       </c>
       <c r="D69" s="4" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="F69" s="1" t="s">
         <v>69</v>
@@ -2403,10 +2476,10 @@
         <v>113</v>
       </c>
       <c r="D70" s="4" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>128</v>
+        <v>118</v>
       </c>
       <c r="F70" s="1" t="s">
         <v>69</v>
@@ -2423,10 +2496,10 @@
         <v>92</v>
       </c>
       <c r="D71" s="4" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>107</v>
+        <v>97</v>
       </c>
       <c r="F71" s="1" t="s">
         <v>69</v>
@@ -2443,10 +2516,10 @@
         <v>113</v>
       </c>
       <c r="D72" s="4" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="E72" s="1" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
       <c r="F72" s="1" t="s">
         <v>69</v>
@@ -2463,10 +2536,10 @@
         <v>92</v>
       </c>
       <c r="D73" s="4" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="F73" s="1" t="s">
         <v>69</v>
@@ -2483,10 +2556,10 @@
         <v>113</v>
       </c>
       <c r="D74" s="4" t="s">
-        <v>26</v>
+        <v>36</v>
       </c>
       <c r="E74" s="1" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="F74" s="1" t="s">
         <v>69</v>
@@ -2503,10 +2576,10 @@
         <v>92</v>
       </c>
       <c r="D75" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="E75" s="6" t="s">
-        <v>109</v>
+        <v>36</v>
+      </c>
+      <c r="E75" s="1" t="s">
+        <v>99</v>
       </c>
       <c r="F75" s="1" t="s">
         <v>69</v>
@@ -2523,10 +2596,10 @@
         <v>113</v>
       </c>
       <c r="D76" s="4" t="s">
-        <v>31</v>
+        <v>14</v>
       </c>
       <c r="E76" s="1" t="s">
-        <v>131</v>
+        <v>121</v>
       </c>
       <c r="F76" s="1" t="s">
         <v>69</v>
@@ -2543,10 +2616,10 @@
         <v>92</v>
       </c>
       <c r="D77" s="4" t="s">
-        <v>31</v>
+        <v>14</v>
       </c>
       <c r="E77" s="1" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="F77" s="1" t="s">
         <v>69</v>
@@ -2563,10 +2636,10 @@
         <v>113</v>
       </c>
       <c r="D78" s="4" t="s">
-        <v>7</v>
+        <v>34</v>
       </c>
       <c r="E78" s="1" t="s">
-        <v>132</v>
+        <v>122</v>
       </c>
       <c r="F78" s="1" t="s">
         <v>69</v>
@@ -2583,10 +2656,10 @@
         <v>92</v>
       </c>
       <c r="D79" s="4" t="s">
-        <v>7</v>
+        <v>34</v>
       </c>
       <c r="E79" s="1" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
       <c r="F79" s="1" t="s">
         <v>69</v>
@@ -2603,10 +2676,10 @@
         <v>113</v>
       </c>
       <c r="D80" s="4" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="E80" s="1" t="s">
-        <v>133</v>
+        <v>123</v>
       </c>
       <c r="F80" s="1" t="s">
         <v>69</v>
@@ -2623,410 +2696,410 @@
         <v>92</v>
       </c>
       <c r="D81" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E81" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="F81" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A82" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="B82" s="7">
+        <v>4</v>
+      </c>
+      <c r="C82" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="D82" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="E82" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="F82" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A83" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="B83" s="7">
+        <v>4</v>
+      </c>
+      <c r="C83" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="D83" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="E83" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="F83" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A84" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="B84" s="7">
+        <v>4</v>
+      </c>
+      <c r="C84" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="D84" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E84" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="F84" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A85" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="B85" s="7">
+        <v>4</v>
+      </c>
+      <c r="C85" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="D85" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E85" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="F85" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A86" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="B86" s="7">
+        <v>4</v>
+      </c>
+      <c r="C86" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="D86" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E86" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="F86" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A87" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="B87" s="7">
+        <v>4</v>
+      </c>
+      <c r="C87" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="D87" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E87" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="F87" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A88" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="B88" s="7">
+        <v>4</v>
+      </c>
+      <c r="C88" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="D88" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E88" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="F88" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A89" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="B89" s="7">
+        <v>4</v>
+      </c>
+      <c r="C89" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="D89" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E89" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="F89" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A90" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="B90" s="7">
+        <v>4</v>
+      </c>
+      <c r="C90" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="D90" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="E90" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="F90" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A91" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="B91" s="7">
+        <v>4</v>
+      </c>
+      <c r="C91" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="D91" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="E91" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="F91" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A92" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="B92" s="7">
+        <v>4</v>
+      </c>
+      <c r="C92" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="D92" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E92" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="F92" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A93" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="B93" s="7">
+        <v>4</v>
+      </c>
+      <c r="C93" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="D93" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E93" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="F93" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A94" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="B94" s="7">
+        <v>4</v>
+      </c>
+      <c r="C94" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="D94" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="E94" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="F94" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A95" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="B95" s="7">
+        <v>4</v>
+      </c>
+      <c r="C95" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="D95" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="E95" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="F95" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A96" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="B96" s="7">
+        <v>4</v>
+      </c>
+      <c r="C96" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="D96" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="E96" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="F96" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A97" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="B97" s="7">
+        <v>4</v>
+      </c>
+      <c r="C97" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="D97" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="E97" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="F97" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A98" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="B98" s="7">
+        <v>4</v>
+      </c>
+      <c r="C98" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="D98" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E98" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="F98" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A99" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="B99" s="7">
+        <v>4</v>
+      </c>
+      <c r="C99" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="D99" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E99" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="F99" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A100" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="B100" s="7">
+        <v>4</v>
+      </c>
+      <c r="C100" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="D100" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="E81" s="1" t="s">
+      <c r="E100" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="F100" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A101" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="B101" s="7">
+        <v>4</v>
+      </c>
+      <c r="C101" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="D101" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E101" s="1" t="s">
         <v>112</v>
-      </c>
-      <c r="F81" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A82" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B82" s="2">
-        <v>5</v>
-      </c>
-      <c r="C82" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D82" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E82" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="F82" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A83" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B83" s="2">
-        <v>5</v>
-      </c>
-      <c r="C83" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="D83" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E83" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="F83" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A84" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B84" s="2">
-        <v>5</v>
-      </c>
-      <c r="C84" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="D84" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E84" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="F84" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A85" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B85" s="2">
-        <v>5</v>
-      </c>
-      <c r="C85" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D85" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="E85" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="F85" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A86" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B86" s="2">
-        <v>5</v>
-      </c>
-      <c r="C86" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="D86" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="E86" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="F86" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A87" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B87" s="2">
-        <v>5</v>
-      </c>
-      <c r="C87" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="D87" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="E87" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="F87" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A88" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B88" s="2">
-        <v>5</v>
-      </c>
-      <c r="C88" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D88" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="E88" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="F88" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A89" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B89" s="2">
-        <v>5</v>
-      </c>
-      <c r="C89" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="D89" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="E89" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="F89" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A90" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B90" s="2">
-        <v>5</v>
-      </c>
-      <c r="C90" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="D90" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="E90" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="F90" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A91" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B91" s="2">
-        <v>5</v>
-      </c>
-      <c r="C91" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D91" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="E91" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F91" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A92" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B92" s="2">
-        <v>5</v>
-      </c>
-      <c r="C92" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="D92" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="E92" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="F92" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A93" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B93" s="2">
-        <v>5</v>
-      </c>
-      <c r="C93" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="D93" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="E93" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="F93" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A94" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B94" s="2">
-        <v>5</v>
-      </c>
-      <c r="C94" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D94" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="E94" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="F94" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A95" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B95" s="2">
-        <v>5</v>
-      </c>
-      <c r="C95" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="D95" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="E95" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="F95" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A96" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B96" s="2">
-        <v>5</v>
-      </c>
-      <c r="C96" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="D96" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="E96" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="F96" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A97" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B97" s="2">
-        <v>5</v>
-      </c>
-      <c r="C97" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D97" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="E97" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="F97" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A98" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B98" s="2">
-        <v>5</v>
-      </c>
-      <c r="C98" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="D98" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="E98" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="F98" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A99" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B99" s="2">
-        <v>5</v>
-      </c>
-      <c r="C99" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="D99" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="E99" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="F99" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A100" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B100" s="2">
-        <v>5</v>
-      </c>
-      <c r="C100" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D100" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="E100" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="F100" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A101" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B101" s="2">
-        <v>5</v>
-      </c>
-      <c r="C101" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="D101" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="E101" s="1" t="s">
-        <v>54</v>
       </c>
       <c r="F101" s="1" t="s">
         <v>69</v>
@@ -3040,13 +3113,13 @@
         <v>5</v>
       </c>
       <c r="C102" s="2" t="s">
-        <v>70</v>
+        <v>5</v>
       </c>
       <c r="D102" s="5" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="E102" s="1" t="s">
-        <v>77</v>
+        <v>27</v>
       </c>
       <c r="F102" s="1" t="s">
         <v>69</v>
@@ -3060,13 +3133,13 @@
         <v>5</v>
       </c>
       <c r="C103" s="2" t="s">
-        <v>5</v>
+        <v>47</v>
       </c>
       <c r="D103" s="5" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="E103" s="1" t="s">
-        <v>12</v>
+        <v>49</v>
       </c>
       <c r="F103" s="1" t="s">
         <v>69</v>
@@ -3080,13 +3153,13 @@
         <v>5</v>
       </c>
       <c r="C104" s="2" t="s">
-        <v>47</v>
+        <v>70</v>
       </c>
       <c r="D104" s="5" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="E104" s="1" t="s">
-        <v>55</v>
+        <v>71</v>
       </c>
       <c r="F104" s="1" t="s">
         <v>69</v>
@@ -3100,13 +3173,13 @@
         <v>5</v>
       </c>
       <c r="C105" s="2" t="s">
-        <v>70</v>
+        <v>5</v>
       </c>
       <c r="D105" s="5" t="s">
-        <v>14</v>
+        <v>43</v>
       </c>
       <c r="E105" s="1" t="s">
-        <v>78</v>
+        <v>42</v>
       </c>
       <c r="F105" s="1" t="s">
         <v>69</v>
@@ -3120,13 +3193,13 @@
         <v>5</v>
       </c>
       <c r="C106" s="2" t="s">
-        <v>5</v>
+        <v>47</v>
       </c>
       <c r="D106" s="5" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="E106" s="1" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="F106" s="1" t="s">
         <v>69</v>
@@ -3140,13 +3213,13 @@
         <v>5</v>
       </c>
       <c r="C107" s="2" t="s">
-        <v>47</v>
+        <v>70</v>
       </c>
       <c r="D107" s="5" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="E107" s="1" t="s">
-        <v>56</v>
+        <v>72</v>
       </c>
       <c r="F107" s="1" t="s">
         <v>69</v>
@@ -3160,13 +3233,13 @@
         <v>5</v>
       </c>
       <c r="C108" s="2" t="s">
-        <v>70</v>
+        <v>5</v>
       </c>
       <c r="D108" s="5" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="E108" s="1" t="s">
-        <v>79</v>
+        <v>29</v>
       </c>
       <c r="F108" s="1" t="s">
         <v>69</v>
@@ -3180,13 +3253,13 @@
         <v>5</v>
       </c>
       <c r="C109" s="2" t="s">
-        <v>5</v>
+        <v>47</v>
       </c>
       <c r="D109" s="5" t="s">
-        <v>16</v>
+        <v>30</v>
       </c>
       <c r="E109" s="1" t="s">
-        <v>15</v>
+        <v>50</v>
       </c>
       <c r="F109" s="1" t="s">
         <v>69</v>
@@ -3200,13 +3273,13 @@
         <v>5</v>
       </c>
       <c r="C110" s="2" t="s">
-        <v>47</v>
+        <v>70</v>
       </c>
       <c r="D110" s="5" t="s">
-        <v>16</v>
+        <v>30</v>
       </c>
       <c r="E110" s="1" t="s">
-        <v>57</v>
+        <v>73</v>
       </c>
       <c r="F110" s="1" t="s">
         <v>69</v>
@@ -3220,13 +3293,13 @@
         <v>5</v>
       </c>
       <c r="C111" s="2" t="s">
-        <v>70</v>
+        <v>5</v>
       </c>
       <c r="D111" s="5" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="E111" s="1" t="s">
-        <v>80</v>
+        <v>11</v>
       </c>
       <c r="F111" s="1" t="s">
         <v>69</v>
@@ -3240,13 +3313,13 @@
         <v>5</v>
       </c>
       <c r="C112" s="2" t="s">
-        <v>5</v>
+        <v>47</v>
       </c>
       <c r="D112" s="5" t="s">
-        <v>40</v>
+        <v>13</v>
       </c>
       <c r="E112" s="1" t="s">
-        <v>39</v>
+        <v>51</v>
       </c>
       <c r="F112" s="1" t="s">
         <v>69</v>
@@ -3260,13 +3333,13 @@
         <v>5</v>
       </c>
       <c r="C113" s="2" t="s">
-        <v>47</v>
+        <v>70</v>
       </c>
       <c r="D113" s="5" t="s">
-        <v>40</v>
+        <v>13</v>
       </c>
       <c r="E113" s="1" t="s">
-        <v>58</v>
+        <v>74</v>
       </c>
       <c r="F113" s="1" t="s">
         <v>69</v>
@@ -3280,13 +3353,13 @@
         <v>5</v>
       </c>
       <c r="C114" s="2" t="s">
-        <v>70</v>
+        <v>5</v>
       </c>
       <c r="D114" s="5" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="E114" s="1" t="s">
-        <v>82</v>
+        <v>45</v>
       </c>
       <c r="F114" s="1" t="s">
         <v>69</v>
@@ -3300,13 +3373,13 @@
         <v>5</v>
       </c>
       <c r="C115" s="2" t="s">
-        <v>5</v>
+        <v>47</v>
       </c>
       <c r="D115" s="5" t="s">
-        <v>18</v>
+        <v>46</v>
       </c>
       <c r="E115" s="1" t="s">
-        <v>17</v>
+        <v>53</v>
       </c>
       <c r="F115" s="1" t="s">
         <v>69</v>
@@ -3320,13 +3393,13 @@
         <v>5</v>
       </c>
       <c r="C116" s="2" t="s">
-        <v>47</v>
+        <v>70</v>
       </c>
       <c r="D116" s="5" t="s">
-        <v>18</v>
+        <v>46</v>
       </c>
       <c r="E116" s="1" t="s">
-        <v>59</v>
+        <v>75</v>
       </c>
       <c r="F116" s="1" t="s">
         <v>69</v>
@@ -3340,13 +3413,13 @@
         <v>5</v>
       </c>
       <c r="C117" s="2" t="s">
-        <v>70</v>
+        <v>5</v>
       </c>
       <c r="D117" s="5" t="s">
-        <v>18</v>
+        <v>33</v>
       </c>
       <c r="E117" s="1" t="s">
-        <v>81</v>
+        <v>32</v>
       </c>
       <c r="F117" s="1" t="s">
         <v>69</v>
@@ -3360,13 +3433,13 @@
         <v>5</v>
       </c>
       <c r="C118" s="2" t="s">
-        <v>5</v>
+        <v>47</v>
       </c>
       <c r="D118" s="5" t="s">
-        <v>20</v>
+        <v>33</v>
       </c>
       <c r="E118" s="1" t="s">
-        <v>19</v>
+        <v>52</v>
       </c>
       <c r="F118" s="1" t="s">
         <v>69</v>
@@ -3380,13 +3453,13 @@
         <v>5</v>
       </c>
       <c r="C119" s="2" t="s">
-        <v>47</v>
+        <v>70</v>
       </c>
       <c r="D119" s="5" t="s">
-        <v>20</v>
+        <v>33</v>
       </c>
       <c r="E119" s="1" t="s">
-        <v>60</v>
+        <v>76</v>
       </c>
       <c r="F119" s="1" t="s">
         <v>69</v>
@@ -3400,13 +3473,13 @@
         <v>5</v>
       </c>
       <c r="C120" s="2" t="s">
-        <v>70</v>
+        <v>5</v>
       </c>
       <c r="D120" s="5" t="s">
-        <v>20</v>
+        <v>36</v>
       </c>
       <c r="E120" s="1" t="s">
-        <v>83</v>
+        <v>35</v>
       </c>
       <c r="F120" s="1" t="s">
         <v>69</v>
@@ -3420,13 +3493,13 @@
         <v>5</v>
       </c>
       <c r="C121" s="2" t="s">
-        <v>5</v>
+        <v>47</v>
       </c>
       <c r="D121" s="5" t="s">
-        <v>22</v>
+        <v>36</v>
       </c>
       <c r="E121" s="1" t="s">
-        <v>21</v>
+        <v>54</v>
       </c>
       <c r="F121" s="1" t="s">
         <v>69</v>
@@ -3440,13 +3513,13 @@
         <v>5</v>
       </c>
       <c r="C122" s="2" t="s">
-        <v>47</v>
+        <v>70</v>
       </c>
       <c r="D122" s="5" t="s">
-        <v>22</v>
+        <v>36</v>
       </c>
       <c r="E122" s="1" t="s">
-        <v>61</v>
+        <v>77</v>
       </c>
       <c r="F122" s="1" t="s">
         <v>69</v>
@@ -3460,13 +3533,13 @@
         <v>5</v>
       </c>
       <c r="C123" s="2" t="s">
-        <v>70</v>
+        <v>5</v>
       </c>
       <c r="D123" s="5" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="E123" s="1" t="s">
-        <v>84</v>
+        <v>12</v>
       </c>
       <c r="F123" s="1" t="s">
         <v>69</v>
@@ -3480,13 +3553,13 @@
         <v>5</v>
       </c>
       <c r="C124" s="2" t="s">
-        <v>5</v>
+        <v>47</v>
       </c>
       <c r="D124" s="5" t="s">
-        <v>38</v>
+        <v>14</v>
       </c>
       <c r="E124" s="1" t="s">
-        <v>37</v>
+        <v>55</v>
       </c>
       <c r="F124" s="1" t="s">
         <v>69</v>
@@ -3500,13 +3573,13 @@
         <v>5</v>
       </c>
       <c r="C125" s="2" t="s">
-        <v>47</v>
+        <v>70</v>
       </c>
       <c r="D125" s="5" t="s">
-        <v>38</v>
+        <v>14</v>
       </c>
       <c r="E125" s="1" t="s">
-        <v>64</v>
+        <v>78</v>
       </c>
       <c r="F125" s="1" t="s">
         <v>69</v>
@@ -3520,13 +3593,13 @@
         <v>5</v>
       </c>
       <c r="C126" s="2" t="s">
-        <v>70</v>
+        <v>5</v>
       </c>
       <c r="D126" s="5" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="E126" s="1" t="s">
-        <v>85</v>
+        <v>41</v>
       </c>
       <c r="F126" s="1" t="s">
         <v>69</v>
@@ -3540,13 +3613,13 @@
         <v>5</v>
       </c>
       <c r="C127" s="2" t="s">
-        <v>5</v>
+        <v>47</v>
       </c>
       <c r="D127" s="5" t="s">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="E127" s="1" t="s">
-        <v>23</v>
+        <v>56</v>
       </c>
       <c r="F127" s="1" t="s">
         <v>69</v>
@@ -3560,13 +3633,13 @@
         <v>5</v>
       </c>
       <c r="C128" s="2" t="s">
-        <v>47</v>
+        <v>70</v>
       </c>
       <c r="D128" s="5" t="s">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="E128" s="1" t="s">
-        <v>62</v>
+        <v>79</v>
       </c>
       <c r="F128" s="1" t="s">
         <v>69</v>
@@ -3580,13 +3653,13 @@
         <v>5</v>
       </c>
       <c r="C129" s="2" t="s">
-        <v>70</v>
+        <v>5</v>
       </c>
       <c r="D129" s="5" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="E129" s="1" t="s">
-        <v>86</v>
+        <v>15</v>
       </c>
       <c r="F129" s="1" t="s">
         <v>69</v>
@@ -3600,13 +3673,13 @@
         <v>5</v>
       </c>
       <c r="C130" s="2" t="s">
-        <v>5</v>
+        <v>47</v>
       </c>
       <c r="D130" s="5" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="E130" s="1" t="s">
-        <v>25</v>
+        <v>57</v>
       </c>
       <c r="F130" s="1" t="s">
         <v>69</v>
@@ -3620,13 +3693,13 @@
         <v>5</v>
       </c>
       <c r="C131" s="2" t="s">
-        <v>47</v>
+        <v>70</v>
       </c>
       <c r="D131" s="5" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="E131" s="1" t="s">
-        <v>63</v>
+        <v>80</v>
       </c>
       <c r="F131" s="1" t="s">
         <v>69</v>
@@ -3640,13 +3713,13 @@
         <v>5</v>
       </c>
       <c r="C132" s="2" t="s">
-        <v>70</v>
+        <v>5</v>
       </c>
       <c r="D132" s="5" t="s">
-        <v>26</v>
+        <v>40</v>
       </c>
       <c r="E132" s="1" t="s">
-        <v>87</v>
+        <v>39</v>
       </c>
       <c r="F132" s="1" t="s">
         <v>69</v>
@@ -3660,13 +3733,13 @@
         <v>5</v>
       </c>
       <c r="C133" s="2" t="s">
-        <v>5</v>
+        <v>47</v>
       </c>
       <c r="D133" s="5" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="E133" s="1" t="s">
-        <v>44</v>
+        <v>58</v>
       </c>
       <c r="F133" s="1" t="s">
         <v>69</v>
@@ -3680,13 +3753,13 @@
         <v>5</v>
       </c>
       <c r="C134" s="2" t="s">
-        <v>47</v>
+        <v>70</v>
       </c>
       <c r="D134" s="5" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="E134" s="1" t="s">
-        <v>65</v>
+        <v>82</v>
       </c>
       <c r="F134" s="1" t="s">
         <v>69</v>
@@ -3700,13 +3773,13 @@
         <v>5</v>
       </c>
       <c r="C135" s="2" t="s">
-        <v>70</v>
+        <v>5</v>
       </c>
       <c r="D135" s="5" t="s">
-        <v>31</v>
+        <v>18</v>
       </c>
       <c r="E135" s="1" t="s">
-        <v>88</v>
+        <v>17</v>
       </c>
       <c r="F135" s="1" t="s">
         <v>69</v>
@@ -3720,13 +3793,13 @@
         <v>5</v>
       </c>
       <c r="C136" s="2" t="s">
-        <v>5</v>
+        <v>47</v>
       </c>
       <c r="D136" s="5" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="E136" s="1" t="s">
-        <v>6</v>
+        <v>59</v>
       </c>
       <c r="F136" s="1" t="s">
         <v>69</v>
@@ -3740,13 +3813,13 @@
         <v>5</v>
       </c>
       <c r="C137" s="2" t="s">
-        <v>47</v>
+        <v>70</v>
       </c>
       <c r="D137" s="5" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="E137" s="1" t="s">
-        <v>66</v>
+        <v>81</v>
       </c>
       <c r="F137" s="1" t="s">
         <v>69</v>
@@ -3760,13 +3833,13 @@
         <v>5</v>
       </c>
       <c r="C138" s="2" t="s">
-        <v>70</v>
+        <v>5</v>
       </c>
       <c r="D138" s="5" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="E138" s="1" t="s">
-        <v>89</v>
+        <v>19</v>
       </c>
       <c r="F138" s="1" t="s">
         <v>69</v>
@@ -3780,13 +3853,13 @@
         <v>5</v>
       </c>
       <c r="C139" s="2" t="s">
-        <v>5</v>
+        <v>47</v>
       </c>
       <c r="D139" s="5" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="E139" s="1" t="s">
-        <v>8</v>
+        <v>60</v>
       </c>
       <c r="F139" s="1" t="s">
         <v>69</v>
@@ -3800,13 +3873,13 @@
         <v>5</v>
       </c>
       <c r="C140" s="2" t="s">
-        <v>47</v>
+        <v>70</v>
       </c>
       <c r="D140" s="5" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="E140" s="1" t="s">
-        <v>67</v>
+        <v>83</v>
       </c>
       <c r="F140" s="1" t="s">
         <v>69</v>
@@ -3820,21 +3893,421 @@
         <v>5</v>
       </c>
       <c r="C141" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D141" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E141" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F141" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="142" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A142" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B142" s="2">
+        <v>5</v>
+      </c>
+      <c r="C142" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D142" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E142" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="F142" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="143" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A143" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B143" s="2">
+        <v>5</v>
+      </c>
+      <c r="C143" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="D141" s="5" t="s">
+      <c r="D143" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E143" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="F143" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="144" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A144" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B144" s="2">
+        <v>5</v>
+      </c>
+      <c r="C144" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D144" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="E144" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F144" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="145" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A145" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B145" s="2">
+        <v>5</v>
+      </c>
+      <c r="C145" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D145" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="E145" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="F145" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="146" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A146" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B146" s="2">
+        <v>5</v>
+      </c>
+      <c r="C146" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D146" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="E146" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="F146" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="147" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A147" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B147" s="2">
+        <v>5</v>
+      </c>
+      <c r="C147" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D147" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E147" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F147" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="148" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A148" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B148" s="2">
+        <v>5</v>
+      </c>
+      <c r="C148" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D148" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E148" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="F148" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="149" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A149" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B149" s="2">
+        <v>5</v>
+      </c>
+      <c r="C149" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D149" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E149" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="F149" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="150" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A150" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B150" s="2">
+        <v>5</v>
+      </c>
+      <c r="C150" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D150" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E150" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F150" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="151" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A151" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B151" s="2">
+        <v>5</v>
+      </c>
+      <c r="C151" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D151" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E151" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="F151" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="152" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A152" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B152" s="2">
+        <v>5</v>
+      </c>
+      <c r="C152" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D152" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E152" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="F152" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="153" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A153" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B153" s="2">
+        <v>5</v>
+      </c>
+      <c r="C153" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D153" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="E153" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F153" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="154" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A154" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B154" s="2">
+        <v>5</v>
+      </c>
+      <c r="C154" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D154" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="E154" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="F154" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="155" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A155" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B155" s="2">
+        <v>5</v>
+      </c>
+      <c r="C155" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D155" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="E155" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="F155" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="156" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A156" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B156" s="2">
+        <v>5</v>
+      </c>
+      <c r="C156" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D156" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E156" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F156" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="157" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A157" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B157" s="2">
+        <v>5</v>
+      </c>
+      <c r="C157" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D157" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E157" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F157" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="158" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A158" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B158" s="2">
+        <v>5</v>
+      </c>
+      <c r="C158" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D158" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E158" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="F158" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="159" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A159" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B159" s="2">
+        <v>5</v>
+      </c>
+      <c r="C159" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D159" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="E141" s="1" t="s">
+      <c r="E159" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F159" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="160" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A160" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B160" s="2">
+        <v>5</v>
+      </c>
+      <c r="C160" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D160" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E160" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F160" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="161" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A161" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B161" s="2">
+        <v>5</v>
+      </c>
+      <c r="C161" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D161" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E161" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="F141" s="1" t="s">
+      <c r="F161" s="1" t="s">
         <v>69</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A82:E121">
-    <sortCondition ref="D84:D121"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A102:E141">
+    <sortCondition ref="D104:D141"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Add US related to Economics domain
</commit_message>
<xml_diff>
--- a/refair-server/datasets/few shot dataset/FSDataset.xlsx
+++ b/refair-server/datasets/few shot dataset/FSDataset.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\morel\Desktop\Refair\ReFair-App\refair-server\datasets\few shot dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B859DB2D-0B7B-4DE6-A75C-D15ADA85659F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C520E58-8C61-420B-AF27-501CF1917991}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{80773445-FB61-4F04-A882-1600FD96C55A}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="806" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="886" uniqueCount="220">
   <si>
     <t>Domain cluster</t>
   </si>
@@ -633,6 +633,69 @@
   </si>
   <si>
     <t>As a marketer, I want to apply word embedding techniques to analyze customer reviews and social media comments about our products, identifying key product features and sentiments that influence consumer preferences and purchasing decisions.</t>
+  </si>
+  <si>
+    <t>Economics</t>
+  </si>
+  <si>
+    <t>As an economist, I want to apply adversarial learning techniques to detect anomalies and fraudulent activities in financial transactions, so that I can protect financial systems from cyber threats and maintain market integrity.</t>
+  </si>
+  <si>
+    <t>As an economist, I want to utilize CNNs to analyze historical economic data and extract spatial and temporal patterns, facilitating better understanding of economic cycles and trends</t>
+  </si>
+  <si>
+    <t>As an economist, I need a conversational agent capable of interpreting complex economic policies and explaining their implications to stakeholders, ensuring transparency and informed public discourse.</t>
+  </si>
+  <si>
+    <t>As an economist, I want to use decision trees to classify economic sectors based on their growth potential and risk profiles, aiding in portfolio diversification strategies for investment firms.</t>
+  </si>
+  <si>
+    <t>As an economist, I want to implement document classification systems to automatically organize and prioritize incoming economic research publications based on their relevance and impact, supporting efficient knowledge discovery and academic collaboration.</t>
+  </si>
+  <si>
+    <t>As an economist, I want to apply entity extraction techniques to automatically identify and categorize economic indicators (e.g., GDP, inflation rate, unemployment rate) mentioned in textual data such as news articles and economic reports, to facilitate quantitative analysis and trend monitoring.</t>
+  </si>
+  <si>
+    <t>As an economist, I want to employ feature selection techniques to identify the most relevant economic indicators (e.g., GDP growth rate, inflation index) for predicting stock market movements, optimizing forecasting models used by financial institutions.</t>
+  </si>
+  <si>
+    <t>As an economist, I need to handle imbalanced datasets when predicting economic downturns to improve the reliability of early warning systems, enabling proactive policy responses and mitigation measures.</t>
+  </si>
+  <si>
+    <t>As an economist, I want to apply keyword extraction techniques to analyze customer feedback and reviews related to economic products and services, extracting sentiments and key concerns to guide market strategies and product development.</t>
+  </si>
+  <si>
+    <t>As an economist, I need k-NN models to analyze regional economic data and identify neighboring regions with similar economic profiles, enabling comparative analysis and policy recommendations for regional development.</t>
+  </si>
+  <si>
+    <t>As an economist, I want to use multi-label classification techniques to segment economic indicators (e.g., inflation rate, unemployment rate, GDP growth) based on their impact on various demographic groups, aiding in equitable economic policy formulation.</t>
+  </si>
+  <si>
+    <t>As an economist, I want to leverage neural networks to predict stock market movements based on historical market data and economic indicators, enhancing investment decision-making and portfolio management.</t>
+  </si>
+  <si>
+    <t>As an economist, I aim to use random forest techniques to analyze the impact of environmental policies on industries such as renewable energy and sustainable agriculture, facilitating evidence-based policy evaluations for green economic growth.</t>
+  </si>
+  <si>
+    <t>As an economist, I want to utilize semantic similarity models to assess the coherence and consistency of economic forecasts generated by different analytical methods, enhancing the reliability of economic projections for strategic planning.</t>
+  </si>
+  <si>
+    <t>As an economist, I need sentiment analysis tools to analyze investor sentiment based on financial news and market reports, predicting market movements and investor behavior for effective risk management.</t>
+  </si>
+  <si>
+    <t>As an economist, I want to utilize speech to text technology to transcribe meetings with clients and stakeholders discussing economic forecasts and investment strategies, ensuring comprehensive and searchable records for future reference.</t>
+  </si>
+  <si>
+    <t>As an economist, I want to use text categorization techniques to classify research papers and articles into economic sub-disciplines such as behavioral economics, development economics, and monetary economics, facilitating targeted literature reviews and research synthesis.</t>
+  </si>
+  <si>
+    <t>As an economist, I aim to deploy unsupervised clustering models to group similar industries based on their economic contributions and market behaviors, facilitating sector-specific economic analysis and policy formulation.</t>
+  </si>
+  <si>
+    <t>As an economist, I want to utilize voice recognition technology to transcribe meetings with clients and stakeholders discussing economic strategies and investment opportunities, maintaining detailed records for strategic decision-making.</t>
+  </si>
+  <si>
+    <t>As an economist, I want to use word embedding techniques to analyze customer feedback and reviews on economic products and services, extracting underlying sentiments and preferences to guide product development and market positioning strategies.</t>
   </si>
 </sst>
 </file>
@@ -716,7 +779,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -736,6 +799,7 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -1070,10 +1134,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8DF0B04-8323-4309-B759-D1CDDA1FBB0E}">
-  <dimension ref="A1:F161"/>
+  <dimension ref="A1:F181"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1105,27 +1169,24 @@
         <v>68</v>
       </c>
     </row>
-    <row r="2" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" s="3" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A2" s="10" t="s">
         <v>177</v>
       </c>
       <c r="B2" s="10">
         <v>2</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="C2" s="11" t="s">
         <v>178</v>
       </c>
       <c r="D2" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" t="s">
         <v>179</v>
       </c>
-      <c r="F2" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:6" s="3" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A3" s="10" t="s">
         <v>177</v>
       </c>
@@ -1133,19 +1194,16 @@
         <v>2</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>178</v>
+        <v>199</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>180</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+      <c r="E3" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" s="3" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A4" s="10" t="s">
         <v>177</v>
       </c>
@@ -1156,16 +1214,13 @@
         <v>178</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>181</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+      <c r="E4" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" s="3" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A5" s="10" t="s">
         <v>177</v>
       </c>
@@ -1173,19 +1228,16 @@
         <v>2</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>178</v>
+        <v>199</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+      <c r="E5" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" s="3" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A6" s="10" t="s">
         <v>177</v>
       </c>
@@ -1196,16 +1248,13 @@
         <v>178</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+      <c r="E6" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" s="3" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A7" s="10" t="s">
         <v>177</v>
       </c>
@@ -1213,19 +1262,16 @@
         <v>2</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>178</v>
+        <v>199</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+      <c r="E7" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" s="3" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A8" s="10" t="s">
         <v>177</v>
       </c>
@@ -1236,16 +1282,13 @@
         <v>178</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+      <c r="E8" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" s="3" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A9" s="10" t="s">
         <v>177</v>
       </c>
@@ -1253,19 +1296,16 @@
         <v>2</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>178</v>
+        <v>199</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>186</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+      <c r="E9" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" s="3" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A10" s="10" t="s">
         <v>177</v>
       </c>
@@ -1276,16 +1316,13 @@
         <v>178</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>187</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+      <c r="E10" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" s="3" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A11" s="10" t="s">
         <v>177</v>
       </c>
@@ -1293,19 +1330,16 @@
         <v>2</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>178</v>
+        <v>199</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+      <c r="E11" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" s="3" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A12" s="10" t="s">
         <v>177</v>
       </c>
@@ -1316,16 +1350,13 @@
         <v>178</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+      <c r="E12" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" s="3" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A13" s="10" t="s">
         <v>177</v>
       </c>
@@ -1333,19 +1364,16 @@
         <v>2</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>178</v>
+        <v>199</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+      <c r="E13" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" s="3" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A14" s="10" t="s">
         <v>177</v>
       </c>
@@ -1356,16 +1384,13 @@
         <v>178</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+      <c r="E14" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" s="3" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A15" s="10" t="s">
         <v>177</v>
       </c>
@@ -1373,19 +1398,16 @@
         <v>2</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>178</v>
+        <v>199</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>192</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+      <c r="E15" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" s="3" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A16" s="10" t="s">
         <v>177</v>
       </c>
@@ -1396,16 +1418,13 @@
         <v>178</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+      <c r="E16" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" s="3" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A17" s="10" t="s">
         <v>177</v>
       </c>
@@ -1413,19 +1432,16 @@
         <v>2</v>
       </c>
       <c r="C17" s="10" t="s">
-        <v>178</v>
+        <v>199</v>
       </c>
       <c r="D17" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>194</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+      <c r="E17" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" s="3" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A18" s="10" t="s">
         <v>177</v>
       </c>
@@ -1436,16 +1452,13 @@
         <v>178</v>
       </c>
       <c r="D18" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>195</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+      <c r="E18" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" s="3" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A19" s="10" t="s">
         <v>177</v>
       </c>
@@ -1453,19 +1466,16 @@
         <v>2</v>
       </c>
       <c r="C19" s="10" t="s">
-        <v>178</v>
+        <v>199</v>
       </c>
       <c r="D19" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>196</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+      <c r="E19" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" s="3" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A20" s="10" t="s">
         <v>177</v>
       </c>
@@ -1476,16 +1486,13 @@
         <v>178</v>
       </c>
       <c r="D20" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+      <c r="E20" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" s="3" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A21" s="10" t="s">
         <v>177</v>
       </c>
@@ -1493,413 +1500,410 @@
         <v>2</v>
       </c>
       <c r="C21" s="10" t="s">
+        <v>199</v>
+      </c>
+      <c r="D21" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="E21" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" s="3" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A22" s="10" t="s">
+        <v>177</v>
+      </c>
+      <c r="B22" s="10">
+        <v>2</v>
+      </c>
+      <c r="C22" s="10" t="s">
         <v>178</v>
       </c>
-      <c r="D21" s="9" t="s">
+      <c r="D22" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="E22" t="s">
+        <v>189</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" s="3" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A23" s="10" t="s">
+        <v>177</v>
+      </c>
+      <c r="B23" s="10">
+        <v>2</v>
+      </c>
+      <c r="C23" s="10" t="s">
+        <v>199</v>
+      </c>
+      <c r="D23" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="E23" t="s">
+        <v>210</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" s="3" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A24" s="10" t="s">
+        <v>177</v>
+      </c>
+      <c r="B24" s="10">
+        <v>2</v>
+      </c>
+      <c r="C24" s="10" t="s">
+        <v>178</v>
+      </c>
+      <c r="D24" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="E24" t="s">
+        <v>190</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" s="3" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A25" s="10" t="s">
+        <v>177</v>
+      </c>
+      <c r="B25" s="10">
+        <v>2</v>
+      </c>
+      <c r="C25" s="10" t="s">
+        <v>199</v>
+      </c>
+      <c r="D25" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="E25" t="s">
+        <v>211</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" s="3" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A26" s="10" t="s">
+        <v>177</v>
+      </c>
+      <c r="B26" s="10">
+        <v>2</v>
+      </c>
+      <c r="C26" s="10" t="s">
+        <v>178</v>
+      </c>
+      <c r="D26" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="E26" t="s">
+        <v>191</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" s="3" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A27" s="10" t="s">
+        <v>177</v>
+      </c>
+      <c r="B27" s="10">
+        <v>2</v>
+      </c>
+      <c r="C27" s="10" t="s">
+        <v>199</v>
+      </c>
+      <c r="D27" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="E27" t="s">
+        <v>212</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" s="3" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A28" s="10" t="s">
+        <v>177</v>
+      </c>
+      <c r="B28" s="10">
+        <v>2</v>
+      </c>
+      <c r="C28" s="10" t="s">
+        <v>178</v>
+      </c>
+      <c r="D28" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="E28" t="s">
+        <v>192</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" s="3" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A29" s="10" t="s">
+        <v>177</v>
+      </c>
+      <c r="B29" s="10">
+        <v>2</v>
+      </c>
+      <c r="C29" s="10" t="s">
+        <v>199</v>
+      </c>
+      <c r="D29" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="E29" t="s">
+        <v>213</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" s="3" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A30" s="10" t="s">
+        <v>177</v>
+      </c>
+      <c r="B30" s="10">
+        <v>2</v>
+      </c>
+      <c r="C30" s="10" t="s">
+        <v>178</v>
+      </c>
+      <c r="D30" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="E30" t="s">
+        <v>193</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" s="3" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A31" s="10" t="s">
+        <v>177</v>
+      </c>
+      <c r="B31" s="10">
+        <v>2</v>
+      </c>
+      <c r="C31" s="10" t="s">
+        <v>199</v>
+      </c>
+      <c r="D31" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="E31" t="s">
+        <v>214</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" s="3" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A32" s="10" t="s">
+        <v>177</v>
+      </c>
+      <c r="B32" s="10">
+        <v>2</v>
+      </c>
+      <c r="C32" s="10" t="s">
+        <v>178</v>
+      </c>
+      <c r="D32" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="E32" t="s">
+        <v>194</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" s="3" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A33" s="10" t="s">
+        <v>177</v>
+      </c>
+      <c r="B33" s="10">
+        <v>2</v>
+      </c>
+      <c r="C33" s="10" t="s">
+        <v>199</v>
+      </c>
+      <c r="D33" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="E33" t="s">
+        <v>215</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" s="3" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A34" s="10" t="s">
+        <v>177</v>
+      </c>
+      <c r="B34" s="10">
+        <v>2</v>
+      </c>
+      <c r="C34" s="10" t="s">
+        <v>178</v>
+      </c>
+      <c r="D34" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="E34" t="s">
+        <v>195</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" s="3" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A35" s="10" t="s">
+        <v>177</v>
+      </c>
+      <c r="B35" s="10">
+        <v>2</v>
+      </c>
+      <c r="C35" s="10" t="s">
+        <v>199</v>
+      </c>
+      <c r="D35" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="E35" t="s">
+        <v>216</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" s="3" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A36" s="10" t="s">
+        <v>177</v>
+      </c>
+      <c r="B36" s="10">
+        <v>2</v>
+      </c>
+      <c r="C36" s="10" t="s">
+        <v>178</v>
+      </c>
+      <c r="D36" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="E36" t="s">
+        <v>196</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" s="3" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A37" s="10" t="s">
+        <v>177</v>
+      </c>
+      <c r="B37" s="10">
+        <v>2</v>
+      </c>
+      <c r="C37" s="10" t="s">
+        <v>199</v>
+      </c>
+      <c r="D37" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="E37" t="s">
+        <v>217</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" s="3" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A38" s="10" t="s">
+        <v>177</v>
+      </c>
+      <c r="B38" s="10">
+        <v>2</v>
+      </c>
+      <c r="C38" s="10" t="s">
+        <v>178</v>
+      </c>
+      <c r="D38" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="E38" t="s">
+        <v>197</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" s="3" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A39" s="10" t="s">
+        <v>177</v>
+      </c>
+      <c r="B39" s="10">
+        <v>2</v>
+      </c>
+      <c r="C39" s="10" t="s">
+        <v>199</v>
+      </c>
+      <c r="D39" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="E39" t="s">
+        <v>218</v>
+      </c>
+      <c r="F39" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" s="3" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A40" s="10" t="s">
+        <v>177</v>
+      </c>
+      <c r="B40" s="10">
+        <v>2</v>
+      </c>
+      <c r="C40" s="10" t="s">
+        <v>178</v>
+      </c>
+      <c r="D40" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="E21" s="1" t="s">
+      <c r="E40" t="s">
         <v>198</v>
       </c>
-      <c r="F21" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="8" t="s">
-        <v>134</v>
-      </c>
-      <c r="B22" s="8">
-        <v>3</v>
-      </c>
-      <c r="C22" s="8" t="s">
-        <v>135</v>
-      </c>
-      <c r="D22" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="8" t="s">
-        <v>134</v>
-      </c>
-      <c r="B23" s="8">
-        <v>3</v>
-      </c>
-      <c r="C23" s="8" t="s">
-        <v>156</v>
-      </c>
-      <c r="D23" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="F23" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="8" t="s">
-        <v>134</v>
-      </c>
-      <c r="B24" s="8">
-        <v>3</v>
-      </c>
-      <c r="C24" s="8" t="s">
-        <v>135</v>
-      </c>
-      <c r="D24" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="F24" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="8" t="s">
-        <v>134</v>
-      </c>
-      <c r="B25" s="8">
-        <v>3</v>
-      </c>
-      <c r="C25" s="8" t="s">
-        <v>156</v>
-      </c>
-      <c r="D25" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="F25" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="8" t="s">
-        <v>134</v>
-      </c>
-      <c r="B26" s="8">
-        <v>3</v>
-      </c>
-      <c r="C26" s="8" t="s">
-        <v>135</v>
-      </c>
-      <c r="D26" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="E26" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="F26" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="8" t="s">
-        <v>134</v>
-      </c>
-      <c r="B27" s="8">
-        <v>3</v>
-      </c>
-      <c r="C27" s="8" t="s">
-        <v>156</v>
-      </c>
-      <c r="D27" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="E27" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="F27" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="8" t="s">
-        <v>134</v>
-      </c>
-      <c r="B28" s="8">
-        <v>3</v>
-      </c>
-      <c r="C28" s="8" t="s">
-        <v>135</v>
-      </c>
-      <c r="D28" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="E28" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="F28" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="8" t="s">
-        <v>134</v>
-      </c>
-      <c r="B29" s="8">
-        <v>3</v>
-      </c>
-      <c r="C29" s="8" t="s">
-        <v>156</v>
-      </c>
-      <c r="D29" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="E29" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="F29" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="8" t="s">
-        <v>134</v>
-      </c>
-      <c r="B30" s="8">
-        <v>3</v>
-      </c>
-      <c r="C30" s="8" t="s">
-        <v>135</v>
-      </c>
-      <c r="D30" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="E30" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="F30" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="8" t="s">
-        <v>134</v>
-      </c>
-      <c r="B31" s="8">
-        <v>3</v>
-      </c>
-      <c r="C31" s="8" t="s">
-        <v>156</v>
-      </c>
-      <c r="D31" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="E31" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="F31" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="8" t="s">
-        <v>134</v>
-      </c>
-      <c r="B32" s="8">
-        <v>3</v>
-      </c>
-      <c r="C32" s="8" t="s">
-        <v>135</v>
-      </c>
-      <c r="D32" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="E32" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="F32" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="8" t="s">
-        <v>134</v>
-      </c>
-      <c r="B33" s="8">
-        <v>3</v>
-      </c>
-      <c r="C33" s="8" t="s">
-        <v>156</v>
-      </c>
-      <c r="D33" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="E33" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="F33" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="8" t="s">
-        <v>134</v>
-      </c>
-      <c r="B34" s="8">
-        <v>3</v>
-      </c>
-      <c r="C34" s="8" t="s">
-        <v>135</v>
-      </c>
-      <c r="D34" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="E34" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="F34" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="8" t="s">
-        <v>134</v>
-      </c>
-      <c r="B35" s="8">
-        <v>3</v>
-      </c>
-      <c r="C35" s="8" t="s">
-        <v>156</v>
-      </c>
-      <c r="D35" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="E35" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="F35" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="8" t="s">
-        <v>134</v>
-      </c>
-      <c r="B36" s="8">
-        <v>3</v>
-      </c>
-      <c r="C36" s="8" t="s">
-        <v>135</v>
-      </c>
-      <c r="D36" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="E36" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="F36" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="8" t="s">
-        <v>134</v>
-      </c>
-      <c r="B37" s="8">
-        <v>3</v>
-      </c>
-      <c r="C37" s="8" t="s">
-        <v>156</v>
-      </c>
-      <c r="D37" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="E37" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="F37" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="8" t="s">
-        <v>134</v>
-      </c>
-      <c r="B38" s="8">
-        <v>3</v>
-      </c>
-      <c r="C38" s="8" t="s">
-        <v>135</v>
-      </c>
-      <c r="D38" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="E38" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="F38" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="8" t="s">
-        <v>134</v>
-      </c>
-      <c r="B39" s="8">
-        <v>3</v>
-      </c>
-      <c r="C39" s="8" t="s">
-        <v>156</v>
-      </c>
-      <c r="D39" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="E39" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="F39" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="8" t="s">
-        <v>134</v>
-      </c>
-      <c r="B40" s="8">
-        <v>3</v>
-      </c>
-      <c r="C40" s="8" t="s">
-        <v>135</v>
-      </c>
-      <c r="D40" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="E40" s="1" t="s">
-        <v>145</v>
-      </c>
       <c r="F40" s="1" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="41" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="8" t="s">
-        <v>134</v>
-      </c>
-      <c r="B41" s="8">
-        <v>3</v>
-      </c>
-      <c r="C41" s="8" t="s">
-        <v>156</v>
+    <row r="41" spans="1:6" s="3" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A41" s="10" t="s">
+        <v>177</v>
+      </c>
+      <c r="B41" s="10">
+        <v>2</v>
+      </c>
+      <c r="C41" s="10" t="s">
+        <v>199</v>
       </c>
       <c r="D41" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="E41" s="1" t="s">
-        <v>166</v>
+        <v>9</v>
+      </c>
+      <c r="E41" t="s">
+        <v>219</v>
       </c>
       <c r="F41" s="1" t="s">
         <v>69</v>
@@ -1916,10 +1920,10 @@
         <v>135</v>
       </c>
       <c r="D42" s="5" t="s">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>146</v>
+        <v>136</v>
       </c>
       <c r="F42" s="1" t="s">
         <v>69</v>
@@ -1936,10 +1940,10 @@
         <v>156</v>
       </c>
       <c r="D43" s="9" t="s">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>167</v>
+        <v>157</v>
       </c>
       <c r="F43" s="1" t="s">
         <v>69</v>
@@ -1956,10 +1960,10 @@
         <v>135</v>
       </c>
       <c r="D44" s="5" t="s">
-        <v>18</v>
+        <v>43</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>147</v>
+        <v>137</v>
       </c>
       <c r="F44" s="1" t="s">
         <v>69</v>
@@ -1976,10 +1980,10 @@
         <v>156</v>
       </c>
       <c r="D45" s="9" t="s">
-        <v>18</v>
+        <v>43</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>168</v>
+        <v>158</v>
       </c>
       <c r="F45" s="1" t="s">
         <v>69</v>
@@ -1996,10 +2000,10 @@
         <v>135</v>
       </c>
       <c r="D46" s="5" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>148</v>
+        <v>138</v>
       </c>
       <c r="F46" s="1" t="s">
         <v>69</v>
@@ -2016,10 +2020,10 @@
         <v>156</v>
       </c>
       <c r="D47" s="9" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>169</v>
+        <v>159</v>
       </c>
       <c r="F47" s="1" t="s">
         <v>69</v>
@@ -2036,10 +2040,10 @@
         <v>135</v>
       </c>
       <c r="D48" s="5" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>149</v>
+        <v>139</v>
       </c>
       <c r="F48" s="1" t="s">
         <v>69</v>
@@ -2056,10 +2060,10 @@
         <v>156</v>
       </c>
       <c r="D49" s="9" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>170</v>
+        <v>160</v>
       </c>
       <c r="F49" s="1" t="s">
         <v>69</v>
@@ -2076,10 +2080,10 @@
         <v>135</v>
       </c>
       <c r="D50" s="5" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>150</v>
+        <v>140</v>
       </c>
       <c r="F50" s="1" t="s">
         <v>69</v>
@@ -2096,10 +2100,10 @@
         <v>156</v>
       </c>
       <c r="D51" s="9" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>171</v>
+        <v>161</v>
       </c>
       <c r="F51" s="1" t="s">
         <v>69</v>
@@ -2116,10 +2120,10 @@
         <v>135</v>
       </c>
       <c r="D52" s="5" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>151</v>
+        <v>141</v>
       </c>
       <c r="F52" s="1" t="s">
         <v>69</v>
@@ -2136,10 +2140,10 @@
         <v>156</v>
       </c>
       <c r="D53" s="9" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>172</v>
+        <v>162</v>
       </c>
       <c r="F53" s="1" t="s">
         <v>69</v>
@@ -2156,10 +2160,10 @@
         <v>135</v>
       </c>
       <c r="D54" s="5" t="s">
-        <v>26</v>
+        <v>36</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>152</v>
+        <v>142</v>
       </c>
       <c r="F54" s="1" t="s">
         <v>69</v>
@@ -2176,10 +2180,10 @@
         <v>156</v>
       </c>
       <c r="D55" s="9" t="s">
-        <v>26</v>
+        <v>36</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>173</v>
+        <v>163</v>
       </c>
       <c r="F55" s="1" t="s">
         <v>69</v>
@@ -2196,10 +2200,10 @@
         <v>135</v>
       </c>
       <c r="D56" s="5" t="s">
-        <v>31</v>
+        <v>14</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>153</v>
+        <v>143</v>
       </c>
       <c r="F56" s="1" t="s">
         <v>69</v>
@@ -2216,10 +2220,10 @@
         <v>156</v>
       </c>
       <c r="D57" s="9" t="s">
-        <v>31</v>
+        <v>14</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>174</v>
+        <v>164</v>
       </c>
       <c r="F57" s="1" t="s">
         <v>69</v>
@@ -2236,10 +2240,10 @@
         <v>135</v>
       </c>
       <c r="D58" s="5" t="s">
-        <v>7</v>
+        <v>34</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>154</v>
+        <v>144</v>
       </c>
       <c r="F58" s="1" t="s">
         <v>69</v>
@@ -2256,10 +2260,10 @@
         <v>156</v>
       </c>
       <c r="D59" s="9" t="s">
-        <v>7</v>
+        <v>34</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>175</v>
+        <v>165</v>
       </c>
       <c r="F59" s="1" t="s">
         <v>69</v>
@@ -2276,10 +2280,10 @@
         <v>135</v>
       </c>
       <c r="D60" s="5" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>155</v>
+        <v>145</v>
       </c>
       <c r="F60" s="1" t="s">
         <v>69</v>
@@ -2296,410 +2300,410 @@
         <v>156</v>
       </c>
       <c r="D61" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="E61" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="F61" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="B62" s="8">
+        <v>3</v>
+      </c>
+      <c r="C62" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="D62" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="E62" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="F62" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="B63" s="8">
+        <v>3</v>
+      </c>
+      <c r="C63" s="8" t="s">
+        <v>156</v>
+      </c>
+      <c r="D63" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="E63" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="F63" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="B64" s="8">
+        <v>3</v>
+      </c>
+      <c r="C64" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="D64" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E64" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="F64" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="B65" s="8">
+        <v>3</v>
+      </c>
+      <c r="C65" s="8" t="s">
+        <v>156</v>
+      </c>
+      <c r="D65" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="E65" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="F65" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="B66" s="8">
+        <v>3</v>
+      </c>
+      <c r="C66" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="D66" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E66" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="F66" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A67" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="B67" s="8">
+        <v>3</v>
+      </c>
+      <c r="C67" s="8" t="s">
+        <v>156</v>
+      </c>
+      <c r="D67" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="E67" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="F67" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A68" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="B68" s="8">
+        <v>3</v>
+      </c>
+      <c r="C68" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="D68" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E68" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="F68" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="B69" s="8">
+        <v>3</v>
+      </c>
+      <c r="C69" s="8" t="s">
+        <v>156</v>
+      </c>
+      <c r="D69" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="E69" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="F69" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A70" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="B70" s="8">
+        <v>3</v>
+      </c>
+      <c r="C70" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="D70" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="E70" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="F70" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A71" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="B71" s="8">
+        <v>3</v>
+      </c>
+      <c r="C71" s="8" t="s">
+        <v>156</v>
+      </c>
+      <c r="D71" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="E71" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="F71" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A72" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="B72" s="8">
+        <v>3</v>
+      </c>
+      <c r="C72" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="D72" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E72" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="F72" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A73" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="B73" s="8">
+        <v>3</v>
+      </c>
+      <c r="C73" s="8" t="s">
+        <v>156</v>
+      </c>
+      <c r="D73" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="E73" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="F73" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A74" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="B74" s="8">
+        <v>3</v>
+      </c>
+      <c r="C74" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="D74" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E74" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="F74" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A75" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="B75" s="8">
+        <v>3</v>
+      </c>
+      <c r="C75" s="8" t="s">
+        <v>156</v>
+      </c>
+      <c r="D75" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="E75" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="F75" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A76" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="B76" s="8">
+        <v>3</v>
+      </c>
+      <c r="C76" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="D76" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="E76" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="F76" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A77" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="B77" s="8">
+        <v>3</v>
+      </c>
+      <c r="C77" s="8" t="s">
+        <v>156</v>
+      </c>
+      <c r="D77" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="E77" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="F77" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A78" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="B78" s="8">
+        <v>3</v>
+      </c>
+      <c r="C78" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="D78" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E78" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="F78" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A79" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="B79" s="8">
+        <v>3</v>
+      </c>
+      <c r="C79" s="8" t="s">
+        <v>156</v>
+      </c>
+      <c r="D79" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="E79" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="F79" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A80" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="B80" s="8">
+        <v>3</v>
+      </c>
+      <c r="C80" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="D80" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="E61" s="1" t="s">
+      <c r="E80" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="F80" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A81" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="B81" s="8">
+        <v>3</v>
+      </c>
+      <c r="C81" s="8" t="s">
+        <v>156</v>
+      </c>
+      <c r="D81" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E81" s="1" t="s">
         <v>176</v>
-      </c>
-      <c r="F61" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="62" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="B62" s="7">
-        <v>4</v>
-      </c>
-      <c r="C62" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="D62" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="E62" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="F62" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="B63" s="7">
-        <v>4</v>
-      </c>
-      <c r="C63" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="D63" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="E63" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="F63" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="64" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="B64" s="7">
-        <v>4</v>
-      </c>
-      <c r="C64" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="D64" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="E64" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="F64" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="65" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="B65" s="7">
-        <v>4</v>
-      </c>
-      <c r="C65" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="D65" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="E65" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="F65" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="66" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="B66" s="7">
-        <v>4</v>
-      </c>
-      <c r="C66" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="D66" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="E66" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="F66" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="67" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="B67" s="7">
-        <v>4</v>
-      </c>
-      <c r="C67" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="D67" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="E67" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="F67" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="68" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="B68" s="7">
-        <v>4</v>
-      </c>
-      <c r="C68" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="D68" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E68" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="F68" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="69" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="B69" s="7">
-        <v>4</v>
-      </c>
-      <c r="C69" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="D69" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E69" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="F69" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="70" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="B70" s="7">
-        <v>4</v>
-      </c>
-      <c r="C70" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="D70" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="E70" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="F70" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="71" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="B71" s="7">
-        <v>4</v>
-      </c>
-      <c r="C71" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="D71" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="E71" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="F71" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="72" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="B72" s="7">
-        <v>4</v>
-      </c>
-      <c r="C72" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="D72" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="E72" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="F72" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="73" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="B73" s="7">
-        <v>4</v>
-      </c>
-      <c r="C73" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="D73" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="E73" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="F73" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="74" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="B74" s="7">
-        <v>4</v>
-      </c>
-      <c r="C74" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="D74" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="E74" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="F74" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="75" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="B75" s="7">
-        <v>4</v>
-      </c>
-      <c r="C75" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="D75" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="E75" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="F75" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="76" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="B76" s="7">
-        <v>4</v>
-      </c>
-      <c r="C76" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="D76" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="E76" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="F76" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="77" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="B77" s="7">
-        <v>4</v>
-      </c>
-      <c r="C77" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="D77" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="E77" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="F77" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="78" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="B78" s="7">
-        <v>4</v>
-      </c>
-      <c r="C78" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="D78" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="E78" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="F78" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="79" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="B79" s="7">
-        <v>4</v>
-      </c>
-      <c r="C79" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="D79" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="E79" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="F79" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="80" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="B80" s="7">
-        <v>4</v>
-      </c>
-      <c r="C80" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="D80" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="E80" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="F80" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="81" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="B81" s="7">
-        <v>4</v>
-      </c>
-      <c r="C81" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="D81" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="E81" s="1" t="s">
-        <v>102</v>
       </c>
       <c r="F81" s="1" t="s">
         <v>69</v>
@@ -2716,10 +2720,10 @@
         <v>113</v>
       </c>
       <c r="D82" s="4" t="s">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="E82" s="1" t="s">
-        <v>124</v>
+        <v>114</v>
       </c>
       <c r="F82" s="1" t="s">
         <v>69</v>
@@ -2736,10 +2740,10 @@
         <v>92</v>
       </c>
       <c r="D83" s="4" t="s">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="E83" s="1" t="s">
-        <v>103</v>
+        <v>93</v>
       </c>
       <c r="F83" s="1" t="s">
         <v>69</v>
@@ -2756,10 +2760,10 @@
         <v>113</v>
       </c>
       <c r="D84" s="4" t="s">
-        <v>18</v>
+        <v>43</v>
       </c>
       <c r="E84" s="1" t="s">
-        <v>125</v>
+        <v>115</v>
       </c>
       <c r="F84" s="1" t="s">
         <v>69</v>
@@ -2776,10 +2780,10 @@
         <v>92</v>
       </c>
       <c r="D85" s="4" t="s">
-        <v>18</v>
+        <v>43</v>
       </c>
       <c r="E85" s="1" t="s">
-        <v>104</v>
+        <v>94</v>
       </c>
       <c r="F85" s="1" t="s">
         <v>69</v>
@@ -2796,10 +2800,10 @@
         <v>113</v>
       </c>
       <c r="D86" s="4" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="E86" s="1" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
       <c r="F86" s="1" t="s">
         <v>69</v>
@@ -2816,10 +2820,10 @@
         <v>92</v>
       </c>
       <c r="D87" s="4" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="E87" s="1" t="s">
-        <v>105</v>
+        <v>95</v>
       </c>
       <c r="F87" s="1" t="s">
         <v>69</v>
@@ -2836,10 +2840,10 @@
         <v>113</v>
       </c>
       <c r="D88" s="4" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="E88" s="1" t="s">
-        <v>127</v>
+        <v>117</v>
       </c>
       <c r="F88" s="1" t="s">
         <v>69</v>
@@ -2856,10 +2860,10 @@
         <v>92</v>
       </c>
       <c r="D89" s="4" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="E89" s="1" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="F89" s="1" t="s">
         <v>69</v>
@@ -2876,10 +2880,10 @@
         <v>113</v>
       </c>
       <c r="D90" s="4" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="E90" s="1" t="s">
-        <v>128</v>
+        <v>118</v>
       </c>
       <c r="F90" s="1" t="s">
         <v>69</v>
@@ -2896,10 +2900,10 @@
         <v>92</v>
       </c>
       <c r="D91" s="4" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="E91" s="1" t="s">
-        <v>107</v>
+        <v>97</v>
       </c>
       <c r="F91" s="1" t="s">
         <v>69</v>
@@ -2916,10 +2920,10 @@
         <v>113</v>
       </c>
       <c r="D92" s="4" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="E92" s="1" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
       <c r="F92" s="1" t="s">
         <v>69</v>
@@ -2936,10 +2940,10 @@
         <v>92</v>
       </c>
       <c r="D93" s="4" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="E93" s="1" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="F93" s="1" t="s">
         <v>69</v>
@@ -2956,10 +2960,10 @@
         <v>113</v>
       </c>
       <c r="D94" s="4" t="s">
-        <v>26</v>
+        <v>36</v>
       </c>
       <c r="E94" s="1" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="F94" s="1" t="s">
         <v>69</v>
@@ -2976,10 +2980,10 @@
         <v>92</v>
       </c>
       <c r="D95" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="E95" s="6" t="s">
-        <v>109</v>
+        <v>36</v>
+      </c>
+      <c r="E95" s="1" t="s">
+        <v>99</v>
       </c>
       <c r="F95" s="1" t="s">
         <v>69</v>
@@ -2996,10 +3000,10 @@
         <v>113</v>
       </c>
       <c r="D96" s="4" t="s">
-        <v>31</v>
+        <v>14</v>
       </c>
       <c r="E96" s="1" t="s">
-        <v>131</v>
+        <v>121</v>
       </c>
       <c r="F96" s="1" t="s">
         <v>69</v>
@@ -3016,10 +3020,10 @@
         <v>92</v>
       </c>
       <c r="D97" s="4" t="s">
-        <v>31</v>
+        <v>14</v>
       </c>
       <c r="E97" s="1" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="F97" s="1" t="s">
         <v>69</v>
@@ -3036,10 +3040,10 @@
         <v>113</v>
       </c>
       <c r="D98" s="4" t="s">
-        <v>7</v>
+        <v>34</v>
       </c>
       <c r="E98" s="1" t="s">
-        <v>132</v>
+        <v>122</v>
       </c>
       <c r="F98" s="1" t="s">
         <v>69</v>
@@ -3056,10 +3060,10 @@
         <v>92</v>
       </c>
       <c r="D99" s="4" t="s">
-        <v>7</v>
+        <v>34</v>
       </c>
       <c r="E99" s="1" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
       <c r="F99" s="1" t="s">
         <v>69</v>
@@ -3076,10 +3080,10 @@
         <v>113</v>
       </c>
       <c r="D100" s="4" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="E100" s="1" t="s">
-        <v>133</v>
+        <v>123</v>
       </c>
       <c r="F100" s="1" t="s">
         <v>69</v>
@@ -3096,410 +3100,410 @@
         <v>92</v>
       </c>
       <c r="D101" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E101" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="F101" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A102" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="B102" s="7">
+        <v>4</v>
+      </c>
+      <c r="C102" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="D102" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="E102" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="F102" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A103" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="B103" s="7">
+        <v>4</v>
+      </c>
+      <c r="C103" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="D103" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="E103" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="F103" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A104" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="B104" s="7">
+        <v>4</v>
+      </c>
+      <c r="C104" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="D104" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E104" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="F104" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A105" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="B105" s="7">
+        <v>4</v>
+      </c>
+      <c r="C105" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="D105" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E105" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="F105" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A106" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="B106" s="7">
+        <v>4</v>
+      </c>
+      <c r="C106" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="D106" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E106" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="F106" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A107" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="B107" s="7">
+        <v>4</v>
+      </c>
+      <c r="C107" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="D107" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E107" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="F107" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A108" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="B108" s="7">
+        <v>4</v>
+      </c>
+      <c r="C108" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="D108" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E108" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="F108" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A109" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="B109" s="7">
+        <v>4</v>
+      </c>
+      <c r="C109" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="D109" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E109" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="F109" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A110" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="B110" s="7">
+        <v>4</v>
+      </c>
+      <c r="C110" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="D110" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="E110" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="F110" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A111" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="B111" s="7">
+        <v>4</v>
+      </c>
+      <c r="C111" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="D111" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="E111" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="F111" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A112" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="B112" s="7">
+        <v>4</v>
+      </c>
+      <c r="C112" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="D112" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E112" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="F112" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="113" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A113" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="B113" s="7">
+        <v>4</v>
+      </c>
+      <c r="C113" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="D113" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E113" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="F113" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="114" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A114" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="B114" s="7">
+        <v>4</v>
+      </c>
+      <c r="C114" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="D114" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="E114" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="F114" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="115" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A115" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="B115" s="7">
+        <v>4</v>
+      </c>
+      <c r="C115" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="D115" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="E115" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="F115" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="116" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A116" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="B116" s="7">
+        <v>4</v>
+      </c>
+      <c r="C116" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="D116" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="E116" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="F116" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="117" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A117" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="B117" s="7">
+        <v>4</v>
+      </c>
+      <c r="C117" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="D117" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="E117" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="F117" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="118" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A118" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="B118" s="7">
+        <v>4</v>
+      </c>
+      <c r="C118" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="D118" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E118" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="F118" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="119" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A119" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="B119" s="7">
+        <v>4</v>
+      </c>
+      <c r="C119" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="D119" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E119" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="F119" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="120" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A120" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="B120" s="7">
+        <v>4</v>
+      </c>
+      <c r="C120" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="D120" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="E101" s="1" t="s">
+      <c r="E120" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="F120" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="121" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A121" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="B121" s="7">
+        <v>4</v>
+      </c>
+      <c r="C121" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="D121" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E121" s="1" t="s">
         <v>112</v>
-      </c>
-      <c r="F101" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A102" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B102" s="2">
-        <v>5</v>
-      </c>
-      <c r="C102" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D102" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E102" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="F102" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A103" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B103" s="2">
-        <v>5</v>
-      </c>
-      <c r="C103" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="D103" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E103" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="F103" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A104" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B104" s="2">
-        <v>5</v>
-      </c>
-      <c r="C104" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="D104" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E104" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="F104" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A105" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B105" s="2">
-        <v>5</v>
-      </c>
-      <c r="C105" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D105" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="E105" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="F105" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A106" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B106" s="2">
-        <v>5</v>
-      </c>
-      <c r="C106" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="D106" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="E106" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="F106" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A107" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B107" s="2">
-        <v>5</v>
-      </c>
-      <c r="C107" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="D107" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="E107" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="F107" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A108" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B108" s="2">
-        <v>5</v>
-      </c>
-      <c r="C108" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D108" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="E108" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="F108" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A109" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B109" s="2">
-        <v>5</v>
-      </c>
-      <c r="C109" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="D109" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="E109" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="F109" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A110" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B110" s="2">
-        <v>5</v>
-      </c>
-      <c r="C110" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="D110" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="E110" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="F110" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A111" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B111" s="2">
-        <v>5</v>
-      </c>
-      <c r="C111" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D111" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="E111" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F111" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A112" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B112" s="2">
-        <v>5</v>
-      </c>
-      <c r="C112" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="D112" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="E112" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="F112" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A113" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B113" s="2">
-        <v>5</v>
-      </c>
-      <c r="C113" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="D113" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="E113" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="F113" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A114" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B114" s="2">
-        <v>5</v>
-      </c>
-      <c r="C114" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D114" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="E114" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="F114" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A115" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B115" s="2">
-        <v>5</v>
-      </c>
-      <c r="C115" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="D115" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="E115" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="F115" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A116" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B116" s="2">
-        <v>5</v>
-      </c>
-      <c r="C116" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="D116" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="E116" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="F116" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A117" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B117" s="2">
-        <v>5</v>
-      </c>
-      <c r="C117" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D117" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="E117" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="F117" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A118" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B118" s="2">
-        <v>5</v>
-      </c>
-      <c r="C118" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="D118" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="E118" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="F118" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A119" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B119" s="2">
-        <v>5</v>
-      </c>
-      <c r="C119" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="D119" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="E119" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="F119" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A120" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B120" s="2">
-        <v>5</v>
-      </c>
-      <c r="C120" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D120" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="E120" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="F120" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A121" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B121" s="2">
-        <v>5</v>
-      </c>
-      <c r="C121" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="D121" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="E121" s="1" t="s">
-        <v>54</v>
       </c>
       <c r="F121" s="1" t="s">
         <v>69</v>
@@ -3513,13 +3517,13 @@
         <v>5</v>
       </c>
       <c r="C122" s="2" t="s">
-        <v>70</v>
+        <v>5</v>
       </c>
       <c r="D122" s="5" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="E122" s="1" t="s">
-        <v>77</v>
+        <v>27</v>
       </c>
       <c r="F122" s="1" t="s">
         <v>69</v>
@@ -3533,13 +3537,13 @@
         <v>5</v>
       </c>
       <c r="C123" s="2" t="s">
-        <v>5</v>
+        <v>47</v>
       </c>
       <c r="D123" s="5" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="E123" s="1" t="s">
-        <v>12</v>
+        <v>49</v>
       </c>
       <c r="F123" s="1" t="s">
         <v>69</v>
@@ -3553,13 +3557,13 @@
         <v>5</v>
       </c>
       <c r="C124" s="2" t="s">
-        <v>47</v>
+        <v>70</v>
       </c>
       <c r="D124" s="5" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="E124" s="1" t="s">
-        <v>55</v>
+        <v>71</v>
       </c>
       <c r="F124" s="1" t="s">
         <v>69</v>
@@ -3573,13 +3577,13 @@
         <v>5</v>
       </c>
       <c r="C125" s="2" t="s">
-        <v>70</v>
+        <v>5</v>
       </c>
       <c r="D125" s="5" t="s">
-        <v>14</v>
+        <v>43</v>
       </c>
       <c r="E125" s="1" t="s">
-        <v>78</v>
+        <v>42</v>
       </c>
       <c r="F125" s="1" t="s">
         <v>69</v>
@@ -3593,13 +3597,13 @@
         <v>5</v>
       </c>
       <c r="C126" s="2" t="s">
-        <v>5</v>
+        <v>47</v>
       </c>
       <c r="D126" s="5" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="E126" s="1" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="F126" s="1" t="s">
         <v>69</v>
@@ -3613,13 +3617,13 @@
         <v>5</v>
       </c>
       <c r="C127" s="2" t="s">
-        <v>47</v>
+        <v>70</v>
       </c>
       <c r="D127" s="5" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="E127" s="1" t="s">
-        <v>56</v>
+        <v>72</v>
       </c>
       <c r="F127" s="1" t="s">
         <v>69</v>
@@ -3633,13 +3637,13 @@
         <v>5</v>
       </c>
       <c r="C128" s="2" t="s">
-        <v>70</v>
+        <v>5</v>
       </c>
       <c r="D128" s="5" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="E128" s="1" t="s">
-        <v>79</v>
+        <v>29</v>
       </c>
       <c r="F128" s="1" t="s">
         <v>69</v>
@@ -3653,13 +3657,13 @@
         <v>5</v>
       </c>
       <c r="C129" s="2" t="s">
-        <v>5</v>
+        <v>47</v>
       </c>
       <c r="D129" s="5" t="s">
-        <v>16</v>
+        <v>30</v>
       </c>
       <c r="E129" s="1" t="s">
-        <v>15</v>
+        <v>50</v>
       </c>
       <c r="F129" s="1" t="s">
         <v>69</v>
@@ -3673,13 +3677,13 @@
         <v>5</v>
       </c>
       <c r="C130" s="2" t="s">
-        <v>47</v>
+        <v>70</v>
       </c>
       <c r="D130" s="5" t="s">
-        <v>16</v>
+        <v>30</v>
       </c>
       <c r="E130" s="1" t="s">
-        <v>57</v>
+        <v>73</v>
       </c>
       <c r="F130" s="1" t="s">
         <v>69</v>
@@ -3693,13 +3697,13 @@
         <v>5</v>
       </c>
       <c r="C131" s="2" t="s">
-        <v>70</v>
+        <v>5</v>
       </c>
       <c r="D131" s="5" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="E131" s="1" t="s">
-        <v>80</v>
+        <v>11</v>
       </c>
       <c r="F131" s="1" t="s">
         <v>69</v>
@@ -3713,13 +3717,13 @@
         <v>5</v>
       </c>
       <c r="C132" s="2" t="s">
-        <v>5</v>
+        <v>47</v>
       </c>
       <c r="D132" s="5" t="s">
-        <v>40</v>
+        <v>13</v>
       </c>
       <c r="E132" s="1" t="s">
-        <v>39</v>
+        <v>51</v>
       </c>
       <c r="F132" s="1" t="s">
         <v>69</v>
@@ -3733,13 +3737,13 @@
         <v>5</v>
       </c>
       <c r="C133" s="2" t="s">
-        <v>47</v>
+        <v>70</v>
       </c>
       <c r="D133" s="5" t="s">
-        <v>40</v>
+        <v>13</v>
       </c>
       <c r="E133" s="1" t="s">
-        <v>58</v>
+        <v>74</v>
       </c>
       <c r="F133" s="1" t="s">
         <v>69</v>
@@ -3753,13 +3757,13 @@
         <v>5</v>
       </c>
       <c r="C134" s="2" t="s">
-        <v>70</v>
+        <v>5</v>
       </c>
       <c r="D134" s="5" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="E134" s="1" t="s">
-        <v>82</v>
+        <v>45</v>
       </c>
       <c r="F134" s="1" t="s">
         <v>69</v>
@@ -3773,13 +3777,13 @@
         <v>5</v>
       </c>
       <c r="C135" s="2" t="s">
-        <v>5</v>
+        <v>47</v>
       </c>
       <c r="D135" s="5" t="s">
-        <v>18</v>
+        <v>46</v>
       </c>
       <c r="E135" s="1" t="s">
-        <v>17</v>
+        <v>53</v>
       </c>
       <c r="F135" s="1" t="s">
         <v>69</v>
@@ -3793,13 +3797,13 @@
         <v>5</v>
       </c>
       <c r="C136" s="2" t="s">
-        <v>47</v>
+        <v>70</v>
       </c>
       <c r="D136" s="5" t="s">
-        <v>18</v>
+        <v>46</v>
       </c>
       <c r="E136" s="1" t="s">
-        <v>59</v>
+        <v>75</v>
       </c>
       <c r="F136" s="1" t="s">
         <v>69</v>
@@ -3813,13 +3817,13 @@
         <v>5</v>
       </c>
       <c r="C137" s="2" t="s">
-        <v>70</v>
+        <v>5</v>
       </c>
       <c r="D137" s="5" t="s">
-        <v>18</v>
+        <v>33</v>
       </c>
       <c r="E137" s="1" t="s">
-        <v>81</v>
+        <v>32</v>
       </c>
       <c r="F137" s="1" t="s">
         <v>69</v>
@@ -3833,13 +3837,13 @@
         <v>5</v>
       </c>
       <c r="C138" s="2" t="s">
-        <v>5</v>
+        <v>47</v>
       </c>
       <c r="D138" s="5" t="s">
-        <v>20</v>
+        <v>33</v>
       </c>
       <c r="E138" s="1" t="s">
-        <v>19</v>
+        <v>52</v>
       </c>
       <c r="F138" s="1" t="s">
         <v>69</v>
@@ -3853,13 +3857,13 @@
         <v>5</v>
       </c>
       <c r="C139" s="2" t="s">
-        <v>47</v>
+        <v>70</v>
       </c>
       <c r="D139" s="5" t="s">
-        <v>20</v>
+        <v>33</v>
       </c>
       <c r="E139" s="1" t="s">
-        <v>60</v>
+        <v>76</v>
       </c>
       <c r="F139" s="1" t="s">
         <v>69</v>
@@ -3873,13 +3877,13 @@
         <v>5</v>
       </c>
       <c r="C140" s="2" t="s">
-        <v>70</v>
+        <v>5</v>
       </c>
       <c r="D140" s="5" t="s">
-        <v>20</v>
+        <v>36</v>
       </c>
       <c r="E140" s="1" t="s">
-        <v>83</v>
+        <v>35</v>
       </c>
       <c r="F140" s="1" t="s">
         <v>69</v>
@@ -3893,13 +3897,13 @@
         <v>5</v>
       </c>
       <c r="C141" s="2" t="s">
-        <v>5</v>
+        <v>47</v>
       </c>
       <c r="D141" s="5" t="s">
-        <v>22</v>
+        <v>36</v>
       </c>
       <c r="E141" s="1" t="s">
-        <v>21</v>
+        <v>54</v>
       </c>
       <c r="F141" s="1" t="s">
         <v>69</v>
@@ -3913,13 +3917,13 @@
         <v>5</v>
       </c>
       <c r="C142" s="2" t="s">
-        <v>47</v>
+        <v>70</v>
       </c>
       <c r="D142" s="5" t="s">
-        <v>22</v>
+        <v>36</v>
       </c>
       <c r="E142" s="1" t="s">
-        <v>61</v>
+        <v>77</v>
       </c>
       <c r="F142" s="1" t="s">
         <v>69</v>
@@ -3933,13 +3937,13 @@
         <v>5</v>
       </c>
       <c r="C143" s="2" t="s">
-        <v>70</v>
+        <v>5</v>
       </c>
       <c r="D143" s="5" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="E143" s="1" t="s">
-        <v>84</v>
+        <v>12</v>
       </c>
       <c r="F143" s="1" t="s">
         <v>69</v>
@@ -3953,13 +3957,13 @@
         <v>5</v>
       </c>
       <c r="C144" s="2" t="s">
-        <v>5</v>
+        <v>47</v>
       </c>
       <c r="D144" s="5" t="s">
-        <v>38</v>
+        <v>14</v>
       </c>
       <c r="E144" s="1" t="s">
-        <v>37</v>
+        <v>55</v>
       </c>
       <c r="F144" s="1" t="s">
         <v>69</v>
@@ -3973,13 +3977,13 @@
         <v>5</v>
       </c>
       <c r="C145" s="2" t="s">
-        <v>47</v>
+        <v>70</v>
       </c>
       <c r="D145" s="5" t="s">
-        <v>38</v>
+        <v>14</v>
       </c>
       <c r="E145" s="1" t="s">
-        <v>64</v>
+        <v>78</v>
       </c>
       <c r="F145" s="1" t="s">
         <v>69</v>
@@ -3993,13 +3997,13 @@
         <v>5</v>
       </c>
       <c r="C146" s="2" t="s">
-        <v>70</v>
+        <v>5</v>
       </c>
       <c r="D146" s="5" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="E146" s="1" t="s">
-        <v>85</v>
+        <v>41</v>
       </c>
       <c r="F146" s="1" t="s">
         <v>69</v>
@@ -4013,13 +4017,13 @@
         <v>5</v>
       </c>
       <c r="C147" s="2" t="s">
-        <v>5</v>
+        <v>47</v>
       </c>
       <c r="D147" s="5" t="s">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="E147" s="1" t="s">
-        <v>23</v>
+        <v>56</v>
       </c>
       <c r="F147" s="1" t="s">
         <v>69</v>
@@ -4033,13 +4037,13 @@
         <v>5</v>
       </c>
       <c r="C148" s="2" t="s">
-        <v>47</v>
+        <v>70</v>
       </c>
       <c r="D148" s="5" t="s">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="E148" s="1" t="s">
-        <v>62</v>
+        <v>79</v>
       </c>
       <c r="F148" s="1" t="s">
         <v>69</v>
@@ -4053,13 +4057,13 @@
         <v>5</v>
       </c>
       <c r="C149" s="2" t="s">
-        <v>70</v>
+        <v>5</v>
       </c>
       <c r="D149" s="5" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="E149" s="1" t="s">
-        <v>86</v>
+        <v>15</v>
       </c>
       <c r="F149" s="1" t="s">
         <v>69</v>
@@ -4073,13 +4077,13 @@
         <v>5</v>
       </c>
       <c r="C150" s="2" t="s">
-        <v>5</v>
+        <v>47</v>
       </c>
       <c r="D150" s="5" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="E150" s="1" t="s">
-        <v>25</v>
+        <v>57</v>
       </c>
       <c r="F150" s="1" t="s">
         <v>69</v>
@@ -4093,13 +4097,13 @@
         <v>5</v>
       </c>
       <c r="C151" s="2" t="s">
-        <v>47</v>
+        <v>70</v>
       </c>
       <c r="D151" s="5" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="E151" s="1" t="s">
-        <v>63</v>
+        <v>80</v>
       </c>
       <c r="F151" s="1" t="s">
         <v>69</v>
@@ -4113,13 +4117,13 @@
         <v>5</v>
       </c>
       <c r="C152" s="2" t="s">
-        <v>70</v>
+        <v>5</v>
       </c>
       <c r="D152" s="5" t="s">
-        <v>26</v>
+        <v>40</v>
       </c>
       <c r="E152" s="1" t="s">
-        <v>87</v>
+        <v>39</v>
       </c>
       <c r="F152" s="1" t="s">
         <v>69</v>
@@ -4133,13 +4137,13 @@
         <v>5</v>
       </c>
       <c r="C153" s="2" t="s">
-        <v>5</v>
+        <v>47</v>
       </c>
       <c r="D153" s="5" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="E153" s="1" t="s">
-        <v>44</v>
+        <v>58</v>
       </c>
       <c r="F153" s="1" t="s">
         <v>69</v>
@@ -4153,13 +4157,13 @@
         <v>5</v>
       </c>
       <c r="C154" s="2" t="s">
-        <v>47</v>
+        <v>70</v>
       </c>
       <c r="D154" s="5" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="E154" s="1" t="s">
-        <v>65</v>
+        <v>82</v>
       </c>
       <c r="F154" s="1" t="s">
         <v>69</v>
@@ -4173,13 +4177,13 @@
         <v>5</v>
       </c>
       <c r="C155" s="2" t="s">
-        <v>70</v>
+        <v>5</v>
       </c>
       <c r="D155" s="5" t="s">
-        <v>31</v>
+        <v>18</v>
       </c>
       <c r="E155" s="1" t="s">
-        <v>88</v>
+        <v>17</v>
       </c>
       <c r="F155" s="1" t="s">
         <v>69</v>
@@ -4193,13 +4197,13 @@
         <v>5</v>
       </c>
       <c r="C156" s="2" t="s">
-        <v>5</v>
+        <v>47</v>
       </c>
       <c r="D156" s="5" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="E156" s="1" t="s">
-        <v>6</v>
+        <v>59</v>
       </c>
       <c r="F156" s="1" t="s">
         <v>69</v>
@@ -4213,13 +4217,13 @@
         <v>5</v>
       </c>
       <c r="C157" s="2" t="s">
-        <v>47</v>
+        <v>70</v>
       </c>
       <c r="D157" s="5" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="E157" s="1" t="s">
-        <v>66</v>
+        <v>81</v>
       </c>
       <c r="F157" s="1" t="s">
         <v>69</v>
@@ -4233,13 +4237,13 @@
         <v>5</v>
       </c>
       <c r="C158" s="2" t="s">
-        <v>70</v>
+        <v>5</v>
       </c>
       <c r="D158" s="5" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="E158" s="1" t="s">
-        <v>89</v>
+        <v>19</v>
       </c>
       <c r="F158" s="1" t="s">
         <v>69</v>
@@ -4253,13 +4257,13 @@
         <v>5</v>
       </c>
       <c r="C159" s="2" t="s">
-        <v>5</v>
+        <v>47</v>
       </c>
       <c r="D159" s="5" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="E159" s="1" t="s">
-        <v>8</v>
+        <v>60</v>
       </c>
       <c r="F159" s="1" t="s">
         <v>69</v>
@@ -4273,13 +4277,13 @@
         <v>5</v>
       </c>
       <c r="C160" s="2" t="s">
-        <v>47</v>
+        <v>70</v>
       </c>
       <c r="D160" s="5" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="E160" s="1" t="s">
-        <v>67</v>
+        <v>83</v>
       </c>
       <c r="F160" s="1" t="s">
         <v>69</v>
@@ -4293,21 +4297,421 @@
         <v>5</v>
       </c>
       <c r="C161" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D161" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E161" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F161" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="162" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A162" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B162" s="2">
+        <v>5</v>
+      </c>
+      <c r="C162" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D162" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E162" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="F162" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="163" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A163" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B163" s="2">
+        <v>5</v>
+      </c>
+      <c r="C163" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="D161" s="5" t="s">
+      <c r="D163" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E163" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="F163" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="164" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A164" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B164" s="2">
+        <v>5</v>
+      </c>
+      <c r="C164" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D164" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="E164" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F164" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="165" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A165" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B165" s="2">
+        <v>5</v>
+      </c>
+      <c r="C165" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D165" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="E165" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="F165" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="166" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A166" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B166" s="2">
+        <v>5</v>
+      </c>
+      <c r="C166" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D166" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="E166" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="F166" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="167" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A167" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B167" s="2">
+        <v>5</v>
+      </c>
+      <c r="C167" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D167" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E167" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F167" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="168" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A168" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B168" s="2">
+        <v>5</v>
+      </c>
+      <c r="C168" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D168" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E168" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="F168" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="169" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A169" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B169" s="2">
+        <v>5</v>
+      </c>
+      <c r="C169" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D169" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E169" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="F169" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="170" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A170" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B170" s="2">
+        <v>5</v>
+      </c>
+      <c r="C170" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D170" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E170" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F170" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="171" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A171" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B171" s="2">
+        <v>5</v>
+      </c>
+      <c r="C171" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D171" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E171" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="F171" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="172" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A172" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B172" s="2">
+        <v>5</v>
+      </c>
+      <c r="C172" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D172" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E172" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="F172" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="173" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A173" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B173" s="2">
+        <v>5</v>
+      </c>
+      <c r="C173" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D173" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="E173" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F173" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="174" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A174" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B174" s="2">
+        <v>5</v>
+      </c>
+      <c r="C174" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D174" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="E174" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="F174" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="175" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A175" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B175" s="2">
+        <v>5</v>
+      </c>
+      <c r="C175" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D175" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="E175" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="F175" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="176" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A176" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B176" s="2">
+        <v>5</v>
+      </c>
+      <c r="C176" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D176" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E176" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F176" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="177" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A177" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B177" s="2">
+        <v>5</v>
+      </c>
+      <c r="C177" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D177" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E177" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F177" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="178" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A178" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B178" s="2">
+        <v>5</v>
+      </c>
+      <c r="C178" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D178" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E178" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="F178" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="179" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A179" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B179" s="2">
+        <v>5</v>
+      </c>
+      <c r="C179" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D179" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="E161" s="1" t="s">
+      <c r="E179" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F179" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="180" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A180" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B180" s="2">
+        <v>5</v>
+      </c>
+      <c r="C180" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D180" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E180" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F180" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="181" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A181" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B181" s="2">
+        <v>5</v>
+      </c>
+      <c r="C181" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D181" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E181" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="F161" s="1" t="s">
+      <c r="F181" s="1" t="s">
         <v>69</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A102:E141">
-    <sortCondition ref="D104:D141"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A122:E161">
+    <sortCondition ref="D124:D161"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Add US related to Cardiology domain
</commit_message>
<xml_diff>
--- a/refair-server/datasets/few shot dataset/FSDataset.xlsx
+++ b/refair-server/datasets/few shot dataset/FSDataset.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\morel\Desktop\Refair\ReFair-App\refair-server\datasets\few shot dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C520E58-8C61-420B-AF27-501CF1917991}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A4005DB-21BB-4043-BDFB-AD864B8A211B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{80773445-FB61-4F04-A882-1600FD96C55A}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="886" uniqueCount="220">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="986" uniqueCount="242">
   <si>
     <t>Domain cluster</t>
   </si>
@@ -696,6 +696,72 @@
   </si>
   <si>
     <t>As an economist, I want to use word embedding techniques to analyze customer feedback and reviews on economic products and services, extracting underlying sentiments and preferences to guide product development and market positioning strategies.</t>
+  </si>
+  <si>
+    <t>Medicine &amp; Health</t>
+  </si>
+  <si>
+    <t>Cardiology</t>
+  </si>
+  <si>
+    <t>As a cardiologist, I want to apply adversarial learning techniques to detect and mitigate potential adversarial attacks on ECG data classifiers, ensuring the reliability and robustness of heart abnormality diagnoses.</t>
+  </si>
+  <si>
+    <t>As a cardiologist, I want to explore CNN-based techniques for real-time analysis of wearable device data, such as continuous heart rate monitoring, to detect anomalies and provide timely alerts for patients with underlying cardiac conditions.</t>
+  </si>
+  <si>
+    <t>As a cardiologist, I want to integrate a conversational agent into electronic health records (EHR) systems, enabling patients to easily access and update their medical histories and symptoms, facilitating more efficient and accurate clinical assessments.</t>
+  </si>
+  <si>
+    <t>As a cardiologist, I want to construct decision tree models using patient demographics and medical history to predict the likelihood of adverse cardiac events within the next five years, aiding in early intervention and risk management strategies.</t>
+  </si>
+  <si>
+    <t>As a cardiologist, I want to develop a document classification system to classify electronic health records (EHRs) based on patient symptoms and diagnostic tests, aiding in the identification of patterns and trends in cardiovascular diseases.</t>
+  </si>
+  <si>
+    <t>As a cardiologist, I want to develop an entity extraction system to automatically identify and extract key cardiac parameters (e.g., ejection fraction, QT interval) from clinical notes and reports, enabling faster analysis and decision-making.</t>
+  </si>
+  <si>
+    <t>As a cardiologist, I want to apply feature selection methods to filter out irrelevant or redundant features from ECG data, so that I can enhance the performance of algorithms detecting cardiac arrhythmias.</t>
+  </si>
+  <si>
+    <t>As a cardiologist, I want to use keyword extraction algorithms to extract relevant terms from medical literature and clinical guidelines pertaining to cardiac rehabilitation protocols, aiding in the development of evidence-based treatment plans.</t>
+  </si>
+  <si>
+    <t>As a cardiologist, I want to address class imbalance in datasets used for predicting rare cardiac conditions using machine learning algorithms, ensuring accurate identification and early intervention for patients at higher risk.</t>
+  </si>
+  <si>
+    <t>As a cardiologist, I want to use k-NN models to predict patient-specific responses to different cardiac medications based on similar patient profiles, facilitating personalized treatment plans for heart disease management.</t>
+  </si>
+  <si>
+    <t>As a cardiologist, I want to implement multi-label classification algorithms to classify cardiac imaging studies (e.g., echocardiograms, CT scans) into multiple diagnostic categories (e.g., valve disease, myocardial infarction), aiding in accurate disease characterization.</t>
+  </si>
+  <si>
+    <t>As a cardiologist, I want to develop a neural network-based system to predict the progression of heart failure in patients based on dynamic changes in biomarkers and clinical indicators, guiding timely interventions and patient monitoring.</t>
+  </si>
+  <si>
+    <t>As a cardiologist, I want to deploy a random forest model to predict the likelihood of adverse drug reactions in cardiac patients based on medication history, comorbidities, and genetic predispositions, optimizing medication management strategies.</t>
+  </si>
+  <si>
+    <t>As a cardiologist, I want to develop a semantic similarity model to compare clinical notes and identify similar cases of coronary artery disease, aiding in pattern recognition and treatment planning.</t>
+  </si>
+  <si>
+    <t>As a cardiologist, I want to implement sentiment analysis on patient feedback from cardiac rehabilitation programs to assess overall patient satisfaction and identify areas for program improvement.</t>
+  </si>
+  <si>
+    <t>As a cardiologist, I want to develop a speech to text system to transcribe cardiology consultations and patient histories accurately, improving documentation efficiency and clinical workflow.</t>
+  </si>
+  <si>
+    <t>As a cardiologist, I want to develop a text categorization model to classify medical literature and research articles on various cardiac conditions (e.g., myocardial infarction, arrhythmias) for easier access and knowledge synthesis.</t>
+  </si>
+  <si>
+    <t>As a cardiologist, I want to apply unsupervised clustering algorithms to group patients based on similar risk factor profiles (e.g., smoking history, cholesterol levels), enabling targeted preventive interventions for cardiovascular diseases.</t>
+  </si>
+  <si>
+    <t>As a cardiologist, I want to develop a voice recognition system to accurately transcribe cardiology consultations and patient histories from audio recordings, improving documentation accuracy and efficiency.</t>
+  </si>
+  <si>
+    <t>As a cardiologist, I want to utilize word embedding techniques to represent clinical terms and medical concepts from cardiology literature, enabling more accurate semantic understanding and retrieval of relevant research findings.</t>
   </si>
 </sst>
 </file>
@@ -735,7 +801,7 @@
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -766,6 +832,12 @@
         <bgColor rgb="FFFFFF00"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF6D9EEB"/>
+        <bgColor rgb="FF6D9EEB"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -779,7 +851,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -800,6 +872,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -1134,10 +1207,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8DF0B04-8323-4309-B759-D1CDDA1FBB0E}">
-  <dimension ref="A1:F181"/>
+  <dimension ref="A1:F201"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" topLeftCell="A175" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D199" sqref="D199"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1169,7 +1242,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="2" spans="1:6" s="3" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
         <v>177</v>
       </c>
@@ -1182,11 +1255,11 @@
       <c r="D2" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="1" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="3" spans="1:6" s="3" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
         <v>177</v>
       </c>
@@ -1199,11 +1272,11 @@
       <c r="D3" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="1" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="4" spans="1:6" s="3" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
         <v>177</v>
       </c>
@@ -1216,11 +1289,11 @@
       <c r="D4" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="1" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="5" spans="1:6" s="3" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
         <v>177</v>
       </c>
@@ -1233,11 +1306,11 @@
       <c r="D5" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="1" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="6" spans="1:6" s="3" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
         <v>177</v>
       </c>
@@ -1250,11 +1323,11 @@
       <c r="D6" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="1" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="7" spans="1:6" s="3" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
         <v>177</v>
       </c>
@@ -1267,11 +1340,11 @@
       <c r="D7" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7" s="1" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="8" spans="1:6" s="3" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="10" t="s">
         <v>177</v>
       </c>
@@ -1284,11 +1357,11 @@
       <c r="D8" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8" s="1" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="9" spans="1:6" s="3" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="10" t="s">
         <v>177</v>
       </c>
@@ -1301,11 +1374,11 @@
       <c r="D9" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9" s="1" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="10" spans="1:6" s="3" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="10" t="s">
         <v>177</v>
       </c>
@@ -1318,11 +1391,11 @@
       <c r="D10" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E10" s="1" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="11" spans="1:6" s="3" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="10" t="s">
         <v>177</v>
       </c>
@@ -1335,11 +1408,11 @@
       <c r="D11" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E11" s="1" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="12" spans="1:6" s="3" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
         <v>177</v>
       </c>
@@ -1352,11 +1425,11 @@
       <c r="D12" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E12" s="1" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="13" spans="1:6" s="3" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="10" t="s">
         <v>177</v>
       </c>
@@ -1369,11 +1442,11 @@
       <c r="D13" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E13" s="1" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="14" spans="1:6" s="3" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="10" t="s">
         <v>177</v>
       </c>
@@ -1386,11 +1459,11 @@
       <c r="D14" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="E14" t="s">
+      <c r="E14" s="1" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="15" spans="1:6" s="3" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="10" t="s">
         <v>177</v>
       </c>
@@ -1403,11 +1476,11 @@
       <c r="D15" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="E15" t="s">
+      <c r="E15" s="1" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="16" spans="1:6" s="3" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="10" t="s">
         <v>177</v>
       </c>
@@ -1420,11 +1493,11 @@
       <c r="D16" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="E16" t="s">
+      <c r="E16" s="1" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="17" spans="1:6" s="3" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="10" t="s">
         <v>177</v>
       </c>
@@ -1437,11 +1510,11 @@
       <c r="D17" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="E17" t="s">
+      <c r="E17" s="1" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="18" spans="1:6" s="3" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="10" t="s">
         <v>177</v>
       </c>
@@ -1454,11 +1527,11 @@
       <c r="D18" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="E18" t="s">
+      <c r="E18" s="1" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="19" spans="1:6" s="3" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="10" t="s">
         <v>177</v>
       </c>
@@ -1471,11 +1544,11 @@
       <c r="D19" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="E19" t="s">
+      <c r="E19" s="1" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="20" spans="1:6" s="3" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="10" t="s">
         <v>177</v>
       </c>
@@ -1488,11 +1561,11 @@
       <c r="D20" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="E20" t="s">
+      <c r="E20" s="1" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="21" spans="1:6" s="3" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="10" t="s">
         <v>177</v>
       </c>
@@ -1505,11 +1578,11 @@
       <c r="D21" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="E21" t="s">
+      <c r="E21" s="1" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="22" spans="1:6" s="3" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="10" t="s">
         <v>177</v>
       </c>
@@ -1522,14 +1595,14 @@
       <c r="D22" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="E22" t="s">
+      <c r="E22" s="1" t="s">
         <v>189</v>
       </c>
       <c r="F22" s="1" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="23" spans="1:6" s="3" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="10" t="s">
         <v>177</v>
       </c>
@@ -1542,14 +1615,14 @@
       <c r="D23" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="E23" t="s">
+      <c r="E23" s="1" t="s">
         <v>210</v>
       </c>
       <c r="F23" s="1" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="24" spans="1:6" s="3" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="10" t="s">
         <v>177</v>
       </c>
@@ -1562,14 +1635,14 @@
       <c r="D24" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="E24" t="s">
+      <c r="E24" s="1" t="s">
         <v>190</v>
       </c>
       <c r="F24" s="1" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="25" spans="1:6" s="3" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="10" t="s">
         <v>177</v>
       </c>
@@ -1582,14 +1655,14 @@
       <c r="D25" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="E25" t="s">
+      <c r="E25" s="1" t="s">
         <v>211</v>
       </c>
       <c r="F25" s="1" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="26" spans="1:6" s="3" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="10" t="s">
         <v>177</v>
       </c>
@@ -1602,14 +1675,14 @@
       <c r="D26" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="E26" t="s">
+      <c r="E26" s="1" t="s">
         <v>191</v>
       </c>
       <c r="F26" s="1" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="27" spans="1:6" s="3" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="10" t="s">
         <v>177</v>
       </c>
@@ -1622,14 +1695,14 @@
       <c r="D27" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="E27" t="s">
+      <c r="E27" s="1" t="s">
         <v>212</v>
       </c>
       <c r="F27" s="1" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="28" spans="1:6" s="3" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="10" t="s">
         <v>177</v>
       </c>
@@ -1642,14 +1715,14 @@
       <c r="D28" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="E28" t="s">
+      <c r="E28" s="1" t="s">
         <v>192</v>
       </c>
       <c r="F28" s="1" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="29" spans="1:6" s="3" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="10" t="s">
         <v>177</v>
       </c>
@@ -1662,14 +1735,14 @@
       <c r="D29" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="E29" t="s">
+      <c r="E29" s="1" t="s">
         <v>213</v>
       </c>
       <c r="F29" s="1" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="30" spans="1:6" s="3" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="10" t="s">
         <v>177</v>
       </c>
@@ -1682,14 +1755,14 @@
       <c r="D30" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="E30" t="s">
+      <c r="E30" s="1" t="s">
         <v>193</v>
       </c>
       <c r="F30" s="1" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="31" spans="1:6" s="3" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="10" t="s">
         <v>177</v>
       </c>
@@ -1702,14 +1775,14 @@
       <c r="D31" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="E31" t="s">
+      <c r="E31" s="1" t="s">
         <v>214</v>
       </c>
       <c r="F31" s="1" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="32" spans="1:6" s="3" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="10" t="s">
         <v>177</v>
       </c>
@@ -1722,14 +1795,14 @@
       <c r="D32" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="E32" t="s">
+      <c r="E32" s="1" t="s">
         <v>194</v>
       </c>
       <c r="F32" s="1" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="33" spans="1:6" s="3" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="10" t="s">
         <v>177</v>
       </c>
@@ -1742,14 +1815,14 @@
       <c r="D33" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="E33" t="s">
+      <c r="E33" s="1" t="s">
         <v>215</v>
       </c>
       <c r="F33" s="1" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="34" spans="1:6" s="3" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="10" t="s">
         <v>177</v>
       </c>
@@ -1762,14 +1835,14 @@
       <c r="D34" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="E34" t="s">
+      <c r="E34" s="1" t="s">
         <v>195</v>
       </c>
       <c r="F34" s="1" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="35" spans="1:6" s="3" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="10" t="s">
         <v>177</v>
       </c>
@@ -1782,14 +1855,14 @@
       <c r="D35" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="E35" t="s">
+      <c r="E35" s="1" t="s">
         <v>216</v>
       </c>
       <c r="F35" s="1" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="36" spans="1:6" s="3" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="10" t="s">
         <v>177</v>
       </c>
@@ -1802,14 +1875,14 @@
       <c r="D36" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="E36" t="s">
+      <c r="E36" s="1" t="s">
         <v>196</v>
       </c>
       <c r="F36" s="1" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="37" spans="1:6" s="3" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="10" t="s">
         <v>177</v>
       </c>
@@ -1822,14 +1895,14 @@
       <c r="D37" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="E37" t="s">
+      <c r="E37" s="1" t="s">
         <v>217</v>
       </c>
       <c r="F37" s="1" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="38" spans="1:6" s="3" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="10" t="s">
         <v>177</v>
       </c>
@@ -1842,14 +1915,14 @@
       <c r="D38" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="E38" t="s">
+      <c r="E38" s="1" t="s">
         <v>197</v>
       </c>
       <c r="F38" s="1" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="39" spans="1:6" s="3" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="10" t="s">
         <v>177</v>
       </c>
@@ -1862,14 +1935,14 @@
       <c r="D39" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="E39" t="s">
+      <c r="E39" s="1" t="s">
         <v>218</v>
       </c>
       <c r="F39" s="1" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="40" spans="1:6" s="3" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="10" t="s">
         <v>177</v>
       </c>
@@ -1882,14 +1955,14 @@
       <c r="D40" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="E40" t="s">
+      <c r="E40" s="1" t="s">
         <v>198</v>
       </c>
       <c r="F40" s="1" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="41" spans="1:6" s="3" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="10" t="s">
         <v>177</v>
       </c>
@@ -1902,7 +1975,7 @@
       <c r="D41" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="E41" t="s">
+      <c r="E41" s="1" t="s">
         <v>219</v>
       </c>
       <c r="F41" s="1" t="s">
@@ -4706,6 +4779,406 @@
         <v>90</v>
       </c>
       <c r="F181" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="182" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A182" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="B182" s="12">
+        <v>6</v>
+      </c>
+      <c r="C182" s="12" t="s">
+        <v>221</v>
+      </c>
+      <c r="D182" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="E182" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="F182" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="183" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A183" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="B183" s="12">
+        <v>6</v>
+      </c>
+      <c r="C183" s="12" t="s">
+        <v>221</v>
+      </c>
+      <c r="D183" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="E183" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="F183" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="184" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A184" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="B184" s="12">
+        <v>6</v>
+      </c>
+      <c r="C184" s="12" t="s">
+        <v>221</v>
+      </c>
+      <c r="D184" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="E184" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="F184" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="185" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A185" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="B185" s="12">
+        <v>6</v>
+      </c>
+      <c r="C185" s="12" t="s">
+        <v>221</v>
+      </c>
+      <c r="D185" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="E185" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="F185" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="186" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A186" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="B186" s="12">
+        <v>6</v>
+      </c>
+      <c r="C186" s="12" t="s">
+        <v>221</v>
+      </c>
+      <c r="D186" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="E186" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="F186" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="187" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A187" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="B187" s="12">
+        <v>6</v>
+      </c>
+      <c r="C187" s="12" t="s">
+        <v>221</v>
+      </c>
+      <c r="D187" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="E187" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="F187" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="188" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A188" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="B188" s="12">
+        <v>6</v>
+      </c>
+      <c r="C188" s="12" t="s">
+        <v>221</v>
+      </c>
+      <c r="D188" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="E188" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="F188" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="189" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A189" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="B189" s="12">
+        <v>6</v>
+      </c>
+      <c r="C189" s="12" t="s">
+        <v>221</v>
+      </c>
+      <c r="D189" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="E189" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="F189" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="190" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A190" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="B190" s="12">
+        <v>6</v>
+      </c>
+      <c r="C190" s="12" t="s">
+        <v>221</v>
+      </c>
+      <c r="D190" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="E190" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="F190" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="191" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A191" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="B191" s="12">
+        <v>6</v>
+      </c>
+      <c r="C191" s="12" t="s">
+        <v>221</v>
+      </c>
+      <c r="D191" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="E191" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="F191" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="192" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A192" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="B192" s="12">
+        <v>6</v>
+      </c>
+      <c r="C192" s="12" t="s">
+        <v>221</v>
+      </c>
+      <c r="D192" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="E192" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="F192" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="193" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A193" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="B193" s="12">
+        <v>6</v>
+      </c>
+      <c r="C193" s="12" t="s">
+        <v>221</v>
+      </c>
+      <c r="D193" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="E193" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="F193" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="194" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A194" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="B194" s="12">
+        <v>6</v>
+      </c>
+      <c r="C194" s="12" t="s">
+        <v>221</v>
+      </c>
+      <c r="D194" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="E194" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="F194" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="195" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A195" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="B195" s="12">
+        <v>6</v>
+      </c>
+      <c r="C195" s="12" t="s">
+        <v>221</v>
+      </c>
+      <c r="D195" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="E195" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="F195" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="196" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A196" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="B196" s="12">
+        <v>6</v>
+      </c>
+      <c r="C196" s="12" t="s">
+        <v>221</v>
+      </c>
+      <c r="D196" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="E196" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="F196" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="197" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A197" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="B197" s="12">
+        <v>6</v>
+      </c>
+      <c r="C197" s="12" t="s">
+        <v>221</v>
+      </c>
+      <c r="D197" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="E197" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="F197" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="198" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A198" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="B198" s="12">
+        <v>6</v>
+      </c>
+      <c r="C198" s="12" t="s">
+        <v>221</v>
+      </c>
+      <c r="D198" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="E198" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="F198" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="199" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A199" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="B199" s="12">
+        <v>6</v>
+      </c>
+      <c r="C199" s="12" t="s">
+        <v>221</v>
+      </c>
+      <c r="D199" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="E199" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="F199" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="200" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A200" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="B200" s="12">
+        <v>6</v>
+      </c>
+      <c r="C200" s="12" t="s">
+        <v>221</v>
+      </c>
+      <c r="D200" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="E200" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="F200" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="201" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A201" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="B201" s="12">
+        <v>6</v>
+      </c>
+      <c r="C201" s="12" t="s">
+        <v>221</v>
+      </c>
+      <c r="D201" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E201" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="F201" s="1" t="s">
         <v>69</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add US related to Dermatology domain
</commit_message>
<xml_diff>
--- a/refair-server/datasets/few shot dataset/FSDataset.xlsx
+++ b/refair-server/datasets/few shot dataset/FSDataset.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\morel\Desktop\Refair\ReFair-App\refair-server\datasets\few shot dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A4005DB-21BB-4043-BDFB-AD864B8A211B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FD81A2F-5595-45D7-8363-5DAC2B77152C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{80773445-FB61-4F04-A882-1600FD96C55A}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="986" uniqueCount="242">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1086" uniqueCount="263">
   <si>
     <t>Domain cluster</t>
   </si>
@@ -762,6 +762,69 @@
   </si>
   <si>
     <t>As a cardiologist, I want to utilize word embedding techniques to represent clinical terms and medical concepts from cardiology literature, enabling more accurate semantic understanding and retrieval of relevant research findings.</t>
+  </si>
+  <si>
+    <t>Dermatology</t>
+  </si>
+  <si>
+    <t>As a dermatologist, I want to apply adversarial learning techniques to detect and mitigate potential attacks on dermatological image recognition models, ensuring robustness and reliability in automated diagnosis systems.</t>
+  </si>
+  <si>
+    <t>As a dermatologist, I want to train a CNN model on a large dataset of dermatological images to accurately classify skin lesions into different diagnostic categories, improving diagnostic precision and reducing misdiagnosis rates.</t>
+  </si>
+  <si>
+    <t>As a dermatologist, I want to implement a conversational agent that can provide personalized skincare recommendations based on patient preferences, skin type, and specific dermatological concerns.</t>
+  </si>
+  <si>
+    <t>As a dermatologist, I want to utilize decision tree analysis to identify key risk factors for developing common dermatological conditions such as acne or eczema, enabling proactive preventive measures and patient education.</t>
+  </si>
+  <si>
+    <t>As a dermatologist, I want to develop a document classification model to automatically categorize research papers and clinical studies related to dermatological diseases, facilitating easier access to relevant literature for evidence-based practice.</t>
+  </si>
+  <si>
+    <t>As a dermatologist, I want to develop an entity extraction system to automatically identify and extract key information from dermatological patient records, such as symptoms, diagnoses, and treatment histories, to assist in comprehensive patient management.</t>
+  </si>
+  <si>
+    <t>As a dermatologist, I want to perform feature selection on dermatological image data to identify the most discriminative features that contribute to accurate classification of skin lesions, enhancing diagnostic precision.</t>
+  </si>
+  <si>
+    <t>As a dermatologist, I want to address class imbalance in dermatological datasets when developing AI models to detect rare skin conditions with limited training examples, ensuring robust and reliable diagnostic capabilities.</t>
+  </si>
+  <si>
+    <t>As a dermatologist, I want to develop a keyword extraction system to automatically identify and prioritize key terms from dermatological patient notes and reports, aiding in efficient data summarization and retrieval.</t>
+  </si>
+  <si>
+    <t>As a dermatologist, I want to implement a k-Nearest Neighbor algorithm to classify skin lesions based on their visual similarities to known dermatological conditions, aiding in accurate and rapid diagnosis.</t>
+  </si>
+  <si>
+    <t>As a dermatologist, I want to implement multi-label classification techniques to categorize skin lesions into multiple diagnostic categories (e.g., benign, malignant, inflammatory) based on clinical features and histopathological findings.</t>
+  </si>
+  <si>
+    <t>As a dermatologist, I want to train a neural network to analyze dermatological images and classify skin lesions with high accuracy, supporting early detection and treatment of melanoma and other malignancies.</t>
+  </si>
+  <si>
+    <t>As a dermatologist, I want to develop a random forest model to classify dermatological images into different diagnostic categories (e.g., melanoma, basal cell carcinoma) with high accuracy, aiding in early detection and treatment planning.</t>
+  </si>
+  <si>
+    <t>As a dermatologist, I want to implement semantic similarity algorithms to analyze dermatological research papers and identify relevant studies based on shared concepts and findings, facilitating literature review and evidence synthesis.</t>
+  </si>
+  <si>
+    <t>As a dermatologist, I want to develop a sentiment analysis model to analyze social media posts and reviews related to skincare products, identifying sentiments and trends among consumers to inform product recommendations.</t>
+  </si>
+  <si>
+    <t>As a dermatologist, I want to develop a speech-to-text system to transcribe verbal descriptions of skin conditions provided by patients during consultations, facilitating accurate documentation and diagnosis.</t>
+  </si>
+  <si>
+    <t>As a dermatologist, I want to develop a text categorization model to classify dermatological research articles into specific topics (e.g., melanoma, acne treatments) to facilitate literature review and evidence synthesis.</t>
+  </si>
+  <si>
+    <t>As a dermatologist, I want to apply unsupervised clustering algorithms to group dermatological patient profiles based on similar symptoms and disease progression patterns, enabling personalized treatment plans for patient clusters.</t>
+  </si>
+  <si>
+    <t>As a dermatologist, I want to implement voice recognition technology to capture patient-reported symptoms and medical histories accurately during dermatological consultations, enhancing data quality and clinical decision-making.</t>
+  </si>
+  <si>
+    <t>As a dermatologist, I want to develop word embedding models to capture semantic relationships between dermatological terms (e.g., skin conditions, treatment modalities) from medical literature, enhancing knowledge discovery and research.</t>
   </si>
 </sst>
 </file>
@@ -799,6 +862,7 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="7">
@@ -872,7 +936,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -1207,10 +1271,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8DF0B04-8323-4309-B759-D1CDDA1FBB0E}">
-  <dimension ref="A1:F201"/>
+  <dimension ref="A1:F221"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A175" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D199" sqref="D199"/>
+    <sheetView tabSelected="1" topLeftCell="A200" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H219" sqref="H219"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -4782,7 +4846,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="182" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A182" s="12" t="s">
         <v>220</v>
       </c>
@@ -4795,14 +4859,14 @@
       <c r="D182" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="E182" s="1" t="s">
+      <c r="E182" t="s">
         <v>222</v>
       </c>
       <c r="F182" s="1" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="183" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A183" s="12" t="s">
         <v>220</v>
       </c>
@@ -4810,19 +4874,19 @@
         <v>6</v>
       </c>
       <c r="C183" s="12" t="s">
-        <v>221</v>
+        <v>242</v>
       </c>
       <c r="D183" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="E183" s="1" t="s">
-        <v>223</v>
+        <v>28</v>
+      </c>
+      <c r="E183" t="s">
+        <v>243</v>
       </c>
       <c r="F183" s="1" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="184" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A184" s="12" t="s">
         <v>220</v>
       </c>
@@ -4833,16 +4897,16 @@
         <v>221</v>
       </c>
       <c r="D184" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="E184" s="1" t="s">
-        <v>224</v>
+        <v>43</v>
+      </c>
+      <c r="E184" t="s">
+        <v>223</v>
       </c>
       <c r="F184" s="1" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="185" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A185" s="12" t="s">
         <v>220</v>
       </c>
@@ -4850,19 +4914,19 @@
         <v>6</v>
       </c>
       <c r="C185" s="12" t="s">
-        <v>221</v>
+        <v>242</v>
       </c>
       <c r="D185" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="E185" s="1" t="s">
-        <v>225</v>
+        <v>43</v>
+      </c>
+      <c r="E185" t="s">
+        <v>244</v>
       </c>
       <c r="F185" s="1" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="186" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A186" s="12" t="s">
         <v>220</v>
       </c>
@@ -4873,16 +4937,16 @@
         <v>221</v>
       </c>
       <c r="D186" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="E186" s="1" t="s">
-        <v>226</v>
+        <v>30</v>
+      </c>
+      <c r="E186" t="s">
+        <v>224</v>
       </c>
       <c r="F186" s="1" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="187" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A187" s="12" t="s">
         <v>220</v>
       </c>
@@ -4890,19 +4954,19 @@
         <v>6</v>
       </c>
       <c r="C187" s="12" t="s">
-        <v>221</v>
+        <v>242</v>
       </c>
       <c r="D187" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="E187" s="1" t="s">
-        <v>227</v>
+        <v>30</v>
+      </c>
+      <c r="E187" t="s">
+        <v>245</v>
       </c>
       <c r="F187" s="1" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="188" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A188" s="12" t="s">
         <v>220</v>
       </c>
@@ -4913,16 +4977,16 @@
         <v>221</v>
       </c>
       <c r="D188" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="E188" s="1" t="s">
-        <v>228</v>
+        <v>13</v>
+      </c>
+      <c r="E188" t="s">
+        <v>225</v>
       </c>
       <c r="F188" s="1" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="189" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A189" s="12" t="s">
         <v>220</v>
       </c>
@@ -4930,19 +4994,19 @@
         <v>6</v>
       </c>
       <c r="C189" s="12" t="s">
-        <v>221</v>
+        <v>242</v>
       </c>
       <c r="D189" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="E189" s="1" t="s">
-        <v>229</v>
+        <v>13</v>
+      </c>
+      <c r="E189" t="s">
+        <v>246</v>
       </c>
       <c r="F189" s="1" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="190" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A190" s="12" t="s">
         <v>220</v>
       </c>
@@ -4953,16 +5017,16 @@
         <v>221</v>
       </c>
       <c r="D190" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="E190" s="1" t="s">
-        <v>230</v>
+        <v>46</v>
+      </c>
+      <c r="E190" t="s">
+        <v>226</v>
       </c>
       <c r="F190" s="1" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="191" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A191" s="12" t="s">
         <v>220</v>
       </c>
@@ -4970,19 +5034,19 @@
         <v>6</v>
       </c>
       <c r="C191" s="12" t="s">
-        <v>221</v>
+        <v>242</v>
       </c>
       <c r="D191" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="E191" s="1" t="s">
-        <v>231</v>
+        <v>46</v>
+      </c>
+      <c r="E191" t="s">
+        <v>247</v>
       </c>
       <c r="F191" s="1" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="192" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A192" s="12" t="s">
         <v>220</v>
       </c>
@@ -4993,16 +5057,16 @@
         <v>221</v>
       </c>
       <c r="D192" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="E192" s="1" t="s">
-        <v>232</v>
+        <v>33</v>
+      </c>
+      <c r="E192" t="s">
+        <v>227</v>
       </c>
       <c r="F192" s="1" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="193" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A193" s="12" t="s">
         <v>220</v>
       </c>
@@ -5010,19 +5074,19 @@
         <v>6</v>
       </c>
       <c r="C193" s="12" t="s">
-        <v>221</v>
+        <v>242</v>
       </c>
       <c r="D193" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="E193" s="1" t="s">
-        <v>233</v>
+        <v>33</v>
+      </c>
+      <c r="E193" t="s">
+        <v>248</v>
       </c>
       <c r="F193" s="1" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="194" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A194" s="12" t="s">
         <v>220</v>
       </c>
@@ -5033,16 +5097,16 @@
         <v>221</v>
       </c>
       <c r="D194" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="E194" s="1" t="s">
-        <v>234</v>
+        <v>36</v>
+      </c>
+      <c r="E194" t="s">
+        <v>228</v>
       </c>
       <c r="F194" s="1" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="195" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A195" s="12" t="s">
         <v>220</v>
       </c>
@@ -5050,19 +5114,19 @@
         <v>6</v>
       </c>
       <c r="C195" s="12" t="s">
-        <v>221</v>
+        <v>242</v>
       </c>
       <c r="D195" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="E195" s="1" t="s">
-        <v>235</v>
+        <v>36</v>
+      </c>
+      <c r="E195" t="s">
+        <v>249</v>
       </c>
       <c r="F195" s="1" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="196" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A196" s="12" t="s">
         <v>220</v>
       </c>
@@ -5073,16 +5137,16 @@
         <v>221</v>
       </c>
       <c r="D196" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="E196" s="1" t="s">
-        <v>236</v>
+        <v>14</v>
+      </c>
+      <c r="E196" t="s">
+        <v>229</v>
       </c>
       <c r="F196" s="1" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="197" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A197" s="12" t="s">
         <v>220</v>
       </c>
@@ -5090,19 +5154,19 @@
         <v>6</v>
       </c>
       <c r="C197" s="12" t="s">
-        <v>221</v>
+        <v>242</v>
       </c>
       <c r="D197" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="E197" s="1" t="s">
-        <v>237</v>
+        <v>14</v>
+      </c>
+      <c r="E197" t="s">
+        <v>250</v>
       </c>
       <c r="F197" s="1" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="198" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A198" s="12" t="s">
         <v>220</v>
       </c>
@@ -5113,16 +5177,16 @@
         <v>221</v>
       </c>
       <c r="D198" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="E198" s="1" t="s">
-        <v>238</v>
+        <v>34</v>
+      </c>
+      <c r="E198" t="s">
+        <v>230</v>
       </c>
       <c r="F198" s="1" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="199" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A199" s="12" t="s">
         <v>220</v>
       </c>
@@ -5130,19 +5194,19 @@
         <v>6</v>
       </c>
       <c r="C199" s="12" t="s">
-        <v>221</v>
+        <v>242</v>
       </c>
       <c r="D199" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="E199" s="1" t="s">
-        <v>239</v>
+        <v>34</v>
+      </c>
+      <c r="E199" t="s">
+        <v>251</v>
       </c>
       <c r="F199" s="1" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="200" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A200" s="12" t="s">
         <v>220</v>
       </c>
@@ -5153,16 +5217,16 @@
         <v>221</v>
       </c>
       <c r="D200" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="E200" s="1" t="s">
-        <v>240</v>
+        <v>16</v>
+      </c>
+      <c r="E200" t="s">
+        <v>231</v>
       </c>
       <c r="F200" s="1" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="201" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A201" s="12" t="s">
         <v>220</v>
       </c>
@@ -5170,15 +5234,415 @@
         <v>6</v>
       </c>
       <c r="C201" s="12" t="s">
+        <v>242</v>
+      </c>
+      <c r="D201" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="E201" t="s">
+        <v>252</v>
+      </c>
+      <c r="F201" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="202" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A202" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="B202" s="12">
+        <v>6</v>
+      </c>
+      <c r="C202" s="12" t="s">
         <v>221</v>
       </c>
-      <c r="D201" s="9" t="s">
+      <c r="D202" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="E202" t="s">
+        <v>232</v>
+      </c>
+      <c r="F202" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="203" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A203" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="B203" s="12">
+        <v>6</v>
+      </c>
+      <c r="C203" s="12" t="s">
+        <v>242</v>
+      </c>
+      <c r="D203" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="E203" t="s">
+        <v>253</v>
+      </c>
+      <c r="F203" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="204" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A204" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="B204" s="12">
+        <v>6</v>
+      </c>
+      <c r="C204" s="12" t="s">
+        <v>221</v>
+      </c>
+      <c r="D204" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="E204" t="s">
+        <v>233</v>
+      </c>
+      <c r="F204" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="205" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A205" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="B205" s="12">
+        <v>6</v>
+      </c>
+      <c r="C205" s="12" t="s">
+        <v>242</v>
+      </c>
+      <c r="D205" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="E205" t="s">
+        <v>254</v>
+      </c>
+      <c r="F205" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="206" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A206" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="B206" s="12">
+        <v>6</v>
+      </c>
+      <c r="C206" s="12" t="s">
+        <v>221</v>
+      </c>
+      <c r="D206" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="E206" t="s">
+        <v>234</v>
+      </c>
+      <c r="F206" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="207" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A207" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="B207" s="12">
+        <v>6</v>
+      </c>
+      <c r="C207" s="12" t="s">
+        <v>242</v>
+      </c>
+      <c r="D207" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="E207" t="s">
+        <v>255</v>
+      </c>
+      <c r="F207" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="208" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A208" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="B208" s="12">
+        <v>6</v>
+      </c>
+      <c r="C208" s="12" t="s">
+        <v>221</v>
+      </c>
+      <c r="D208" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="E208" t="s">
+        <v>235</v>
+      </c>
+      <c r="F208" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="209" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A209" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="B209" s="12">
+        <v>6</v>
+      </c>
+      <c r="C209" s="12" t="s">
+        <v>242</v>
+      </c>
+      <c r="D209" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="E209" t="s">
+        <v>256</v>
+      </c>
+      <c r="F209" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="210" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A210" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="B210" s="12">
+        <v>6</v>
+      </c>
+      <c r="C210" s="12" t="s">
+        <v>221</v>
+      </c>
+      <c r="D210" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="E210" t="s">
+        <v>236</v>
+      </c>
+      <c r="F210" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="211" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A211" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="B211" s="12">
+        <v>6</v>
+      </c>
+      <c r="C211" s="12" t="s">
+        <v>242</v>
+      </c>
+      <c r="D211" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="E211" t="s">
+        <v>257</v>
+      </c>
+      <c r="F211" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="212" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A212" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="B212" s="12">
+        <v>6</v>
+      </c>
+      <c r="C212" s="12" t="s">
+        <v>221</v>
+      </c>
+      <c r="D212" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="E212" t="s">
+        <v>237</v>
+      </c>
+      <c r="F212" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="213" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A213" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="B213" s="12">
+        <v>6</v>
+      </c>
+      <c r="C213" s="12" t="s">
+        <v>242</v>
+      </c>
+      <c r="D213" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="E213" t="s">
+        <v>258</v>
+      </c>
+      <c r="F213" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="214" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A214" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="B214" s="12">
+        <v>6</v>
+      </c>
+      <c r="C214" s="12" t="s">
+        <v>221</v>
+      </c>
+      <c r="D214" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="E214" t="s">
+        <v>238</v>
+      </c>
+      <c r="F214" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="215" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A215" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="B215" s="12">
+        <v>6</v>
+      </c>
+      <c r="C215" s="12" t="s">
+        <v>242</v>
+      </c>
+      <c r="D215" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="E215" t="s">
+        <v>259</v>
+      </c>
+      <c r="F215" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="216" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A216" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="B216" s="12">
+        <v>6</v>
+      </c>
+      <c r="C216" s="12" t="s">
+        <v>221</v>
+      </c>
+      <c r="D216" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="E216" t="s">
+        <v>239</v>
+      </c>
+      <c r="F216" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="217" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A217" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="B217" s="12">
+        <v>6</v>
+      </c>
+      <c r="C217" s="12" t="s">
+        <v>242</v>
+      </c>
+      <c r="D217" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="E217" t="s">
+        <v>260</v>
+      </c>
+      <c r="F217" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="218" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A218" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="B218" s="12">
+        <v>6</v>
+      </c>
+      <c r="C218" s="12" t="s">
+        <v>221</v>
+      </c>
+      <c r="D218" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="E218" t="s">
+        <v>240</v>
+      </c>
+      <c r="F218" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="219" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A219" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="B219" s="12">
+        <v>6</v>
+      </c>
+      <c r="C219" s="12" t="s">
+        <v>242</v>
+      </c>
+      <c r="D219" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="E219" t="s">
+        <v>261</v>
+      </c>
+      <c r="F219" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="220" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A220" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="B220" s="12">
+        <v>6</v>
+      </c>
+      <c r="C220" s="12" t="s">
+        <v>221</v>
+      </c>
+      <c r="D220" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="E201" s="1" t="s">
+      <c r="E220" t="s">
         <v>241</v>
       </c>
-      <c r="F201" s="1" t="s">
+      <c r="F220" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="221" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A221" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="B221" s="12">
+        <v>6</v>
+      </c>
+      <c r="C221" s="12" t="s">
+        <v>242</v>
+      </c>
+      <c r="D221" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E221" t="s">
+        <v>262</v>
+      </c>
+      <c r="F221" s="1" t="s">
         <v>69</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add US related to Endocrinology domain
</commit_message>
<xml_diff>
--- a/refair-server/datasets/few shot dataset/FSDataset.xlsx
+++ b/refair-server/datasets/few shot dataset/FSDataset.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\morel\Desktop\Refair\ReFair-App\refair-server\datasets\few shot dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FD81A2F-5595-45D7-8363-5DAC2B77152C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D8EBB82-08A4-43B0-8791-1EC8CDADE1C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{80773445-FB61-4F04-A882-1600FD96C55A}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1086" uniqueCount="263">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1186" uniqueCount="284">
   <si>
     <t>Domain cluster</t>
   </si>
@@ -825,6 +825,69 @@
   </si>
   <si>
     <t>As a dermatologist, I want to develop word embedding models to capture semantic relationships between dermatological terms (e.g., skin conditions, treatment modalities) from medical literature, enhancing knowledge discovery and research.</t>
+  </si>
+  <si>
+    <t>Endocrinology</t>
+  </si>
+  <si>
+    <t>As an endocrinologist, I want to apply adversarial learning techniques to identify and mitigate potential vulnerabilities in hormone imbalance prediction models, ensuring robustness against adversarial attacks.</t>
+  </si>
+  <si>
+    <t>As an endocrinologist, I want to utilize CNN architectures to classify histopathological images of endocrine tumors, aiding in accurate diagnosis and personalized treatment planning for patients.</t>
+  </si>
+  <si>
+    <t>As an endocrinologist, I want to develop a conversational agent powered by natural language processing to interact with patients, providing personalized guidance on managing diabetes through diet and lifestyle recommendations.</t>
+  </si>
+  <si>
+    <t>As an endocrinologist, I want to use a decision tree algorithm to predict the risk of developing type 2 diabetes based on patient demographics, lifestyle factors, and genetic predispositions, enabling early intervention strategies.</t>
+  </si>
+  <si>
+    <t>As an endocrinologist, I want to develop a document classification system to automatically categorize patient medical records based on hormone profile data, streamlining the retrieval of information for treatment planning and research purposes.</t>
+  </si>
+  <si>
+    <t>As an endocrinologist, I want to implement entity extraction techniques to extract relevant hormone biomarkers from patient laboratory reports, enabling comprehensive analysis and monitoring of hormone levels over time.</t>
+  </si>
+  <si>
+    <t>As an endocrinologist, I want to use feature selection algorithms to prioritize genetic markers linked to thyroid cancer susceptibility in familial studies, facilitating targeted screening and early detection strategies.</t>
+  </si>
+  <si>
+    <t>As an endocrinologist, I want to address class imbalance in datasets related to rare endocrine disorders such as acromegaly, by applying oversampling techniques to ensure robust model training and accurate diagnosis.</t>
+  </si>
+  <si>
+    <t>As an endocrinologist, I want to develop a keyword extraction system to automatically identify relevant terms from clinical notes and research articles related to hypothyroidism, facilitating comprehensive literature review and evidence synthesis.</t>
+  </si>
+  <si>
+    <t>As an endocrinologist, I want to implement k-Nearest Neighbor (k-NN) algorithms to predict insulin resistance in diabetic patients based on similar patient profiles, facilitating personalized treatment plans and monitoring strategies.</t>
+  </si>
+  <si>
+    <t>As an endocrinologist, I want to implement multi-label classification algorithms to classify patients with adrenal gland disorders into multiple categories (e.g., Cushing's syndrome, adrenal insufficiency), facilitating accurate diagnosis and tailored management approaches.</t>
+  </si>
+  <si>
+    <t>As an endocrinologist, I want to develop a neural network model to predict the risk of gestational diabetes mellitus based on maternal health data, enabling early interventions and personalized prenatal care plans.</t>
+  </si>
+  <si>
+    <t>As an endocrinologist, I want to use random forest models to classify patients with different subtypes of diabetes (e.g., type 1, type 2, gestational) based on clinical data and genetic predispositions, guiding tailored management strategies.</t>
+  </si>
+  <si>
+    <t>As an endocrinologist, I want to use semantic similarity techniques to match patient symptoms with known disease patterns in rare endocrine disorders, supporting early detection and personalized treatment approaches.</t>
+  </si>
+  <si>
+    <t>As an endocrinologist, I want to conduct sentiment analysis on social media posts related to weight management strategies in diabetes care, understanding patient attitudes towards dietary recommendations and lifestyle changes.</t>
+  </si>
+  <si>
+    <t>As an endocrinologist, I want to use speech to text capabilities to convert endocrine conference recordings into text format, enabling easy access to discussions on recent research findings and clinical case studies.</t>
+  </si>
+  <si>
+    <t>As an endocrinologist, I want to use text categorization techniques to classify patient electronic health records based on different types of hormonal disorders (e.g., adrenal gland disorders, pituitary gland disorders), enabling efficient retrieval and analysis of relevant patient data.</t>
+  </si>
+  <si>
+    <t>As an endocrinologist, I want to use unsupervised clustering techniques to cluster symptoms reported by patients with polycystic ovary syndrome (PCOS), identifying common symptom patterns and guiding individualized management plans.</t>
+  </si>
+  <si>
+    <t>As an endocrinologist, I want to implement voice recognition technology to transcribe patient conversations during consultations about diabetes management, improving documentation accuracy and workflow efficiency.</t>
+  </si>
+  <si>
+    <t>As an endocrinologist, I want to use word embedding techniques to analyze similarities and relationships between medical terms in research literature on insulin resistance, aiding in the discovery of novel associations and mechanisms.</t>
   </si>
 </sst>
 </file>
@@ -1271,10 +1334,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8DF0B04-8323-4309-B759-D1CDDA1FBB0E}">
-  <dimension ref="A1:F221"/>
+  <dimension ref="A1:F241"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A200" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H219" sqref="H219"/>
+    <sheetView tabSelected="1" topLeftCell="A220" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F181" sqref="F181:F241"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -4894,13 +4957,13 @@
         <v>6</v>
       </c>
       <c r="C184" s="12" t="s">
-        <v>221</v>
+        <v>263</v>
       </c>
       <c r="D184" s="9" t="s">
-        <v>43</v>
+        <v>28</v>
       </c>
       <c r="E184" t="s">
-        <v>223</v>
+        <v>264</v>
       </c>
       <c r="F184" s="1" t="s">
         <v>69</v>
@@ -4914,13 +4977,13 @@
         <v>6</v>
       </c>
       <c r="C185" s="12" t="s">
-        <v>242</v>
+        <v>221</v>
       </c>
       <c r="D185" s="9" t="s">
         <v>43</v>
       </c>
       <c r="E185" t="s">
-        <v>244</v>
+        <v>223</v>
       </c>
       <c r="F185" s="1" t="s">
         <v>69</v>
@@ -4934,13 +4997,13 @@
         <v>6</v>
       </c>
       <c r="C186" s="12" t="s">
-        <v>221</v>
+        <v>242</v>
       </c>
       <c r="D186" s="9" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="E186" t="s">
-        <v>224</v>
+        <v>244</v>
       </c>
       <c r="F186" s="1" t="s">
         <v>69</v>
@@ -4954,13 +5017,13 @@
         <v>6</v>
       </c>
       <c r="C187" s="12" t="s">
-        <v>242</v>
+        <v>263</v>
       </c>
       <c r="D187" s="9" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="E187" t="s">
-        <v>245</v>
+        <v>265</v>
       </c>
       <c r="F187" s="1" t="s">
         <v>69</v>
@@ -4977,10 +5040,10 @@
         <v>221</v>
       </c>
       <c r="D188" s="9" t="s">
-        <v>13</v>
+        <v>30</v>
       </c>
       <c r="E188" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="F188" s="1" t="s">
         <v>69</v>
@@ -4997,10 +5060,10 @@
         <v>242</v>
       </c>
       <c r="D189" s="9" t="s">
-        <v>13</v>
+        <v>30</v>
       </c>
       <c r="E189" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="F189" s="1" t="s">
         <v>69</v>
@@ -5014,13 +5077,13 @@
         <v>6</v>
       </c>
       <c r="C190" s="12" t="s">
-        <v>221</v>
+        <v>263</v>
       </c>
       <c r="D190" s="9" t="s">
-        <v>46</v>
+        <v>30</v>
       </c>
       <c r="E190" t="s">
-        <v>226</v>
+        <v>266</v>
       </c>
       <c r="F190" s="1" t="s">
         <v>69</v>
@@ -5034,13 +5097,13 @@
         <v>6</v>
       </c>
       <c r="C191" s="12" t="s">
-        <v>242</v>
+        <v>221</v>
       </c>
       <c r="D191" s="9" t="s">
-        <v>46</v>
+        <v>13</v>
       </c>
       <c r="E191" t="s">
-        <v>247</v>
+        <v>225</v>
       </c>
       <c r="F191" s="1" t="s">
         <v>69</v>
@@ -5054,13 +5117,13 @@
         <v>6</v>
       </c>
       <c r="C192" s="12" t="s">
-        <v>221</v>
+        <v>242</v>
       </c>
       <c r="D192" s="9" t="s">
-        <v>33</v>
+        <v>13</v>
       </c>
       <c r="E192" t="s">
-        <v>227</v>
+        <v>246</v>
       </c>
       <c r="F192" s="1" t="s">
         <v>69</v>
@@ -5074,13 +5137,13 @@
         <v>6</v>
       </c>
       <c r="C193" s="12" t="s">
-        <v>242</v>
+        <v>263</v>
       </c>
       <c r="D193" s="9" t="s">
-        <v>33</v>
+        <v>13</v>
       </c>
       <c r="E193" t="s">
-        <v>248</v>
+        <v>267</v>
       </c>
       <c r="F193" s="1" t="s">
         <v>69</v>
@@ -5097,10 +5160,10 @@
         <v>221</v>
       </c>
       <c r="D194" s="9" t="s">
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="E194" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="F194" s="1" t="s">
         <v>69</v>
@@ -5117,10 +5180,10 @@
         <v>242</v>
       </c>
       <c r="D195" s="9" t="s">
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="E195" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="F195" s="1" t="s">
         <v>69</v>
@@ -5134,13 +5197,13 @@
         <v>6</v>
       </c>
       <c r="C196" s="12" t="s">
-        <v>221</v>
+        <v>263</v>
       </c>
       <c r="D196" s="9" t="s">
-        <v>14</v>
+        <v>46</v>
       </c>
       <c r="E196" t="s">
-        <v>229</v>
+        <v>268</v>
       </c>
       <c r="F196" s="1" t="s">
         <v>69</v>
@@ -5154,13 +5217,13 @@
         <v>6</v>
       </c>
       <c r="C197" s="12" t="s">
-        <v>242</v>
+        <v>221</v>
       </c>
       <c r="D197" s="9" t="s">
-        <v>14</v>
+        <v>33</v>
       </c>
       <c r="E197" t="s">
-        <v>250</v>
+        <v>227</v>
       </c>
       <c r="F197" s="1" t="s">
         <v>69</v>
@@ -5174,13 +5237,13 @@
         <v>6</v>
       </c>
       <c r="C198" s="12" t="s">
-        <v>221</v>
+        <v>242</v>
       </c>
       <c r="D198" s="9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E198" t="s">
-        <v>230</v>
+        <v>248</v>
       </c>
       <c r="F198" s="1" t="s">
         <v>69</v>
@@ -5194,13 +5257,13 @@
         <v>6</v>
       </c>
       <c r="C199" s="12" t="s">
-        <v>242</v>
+        <v>263</v>
       </c>
       <c r="D199" s="9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E199" t="s">
-        <v>251</v>
+        <v>269</v>
       </c>
       <c r="F199" s="1" t="s">
         <v>69</v>
@@ -5217,10 +5280,10 @@
         <v>221</v>
       </c>
       <c r="D200" s="9" t="s">
-        <v>16</v>
+        <v>36</v>
       </c>
       <c r="E200" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="F200" s="1" t="s">
         <v>69</v>
@@ -5237,10 +5300,10 @@
         <v>242</v>
       </c>
       <c r="D201" s="9" t="s">
-        <v>16</v>
+        <v>36</v>
       </c>
       <c r="E201" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="F201" s="1" t="s">
         <v>69</v>
@@ -5254,13 +5317,13 @@
         <v>6</v>
       </c>
       <c r="C202" s="12" t="s">
-        <v>221</v>
+        <v>263</v>
       </c>
       <c r="D202" s="9" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="E202" t="s">
-        <v>232</v>
+        <v>270</v>
       </c>
       <c r="F202" s="1" t="s">
         <v>69</v>
@@ -5274,13 +5337,13 @@
         <v>6</v>
       </c>
       <c r="C203" s="12" t="s">
-        <v>242</v>
+        <v>221</v>
       </c>
       <c r="D203" s="9" t="s">
-        <v>40</v>
+        <v>14</v>
       </c>
       <c r="E203" t="s">
-        <v>253</v>
+        <v>229</v>
       </c>
       <c r="F203" s="1" t="s">
         <v>69</v>
@@ -5294,13 +5357,13 @@
         <v>6</v>
       </c>
       <c r="C204" s="12" t="s">
-        <v>221</v>
+        <v>242</v>
       </c>
       <c r="D204" s="9" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="E204" t="s">
-        <v>233</v>
+        <v>250</v>
       </c>
       <c r="F204" s="1" t="s">
         <v>69</v>
@@ -5314,13 +5377,13 @@
         <v>6</v>
       </c>
       <c r="C205" s="12" t="s">
-        <v>242</v>
+        <v>263</v>
       </c>
       <c r="D205" s="9" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="E205" t="s">
-        <v>254</v>
+        <v>271</v>
       </c>
       <c r="F205" s="1" t="s">
         <v>69</v>
@@ -5337,10 +5400,10 @@
         <v>221</v>
       </c>
       <c r="D206" s="9" t="s">
-        <v>20</v>
+        <v>34</v>
       </c>
       <c r="E206" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="F206" s="1" t="s">
         <v>69</v>
@@ -5357,10 +5420,10 @@
         <v>242</v>
       </c>
       <c r="D207" s="9" t="s">
-        <v>20</v>
+        <v>34</v>
       </c>
       <c r="E207" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="F207" s="1" t="s">
         <v>69</v>
@@ -5374,13 +5437,13 @@
         <v>6</v>
       </c>
       <c r="C208" s="12" t="s">
-        <v>221</v>
+        <v>263</v>
       </c>
       <c r="D208" s="9" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="E208" t="s">
-        <v>235</v>
+        <v>272</v>
       </c>
       <c r="F208" s="1" t="s">
         <v>69</v>
@@ -5394,13 +5457,13 @@
         <v>6</v>
       </c>
       <c r="C209" s="12" t="s">
-        <v>242</v>
+        <v>221</v>
       </c>
       <c r="D209" s="9" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="E209" t="s">
-        <v>256</v>
+        <v>231</v>
       </c>
       <c r="F209" s="1" t="s">
         <v>69</v>
@@ -5414,13 +5477,13 @@
         <v>6</v>
       </c>
       <c r="C210" s="12" t="s">
-        <v>221</v>
+        <v>242</v>
       </c>
       <c r="D210" s="9" t="s">
-        <v>38</v>
+        <v>16</v>
       </c>
       <c r="E210" t="s">
-        <v>236</v>
+        <v>252</v>
       </c>
       <c r="F210" s="1" t="s">
         <v>69</v>
@@ -5434,13 +5497,13 @@
         <v>6</v>
       </c>
       <c r="C211" s="12" t="s">
-        <v>242</v>
+        <v>263</v>
       </c>
       <c r="D211" s="9" t="s">
-        <v>38</v>
+        <v>16</v>
       </c>
       <c r="E211" t="s">
-        <v>257</v>
+        <v>273</v>
       </c>
       <c r="F211" s="1" t="s">
         <v>69</v>
@@ -5457,10 +5520,10 @@
         <v>221</v>
       </c>
       <c r="D212" s="9" t="s">
-        <v>24</v>
+        <v>40</v>
       </c>
       <c r="E212" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
       <c r="F212" s="1" t="s">
         <v>69</v>
@@ -5477,10 +5540,10 @@
         <v>242</v>
       </c>
       <c r="D213" s="9" t="s">
-        <v>24</v>
+        <v>40</v>
       </c>
       <c r="E213" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="F213" s="1" t="s">
         <v>69</v>
@@ -5494,13 +5557,13 @@
         <v>6</v>
       </c>
       <c r="C214" s="12" t="s">
-        <v>221</v>
+        <v>263</v>
       </c>
       <c r="D214" s="9" t="s">
-        <v>26</v>
+        <v>40</v>
       </c>
       <c r="E214" t="s">
-        <v>238</v>
+        <v>274</v>
       </c>
       <c r="F214" s="1" t="s">
         <v>69</v>
@@ -5514,13 +5577,13 @@
         <v>6</v>
       </c>
       <c r="C215" s="12" t="s">
-        <v>242</v>
+        <v>221</v>
       </c>
       <c r="D215" s="9" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="E215" t="s">
-        <v>259</v>
+        <v>233</v>
       </c>
       <c r="F215" s="1" t="s">
         <v>69</v>
@@ -5534,13 +5597,13 @@
         <v>6</v>
       </c>
       <c r="C216" s="12" t="s">
-        <v>221</v>
+        <v>242</v>
       </c>
       <c r="D216" s="9" t="s">
-        <v>31</v>
+        <v>18</v>
       </c>
       <c r="E216" t="s">
-        <v>239</v>
+        <v>254</v>
       </c>
       <c r="F216" s="1" t="s">
         <v>69</v>
@@ -5554,13 +5617,13 @@
         <v>6</v>
       </c>
       <c r="C217" s="12" t="s">
-        <v>242</v>
+        <v>263</v>
       </c>
       <c r="D217" s="9" t="s">
-        <v>31</v>
+        <v>18</v>
       </c>
       <c r="E217" t="s">
-        <v>260</v>
+        <v>275</v>
       </c>
       <c r="F217" s="1" t="s">
         <v>69</v>
@@ -5577,10 +5640,10 @@
         <v>221</v>
       </c>
       <c r="D218" s="9" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="E218" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="F218" s="1" t="s">
         <v>69</v>
@@ -5597,10 +5660,10 @@
         <v>242</v>
       </c>
       <c r="D219" s="9" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="E219" t="s">
-        <v>261</v>
+        <v>255</v>
       </c>
       <c r="F219" s="1" t="s">
         <v>69</v>
@@ -5614,13 +5677,13 @@
         <v>6</v>
       </c>
       <c r="C220" s="12" t="s">
-        <v>221</v>
+        <v>263</v>
       </c>
       <c r="D220" s="9" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="E220" t="s">
-        <v>241</v>
+        <v>276</v>
       </c>
       <c r="F220" s="1" t="s">
         <v>69</v>
@@ -5634,15 +5697,415 @@
         <v>6</v>
       </c>
       <c r="C221" s="12" t="s">
+        <v>221</v>
+      </c>
+      <c r="D221" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="E221" t="s">
+        <v>235</v>
+      </c>
+      <c r="F221" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="222" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A222" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="B222" s="12">
+        <v>6</v>
+      </c>
+      <c r="C222" s="12" t="s">
         <v>242</v>
       </c>
-      <c r="D221" s="9" t="s">
+      <c r="D222" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="E222" t="s">
+        <v>256</v>
+      </c>
+      <c r="F222" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="223" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A223" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="B223" s="12">
+        <v>6</v>
+      </c>
+      <c r="C223" s="12" t="s">
+        <v>263</v>
+      </c>
+      <c r="D223" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="E223" t="s">
+        <v>277</v>
+      </c>
+      <c r="F223" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="224" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A224" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="B224" s="12">
+        <v>6</v>
+      </c>
+      <c r="C224" s="12" t="s">
+        <v>221</v>
+      </c>
+      <c r="D224" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="E224" t="s">
+        <v>236</v>
+      </c>
+      <c r="F224" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="225" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A225" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="B225" s="12">
+        <v>6</v>
+      </c>
+      <c r="C225" s="12" t="s">
+        <v>242</v>
+      </c>
+      <c r="D225" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="E225" t="s">
+        <v>257</v>
+      </c>
+      <c r="F225" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="226" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A226" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="B226" s="12">
+        <v>6</v>
+      </c>
+      <c r="C226" s="12" t="s">
+        <v>263</v>
+      </c>
+      <c r="D226" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="E226" t="s">
+        <v>278</v>
+      </c>
+      <c r="F226" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="227" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A227" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="B227" s="12">
+        <v>6</v>
+      </c>
+      <c r="C227" s="12" t="s">
+        <v>221</v>
+      </c>
+      <c r="D227" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="E227" t="s">
+        <v>237</v>
+      </c>
+      <c r="F227" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="228" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A228" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="B228" s="12">
+        <v>6</v>
+      </c>
+      <c r="C228" s="12" t="s">
+        <v>242</v>
+      </c>
+      <c r="D228" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="E228" t="s">
+        <v>258</v>
+      </c>
+      <c r="F228" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="229" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A229" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="B229" s="12">
+        <v>6</v>
+      </c>
+      <c r="C229" s="12" t="s">
+        <v>263</v>
+      </c>
+      <c r="D229" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="E229" t="s">
+        <v>279</v>
+      </c>
+      <c r="F229" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="230" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A230" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="B230" s="12">
+        <v>6</v>
+      </c>
+      <c r="C230" s="12" t="s">
+        <v>221</v>
+      </c>
+      <c r="D230" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="E230" t="s">
+        <v>238</v>
+      </c>
+      <c r="F230" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="231" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A231" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="B231" s="12">
+        <v>6</v>
+      </c>
+      <c r="C231" s="12" t="s">
+        <v>242</v>
+      </c>
+      <c r="D231" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="E231" t="s">
+        <v>259</v>
+      </c>
+      <c r="F231" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="232" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A232" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="B232" s="12">
+        <v>6</v>
+      </c>
+      <c r="C232" s="12" t="s">
+        <v>263</v>
+      </c>
+      <c r="D232" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="E232" t="s">
+        <v>280</v>
+      </c>
+      <c r="F232" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="233" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A233" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="B233" s="12">
+        <v>6</v>
+      </c>
+      <c r="C233" s="12" t="s">
+        <v>221</v>
+      </c>
+      <c r="D233" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="E233" t="s">
+        <v>239</v>
+      </c>
+      <c r="F233" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="234" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A234" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="B234" s="12">
+        <v>6</v>
+      </c>
+      <c r="C234" s="12" t="s">
+        <v>242</v>
+      </c>
+      <c r="D234" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="E234" t="s">
+        <v>260</v>
+      </c>
+      <c r="F234" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="235" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A235" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="B235" s="12">
+        <v>6</v>
+      </c>
+      <c r="C235" s="12" t="s">
+        <v>263</v>
+      </c>
+      <c r="D235" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="E235" t="s">
+        <v>281</v>
+      </c>
+      <c r="F235" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="236" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A236" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="B236" s="12">
+        <v>6</v>
+      </c>
+      <c r="C236" s="12" t="s">
+        <v>221</v>
+      </c>
+      <c r="D236" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="E236" t="s">
+        <v>240</v>
+      </c>
+      <c r="F236" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="237" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A237" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="B237" s="12">
+        <v>6</v>
+      </c>
+      <c r="C237" s="12" t="s">
+        <v>242</v>
+      </c>
+      <c r="D237" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="E237" t="s">
+        <v>261</v>
+      </c>
+      <c r="F237" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="238" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A238" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="B238" s="12">
+        <v>6</v>
+      </c>
+      <c r="C238" s="12" t="s">
+        <v>263</v>
+      </c>
+      <c r="D238" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="E238" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="F238" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="239" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A239" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="B239" s="12">
+        <v>6</v>
+      </c>
+      <c r="C239" s="12" t="s">
+        <v>221</v>
+      </c>
+      <c r="D239" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="E221" t="s">
+      <c r="E239" t="s">
+        <v>241</v>
+      </c>
+      <c r="F239" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="240" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A240" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="B240" s="12">
+        <v>6</v>
+      </c>
+      <c r="C240" s="12" t="s">
+        <v>242</v>
+      </c>
+      <c r="D240" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E240" t="s">
         <v>262</v>
       </c>
-      <c r="F221" s="1" t="s">
+      <c r="F240" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="241" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A241" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="B241" s="12">
+        <v>6</v>
+      </c>
+      <c r="C241" s="12" t="s">
+        <v>263</v>
+      </c>
+      <c r="D241" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E241" t="s">
+        <v>283</v>
+      </c>
+      <c r="F241" s="1" t="s">
         <v>69</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add US related to Health domain
Co-authored-by: MarioPeluso <mariopeluso00@gmail.com>
</commit_message>
<xml_diff>
--- a/refair-server/datasets/few shot dataset/FSDataset.xlsx
+++ b/refair-server/datasets/few shot dataset/FSDataset.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\morel\Desktop\Refair\ReFair-App\refair-server\datasets\few shot dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D8EBB82-08A4-43B0-8791-1EC8CDADE1C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9EFBE13-4D75-47E4-9B93-65D9E5EBFE37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{80773445-FB61-4F04-A882-1600FD96C55A}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1186" uniqueCount="284">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1286" uniqueCount="305">
   <si>
     <t>Domain cluster</t>
   </si>
@@ -888,13 +888,76 @@
   </si>
   <si>
     <t>As an endocrinologist, I want to use word embedding techniques to analyze similarities and relationships between medical terms in research literature on insulin resistance, aiding in the discovery of novel associations and mechanisms.</t>
+  </si>
+  <si>
+    <t>Health</t>
+  </si>
+  <si>
+    <t>As a healthcare provider, I want to apply adversarial learning techniques to detect and mitigate adversarial attacks on medical imaging systems, ensuring the integrity and reliability of diagnostic outcomes for patient care.</t>
+  </si>
+  <si>
+    <t>As a healthcare provider, I want to integrate CNN models into wearable health devices to monitor real-time physiological signals, enabling continuous health monitoring and early detection of cardiac abnormalities or respiratory distress.</t>
+  </si>
+  <si>
+    <t>As a healthcare administrator, I want to develop a multilingual conversational agent using machine learning algorithms to assist international patients in navigating healthcare services, including appointment scheduling, insurance inquiries, and medical translation services.</t>
+  </si>
+  <si>
+    <t>As a healthcare administrator, I want to utilize decision tree models to optimize hospital bed allocation based on patient admission criteria, ensuring efficient resource management and reducing emergency room overcrowding during peak periods.</t>
+  </si>
+  <si>
+    <t>As a healthcare administrator, I want to implement document classification algorithms to categorize and prioritize incoming medical reports (e.g., radiology, pathology) based on urgency and clinical significance, facilitating timely review and decision-making by healthcare professionals.</t>
+  </si>
+  <si>
+    <t>As a healthcare provider, I want to deploy machine learning models for entity extraction in clinical trials documentation, to automatically extract and categorize information on study protocols, participant demographics, and treatment outcomes, facilitating efficient research data management and analysis.</t>
+  </si>
+  <si>
+    <t>As a healthcare provider, I want to utilize feature selection techniques in machine learning models to extract meaningful patterns from wearable device data (e.g., heart rate variability, activity levels) for early detection and management of chronic conditions like hypertension and diabetes.</t>
+  </si>
+  <si>
+    <t>As a healthcare administrator, I want to handle imbalanced datasets in predictive models for disease outbreak detection, focusing on early identification of emerging infectious diseases with low prevalence rates, to enable timely public health responses and containment strategies.</t>
+  </si>
+  <si>
+    <t>As a healthcare administrator, I want to implement keyword extraction techniques in healthcare surveys and feedback forms, automatically identifying recurring themes and patient concerns to improve service delivery and patient satisfaction across hospital departments.</t>
+  </si>
+  <si>
+    <t>As a healthcare provider, I want to implement k-nearest neighbor models for predicting patient medication responses based on similarities with historical patient data, enhancing personalized medicine approaches and optimizing drug therapy plans for chronic conditions like hypertension and diabetes.</t>
+  </si>
+  <si>
+    <t>As a healthcare provider, I want to deploy a multi-label classification algorithm to identify mental health conditions such as depression, anxiety, and PTSD simultaneously from patient psychological assessments, facilitating integrated treatment plans and improved mental health outcomes.</t>
+  </si>
+  <si>
+    <t>As a healthcare provider, I want to implement a neural network architecture to analyze patient brain imaging data (fMRI scans) to identify neural correlates of Alzheimer's disease progression, aiding in early diagnosis and intervention planning.</t>
+  </si>
+  <si>
+    <t>As a healthcare administrator, I want to implement random forest models to predict patient hospitalization risks based on historical medical records, optimizing resource allocation and improving patient management in hospital settings.</t>
+  </si>
+  <si>
+    <t>As a healthcare provider, I want to develop a random forest-based system to classify medical images (e.g., X-rays, MRIs) into diagnostic categories such as benign vs. malignant tumors, supporting radiologists in accurate and timely diagnosis for improved patient treatment planning.</t>
+  </si>
+  <si>
+    <t>As a healthcare administrator, I want to develop a sentiment analysis model to analyze social media posts and online forums related to public perceptions of vaccination, identifying sentiment trends and addressing vaccine hesitancy through targeted communication strategies.</t>
+  </si>
+  <si>
+    <t>As a healthcare provider, I want to implement speech-to-text technology in medical transcription to accurately convert clinician dictations into electronic health records (EHRs), improving documentation efficiency and reducing errors in patient medical records.</t>
+  </si>
+  <si>
+    <t>As a healthcare administrator, I want to deploy text categorization algorithms to categorize electronic health record (EHR) notes into administrative and clinical categories, streamlining data management processes and enhancing operational efficiency in healthcare facilities.</t>
+  </si>
+  <si>
+    <t>As a healthcare provider, I want to utilize unsupervised clustering techniques on medical imaging data (e.g., MRI scans) to categorize brain tumor types based on radiological features, supporting accurate diagnosis and treatment planning in neuro-oncology.</t>
+  </si>
+  <si>
+    <t>As a healthcare administrator, I want to integrate voice recognition technology into hospital admission systems to allow patients to verbally provide their medical history and consent information, enhancing patient registration processes and reducing paperwork errors.</t>
+  </si>
+  <si>
+    <t>As a healthcare provider, I want to utilize word embedding techniques to analyze electronic health records (EHRs) and extract meaningful semantic relationships between medical terminologies and patient conditions, improving information retrieval and clinical decision support systems.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -926,6 +989,11 @@
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="7">
@@ -978,7 +1046,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1000,6 +1068,7 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -1334,10 +1403,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8DF0B04-8323-4309-B759-D1CDDA1FBB0E}">
-  <dimension ref="A1:F241"/>
+  <dimension ref="A1:F261"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A220" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F181" sqref="F181:F241"/>
+    <sheetView tabSelected="1" topLeftCell="A247" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -4909,27 +4978,27 @@
         <v>69</v>
       </c>
     </row>
-    <row r="182" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A182" s="12" t="s">
         <v>220</v>
       </c>
-      <c r="B182" s="12">
-        <v>6</v>
-      </c>
-      <c r="C182" s="12" t="s">
+      <c r="B182" s="13">
+        <v>6</v>
+      </c>
+      <c r="C182" s="13" t="s">
         <v>221</v>
       </c>
       <c r="D182" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="E182" t="s">
+      <c r="E182" s="1" t="s">
         <v>222</v>
       </c>
       <c r="F182" s="1" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="183" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A183" s="12" t="s">
         <v>220</v>
       </c>
@@ -4942,74 +5011,74 @@
       <c r="D183" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="E183" t="s">
+      <c r="E183" s="1" t="s">
         <v>243</v>
       </c>
       <c r="F183" s="1" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="184" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A184" s="12" t="s">
-        <v>220</v>
-      </c>
-      <c r="B184" s="12">
-        <v>6</v>
-      </c>
-      <c r="C184" s="12" t="s">
+    <row r="184" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A184" s="13" t="s">
+        <v>220</v>
+      </c>
+      <c r="B184" s="13">
+        <v>6</v>
+      </c>
+      <c r="C184" s="13" t="s">
         <v>263</v>
       </c>
       <c r="D184" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="E184" t="s">
+      <c r="E184" s="1" t="s">
         <v>264</v>
       </c>
       <c r="F184" s="1" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="185" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A185" s="12" t="s">
-        <v>220</v>
-      </c>
-      <c r="B185" s="12">
-        <v>6</v>
-      </c>
-      <c r="C185" s="12" t="s">
+    <row r="185" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A185" s="13" t="s">
+        <v>220</v>
+      </c>
+      <c r="B185" s="13">
+        <v>6</v>
+      </c>
+      <c r="C185" s="13" t="s">
+        <v>284</v>
+      </c>
+      <c r="D185" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="E185" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="F185" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="186" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A186" s="13" t="s">
+        <v>220</v>
+      </c>
+      <c r="B186" s="13">
+        <v>6</v>
+      </c>
+      <c r="C186" s="13" t="s">
         <v>221</v>
-      </c>
-      <c r="D185" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="E185" t="s">
-        <v>223</v>
-      </c>
-      <c r="F185" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="186" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A186" s="12" t="s">
-        <v>220</v>
-      </c>
-      <c r="B186" s="12">
-        <v>6</v>
-      </c>
-      <c r="C186" s="12" t="s">
-        <v>242</v>
       </c>
       <c r="D186" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="E186" t="s">
-        <v>244</v>
+      <c r="E186" s="1" t="s">
+        <v>223</v>
       </c>
       <c r="F186" s="1" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="187" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A187" s="12" t="s">
         <v>220</v>
       </c>
@@ -5017,159 +5086,159 @@
         <v>6</v>
       </c>
       <c r="C187" s="12" t="s">
-        <v>263</v>
+        <v>242</v>
       </c>
       <c r="D187" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="E187" t="s">
+      <c r="E187" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="F187" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="188" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A188" s="13" t="s">
+        <v>220</v>
+      </c>
+      <c r="B188" s="13">
+        <v>6</v>
+      </c>
+      <c r="C188" s="13" t="s">
+        <v>263</v>
+      </c>
+      <c r="D188" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="E188" s="1" t="s">
         <v>265</v>
       </c>
-      <c r="F187" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="188" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A188" s="12" t="s">
-        <v>220</v>
-      </c>
-      <c r="B188" s="12">
-        <v>6</v>
-      </c>
-      <c r="C188" s="12" t="s">
+      <c r="F188" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="189" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A189" s="13" t="s">
+        <v>220</v>
+      </c>
+      <c r="B189" s="13">
+        <v>6</v>
+      </c>
+      <c r="C189" s="13" t="s">
+        <v>284</v>
+      </c>
+      <c r="D189" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="E189" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="F189" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="190" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A190" s="13" t="s">
+        <v>220</v>
+      </c>
+      <c r="B190" s="13">
+        <v>6</v>
+      </c>
+      <c r="C190" s="13" t="s">
         <v>221</v>
-      </c>
-      <c r="D188" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="E188" t="s">
-        <v>224</v>
-      </c>
-      <c r="F188" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="189" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A189" s="12" t="s">
-        <v>220</v>
-      </c>
-      <c r="B189" s="12">
-        <v>6</v>
-      </c>
-      <c r="C189" s="12" t="s">
-        <v>242</v>
-      </c>
-      <c r="D189" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="E189" t="s">
-        <v>245</v>
-      </c>
-      <c r="F189" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="190" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A190" s="12" t="s">
-        <v>220</v>
-      </c>
-      <c r="B190" s="12">
-        <v>6</v>
-      </c>
-      <c r="C190" s="12" t="s">
-        <v>263</v>
       </c>
       <c r="D190" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="E190" t="s">
+      <c r="E190" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="F190" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="191" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A191" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="B191" s="12">
+        <v>6</v>
+      </c>
+      <c r="C191" s="12" t="s">
+        <v>242</v>
+      </c>
+      <c r="D191" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="E191" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="F191" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="192" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A192" s="13" t="s">
+        <v>220</v>
+      </c>
+      <c r="B192" s="13">
+        <v>6</v>
+      </c>
+      <c r="C192" s="13" t="s">
+        <v>263</v>
+      </c>
+      <c r="D192" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="E192" s="1" t="s">
         <v>266</v>
       </c>
-      <c r="F190" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="191" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A191" s="12" t="s">
-        <v>220</v>
-      </c>
-      <c r="B191" s="12">
-        <v>6</v>
-      </c>
-      <c r="C191" s="12" t="s">
+      <c r="F192" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="193" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A193" s="13" t="s">
+        <v>220</v>
+      </c>
+      <c r="B193" s="13">
+        <v>6</v>
+      </c>
+      <c r="C193" s="13" t="s">
+        <v>284</v>
+      </c>
+      <c r="D193" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="E193" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="F193" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="194" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A194" s="13" t="s">
+        <v>220</v>
+      </c>
+      <c r="B194" s="13">
+        <v>6</v>
+      </c>
+      <c r="C194" s="13" t="s">
         <v>221</v>
       </c>
-      <c r="D191" s="9" t="s">
+      <c r="D194" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="E191" t="s">
+      <c r="E194" s="1" t="s">
         <v>225</v>
       </c>
-      <c r="F191" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="192" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A192" s="12" t="s">
-        <v>220</v>
-      </c>
-      <c r="B192" s="12">
-        <v>6</v>
-      </c>
-      <c r="C192" s="12" t="s">
-        <v>242</v>
-      </c>
-      <c r="D192" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="E192" t="s">
-        <v>246</v>
-      </c>
-      <c r="F192" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="193" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A193" s="12" t="s">
-        <v>220</v>
-      </c>
-      <c r="B193" s="12">
-        <v>6</v>
-      </c>
-      <c r="C193" s="12" t="s">
-        <v>263</v>
-      </c>
-      <c r="D193" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="E193" t="s">
-        <v>267</v>
-      </c>
-      <c r="F193" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="194" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A194" s="12" t="s">
-        <v>220</v>
-      </c>
-      <c r="B194" s="12">
-        <v>6</v>
-      </c>
-      <c r="C194" s="12" t="s">
-        <v>221</v>
-      </c>
-      <c r="D194" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="E194" t="s">
-        <v>226</v>
-      </c>
       <c r="F194" s="1" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="195" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A195" s="12" t="s">
         <v>220</v>
       </c>
@@ -5180,236 +5249,236 @@
         <v>242</v>
       </c>
       <c r="D195" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="E195" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="F195" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="196" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A196" s="13" t="s">
+        <v>220</v>
+      </c>
+      <c r="B196" s="13">
+        <v>6</v>
+      </c>
+      <c r="C196" s="13" t="s">
+        <v>263</v>
+      </c>
+      <c r="D196" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="E196" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="F196" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="197" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A197" s="13" t="s">
+        <v>220</v>
+      </c>
+      <c r="B197" s="13">
+        <v>6</v>
+      </c>
+      <c r="C197" s="13" t="s">
+        <v>284</v>
+      </c>
+      <c r="D197" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="E197" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="F197" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="198" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A198" s="13" t="s">
+        <v>220</v>
+      </c>
+      <c r="B198" s="13">
+        <v>6</v>
+      </c>
+      <c r="C198" s="13" t="s">
+        <v>221</v>
+      </c>
+      <c r="D198" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="E195" t="s">
+      <c r="E198" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="F198" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="199" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A199" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="B199" s="12">
+        <v>6</v>
+      </c>
+      <c r="C199" s="12" t="s">
+        <v>242</v>
+      </c>
+      <c r="D199" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="E199" s="1" t="s">
         <v>247</v>
       </c>
-      <c r="F195" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="196" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A196" s="12" t="s">
-        <v>220</v>
-      </c>
-      <c r="B196" s="12">
-        <v>6</v>
-      </c>
-      <c r="C196" s="12" t="s">
+      <c r="F199" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="200" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A200" s="13" t="s">
+        <v>220</v>
+      </c>
+      <c r="B200" s="13">
+        <v>6</v>
+      </c>
+      <c r="C200" s="13" t="s">
         <v>263</v>
       </c>
-      <c r="D196" s="9" t="s">
+      <c r="D200" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="E196" t="s">
+      <c r="E200" s="1" t="s">
         <v>268</v>
       </c>
-      <c r="F196" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="197" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A197" s="12" t="s">
-        <v>220</v>
-      </c>
-      <c r="B197" s="12">
-        <v>6</v>
-      </c>
-      <c r="C197" s="12" t="s">
+      <c r="F200" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="201" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A201" s="13" t="s">
+        <v>220</v>
+      </c>
+      <c r="B201" s="13">
+        <v>6</v>
+      </c>
+      <c r="C201" s="13" t="s">
+        <v>284</v>
+      </c>
+      <c r="D201" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="E201" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="F201" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="202" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A202" s="13" t="s">
+        <v>220</v>
+      </c>
+      <c r="B202" s="13">
+        <v>6</v>
+      </c>
+      <c r="C202" s="13" t="s">
         <v>221</v>
       </c>
-      <c r="D197" s="9" t="s">
+      <c r="D202" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="E197" t="s">
+      <c r="E202" s="1" t="s">
         <v>227</v>
       </c>
-      <c r="F197" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="198" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A198" s="12" t="s">
-        <v>220</v>
-      </c>
-      <c r="B198" s="12">
-        <v>6</v>
-      </c>
-      <c r="C198" s="12" t="s">
+      <c r="F202" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="203" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A203" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="B203" s="12">
+        <v>6</v>
+      </c>
+      <c r="C203" s="12" t="s">
         <v>242</v>
       </c>
-      <c r="D198" s="9" t="s">
+      <c r="D203" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="E198" t="s">
+      <c r="E203" s="1" t="s">
         <v>248</v>
       </c>
-      <c r="F198" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="199" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A199" s="12" t="s">
-        <v>220</v>
-      </c>
-      <c r="B199" s="12">
-        <v>6</v>
-      </c>
-      <c r="C199" s="12" t="s">
+      <c r="F203" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="204" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A204" s="13" t="s">
+        <v>220</v>
+      </c>
+      <c r="B204" s="13">
+        <v>6</v>
+      </c>
+      <c r="C204" s="13" t="s">
         <v>263</v>
       </c>
-      <c r="D199" s="9" t="s">
+      <c r="D204" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="E199" t="s">
+      <c r="E204" s="1" t="s">
         <v>269</v>
       </c>
-      <c r="F199" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="200" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A200" s="12" t="s">
-        <v>220</v>
-      </c>
-      <c r="B200" s="12">
-        <v>6</v>
-      </c>
-      <c r="C200" s="12" t="s">
+      <c r="F204" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="205" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A205" s="13" t="s">
+        <v>220</v>
+      </c>
+      <c r="B205" s="13">
+        <v>6</v>
+      </c>
+      <c r="C205" s="13" t="s">
+        <v>284</v>
+      </c>
+      <c r="D205" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="E205" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="F205" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="206" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A206" s="13" t="s">
+        <v>220</v>
+      </c>
+      <c r="B206" s="13">
+        <v>6</v>
+      </c>
+      <c r="C206" s="13" t="s">
         <v>221</v>
       </c>
-      <c r="D200" s="9" t="s">
+      <c r="D206" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="E200" t="s">
+      <c r="E206" s="1" t="s">
         <v>228</v>
       </c>
-      <c r="F200" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="201" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A201" s="12" t="s">
-        <v>220</v>
-      </c>
-      <c r="B201" s="12">
-        <v>6</v>
-      </c>
-      <c r="C201" s="12" t="s">
-        <v>242</v>
-      </c>
-      <c r="D201" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="E201" t="s">
-        <v>249</v>
-      </c>
-      <c r="F201" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="202" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A202" s="12" t="s">
-        <v>220</v>
-      </c>
-      <c r="B202" s="12">
-        <v>6</v>
-      </c>
-      <c r="C202" s="12" t="s">
-        <v>263</v>
-      </c>
-      <c r="D202" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="E202" t="s">
-        <v>270</v>
-      </c>
-      <c r="F202" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="203" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A203" s="12" t="s">
-        <v>220</v>
-      </c>
-      <c r="B203" s="12">
-        <v>6</v>
-      </c>
-      <c r="C203" s="12" t="s">
-        <v>221</v>
-      </c>
-      <c r="D203" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="E203" t="s">
-        <v>229</v>
-      </c>
-      <c r="F203" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="204" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A204" s="12" t="s">
-        <v>220</v>
-      </c>
-      <c r="B204" s="12">
-        <v>6</v>
-      </c>
-      <c r="C204" s="12" t="s">
-        <v>242</v>
-      </c>
-      <c r="D204" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="E204" t="s">
-        <v>250</v>
-      </c>
-      <c r="F204" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="205" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A205" s="12" t="s">
-        <v>220</v>
-      </c>
-      <c r="B205" s="12">
-        <v>6</v>
-      </c>
-      <c r="C205" s="12" t="s">
-        <v>263</v>
-      </c>
-      <c r="D205" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="E205" t="s">
-        <v>271</v>
-      </c>
-      <c r="F205" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="206" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A206" s="12" t="s">
-        <v>220</v>
-      </c>
-      <c r="B206" s="12">
-        <v>6</v>
-      </c>
-      <c r="C206" s="12" t="s">
-        <v>221</v>
-      </c>
-      <c r="D206" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="E206" t="s">
-        <v>230</v>
-      </c>
       <c r="F206" s="1" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="207" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A207" s="12" t="s">
         <v>220</v>
       </c>
@@ -5420,236 +5489,236 @@
         <v>242</v>
       </c>
       <c r="D207" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="E207" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="F207" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="208" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A208" s="13" t="s">
+        <v>220</v>
+      </c>
+      <c r="B208" s="13">
+        <v>6</v>
+      </c>
+      <c r="C208" s="13" t="s">
+        <v>263</v>
+      </c>
+      <c r="D208" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="E208" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="F208" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="209" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A209" s="13" t="s">
+        <v>220</v>
+      </c>
+      <c r="B209" s="13">
+        <v>6</v>
+      </c>
+      <c r="C209" s="13" t="s">
+        <v>284</v>
+      </c>
+      <c r="D209" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="E209" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="F209" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="210" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A210" s="13" t="s">
+        <v>220</v>
+      </c>
+      <c r="B210" s="13">
+        <v>6</v>
+      </c>
+      <c r="C210" s="13" t="s">
+        <v>221</v>
+      </c>
+      <c r="D210" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="E210" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="F210" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="211" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A211" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="B211" s="12">
+        <v>6</v>
+      </c>
+      <c r="C211" s="12" t="s">
+        <v>242</v>
+      </c>
+      <c r="D211" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="E211" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="F211" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="212" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A212" s="13" t="s">
+        <v>220</v>
+      </c>
+      <c r="B212" s="13">
+        <v>6</v>
+      </c>
+      <c r="C212" s="13" t="s">
+        <v>263</v>
+      </c>
+      <c r="D212" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="E212" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="F212" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="213" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A213" s="13" t="s">
+        <v>220</v>
+      </c>
+      <c r="B213" s="13">
+        <v>6</v>
+      </c>
+      <c r="C213" s="13" t="s">
+        <v>284</v>
+      </c>
+      <c r="D213" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="E213" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="F213" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="214" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A214" s="13" t="s">
+        <v>220</v>
+      </c>
+      <c r="B214" s="13">
+        <v>6</v>
+      </c>
+      <c r="C214" s="13" t="s">
+        <v>221</v>
+      </c>
+      <c r="D214" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="E207" t="s">
+      <c r="E214" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="F214" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="215" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A215" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="B215" s="12">
+        <v>6</v>
+      </c>
+      <c r="C215" s="12" t="s">
+        <v>242</v>
+      </c>
+      <c r="D215" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="E215" s="1" t="s">
         <v>251</v>
       </c>
-      <c r="F207" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="208" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A208" s="12" t="s">
-        <v>220</v>
-      </c>
-      <c r="B208" s="12">
-        <v>6</v>
-      </c>
-      <c r="C208" s="12" t="s">
+      <c r="F215" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="216" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A216" s="13" t="s">
+        <v>220</v>
+      </c>
+      <c r="B216" s="13">
+        <v>6</v>
+      </c>
+      <c r="C216" s="13" t="s">
         <v>263</v>
       </c>
-      <c r="D208" s="9" t="s">
+      <c r="D216" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="E208" t="s">
+      <c r="E216" s="1" t="s">
         <v>272</v>
       </c>
-      <c r="F208" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="209" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A209" s="12" t="s">
-        <v>220</v>
-      </c>
-      <c r="B209" s="12">
-        <v>6</v>
-      </c>
-      <c r="C209" s="12" t="s">
+      <c r="F216" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="217" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A217" s="13" t="s">
+        <v>220</v>
+      </c>
+      <c r="B217" s="13">
+        <v>6</v>
+      </c>
+      <c r="C217" s="13" t="s">
+        <v>284</v>
+      </c>
+      <c r="D217" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="E217" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="F217" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="218" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A218" s="13" t="s">
+        <v>220</v>
+      </c>
+      <c r="B218" s="13">
+        <v>6</v>
+      </c>
+      <c r="C218" s="13" t="s">
         <v>221</v>
       </c>
-      <c r="D209" s="9" t="s">
+      <c r="D218" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="E209" t="s">
+      <c r="E218" s="1" t="s">
         <v>231</v>
       </c>
-      <c r="F209" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="210" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A210" s="12" t="s">
-        <v>220</v>
-      </c>
-      <c r="B210" s="12">
-        <v>6</v>
-      </c>
-      <c r="C210" s="12" t="s">
-        <v>242</v>
-      </c>
-      <c r="D210" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="E210" t="s">
-        <v>252</v>
-      </c>
-      <c r="F210" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="211" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A211" s="12" t="s">
-        <v>220</v>
-      </c>
-      <c r="B211" s="12">
-        <v>6</v>
-      </c>
-      <c r="C211" s="12" t="s">
-        <v>263</v>
-      </c>
-      <c r="D211" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="E211" t="s">
-        <v>273</v>
-      </c>
-      <c r="F211" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="212" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A212" s="12" t="s">
-        <v>220</v>
-      </c>
-      <c r="B212" s="12">
-        <v>6</v>
-      </c>
-      <c r="C212" s="12" t="s">
-        <v>221</v>
-      </c>
-      <c r="D212" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="E212" t="s">
-        <v>232</v>
-      </c>
-      <c r="F212" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="213" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A213" s="12" t="s">
-        <v>220</v>
-      </c>
-      <c r="B213" s="12">
-        <v>6</v>
-      </c>
-      <c r="C213" s="12" t="s">
-        <v>242</v>
-      </c>
-      <c r="D213" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="E213" t="s">
-        <v>253</v>
-      </c>
-      <c r="F213" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="214" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A214" s="12" t="s">
-        <v>220</v>
-      </c>
-      <c r="B214" s="12">
-        <v>6</v>
-      </c>
-      <c r="C214" s="12" t="s">
-        <v>263</v>
-      </c>
-      <c r="D214" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="E214" t="s">
-        <v>274</v>
-      </c>
-      <c r="F214" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="215" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A215" s="12" t="s">
-        <v>220</v>
-      </c>
-      <c r="B215" s="12">
-        <v>6</v>
-      </c>
-      <c r="C215" s="12" t="s">
-        <v>221</v>
-      </c>
-      <c r="D215" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="E215" t="s">
-        <v>233</v>
-      </c>
-      <c r="F215" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="216" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A216" s="12" t="s">
-        <v>220</v>
-      </c>
-      <c r="B216" s="12">
-        <v>6</v>
-      </c>
-      <c r="C216" s="12" t="s">
-        <v>242</v>
-      </c>
-      <c r="D216" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="E216" t="s">
-        <v>254</v>
-      </c>
-      <c r="F216" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="217" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A217" s="12" t="s">
-        <v>220</v>
-      </c>
-      <c r="B217" s="12">
-        <v>6</v>
-      </c>
-      <c r="C217" s="12" t="s">
-        <v>263</v>
-      </c>
-      <c r="D217" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="E217" t="s">
-        <v>275</v>
-      </c>
-      <c r="F217" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="218" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A218" s="12" t="s">
-        <v>220</v>
-      </c>
-      <c r="B218" s="12">
-        <v>6</v>
-      </c>
-      <c r="C218" s="12" t="s">
-        <v>221</v>
-      </c>
-      <c r="D218" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="E218" t="s">
-        <v>234</v>
-      </c>
       <c r="F218" s="1" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="219" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A219" s="12" t="s">
         <v>220</v>
       </c>
@@ -5660,236 +5729,236 @@
         <v>242</v>
       </c>
       <c r="D219" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="E219" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="F219" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="220" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A220" s="13" t="s">
+        <v>220</v>
+      </c>
+      <c r="B220" s="13">
+        <v>6</v>
+      </c>
+      <c r="C220" s="13" t="s">
+        <v>263</v>
+      </c>
+      <c r="D220" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="E220" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="F220" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="221" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A221" s="13" t="s">
+        <v>220</v>
+      </c>
+      <c r="B221" s="13">
+        <v>6</v>
+      </c>
+      <c r="C221" s="13" t="s">
+        <v>284</v>
+      </c>
+      <c r="D221" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="E221" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="F221" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="222" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A222" s="13" t="s">
+        <v>220</v>
+      </c>
+      <c r="B222" s="13">
+        <v>6</v>
+      </c>
+      <c r="C222" s="13" t="s">
+        <v>221</v>
+      </c>
+      <c r="D222" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="E222" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="F222" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="223" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A223" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="B223" s="12">
+        <v>6</v>
+      </c>
+      <c r="C223" s="12" t="s">
+        <v>242</v>
+      </c>
+      <c r="D223" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="E223" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="F223" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="224" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A224" s="13" t="s">
+        <v>220</v>
+      </c>
+      <c r="B224" s="13">
+        <v>6</v>
+      </c>
+      <c r="C224" s="13" t="s">
+        <v>263</v>
+      </c>
+      <c r="D224" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="E224" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="F224" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="225" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A225" s="13" t="s">
+        <v>220</v>
+      </c>
+      <c r="B225" s="13">
+        <v>6</v>
+      </c>
+      <c r="C225" s="13" t="s">
+        <v>284</v>
+      </c>
+      <c r="D225" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="E225" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="F225" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="226" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A226" s="13" t="s">
+        <v>220</v>
+      </c>
+      <c r="B226" s="13">
+        <v>6</v>
+      </c>
+      <c r="C226" s="13" t="s">
+        <v>221</v>
+      </c>
+      <c r="D226" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="E226" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="F226" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="227" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A227" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="B227" s="12">
+        <v>6</v>
+      </c>
+      <c r="C227" s="12" t="s">
+        <v>242</v>
+      </c>
+      <c r="D227" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="E227" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="F227" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="228" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A228" s="13" t="s">
+        <v>220</v>
+      </c>
+      <c r="B228" s="13">
+        <v>6</v>
+      </c>
+      <c r="C228" s="13" t="s">
+        <v>263</v>
+      </c>
+      <c r="D228" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="E228" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="F228" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="229" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A229" s="13" t="s">
+        <v>220</v>
+      </c>
+      <c r="B229" s="13">
+        <v>6</v>
+      </c>
+      <c r="C229" s="13" t="s">
+        <v>284</v>
+      </c>
+      <c r="D229" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="E229" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="F229" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="230" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A230" s="13" t="s">
+        <v>220</v>
+      </c>
+      <c r="B230" s="13">
+        <v>6</v>
+      </c>
+      <c r="C230" s="13" t="s">
+        <v>221</v>
+      </c>
+      <c r="D230" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="E219" t="s">
-        <v>255</v>
-      </c>
-      <c r="F219" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="220" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A220" s="12" t="s">
-        <v>220</v>
-      </c>
-      <c r="B220" s="12">
-        <v>6</v>
-      </c>
-      <c r="C220" s="12" t="s">
-        <v>263</v>
-      </c>
-      <c r="D220" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="E220" t="s">
-        <v>276</v>
-      </c>
-      <c r="F220" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="221" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A221" s="12" t="s">
-        <v>220</v>
-      </c>
-      <c r="B221" s="12">
-        <v>6</v>
-      </c>
-      <c r="C221" s="12" t="s">
-        <v>221</v>
-      </c>
-      <c r="D221" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="E221" t="s">
-        <v>235</v>
-      </c>
-      <c r="F221" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="222" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A222" s="12" t="s">
-        <v>220</v>
-      </c>
-      <c r="B222" s="12">
-        <v>6</v>
-      </c>
-      <c r="C222" s="12" t="s">
-        <v>242</v>
-      </c>
-      <c r="D222" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="E222" t="s">
-        <v>256</v>
-      </c>
-      <c r="F222" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="223" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A223" s="12" t="s">
-        <v>220</v>
-      </c>
-      <c r="B223" s="12">
-        <v>6</v>
-      </c>
-      <c r="C223" s="12" t="s">
-        <v>263</v>
-      </c>
-      <c r="D223" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="E223" t="s">
-        <v>277</v>
-      </c>
-      <c r="F223" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="224" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A224" s="12" t="s">
-        <v>220</v>
-      </c>
-      <c r="B224" s="12">
-        <v>6</v>
-      </c>
-      <c r="C224" s="12" t="s">
-        <v>221</v>
-      </c>
-      <c r="D224" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="E224" t="s">
-        <v>236</v>
-      </c>
-      <c r="F224" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="225" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A225" s="12" t="s">
-        <v>220</v>
-      </c>
-      <c r="B225" s="12">
-        <v>6</v>
-      </c>
-      <c r="C225" s="12" t="s">
-        <v>242</v>
-      </c>
-      <c r="D225" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="E225" t="s">
-        <v>257</v>
-      </c>
-      <c r="F225" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="226" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A226" s="12" t="s">
-        <v>220</v>
-      </c>
-      <c r="B226" s="12">
-        <v>6</v>
-      </c>
-      <c r="C226" s="12" t="s">
-        <v>263</v>
-      </c>
-      <c r="D226" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="E226" t="s">
-        <v>278</v>
-      </c>
-      <c r="F226" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="227" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A227" s="12" t="s">
-        <v>220</v>
-      </c>
-      <c r="B227" s="12">
-        <v>6</v>
-      </c>
-      <c r="C227" s="12" t="s">
-        <v>221</v>
-      </c>
-      <c r="D227" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="E227" t="s">
-        <v>237</v>
-      </c>
-      <c r="F227" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="228" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A228" s="12" t="s">
-        <v>220</v>
-      </c>
-      <c r="B228" s="12">
-        <v>6</v>
-      </c>
-      <c r="C228" s="12" t="s">
-        <v>242</v>
-      </c>
-      <c r="D228" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="E228" t="s">
-        <v>258</v>
-      </c>
-      <c r="F228" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="229" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A229" s="12" t="s">
-        <v>220</v>
-      </c>
-      <c r="B229" s="12">
-        <v>6</v>
-      </c>
-      <c r="C229" s="12" t="s">
-        <v>263</v>
-      </c>
-      <c r="D229" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="E229" t="s">
-        <v>279</v>
-      </c>
-      <c r="F229" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="230" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A230" s="12" t="s">
-        <v>220</v>
-      </c>
-      <c r="B230" s="12">
-        <v>6</v>
-      </c>
-      <c r="C230" s="12" t="s">
-        <v>221</v>
-      </c>
-      <c r="D230" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="E230" t="s">
-        <v>238</v>
+      <c r="E230" s="1" t="s">
+        <v>234</v>
       </c>
       <c r="F230" s="1" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="231" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="231" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A231" s="12" t="s">
         <v>220</v>
       </c>
@@ -5900,212 +5969,612 @@
         <v>242</v>
       </c>
       <c r="D231" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="E231" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="F231" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="232" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A232" s="13" t="s">
+        <v>220</v>
+      </c>
+      <c r="B232" s="13">
+        <v>6</v>
+      </c>
+      <c r="C232" s="13" t="s">
+        <v>263</v>
+      </c>
+      <c r="D232" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="E232" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="F232" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="233" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A233" s="13" t="s">
+        <v>220</v>
+      </c>
+      <c r="B233" s="13">
+        <v>6</v>
+      </c>
+      <c r="C233" s="13" t="s">
+        <v>284</v>
+      </c>
+      <c r="D233" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="E233" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="F233" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="234" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A234" s="13" t="s">
+        <v>220</v>
+      </c>
+      <c r="B234" s="13">
+        <v>6</v>
+      </c>
+      <c r="C234" s="13" t="s">
+        <v>221</v>
+      </c>
+      <c r="D234" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="E234" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="F234" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="235" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A235" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="B235" s="12">
+        <v>6</v>
+      </c>
+      <c r="C235" s="12" t="s">
+        <v>242</v>
+      </c>
+      <c r="D235" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="E235" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="F235" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="236" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A236" s="13" t="s">
+        <v>220</v>
+      </c>
+      <c r="B236" s="13">
+        <v>6</v>
+      </c>
+      <c r="C236" s="13" t="s">
+        <v>263</v>
+      </c>
+      <c r="D236" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="E236" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="F236" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="237" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A237" s="13" t="s">
+        <v>220</v>
+      </c>
+      <c r="B237" s="13">
+        <v>6</v>
+      </c>
+      <c r="C237" s="13" t="s">
+        <v>284</v>
+      </c>
+      <c r="D237" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="E237" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="F237" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="238" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A238" s="13" t="s">
+        <v>220</v>
+      </c>
+      <c r="B238" s="13">
+        <v>6</v>
+      </c>
+      <c r="C238" s="13" t="s">
+        <v>221</v>
+      </c>
+      <c r="D238" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="E238" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="F238" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="239" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A239" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="B239" s="12">
+        <v>6</v>
+      </c>
+      <c r="C239" s="12" t="s">
+        <v>242</v>
+      </c>
+      <c r="D239" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="E239" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="F239" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="240" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A240" s="13" t="s">
+        <v>220</v>
+      </c>
+      <c r="B240" s="13">
+        <v>6</v>
+      </c>
+      <c r="C240" s="13" t="s">
+        <v>263</v>
+      </c>
+      <c r="D240" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="E240" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="F240" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="241" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A241" s="13" t="s">
+        <v>220</v>
+      </c>
+      <c r="B241" s="13">
+        <v>6</v>
+      </c>
+      <c r="C241" s="13" t="s">
+        <v>284</v>
+      </c>
+      <c r="D241" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="E241" s="1" t="s">
+        <v>299</v>
+      </c>
+      <c r="F241" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="242" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A242" s="13" t="s">
+        <v>220</v>
+      </c>
+      <c r="B242" s="13">
+        <v>6</v>
+      </c>
+      <c r="C242" s="13" t="s">
+        <v>221</v>
+      </c>
+      <c r="D242" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="E242" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="F242" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="243" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A243" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="B243" s="12">
+        <v>6</v>
+      </c>
+      <c r="C243" s="12" t="s">
+        <v>242</v>
+      </c>
+      <c r="D243" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="E243" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="F243" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="244" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A244" s="13" t="s">
+        <v>220</v>
+      </c>
+      <c r="B244" s="13">
+        <v>6</v>
+      </c>
+      <c r="C244" s="13" t="s">
+        <v>263</v>
+      </c>
+      <c r="D244" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="E244" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="F244" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="245" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A245" s="13" t="s">
+        <v>220</v>
+      </c>
+      <c r="B245" s="13">
+        <v>6</v>
+      </c>
+      <c r="C245" s="13" t="s">
+        <v>284</v>
+      </c>
+      <c r="D245" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="E245" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="F245" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="246" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A246" s="13" t="s">
+        <v>220</v>
+      </c>
+      <c r="B246" s="13">
+        <v>6</v>
+      </c>
+      <c r="C246" s="13" t="s">
+        <v>221</v>
+      </c>
+      <c r="D246" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="E231" t="s">
+      <c r="E246" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="F246" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="247" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A247" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="B247" s="12">
+        <v>6</v>
+      </c>
+      <c r="C247" s="12" t="s">
+        <v>242</v>
+      </c>
+      <c r="D247" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="E247" s="1" t="s">
         <v>259</v>
       </c>
-      <c r="F231" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="232" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A232" s="12" t="s">
-        <v>220</v>
-      </c>
-      <c r="B232" s="12">
-        <v>6</v>
-      </c>
-      <c r="C232" s="12" t="s">
+      <c r="F247" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="248" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A248" s="13" t="s">
+        <v>220</v>
+      </c>
+      <c r="B248" s="13">
+        <v>6</v>
+      </c>
+      <c r="C248" s="13" t="s">
         <v>263</v>
       </c>
-      <c r="D232" s="9" t="s">
+      <c r="D248" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="E232" t="s">
+      <c r="E248" s="1" t="s">
         <v>280</v>
       </c>
-      <c r="F232" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="233" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A233" s="12" t="s">
-        <v>220</v>
-      </c>
-      <c r="B233" s="12">
-        <v>6</v>
-      </c>
-      <c r="C233" s="12" t="s">
+      <c r="F248" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="249" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A249" s="13" t="s">
+        <v>220</v>
+      </c>
+      <c r="B249" s="13">
+        <v>6</v>
+      </c>
+      <c r="C249" s="13" t="s">
+        <v>284</v>
+      </c>
+      <c r="D249" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="E249" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="F249" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="250" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A250" s="13" t="s">
+        <v>220</v>
+      </c>
+      <c r="B250" s="13">
+        <v>6</v>
+      </c>
+      <c r="C250" s="12" t="s">
         <v>221</v>
       </c>
-      <c r="D233" s="9" t="s">
+      <c r="D250" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="E233" t="s">
+      <c r="E250" s="1" t="s">
         <v>239</v>
       </c>
-      <c r="F233" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="234" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A234" s="12" t="s">
-        <v>220</v>
-      </c>
-      <c r="B234" s="12">
-        <v>6</v>
-      </c>
-      <c r="C234" s="12" t="s">
+      <c r="F250" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="251" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A251" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="B251" s="12">
+        <v>6</v>
+      </c>
+      <c r="C251" s="12" t="s">
         <v>242</v>
       </c>
-      <c r="D234" s="9" t="s">
+      <c r="D251" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="E234" t="s">
+      <c r="E251" s="1" t="s">
         <v>260</v>
       </c>
-      <c r="F234" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="235" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A235" s="12" t="s">
-        <v>220</v>
-      </c>
-      <c r="B235" s="12">
-        <v>6</v>
-      </c>
-      <c r="C235" s="12" t="s">
+      <c r="F251" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="252" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A252" s="13" t="s">
+        <v>220</v>
+      </c>
+      <c r="B252" s="13">
+        <v>6</v>
+      </c>
+      <c r="C252" s="13" t="s">
         <v>263</v>
       </c>
-      <c r="D235" s="9" t="s">
+      <c r="D252" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="E235" t="s">
+      <c r="E252" s="1" t="s">
         <v>281</v>
       </c>
-      <c r="F235" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="236" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A236" s="12" t="s">
-        <v>220</v>
-      </c>
-      <c r="B236" s="12">
-        <v>6</v>
-      </c>
-      <c r="C236" s="12" t="s">
+      <c r="F252" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="253" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A253" s="13" t="s">
+        <v>220</v>
+      </c>
+      <c r="B253" s="13">
+        <v>6</v>
+      </c>
+      <c r="C253" s="13" t="s">
+        <v>284</v>
+      </c>
+      <c r="D253" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="E253" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="F253" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="254" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A254" s="13" t="s">
+        <v>220</v>
+      </c>
+      <c r="B254" s="13">
+        <v>6</v>
+      </c>
+      <c r="C254" s="13" t="s">
         <v>221</v>
       </c>
-      <c r="D236" s="9" t="s">
+      <c r="D254" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="E236" t="s">
+      <c r="E254" s="1" t="s">
         <v>240</v>
       </c>
-      <c r="F236" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="237" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A237" s="12" t="s">
-        <v>220</v>
-      </c>
-      <c r="B237" s="12">
-        <v>6</v>
-      </c>
-      <c r="C237" s="12" t="s">
+      <c r="F254" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="255" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A255" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="B255" s="12">
+        <v>6</v>
+      </c>
+      <c r="C255" s="12" t="s">
         <v>242</v>
       </c>
-      <c r="D237" s="9" t="s">
+      <c r="D255" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="E237" t="s">
+      <c r="E255" s="1" t="s">
         <v>261</v>
       </c>
-      <c r="F237" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="238" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A238" s="12" t="s">
-        <v>220</v>
-      </c>
-      <c r="B238" s="12">
-        <v>6</v>
-      </c>
-      <c r="C238" s="12" t="s">
+      <c r="F255" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="256" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A256" s="13" t="s">
+        <v>220</v>
+      </c>
+      <c r="B256" s="13">
+        <v>6</v>
+      </c>
+      <c r="C256" s="13" t="s">
         <v>263</v>
       </c>
-      <c r="D238" s="9" t="s">
+      <c r="D256" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="E238" s="1" t="s">
+      <c r="E256" s="1" t="s">
         <v>282</v>
       </c>
-      <c r="F238" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="239" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A239" s="12" t="s">
-        <v>220</v>
-      </c>
-      <c r="B239" s="12">
-        <v>6</v>
-      </c>
-      <c r="C239" s="12" t="s">
+      <c r="F256" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="257" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A257" s="13" t="s">
+        <v>220</v>
+      </c>
+      <c r="B257" s="13">
+        <v>6</v>
+      </c>
+      <c r="C257" s="13" t="s">
+        <v>284</v>
+      </c>
+      <c r="D257" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="E257" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="F257" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="258" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A258" s="13" t="s">
+        <v>220</v>
+      </c>
+      <c r="B258" s="13">
+        <v>6</v>
+      </c>
+      <c r="C258" s="13" t="s">
         <v>221</v>
       </c>
-      <c r="D239" s="9" t="s">
+      <c r="D258" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="E239" t="s">
+      <c r="E258" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="F239" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="240" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A240" s="12" t="s">
-        <v>220</v>
-      </c>
-      <c r="B240" s="12">
-        <v>6</v>
-      </c>
-      <c r="C240" s="12" t="s">
+      <c r="F258" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="259" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A259" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="B259" s="12">
+        <v>6</v>
+      </c>
+      <c r="C259" s="12" t="s">
         <v>242</v>
       </c>
-      <c r="D240" s="9" t="s">
+      <c r="D259" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="E240" t="s">
+      <c r="E259" s="1" t="s">
         <v>262</v>
       </c>
-      <c r="F240" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="241" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A241" s="12" t="s">
-        <v>220</v>
-      </c>
-      <c r="B241" s="12">
-        <v>6</v>
-      </c>
-      <c r="C241" s="12" t="s">
+      <c r="F259" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="260" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A260" s="13" t="s">
+        <v>220</v>
+      </c>
+      <c r="B260" s="13">
+        <v>6</v>
+      </c>
+      <c r="C260" s="13" t="s">
         <v>263</v>
       </c>
-      <c r="D241" s="9" t="s">
+      <c r="D260" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="E241" t="s">
+      <c r="E260" s="1" t="s">
         <v>283</v>
       </c>
-      <c r="F241" s="1" t="s">
+      <c r="F260" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="261" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A261" s="13" t="s">
+        <v>220</v>
+      </c>
+      <c r="B261" s="13">
+        <v>6</v>
+      </c>
+      <c r="C261" s="13" t="s">
+        <v>284</v>
+      </c>
+      <c r="D261" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E261" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="F261" s="1" t="s">
         <v>69</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add US related to Medicine domain
</commit_message>
<xml_diff>
--- a/refair-server/datasets/few shot dataset/FSDataset.xlsx
+++ b/refair-server/datasets/few shot dataset/FSDataset.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\morel\Desktop\Refair\ReFair-App\refair-server\datasets\few shot dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9EFBE13-4D75-47E4-9B93-65D9E5EBFE37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F85927B-4F7E-468F-BFA0-BCA2F5A88487}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{80773445-FB61-4F04-A882-1600FD96C55A}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1286" uniqueCount="305">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1406" uniqueCount="326">
   <si>
     <t>Domain cluster</t>
   </si>
@@ -951,6 +951,69 @@
   </si>
   <si>
     <t>As a healthcare provider, I want to utilize word embedding techniques to analyze electronic health records (EHRs) and extract meaningful semantic relationships between medical terminologies and patient conditions, improving information retrieval and clinical decision support systems.</t>
+  </si>
+  <si>
+    <t>Medicine</t>
+  </si>
+  <si>
+    <t>As a medical researcher, I want to apply adversarial learning techniques to analyze medical imaging data, so that I can identify and mitigate potential vulnerabilities and ensure the robustness of diagnostic models against adversarial attacks.</t>
+  </si>
+  <si>
+    <t>As a medical researcher, I want to apply CNNs to analyze EEG data and identify patterns indicative of neurological disorders, so that I can assist in early diagnosis and intervention strategies for patients with conditions like epilepsy or Alzheimer's disease.</t>
+  </si>
+  <si>
+    <t>As a medical researcher, I want to deploy a conversational agent for medical students to practice clinical case simulations and receive feedback on diagnostic reasoning and treatment planning, so that I can enhance medical training and competency development.</t>
+  </si>
+  <si>
+    <t>As a medical researcher, I want to utilize decision tree models to analyze patient satisfaction survey data and identify key factors influencing patient experience, so that I can implement quality improvement initiatives to enhance overall patient care and satisfaction.</t>
+  </si>
+  <si>
+    <t>As a medical researcher, I want to use document classification algorithms to categorize medical research papers based on disease types and treatment outcomes, so that I can quickly access relevant literature for evidence-based medicine.</t>
+  </si>
+  <si>
+    <t>As a medical researcher, I want to develop entity extraction models to automatically identify and extract key medical entities (e.g., diseases, medications, symptoms) from clinical notes and patient records, so that I can build comprehensive patient profiles for personalized treatment planning.</t>
+  </si>
+  <si>
+    <t>As a medical researcher, I want to use feature selection algorithms to identify clinical variables (e.g., patient demographics, comorbidities) that significantly impact treatment response in cancer patients, so that I can personalize treatment plans and improve patient outcomes.</t>
+  </si>
+  <si>
+    <t>As a medical researcher, I want to handle imbalanced datasets in predictive models for rare diseases to ensure accurate early detection and timely intervention, so that I can improve patient prognosis and treatment outcomes.</t>
+  </si>
+  <si>
+    <t>As a medical researcher, I want to utilize keyword extraction techniques to analyze patient reviews and feedback regarding healthcare services, extracting key themes and concerns to improve patient satisfaction and quality of care in medical facilities.</t>
+  </si>
+  <si>
+    <t>As a medical researcher, I want to implement k-nearest neighbor algorithms to predict patient outcomes based on similar cases in the electronic health records, so that I can tailor personalized treatment plans and improve patient care management.</t>
+  </si>
+  <si>
+    <t>As a medical researcher, I want to implement a multi-label classification system to classify medical images into multiple categories of abnormalities (e.g., tumors, fractures, inflammation), so that I can assist radiologists in comprehensive diagnosis and treatment planning.</t>
+  </si>
+  <si>
+    <t>As a medical researcher, I want to use a neural network architecture to analyze patient ECG data and predict the risk of cardiac events such as arrhythmias or myocardial infarctions, so that I can implement timely preventive measures and improve patient outcomes.</t>
+  </si>
+  <si>
+    <t>As a medical researcher, I want to utilize random forest algorithms to analyze electronic health records and predict patient outcomes such as hospital readmission or mortality, so that I can identify at-risk patients and improve care management strategies.</t>
+  </si>
+  <si>
+    <t>As a medical researcher, I want to develop a semantic similarity model to compare clinical notes and identify similarities in patient symptoms across different medical specialties, so that I can facilitate interdisciplinary collaboration and holistic patient care.</t>
+  </si>
+  <si>
+    <t>As a medical researcher, I want to use sentiment analysis on social media posts related to mental health conditions to identify trends and public perceptions, so that I can develop targeted mental health awareness campaigns and interventions.</t>
+  </si>
+  <si>
+    <t>As a medical researcher, I want to develop a speech to text system for transcribing patient-doctor consultations accurately, so that I can facilitate comprehensive documentation of medical histories and treatment discussions.</t>
+  </si>
+  <si>
+    <t>As a medical researcher, I want to develop a text categorization system to classify patient electronic health records into different disease categories (e.g., cardiovascular diseases, respiratory disorders), so that I can facilitate epidemiological studies and clinical research</t>
+  </si>
+  <si>
+    <t>As a medical researcher, I want to use unsupervised clustering algorithms to group patient genomic profiles based on shared genetic mutations, so that I can identify genetic subtypes of diseases and personalize treatment approaches in precision medicine.</t>
+  </si>
+  <si>
+    <t>As a medical researcher, I want to develop a voice recognition system to transcribe patient-doctor consultations accurately in real-time, so that I can enhance documentation efficiency and ensure comprehensive medical records.</t>
+  </si>
+  <si>
+    <t>As a medical researcher, I want to apply word embedding techniques to analyze electronic health record narratives and extract meaningful clinical insights (e.g., disease progression markers, treatment effectiveness), so that I can support clinical decision-making and improve patient outcomes.</t>
   </si>
 </sst>
 </file>
@@ -1403,10 +1466,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8DF0B04-8323-4309-B759-D1CDDA1FBB0E}">
-  <dimension ref="A1:F261"/>
+  <dimension ref="A1:F281"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A247" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView tabSelected="1" topLeftCell="A183" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F261" sqref="F261:F281"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1454,6 +1517,9 @@
       <c r="E2" s="1" t="s">
         <v>179</v>
       </c>
+      <c r="F2" s="1" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="3" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
@@ -1471,6 +1537,9 @@
       <c r="E3" s="1" t="s">
         <v>200</v>
       </c>
+      <c r="F3" s="1" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="4" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
@@ -1488,6 +1557,9 @@
       <c r="E4" s="1" t="s">
         <v>180</v>
       </c>
+      <c r="F4" s="1" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="5" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
@@ -1505,6 +1577,9 @@
       <c r="E5" s="1" t="s">
         <v>201</v>
       </c>
+      <c r="F5" s="1" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="6" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
@@ -1522,6 +1597,9 @@
       <c r="E6" s="1" t="s">
         <v>181</v>
       </c>
+      <c r="F6" s="1" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="7" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
@@ -1539,6 +1617,9 @@
       <c r="E7" s="1" t="s">
         <v>202</v>
       </c>
+      <c r="F7" s="1" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="8" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="10" t="s">
@@ -1556,6 +1637,9 @@
       <c r="E8" s="1" t="s">
         <v>182</v>
       </c>
+      <c r="F8" s="1" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="9" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="10" t="s">
@@ -1573,6 +1657,9 @@
       <c r="E9" s="1" t="s">
         <v>203</v>
       </c>
+      <c r="F9" s="1" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="10" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="10" t="s">
@@ -1590,6 +1677,9 @@
       <c r="E10" s="1" t="s">
         <v>183</v>
       </c>
+      <c r="F10" s="1" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="11" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="10" t="s">
@@ -1607,6 +1697,9 @@
       <c r="E11" s="1" t="s">
         <v>204</v>
       </c>
+      <c r="F11" s="1" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="12" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
@@ -1624,6 +1717,9 @@
       <c r="E12" s="1" t="s">
         <v>184</v>
       </c>
+      <c r="F12" s="1" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="13" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="10" t="s">
@@ -1641,6 +1737,9 @@
       <c r="E13" s="1" t="s">
         <v>205</v>
       </c>
+      <c r="F13" s="1" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="14" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="10" t="s">
@@ -1658,6 +1757,9 @@
       <c r="E14" s="1" t="s">
         <v>185</v>
       </c>
+      <c r="F14" s="1" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="15" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="10" t="s">
@@ -1675,6 +1777,9 @@
       <c r="E15" s="1" t="s">
         <v>206</v>
       </c>
+      <c r="F15" s="1" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="16" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="10" t="s">
@@ -1692,6 +1797,9 @@
       <c r="E16" s="1" t="s">
         <v>186</v>
       </c>
+      <c r="F16" s="1" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="17" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="10" t="s">
@@ -1709,6 +1817,9 @@
       <c r="E17" s="1" t="s">
         <v>207</v>
       </c>
+      <c r="F17" s="1" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="18" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="10" t="s">
@@ -1726,6 +1837,9 @@
       <c r="E18" s="1" t="s">
         <v>187</v>
       </c>
+      <c r="F18" s="1" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="19" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="10" t="s">
@@ -1743,6 +1857,9 @@
       <c r="E19" s="1" t="s">
         <v>208</v>
       </c>
+      <c r="F19" s="1" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="20" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="10" t="s">
@@ -1760,6 +1877,9 @@
       <c r="E20" s="1" t="s">
         <v>188</v>
       </c>
+      <c r="F20" s="1" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="21" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="10" t="s">
@@ -1777,6 +1897,9 @@
       <c r="E21" s="1" t="s">
         <v>209</v>
       </c>
+      <c r="F21" s="1" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="22" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="10" t="s">
@@ -5066,53 +5189,53 @@
         <v>6</v>
       </c>
       <c r="C186" s="13" t="s">
+        <v>305</v>
+      </c>
+      <c r="D186" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="E186" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="F186" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="187" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A187" s="13" t="s">
+        <v>220</v>
+      </c>
+      <c r="B187" s="13">
+        <v>6</v>
+      </c>
+      <c r="C187" s="13" t="s">
         <v>221</v>
-      </c>
-      <c r="D186" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="E186" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="F186" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="187" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A187" s="12" t="s">
-        <v>220</v>
-      </c>
-      <c r="B187" s="12">
-        <v>6</v>
-      </c>
-      <c r="C187" s="12" t="s">
-        <v>242</v>
       </c>
       <c r="D187" s="9" t="s">
         <v>43</v>
       </c>
       <c r="E187" s="1" t="s">
-        <v>244</v>
+        <v>223</v>
       </c>
       <c r="F187" s="1" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="188" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A188" s="13" t="s">
-        <v>220</v>
-      </c>
-      <c r="B188" s="13">
-        <v>6</v>
-      </c>
-      <c r="C188" s="13" t="s">
-        <v>263</v>
+      <c r="A188" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="B188" s="12">
+        <v>6</v>
+      </c>
+      <c r="C188" s="12" t="s">
+        <v>242</v>
       </c>
       <c r="D188" s="9" t="s">
         <v>43</v>
       </c>
       <c r="E188" s="1" t="s">
-        <v>265</v>
+        <v>244</v>
       </c>
       <c r="F188" s="1" t="s">
         <v>69</v>
@@ -5126,13 +5249,13 @@
         <v>6</v>
       </c>
       <c r="C189" s="13" t="s">
-        <v>284</v>
+        <v>263</v>
       </c>
       <c r="D189" s="9" t="s">
         <v>43</v>
       </c>
       <c r="E189" s="1" t="s">
-        <v>286</v>
+        <v>265</v>
       </c>
       <c r="F189" s="1" t="s">
         <v>69</v>
@@ -5146,33 +5269,33 @@
         <v>6</v>
       </c>
       <c r="C190" s="13" t="s">
-        <v>221</v>
+        <v>284</v>
       </c>
       <c r="D190" s="9" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="E190" s="1" t="s">
-        <v>224</v>
+        <v>286</v>
       </c>
       <c r="F190" s="1" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="191" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A191" s="12" t="s">
-        <v>220</v>
-      </c>
-      <c r="B191" s="12">
-        <v>6</v>
-      </c>
-      <c r="C191" s="12" t="s">
-        <v>242</v>
+      <c r="A191" s="13" t="s">
+        <v>220</v>
+      </c>
+      <c r="B191" s="13">
+        <v>6</v>
+      </c>
+      <c r="C191" s="13" t="s">
+        <v>305</v>
       </c>
       <c r="D191" s="9" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="E191" s="1" t="s">
-        <v>245</v>
+        <v>307</v>
       </c>
       <c r="F191" s="1" t="s">
         <v>69</v>
@@ -5186,33 +5309,33 @@
         <v>6</v>
       </c>
       <c r="C192" s="13" t="s">
-        <v>263</v>
+        <v>221</v>
       </c>
       <c r="D192" s="9" t="s">
         <v>30</v>
       </c>
       <c r="E192" s="1" t="s">
-        <v>266</v>
+        <v>224</v>
       </c>
       <c r="F192" s="1" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="193" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A193" s="13" t="s">
-        <v>220</v>
-      </c>
-      <c r="B193" s="13">
-        <v>6</v>
-      </c>
-      <c r="C193" s="13" t="s">
-        <v>284</v>
+      <c r="A193" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="B193" s="12">
+        <v>6</v>
+      </c>
+      <c r="C193" s="12" t="s">
+        <v>242</v>
       </c>
       <c r="D193" s="9" t="s">
         <v>30</v>
       </c>
       <c r="E193" s="1" t="s">
-        <v>287</v>
+        <v>245</v>
       </c>
       <c r="F193" s="1" t="s">
         <v>69</v>
@@ -5226,33 +5349,33 @@
         <v>6</v>
       </c>
       <c r="C194" s="13" t="s">
-        <v>221</v>
+        <v>263</v>
       </c>
       <c r="D194" s="9" t="s">
-        <v>13</v>
+        <v>30</v>
       </c>
       <c r="E194" s="1" t="s">
-        <v>225</v>
+        <v>266</v>
       </c>
       <c r="F194" s="1" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="195" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A195" s="12" t="s">
-        <v>220</v>
-      </c>
-      <c r="B195" s="12">
-        <v>6</v>
-      </c>
-      <c r="C195" s="12" t="s">
-        <v>242</v>
+      <c r="A195" s="13" t="s">
+        <v>220</v>
+      </c>
+      <c r="B195" s="13">
+        <v>6</v>
+      </c>
+      <c r="C195" s="13" t="s">
+        <v>284</v>
       </c>
       <c r="D195" s="9" t="s">
-        <v>13</v>
+        <v>30</v>
       </c>
       <c r="E195" s="1" t="s">
-        <v>246</v>
+        <v>287</v>
       </c>
       <c r="F195" s="1" t="s">
         <v>69</v>
@@ -5266,13 +5389,13 @@
         <v>6</v>
       </c>
       <c r="C196" s="13" t="s">
-        <v>263</v>
+        <v>305</v>
       </c>
       <c r="D196" s="9" t="s">
-        <v>13</v>
+        <v>30</v>
       </c>
       <c r="E196" s="1" t="s">
-        <v>267</v>
+        <v>308</v>
       </c>
       <c r="F196" s="1" t="s">
         <v>69</v>
@@ -5286,53 +5409,53 @@
         <v>6</v>
       </c>
       <c r="C197" s="13" t="s">
-        <v>284</v>
+        <v>221</v>
       </c>
       <c r="D197" s="9" t="s">
         <v>13</v>
       </c>
       <c r="E197" s="1" t="s">
-        <v>288</v>
+        <v>225</v>
       </c>
       <c r="F197" s="1" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="198" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A198" s="13" t="s">
-        <v>220</v>
-      </c>
-      <c r="B198" s="13">
-        <v>6</v>
-      </c>
-      <c r="C198" s="13" t="s">
-        <v>221</v>
+      <c r="A198" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="B198" s="12">
+        <v>6</v>
+      </c>
+      <c r="C198" s="12" t="s">
+        <v>242</v>
       </c>
       <c r="D198" s="9" t="s">
-        <v>46</v>
+        <v>13</v>
       </c>
       <c r="E198" s="1" t="s">
-        <v>226</v>
+        <v>246</v>
       </c>
       <c r="F198" s="1" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="199" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A199" s="12" t="s">
-        <v>220</v>
-      </c>
-      <c r="B199" s="12">
-        <v>6</v>
-      </c>
-      <c r="C199" s="12" t="s">
-        <v>242</v>
+      <c r="A199" s="13" t="s">
+        <v>220</v>
+      </c>
+      <c r="B199" s="13">
+        <v>6</v>
+      </c>
+      <c r="C199" s="13" t="s">
+        <v>263</v>
       </c>
       <c r="D199" s="9" t="s">
-        <v>46</v>
+        <v>13</v>
       </c>
       <c r="E199" s="1" t="s">
-        <v>247</v>
+        <v>267</v>
       </c>
       <c r="F199" s="1" t="s">
         <v>69</v>
@@ -5346,13 +5469,13 @@
         <v>6</v>
       </c>
       <c r="C200" s="13" t="s">
-        <v>263</v>
+        <v>284</v>
       </c>
       <c r="D200" s="9" t="s">
-        <v>46</v>
+        <v>13</v>
       </c>
       <c r="E200" s="1" t="s">
-        <v>268</v>
+        <v>288</v>
       </c>
       <c r="F200" s="1" t="s">
         <v>69</v>
@@ -5366,13 +5489,13 @@
         <v>6</v>
       </c>
       <c r="C201" s="13" t="s">
-        <v>284</v>
+        <v>305</v>
       </c>
       <c r="D201" s="9" t="s">
-        <v>46</v>
+        <v>13</v>
       </c>
       <c r="E201" s="1" t="s">
-        <v>289</v>
+        <v>309</v>
       </c>
       <c r="F201" s="1" t="s">
         <v>69</v>
@@ -5389,10 +5512,10 @@
         <v>221</v>
       </c>
       <c r="D202" s="9" t="s">
-        <v>33</v>
+        <v>46</v>
       </c>
       <c r="E202" s="1" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="F202" s="1" t="s">
         <v>69</v>
@@ -5409,10 +5532,10 @@
         <v>242</v>
       </c>
       <c r="D203" s="9" t="s">
-        <v>33</v>
+        <v>46</v>
       </c>
       <c r="E203" s="1" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="F203" s="1" t="s">
         <v>69</v>
@@ -5429,10 +5552,10 @@
         <v>263</v>
       </c>
       <c r="D204" s="9" t="s">
-        <v>33</v>
+        <v>46</v>
       </c>
       <c r="E204" s="1" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="F204" s="1" t="s">
         <v>69</v>
@@ -5449,10 +5572,10 @@
         <v>284</v>
       </c>
       <c r="D205" s="9" t="s">
-        <v>33</v>
+        <v>46</v>
       </c>
       <c r="E205" s="1" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="F205" s="1" t="s">
         <v>69</v>
@@ -5466,53 +5589,53 @@
         <v>6</v>
       </c>
       <c r="C206" s="13" t="s">
+        <v>305</v>
+      </c>
+      <c r="D206" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="E206" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="F206" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="207" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A207" s="13" t="s">
+        <v>220</v>
+      </c>
+      <c r="B207" s="13">
+        <v>6</v>
+      </c>
+      <c r="C207" s="13" t="s">
         <v>221</v>
       </c>
-      <c r="D206" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="E206" s="1" t="s">
-        <v>228</v>
-      </c>
-      <c r="F206" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="207" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A207" s="12" t="s">
-        <v>220</v>
-      </c>
-      <c r="B207" s="12">
-        <v>6</v>
-      </c>
-      <c r="C207" s="12" t="s">
+      <c r="D207" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="E207" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="F207" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="208" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A208" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="B208" s="12">
+        <v>6</v>
+      </c>
+      <c r="C208" s="12" t="s">
         <v>242</v>
       </c>
-      <c r="D207" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="E207" s="1" t="s">
-        <v>249</v>
-      </c>
-      <c r="F207" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="208" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A208" s="13" t="s">
-        <v>220</v>
-      </c>
-      <c r="B208" s="13">
-        <v>6</v>
-      </c>
-      <c r="C208" s="13" t="s">
-        <v>263</v>
-      </c>
       <c r="D208" s="9" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E208" s="1" t="s">
-        <v>270</v>
+        <v>248</v>
       </c>
       <c r="F208" s="1" t="s">
         <v>69</v>
@@ -5526,13 +5649,13 @@
         <v>6</v>
       </c>
       <c r="C209" s="13" t="s">
-        <v>284</v>
+        <v>263</v>
       </c>
       <c r="D209" s="9" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E209" s="1" t="s">
-        <v>291</v>
+        <v>269</v>
       </c>
       <c r="F209" s="1" t="s">
         <v>69</v>
@@ -5546,33 +5669,33 @@
         <v>6</v>
       </c>
       <c r="C210" s="13" t="s">
-        <v>221</v>
+        <v>284</v>
       </c>
       <c r="D210" s="9" t="s">
-        <v>14</v>
+        <v>33</v>
       </c>
       <c r="E210" s="1" t="s">
-        <v>229</v>
+        <v>290</v>
       </c>
       <c r="F210" s="1" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="211" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A211" s="12" t="s">
-        <v>220</v>
-      </c>
-      <c r="B211" s="12">
-        <v>6</v>
-      </c>
-      <c r="C211" s="12" t="s">
-        <v>242</v>
+      <c r="A211" s="13" t="s">
+        <v>220</v>
+      </c>
+      <c r="B211" s="13">
+        <v>6</v>
+      </c>
+      <c r="C211" s="13" t="s">
+        <v>305</v>
       </c>
       <c r="D211" s="9" t="s">
-        <v>14</v>
+        <v>33</v>
       </c>
       <c r="E211" s="1" t="s">
-        <v>250</v>
+        <v>311</v>
       </c>
       <c r="F211" s="1" t="s">
         <v>69</v>
@@ -5586,33 +5709,33 @@
         <v>6</v>
       </c>
       <c r="C212" s="13" t="s">
-        <v>263</v>
+        <v>221</v>
       </c>
       <c r="D212" s="9" t="s">
-        <v>14</v>
+        <v>36</v>
       </c>
       <c r="E212" s="1" t="s">
-        <v>271</v>
+        <v>228</v>
       </c>
       <c r="F212" s="1" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="213" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A213" s="13" t="s">
-        <v>220</v>
-      </c>
-      <c r="B213" s="13">
-        <v>6</v>
-      </c>
-      <c r="C213" s="13" t="s">
-        <v>284</v>
+      <c r="A213" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="B213" s="12">
+        <v>6</v>
+      </c>
+      <c r="C213" s="12" t="s">
+        <v>242</v>
       </c>
       <c r="D213" s="9" t="s">
-        <v>14</v>
+        <v>36</v>
       </c>
       <c r="E213" s="1" t="s">
-        <v>292</v>
+        <v>249</v>
       </c>
       <c r="F213" s="1" t="s">
         <v>69</v>
@@ -5626,33 +5749,33 @@
         <v>6</v>
       </c>
       <c r="C214" s="13" t="s">
-        <v>221</v>
+        <v>263</v>
       </c>
       <c r="D214" s="9" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="E214" s="1" t="s">
-        <v>230</v>
+        <v>270</v>
       </c>
       <c r="F214" s="1" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="215" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A215" s="12" t="s">
-        <v>220</v>
-      </c>
-      <c r="B215" s="12">
-        <v>6</v>
-      </c>
-      <c r="C215" s="12" t="s">
-        <v>242</v>
+      <c r="A215" s="13" t="s">
+        <v>220</v>
+      </c>
+      <c r="B215" s="13">
+        <v>6</v>
+      </c>
+      <c r="C215" s="13" t="s">
+        <v>284</v>
       </c>
       <c r="D215" s="9" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="E215" s="1" t="s">
-        <v>251</v>
+        <v>291</v>
       </c>
       <c r="F215" s="1" t="s">
         <v>69</v>
@@ -5666,13 +5789,13 @@
         <v>6</v>
       </c>
       <c r="C216" s="13" t="s">
-        <v>263</v>
+        <v>305</v>
       </c>
       <c r="D216" s="9" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="E216" s="1" t="s">
-        <v>272</v>
+        <v>312</v>
       </c>
       <c r="F216" s="1" t="s">
         <v>69</v>
@@ -5686,53 +5809,53 @@
         <v>6</v>
       </c>
       <c r="C217" s="13" t="s">
-        <v>284</v>
+        <v>221</v>
       </c>
       <c r="D217" s="9" t="s">
-        <v>34</v>
+        <v>14</v>
       </c>
       <c r="E217" s="1" t="s">
-        <v>293</v>
+        <v>229</v>
       </c>
       <c r="F217" s="1" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="218" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A218" s="13" t="s">
-        <v>220</v>
-      </c>
-      <c r="B218" s="13">
-        <v>6</v>
-      </c>
-      <c r="C218" s="13" t="s">
-        <v>221</v>
+      <c r="A218" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="B218" s="12">
+        <v>6</v>
+      </c>
+      <c r="C218" s="12" t="s">
+        <v>242</v>
       </c>
       <c r="D218" s="9" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E218" s="1" t="s">
-        <v>231</v>
+        <v>250</v>
       </c>
       <c r="F218" s="1" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="219" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A219" s="12" t="s">
-        <v>220</v>
-      </c>
-      <c r="B219" s="12">
-        <v>6</v>
-      </c>
-      <c r="C219" s="12" t="s">
-        <v>242</v>
+      <c r="A219" s="13" t="s">
+        <v>220</v>
+      </c>
+      <c r="B219" s="13">
+        <v>6</v>
+      </c>
+      <c r="C219" s="13" t="s">
+        <v>263</v>
       </c>
       <c r="D219" s="9" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E219" s="1" t="s">
-        <v>252</v>
+        <v>271</v>
       </c>
       <c r="F219" s="1" t="s">
         <v>69</v>
@@ -5746,13 +5869,13 @@
         <v>6</v>
       </c>
       <c r="C220" s="13" t="s">
-        <v>263</v>
+        <v>284</v>
       </c>
       <c r="D220" s="9" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E220" s="1" t="s">
-        <v>273</v>
+        <v>292</v>
       </c>
       <c r="F220" s="1" t="s">
         <v>69</v>
@@ -5766,13 +5889,13 @@
         <v>6</v>
       </c>
       <c r="C221" s="13" t="s">
-        <v>284</v>
+        <v>305</v>
       </c>
       <c r="D221" s="9" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E221" s="1" t="s">
-        <v>294</v>
+        <v>313</v>
       </c>
       <c r="F221" s="1" t="s">
         <v>69</v>
@@ -5789,10 +5912,10 @@
         <v>221</v>
       </c>
       <c r="D222" s="9" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="E222" s="1" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="F222" s="1" t="s">
         <v>69</v>
@@ -5809,10 +5932,10 @@
         <v>242</v>
       </c>
       <c r="D223" s="9" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="E223" s="1" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="F223" s="1" t="s">
         <v>69</v>
@@ -5829,10 +5952,10 @@
         <v>263</v>
       </c>
       <c r="D224" s="9" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="E224" s="1" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="F224" s="1" t="s">
         <v>69</v>
@@ -5849,10 +5972,10 @@
         <v>284</v>
       </c>
       <c r="D225" s="9" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="E225" s="1" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="F225" s="1" t="s">
         <v>69</v>
@@ -5866,53 +5989,53 @@
         <v>6</v>
       </c>
       <c r="C226" s="13" t="s">
+        <v>305</v>
+      </c>
+      <c r="D226" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="E226" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="F226" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="227" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A227" s="13" t="s">
+        <v>220</v>
+      </c>
+      <c r="B227" s="13">
+        <v>6</v>
+      </c>
+      <c r="C227" s="13" t="s">
         <v>221</v>
       </c>
-      <c r="D226" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="E226" s="1" t="s">
-        <v>233</v>
-      </c>
-      <c r="F226" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="227" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A227" s="12" t="s">
-        <v>220</v>
-      </c>
-      <c r="B227" s="12">
-        <v>6</v>
-      </c>
-      <c r="C227" s="12" t="s">
+      <c r="D227" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="E227" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="F227" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="228" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A228" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="B228" s="12">
+        <v>6</v>
+      </c>
+      <c r="C228" s="12" t="s">
         <v>242</v>
       </c>
-      <c r="D227" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="E227" s="1" t="s">
-        <v>254</v>
-      </c>
-      <c r="F227" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="228" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A228" s="13" t="s">
-        <v>220</v>
-      </c>
-      <c r="B228" s="13">
-        <v>6</v>
-      </c>
-      <c r="C228" s="13" t="s">
-        <v>263</v>
-      </c>
       <c r="D228" s="9" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E228" s="1" t="s">
-        <v>275</v>
+        <v>252</v>
       </c>
       <c r="F228" s="1" t="s">
         <v>69</v>
@@ -5926,13 +6049,13 @@
         <v>6</v>
       </c>
       <c r="C229" s="13" t="s">
-        <v>284</v>
+        <v>263</v>
       </c>
       <c r="D229" s="9" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E229" s="1" t="s">
-        <v>296</v>
+        <v>273</v>
       </c>
       <c r="F229" s="1" t="s">
         <v>69</v>
@@ -5946,33 +6069,33 @@
         <v>6</v>
       </c>
       <c r="C230" s="13" t="s">
-        <v>221</v>
+        <v>284</v>
       </c>
       <c r="D230" s="9" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="E230" s="1" t="s">
-        <v>234</v>
+        <v>294</v>
       </c>
       <c r="F230" s="1" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="231" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A231" s="12" t="s">
-        <v>220</v>
-      </c>
-      <c r="B231" s="12">
-        <v>6</v>
-      </c>
-      <c r="C231" s="12" t="s">
-        <v>242</v>
+      <c r="A231" s="13" t="s">
+        <v>220</v>
+      </c>
+      <c r="B231" s="13">
+        <v>6</v>
+      </c>
+      <c r="C231" s="13" t="s">
+        <v>305</v>
       </c>
       <c r="D231" s="9" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="E231" s="1" t="s">
-        <v>255</v>
+        <v>315</v>
       </c>
       <c r="F231" s="1" t="s">
         <v>69</v>
@@ -5986,33 +6109,33 @@
         <v>6</v>
       </c>
       <c r="C232" s="13" t="s">
-        <v>263</v>
+        <v>221</v>
       </c>
       <c r="D232" s="9" t="s">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="E232" s="1" t="s">
-        <v>276</v>
+        <v>232</v>
       </c>
       <c r="F232" s="1" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="233" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A233" s="13" t="s">
-        <v>220</v>
-      </c>
-      <c r="B233" s="13">
-        <v>6</v>
-      </c>
-      <c r="C233" s="13" t="s">
-        <v>284</v>
+      <c r="A233" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="B233" s="12">
+        <v>6</v>
+      </c>
+      <c r="C233" s="12" t="s">
+        <v>242</v>
       </c>
       <c r="D233" s="9" t="s">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="E233" s="1" t="s">
-        <v>297</v>
+        <v>253</v>
       </c>
       <c r="F233" s="1" t="s">
         <v>69</v>
@@ -6026,33 +6149,33 @@
         <v>6</v>
       </c>
       <c r="C234" s="13" t="s">
-        <v>221</v>
+        <v>263</v>
       </c>
       <c r="D234" s="9" t="s">
-        <v>22</v>
+        <v>40</v>
       </c>
       <c r="E234" s="1" t="s">
-        <v>235</v>
+        <v>274</v>
       </c>
       <c r="F234" s="1" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="235" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A235" s="12" t="s">
-        <v>220</v>
-      </c>
-      <c r="B235" s="12">
-        <v>6</v>
-      </c>
-      <c r="C235" s="12" t="s">
-        <v>242</v>
+      <c r="A235" s="13" t="s">
+        <v>220</v>
+      </c>
+      <c r="B235" s="13">
+        <v>6</v>
+      </c>
+      <c r="C235" s="13" t="s">
+        <v>284</v>
       </c>
       <c r="D235" s="9" t="s">
-        <v>22</v>
+        <v>40</v>
       </c>
       <c r="E235" s="1" t="s">
-        <v>256</v>
+        <v>295</v>
       </c>
       <c r="F235" s="1" t="s">
         <v>69</v>
@@ -6066,13 +6189,13 @@
         <v>6</v>
       </c>
       <c r="C236" s="13" t="s">
-        <v>263</v>
+        <v>305</v>
       </c>
       <c r="D236" s="9" t="s">
-        <v>22</v>
+        <v>40</v>
       </c>
       <c r="E236" s="1" t="s">
-        <v>277</v>
+        <v>316</v>
       </c>
       <c r="F236" s="1" t="s">
         <v>69</v>
@@ -6086,53 +6209,53 @@
         <v>6</v>
       </c>
       <c r="C237" s="13" t="s">
-        <v>284</v>
+        <v>221</v>
       </c>
       <c r="D237" s="9" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="E237" s="1" t="s">
-        <v>298</v>
+        <v>233</v>
       </c>
       <c r="F237" s="1" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="238" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A238" s="13" t="s">
-        <v>220</v>
-      </c>
-      <c r="B238" s="13">
-        <v>6</v>
-      </c>
-      <c r="C238" s="13" t="s">
-        <v>221</v>
+      <c r="A238" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="B238" s="12">
+        <v>6</v>
+      </c>
+      <c r="C238" s="12" t="s">
+        <v>242</v>
       </c>
       <c r="D238" s="9" t="s">
-        <v>38</v>
+        <v>18</v>
       </c>
       <c r="E238" s="1" t="s">
-        <v>236</v>
+        <v>254</v>
       </c>
       <c r="F238" s="1" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="239" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A239" s="12" t="s">
-        <v>220</v>
-      </c>
-      <c r="B239" s="12">
-        <v>6</v>
-      </c>
-      <c r="C239" s="12" t="s">
-        <v>242</v>
+      <c r="A239" s="13" t="s">
+        <v>220</v>
+      </c>
+      <c r="B239" s="13">
+        <v>6</v>
+      </c>
+      <c r="C239" s="13" t="s">
+        <v>263</v>
       </c>
       <c r="D239" s="9" t="s">
-        <v>38</v>
+        <v>18</v>
       </c>
       <c r="E239" s="1" t="s">
-        <v>257</v>
+        <v>275</v>
       </c>
       <c r="F239" s="1" t="s">
         <v>69</v>
@@ -6146,13 +6269,13 @@
         <v>6</v>
       </c>
       <c r="C240" s="13" t="s">
-        <v>263</v>
+        <v>284</v>
       </c>
       <c r="D240" s="9" t="s">
-        <v>38</v>
+        <v>18</v>
       </c>
       <c r="E240" s="1" t="s">
-        <v>278</v>
+        <v>296</v>
       </c>
       <c r="F240" s="1" t="s">
         <v>69</v>
@@ -6166,13 +6289,13 @@
         <v>6</v>
       </c>
       <c r="C241" s="13" t="s">
-        <v>284</v>
+        <v>305</v>
       </c>
       <c r="D241" s="9" t="s">
-        <v>38</v>
+        <v>18</v>
       </c>
       <c r="E241" s="1" t="s">
-        <v>299</v>
+        <v>317</v>
       </c>
       <c r="F241" s="1" t="s">
         <v>69</v>
@@ -6189,10 +6312,10 @@
         <v>221</v>
       </c>
       <c r="D242" s="9" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="E242" s="1" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="F242" s="1" t="s">
         <v>69</v>
@@ -6209,10 +6332,10 @@
         <v>242</v>
       </c>
       <c r="D243" s="9" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="E243" s="1" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="F243" s="1" t="s">
         <v>69</v>
@@ -6229,10 +6352,10 @@
         <v>263</v>
       </c>
       <c r="D244" s="9" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="E244" s="1" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="F244" s="1" t="s">
         <v>69</v>
@@ -6249,10 +6372,10 @@
         <v>284</v>
       </c>
       <c r="D245" s="9" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="E245" s="1" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="F245" s="1" t="s">
         <v>69</v>
@@ -6266,53 +6389,53 @@
         <v>6</v>
       </c>
       <c r="C246" s="13" t="s">
+        <v>305</v>
+      </c>
+      <c r="D246" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="E246" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="F246" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="247" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A247" s="13" t="s">
+        <v>220</v>
+      </c>
+      <c r="B247" s="13">
+        <v>6</v>
+      </c>
+      <c r="C247" s="13" t="s">
         <v>221</v>
       </c>
-      <c r="D246" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="E246" s="1" t="s">
-        <v>238</v>
-      </c>
-      <c r="F246" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="247" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A247" s="12" t="s">
-        <v>220</v>
-      </c>
-      <c r="B247" s="12">
-        <v>6</v>
-      </c>
-      <c r="C247" s="12" t="s">
+      <c r="D247" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="E247" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="F247" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="248" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A248" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="B248" s="12">
+        <v>6</v>
+      </c>
+      <c r="C248" s="12" t="s">
         <v>242</v>
       </c>
-      <c r="D247" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="E247" s="1" t="s">
-        <v>259</v>
-      </c>
-      <c r="F247" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="248" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A248" s="13" t="s">
-        <v>220</v>
-      </c>
-      <c r="B248" s="13">
-        <v>6</v>
-      </c>
-      <c r="C248" s="13" t="s">
-        <v>263</v>
-      </c>
       <c r="D248" s="9" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="E248" s="1" t="s">
-        <v>280</v>
+        <v>256</v>
       </c>
       <c r="F248" s="1" t="s">
         <v>69</v>
@@ -6326,13 +6449,13 @@
         <v>6</v>
       </c>
       <c r="C249" s="13" t="s">
-        <v>284</v>
+        <v>263</v>
       </c>
       <c r="D249" s="9" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="E249" s="1" t="s">
-        <v>301</v>
+        <v>277</v>
       </c>
       <c r="F249" s="1" t="s">
         <v>69</v>
@@ -6345,34 +6468,34 @@
       <c r="B250" s="13">
         <v>6</v>
       </c>
-      <c r="C250" s="12" t="s">
-        <v>221</v>
+      <c r="C250" s="13" t="s">
+        <v>284</v>
       </c>
       <c r="D250" s="9" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="E250" s="1" t="s">
-        <v>239</v>
+        <v>298</v>
       </c>
       <c r="F250" s="1" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="251" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A251" s="12" t="s">
-        <v>220</v>
-      </c>
-      <c r="B251" s="12">
-        <v>6</v>
-      </c>
-      <c r="C251" s="12" t="s">
-        <v>242</v>
+      <c r="A251" s="13" t="s">
+        <v>220</v>
+      </c>
+      <c r="B251" s="13">
+        <v>6</v>
+      </c>
+      <c r="C251" s="13" t="s">
+        <v>305</v>
       </c>
       <c r="D251" s="9" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="E251" s="1" t="s">
-        <v>260</v>
+        <v>319</v>
       </c>
       <c r="F251" s="1" t="s">
         <v>69</v>
@@ -6386,33 +6509,33 @@
         <v>6</v>
       </c>
       <c r="C252" s="13" t="s">
-        <v>263</v>
+        <v>221</v>
       </c>
       <c r="D252" s="9" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="E252" s="1" t="s">
-        <v>281</v>
+        <v>236</v>
       </c>
       <c r="F252" s="1" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="253" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A253" s="13" t="s">
-        <v>220</v>
-      </c>
-      <c r="B253" s="13">
-        <v>6</v>
-      </c>
-      <c r="C253" s="13" t="s">
-        <v>284</v>
+      <c r="A253" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="B253" s="12">
+        <v>6</v>
+      </c>
+      <c r="C253" s="12" t="s">
+        <v>242</v>
       </c>
       <c r="D253" s="9" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="E253" s="1" t="s">
-        <v>302</v>
+        <v>257</v>
       </c>
       <c r="F253" s="1" t="s">
         <v>69</v>
@@ -6426,33 +6549,33 @@
         <v>6</v>
       </c>
       <c r="C254" s="13" t="s">
-        <v>221</v>
+        <v>263</v>
       </c>
       <c r="D254" s="9" t="s">
-        <v>7</v>
+        <v>38</v>
       </c>
       <c r="E254" s="1" t="s">
-        <v>240</v>
+        <v>278</v>
       </c>
       <c r="F254" s="1" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="255" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A255" s="12" t="s">
-        <v>220</v>
-      </c>
-      <c r="B255" s="12">
-        <v>6</v>
-      </c>
-      <c r="C255" s="12" t="s">
-        <v>242</v>
+      <c r="A255" s="13" t="s">
+        <v>220</v>
+      </c>
+      <c r="B255" s="13">
+        <v>6</v>
+      </c>
+      <c r="C255" s="13" t="s">
+        <v>284</v>
       </c>
       <c r="D255" s="9" t="s">
-        <v>7</v>
+        <v>38</v>
       </c>
       <c r="E255" s="1" t="s">
-        <v>261</v>
+        <v>299</v>
       </c>
       <c r="F255" s="1" t="s">
         <v>69</v>
@@ -6466,13 +6589,13 @@
         <v>6</v>
       </c>
       <c r="C256" s="13" t="s">
-        <v>263</v>
+        <v>305</v>
       </c>
       <c r="D256" s="9" t="s">
-        <v>7</v>
+        <v>38</v>
       </c>
       <c r="E256" s="1" t="s">
-        <v>282</v>
+        <v>320</v>
       </c>
       <c r="F256" s="1" t="s">
         <v>69</v>
@@ -6486,53 +6609,53 @@
         <v>6</v>
       </c>
       <c r="C257" s="13" t="s">
-        <v>284</v>
+        <v>221</v>
       </c>
       <c r="D257" s="9" t="s">
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="E257" s="1" t="s">
-        <v>303</v>
+        <v>237</v>
       </c>
       <c r="F257" s="1" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="258" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A258" s="13" t="s">
-        <v>220</v>
-      </c>
-      <c r="B258" s="13">
-        <v>6</v>
-      </c>
-      <c r="C258" s="13" t="s">
-        <v>221</v>
+      <c r="A258" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="B258" s="12">
+        <v>6</v>
+      </c>
+      <c r="C258" s="12" t="s">
+        <v>242</v>
       </c>
       <c r="D258" s="9" t="s">
-        <v>9</v>
+        <v>24</v>
       </c>
       <c r="E258" s="1" t="s">
-        <v>241</v>
+        <v>258</v>
       </c>
       <c r="F258" s="1" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="259" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A259" s="12" t="s">
-        <v>220</v>
-      </c>
-      <c r="B259" s="12">
-        <v>6</v>
-      </c>
-      <c r="C259" s="12" t="s">
-        <v>242</v>
+      <c r="A259" s="13" t="s">
+        <v>220</v>
+      </c>
+      <c r="B259" s="13">
+        <v>6</v>
+      </c>
+      <c r="C259" s="13" t="s">
+        <v>263</v>
       </c>
       <c r="D259" s="9" t="s">
-        <v>9</v>
+        <v>24</v>
       </c>
       <c r="E259" s="1" t="s">
-        <v>262</v>
+        <v>279</v>
       </c>
       <c r="F259" s="1" t="s">
         <v>69</v>
@@ -6546,13 +6669,13 @@
         <v>6</v>
       </c>
       <c r="C260" s="13" t="s">
-        <v>263</v>
+        <v>284</v>
       </c>
       <c r="D260" s="9" t="s">
-        <v>9</v>
+        <v>24</v>
       </c>
       <c r="E260" s="1" t="s">
-        <v>283</v>
+        <v>300</v>
       </c>
       <c r="F260" s="1" t="s">
         <v>69</v>
@@ -6566,15 +6689,415 @@
         <v>6</v>
       </c>
       <c r="C261" s="13" t="s">
+        <v>305</v>
+      </c>
+      <c r="D261" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="E261" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="F261" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="262" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A262" s="13" t="s">
+        <v>220</v>
+      </c>
+      <c r="B262" s="13">
+        <v>6</v>
+      </c>
+      <c r="C262" s="13" t="s">
+        <v>221</v>
+      </c>
+      <c r="D262" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="E262" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="F262" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="263" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A263" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="B263" s="12">
+        <v>6</v>
+      </c>
+      <c r="C263" s="12" t="s">
+        <v>242</v>
+      </c>
+      <c r="D263" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="E263" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="F263" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="264" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A264" s="13" t="s">
+        <v>220</v>
+      </c>
+      <c r="B264" s="13">
+        <v>6</v>
+      </c>
+      <c r="C264" s="13" t="s">
+        <v>263</v>
+      </c>
+      <c r="D264" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="E264" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="F264" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="265" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A265" s="13" t="s">
+        <v>220</v>
+      </c>
+      <c r="B265" s="13">
+        <v>6</v>
+      </c>
+      <c r="C265" s="13" t="s">
         <v>284</v>
       </c>
-      <c r="D261" s="9" t="s">
+      <c r="D265" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="E265" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="F265" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="266" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A266" s="13" t="s">
+        <v>220</v>
+      </c>
+      <c r="B266" s="13">
+        <v>6</v>
+      </c>
+      <c r="C266" s="13" t="s">
+        <v>305</v>
+      </c>
+      <c r="D266" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="E266" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="F266" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="267" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A267" s="13" t="s">
+        <v>220</v>
+      </c>
+      <c r="B267" s="13">
+        <v>6</v>
+      </c>
+      <c r="C267" s="12" t="s">
+        <v>221</v>
+      </c>
+      <c r="D267" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="E267" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="F267" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="268" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A268" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="B268" s="12">
+        <v>6</v>
+      </c>
+      <c r="C268" s="12" t="s">
+        <v>242</v>
+      </c>
+      <c r="D268" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="E268" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="F268" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="269" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A269" s="13" t="s">
+        <v>220</v>
+      </c>
+      <c r="B269" s="13">
+        <v>6</v>
+      </c>
+      <c r="C269" s="13" t="s">
+        <v>263</v>
+      </c>
+      <c r="D269" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="E269" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="F269" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="270" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A270" s="13" t="s">
+        <v>220</v>
+      </c>
+      <c r="B270" s="13">
+        <v>6</v>
+      </c>
+      <c r="C270" s="13" t="s">
+        <v>284</v>
+      </c>
+      <c r="D270" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="E270" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="F270" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="271" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A271" s="13" t="s">
+        <v>220</v>
+      </c>
+      <c r="B271" s="13">
+        <v>6</v>
+      </c>
+      <c r="C271" s="13" t="s">
+        <v>305</v>
+      </c>
+      <c r="D271" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="E271" s="1" t="s">
+        <v>323</v>
+      </c>
+      <c r="F271" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="272" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A272" s="13" t="s">
+        <v>220</v>
+      </c>
+      <c r="B272" s="13">
+        <v>6</v>
+      </c>
+      <c r="C272" s="13" t="s">
+        <v>221</v>
+      </c>
+      <c r="D272" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="E272" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="F272" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="273" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A273" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="B273" s="12">
+        <v>6</v>
+      </c>
+      <c r="C273" s="12" t="s">
+        <v>242</v>
+      </c>
+      <c r="D273" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="E273" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="F273" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="274" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A274" s="13" t="s">
+        <v>220</v>
+      </c>
+      <c r="B274" s="13">
+        <v>6</v>
+      </c>
+      <c r="C274" s="13" t="s">
+        <v>263</v>
+      </c>
+      <c r="D274" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="E274" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="F274" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="275" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A275" s="13" t="s">
+        <v>220</v>
+      </c>
+      <c r="B275" s="13">
+        <v>6</v>
+      </c>
+      <c r="C275" s="13" t="s">
+        <v>284</v>
+      </c>
+      <c r="D275" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="E275" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="F275" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="276" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A276" s="13" t="s">
+        <v>220</v>
+      </c>
+      <c r="B276" s="13">
+        <v>6</v>
+      </c>
+      <c r="C276" s="13" t="s">
+        <v>305</v>
+      </c>
+      <c r="D276" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="E276" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="F276" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="277" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A277" s="13" t="s">
+        <v>220</v>
+      </c>
+      <c r="B277" s="13">
+        <v>6</v>
+      </c>
+      <c r="C277" s="13" t="s">
+        <v>221</v>
+      </c>
+      <c r="D277" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="E261" s="1" t="s">
+      <c r="E277" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="F277" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="278" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A278" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="B278" s="12">
+        <v>6</v>
+      </c>
+      <c r="C278" s="12" t="s">
+        <v>242</v>
+      </c>
+      <c r="D278" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E278" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="F278" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="279" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A279" s="13" t="s">
+        <v>220</v>
+      </c>
+      <c r="B279" s="13">
+        <v>6</v>
+      </c>
+      <c r="C279" s="13" t="s">
+        <v>263</v>
+      </c>
+      <c r="D279" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E279" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="F279" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="280" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A280" s="13" t="s">
+        <v>220</v>
+      </c>
+      <c r="B280" s="13">
+        <v>6</v>
+      </c>
+      <c r="C280" s="13" t="s">
+        <v>284</v>
+      </c>
+      <c r="D280" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E280" s="1" t="s">
         <v>304</v>
       </c>
-      <c r="F261" s="1" t="s">
+      <c r="F280" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="281" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A281" s="13" t="s">
+        <v>220</v>
+      </c>
+      <c r="B281" s="13">
+        <v>6</v>
+      </c>
+      <c r="C281" s="13" t="s">
+        <v>305</v>
+      </c>
+      <c r="D281" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E281" s="1" t="s">
+        <v>325</v>
+      </c>
+      <c r="F281" s="1" t="s">
         <v>69</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add US related to Nephrology domain
</commit_message>
<xml_diff>
--- a/refair-server/datasets/few shot dataset/FSDataset.xlsx
+++ b/refair-server/datasets/few shot dataset/FSDataset.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\morel\Desktop\Refair\ReFair-App\refair-server\datasets\few shot dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F85927B-4F7E-468F-BFA0-BCA2F5A88487}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CF237B1-24A3-4916-A1FE-00BC57F13E65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{80773445-FB61-4F04-A882-1600FD96C55A}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1406" uniqueCount="326">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1506" uniqueCount="347">
   <si>
     <t>Domain cluster</t>
   </si>
@@ -1014,13 +1014,76 @@
   </si>
   <si>
     <t>As a medical researcher, I want to apply word embedding techniques to analyze electronic health record narratives and extract meaningful clinical insights (e.g., disease progression markers, treatment effectiveness), so that I can support clinical decision-making and improve patient outcomes.</t>
+  </si>
+  <si>
+    <t>Nephrology</t>
+  </si>
+  <si>
+    <t>As a nephrologist, I want to employ adversarial learning techniques to detect and mitigate adversarial attacks on medical imaging data used for diagnosing kidney diseases, ensuring the reliability and integrity of diagnostic systems.</t>
+  </si>
+  <si>
+    <t>As a nephrologist, I want to utilize CNN models to predict the risk of acute kidney injury (AKI) in hospitalized patients based on a combination of clinical data and imaging findings, facilitating early intervention and patient management.</t>
+  </si>
+  <si>
+    <t>As a nephrologist, I want to deploy a conversational agent that can provide patients with personalized information about kidney disease management, including diet recommendations and lifestyle changes, to improve patient adherence and outcomes.</t>
+  </si>
+  <si>
+    <t>As a nephrologist, I want to utilize a decision tree model to classify patients into different stages of chronic kidney disease based on their clinical parameters, facilitating targeted interventions and personalized treatment plans.</t>
+  </si>
+  <si>
+    <t>As a nephrologist, I want to implement document classification algorithms to automatically categorize research papers and clinical guidelines related to nephrology, facilitating efficient literature review and evidence-based decision-making.</t>
+  </si>
+  <si>
+    <t>As a nephrologist, I want to employ entity extraction techniques to automatically identify and extract key clinical entities from nephrology patient notes, such as laboratory results (e.g., serum creatinine levels), medications, and comorbidities, enhancing clinical documentation accuracy and efficiency.</t>
+  </si>
+  <si>
+    <t>As a nephrologist, I want to utilize feature selection techniques to analyze electronic health records and identify clinical variables (e.g., medication history, comorbidities) that contribute most to adverse renal outcomes, optimizing predictive models for patient management.</t>
+  </si>
+  <si>
+    <t>As a nephrologist, I want to address class imbalance in patient datasets related to rare kidney diseases, using oversampling and undersampling techniques to improve the detection and classification accuracy of these conditions.</t>
+  </si>
+  <si>
+    <t>As a nephrologist, I want to employ keyword extraction methods to analyze patient feedback forms and surveys related to kidney disease management, extracting recurring themes and patient-reported outcomes to inform quality improvement initiatives in nephrology care.</t>
+  </si>
+  <si>
+    <t>As a nephrologist, I want to use k-Nearest Neighbor (k-NN) algorithms to predict the risk of acute kidney injury (AKI) in hospitalized patients based on similarities to previous AKI cases with similar clinical profiles, enabling early intervention strategies.</t>
+  </si>
+  <si>
+    <t>As a nephrologist, I want to utilize multi-label classification techniques to classify renal biopsy results into multiple histopathological categories (e.g., glomerulonephritis, tubulointerstitial diseases), supporting precise diagnosis and treatment recommendations.</t>
+  </si>
+  <si>
+    <t>As a nephrologist, I want to implement neural networks to analyze high-dimensional genomic data and identify gene expression patterns associated with progressive kidney diseases, facilitating the discovery of novel biomarkers and therapeutic targets.</t>
+  </si>
+  <si>
+    <t>As a nephrologist, I want to develop a random forest model to classify renal biopsy specimens into different pathological categories (e.g., glomerulonephritis, interstitial nephritis) based on histological features, aiding in accurate diagnosis and treatment planning.</t>
+  </si>
+  <si>
+    <t>As a nephrologist, I want to develop semantic similarity algorithms to compare and categorize nephrology research articles based on shared concepts and biomedical terms, facilitating systematic literature reviews and knowledge synthesis.</t>
+  </si>
+  <si>
+    <t>As a nephrologist, I want to develop a sentiment analysis model to analyze social media discussions and patient forums related to kidney transplantation experiences, to gauge patient emotions and concerns post-surgery.</t>
+  </si>
+  <si>
+    <t>As a nephrologist, I want to use speech to text algorithms to transcribe patient-doctor interactions during clinic visits, to streamline documentation processes and ensure comprehensive recording of medical histories and treatment plans.</t>
+  </si>
+  <si>
+    <t>As a nephrologist, I want to develop a text categorization system to classify nephrology research articles into categories such as chronic kidney disease epidemiology, renal replacement therapies, and nephrotoxicity studies, facilitating literature review and research synthesis.</t>
+  </si>
+  <si>
+    <t>As a nephrologist, I want to apply unsupervised clustering algorithms to group patients based on similar clinical profiles and treatment responses, enabling personalized medicine approaches in nephrology care.</t>
+  </si>
+  <si>
+    <t>As a nephrologist, I want to use voice recognition algorithms to transcribe patient-doctor interactions during nephrology clinic visits, ensuring accurate capture of medical histories, treatment discussions, and patient concerns.</t>
+  </si>
+  <si>
+    <t>As a nephrologist, I want to deploy word embedding models to support automated summarization of nephrology research articles and clinical trials, extracting key concepts and findings to aid in evidence-based decision-making and research synthesis.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1052,11 +1115,6 @@
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="7">
@@ -1109,7 +1167,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1131,7 +1189,6 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -1466,10 +1523,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8DF0B04-8323-4309-B759-D1CDDA1FBB0E}">
-  <dimension ref="A1:F281"/>
+  <dimension ref="A1:F301"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A183" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F261" sqref="F261:F281"/>
+    <sheetView tabSelected="1" topLeftCell="A281" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -5105,10 +5162,10 @@
       <c r="A182" s="12" t="s">
         <v>220</v>
       </c>
-      <c r="B182" s="13">
-        <v>6</v>
-      </c>
-      <c r="C182" s="13" t="s">
+      <c r="B182" s="12">
+        <v>6</v>
+      </c>
+      <c r="C182" s="12" t="s">
         <v>221</v>
       </c>
       <c r="D182" s="9" t="s">
@@ -5142,13 +5199,13 @@
       </c>
     </row>
     <row r="184" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A184" s="13" t="s">
-        <v>220</v>
-      </c>
-      <c r="B184" s="13">
-        <v>6</v>
-      </c>
-      <c r="C184" s="13" t="s">
+      <c r="A184" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="B184" s="12">
+        <v>6</v>
+      </c>
+      <c r="C184" s="12" t="s">
         <v>263</v>
       </c>
       <c r="D184" s="9" t="s">
@@ -5162,13 +5219,13 @@
       </c>
     </row>
     <row r="185" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A185" s="13" t="s">
-        <v>220</v>
-      </c>
-      <c r="B185" s="13">
-        <v>6</v>
-      </c>
-      <c r="C185" s="13" t="s">
+      <c r="A185" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="B185" s="12">
+        <v>6</v>
+      </c>
+      <c r="C185" s="12" t="s">
         <v>284</v>
       </c>
       <c r="D185" s="9" t="s">
@@ -5182,13 +5239,13 @@
       </c>
     </row>
     <row r="186" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A186" s="13" t="s">
-        <v>220</v>
-      </c>
-      <c r="B186" s="13">
-        <v>6</v>
-      </c>
-      <c r="C186" s="13" t="s">
+      <c r="A186" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="B186" s="12">
+        <v>6</v>
+      </c>
+      <c r="C186" s="12" t="s">
         <v>305</v>
       </c>
       <c r="D186" s="9" t="s">
@@ -5202,20 +5259,20 @@
       </c>
     </row>
     <row r="187" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A187" s="13" t="s">
-        <v>220</v>
-      </c>
-      <c r="B187" s="13">
-        <v>6</v>
-      </c>
-      <c r="C187" s="13" t="s">
-        <v>221</v>
+      <c r="A187" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="B187" s="12">
+        <v>6</v>
+      </c>
+      <c r="C187" s="12" t="s">
+        <v>326</v>
       </c>
       <c r="D187" s="9" t="s">
-        <v>43</v>
+        <v>28</v>
       </c>
       <c r="E187" s="1" t="s">
-        <v>223</v>
+        <v>327</v>
       </c>
       <c r="F187" s="1" t="s">
         <v>69</v>
@@ -5229,93 +5286,93 @@
         <v>6</v>
       </c>
       <c r="C188" s="12" t="s">
-        <v>242</v>
+        <v>221</v>
       </c>
       <c r="D188" s="9" t="s">
         <v>43</v>
       </c>
       <c r="E188" s="1" t="s">
-        <v>244</v>
+        <v>223</v>
       </c>
       <c r="F188" s="1" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="189" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A189" s="13" t="s">
-        <v>220</v>
-      </c>
-      <c r="B189" s="13">
-        <v>6</v>
-      </c>
-      <c r="C189" s="13" t="s">
-        <v>263</v>
+      <c r="A189" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="B189" s="12">
+        <v>6</v>
+      </c>
+      <c r="C189" s="12" t="s">
+        <v>242</v>
       </c>
       <c r="D189" s="9" t="s">
         <v>43</v>
       </c>
       <c r="E189" s="1" t="s">
-        <v>265</v>
+        <v>244</v>
       </c>
       <c r="F189" s="1" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="190" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A190" s="13" t="s">
-        <v>220</v>
-      </c>
-      <c r="B190" s="13">
-        <v>6</v>
-      </c>
-      <c r="C190" s="13" t="s">
-        <v>284</v>
+      <c r="A190" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="B190" s="12">
+        <v>6</v>
+      </c>
+      <c r="C190" s="12" t="s">
+        <v>263</v>
       </c>
       <c r="D190" s="9" t="s">
         <v>43</v>
       </c>
       <c r="E190" s="1" t="s">
-        <v>286</v>
+        <v>265</v>
       </c>
       <c r="F190" s="1" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="191" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A191" s="13" t="s">
-        <v>220</v>
-      </c>
-      <c r="B191" s="13">
-        <v>6</v>
-      </c>
-      <c r="C191" s="13" t="s">
-        <v>305</v>
+      <c r="A191" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="B191" s="12">
+        <v>6</v>
+      </c>
+      <c r="C191" s="12" t="s">
+        <v>284</v>
       </c>
       <c r="D191" s="9" t="s">
         <v>43</v>
       </c>
       <c r="E191" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="F191" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="192" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A192" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="B192" s="12">
+        <v>6</v>
+      </c>
+      <c r="C192" s="12" t="s">
+        <v>305</v>
+      </c>
+      <c r="D192" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="E192" s="1" t="s">
         <v>307</v>
-      </c>
-      <c r="F191" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="192" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A192" s="13" t="s">
-        <v>220</v>
-      </c>
-      <c r="B192" s="13">
-        <v>6</v>
-      </c>
-      <c r="C192" s="13" t="s">
-        <v>221</v>
-      </c>
-      <c r="D192" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="E192" s="1" t="s">
-        <v>224</v>
       </c>
       <c r="F192" s="1" t="s">
         <v>69</v>
@@ -5329,93 +5386,93 @@
         <v>6</v>
       </c>
       <c r="C193" s="12" t="s">
-        <v>242</v>
+        <v>326</v>
       </c>
       <c r="D193" s="9" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="E193" s="1" t="s">
-        <v>245</v>
+        <v>328</v>
       </c>
       <c r="F193" s="1" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="194" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A194" s="13" t="s">
-        <v>220</v>
-      </c>
-      <c r="B194" s="13">
-        <v>6</v>
-      </c>
-      <c r="C194" s="13" t="s">
-        <v>263</v>
+      <c r="A194" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="B194" s="12">
+        <v>6</v>
+      </c>
+      <c r="C194" s="12" t="s">
+        <v>221</v>
       </c>
       <c r="D194" s="9" t="s">
         <v>30</v>
       </c>
       <c r="E194" s="1" t="s">
-        <v>266</v>
+        <v>224</v>
       </c>
       <c r="F194" s="1" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="195" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A195" s="13" t="s">
-        <v>220</v>
-      </c>
-      <c r="B195" s="13">
-        <v>6</v>
-      </c>
-      <c r="C195" s="13" t="s">
-        <v>284</v>
+      <c r="A195" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="B195" s="12">
+        <v>6</v>
+      </c>
+      <c r="C195" s="12" t="s">
+        <v>242</v>
       </c>
       <c r="D195" s="9" t="s">
         <v>30</v>
       </c>
       <c r="E195" s="1" t="s">
-        <v>287</v>
+        <v>245</v>
       </c>
       <c r="F195" s="1" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="196" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A196" s="13" t="s">
-        <v>220</v>
-      </c>
-      <c r="B196" s="13">
-        <v>6</v>
-      </c>
-      <c r="C196" s="13" t="s">
-        <v>305</v>
+      <c r="A196" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="B196" s="12">
+        <v>6</v>
+      </c>
+      <c r="C196" s="12" t="s">
+        <v>263</v>
       </c>
       <c r="D196" s="9" t="s">
         <v>30</v>
       </c>
       <c r="E196" s="1" t="s">
-        <v>308</v>
+        <v>266</v>
       </c>
       <c r="F196" s="1" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="197" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A197" s="13" t="s">
-        <v>220</v>
-      </c>
-      <c r="B197" s="13">
-        <v>6</v>
-      </c>
-      <c r="C197" s="13" t="s">
-        <v>221</v>
+      <c r="A197" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="B197" s="12">
+        <v>6</v>
+      </c>
+      <c r="C197" s="12" t="s">
+        <v>284</v>
       </c>
       <c r="D197" s="9" t="s">
-        <v>13</v>
+        <v>30</v>
       </c>
       <c r="E197" s="1" t="s">
-        <v>225</v>
+        <v>287</v>
       </c>
       <c r="F197" s="1" t="s">
         <v>69</v>
@@ -5429,93 +5486,93 @@
         <v>6</v>
       </c>
       <c r="C198" s="12" t="s">
-        <v>242</v>
+        <v>305</v>
       </c>
       <c r="D198" s="9" t="s">
-        <v>13</v>
+        <v>30</v>
       </c>
       <c r="E198" s="1" t="s">
-        <v>246</v>
+        <v>308</v>
       </c>
       <c r="F198" s="1" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="199" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A199" s="13" t="s">
-        <v>220</v>
-      </c>
-      <c r="B199" s="13">
-        <v>6</v>
-      </c>
-      <c r="C199" s="13" t="s">
-        <v>263</v>
+      <c r="A199" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="B199" s="12">
+        <v>6</v>
+      </c>
+      <c r="C199" s="12" t="s">
+        <v>326</v>
       </c>
       <c r="D199" s="9" t="s">
-        <v>13</v>
+        <v>30</v>
       </c>
       <c r="E199" s="1" t="s">
-        <v>267</v>
+        <v>329</v>
       </c>
       <c r="F199" s="1" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="200" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A200" s="13" t="s">
-        <v>220</v>
-      </c>
-      <c r="B200" s="13">
-        <v>6</v>
-      </c>
-      <c r="C200" s="13" t="s">
-        <v>284</v>
+      <c r="A200" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="B200" s="12">
+        <v>6</v>
+      </c>
+      <c r="C200" s="12" t="s">
+        <v>221</v>
       </c>
       <c r="D200" s="9" t="s">
         <v>13</v>
       </c>
       <c r="E200" s="1" t="s">
-        <v>288</v>
+        <v>225</v>
       </c>
       <c r="F200" s="1" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="201" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A201" s="13" t="s">
-        <v>220</v>
-      </c>
-      <c r="B201" s="13">
-        <v>6</v>
-      </c>
-      <c r="C201" s="13" t="s">
-        <v>305</v>
+      <c r="A201" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="B201" s="12">
+        <v>6</v>
+      </c>
+      <c r="C201" s="12" t="s">
+        <v>242</v>
       </c>
       <c r="D201" s="9" t="s">
         <v>13</v>
       </c>
       <c r="E201" s="1" t="s">
-        <v>309</v>
+        <v>246</v>
       </c>
       <c r="F201" s="1" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="202" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A202" s="13" t="s">
-        <v>220</v>
-      </c>
-      <c r="B202" s="13">
-        <v>6</v>
-      </c>
-      <c r="C202" s="13" t="s">
-        <v>221</v>
+      <c r="A202" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="B202" s="12">
+        <v>6</v>
+      </c>
+      <c r="C202" s="12" t="s">
+        <v>263</v>
       </c>
       <c r="D202" s="9" t="s">
-        <v>46</v>
+        <v>13</v>
       </c>
       <c r="E202" s="1" t="s">
-        <v>226</v>
+        <v>267</v>
       </c>
       <c r="F202" s="1" t="s">
         <v>69</v>
@@ -5529,93 +5586,93 @@
         <v>6</v>
       </c>
       <c r="C203" s="12" t="s">
-        <v>242</v>
+        <v>284</v>
       </c>
       <c r="D203" s="9" t="s">
-        <v>46</v>
+        <v>13</v>
       </c>
       <c r="E203" s="1" t="s">
-        <v>247</v>
+        <v>288</v>
       </c>
       <c r="F203" s="1" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="204" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A204" s="13" t="s">
-        <v>220</v>
-      </c>
-      <c r="B204" s="13">
-        <v>6</v>
-      </c>
-      <c r="C204" s="13" t="s">
-        <v>263</v>
+      <c r="A204" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="B204" s="12">
+        <v>6</v>
+      </c>
+      <c r="C204" s="12" t="s">
+        <v>305</v>
       </c>
       <c r="D204" s="9" t="s">
-        <v>46</v>
+        <v>13</v>
       </c>
       <c r="E204" s="1" t="s">
-        <v>268</v>
+        <v>309</v>
       </c>
       <c r="F204" s="1" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="205" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A205" s="13" t="s">
-        <v>220</v>
-      </c>
-      <c r="B205" s="13">
-        <v>6</v>
-      </c>
-      <c r="C205" s="13" t="s">
-        <v>284</v>
+      <c r="A205" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="B205" s="12">
+        <v>6</v>
+      </c>
+      <c r="C205" s="12" t="s">
+        <v>326</v>
       </c>
       <c r="D205" s="9" t="s">
-        <v>46</v>
+        <v>13</v>
       </c>
       <c r="E205" s="1" t="s">
-        <v>289</v>
+        <v>330</v>
       </c>
       <c r="F205" s="1" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="206" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A206" s="13" t="s">
-        <v>220</v>
-      </c>
-      <c r="B206" s="13">
-        <v>6</v>
-      </c>
-      <c r="C206" s="13" t="s">
-        <v>305</v>
+      <c r="A206" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="B206" s="12">
+        <v>6</v>
+      </c>
+      <c r="C206" s="12" t="s">
+        <v>221</v>
       </c>
       <c r="D206" s="9" t="s">
         <v>46</v>
       </c>
       <c r="E206" s="1" t="s">
-        <v>310</v>
+        <v>226</v>
       </c>
       <c r="F206" s="1" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="207" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A207" s="13" t="s">
-        <v>220</v>
-      </c>
-      <c r="B207" s="13">
-        <v>6</v>
-      </c>
-      <c r="C207" s="13" t="s">
-        <v>221</v>
+      <c r="A207" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="B207" s="12">
+        <v>6</v>
+      </c>
+      <c r="C207" s="12" t="s">
+        <v>242</v>
       </c>
       <c r="D207" s="9" t="s">
-        <v>33</v>
+        <v>46</v>
       </c>
       <c r="E207" s="1" t="s">
-        <v>227</v>
+        <v>247</v>
       </c>
       <c r="F207" s="1" t="s">
         <v>69</v>
@@ -5629,93 +5686,93 @@
         <v>6</v>
       </c>
       <c r="C208" s="12" t="s">
-        <v>242</v>
+        <v>263</v>
       </c>
       <c r="D208" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="E208" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="F208" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="209" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A209" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="B209" s="12">
+        <v>6</v>
+      </c>
+      <c r="C209" s="12" t="s">
+        <v>284</v>
+      </c>
+      <c r="D209" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="E209" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="F209" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="210" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A210" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="B210" s="12">
+        <v>6</v>
+      </c>
+      <c r="C210" s="12" t="s">
+        <v>305</v>
+      </c>
+      <c r="D210" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="E210" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="F210" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="211" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A211" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="B211" s="12">
+        <v>6</v>
+      </c>
+      <c r="C211" s="12" t="s">
+        <v>326</v>
+      </c>
+      <c r="D211" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="E211" s="1" t="s">
+        <v>331</v>
+      </c>
+      <c r="F211" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="212" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A212" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="B212" s="12">
+        <v>6</v>
+      </c>
+      <c r="C212" s="12" t="s">
+        <v>221</v>
+      </c>
+      <c r="D212" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="E208" s="1" t="s">
-        <v>248</v>
-      </c>
-      <c r="F208" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="209" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A209" s="13" t="s">
-        <v>220</v>
-      </c>
-      <c r="B209" s="13">
-        <v>6</v>
-      </c>
-      <c r="C209" s="13" t="s">
-        <v>263</v>
-      </c>
-      <c r="D209" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="E209" s="1" t="s">
-        <v>269</v>
-      </c>
-      <c r="F209" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="210" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A210" s="13" t="s">
-        <v>220</v>
-      </c>
-      <c r="B210" s="13">
-        <v>6</v>
-      </c>
-      <c r="C210" s="13" t="s">
-        <v>284</v>
-      </c>
-      <c r="D210" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="E210" s="1" t="s">
-        <v>290</v>
-      </c>
-      <c r="F210" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="211" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A211" s="13" t="s">
-        <v>220</v>
-      </c>
-      <c r="B211" s="13">
-        <v>6</v>
-      </c>
-      <c r="C211" s="13" t="s">
-        <v>305</v>
-      </c>
-      <c r="D211" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="E211" s="1" t="s">
-        <v>311</v>
-      </c>
-      <c r="F211" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="212" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A212" s="13" t="s">
-        <v>220</v>
-      </c>
-      <c r="B212" s="13">
-        <v>6</v>
-      </c>
-      <c r="C212" s="13" t="s">
-        <v>221</v>
-      </c>
-      <c r="D212" s="9" t="s">
-        <v>36</v>
-      </c>
       <c r="E212" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F212" s="1" t="s">
         <v>69</v>
@@ -5732,90 +5789,90 @@
         <v>242</v>
       </c>
       <c r="D213" s="9" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E213" s="1" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="F213" s="1" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="214" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A214" s="13" t="s">
-        <v>220</v>
-      </c>
-      <c r="B214" s="13">
-        <v>6</v>
-      </c>
-      <c r="C214" s="13" t="s">
+      <c r="A214" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="B214" s="12">
+        <v>6</v>
+      </c>
+      <c r="C214" s="12" t="s">
         <v>263</v>
       </c>
       <c r="D214" s="9" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E214" s="1" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="F214" s="1" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="215" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A215" s="13" t="s">
-        <v>220</v>
-      </c>
-      <c r="B215" s="13">
-        <v>6</v>
-      </c>
-      <c r="C215" s="13" t="s">
+      <c r="A215" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="B215" s="12">
+        <v>6</v>
+      </c>
+      <c r="C215" s="12" t="s">
         <v>284</v>
       </c>
       <c r="D215" s="9" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E215" s="1" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="F215" s="1" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="216" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A216" s="13" t="s">
-        <v>220</v>
-      </c>
-      <c r="B216" s="13">
-        <v>6</v>
-      </c>
-      <c r="C216" s="13" t="s">
+      <c r="A216" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="B216" s="12">
+        <v>6</v>
+      </c>
+      <c r="C216" s="12" t="s">
         <v>305</v>
       </c>
       <c r="D216" s="9" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E216" s="1" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="F216" s="1" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="217" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A217" s="13" t="s">
-        <v>220</v>
-      </c>
-      <c r="B217" s="13">
-        <v>6</v>
-      </c>
-      <c r="C217" s="13" t="s">
-        <v>221</v>
+      <c r="A217" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="B217" s="12">
+        <v>6</v>
+      </c>
+      <c r="C217" s="12" t="s">
+        <v>326</v>
       </c>
       <c r="D217" s="9" t="s">
-        <v>14</v>
+        <v>33</v>
       </c>
       <c r="E217" s="1" t="s">
-        <v>229</v>
+        <v>332</v>
       </c>
       <c r="F217" s="1" t="s">
         <v>69</v>
@@ -5829,93 +5886,93 @@
         <v>6</v>
       </c>
       <c r="C218" s="12" t="s">
+        <v>221</v>
+      </c>
+      <c r="D218" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="E218" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="F218" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="219" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A219" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="B219" s="12">
+        <v>6</v>
+      </c>
+      <c r="C219" s="12" t="s">
         <v>242</v>
       </c>
-      <c r="D218" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="E218" s="1" t="s">
-        <v>250</v>
-      </c>
-      <c r="F218" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="219" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A219" s="13" t="s">
-        <v>220</v>
-      </c>
-      <c r="B219" s="13">
-        <v>6</v>
-      </c>
-      <c r="C219" s="13" t="s">
+      <c r="D219" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="E219" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="F219" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="220" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A220" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="B220" s="12">
+        <v>6</v>
+      </c>
+      <c r="C220" s="12" t="s">
         <v>263</v>
       </c>
-      <c r="D219" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="E219" s="1" t="s">
-        <v>271</v>
-      </c>
-      <c r="F219" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="220" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A220" s="13" t="s">
-        <v>220</v>
-      </c>
-      <c r="B220" s="13">
-        <v>6</v>
-      </c>
-      <c r="C220" s="13" t="s">
+      <c r="D220" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="E220" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="F220" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="221" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A221" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="B221" s="12">
+        <v>6</v>
+      </c>
+      <c r="C221" s="12" t="s">
         <v>284</v>
       </c>
-      <c r="D220" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="E220" s="1" t="s">
-        <v>292</v>
-      </c>
-      <c r="F220" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="221" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A221" s="13" t="s">
-        <v>220</v>
-      </c>
-      <c r="B221" s="13">
-        <v>6</v>
-      </c>
-      <c r="C221" s="13" t="s">
+      <c r="D221" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="E221" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="F221" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="222" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A222" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="B222" s="12">
+        <v>6</v>
+      </c>
+      <c r="C222" s="12" t="s">
         <v>305</v>
       </c>
-      <c r="D221" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="E221" s="1" t="s">
-        <v>313</v>
-      </c>
-      <c r="F221" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="222" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A222" s="13" t="s">
-        <v>220</v>
-      </c>
-      <c r="B222" s="13">
-        <v>6</v>
-      </c>
-      <c r="C222" s="13" t="s">
-        <v>221</v>
-      </c>
       <c r="D222" s="9" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="E222" s="1" t="s">
-        <v>230</v>
+        <v>312</v>
       </c>
       <c r="F222" s="1" t="s">
         <v>69</v>
@@ -5929,93 +5986,93 @@
         <v>6</v>
       </c>
       <c r="C223" s="12" t="s">
+        <v>326</v>
+      </c>
+      <c r="D223" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="E223" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="F223" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="224" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A224" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="B224" s="12">
+        <v>6</v>
+      </c>
+      <c r="C224" s="12" t="s">
+        <v>221</v>
+      </c>
+      <c r="D224" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="E224" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="F224" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="225" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A225" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="B225" s="12">
+        <v>6</v>
+      </c>
+      <c r="C225" s="12" t="s">
         <v>242</v>
       </c>
-      <c r="D223" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="E223" s="1" t="s">
-        <v>251</v>
-      </c>
-      <c r="F223" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="224" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A224" s="13" t="s">
-        <v>220</v>
-      </c>
-      <c r="B224" s="13">
-        <v>6</v>
-      </c>
-      <c r="C224" s="13" t="s">
+      <c r="D225" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="E225" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="F225" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="226" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A226" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="B226" s="12">
+        <v>6</v>
+      </c>
+      <c r="C226" s="12" t="s">
         <v>263</v>
       </c>
-      <c r="D224" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="E224" s="1" t="s">
-        <v>272</v>
-      </c>
-      <c r="F224" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="225" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A225" s="13" t="s">
-        <v>220</v>
-      </c>
-      <c r="B225" s="13">
-        <v>6</v>
-      </c>
-      <c r="C225" s="13" t="s">
+      <c r="D226" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="E226" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="F226" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="227" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A227" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="B227" s="12">
+        <v>6</v>
+      </c>
+      <c r="C227" s="12" t="s">
         <v>284</v>
       </c>
-      <c r="D225" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="E225" s="1" t="s">
-        <v>293</v>
-      </c>
-      <c r="F225" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="226" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A226" s="13" t="s">
-        <v>220</v>
-      </c>
-      <c r="B226" s="13">
-        <v>6</v>
-      </c>
-      <c r="C226" s="13" t="s">
-        <v>305</v>
-      </c>
-      <c r="D226" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="E226" s="1" t="s">
-        <v>314</v>
-      </c>
-      <c r="F226" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="227" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A227" s="13" t="s">
-        <v>220</v>
-      </c>
-      <c r="B227" s="13">
-        <v>6</v>
-      </c>
-      <c r="C227" s="13" t="s">
-        <v>221</v>
-      </c>
       <c r="D227" s="9" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E227" s="1" t="s">
-        <v>231</v>
+        <v>292</v>
       </c>
       <c r="F227" s="1" t="s">
         <v>69</v>
@@ -6029,93 +6086,93 @@
         <v>6</v>
       </c>
       <c r="C228" s="12" t="s">
+        <v>305</v>
+      </c>
+      <c r="D228" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="E228" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="F228" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="229" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A229" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="B229" s="12">
+        <v>6</v>
+      </c>
+      <c r="C229" s="12" t="s">
+        <v>326</v>
+      </c>
+      <c r="D229" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="E229" s="1" t="s">
+        <v>334</v>
+      </c>
+      <c r="F229" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="230" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A230" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="B230" s="12">
+        <v>6</v>
+      </c>
+      <c r="C230" s="12" t="s">
+        <v>221</v>
+      </c>
+      <c r="D230" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="E230" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="F230" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="231" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A231" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="B231" s="12">
+        <v>6</v>
+      </c>
+      <c r="C231" s="12" t="s">
         <v>242</v>
       </c>
-      <c r="D228" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="E228" s="1" t="s">
-        <v>252</v>
-      </c>
-      <c r="F228" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="229" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A229" s="13" t="s">
-        <v>220</v>
-      </c>
-      <c r="B229" s="13">
-        <v>6</v>
-      </c>
-      <c r="C229" s="13" t="s">
+      <c r="D231" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="E231" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="F231" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="232" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A232" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="B232" s="12">
+        <v>6</v>
+      </c>
+      <c r="C232" s="12" t="s">
         <v>263</v>
       </c>
-      <c r="D229" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="E229" s="1" t="s">
-        <v>273</v>
-      </c>
-      <c r="F229" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="230" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A230" s="13" t="s">
-        <v>220</v>
-      </c>
-      <c r="B230" s="13">
-        <v>6</v>
-      </c>
-      <c r="C230" s="13" t="s">
-        <v>284</v>
-      </c>
-      <c r="D230" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="E230" s="1" t="s">
-        <v>294</v>
-      </c>
-      <c r="F230" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="231" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A231" s="13" t="s">
-        <v>220</v>
-      </c>
-      <c r="B231" s="13">
-        <v>6</v>
-      </c>
-      <c r="C231" s="13" t="s">
-        <v>305</v>
-      </c>
-      <c r="D231" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="E231" s="1" t="s">
-        <v>315</v>
-      </c>
-      <c r="F231" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="232" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A232" s="13" t="s">
-        <v>220</v>
-      </c>
-      <c r="B232" s="13">
-        <v>6</v>
-      </c>
-      <c r="C232" s="13" t="s">
-        <v>221</v>
-      </c>
       <c r="D232" s="9" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="E232" s="1" t="s">
-        <v>232</v>
+        <v>272</v>
       </c>
       <c r="F232" s="1" t="s">
         <v>69</v>
@@ -6129,93 +6186,93 @@
         <v>6</v>
       </c>
       <c r="C233" s="12" t="s">
+        <v>284</v>
+      </c>
+      <c r="D233" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="E233" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="F233" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="234" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A234" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="B234" s="12">
+        <v>6</v>
+      </c>
+      <c r="C234" s="12" t="s">
+        <v>305</v>
+      </c>
+      <c r="D234" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="E234" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="F234" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="235" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A235" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="B235" s="12">
+        <v>6</v>
+      </c>
+      <c r="C235" s="12" t="s">
+        <v>326</v>
+      </c>
+      <c r="D235" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="E235" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="F235" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="236" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A236" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="B236" s="12">
+        <v>6</v>
+      </c>
+      <c r="C236" s="12" t="s">
+        <v>221</v>
+      </c>
+      <c r="D236" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="E236" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="F236" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="237" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A237" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="B237" s="12">
+        <v>6</v>
+      </c>
+      <c r="C237" s="12" t="s">
         <v>242</v>
       </c>
-      <c r="D233" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="E233" s="1" t="s">
-        <v>253</v>
-      </c>
-      <c r="F233" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="234" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A234" s="13" t="s">
-        <v>220</v>
-      </c>
-      <c r="B234" s="13">
-        <v>6</v>
-      </c>
-      <c r="C234" s="13" t="s">
-        <v>263</v>
-      </c>
-      <c r="D234" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="E234" s="1" t="s">
-        <v>274</v>
-      </c>
-      <c r="F234" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="235" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A235" s="13" t="s">
-        <v>220</v>
-      </c>
-      <c r="B235" s="13">
-        <v>6</v>
-      </c>
-      <c r="C235" s="13" t="s">
-        <v>284</v>
-      </c>
-      <c r="D235" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="E235" s="1" t="s">
-        <v>295</v>
-      </c>
-      <c r="F235" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="236" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A236" s="13" t="s">
-        <v>220</v>
-      </c>
-      <c r="B236" s="13">
-        <v>6</v>
-      </c>
-      <c r="C236" s="13" t="s">
-        <v>305</v>
-      </c>
-      <c r="D236" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="E236" s="1" t="s">
-        <v>316</v>
-      </c>
-      <c r="F236" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="237" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A237" s="13" t="s">
-        <v>220</v>
-      </c>
-      <c r="B237" s="13">
-        <v>6</v>
-      </c>
-      <c r="C237" s="13" t="s">
-        <v>221</v>
-      </c>
       <c r="D237" s="9" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E237" s="1" t="s">
-        <v>233</v>
+        <v>252</v>
       </c>
       <c r="F237" s="1" t="s">
         <v>69</v>
@@ -6229,93 +6286,93 @@
         <v>6</v>
       </c>
       <c r="C238" s="12" t="s">
-        <v>242</v>
+        <v>263</v>
       </c>
       <c r="D238" s="9" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E238" s="1" t="s">
-        <v>254</v>
+        <v>273</v>
       </c>
       <c r="F238" s="1" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="239" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A239" s="13" t="s">
-        <v>220</v>
-      </c>
-      <c r="B239" s="13">
-        <v>6</v>
-      </c>
-      <c r="C239" s="13" t="s">
-        <v>263</v>
+      <c r="A239" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="B239" s="12">
+        <v>6</v>
+      </c>
+      <c r="C239" s="12" t="s">
+        <v>284</v>
       </c>
       <c r="D239" s="9" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E239" s="1" t="s">
-        <v>275</v>
+        <v>294</v>
       </c>
       <c r="F239" s="1" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="240" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A240" s="13" t="s">
-        <v>220</v>
-      </c>
-      <c r="B240" s="13">
-        <v>6</v>
-      </c>
-      <c r="C240" s="13" t="s">
-        <v>284</v>
+      <c r="A240" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="B240" s="12">
+        <v>6</v>
+      </c>
+      <c r="C240" s="12" t="s">
+        <v>305</v>
       </c>
       <c r="D240" s="9" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E240" s="1" t="s">
-        <v>296</v>
+        <v>315</v>
       </c>
       <c r="F240" s="1" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="241" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A241" s="13" t="s">
-        <v>220</v>
-      </c>
-      <c r="B241" s="13">
-        <v>6</v>
-      </c>
-      <c r="C241" s="13" t="s">
-        <v>305</v>
+      <c r="A241" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="B241" s="12">
+        <v>6</v>
+      </c>
+      <c r="C241" s="12" t="s">
+        <v>326</v>
       </c>
       <c r="D241" s="9" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E241" s="1" t="s">
-        <v>317</v>
+        <v>336</v>
       </c>
       <c r="F241" s="1" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="242" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A242" s="13" t="s">
-        <v>220</v>
-      </c>
-      <c r="B242" s="13">
-        <v>6</v>
-      </c>
-      <c r="C242" s="13" t="s">
+      <c r="A242" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="B242" s="12">
+        <v>6</v>
+      </c>
+      <c r="C242" s="12" t="s">
         <v>221</v>
       </c>
       <c r="D242" s="9" t="s">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="E242" s="1" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="F242" s="1" t="s">
         <v>69</v>
@@ -6332,90 +6389,90 @@
         <v>242</v>
       </c>
       <c r="D243" s="9" t="s">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="E243" s="1" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="F243" s="1" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="244" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A244" s="13" t="s">
-        <v>220</v>
-      </c>
-      <c r="B244" s="13">
-        <v>6</v>
-      </c>
-      <c r="C244" s="13" t="s">
+      <c r="A244" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="B244" s="12">
+        <v>6</v>
+      </c>
+      <c r="C244" s="12" t="s">
         <v>263</v>
       </c>
       <c r="D244" s="9" t="s">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="E244" s="1" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="F244" s="1" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="245" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A245" s="13" t="s">
-        <v>220</v>
-      </c>
-      <c r="B245" s="13">
-        <v>6</v>
-      </c>
-      <c r="C245" s="13" t="s">
+      <c r="A245" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="B245" s="12">
+        <v>6</v>
+      </c>
+      <c r="C245" s="12" t="s">
         <v>284</v>
       </c>
       <c r="D245" s="9" t="s">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="E245" s="1" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="F245" s="1" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="246" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A246" s="13" t="s">
-        <v>220</v>
-      </c>
-      <c r="B246" s="13">
-        <v>6</v>
-      </c>
-      <c r="C246" s="13" t="s">
+      <c r="A246" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="B246" s="12">
+        <v>6</v>
+      </c>
+      <c r="C246" s="12" t="s">
         <v>305</v>
       </c>
       <c r="D246" s="9" t="s">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="E246" s="1" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="F246" s="1" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="247" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A247" s="13" t="s">
-        <v>220</v>
-      </c>
-      <c r="B247" s="13">
-        <v>6</v>
-      </c>
-      <c r="C247" s="13" t="s">
-        <v>221</v>
+      <c r="A247" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="B247" s="12">
+        <v>6</v>
+      </c>
+      <c r="C247" s="12" t="s">
+        <v>326</v>
       </c>
       <c r="D247" s="9" t="s">
-        <v>22</v>
+        <v>40</v>
       </c>
       <c r="E247" s="1" t="s">
-        <v>235</v>
+        <v>337</v>
       </c>
       <c r="F247" s="1" t="s">
         <v>69</v>
@@ -6429,93 +6486,93 @@
         <v>6</v>
       </c>
       <c r="C248" s="12" t="s">
+        <v>221</v>
+      </c>
+      <c r="D248" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="E248" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="F248" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="249" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A249" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="B249" s="12">
+        <v>6</v>
+      </c>
+      <c r="C249" s="12" t="s">
         <v>242</v>
       </c>
-      <c r="D248" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="E248" s="1" t="s">
-        <v>256</v>
-      </c>
-      <c r="F248" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="249" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A249" s="13" t="s">
-        <v>220</v>
-      </c>
-      <c r="B249" s="13">
-        <v>6</v>
-      </c>
-      <c r="C249" s="13" t="s">
+      <c r="D249" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="E249" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="F249" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="250" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A250" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="B250" s="12">
+        <v>6</v>
+      </c>
+      <c r="C250" s="12" t="s">
         <v>263</v>
       </c>
-      <c r="D249" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="E249" s="1" t="s">
-        <v>277</v>
-      </c>
-      <c r="F249" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="250" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A250" s="13" t="s">
-        <v>220</v>
-      </c>
-      <c r="B250" s="13">
-        <v>6</v>
-      </c>
-      <c r="C250" s="13" t="s">
+      <c r="D250" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="E250" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="F250" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="251" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A251" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="B251" s="12">
+        <v>6</v>
+      </c>
+      <c r="C251" s="12" t="s">
         <v>284</v>
       </c>
-      <c r="D250" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="E250" s="1" t="s">
-        <v>298</v>
-      </c>
-      <c r="F250" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="251" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A251" s="13" t="s">
-        <v>220</v>
-      </c>
-      <c r="B251" s="13">
-        <v>6</v>
-      </c>
-      <c r="C251" s="13" t="s">
+      <c r="D251" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="E251" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="F251" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="252" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A252" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="B252" s="12">
+        <v>6</v>
+      </c>
+      <c r="C252" s="12" t="s">
         <v>305</v>
       </c>
-      <c r="D251" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="E251" s="1" t="s">
-        <v>319</v>
-      </c>
-      <c r="F251" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="252" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A252" s="13" t="s">
-        <v>220</v>
-      </c>
-      <c r="B252" s="13">
-        <v>6</v>
-      </c>
-      <c r="C252" s="13" t="s">
-        <v>221</v>
-      </c>
       <c r="D252" s="9" t="s">
-        <v>38</v>
+        <v>18</v>
       </c>
       <c r="E252" s="1" t="s">
-        <v>236</v>
+        <v>317</v>
       </c>
       <c r="F252" s="1" t="s">
         <v>69</v>
@@ -6529,93 +6586,93 @@
         <v>6</v>
       </c>
       <c r="C253" s="12" t="s">
+        <v>326</v>
+      </c>
+      <c r="D253" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="E253" s="1" t="s">
+        <v>338</v>
+      </c>
+      <c r="F253" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="254" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A254" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="B254" s="12">
+        <v>6</v>
+      </c>
+      <c r="C254" s="12" t="s">
+        <v>221</v>
+      </c>
+      <c r="D254" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="E254" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="F254" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="255" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A255" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="B255" s="12">
+        <v>6</v>
+      </c>
+      <c r="C255" s="12" t="s">
         <v>242</v>
       </c>
-      <c r="D253" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="E253" s="1" t="s">
-        <v>257</v>
-      </c>
-      <c r="F253" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="254" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A254" s="13" t="s">
-        <v>220</v>
-      </c>
-      <c r="B254" s="13">
-        <v>6</v>
-      </c>
-      <c r="C254" s="13" t="s">
+      <c r="D255" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="E255" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="F255" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="256" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A256" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="B256" s="12">
+        <v>6</v>
+      </c>
+      <c r="C256" s="12" t="s">
         <v>263</v>
       </c>
-      <c r="D254" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="E254" s="1" t="s">
-        <v>278</v>
-      </c>
-      <c r="F254" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="255" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A255" s="13" t="s">
-        <v>220</v>
-      </c>
-      <c r="B255" s="13">
-        <v>6</v>
-      </c>
-      <c r="C255" s="13" t="s">
+      <c r="D256" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="E256" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="F256" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="257" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A257" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="B257" s="12">
+        <v>6</v>
+      </c>
+      <c r="C257" s="12" t="s">
         <v>284</v>
       </c>
-      <c r="D255" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="E255" s="1" t="s">
-        <v>299</v>
-      </c>
-      <c r="F255" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="256" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A256" s="13" t="s">
-        <v>220</v>
-      </c>
-      <c r="B256" s="13">
-        <v>6</v>
-      </c>
-      <c r="C256" s="13" t="s">
-        <v>305</v>
-      </c>
-      <c r="D256" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="E256" s="1" t="s">
-        <v>320</v>
-      </c>
-      <c r="F256" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="257" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A257" s="13" t="s">
-        <v>220</v>
-      </c>
-      <c r="B257" s="13">
-        <v>6</v>
-      </c>
-      <c r="C257" s="13" t="s">
-        <v>221</v>
-      </c>
       <c r="D257" s="9" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="E257" s="1" t="s">
-        <v>237</v>
+        <v>297</v>
       </c>
       <c r="F257" s="1" t="s">
         <v>69</v>
@@ -6629,93 +6686,93 @@
         <v>6</v>
       </c>
       <c r="C258" s="12" t="s">
+        <v>305</v>
+      </c>
+      <c r="D258" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="E258" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="F258" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="259" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A259" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="B259" s="12">
+        <v>6</v>
+      </c>
+      <c r="C259" s="12" t="s">
+        <v>326</v>
+      </c>
+      <c r="D259" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="E259" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="F259" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="260" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A260" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="B260" s="12">
+        <v>6</v>
+      </c>
+      <c r="C260" s="12" t="s">
+        <v>221</v>
+      </c>
+      <c r="D260" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="E260" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="F260" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="261" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A261" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="B261" s="12">
+        <v>6</v>
+      </c>
+      <c r="C261" s="12" t="s">
         <v>242</v>
       </c>
-      <c r="D258" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="E258" s="1" t="s">
-        <v>258</v>
-      </c>
-      <c r="F258" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="259" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A259" s="13" t="s">
-        <v>220</v>
-      </c>
-      <c r="B259" s="13">
-        <v>6</v>
-      </c>
-      <c r="C259" s="13" t="s">
+      <c r="D261" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="E261" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="F261" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="262" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A262" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="B262" s="12">
+        <v>6</v>
+      </c>
+      <c r="C262" s="12" t="s">
         <v>263</v>
       </c>
-      <c r="D259" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="E259" s="1" t="s">
-        <v>279</v>
-      </c>
-      <c r="F259" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="260" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A260" s="13" t="s">
-        <v>220</v>
-      </c>
-      <c r="B260" s="13">
-        <v>6</v>
-      </c>
-      <c r="C260" s="13" t="s">
-        <v>284</v>
-      </c>
-      <c r="D260" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="E260" s="1" t="s">
-        <v>300</v>
-      </c>
-      <c r="F260" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="261" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A261" s="13" t="s">
-        <v>220</v>
-      </c>
-      <c r="B261" s="13">
-        <v>6</v>
-      </c>
-      <c r="C261" s="13" t="s">
-        <v>305</v>
-      </c>
-      <c r="D261" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="E261" s="1" t="s">
-        <v>321</v>
-      </c>
-      <c r="F261" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="262" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A262" s="13" t="s">
-        <v>220</v>
-      </c>
-      <c r="B262" s="13">
-        <v>6</v>
-      </c>
-      <c r="C262" s="13" t="s">
-        <v>221</v>
-      </c>
       <c r="D262" s="9" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="E262" s="1" t="s">
-        <v>238</v>
+        <v>277</v>
       </c>
       <c r="F262" s="1" t="s">
         <v>69</v>
@@ -6729,93 +6786,93 @@
         <v>6</v>
       </c>
       <c r="C263" s="12" t="s">
+        <v>284</v>
+      </c>
+      <c r="D263" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="E263" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="F263" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="264" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A264" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="B264" s="12">
+        <v>6</v>
+      </c>
+      <c r="C264" s="12" t="s">
+        <v>305</v>
+      </c>
+      <c r="D264" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="E264" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="F264" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="265" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A265" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="B265" s="12">
+        <v>6</v>
+      </c>
+      <c r="C265" s="12" t="s">
+        <v>326</v>
+      </c>
+      <c r="D265" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="E265" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="F265" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="266" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A266" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="B266" s="12">
+        <v>6</v>
+      </c>
+      <c r="C266" s="12" t="s">
+        <v>221</v>
+      </c>
+      <c r="D266" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="E266" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="F266" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="267" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A267" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="B267" s="12">
+        <v>6</v>
+      </c>
+      <c r="C267" s="12" t="s">
         <v>242</v>
       </c>
-      <c r="D263" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="E263" s="1" t="s">
-        <v>259</v>
-      </c>
-      <c r="F263" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="264" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A264" s="13" t="s">
-        <v>220</v>
-      </c>
-      <c r="B264" s="13">
-        <v>6</v>
-      </c>
-      <c r="C264" s="13" t="s">
-        <v>263</v>
-      </c>
-      <c r="D264" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="E264" s="1" t="s">
-        <v>280</v>
-      </c>
-      <c r="F264" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="265" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A265" s="13" t="s">
-        <v>220</v>
-      </c>
-      <c r="B265" s="13">
-        <v>6</v>
-      </c>
-      <c r="C265" s="13" t="s">
-        <v>284</v>
-      </c>
-      <c r="D265" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="E265" s="1" t="s">
-        <v>301</v>
-      </c>
-      <c r="F265" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="266" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A266" s="13" t="s">
-        <v>220</v>
-      </c>
-      <c r="B266" s="13">
-        <v>6</v>
-      </c>
-      <c r="C266" s="13" t="s">
-        <v>305</v>
-      </c>
-      <c r="D266" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="E266" s="1" t="s">
-        <v>322</v>
-      </c>
-      <c r="F266" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="267" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A267" s="13" t="s">
-        <v>220</v>
-      </c>
-      <c r="B267" s="13">
-        <v>6</v>
-      </c>
-      <c r="C267" s="12" t="s">
-        <v>221</v>
-      </c>
       <c r="D267" s="9" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="E267" s="1" t="s">
-        <v>239</v>
+        <v>257</v>
       </c>
       <c r="F267" s="1" t="s">
         <v>69</v>
@@ -6829,93 +6886,93 @@
         <v>6</v>
       </c>
       <c r="C268" s="12" t="s">
-        <v>242</v>
+        <v>263</v>
       </c>
       <c r="D268" s="9" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="E268" s="1" t="s">
-        <v>260</v>
+        <v>278</v>
       </c>
       <c r="F268" s="1" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="269" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A269" s="13" t="s">
-        <v>220</v>
-      </c>
-      <c r="B269" s="13">
-        <v>6</v>
-      </c>
-      <c r="C269" s="13" t="s">
-        <v>263</v>
+      <c r="A269" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="B269" s="12">
+        <v>6</v>
+      </c>
+      <c r="C269" s="12" t="s">
+        <v>284</v>
       </c>
       <c r="D269" s="9" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="E269" s="1" t="s">
-        <v>281</v>
+        <v>299</v>
       </c>
       <c r="F269" s="1" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="270" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A270" s="13" t="s">
-        <v>220</v>
-      </c>
-      <c r="B270" s="13">
-        <v>6</v>
-      </c>
-      <c r="C270" s="13" t="s">
-        <v>284</v>
+      <c r="A270" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="B270" s="12">
+        <v>6</v>
+      </c>
+      <c r="C270" s="12" t="s">
+        <v>305</v>
       </c>
       <c r="D270" s="9" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="E270" s="1" t="s">
-        <v>302</v>
+        <v>320</v>
       </c>
       <c r="F270" s="1" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="271" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A271" s="13" t="s">
-        <v>220</v>
-      </c>
-      <c r="B271" s="13">
-        <v>6</v>
-      </c>
-      <c r="C271" s="13" t="s">
-        <v>305</v>
+      <c r="A271" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="B271" s="12">
+        <v>6</v>
+      </c>
+      <c r="C271" s="12" t="s">
+        <v>326</v>
       </c>
       <c r="D271" s="9" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="E271" s="1" t="s">
-        <v>323</v>
+        <v>341</v>
       </c>
       <c r="F271" s="1" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="272" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A272" s="13" t="s">
-        <v>220</v>
-      </c>
-      <c r="B272" s="13">
-        <v>6</v>
-      </c>
-      <c r="C272" s="13" t="s">
+      <c r="A272" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="B272" s="12">
+        <v>6</v>
+      </c>
+      <c r="C272" s="12" t="s">
         <v>221</v>
       </c>
       <c r="D272" s="9" t="s">
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="E272" s="1" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="F272" s="1" t="s">
         <v>69</v>
@@ -6932,90 +6989,90 @@
         <v>242</v>
       </c>
       <c r="D273" s="9" t="s">
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="E273" s="1" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="F273" s="1" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="274" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A274" s="13" t="s">
-        <v>220</v>
-      </c>
-      <c r="B274" s="13">
-        <v>6</v>
-      </c>
-      <c r="C274" s="13" t="s">
+      <c r="A274" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="B274" s="12">
+        <v>6</v>
+      </c>
+      <c r="C274" s="12" t="s">
         <v>263</v>
       </c>
       <c r="D274" s="9" t="s">
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="E274" s="1" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="F274" s="1" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="275" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A275" s="13" t="s">
-        <v>220</v>
-      </c>
-      <c r="B275" s="13">
-        <v>6</v>
-      </c>
-      <c r="C275" s="13" t="s">
+      <c r="A275" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="B275" s="12">
+        <v>6</v>
+      </c>
+      <c r="C275" s="12" t="s">
         <v>284</v>
       </c>
       <c r="D275" s="9" t="s">
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="E275" s="1" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="F275" s="1" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="276" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A276" s="13" t="s">
-        <v>220</v>
-      </c>
-      <c r="B276" s="13">
-        <v>6</v>
-      </c>
-      <c r="C276" s="13" t="s">
+      <c r="A276" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="B276" s="12">
+        <v>6</v>
+      </c>
+      <c r="C276" s="12" t="s">
         <v>305</v>
       </c>
       <c r="D276" s="9" t="s">
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="E276" s="1" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="F276" s="1" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="277" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A277" s="13" t="s">
-        <v>220</v>
-      </c>
-      <c r="B277" s="13">
-        <v>6</v>
-      </c>
-      <c r="C277" s="13" t="s">
-        <v>221</v>
+      <c r="A277" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="B277" s="12">
+        <v>6</v>
+      </c>
+      <c r="C277" s="12" t="s">
+        <v>326</v>
       </c>
       <c r="D277" s="9" t="s">
-        <v>9</v>
+        <v>24</v>
       </c>
       <c r="E277" s="1" t="s">
-        <v>241</v>
+        <v>342</v>
       </c>
       <c r="F277" s="1" t="s">
         <v>69</v>
@@ -7029,75 +7086,475 @@
         <v>6</v>
       </c>
       <c r="C278" s="12" t="s">
+        <v>221</v>
+      </c>
+      <c r="D278" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="E278" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="F278" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="279" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A279" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="B279" s="12">
+        <v>6</v>
+      </c>
+      <c r="C279" s="12" t="s">
         <v>242</v>
       </c>
-      <c r="D278" s="9" t="s">
+      <c r="D279" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="E279" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="F279" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="280" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A280" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="B280" s="12">
+        <v>6</v>
+      </c>
+      <c r="C280" s="12" t="s">
+        <v>263</v>
+      </c>
+      <c r="D280" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="E280" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="F280" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="281" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A281" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="B281" s="12">
+        <v>6</v>
+      </c>
+      <c r="C281" s="12" t="s">
+        <v>284</v>
+      </c>
+      <c r="D281" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="E281" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="F281" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="282" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A282" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="B282" s="12">
+        <v>6</v>
+      </c>
+      <c r="C282" s="12" t="s">
+        <v>305</v>
+      </c>
+      <c r="D282" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="E282" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="F282" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="283" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A283" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="B283" s="12">
+        <v>6</v>
+      </c>
+      <c r="C283" s="12" t="s">
+        <v>326</v>
+      </c>
+      <c r="D283" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="E283" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="F283" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="284" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A284" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="B284" s="12">
+        <v>6</v>
+      </c>
+      <c r="C284" s="12" t="s">
+        <v>221</v>
+      </c>
+      <c r="D284" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="E284" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="F284" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="285" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A285" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="B285" s="12">
+        <v>6</v>
+      </c>
+      <c r="C285" s="12" t="s">
+        <v>242</v>
+      </c>
+      <c r="D285" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="E285" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="F285" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="286" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A286" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="B286" s="12">
+        <v>6</v>
+      </c>
+      <c r="C286" s="12" t="s">
+        <v>263</v>
+      </c>
+      <c r="D286" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="E286" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="F286" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="287" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A287" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="B287" s="12">
+        <v>6</v>
+      </c>
+      <c r="C287" s="12" t="s">
+        <v>284</v>
+      </c>
+      <c r="D287" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="E287" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="F287" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="288" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A288" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="B288" s="12">
+        <v>6</v>
+      </c>
+      <c r="C288" s="12" t="s">
+        <v>305</v>
+      </c>
+      <c r="D288" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="E288" s="1" t="s">
+        <v>323</v>
+      </c>
+      <c r="F288" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="289" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A289" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="B289" s="12">
+        <v>6</v>
+      </c>
+      <c r="C289" s="12" t="s">
+        <v>326</v>
+      </c>
+      <c r="D289" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="E289" s="1" t="s">
+        <v>344</v>
+      </c>
+      <c r="F289" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="290" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A290" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="B290" s="12">
+        <v>6</v>
+      </c>
+      <c r="C290" s="12" t="s">
+        <v>221</v>
+      </c>
+      <c r="D290" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="E290" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="F290" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="291" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A291" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="B291" s="12">
+        <v>6</v>
+      </c>
+      <c r="C291" s="12" t="s">
+        <v>242</v>
+      </c>
+      <c r="D291" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="E291" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="F291" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="292" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A292" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="B292" s="12">
+        <v>6</v>
+      </c>
+      <c r="C292" s="12" t="s">
+        <v>263</v>
+      </c>
+      <c r="D292" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="E292" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="F292" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="293" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A293" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="B293" s="12">
+        <v>6</v>
+      </c>
+      <c r="C293" s="12" t="s">
+        <v>284</v>
+      </c>
+      <c r="D293" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="E293" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="F293" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="294" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A294" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="B294" s="12">
+        <v>6</v>
+      </c>
+      <c r="C294" s="12" t="s">
+        <v>305</v>
+      </c>
+      <c r="D294" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="E294" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="F294" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="295" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A295" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="B295" s="12">
+        <v>6</v>
+      </c>
+      <c r="C295" s="12" t="s">
+        <v>326</v>
+      </c>
+      <c r="D295" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="E295" s="1" t="s">
+        <v>345</v>
+      </c>
+      <c r="F295" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="296" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A296" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="B296" s="12">
+        <v>6</v>
+      </c>
+      <c r="C296" s="12" t="s">
+        <v>221</v>
+      </c>
+      <c r="D296" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="E278" s="1" t="s">
+      <c r="E296" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="F296" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="297" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A297" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="B297" s="12">
+        <v>6</v>
+      </c>
+      <c r="C297" s="12" t="s">
+        <v>242</v>
+      </c>
+      <c r="D297" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E297" s="1" t="s">
         <v>262</v>
       </c>
-      <c r="F278" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="279" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A279" s="13" t="s">
-        <v>220</v>
-      </c>
-      <c r="B279" s="13">
-        <v>6</v>
-      </c>
-      <c r="C279" s="13" t="s">
+      <c r="F297" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="298" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A298" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="B298" s="12">
+        <v>6</v>
+      </c>
+      <c r="C298" s="12" t="s">
         <v>263</v>
       </c>
-      <c r="D279" s="9" t="s">
+      <c r="D298" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="E279" s="1" t="s">
+      <c r="E298" s="1" t="s">
         <v>283</v>
       </c>
-      <c r="F279" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="280" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A280" s="13" t="s">
-        <v>220</v>
-      </c>
-      <c r="B280" s="13">
-        <v>6</v>
-      </c>
-      <c r="C280" s="13" t="s">
+      <c r="F298" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="299" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A299" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="B299" s="12">
+        <v>6</v>
+      </c>
+      <c r="C299" s="12" t="s">
         <v>284</v>
       </c>
-      <c r="D280" s="9" t="s">
+      <c r="D299" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="E280" s="1" t="s">
+      <c r="E299" s="1" t="s">
         <v>304</v>
       </c>
-      <c r="F280" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="281" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A281" s="13" t="s">
-        <v>220</v>
-      </c>
-      <c r="B281" s="13">
-        <v>6</v>
-      </c>
-      <c r="C281" s="13" t="s">
+      <c r="F299" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="300" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A300" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="B300" s="12">
+        <v>6</v>
+      </c>
+      <c r="C300" s="12" t="s">
         <v>305</v>
       </c>
-      <c r="D281" s="9" t="s">
+      <c r="D300" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="E281" s="1" t="s">
+      <c r="E300" s="1" t="s">
         <v>325</v>
       </c>
-      <c r="F281" s="1" t="s">
+      <c r="F300" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="301" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A301" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="B301" s="12">
+        <v>6</v>
+      </c>
+      <c r="C301" s="12" t="s">
+        <v>326</v>
+      </c>
+      <c r="D301" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E301" s="1" t="s">
+        <v>346</v>
+      </c>
+      <c r="F301" s="1" t="s">
         <v>69</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Diversify US related to "News" macro domain
</commit_message>
<xml_diff>
--- a/refair-server/datasets/few shot dataset/FSDataset.xlsx
+++ b/refair-server/datasets/few shot dataset/FSDataset.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maria\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\morel\Desktop\Refair\ReFair-App\refair-server\datasets\few shot dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C09E1C4-3C1B-4AF2-AA4C-A7273F4A8BA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C030B0C-5A4A-4F1E-A9CD-5FFB297AA492}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{80773445-FB61-4F04-A882-1600FD96C55A}"/>
   </bookViews>
@@ -329,39 +329,21 @@
     <t>As a news editor, I want to implement a conversational agent that can conduct interviews with newsmakers and automatically generate summaries or transcripts, accelerating the news reporting process and enhancing coverage depth.</t>
   </si>
   <si>
-    <t>As a journalist, I want to use decision tree models to classify news articles into relevant categories such as politics, sports, and entertainment, optimizing content organization for our news website.</t>
-  </si>
-  <si>
-    <t>As a news editor, I want to implement document classification algorithms to automatically categorize incoming news articles into sections such as politics, business, sports, and entertainment, facilitating efficient content management and navigation for our readers.</t>
-  </si>
-  <si>
     <t>As a journalist, I want to utilize entity extraction models to automatically identify and extract named entities such as people, organizations, and locations mentioned in news articles, enhancing the accuracy and comprehensiveness of our reporting.</t>
   </si>
   <si>
-    <t>As a journalist, I want to apply feature selection algorithms to prioritize and extract key information from multimedia elements (images, videos) accompanying news articles, enhancing the visual storytelling impact of our news reports.</t>
-  </si>
-  <si>
     <t>As a news organization, I want to develop strategies to handle imbalanced datasets in news article classification tasks, ensuring that minority topics or less-covered issues receive adequate representation and visibility.</t>
   </si>
   <si>
-    <t>As a news editor, I want to integrate keyword extraction capabilities into our editorial workflow to automatically suggest relevant hashtags for social media promotion of news articles, enhancing visibility and engagement across digital platforms.</t>
-  </si>
-  <si>
     <t>As a journalist, I want to apply k-nearest neighbor techniques to identify and connect related news stories across different languages or regions, enabling cross-linguistic or international news coverage on our global news platform.</t>
   </si>
   <si>
     <t>As a news editor, I want to implement multi-label classification models to categorize news articles into multiple relevant topics such as politics, economy, and environment, ensuring comprehensive coverage and indexing for our readers.</t>
   </si>
   <si>
-    <t>As a news organization, I want to deploy neural network architectures for natural language processing tasks such as summarizing news articles or generating concise headlines, improving content readability and user engagement.</t>
-  </si>
-  <si>
     <t>As a news editor, I want to utilize random forest algorithms to classify news articles into different categories such as politics, sports, and entertainment based on a combination of textual features and metadata, improving content organization and navigation on our news platform.</t>
   </si>
   <si>
-    <t>As a news editor, I want to implement semantic similarity algorithms to automatically detect and merge duplicate or highly similar news articles in our content management system, optimizing resource allocation and improving content quality.</t>
-  </si>
-  <si>
     <t>As a journalist, I want to apply sentiment analysis to social media comments on news stories so that I can understand public opinion and incorporate it into my reporting.</t>
   </si>
   <si>
@@ -371,9 +353,6 @@
     <t>As a news editor, I want to integrate text categorization tools into our editorial workflow to ensure that breaking news stories are quickly and accurately categorized, allowing for timely and relevant news delivery to our audience.</t>
   </si>
   <si>
-    <t>As a journalist, I want to apply unsupervised clustering techniques to identify emerging trends and hot topics in the news so that I can stay ahead of the curve and provide timely coverage.</t>
-  </si>
-  <si>
     <t>As a journalist, I want to use voice recognition technology to transcribe interviews and press conferences so that I can quickly and accurately produce written articles from spoken content.</t>
   </si>
   <si>
@@ -1077,6 +1056,27 @@
   </si>
   <si>
     <t>As a legal tech developer, I want to build word embedding models to enhance the search and retrieval capabilities of legal databases, enabling faster and more accurate information retrieval for legal professionals and researchers.</t>
+  </si>
+  <si>
+    <t>As a news analyst, I want to build a decision tree model to classify news articles into different categories (e.g., politics, sports, entertainment) based on their textual content, enabling automated tagging and content organization for efficient archival and retrieval.</t>
+  </si>
+  <si>
+    <t>As a content curator for a news website, I want to deploy document classification algorithms to identify and filter out clickbait articles or sensationalist headlines, maintaining the quality and credibility of our published content.</t>
+  </si>
+  <si>
+    <t>As a content curator for a news website, I want to employ feature selection algorithms to identify and prioritize news articles based on their relevance to trending topics and reader preferences, enhancing the overall user experience.</t>
+  </si>
+  <si>
+    <t>As a journalist covering global events, I want to utilize keyword extraction techniques to summarize news articles by highlighting significant terms and phrases, helping me to distill complex information into concise reports.</t>
+  </si>
+  <si>
+    <t>As a news editor, I want to deploy a neural network-based text summarization model to automatically generate concise summaries of lengthy news articles, improving efficiency in content production and enhancing reader engagement.</t>
+  </si>
+  <si>
+    <t>As a digital archivist, I want to use semantic similarity techniques to identify duplicate or highly similar news articles within large archives, optimizing storage and retrieval processes while ensuring content consistency.</t>
+  </si>
+  <si>
+    <t>As a digital archivist, I want to leverage unsupervised clustering techniques to organize large archives of historical news articles into coherent thematic collections, improving accessibility and facilitating research in media history.</t>
   </si>
 </sst>
 </file>
@@ -1167,7 +1167,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1189,6 +1189,7 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -1525,8 +1526,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8DF0B04-8323-4309-B759-D1CDDA1FBB0E}">
   <dimension ref="A1:F301"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E98" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E120" sqref="E120"/>
+    <sheetView tabSelected="1" topLeftCell="C60" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D81" sqref="D81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1560,19 +1561,19 @@
     </row>
     <row r="2" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="B2" s="10">
         <v>2</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="D2" s="9" t="s">
         <v>22</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>55</v>
@@ -1580,19 +1581,19 @@
     </row>
     <row r="3" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="B3" s="10">
         <v>2</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
       <c r="D3" s="9" t="s">
         <v>22</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>55</v>
@@ -1600,19 +1601,19 @@
     </row>
     <row r="4" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="B4" s="10">
         <v>2</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="D4" s="9" t="s">
         <v>32</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>55</v>
@@ -1620,19 +1621,19 @@
     </row>
     <row r="5" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="B5" s="10">
         <v>2</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
       <c r="D5" s="9" t="s">
         <v>32</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>55</v>
@@ -1640,19 +1641,19 @@
     </row>
     <row r="6" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="B6" s="10">
         <v>2</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="D6" s="9" t="s">
         <v>23</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>55</v>
@@ -1660,19 +1661,19 @@
     </row>
     <row r="7" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="B7" s="10">
         <v>2</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
       <c r="D7" s="9" t="s">
         <v>23</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>55</v>
@@ -1680,19 +1681,19 @@
     </row>
     <row r="8" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="10" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="B8" s="10">
         <v>2</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="D8" s="9" t="s">
         <v>12</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>55</v>
@@ -1700,19 +1701,19 @@
     </row>
     <row r="9" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="10" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="B9" s="10">
         <v>2</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
       <c r="D9" s="9" t="s">
         <v>12</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>55</v>
@@ -1720,19 +1721,19 @@
     </row>
     <row r="10" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="10" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="B10" s="10">
         <v>2</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="D10" s="9" t="s">
         <v>33</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>55</v>
@@ -1740,19 +1741,19 @@
     </row>
     <row r="11" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="10" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="B11" s="10">
         <v>2</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
       <c r="D11" s="9" t="s">
         <v>33</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>55</v>
@@ -1760,19 +1761,19 @@
     </row>
     <row r="12" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="B12" s="10">
         <v>2</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="D12" s="9" t="s">
         <v>25</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>55</v>
@@ -1780,19 +1781,19 @@
     </row>
     <row r="13" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="10" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="B13" s="10">
         <v>2</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
       <c r="D13" s="9" t="s">
         <v>25</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>55</v>
@@ -1800,19 +1801,19 @@
     </row>
     <row r="14" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="10" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="B14" s="10">
         <v>2</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="D14" s="9" t="s">
         <v>28</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="F14" s="1" t="s">
         <v>55</v>
@@ -1820,19 +1821,19 @@
     </row>
     <row r="15" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="10" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="B15" s="10">
         <v>2</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
       <c r="D15" s="9" t="s">
         <v>28</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="F15" s="1" t="s">
         <v>55</v>
@@ -1840,19 +1841,19 @@
     </row>
     <row r="16" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="10" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="B16" s="10">
         <v>2</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="D16" s="9" t="s">
         <v>13</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="F16" s="1" t="s">
         <v>55</v>
@@ -1860,19 +1861,19 @@
     </row>
     <row r="17" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="10" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="B17" s="10">
         <v>2</v>
       </c>
       <c r="C17" s="10" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
       <c r="D17" s="9" t="s">
         <v>13</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="F17" s="1" t="s">
         <v>55</v>
@@ -1880,19 +1881,19 @@
     </row>
     <row r="18" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="10" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="B18" s="10">
         <v>2</v>
       </c>
       <c r="C18" s="10" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="D18" s="9" t="s">
         <v>26</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="F18" s="1" t="s">
         <v>55</v>
@@ -1900,19 +1901,19 @@
     </row>
     <row r="19" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="10" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="B19" s="10">
         <v>2</v>
       </c>
       <c r="C19" s="10" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
       <c r="D19" s="9" t="s">
         <v>26</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
       <c r="F19" s="1" t="s">
         <v>55</v>
@@ -1920,19 +1921,19 @@
     </row>
     <row r="20" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="10" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="B20" s="10">
         <v>2</v>
       </c>
       <c r="C20" s="10" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="D20" s="9" t="s">
         <v>14</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="F20" s="1" t="s">
         <v>55</v>
@@ -1940,19 +1941,19 @@
     </row>
     <row r="21" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="10" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="B21" s="10">
         <v>2</v>
       </c>
       <c r="C21" s="10" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
       <c r="D21" s="9" t="s">
         <v>14</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
       <c r="F21" s="1" t="s">
         <v>55</v>
@@ -1960,19 +1961,19 @@
     </row>
     <row r="22" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="10" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="B22" s="10">
         <v>2</v>
       </c>
       <c r="C22" s="10" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="D22" s="9" t="s">
         <v>30</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="F22" s="1" t="s">
         <v>55</v>
@@ -1980,19 +1981,19 @@
     </row>
     <row r="23" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="10" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="B23" s="10">
         <v>2</v>
       </c>
       <c r="C23" s="10" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
       <c r="D23" s="9" t="s">
         <v>30</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
       <c r="F23" s="1" t="s">
         <v>55</v>
@@ -2000,19 +2001,19 @@
     </row>
     <row r="24" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="10" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="B24" s="10">
         <v>2</v>
       </c>
       <c r="C24" s="10" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="D24" s="9" t="s">
         <v>15</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="F24" s="1" t="s">
         <v>55</v>
@@ -2020,19 +2021,19 @@
     </row>
     <row r="25" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="10" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="B25" s="10">
         <v>2</v>
       </c>
       <c r="C25" s="10" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
       <c r="D25" s="9" t="s">
         <v>15</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
       <c r="F25" s="1" t="s">
         <v>55</v>
@@ -2040,19 +2041,19 @@
     </row>
     <row r="26" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="10" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="B26" s="10">
         <v>2</v>
       </c>
       <c r="C26" s="10" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="D26" s="9" t="s">
         <v>16</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="F26" s="1" t="s">
         <v>55</v>
@@ -2060,19 +2061,19 @@
     </row>
     <row r="27" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="10" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="B27" s="10">
         <v>2</v>
       </c>
       <c r="C27" s="10" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
       <c r="D27" s="9" t="s">
         <v>16</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
       <c r="F27" s="1" t="s">
         <v>55</v>
@@ -2080,19 +2081,19 @@
     </row>
     <row r="28" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="10" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="B28" s="10">
         <v>2</v>
       </c>
       <c r="C28" s="10" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="D28" s="9" t="s">
         <v>17</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="F28" s="1" t="s">
         <v>55</v>
@@ -2100,19 +2101,19 @@
     </row>
     <row r="29" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="10" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="B29" s="10">
         <v>2</v>
       </c>
       <c r="C29" s="10" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
       <c r="D29" s="9" t="s">
         <v>17</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="F29" s="1" t="s">
         <v>55</v>
@@ -2120,19 +2121,19 @@
     </row>
     <row r="30" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="10" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="B30" s="10">
         <v>2</v>
       </c>
       <c r="C30" s="10" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="D30" s="9" t="s">
         <v>29</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
       <c r="F30" s="1" t="s">
         <v>55</v>
@@ -2140,19 +2141,19 @@
     </row>
     <row r="31" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="10" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="B31" s="10">
         <v>2</v>
       </c>
       <c r="C31" s="10" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
       <c r="D31" s="9" t="s">
         <v>29</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
       <c r="F31" s="1" t="s">
         <v>55</v>
@@ -2160,19 +2161,19 @@
     </row>
     <row r="32" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="10" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="B32" s="10">
         <v>2</v>
       </c>
       <c r="C32" s="10" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="D32" s="9" t="s">
         <v>18</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="F32" s="1" t="s">
         <v>55</v>
@@ -2180,19 +2181,19 @@
     </row>
     <row r="33" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="10" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="B33" s="10">
         <v>2</v>
       </c>
       <c r="C33" s="10" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
       <c r="D33" s="9" t="s">
         <v>18</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>152</v>
+        <v>145</v>
       </c>
       <c r="F33" s="1" t="s">
         <v>55</v>
@@ -2200,19 +2201,19 @@
     </row>
     <row r="34" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="10" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="B34" s="10">
         <v>2</v>
       </c>
       <c r="C34" s="10" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="D34" s="9" t="s">
         <v>20</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="F34" s="1" t="s">
         <v>55</v>
@@ -2220,19 +2221,19 @@
     </row>
     <row r="35" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="10" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="B35" s="10">
         <v>2</v>
       </c>
       <c r="C35" s="10" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
       <c r="D35" s="9" t="s">
         <v>20</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
       <c r="F35" s="1" t="s">
         <v>55</v>
@@ -2240,19 +2241,19 @@
     </row>
     <row r="36" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="10" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="B36" s="10">
         <v>2</v>
       </c>
       <c r="C36" s="10" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="D36" s="9" t="s">
         <v>24</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="F36" s="1" t="s">
         <v>55</v>
@@ -2260,19 +2261,19 @@
     </row>
     <row r="37" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="10" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="B37" s="10">
         <v>2</v>
       </c>
       <c r="C37" s="10" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
       <c r="D37" s="9" t="s">
         <v>24</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="F37" s="1" t="s">
         <v>55</v>
@@ -2280,19 +2281,19 @@
     </row>
     <row r="38" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="10" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="B38" s="10">
         <v>2</v>
       </c>
       <c r="C38" s="10" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="D38" s="9" t="s">
         <v>7</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
       <c r="F38" s="1" t="s">
         <v>55</v>
@@ -2300,19 +2301,19 @@
     </row>
     <row r="39" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="10" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="B39" s="10">
         <v>2</v>
       </c>
       <c r="C39" s="10" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
       <c r="D39" s="9" t="s">
         <v>7</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
       <c r="F39" s="1" t="s">
         <v>55</v>
@@ -2320,19 +2321,19 @@
     </row>
     <row r="40" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="10" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="B40" s="10">
         <v>2</v>
       </c>
       <c r="C40" s="10" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="D40" s="9" t="s">
         <v>9</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="F40" s="1" t="s">
         <v>55</v>
@@ -2340,19 +2341,19 @@
     </row>
     <row r="41" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="10" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="B41" s="10">
         <v>2</v>
       </c>
       <c r="C41" s="10" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
       <c r="D41" s="9" t="s">
         <v>9</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="F41" s="1" t="s">
         <v>55</v>
@@ -2512,7 +2513,7 @@
         <v>12</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>97</v>
+        <v>340</v>
       </c>
       <c r="F49" s="1" t="s">
         <v>55</v>
@@ -2552,7 +2553,7 @@
         <v>33</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>98</v>
+        <v>341</v>
       </c>
       <c r="F51" s="1" t="s">
         <v>55</v>
@@ -2592,7 +2593,7 @@
         <v>25</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="F53" s="1" t="s">
         <v>55</v>
@@ -2632,7 +2633,7 @@
         <v>28</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>100</v>
+        <v>342</v>
       </c>
       <c r="F55" s="1" t="s">
         <v>55</v>
@@ -2672,7 +2673,7 @@
         <v>13</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="F57" s="1" t="s">
         <v>55</v>
@@ -2712,7 +2713,7 @@
         <v>26</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>102</v>
+        <v>343</v>
       </c>
       <c r="F59" s="1" t="s">
         <v>55</v>
@@ -2725,7 +2726,7 @@
       <c r="B60" s="8">
         <v>3</v>
       </c>
-      <c r="C60" s="8" t="s">
+      <c r="C60" s="13" t="s">
         <v>72</v>
       </c>
       <c r="D60" s="5" t="s">
@@ -2752,7 +2753,7 @@
         <v>14</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="F61" s="1" t="s">
         <v>55</v>
@@ -2792,7 +2793,7 @@
         <v>30</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="F63" s="1" t="s">
         <v>55</v>
@@ -2832,7 +2833,7 @@
         <v>15</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>105</v>
+        <v>344</v>
       </c>
       <c r="F65" s="1" t="s">
         <v>55</v>
@@ -2872,7 +2873,7 @@
         <v>16</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="F67" s="1" t="s">
         <v>55</v>
@@ -2912,7 +2913,7 @@
         <v>17</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>107</v>
+        <v>345</v>
       </c>
       <c r="F69" s="1" t="s">
         <v>55</v>
@@ -2952,7 +2953,7 @@
         <v>29</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="F71" s="1" t="s">
         <v>55</v>
@@ -2992,7 +2993,7 @@
         <v>18</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="F73" s="1" t="s">
         <v>55</v>
@@ -3032,7 +3033,7 @@
         <v>20</v>
       </c>
       <c r="E75" s="1" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="F75" s="1" t="s">
         <v>55</v>
@@ -3072,7 +3073,7 @@
         <v>24</v>
       </c>
       <c r="E77" s="1" t="s">
-        <v>111</v>
+        <v>346</v>
       </c>
       <c r="F77" s="1" t="s">
         <v>55</v>
@@ -3112,7 +3113,7 @@
         <v>7</v>
       </c>
       <c r="E79" s="1" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="F79" s="1" t="s">
         <v>55</v>
@@ -3152,7 +3153,7 @@
         <v>9</v>
       </c>
       <c r="E81" s="1" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="F81" s="1" t="s">
         <v>55</v>
@@ -3172,7 +3173,7 @@
         <v>22</v>
       </c>
       <c r="E82" s="1" t="s">
-        <v>330</v>
+        <v>323</v>
       </c>
       <c r="F82" s="1" t="s">
         <v>55</v>
@@ -3192,7 +3193,7 @@
         <v>22</v>
       </c>
       <c r="E83" s="1" t="s">
-        <v>313</v>
+        <v>306</v>
       </c>
       <c r="F83" s="1" t="s">
         <v>55</v>
@@ -3212,7 +3213,7 @@
         <v>32</v>
       </c>
       <c r="E84" s="1" t="s">
-        <v>331</v>
+        <v>324</v>
       </c>
       <c r="F84" s="1" t="s">
         <v>55</v>
@@ -3252,7 +3253,7 @@
         <v>23</v>
       </c>
       <c r="E86" s="1" t="s">
-        <v>332</v>
+        <v>325</v>
       </c>
       <c r="F86" s="1" t="s">
         <v>55</v>
@@ -3272,7 +3273,7 @@
         <v>23</v>
       </c>
       <c r="E87" s="1" t="s">
-        <v>314</v>
+        <v>307</v>
       </c>
       <c r="F87" s="1" t="s">
         <v>55</v>
@@ -3312,7 +3313,7 @@
         <v>12</v>
       </c>
       <c r="E89" s="1" t="s">
-        <v>315</v>
+        <v>308</v>
       </c>
       <c r="F89" s="1" t="s">
         <v>55</v>
@@ -3332,7 +3333,7 @@
         <v>33</v>
       </c>
       <c r="E90" s="1" t="s">
-        <v>333</v>
+        <v>326</v>
       </c>
       <c r="F90" s="1" t="s">
         <v>55</v>
@@ -3352,7 +3353,7 @@
         <v>33</v>
       </c>
       <c r="E91" s="1" t="s">
-        <v>316</v>
+        <v>309</v>
       </c>
       <c r="F91" s="1" t="s">
         <v>55</v>
@@ -3372,7 +3373,7 @@
         <v>25</v>
       </c>
       <c r="E92" s="1" t="s">
-        <v>334</v>
+        <v>327</v>
       </c>
       <c r="F92" s="1" t="s">
         <v>55</v>
@@ -3392,7 +3393,7 @@
         <v>25</v>
       </c>
       <c r="E93" s="1" t="s">
-        <v>317</v>
+        <v>310</v>
       </c>
       <c r="F93" s="1" t="s">
         <v>55</v>
@@ -3452,7 +3453,7 @@
         <v>13</v>
       </c>
       <c r="E96" s="1" t="s">
-        <v>335</v>
+        <v>328</v>
       </c>
       <c r="F96" s="1" t="s">
         <v>55</v>
@@ -3472,7 +3473,7 @@
         <v>13</v>
       </c>
       <c r="E97" s="1" t="s">
-        <v>318</v>
+        <v>311</v>
       </c>
       <c r="F97" s="1" t="s">
         <v>55</v>
@@ -3492,7 +3493,7 @@
         <v>26</v>
       </c>
       <c r="E98" s="1" t="s">
-        <v>336</v>
+        <v>329</v>
       </c>
       <c r="F98" s="1" t="s">
         <v>55</v>
@@ -3532,7 +3533,7 @@
         <v>14</v>
       </c>
       <c r="E100" s="1" t="s">
-        <v>338</v>
+        <v>331</v>
       </c>
       <c r="F100" s="1" t="s">
         <v>55</v>
@@ -3552,7 +3553,7 @@
         <v>14</v>
       </c>
       <c r="E101" s="1" t="s">
-        <v>319</v>
+        <v>312</v>
       </c>
       <c r="F101" s="1" t="s">
         <v>55</v>
@@ -3572,7 +3573,7 @@
         <v>30</v>
       </c>
       <c r="E102" s="1" t="s">
-        <v>337</v>
+        <v>330</v>
       </c>
       <c r="F102" s="1" t="s">
         <v>55</v>
@@ -3592,7 +3593,7 @@
         <v>30</v>
       </c>
       <c r="E103" s="1" t="s">
-        <v>320</v>
+        <v>313</v>
       </c>
       <c r="F103" s="1" t="s">
         <v>55</v>
@@ -3612,7 +3613,7 @@
         <v>15</v>
       </c>
       <c r="E104" s="1" t="s">
-        <v>339</v>
+        <v>332</v>
       </c>
       <c r="F104" s="1" t="s">
         <v>55</v>
@@ -3632,7 +3633,7 @@
         <v>15</v>
       </c>
       <c r="E105" s="1" t="s">
-        <v>321</v>
+        <v>314</v>
       </c>
       <c r="F105" s="1" t="s">
         <v>55</v>
@@ -3652,7 +3653,7 @@
         <v>16</v>
       </c>
       <c r="E106" s="1" t="s">
-        <v>340</v>
+        <v>333</v>
       </c>
       <c r="F106" s="1" t="s">
         <v>55</v>
@@ -3672,7 +3673,7 @@
         <v>16</v>
       </c>
       <c r="E107" s="1" t="s">
-        <v>322</v>
+        <v>315</v>
       </c>
       <c r="F107" s="1" t="s">
         <v>55</v>
@@ -3692,7 +3693,7 @@
         <v>17</v>
       </c>
       <c r="E108" s="1" t="s">
-        <v>341</v>
+        <v>334</v>
       </c>
       <c r="F108" s="1" t="s">
         <v>55</v>
@@ -3712,7 +3713,7 @@
         <v>17</v>
       </c>
       <c r="E109" s="1" t="s">
-        <v>323</v>
+        <v>316</v>
       </c>
       <c r="F109" s="1" t="s">
         <v>55</v>
@@ -3732,7 +3733,7 @@
         <v>29</v>
       </c>
       <c r="E110" s="1" t="s">
-        <v>342</v>
+        <v>335</v>
       </c>
       <c r="F110" s="1" t="s">
         <v>55</v>
@@ -3752,7 +3753,7 @@
         <v>29</v>
       </c>
       <c r="E111" s="1" t="s">
-        <v>324</v>
+        <v>317</v>
       </c>
       <c r="F111" s="1" t="s">
         <v>55</v>
@@ -3772,7 +3773,7 @@
         <v>18</v>
       </c>
       <c r="E112" s="1" t="s">
-        <v>343</v>
+        <v>336</v>
       </c>
       <c r="F112" s="1" t="s">
         <v>55</v>
@@ -3792,7 +3793,7 @@
         <v>18</v>
       </c>
       <c r="E113" s="1" t="s">
-        <v>325</v>
+        <v>318</v>
       </c>
       <c r="F113" s="1" t="s">
         <v>55</v>
@@ -3832,7 +3833,7 @@
         <v>20</v>
       </c>
       <c r="E115" s="6" t="s">
-        <v>326</v>
+        <v>319</v>
       </c>
       <c r="F115" s="1" t="s">
         <v>55</v>
@@ -3852,7 +3853,7 @@
         <v>24</v>
       </c>
       <c r="E116" s="1" t="s">
-        <v>344</v>
+        <v>337</v>
       </c>
       <c r="F116" s="1" t="s">
         <v>55</v>
@@ -3872,7 +3873,7 @@
         <v>24</v>
       </c>
       <c r="E117" s="1" t="s">
-        <v>327</v>
+        <v>320</v>
       </c>
       <c r="F117" s="1" t="s">
         <v>55</v>
@@ -3892,7 +3893,7 @@
         <v>7</v>
       </c>
       <c r="E118" s="1" t="s">
-        <v>345</v>
+        <v>338</v>
       </c>
       <c r="F118" s="1" t="s">
         <v>55</v>
@@ -3912,7 +3913,7 @@
         <v>7</v>
       </c>
       <c r="E119" s="1" t="s">
-        <v>328</v>
+        <v>321</v>
       </c>
       <c r="F119" s="1" t="s">
         <v>55</v>
@@ -3932,7 +3933,7 @@
         <v>9</v>
       </c>
       <c r="E120" s="1" t="s">
-        <v>346</v>
+        <v>339</v>
       </c>
       <c r="F120" s="1" t="s">
         <v>55</v>
@@ -3952,7 +3953,7 @@
         <v>9</v>
       </c>
       <c r="E121" s="1" t="s">
-        <v>329</v>
+        <v>322</v>
       </c>
       <c r="F121" s="1" t="s">
         <v>55</v>
@@ -4012,7 +4013,7 @@
         <v>22</v>
       </c>
       <c r="E124" s="1" t="s">
-        <v>297</v>
+        <v>290</v>
       </c>
       <c r="F124" s="1" t="s">
         <v>55</v>
@@ -4032,7 +4033,7 @@
         <v>32</v>
       </c>
       <c r="E125" s="6" t="s">
-        <v>284</v>
+        <v>277</v>
       </c>
       <c r="F125" s="1" t="s">
         <v>55</v>
@@ -4072,7 +4073,7 @@
         <v>32</v>
       </c>
       <c r="E127" s="1" t="s">
-        <v>298</v>
+        <v>291</v>
       </c>
       <c r="F127" s="1" t="s">
         <v>55</v>
@@ -4092,7 +4093,7 @@
         <v>23</v>
       </c>
       <c r="E128" s="1" t="s">
-        <v>285</v>
+        <v>278</v>
       </c>
       <c r="F128" s="1" t="s">
         <v>55</v>
@@ -4132,7 +4133,7 @@
         <v>23</v>
       </c>
       <c r="E130" s="1" t="s">
-        <v>299</v>
+        <v>292</v>
       </c>
       <c r="F130" s="1" t="s">
         <v>55</v>
@@ -4192,7 +4193,7 @@
         <v>12</v>
       </c>
       <c r="E133" s="6" t="s">
-        <v>300</v>
+        <v>293</v>
       </c>
       <c r="F133" s="1" t="s">
         <v>55</v>
@@ -4212,7 +4213,7 @@
         <v>33</v>
       </c>
       <c r="E134" s="1" t="s">
-        <v>286</v>
+        <v>279</v>
       </c>
       <c r="F134" s="1" t="s">
         <v>55</v>
@@ -4252,7 +4253,7 @@
         <v>33</v>
       </c>
       <c r="E136" s="1" t="s">
-        <v>301</v>
+        <v>294</v>
       </c>
       <c r="F136" s="1" t="s">
         <v>55</v>
@@ -4272,7 +4273,7 @@
         <v>25</v>
       </c>
       <c r="E137" s="1" t="s">
-        <v>287</v>
+        <v>280</v>
       </c>
       <c r="F137" s="1" t="s">
         <v>55</v>
@@ -4312,7 +4313,7 @@
         <v>25</v>
       </c>
       <c r="E139" s="1" t="s">
-        <v>302</v>
+        <v>295</v>
       </c>
       <c r="F139" s="1" t="s">
         <v>55</v>
@@ -4372,7 +4373,7 @@
         <v>28</v>
       </c>
       <c r="E142" s="1" t="s">
-        <v>303</v>
+        <v>296</v>
       </c>
       <c r="F142" s="1" t="s">
         <v>55</v>
@@ -4392,7 +4393,7 @@
         <v>13</v>
       </c>
       <c r="E143" s="6" t="s">
-        <v>288</v>
+        <v>281</v>
       </c>
       <c r="F143" s="1" t="s">
         <v>55</v>
@@ -4432,7 +4433,7 @@
         <v>13</v>
       </c>
       <c r="E145" s="1" t="s">
-        <v>304</v>
+        <v>297</v>
       </c>
       <c r="F145" s="1" t="s">
         <v>55</v>
@@ -4492,7 +4493,7 @@
         <v>26</v>
       </c>
       <c r="E148" s="1" t="s">
-        <v>305</v>
+        <v>298</v>
       </c>
       <c r="F148" s="1" t="s">
         <v>55</v>
@@ -4512,7 +4513,7 @@
         <v>14</v>
       </c>
       <c r="E149" s="1" t="s">
-        <v>290</v>
+        <v>283</v>
       </c>
       <c r="F149" s="1" t="s">
         <v>55</v>
@@ -4532,7 +4533,7 @@
         <v>14</v>
       </c>
       <c r="E150" s="1" t="s">
-        <v>312</v>
+        <v>305</v>
       </c>
       <c r="F150" s="1" t="s">
         <v>55</v>
@@ -4552,7 +4553,7 @@
         <v>14</v>
       </c>
       <c r="E151" s="1" t="s">
-        <v>306</v>
+        <v>299</v>
       </c>
       <c r="F151" s="1" t="s">
         <v>55</v>
@@ -4572,7 +4573,7 @@
         <v>30</v>
       </c>
       <c r="E152" s="1" t="s">
-        <v>289</v>
+        <v>282</v>
       </c>
       <c r="F152" s="1" t="s">
         <v>55</v>
@@ -4612,7 +4613,7 @@
         <v>30</v>
       </c>
       <c r="E154" s="1" t="s">
-        <v>307</v>
+        <v>300</v>
       </c>
       <c r="F154" s="1" t="s">
         <v>55</v>
@@ -4632,7 +4633,7 @@
         <v>15</v>
       </c>
       <c r="E155" s="1" t="s">
-        <v>291</v>
+        <v>284</v>
       </c>
       <c r="F155" s="1" t="s">
         <v>55</v>
@@ -4672,7 +4673,7 @@
         <v>15</v>
       </c>
       <c r="E157" s="1" t="s">
-        <v>308</v>
+        <v>301</v>
       </c>
       <c r="F157" s="1" t="s">
         <v>55</v>
@@ -4692,7 +4693,7 @@
         <v>16</v>
       </c>
       <c r="E158" s="1" t="s">
-        <v>292</v>
+        <v>285</v>
       </c>
       <c r="F158" s="1" t="s">
         <v>55</v>
@@ -4752,7 +4753,7 @@
         <v>17</v>
       </c>
       <c r="E161" s="1" t="s">
-        <v>294</v>
+        <v>287</v>
       </c>
       <c r="F161" s="1" t="s">
         <v>55</v>
@@ -4812,7 +4813,7 @@
         <v>29</v>
       </c>
       <c r="E164" s="1" t="s">
-        <v>293</v>
+        <v>286</v>
       </c>
       <c r="F164" s="1" t="s">
         <v>55</v>
@@ -4852,7 +4853,7 @@
         <v>29</v>
       </c>
       <c r="E166" s="1" t="s">
-        <v>309</v>
+        <v>302</v>
       </c>
       <c r="F166" s="1" t="s">
         <v>55</v>
@@ -4872,7 +4873,7 @@
         <v>18</v>
       </c>
       <c r="E167" s="1" t="s">
-        <v>295</v>
+        <v>288</v>
       </c>
       <c r="F167" s="1" t="s">
         <v>55</v>
@@ -4972,7 +4973,7 @@
         <v>20</v>
       </c>
       <c r="E172" s="1" t="s">
-        <v>310</v>
+        <v>303</v>
       </c>
       <c r="F172" s="1" t="s">
         <v>55</v>
@@ -4992,7 +4993,7 @@
         <v>24</v>
       </c>
       <c r="E173" s="1" t="s">
-        <v>296</v>
+        <v>289</v>
       </c>
       <c r="F173" s="1" t="s">
         <v>55</v>
@@ -5092,7 +5093,7 @@
         <v>7</v>
       </c>
       <c r="E178" s="1" t="s">
-        <v>311</v>
+        <v>304</v>
       </c>
       <c r="F178" s="1" t="s">
         <v>55</v>
@@ -5160,19 +5161,19 @@
     </row>
     <row r="182" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A182" s="12" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="B182" s="12">
         <v>6</v>
       </c>
       <c r="C182" s="12" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="D182" s="9" t="s">
         <v>22</v>
       </c>
       <c r="E182" s="1" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="F182" s="1" t="s">
         <v>55</v>
@@ -5180,19 +5181,19 @@
     </row>
     <row r="183" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A183" s="12" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="B183" s="12">
         <v>6</v>
       </c>
       <c r="C183" s="12" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
       <c r="D183" s="9" t="s">
         <v>22</v>
       </c>
       <c r="E183" s="1" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="F183" s="1" t="s">
         <v>55</v>
@@ -5200,19 +5201,19 @@
     </row>
     <row r="184" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A184" s="12" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="B184" s="12">
         <v>6</v>
       </c>
       <c r="C184" s="12" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="D184" s="9" t="s">
         <v>22</v>
       </c>
       <c r="E184" s="1" t="s">
-        <v>201</v>
+        <v>194</v>
       </c>
       <c r="F184" s="1" t="s">
         <v>55</v>
@@ -5220,19 +5221,19 @@
     </row>
     <row r="185" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A185" s="12" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="B185" s="12">
         <v>6</v>
       </c>
       <c r="C185" s="12" t="s">
-        <v>221</v>
+        <v>214</v>
       </c>
       <c r="D185" s="9" t="s">
         <v>22</v>
       </c>
       <c r="E185" s="1" t="s">
-        <v>222</v>
+        <v>215</v>
       </c>
       <c r="F185" s="1" t="s">
         <v>55</v>
@@ -5240,19 +5241,19 @@
     </row>
     <row r="186" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A186" s="12" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="B186" s="12">
         <v>6</v>
       </c>
       <c r="C186" s="12" t="s">
-        <v>242</v>
+        <v>235</v>
       </c>
       <c r="D186" s="9" t="s">
         <v>22</v>
       </c>
       <c r="E186" s="1" t="s">
-        <v>243</v>
+        <v>236</v>
       </c>
       <c r="F186" s="1" t="s">
         <v>55</v>
@@ -5260,19 +5261,19 @@
     </row>
     <row r="187" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A187" s="12" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="B187" s="12">
         <v>6</v>
       </c>
       <c r="C187" s="12" t="s">
-        <v>263</v>
+        <v>256</v>
       </c>
       <c r="D187" s="9" t="s">
         <v>22</v>
       </c>
       <c r="E187" s="1" t="s">
-        <v>264</v>
+        <v>257</v>
       </c>
       <c r="F187" s="1" t="s">
         <v>55</v>
@@ -5280,19 +5281,19 @@
     </row>
     <row r="188" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A188" s="12" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="B188" s="12">
         <v>6</v>
       </c>
       <c r="C188" s="12" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="D188" s="9" t="s">
         <v>32</v>
       </c>
       <c r="E188" s="1" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="F188" s="1" t="s">
         <v>55</v>
@@ -5300,19 +5301,19 @@
     </row>
     <row r="189" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A189" s="12" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="B189" s="12">
         <v>6</v>
       </c>
       <c r="C189" s="12" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
       <c r="D189" s="9" t="s">
         <v>32</v>
       </c>
       <c r="E189" s="1" t="s">
-        <v>181</v>
+        <v>174</v>
       </c>
       <c r="F189" s="1" t="s">
         <v>55</v>
@@ -5320,19 +5321,19 @@
     </row>
     <row r="190" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A190" s="12" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="B190" s="12">
         <v>6</v>
       </c>
       <c r="C190" s="12" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="D190" s="9" t="s">
         <v>32</v>
       </c>
       <c r="E190" s="1" t="s">
-        <v>202</v>
+        <v>195</v>
       </c>
       <c r="F190" s="1" t="s">
         <v>55</v>
@@ -5340,19 +5341,19 @@
     </row>
     <row r="191" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A191" s="12" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="B191" s="12">
         <v>6</v>
       </c>
       <c r="C191" s="12" t="s">
-        <v>221</v>
+        <v>214</v>
       </c>
       <c r="D191" s="9" t="s">
         <v>32</v>
       </c>
       <c r="E191" s="1" t="s">
-        <v>223</v>
+        <v>216</v>
       </c>
       <c r="F191" s="1" t="s">
         <v>55</v>
@@ -5360,19 +5361,19 @@
     </row>
     <row r="192" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A192" s="12" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="B192" s="12">
         <v>6</v>
       </c>
       <c r="C192" s="12" t="s">
-        <v>242</v>
+        <v>235</v>
       </c>
       <c r="D192" s="9" t="s">
         <v>32</v>
       </c>
       <c r="E192" s="1" t="s">
-        <v>244</v>
+        <v>237</v>
       </c>
       <c r="F192" s="1" t="s">
         <v>55</v>
@@ -5380,19 +5381,19 @@
     </row>
     <row r="193" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A193" s="12" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="B193" s="12">
         <v>6</v>
       </c>
       <c r="C193" s="12" t="s">
-        <v>263</v>
+        <v>256</v>
       </c>
       <c r="D193" s="9" t="s">
         <v>32</v>
       </c>
       <c r="E193" s="1" t="s">
-        <v>265</v>
+        <v>258</v>
       </c>
       <c r="F193" s="1" t="s">
         <v>55</v>
@@ -5400,19 +5401,19 @@
     </row>
     <row r="194" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A194" s="12" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="B194" s="12">
         <v>6</v>
       </c>
       <c r="C194" s="12" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="D194" s="9" t="s">
         <v>23</v>
       </c>
       <c r="E194" s="1" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
       <c r="F194" s="1" t="s">
         <v>55</v>
@@ -5420,19 +5421,19 @@
     </row>
     <row r="195" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A195" s="12" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="B195" s="12">
         <v>6</v>
       </c>
       <c r="C195" s="12" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
       <c r="D195" s="9" t="s">
         <v>23</v>
       </c>
       <c r="E195" s="1" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
       <c r="F195" s="1" t="s">
         <v>55</v>
@@ -5440,19 +5441,19 @@
     </row>
     <row r="196" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A196" s="12" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="B196" s="12">
         <v>6</v>
       </c>
       <c r="C196" s="12" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="D196" s="9" t="s">
         <v>23</v>
       </c>
       <c r="E196" s="1" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
       <c r="F196" s="1" t="s">
         <v>55</v>
@@ -5460,19 +5461,19 @@
     </row>
     <row r="197" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A197" s="12" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="B197" s="12">
         <v>6</v>
       </c>
       <c r="C197" s="12" t="s">
-        <v>221</v>
+        <v>214</v>
       </c>
       <c r="D197" s="9" t="s">
         <v>23</v>
       </c>
       <c r="E197" s="1" t="s">
-        <v>224</v>
+        <v>217</v>
       </c>
       <c r="F197" s="1" t="s">
         <v>55</v>
@@ -5480,19 +5481,19 @@
     </row>
     <row r="198" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A198" s="12" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="B198" s="12">
         <v>6</v>
       </c>
       <c r="C198" s="12" t="s">
-        <v>242</v>
+        <v>235</v>
       </c>
       <c r="D198" s="9" t="s">
         <v>23</v>
       </c>
       <c r="E198" s="1" t="s">
-        <v>245</v>
+        <v>238</v>
       </c>
       <c r="F198" s="1" t="s">
         <v>55</v>
@@ -5500,19 +5501,19 @@
     </row>
     <row r="199" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A199" s="12" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="B199" s="12">
         <v>6</v>
       </c>
       <c r="C199" s="12" t="s">
-        <v>263</v>
+        <v>256</v>
       </c>
       <c r="D199" s="9" t="s">
         <v>23</v>
       </c>
       <c r="E199" s="1" t="s">
-        <v>266</v>
+        <v>259</v>
       </c>
       <c r="F199" s="1" t="s">
         <v>55</v>
@@ -5520,19 +5521,19 @@
     </row>
     <row r="200" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A200" s="12" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="B200" s="12">
         <v>6</v>
       </c>
       <c r="C200" s="12" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="D200" s="9" t="s">
         <v>12</v>
       </c>
       <c r="E200" s="1" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="F200" s="1" t="s">
         <v>55</v>
@@ -5540,19 +5541,19 @@
     </row>
     <row r="201" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A201" s="12" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="B201" s="12">
         <v>6</v>
       </c>
       <c r="C201" s="12" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
       <c r="D201" s="9" t="s">
         <v>12</v>
       </c>
       <c r="E201" s="1" t="s">
-        <v>183</v>
+        <v>176</v>
       </c>
       <c r="F201" s="1" t="s">
         <v>55</v>
@@ -5560,19 +5561,19 @@
     </row>
     <row r="202" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A202" s="12" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="B202" s="12">
         <v>6</v>
       </c>
       <c r="C202" s="12" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="D202" s="9" t="s">
         <v>12</v>
       </c>
       <c r="E202" s="1" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="F202" s="1" t="s">
         <v>55</v>
@@ -5580,19 +5581,19 @@
     </row>
     <row r="203" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A203" s="12" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="B203" s="12">
         <v>6</v>
       </c>
       <c r="C203" s="12" t="s">
-        <v>221</v>
+        <v>214</v>
       </c>
       <c r="D203" s="9" t="s">
         <v>12</v>
       </c>
       <c r="E203" s="1" t="s">
-        <v>225</v>
+        <v>218</v>
       </c>
       <c r="F203" s="1" t="s">
         <v>55</v>
@@ -5600,19 +5601,19 @@
     </row>
     <row r="204" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A204" s="12" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="B204" s="12">
         <v>6</v>
       </c>
       <c r="C204" s="12" t="s">
-        <v>242</v>
+        <v>235</v>
       </c>
       <c r="D204" s="9" t="s">
         <v>12</v>
       </c>
       <c r="E204" s="1" t="s">
-        <v>246</v>
+        <v>239</v>
       </c>
       <c r="F204" s="1" t="s">
         <v>55</v>
@@ -5620,19 +5621,19 @@
     </row>
     <row r="205" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A205" s="12" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="B205" s="12">
         <v>6</v>
       </c>
       <c r="C205" s="12" t="s">
-        <v>263</v>
+        <v>256</v>
       </c>
       <c r="D205" s="9" t="s">
         <v>12</v>
       </c>
       <c r="E205" s="1" t="s">
-        <v>267</v>
+        <v>260</v>
       </c>
       <c r="F205" s="1" t="s">
         <v>55</v>
@@ -5640,19 +5641,19 @@
     </row>
     <row r="206" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A206" s="12" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="B206" s="12">
         <v>6</v>
       </c>
       <c r="C206" s="12" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="D206" s="9" t="s">
         <v>33</v>
       </c>
       <c r="E206" s="1" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
       <c r="F206" s="1" t="s">
         <v>55</v>
@@ -5660,19 +5661,19 @@
     </row>
     <row r="207" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A207" s="12" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="B207" s="12">
         <v>6</v>
       </c>
       <c r="C207" s="12" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
       <c r="D207" s="9" t="s">
         <v>33</v>
       </c>
       <c r="E207" s="1" t="s">
-        <v>184</v>
+        <v>177</v>
       </c>
       <c r="F207" s="1" t="s">
         <v>55</v>
@@ -5680,19 +5681,19 @@
     </row>
     <row r="208" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A208" s="12" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="B208" s="12">
         <v>6</v>
       </c>
       <c r="C208" s="12" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="D208" s="9" t="s">
         <v>33</v>
       </c>
       <c r="E208" s="1" t="s">
-        <v>205</v>
+        <v>198</v>
       </c>
       <c r="F208" s="1" t="s">
         <v>55</v>
@@ -5700,19 +5701,19 @@
     </row>
     <row r="209" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A209" s="12" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="B209" s="12">
         <v>6</v>
       </c>
       <c r="C209" s="12" t="s">
-        <v>221</v>
+        <v>214</v>
       </c>
       <c r="D209" s="9" t="s">
         <v>33</v>
       </c>
       <c r="E209" s="1" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
       <c r="F209" s="1" t="s">
         <v>55</v>
@@ -5720,19 +5721,19 @@
     </row>
     <row r="210" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A210" s="12" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="B210" s="12">
         <v>6</v>
       </c>
       <c r="C210" s="12" t="s">
-        <v>242</v>
+        <v>235</v>
       </c>
       <c r="D210" s="9" t="s">
         <v>33</v>
       </c>
       <c r="E210" s="1" t="s">
-        <v>247</v>
+        <v>240</v>
       </c>
       <c r="F210" s="1" t="s">
         <v>55</v>
@@ -5740,19 +5741,19 @@
     </row>
     <row r="211" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A211" s="12" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="B211" s="12">
         <v>6</v>
       </c>
       <c r="C211" s="12" t="s">
-        <v>263</v>
+        <v>256</v>
       </c>
       <c r="D211" s="9" t="s">
         <v>33</v>
       </c>
       <c r="E211" s="1" t="s">
-        <v>268</v>
+        <v>261</v>
       </c>
       <c r="F211" s="1" t="s">
         <v>55</v>
@@ -5760,19 +5761,19 @@
     </row>
     <row r="212" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A212" s="12" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="B212" s="12">
         <v>6</v>
       </c>
       <c r="C212" s="12" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="D212" s="9" t="s">
         <v>25</v>
       </c>
       <c r="E212" s="1" t="s">
-        <v>164</v>
+        <v>157</v>
       </c>
       <c r="F212" s="1" t="s">
         <v>55</v>
@@ -5780,19 +5781,19 @@
     </row>
     <row r="213" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A213" s="12" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="B213" s="12">
         <v>6</v>
       </c>
       <c r="C213" s="12" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
       <c r="D213" s="9" t="s">
         <v>25</v>
       </c>
       <c r="E213" s="1" t="s">
-        <v>185</v>
+        <v>178</v>
       </c>
       <c r="F213" s="1" t="s">
         <v>55</v>
@@ -5800,19 +5801,19 @@
     </row>
     <row r="214" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A214" s="12" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="B214" s="12">
         <v>6</v>
       </c>
       <c r="C214" s="12" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="D214" s="9" t="s">
         <v>25</v>
       </c>
       <c r="E214" s="1" t="s">
-        <v>206</v>
+        <v>199</v>
       </c>
       <c r="F214" s="1" t="s">
         <v>55</v>
@@ -5820,19 +5821,19 @@
     </row>
     <row r="215" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A215" s="12" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="B215" s="12">
         <v>6</v>
       </c>
       <c r="C215" s="12" t="s">
-        <v>221</v>
+        <v>214</v>
       </c>
       <c r="D215" s="9" t="s">
         <v>25</v>
       </c>
       <c r="E215" s="1" t="s">
-        <v>227</v>
+        <v>220</v>
       </c>
       <c r="F215" s="1" t="s">
         <v>55</v>
@@ -5840,19 +5841,19 @@
     </row>
     <row r="216" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A216" s="12" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="B216" s="12">
         <v>6</v>
       </c>
       <c r="C216" s="12" t="s">
-        <v>242</v>
+        <v>235</v>
       </c>
       <c r="D216" s="9" t="s">
         <v>25</v>
       </c>
       <c r="E216" s="1" t="s">
-        <v>248</v>
+        <v>241</v>
       </c>
       <c r="F216" s="1" t="s">
         <v>55</v>
@@ -5860,19 +5861,19 @@
     </row>
     <row r="217" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A217" s="12" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="B217" s="12">
         <v>6</v>
       </c>
       <c r="C217" s="12" t="s">
-        <v>263</v>
+        <v>256</v>
       </c>
       <c r="D217" s="9" t="s">
         <v>25</v>
       </c>
       <c r="E217" s="1" t="s">
-        <v>269</v>
+        <v>262</v>
       </c>
       <c r="F217" s="1" t="s">
         <v>55</v>
@@ -5880,19 +5881,19 @@
     </row>
     <row r="218" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A218" s="12" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="B218" s="12">
         <v>6</v>
       </c>
       <c r="C218" s="12" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="D218" s="9" t="s">
         <v>28</v>
       </c>
       <c r="E218" s="1" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="F218" s="1" t="s">
         <v>55</v>
@@ -5900,19 +5901,19 @@
     </row>
     <row r="219" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A219" s="12" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="B219" s="12">
         <v>6</v>
       </c>
       <c r="C219" s="12" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
       <c r="D219" s="9" t="s">
         <v>28</v>
       </c>
       <c r="E219" s="1" t="s">
-        <v>186</v>
+        <v>179</v>
       </c>
       <c r="F219" s="1" t="s">
         <v>55</v>
@@ -5920,19 +5921,19 @@
     </row>
     <row r="220" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A220" s="12" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="B220" s="12">
         <v>6</v>
       </c>
       <c r="C220" s="12" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="D220" s="9" t="s">
         <v>28</v>
       </c>
       <c r="E220" s="1" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
       <c r="F220" s="1" t="s">
         <v>55</v>
@@ -5940,19 +5941,19 @@
     </row>
     <row r="221" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A221" s="12" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="B221" s="12">
         <v>6</v>
       </c>
       <c r="C221" s="12" t="s">
-        <v>221</v>
+        <v>214</v>
       </c>
       <c r="D221" s="9" t="s">
         <v>28</v>
       </c>
       <c r="E221" s="1" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
       <c r="F221" s="1" t="s">
         <v>55</v>
@@ -5960,19 +5961,19 @@
     </row>
     <row r="222" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A222" s="12" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="B222" s="12">
         <v>6</v>
       </c>
       <c r="C222" s="12" t="s">
-        <v>242</v>
+        <v>235</v>
       </c>
       <c r="D222" s="9" t="s">
         <v>28</v>
       </c>
       <c r="E222" s="1" t="s">
-        <v>249</v>
+        <v>242</v>
       </c>
       <c r="F222" s="1" t="s">
         <v>55</v>
@@ -5980,19 +5981,19 @@
     </row>
     <row r="223" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A223" s="12" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="B223" s="12">
         <v>6</v>
       </c>
       <c r="C223" s="12" t="s">
-        <v>263</v>
+        <v>256</v>
       </c>
       <c r="D223" s="9" t="s">
         <v>28</v>
       </c>
       <c r="E223" s="1" t="s">
-        <v>270</v>
+        <v>263</v>
       </c>
       <c r="F223" s="1" t="s">
         <v>55</v>
@@ -6000,19 +6001,19 @@
     </row>
     <row r="224" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A224" s="12" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="B224" s="12">
         <v>6</v>
       </c>
       <c r="C224" s="12" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="D224" s="9" t="s">
         <v>13</v>
       </c>
       <c r="E224" s="1" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
       <c r="F224" s="1" t="s">
         <v>55</v>
@@ -6020,19 +6021,19 @@
     </row>
     <row r="225" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A225" s="12" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="B225" s="12">
         <v>6</v>
       </c>
       <c r="C225" s="12" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
       <c r="D225" s="9" t="s">
         <v>13</v>
       </c>
       <c r="E225" s="1" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
       <c r="F225" s="1" t="s">
         <v>55</v>
@@ -6040,19 +6041,19 @@
     </row>
     <row r="226" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A226" s="12" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="B226" s="12">
         <v>6</v>
       </c>
       <c r="C226" s="12" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="D226" s="9" t="s">
         <v>13</v>
       </c>
       <c r="E226" s="1" t="s">
-        <v>208</v>
+        <v>201</v>
       </c>
       <c r="F226" s="1" t="s">
         <v>55</v>
@@ -6060,19 +6061,19 @@
     </row>
     <row r="227" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A227" s="12" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="B227" s="12">
         <v>6</v>
       </c>
       <c r="C227" s="12" t="s">
-        <v>221</v>
+        <v>214</v>
       </c>
       <c r="D227" s="9" t="s">
         <v>13</v>
       </c>
       <c r="E227" s="1" t="s">
-        <v>229</v>
+        <v>222</v>
       </c>
       <c r="F227" s="1" t="s">
         <v>55</v>
@@ -6080,19 +6081,19 @@
     </row>
     <row r="228" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A228" s="12" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="B228" s="12">
         <v>6</v>
       </c>
       <c r="C228" s="12" t="s">
-        <v>242</v>
+        <v>235</v>
       </c>
       <c r="D228" s="9" t="s">
         <v>13</v>
       </c>
       <c r="E228" s="1" t="s">
-        <v>250</v>
+        <v>243</v>
       </c>
       <c r="F228" s="1" t="s">
         <v>55</v>
@@ -6100,19 +6101,19 @@
     </row>
     <row r="229" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A229" s="12" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="B229" s="12">
         <v>6</v>
       </c>
       <c r="C229" s="12" t="s">
-        <v>263</v>
+        <v>256</v>
       </c>
       <c r="D229" s="9" t="s">
         <v>13</v>
       </c>
       <c r="E229" s="1" t="s">
-        <v>271</v>
+        <v>264</v>
       </c>
       <c r="F229" s="1" t="s">
         <v>55</v>
@@ -6120,19 +6121,19 @@
     </row>
     <row r="230" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A230" s="12" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="B230" s="12">
         <v>6</v>
       </c>
       <c r="C230" s="12" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="D230" s="9" t="s">
         <v>26</v>
       </c>
       <c r="E230" s="1" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="F230" s="1" t="s">
         <v>55</v>
@@ -6140,19 +6141,19 @@
     </row>
     <row r="231" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A231" s="12" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="B231" s="12">
         <v>6</v>
       </c>
       <c r="C231" s="12" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
       <c r="D231" s="9" t="s">
         <v>26</v>
       </c>
       <c r="E231" s="1" t="s">
-        <v>188</v>
+        <v>181</v>
       </c>
       <c r="F231" s="1" t="s">
         <v>55</v>
@@ -6160,19 +6161,19 @@
     </row>
     <row r="232" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A232" s="12" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="B232" s="12">
         <v>6</v>
       </c>
       <c r="C232" s="12" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="D232" s="9" t="s">
         <v>26</v>
       </c>
       <c r="E232" s="1" t="s">
-        <v>209</v>
+        <v>202</v>
       </c>
       <c r="F232" s="1" t="s">
         <v>55</v>
@@ -6180,19 +6181,19 @@
     </row>
     <row r="233" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A233" s="12" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="B233" s="12">
         <v>6</v>
       </c>
       <c r="C233" s="12" t="s">
-        <v>221</v>
+        <v>214</v>
       </c>
       <c r="D233" s="9" t="s">
         <v>26</v>
       </c>
       <c r="E233" s="1" t="s">
-        <v>230</v>
+        <v>223</v>
       </c>
       <c r="F233" s="1" t="s">
         <v>55</v>
@@ -6200,19 +6201,19 @@
     </row>
     <row r="234" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A234" s="12" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="B234" s="12">
         <v>6</v>
       </c>
       <c r="C234" s="12" t="s">
-        <v>242</v>
+        <v>235</v>
       </c>
       <c r="D234" s="9" t="s">
         <v>26</v>
       </c>
       <c r="E234" s="1" t="s">
-        <v>251</v>
+        <v>244</v>
       </c>
       <c r="F234" s="1" t="s">
         <v>55</v>
@@ -6220,19 +6221,19 @@
     </row>
     <row r="235" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A235" s="12" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="B235" s="12">
         <v>6</v>
       </c>
       <c r="C235" s="12" t="s">
-        <v>263</v>
+        <v>256</v>
       </c>
       <c r="D235" s="9" t="s">
         <v>26</v>
       </c>
       <c r="E235" s="1" t="s">
-        <v>272</v>
+        <v>265</v>
       </c>
       <c r="F235" s="1" t="s">
         <v>55</v>
@@ -6240,19 +6241,19 @@
     </row>
     <row r="236" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A236" s="12" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="B236" s="12">
         <v>6</v>
       </c>
       <c r="C236" s="12" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="D236" s="9" t="s">
         <v>14</v>
       </c>
       <c r="E236" s="1" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="F236" s="1" t="s">
         <v>55</v>
@@ -6260,19 +6261,19 @@
     </row>
     <row r="237" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A237" s="12" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="B237" s="12">
         <v>6</v>
       </c>
       <c r="C237" s="12" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
       <c r="D237" s="9" t="s">
         <v>14</v>
       </c>
       <c r="E237" s="1" t="s">
-        <v>189</v>
+        <v>182</v>
       </c>
       <c r="F237" s="1" t="s">
         <v>55</v>
@@ -6280,19 +6281,19 @@
     </row>
     <row r="238" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A238" s="12" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="B238" s="12">
         <v>6</v>
       </c>
       <c r="C238" s="12" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="D238" s="9" t="s">
         <v>14</v>
       </c>
       <c r="E238" s="1" t="s">
-        <v>210</v>
+        <v>203</v>
       </c>
       <c r="F238" s="1" t="s">
         <v>55</v>
@@ -6300,19 +6301,19 @@
     </row>
     <row r="239" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A239" s="12" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="B239" s="12">
         <v>6</v>
       </c>
       <c r="C239" s="12" t="s">
-        <v>221</v>
+        <v>214</v>
       </c>
       <c r="D239" s="9" t="s">
         <v>14</v>
       </c>
       <c r="E239" s="1" t="s">
-        <v>231</v>
+        <v>224</v>
       </c>
       <c r="F239" s="1" t="s">
         <v>55</v>
@@ -6320,19 +6321,19 @@
     </row>
     <row r="240" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A240" s="12" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="B240" s="12">
         <v>6</v>
       </c>
       <c r="C240" s="12" t="s">
-        <v>242</v>
+        <v>235</v>
       </c>
       <c r="D240" s="9" t="s">
         <v>14</v>
       </c>
       <c r="E240" s="1" t="s">
-        <v>252</v>
+        <v>245</v>
       </c>
       <c r="F240" s="1" t="s">
         <v>55</v>
@@ -6340,19 +6341,19 @@
     </row>
     <row r="241" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A241" s="12" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="B241" s="12">
         <v>6</v>
       </c>
       <c r="C241" s="12" t="s">
-        <v>263</v>
+        <v>256</v>
       </c>
       <c r="D241" s="9" t="s">
         <v>14</v>
       </c>
       <c r="E241" s="1" t="s">
-        <v>273</v>
+        <v>266</v>
       </c>
       <c r="F241" s="1" t="s">
         <v>55</v>
@@ -6360,19 +6361,19 @@
     </row>
     <row r="242" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A242" s="12" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="B242" s="12">
         <v>6</v>
       </c>
       <c r="C242" s="12" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="D242" s="9" t="s">
         <v>30</v>
       </c>
       <c r="E242" s="1" t="s">
-        <v>169</v>
+        <v>162</v>
       </c>
       <c r="F242" s="1" t="s">
         <v>55</v>
@@ -6380,19 +6381,19 @@
     </row>
     <row r="243" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A243" s="12" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="B243" s="12">
         <v>6</v>
       </c>
       <c r="C243" s="12" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
       <c r="D243" s="9" t="s">
         <v>30</v>
       </c>
       <c r="E243" s="1" t="s">
-        <v>190</v>
+        <v>183</v>
       </c>
       <c r="F243" s="1" t="s">
         <v>55</v>
@@ -6400,19 +6401,19 @@
     </row>
     <row r="244" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A244" s="12" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="B244" s="12">
         <v>6</v>
       </c>
       <c r="C244" s="12" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="D244" s="9" t="s">
         <v>30</v>
       </c>
       <c r="E244" s="1" t="s">
-        <v>211</v>
+        <v>204</v>
       </c>
       <c r="F244" s="1" t="s">
         <v>55</v>
@@ -6420,19 +6421,19 @@
     </row>
     <row r="245" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A245" s="12" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="B245" s="12">
         <v>6</v>
       </c>
       <c r="C245" s="12" t="s">
-        <v>221</v>
+        <v>214</v>
       </c>
       <c r="D245" s="9" t="s">
         <v>30</v>
       </c>
       <c r="E245" s="1" t="s">
-        <v>232</v>
+        <v>225</v>
       </c>
       <c r="F245" s="1" t="s">
         <v>55</v>
@@ -6440,19 +6441,19 @@
     </row>
     <row r="246" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A246" s="12" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="B246" s="12">
         <v>6</v>
       </c>
       <c r="C246" s="12" t="s">
-        <v>242</v>
+        <v>235</v>
       </c>
       <c r="D246" s="9" t="s">
         <v>30</v>
       </c>
       <c r="E246" s="1" t="s">
-        <v>253</v>
+        <v>246</v>
       </c>
       <c r="F246" s="1" t="s">
         <v>55</v>
@@ -6460,19 +6461,19 @@
     </row>
     <row r="247" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A247" s="12" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="B247" s="12">
         <v>6</v>
       </c>
       <c r="C247" s="12" t="s">
-        <v>263</v>
+        <v>256</v>
       </c>
       <c r="D247" s="9" t="s">
         <v>30</v>
       </c>
       <c r="E247" s="1" t="s">
-        <v>274</v>
+        <v>267</v>
       </c>
       <c r="F247" s="1" t="s">
         <v>55</v>
@@ -6480,19 +6481,19 @@
     </row>
     <row r="248" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A248" s="12" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="B248" s="12">
         <v>6</v>
       </c>
       <c r="C248" s="12" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="D248" s="9" t="s">
         <v>15</v>
       </c>
       <c r="E248" s="1" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="F248" s="1" t="s">
         <v>55</v>
@@ -6500,19 +6501,19 @@
     </row>
     <row r="249" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A249" s="12" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="B249" s="12">
         <v>6</v>
       </c>
       <c r="C249" s="12" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
       <c r="D249" s="9" t="s">
         <v>15</v>
       </c>
       <c r="E249" s="1" t="s">
-        <v>191</v>
+        <v>184</v>
       </c>
       <c r="F249" s="1" t="s">
         <v>55</v>
@@ -6520,19 +6521,19 @@
     </row>
     <row r="250" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A250" s="12" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="B250" s="12">
         <v>6</v>
       </c>
       <c r="C250" s="12" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="D250" s="9" t="s">
         <v>15</v>
       </c>
       <c r="E250" s="1" t="s">
-        <v>212</v>
+        <v>205</v>
       </c>
       <c r="F250" s="1" t="s">
         <v>55</v>
@@ -6540,19 +6541,19 @@
     </row>
     <row r="251" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A251" s="12" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="B251" s="12">
         <v>6</v>
       </c>
       <c r="C251" s="12" t="s">
-        <v>221</v>
+        <v>214</v>
       </c>
       <c r="D251" s="9" t="s">
         <v>15</v>
       </c>
       <c r="E251" s="1" t="s">
-        <v>233</v>
+        <v>226</v>
       </c>
       <c r="F251" s="1" t="s">
         <v>55</v>
@@ -6560,19 +6561,19 @@
     </row>
     <row r="252" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A252" s="12" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="B252" s="12">
         <v>6</v>
       </c>
       <c r="C252" s="12" t="s">
-        <v>242</v>
+        <v>235</v>
       </c>
       <c r="D252" s="9" t="s">
         <v>15</v>
       </c>
       <c r="E252" s="1" t="s">
-        <v>254</v>
+        <v>247</v>
       </c>
       <c r="F252" s="1" t="s">
         <v>55</v>
@@ -6580,19 +6581,19 @@
     </row>
     <row r="253" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A253" s="12" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="B253" s="12">
         <v>6</v>
       </c>
       <c r="C253" s="12" t="s">
-        <v>263</v>
+        <v>256</v>
       </c>
       <c r="D253" s="9" t="s">
         <v>15</v>
       </c>
       <c r="E253" s="1" t="s">
-        <v>275</v>
+        <v>268</v>
       </c>
       <c r="F253" s="1" t="s">
         <v>55</v>
@@ -6600,19 +6601,19 @@
     </row>
     <row r="254" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A254" s="12" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="B254" s="12">
         <v>6</v>
       </c>
       <c r="C254" s="12" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="D254" s="9" t="s">
         <v>16</v>
       </c>
       <c r="E254" s="1" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="F254" s="1" t="s">
         <v>55</v>
@@ -6620,19 +6621,19 @@
     </row>
     <row r="255" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A255" s="12" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="B255" s="12">
         <v>6</v>
       </c>
       <c r="C255" s="12" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
       <c r="D255" s="9" t="s">
         <v>16</v>
       </c>
       <c r="E255" s="1" t="s">
-        <v>192</v>
+        <v>185</v>
       </c>
       <c r="F255" s="1" t="s">
         <v>55</v>
@@ -6640,19 +6641,19 @@
     </row>
     <row r="256" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A256" s="12" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="B256" s="12">
         <v>6</v>
       </c>
       <c r="C256" s="12" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="D256" s="9" t="s">
         <v>16</v>
       </c>
       <c r="E256" s="1" t="s">
-        <v>213</v>
+        <v>206</v>
       </c>
       <c r="F256" s="1" t="s">
         <v>55</v>
@@ -6660,19 +6661,19 @@
     </row>
     <row r="257" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A257" s="12" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="B257" s="12">
         <v>6</v>
       </c>
       <c r="C257" s="12" t="s">
-        <v>221</v>
+        <v>214</v>
       </c>
       <c r="D257" s="9" t="s">
         <v>16</v>
       </c>
       <c r="E257" s="1" t="s">
-        <v>234</v>
+        <v>227</v>
       </c>
       <c r="F257" s="1" t="s">
         <v>55</v>
@@ -6680,19 +6681,19 @@
     </row>
     <row r="258" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A258" s="12" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="B258" s="12">
         <v>6</v>
       </c>
       <c r="C258" s="12" t="s">
-        <v>242</v>
+        <v>235</v>
       </c>
       <c r="D258" s="9" t="s">
         <v>16</v>
       </c>
       <c r="E258" s="1" t="s">
-        <v>255</v>
+        <v>248</v>
       </c>
       <c r="F258" s="1" t="s">
         <v>55</v>
@@ -6700,19 +6701,19 @@
     </row>
     <row r="259" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A259" s="12" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="B259" s="12">
         <v>6</v>
       </c>
       <c r="C259" s="12" t="s">
-        <v>263</v>
+        <v>256</v>
       </c>
       <c r="D259" s="9" t="s">
         <v>16</v>
       </c>
       <c r="E259" s="1" t="s">
-        <v>276</v>
+        <v>269</v>
       </c>
       <c r="F259" s="1" t="s">
         <v>55</v>
@@ -6720,19 +6721,19 @@
     </row>
     <row r="260" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A260" s="12" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="B260" s="12">
         <v>6</v>
       </c>
       <c r="C260" s="12" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="D260" s="9" t="s">
         <v>17</v>
       </c>
       <c r="E260" s="1" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
       <c r="F260" s="1" t="s">
         <v>55</v>
@@ -6740,19 +6741,19 @@
     </row>
     <row r="261" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A261" s="12" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="B261" s="12">
         <v>6</v>
       </c>
       <c r="C261" s="12" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
       <c r="D261" s="9" t="s">
         <v>17</v>
       </c>
       <c r="E261" s="1" t="s">
-        <v>193</v>
+        <v>186</v>
       </c>
       <c r="F261" s="1" t="s">
         <v>55</v>
@@ -6760,19 +6761,19 @@
     </row>
     <row r="262" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A262" s="12" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="B262" s="12">
         <v>6</v>
       </c>
       <c r="C262" s="12" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="D262" s="9" t="s">
         <v>17</v>
       </c>
       <c r="E262" s="1" t="s">
-        <v>214</v>
+        <v>207</v>
       </c>
       <c r="F262" s="1" t="s">
         <v>55</v>
@@ -6780,19 +6781,19 @@
     </row>
     <row r="263" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A263" s="12" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="B263" s="12">
         <v>6</v>
       </c>
       <c r="C263" s="12" t="s">
-        <v>221</v>
+        <v>214</v>
       </c>
       <c r="D263" s="9" t="s">
         <v>17</v>
       </c>
       <c r="E263" s="1" t="s">
-        <v>235</v>
+        <v>228</v>
       </c>
       <c r="F263" s="1" t="s">
         <v>55</v>
@@ -6800,19 +6801,19 @@
     </row>
     <row r="264" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A264" s="12" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="B264" s="12">
         <v>6</v>
       </c>
       <c r="C264" s="12" t="s">
-        <v>242</v>
+        <v>235</v>
       </c>
       <c r="D264" s="9" t="s">
         <v>17</v>
       </c>
       <c r="E264" s="1" t="s">
-        <v>256</v>
+        <v>249</v>
       </c>
       <c r="F264" s="1" t="s">
         <v>55</v>
@@ -6820,19 +6821,19 @@
     </row>
     <row r="265" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A265" s="12" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="B265" s="12">
         <v>6</v>
       </c>
       <c r="C265" s="12" t="s">
-        <v>263</v>
+        <v>256</v>
       </c>
       <c r="D265" s="9" t="s">
         <v>17</v>
       </c>
       <c r="E265" s="1" t="s">
-        <v>277</v>
+        <v>270</v>
       </c>
       <c r="F265" s="1" t="s">
         <v>55</v>
@@ -6840,19 +6841,19 @@
     </row>
     <row r="266" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A266" s="12" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="B266" s="12">
         <v>6</v>
       </c>
       <c r="C266" s="12" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="D266" s="9" t="s">
         <v>29</v>
       </c>
       <c r="E266" s="1" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
       <c r="F266" s="1" t="s">
         <v>55</v>
@@ -6860,19 +6861,19 @@
     </row>
     <row r="267" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A267" s="12" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="B267" s="12">
         <v>6</v>
       </c>
       <c r="C267" s="12" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
       <c r="D267" s="9" t="s">
         <v>29</v>
       </c>
       <c r="E267" s="1" t="s">
-        <v>194</v>
+        <v>187</v>
       </c>
       <c r="F267" s="1" t="s">
         <v>55</v>
@@ -6880,19 +6881,19 @@
     </row>
     <row r="268" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A268" s="12" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="B268" s="12">
         <v>6</v>
       </c>
       <c r="C268" s="12" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="D268" s="9" t="s">
         <v>29</v>
       </c>
       <c r="E268" s="1" t="s">
-        <v>215</v>
+        <v>208</v>
       </c>
       <c r="F268" s="1" t="s">
         <v>55</v>
@@ -6900,19 +6901,19 @@
     </row>
     <row r="269" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A269" s="12" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="B269" s="12">
         <v>6</v>
       </c>
       <c r="C269" s="12" t="s">
-        <v>221</v>
+        <v>214</v>
       </c>
       <c r="D269" s="9" t="s">
         <v>29</v>
       </c>
       <c r="E269" s="1" t="s">
-        <v>236</v>
+        <v>229</v>
       </c>
       <c r="F269" s="1" t="s">
         <v>55</v>
@@ -6920,19 +6921,19 @@
     </row>
     <row r="270" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A270" s="12" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="B270" s="12">
         <v>6</v>
       </c>
       <c r="C270" s="12" t="s">
-        <v>242</v>
+        <v>235</v>
       </c>
       <c r="D270" s="9" t="s">
         <v>29</v>
       </c>
       <c r="E270" s="1" t="s">
-        <v>257</v>
+        <v>250</v>
       </c>
       <c r="F270" s="1" t="s">
         <v>55</v>
@@ -6940,19 +6941,19 @@
     </row>
     <row r="271" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A271" s="12" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="B271" s="12">
         <v>6</v>
       </c>
       <c r="C271" s="12" t="s">
-        <v>263</v>
+        <v>256</v>
       </c>
       <c r="D271" s="9" t="s">
         <v>29</v>
       </c>
       <c r="E271" s="1" t="s">
-        <v>278</v>
+        <v>271</v>
       </c>
       <c r="F271" s="1" t="s">
         <v>55</v>
@@ -6960,19 +6961,19 @@
     </row>
     <row r="272" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A272" s="12" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="B272" s="12">
         <v>6</v>
       </c>
       <c r="C272" s="12" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="D272" s="9" t="s">
         <v>18</v>
       </c>
       <c r="E272" s="1" t="s">
-        <v>174</v>
+        <v>167</v>
       </c>
       <c r="F272" s="1" t="s">
         <v>55</v>
@@ -6980,19 +6981,19 @@
     </row>
     <row r="273" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A273" s="12" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="B273" s="12">
         <v>6</v>
       </c>
       <c r="C273" s="12" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
       <c r="D273" s="9" t="s">
         <v>18</v>
       </c>
       <c r="E273" s="1" t="s">
-        <v>195</v>
+        <v>188</v>
       </c>
       <c r="F273" s="1" t="s">
         <v>55</v>
@@ -7000,19 +7001,19 @@
     </row>
     <row r="274" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A274" s="12" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="B274" s="12">
         <v>6</v>
       </c>
       <c r="C274" s="12" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="D274" s="9" t="s">
         <v>18</v>
       </c>
       <c r="E274" s="1" t="s">
-        <v>216</v>
+        <v>209</v>
       </c>
       <c r="F274" s="1" t="s">
         <v>55</v>
@@ -7020,19 +7021,19 @@
     </row>
     <row r="275" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A275" s="12" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="B275" s="12">
         <v>6</v>
       </c>
       <c r="C275" s="12" t="s">
-        <v>221</v>
+        <v>214</v>
       </c>
       <c r="D275" s="9" t="s">
         <v>18</v>
       </c>
       <c r="E275" s="1" t="s">
-        <v>237</v>
+        <v>230</v>
       </c>
       <c r="F275" s="1" t="s">
         <v>55</v>
@@ -7040,19 +7041,19 @@
     </row>
     <row r="276" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A276" s="12" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="B276" s="12">
         <v>6</v>
       </c>
       <c r="C276" s="12" t="s">
-        <v>242</v>
+        <v>235</v>
       </c>
       <c r="D276" s="9" t="s">
         <v>18</v>
       </c>
       <c r="E276" s="1" t="s">
-        <v>258</v>
+        <v>251</v>
       </c>
       <c r="F276" s="1" t="s">
         <v>55</v>
@@ -7060,19 +7061,19 @@
     </row>
     <row r="277" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A277" s="12" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="B277" s="12">
         <v>6</v>
       </c>
       <c r="C277" s="12" t="s">
-        <v>263</v>
+        <v>256</v>
       </c>
       <c r="D277" s="9" t="s">
         <v>18</v>
       </c>
       <c r="E277" s="1" t="s">
-        <v>279</v>
+        <v>272</v>
       </c>
       <c r="F277" s="1" t="s">
         <v>55</v>
@@ -7080,19 +7081,19 @@
     </row>
     <row r="278" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A278" s="12" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="B278" s="12">
         <v>6</v>
       </c>
       <c r="C278" s="12" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="D278" s="9" t="s">
         <v>20</v>
       </c>
       <c r="E278" s="1" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
       <c r="F278" s="1" t="s">
         <v>55</v>
@@ -7100,19 +7101,19 @@
     </row>
     <row r="279" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A279" s="12" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="B279" s="12">
         <v>6</v>
       </c>
       <c r="C279" s="12" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
       <c r="D279" s="9" t="s">
         <v>20</v>
       </c>
       <c r="E279" s="1" t="s">
-        <v>196</v>
+        <v>189</v>
       </c>
       <c r="F279" s="1" t="s">
         <v>55</v>
@@ -7120,19 +7121,19 @@
     </row>
     <row r="280" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A280" s="12" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="B280" s="12">
         <v>6</v>
       </c>
       <c r="C280" s="12" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="D280" s="9" t="s">
         <v>20</v>
       </c>
       <c r="E280" s="1" t="s">
-        <v>217</v>
+        <v>210</v>
       </c>
       <c r="F280" s="1" t="s">
         <v>55</v>
@@ -7140,19 +7141,19 @@
     </row>
     <row r="281" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A281" s="12" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="B281" s="12">
         <v>6</v>
       </c>
       <c r="C281" s="12" t="s">
-        <v>221</v>
+        <v>214</v>
       </c>
       <c r="D281" s="9" t="s">
         <v>20</v>
       </c>
       <c r="E281" s="1" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
       <c r="F281" s="1" t="s">
         <v>55</v>
@@ -7160,19 +7161,19 @@
     </row>
     <row r="282" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A282" s="12" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="B282" s="12">
         <v>6</v>
       </c>
       <c r="C282" s="12" t="s">
-        <v>242</v>
+        <v>235</v>
       </c>
       <c r="D282" s="9" t="s">
         <v>20</v>
       </c>
       <c r="E282" s="1" t="s">
-        <v>259</v>
+        <v>252</v>
       </c>
       <c r="F282" s="1" t="s">
         <v>55</v>
@@ -7180,19 +7181,19 @@
     </row>
     <row r="283" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A283" s="12" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="B283" s="12">
         <v>6</v>
       </c>
       <c r="C283" s="12" t="s">
-        <v>263</v>
+        <v>256</v>
       </c>
       <c r="D283" s="9" t="s">
         <v>20</v>
       </c>
       <c r="E283" s="1" t="s">
-        <v>280</v>
+        <v>273</v>
       </c>
       <c r="F283" s="1" t="s">
         <v>55</v>
@@ -7200,19 +7201,19 @@
     </row>
     <row r="284" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A284" s="12" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="B284" s="12">
         <v>6</v>
       </c>
       <c r="C284" s="12" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="D284" s="9" t="s">
         <v>24</v>
       </c>
       <c r="E284" s="1" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
       <c r="F284" s="1" t="s">
         <v>55</v>
@@ -7220,19 +7221,19 @@
     </row>
     <row r="285" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A285" s="12" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="B285" s="12">
         <v>6</v>
       </c>
       <c r="C285" s="12" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
       <c r="D285" s="9" t="s">
         <v>24</v>
       </c>
       <c r="E285" s="1" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
       <c r="F285" s="1" t="s">
         <v>55</v>
@@ -7240,19 +7241,19 @@
     </row>
     <row r="286" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A286" s="12" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="B286" s="12">
         <v>6</v>
       </c>
       <c r="C286" s="12" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="D286" s="9" t="s">
         <v>24</v>
       </c>
       <c r="E286" s="1" t="s">
-        <v>218</v>
+        <v>211</v>
       </c>
       <c r="F286" s="1" t="s">
         <v>55</v>
@@ -7260,19 +7261,19 @@
     </row>
     <row r="287" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A287" s="12" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="B287" s="12">
         <v>6</v>
       </c>
       <c r="C287" s="12" t="s">
-        <v>221</v>
+        <v>214</v>
       </c>
       <c r="D287" s="9" t="s">
         <v>24</v>
       </c>
       <c r="E287" s="1" t="s">
-        <v>239</v>
+        <v>232</v>
       </c>
       <c r="F287" s="1" t="s">
         <v>55</v>
@@ -7280,19 +7281,19 @@
     </row>
     <row r="288" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A288" s="12" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="B288" s="12">
         <v>6</v>
       </c>
       <c r="C288" s="12" t="s">
-        <v>242</v>
+        <v>235</v>
       </c>
       <c r="D288" s="9" t="s">
         <v>24</v>
       </c>
       <c r="E288" s="1" t="s">
-        <v>260</v>
+        <v>253</v>
       </c>
       <c r="F288" s="1" t="s">
         <v>55</v>
@@ -7300,19 +7301,19 @@
     </row>
     <row r="289" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A289" s="12" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="B289" s="12">
         <v>6</v>
       </c>
       <c r="C289" s="12" t="s">
-        <v>263</v>
+        <v>256</v>
       </c>
       <c r="D289" s="9" t="s">
         <v>24</v>
       </c>
       <c r="E289" s="1" t="s">
-        <v>281</v>
+        <v>274</v>
       </c>
       <c r="F289" s="1" t="s">
         <v>55</v>
@@ -7320,19 +7321,19 @@
     </row>
     <row r="290" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A290" s="12" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="B290" s="12">
         <v>6</v>
       </c>
       <c r="C290" s="12" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="D290" s="9" t="s">
         <v>7</v>
       </c>
       <c r="E290" s="1" t="s">
-        <v>177</v>
+        <v>170</v>
       </c>
       <c r="F290" s="1" t="s">
         <v>55</v>
@@ -7340,19 +7341,19 @@
     </row>
     <row r="291" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A291" s="12" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="B291" s="12">
         <v>6</v>
       </c>
       <c r="C291" s="12" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
       <c r="D291" s="9" t="s">
         <v>7</v>
       </c>
       <c r="E291" s="1" t="s">
-        <v>198</v>
+        <v>191</v>
       </c>
       <c r="F291" s="1" t="s">
         <v>55</v>
@@ -7360,19 +7361,19 @@
     </row>
     <row r="292" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A292" s="12" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="B292" s="12">
         <v>6</v>
       </c>
       <c r="C292" s="12" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="D292" s="9" t="s">
         <v>7</v>
       </c>
       <c r="E292" s="1" t="s">
-        <v>219</v>
+        <v>212</v>
       </c>
       <c r="F292" s="1" t="s">
         <v>55</v>
@@ -7380,19 +7381,19 @@
     </row>
     <row r="293" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A293" s="12" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="B293" s="12">
         <v>6</v>
       </c>
       <c r="C293" s="12" t="s">
-        <v>221</v>
+        <v>214</v>
       </c>
       <c r="D293" s="9" t="s">
         <v>7</v>
       </c>
       <c r="E293" s="1" t="s">
-        <v>240</v>
+        <v>233</v>
       </c>
       <c r="F293" s="1" t="s">
         <v>55</v>
@@ -7400,19 +7401,19 @@
     </row>
     <row r="294" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A294" s="12" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="B294" s="12">
         <v>6</v>
       </c>
       <c r="C294" s="12" t="s">
-        <v>242</v>
+        <v>235</v>
       </c>
       <c r="D294" s="9" t="s">
         <v>7</v>
       </c>
       <c r="E294" s="1" t="s">
-        <v>261</v>
+        <v>254</v>
       </c>
       <c r="F294" s="1" t="s">
         <v>55</v>
@@ -7420,19 +7421,19 @@
     </row>
     <row r="295" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A295" s="12" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="B295" s="12">
         <v>6</v>
       </c>
       <c r="C295" s="12" t="s">
-        <v>263</v>
+        <v>256</v>
       </c>
       <c r="D295" s="9" t="s">
         <v>7</v>
       </c>
       <c r="E295" s="1" t="s">
-        <v>282</v>
+        <v>275</v>
       </c>
       <c r="F295" s="1" t="s">
         <v>55</v>
@@ -7440,19 +7441,19 @@
     </row>
     <row r="296" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A296" s="12" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="B296" s="12">
         <v>6</v>
       </c>
       <c r="C296" s="12" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="D296" s="9" t="s">
         <v>9</v>
       </c>
       <c r="E296" s="1" t="s">
-        <v>178</v>
+        <v>171</v>
       </c>
       <c r="F296" s="1" t="s">
         <v>55</v>
@@ -7460,19 +7461,19 @@
     </row>
     <row r="297" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A297" s="12" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="B297" s="12">
         <v>6</v>
       </c>
       <c r="C297" s="12" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
       <c r="D297" s="9" t="s">
         <v>9</v>
       </c>
       <c r="E297" s="1" t="s">
-        <v>199</v>
+        <v>192</v>
       </c>
       <c r="F297" s="1" t="s">
         <v>55</v>
@@ -7480,19 +7481,19 @@
     </row>
     <row r="298" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A298" s="12" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="B298" s="12">
         <v>6</v>
       </c>
       <c r="C298" s="12" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="D298" s="9" t="s">
         <v>9</v>
       </c>
       <c r="E298" s="1" t="s">
-        <v>220</v>
+        <v>213</v>
       </c>
       <c r="F298" s="1" t="s">
         <v>55</v>
@@ -7500,19 +7501,19 @@
     </row>
     <row r="299" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A299" s="12" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="B299" s="12">
         <v>6</v>
       </c>
       <c r="C299" s="12" t="s">
-        <v>221</v>
+        <v>214</v>
       </c>
       <c r="D299" s="9" t="s">
         <v>9</v>
       </c>
       <c r="E299" s="1" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="F299" s="1" t="s">
         <v>55</v>
@@ -7520,19 +7521,19 @@
     </row>
     <row r="300" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A300" s="12" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="B300" s="12">
         <v>6</v>
       </c>
       <c r="C300" s="12" t="s">
-        <v>242</v>
+        <v>235</v>
       </c>
       <c r="D300" s="9" t="s">
         <v>9</v>
       </c>
       <c r="E300" s="1" t="s">
-        <v>262</v>
+        <v>255</v>
       </c>
       <c r="F300" s="1" t="s">
         <v>55</v>
@@ -7540,19 +7541,19 @@
     </row>
     <row r="301" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A301" s="12" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="B301" s="12">
         <v>6</v>
       </c>
       <c r="C301" s="12" t="s">
-        <v>263</v>
+        <v>256</v>
       </c>
       <c r="D301" s="9" t="s">
         <v>9</v>
       </c>
       <c r="E301" s="1" t="s">
-        <v>283</v>
+        <v>276</v>
       </c>
       <c r="F301" s="1" t="s">
         <v>55</v>

</xml_diff>

<commit_message>
Diversify US related to "Economics" domain
</commit_message>
<xml_diff>
--- a/refair-server/datasets/few shot dataset/FSDataset.xlsx
+++ b/refair-server/datasets/few shot dataset/FSDataset.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\morel\Desktop\Refair\ReFair-App\refair-server\datasets\few shot dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C030B0C-5A4A-4F1E-A9CD-5FFB297AA492}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97058292-C55F-48FC-8EB5-79540C9FA813}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{80773445-FB61-4F04-A882-1600FD96C55A}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{80773445-FB61-4F04-A882-1600FD96C55A}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -434,33 +434,15 @@
     <t>As an economist, I want to utilize CNNs to analyze historical economic data and extract spatial and temporal patterns, facilitating better understanding of economic cycles and trends</t>
   </si>
   <si>
-    <t>As an economist, I need a conversational agent capable of interpreting complex economic policies and explaining their implications to stakeholders, ensuring transparency and informed public discourse.</t>
-  </si>
-  <si>
-    <t>As an economist, I want to use decision trees to classify economic sectors based on their growth potential and risk profiles, aiding in portfolio diversification strategies for investment firms.</t>
-  </si>
-  <si>
-    <t>As an economist, I want to implement document classification systems to automatically organize and prioritize incoming economic research publications based on their relevance and impact, supporting efficient knowledge discovery and academic collaboration.</t>
-  </si>
-  <si>
     <t>As an economist, I want to apply entity extraction techniques to automatically identify and categorize economic indicators (e.g., GDP, inflation rate, unemployment rate) mentioned in textual data such as news articles and economic reports, to facilitate quantitative analysis and trend monitoring.</t>
   </si>
   <si>
-    <t>As an economist, I want to employ feature selection techniques to identify the most relevant economic indicators (e.g., GDP growth rate, inflation index) for predicting stock market movements, optimizing forecasting models used by financial institutions.</t>
-  </si>
-  <si>
     <t>As an economist, I need to handle imbalanced datasets when predicting economic downturns to improve the reliability of early warning systems, enabling proactive policy responses and mitigation measures.</t>
   </si>
   <si>
     <t>As an economist, I want to apply keyword extraction techniques to analyze customer feedback and reviews related to economic products and services, extracting sentiments and key concerns to guide market strategies and product development.</t>
   </si>
   <si>
-    <t>As an economist, I need k-NN models to analyze regional economic data and identify neighboring regions with similar economic profiles, enabling comparative analysis and policy recommendations for regional development.</t>
-  </si>
-  <si>
-    <t>As an economist, I want to use multi-label classification techniques to segment economic indicators (e.g., inflation rate, unemployment rate, GDP growth) based on their impact on various demographic groups, aiding in equitable economic policy formulation.</t>
-  </si>
-  <si>
     <t>As an economist, I want to leverage neural networks to predict stock market movements based on historical market data and economic indicators, enhancing investment decision-making and portfolio management.</t>
   </si>
   <si>
@@ -473,21 +455,12 @@
     <t>As an economist, I need sentiment analysis tools to analyze investor sentiment based on financial news and market reports, predicting market movements and investor behavior for effective risk management.</t>
   </si>
   <si>
-    <t>As an economist, I want to utilize speech to text technology to transcribe meetings with clients and stakeholders discussing economic forecasts and investment strategies, ensuring comprehensive and searchable records for future reference.</t>
-  </si>
-  <si>
     <t>As an economist, I want to use text categorization techniques to classify research papers and articles into economic sub-disciplines such as behavioral economics, development economics, and monetary economics, facilitating targeted literature reviews and research synthesis.</t>
   </si>
   <si>
-    <t>As an economist, I aim to deploy unsupervised clustering models to group similar industries based on their economic contributions and market behaviors, facilitating sector-specific economic analysis and policy formulation.</t>
-  </si>
-  <si>
     <t>As an economist, I want to utilize voice recognition technology to transcribe meetings with clients and stakeholders discussing economic strategies and investment opportunities, maintaining detailed records for strategic decision-making.</t>
   </si>
   <si>
-    <t>As an economist, I want to use word embedding techniques to analyze customer feedback and reviews on economic products and services, extracting underlying sentiments and preferences to guide product development and market positioning strategies.</t>
-  </si>
-  <si>
     <t>Medicine &amp; Health</t>
   </si>
   <si>
@@ -1077,6 +1050,33 @@
   </si>
   <si>
     <t>As a digital archivist, I want to leverage unsupervised clustering techniques to organize large archives of historical news articles into coherent thematic collections, improving accessibility and facilitating research in media history.</t>
+  </si>
+  <si>
+    <t>As an economic advisor, I want to develop a conversational agent powered by natural language processing to provide personalized financial advice to clients, helping them make informed investment decisions based on their financial goals and risk tolerance.</t>
+  </si>
+  <si>
+    <t>As an economic analyst, I want to utilize decision tree models to classify different types of economic indicators (e.g., leading, lagging, coincident) based on historical data, aiding in the identification of key economic trends and turning points.</t>
+  </si>
+  <si>
+    <t>As an economic researcher, I want to develop a document classification system to categorize research papers into economic theories (e.g., Keynesian economics, supply-side economics) based on their content, facilitating easier literature review and analysis.</t>
+  </si>
+  <si>
+    <t>As an economic policy advisor, I want to apply feature selection methods to labor market data to pinpoint the crucial variables (e.g., unemployment rate, job openings) affecting employment trends, guiding policy recommendations.</t>
+  </si>
+  <si>
+    <t>As a trade economist, I want to apply k-nearest neighbor algorithms to identify countries with similar trade patterns based on economic indicators such as export-import ratios and GDP growth rates, facilitating comparative trade analysis and policy recommendations.</t>
+  </si>
+  <si>
+    <t>As a trade economist, I seek to use multi-label classification techniques to classify trade agreements between countries into multiple categories (e.g., tariff reduction, trade facilitation, dispute resolution), helping analyze the impact on global trade flows.</t>
+  </si>
+  <si>
+    <t>As a business consultant, I want to implement speech to text capabilities to analyze focus group discussions and customer interviews about economic products and services, extracting actionable insights for business strategies.</t>
+  </si>
+  <si>
+    <t>As a trade economist, I want to use unsupervised clustering techniques to identify clusters of countries based on their trade patterns and economic similarities, aiding in comparative trade analysis and policy recommendations.</t>
+  </si>
+  <si>
+    <t>As an economic consultant, I seek to use word embedding techniques to analyze economic policy documents and identify clusters of related policy initiatives and their potential impacts on economic outcomes.</t>
   </si>
 </sst>
 </file>
@@ -1526,8 +1526,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8DF0B04-8323-4309-B759-D1CDDA1FBB0E}">
   <dimension ref="A1:F301"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C60" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D81" sqref="D81"/>
+    <sheetView tabSelected="1" topLeftCell="E2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1626,7 +1626,7 @@
       <c r="B5" s="10">
         <v>2</v>
       </c>
-      <c r="C5" s="10" t="s">
+      <c r="C5" s="11" t="s">
         <v>129</v>
       </c>
       <c r="D5" s="9" t="s">
@@ -1673,7 +1673,7 @@
         <v>23</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>132</v>
+        <v>338</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>55</v>
@@ -1713,7 +1713,7 @@
         <v>12</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>133</v>
+        <v>339</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>55</v>
@@ -1753,7 +1753,7 @@
         <v>33</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>134</v>
+        <v>340</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>55</v>
@@ -1793,7 +1793,7 @@
         <v>25</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>55</v>
@@ -1833,7 +1833,7 @@
         <v>28</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>136</v>
+        <v>341</v>
       </c>
       <c r="F15" s="1" t="s">
         <v>55</v>
@@ -1873,7 +1873,7 @@
         <v>13</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="F17" s="1" t="s">
         <v>55</v>
@@ -1913,7 +1913,7 @@
         <v>26</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="F19" s="1" t="s">
         <v>55</v>
@@ -1953,7 +1953,7 @@
         <v>14</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>139</v>
+        <v>342</v>
       </c>
       <c r="F21" s="1" t="s">
         <v>55</v>
@@ -1993,7 +1993,7 @@
         <v>30</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>140</v>
+        <v>343</v>
       </c>
       <c r="F23" s="1" t="s">
         <v>55</v>
@@ -2033,7 +2033,7 @@
         <v>15</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="F25" s="1" t="s">
         <v>55</v>
@@ -2073,7 +2073,7 @@
         <v>16</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="F27" s="1" t="s">
         <v>55</v>
@@ -2086,7 +2086,7 @@
       <c r="B28" s="10">
         <v>2</v>
       </c>
-      <c r="C28" s="10" t="s">
+      <c r="C28" s="11" t="s">
         <v>108</v>
       </c>
       <c r="D28" s="9" t="s">
@@ -2113,7 +2113,7 @@
         <v>17</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="F29" s="1" t="s">
         <v>55</v>
@@ -2153,7 +2153,7 @@
         <v>29</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="F31" s="1" t="s">
         <v>55</v>
@@ -2193,7 +2193,7 @@
         <v>18</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>145</v>
+        <v>344</v>
       </c>
       <c r="F33" s="1" t="s">
         <v>55</v>
@@ -2233,7 +2233,7 @@
         <v>20</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
       <c r="F35" s="1" t="s">
         <v>55</v>
@@ -2273,7 +2273,7 @@
         <v>24</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>147</v>
+        <v>345</v>
       </c>
       <c r="F37" s="1" t="s">
         <v>55</v>
@@ -2313,7 +2313,7 @@
         <v>7</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>148</v>
+        <v>140</v>
       </c>
       <c r="F39" s="1" t="s">
         <v>55</v>
@@ -2353,7 +2353,7 @@
         <v>9</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>149</v>
+        <v>346</v>
       </c>
       <c r="F41" s="1" t="s">
         <v>55</v>
@@ -2513,7 +2513,7 @@
         <v>12</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>340</v>
+        <v>331</v>
       </c>
       <c r="F49" s="1" t="s">
         <v>55</v>
@@ -2553,7 +2553,7 @@
         <v>33</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>341</v>
+        <v>332</v>
       </c>
       <c r="F51" s="1" t="s">
         <v>55</v>
@@ -2633,7 +2633,7 @@
         <v>28</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>342</v>
+        <v>333</v>
       </c>
       <c r="F55" s="1" t="s">
         <v>55</v>
@@ -2713,7 +2713,7 @@
         <v>26</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>343</v>
+        <v>334</v>
       </c>
       <c r="F59" s="1" t="s">
         <v>55</v>
@@ -2833,7 +2833,7 @@
         <v>15</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>344</v>
+        <v>335</v>
       </c>
       <c r="F65" s="1" t="s">
         <v>55</v>
@@ -2913,7 +2913,7 @@
         <v>17</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>345</v>
+        <v>336</v>
       </c>
       <c r="F69" s="1" t="s">
         <v>55</v>
@@ -3073,7 +3073,7 @@
         <v>24</v>
       </c>
       <c r="E77" s="1" t="s">
-        <v>346</v>
+        <v>337</v>
       </c>
       <c r="F77" s="1" t="s">
         <v>55</v>
@@ -3173,7 +3173,7 @@
         <v>22</v>
       </c>
       <c r="E82" s="1" t="s">
-        <v>323</v>
+        <v>314</v>
       </c>
       <c r="F82" s="1" t="s">
         <v>55</v>
@@ -3193,7 +3193,7 @@
         <v>22</v>
       </c>
       <c r="E83" s="1" t="s">
-        <v>306</v>
+        <v>297</v>
       </c>
       <c r="F83" s="1" t="s">
         <v>55</v>
@@ -3213,7 +3213,7 @@
         <v>32</v>
       </c>
       <c r="E84" s="1" t="s">
-        <v>324</v>
+        <v>315</v>
       </c>
       <c r="F84" s="1" t="s">
         <v>55</v>
@@ -3253,7 +3253,7 @@
         <v>23</v>
       </c>
       <c r="E86" s="1" t="s">
-        <v>325</v>
+        <v>316</v>
       </c>
       <c r="F86" s="1" t="s">
         <v>55</v>
@@ -3273,7 +3273,7 @@
         <v>23</v>
       </c>
       <c r="E87" s="1" t="s">
-        <v>307</v>
+        <v>298</v>
       </c>
       <c r="F87" s="1" t="s">
         <v>55</v>
@@ -3313,7 +3313,7 @@
         <v>12</v>
       </c>
       <c r="E89" s="1" t="s">
-        <v>308</v>
+        <v>299</v>
       </c>
       <c r="F89" s="1" t="s">
         <v>55</v>
@@ -3333,7 +3333,7 @@
         <v>33</v>
       </c>
       <c r="E90" s="1" t="s">
-        <v>326</v>
+        <v>317</v>
       </c>
       <c r="F90" s="1" t="s">
         <v>55</v>
@@ -3353,7 +3353,7 @@
         <v>33</v>
       </c>
       <c r="E91" s="1" t="s">
-        <v>309</v>
+        <v>300</v>
       </c>
       <c r="F91" s="1" t="s">
         <v>55</v>
@@ -3373,7 +3373,7 @@
         <v>25</v>
       </c>
       <c r="E92" s="1" t="s">
-        <v>327</v>
+        <v>318</v>
       </c>
       <c r="F92" s="1" t="s">
         <v>55</v>
@@ -3393,7 +3393,7 @@
         <v>25</v>
       </c>
       <c r="E93" s="1" t="s">
-        <v>310</v>
+        <v>301</v>
       </c>
       <c r="F93" s="1" t="s">
         <v>55</v>
@@ -3453,7 +3453,7 @@
         <v>13</v>
       </c>
       <c r="E96" s="1" t="s">
-        <v>328</v>
+        <v>319</v>
       </c>
       <c r="F96" s="1" t="s">
         <v>55</v>
@@ -3473,7 +3473,7 @@
         <v>13</v>
       </c>
       <c r="E97" s="1" t="s">
-        <v>311</v>
+        <v>302</v>
       </c>
       <c r="F97" s="1" t="s">
         <v>55</v>
@@ -3493,7 +3493,7 @@
         <v>26</v>
       </c>
       <c r="E98" s="1" t="s">
-        <v>329</v>
+        <v>320</v>
       </c>
       <c r="F98" s="1" t="s">
         <v>55</v>
@@ -3533,7 +3533,7 @@
         <v>14</v>
       </c>
       <c r="E100" s="1" t="s">
-        <v>331</v>
+        <v>322</v>
       </c>
       <c r="F100" s="1" t="s">
         <v>55</v>
@@ -3553,7 +3553,7 @@
         <v>14</v>
       </c>
       <c r="E101" s="1" t="s">
-        <v>312</v>
+        <v>303</v>
       </c>
       <c r="F101" s="1" t="s">
         <v>55</v>
@@ -3573,7 +3573,7 @@
         <v>30</v>
       </c>
       <c r="E102" s="1" t="s">
-        <v>330</v>
+        <v>321</v>
       </c>
       <c r="F102" s="1" t="s">
         <v>55</v>
@@ -3593,7 +3593,7 @@
         <v>30</v>
       </c>
       <c r="E103" s="1" t="s">
-        <v>313</v>
+        <v>304</v>
       </c>
       <c r="F103" s="1" t="s">
         <v>55</v>
@@ -3613,7 +3613,7 @@
         <v>15</v>
       </c>
       <c r="E104" s="1" t="s">
-        <v>332</v>
+        <v>323</v>
       </c>
       <c r="F104" s="1" t="s">
         <v>55</v>
@@ -3633,7 +3633,7 @@
         <v>15</v>
       </c>
       <c r="E105" s="1" t="s">
-        <v>314</v>
+        <v>305</v>
       </c>
       <c r="F105" s="1" t="s">
         <v>55</v>
@@ -3653,7 +3653,7 @@
         <v>16</v>
       </c>
       <c r="E106" s="1" t="s">
-        <v>333</v>
+        <v>324</v>
       </c>
       <c r="F106" s="1" t="s">
         <v>55</v>
@@ -3673,7 +3673,7 @@
         <v>16</v>
       </c>
       <c r="E107" s="1" t="s">
-        <v>315</v>
+        <v>306</v>
       </c>
       <c r="F107" s="1" t="s">
         <v>55</v>
@@ -3693,7 +3693,7 @@
         <v>17</v>
       </c>
       <c r="E108" s="1" t="s">
-        <v>334</v>
+        <v>325</v>
       </c>
       <c r="F108" s="1" t="s">
         <v>55</v>
@@ -3713,7 +3713,7 @@
         <v>17</v>
       </c>
       <c r="E109" s="1" t="s">
-        <v>316</v>
+        <v>307</v>
       </c>
       <c r="F109" s="1" t="s">
         <v>55</v>
@@ -3733,7 +3733,7 @@
         <v>29</v>
       </c>
       <c r="E110" s="1" t="s">
-        <v>335</v>
+        <v>326</v>
       </c>
       <c r="F110" s="1" t="s">
         <v>55</v>
@@ -3753,7 +3753,7 @@
         <v>29</v>
       </c>
       <c r="E111" s="1" t="s">
-        <v>317</v>
+        <v>308</v>
       </c>
       <c r="F111" s="1" t="s">
         <v>55</v>
@@ -3773,7 +3773,7 @@
         <v>18</v>
       </c>
       <c r="E112" s="1" t="s">
-        <v>336</v>
+        <v>327</v>
       </c>
       <c r="F112" s="1" t="s">
         <v>55</v>
@@ -3793,7 +3793,7 @@
         <v>18</v>
       </c>
       <c r="E113" s="1" t="s">
-        <v>318</v>
+        <v>309</v>
       </c>
       <c r="F113" s="1" t="s">
         <v>55</v>
@@ -3833,7 +3833,7 @@
         <v>20</v>
       </c>
       <c r="E115" s="6" t="s">
-        <v>319</v>
+        <v>310</v>
       </c>
       <c r="F115" s="1" t="s">
         <v>55</v>
@@ -3853,7 +3853,7 @@
         <v>24</v>
       </c>
       <c r="E116" s="1" t="s">
-        <v>337</v>
+        <v>328</v>
       </c>
       <c r="F116" s="1" t="s">
         <v>55</v>
@@ -3873,7 +3873,7 @@
         <v>24</v>
       </c>
       <c r="E117" s="1" t="s">
-        <v>320</v>
+        <v>311</v>
       </c>
       <c r="F117" s="1" t="s">
         <v>55</v>
@@ -3893,7 +3893,7 @@
         <v>7</v>
       </c>
       <c r="E118" s="1" t="s">
-        <v>338</v>
+        <v>329</v>
       </c>
       <c r="F118" s="1" t="s">
         <v>55</v>
@@ -3913,7 +3913,7 @@
         <v>7</v>
       </c>
       <c r="E119" s="1" t="s">
-        <v>321</v>
+        <v>312</v>
       </c>
       <c r="F119" s="1" t="s">
         <v>55</v>
@@ -3933,7 +3933,7 @@
         <v>9</v>
       </c>
       <c r="E120" s="1" t="s">
-        <v>339</v>
+        <v>330</v>
       </c>
       <c r="F120" s="1" t="s">
         <v>55</v>
@@ -3953,7 +3953,7 @@
         <v>9</v>
       </c>
       <c r="E121" s="1" t="s">
-        <v>322</v>
+        <v>313</v>
       </c>
       <c r="F121" s="1" t="s">
         <v>55</v>
@@ -4013,7 +4013,7 @@
         <v>22</v>
       </c>
       <c r="E124" s="1" t="s">
-        <v>290</v>
+        <v>281</v>
       </c>
       <c r="F124" s="1" t="s">
         <v>55</v>
@@ -4033,7 +4033,7 @@
         <v>32</v>
       </c>
       <c r="E125" s="6" t="s">
-        <v>277</v>
+        <v>268</v>
       </c>
       <c r="F125" s="1" t="s">
         <v>55</v>
@@ -4073,7 +4073,7 @@
         <v>32</v>
       </c>
       <c r="E127" s="1" t="s">
-        <v>291</v>
+        <v>282</v>
       </c>
       <c r="F127" s="1" t="s">
         <v>55</v>
@@ -4093,7 +4093,7 @@
         <v>23</v>
       </c>
       <c r="E128" s="1" t="s">
-        <v>278</v>
+        <v>269</v>
       </c>
       <c r="F128" s="1" t="s">
         <v>55</v>
@@ -4133,7 +4133,7 @@
         <v>23</v>
       </c>
       <c r="E130" s="1" t="s">
-        <v>292</v>
+        <v>283</v>
       </c>
       <c r="F130" s="1" t="s">
         <v>55</v>
@@ -4193,7 +4193,7 @@
         <v>12</v>
       </c>
       <c r="E133" s="6" t="s">
-        <v>293</v>
+        <v>284</v>
       </c>
       <c r="F133" s="1" t="s">
         <v>55</v>
@@ -4213,7 +4213,7 @@
         <v>33</v>
       </c>
       <c r="E134" s="1" t="s">
-        <v>279</v>
+        <v>270</v>
       </c>
       <c r="F134" s="1" t="s">
         <v>55</v>
@@ -4253,7 +4253,7 @@
         <v>33</v>
       </c>
       <c r="E136" s="1" t="s">
-        <v>294</v>
+        <v>285</v>
       </c>
       <c r="F136" s="1" t="s">
         <v>55</v>
@@ -4273,7 +4273,7 @@
         <v>25</v>
       </c>
       <c r="E137" s="1" t="s">
-        <v>280</v>
+        <v>271</v>
       </c>
       <c r="F137" s="1" t="s">
         <v>55</v>
@@ -4313,7 +4313,7 @@
         <v>25</v>
       </c>
       <c r="E139" s="1" t="s">
-        <v>295</v>
+        <v>286</v>
       </c>
       <c r="F139" s="1" t="s">
         <v>55</v>
@@ -4373,7 +4373,7 @@
         <v>28</v>
       </c>
       <c r="E142" s="1" t="s">
-        <v>296</v>
+        <v>287</v>
       </c>
       <c r="F142" s="1" t="s">
         <v>55</v>
@@ -4393,7 +4393,7 @@
         <v>13</v>
       </c>
       <c r="E143" s="6" t="s">
-        <v>281</v>
+        <v>272</v>
       </c>
       <c r="F143" s="1" t="s">
         <v>55</v>
@@ -4433,7 +4433,7 @@
         <v>13</v>
       </c>
       <c r="E145" s="1" t="s">
-        <v>297</v>
+        <v>288</v>
       </c>
       <c r="F145" s="1" t="s">
         <v>55</v>
@@ -4493,7 +4493,7 @@
         <v>26</v>
       </c>
       <c r="E148" s="1" t="s">
-        <v>298</v>
+        <v>289</v>
       </c>
       <c r="F148" s="1" t="s">
         <v>55</v>
@@ -4513,7 +4513,7 @@
         <v>14</v>
       </c>
       <c r="E149" s="1" t="s">
-        <v>283</v>
+        <v>274</v>
       </c>
       <c r="F149" s="1" t="s">
         <v>55</v>
@@ -4533,7 +4533,7 @@
         <v>14</v>
       </c>
       <c r="E150" s="1" t="s">
-        <v>305</v>
+        <v>296</v>
       </c>
       <c r="F150" s="1" t="s">
         <v>55</v>
@@ -4553,7 +4553,7 @@
         <v>14</v>
       </c>
       <c r="E151" s="1" t="s">
-        <v>299</v>
+        <v>290</v>
       </c>
       <c r="F151" s="1" t="s">
         <v>55</v>
@@ -4573,7 +4573,7 @@
         <v>30</v>
       </c>
       <c r="E152" s="1" t="s">
-        <v>282</v>
+        <v>273</v>
       </c>
       <c r="F152" s="1" t="s">
         <v>55</v>
@@ -4613,7 +4613,7 @@
         <v>30</v>
       </c>
       <c r="E154" s="1" t="s">
-        <v>300</v>
+        <v>291</v>
       </c>
       <c r="F154" s="1" t="s">
         <v>55</v>
@@ -4633,7 +4633,7 @@
         <v>15</v>
       </c>
       <c r="E155" s="1" t="s">
-        <v>284</v>
+        <v>275</v>
       </c>
       <c r="F155" s="1" t="s">
         <v>55</v>
@@ -4673,7 +4673,7 @@
         <v>15</v>
       </c>
       <c r="E157" s="1" t="s">
-        <v>301</v>
+        <v>292</v>
       </c>
       <c r="F157" s="1" t="s">
         <v>55</v>
@@ -4693,7 +4693,7 @@
         <v>16</v>
       </c>
       <c r="E158" s="1" t="s">
-        <v>285</v>
+        <v>276</v>
       </c>
       <c r="F158" s="1" t="s">
         <v>55</v>
@@ -4753,7 +4753,7 @@
         <v>17</v>
       </c>
       <c r="E161" s="1" t="s">
-        <v>287</v>
+        <v>278</v>
       </c>
       <c r="F161" s="1" t="s">
         <v>55</v>
@@ -4813,7 +4813,7 @@
         <v>29</v>
       </c>
       <c r="E164" s="1" t="s">
-        <v>286</v>
+        <v>277</v>
       </c>
       <c r="F164" s="1" t="s">
         <v>55</v>
@@ -4853,7 +4853,7 @@
         <v>29</v>
       </c>
       <c r="E166" s="1" t="s">
-        <v>302</v>
+        <v>293</v>
       </c>
       <c r="F166" s="1" t="s">
         <v>55</v>
@@ -4873,7 +4873,7 @@
         <v>18</v>
       </c>
       <c r="E167" s="1" t="s">
-        <v>288</v>
+        <v>279</v>
       </c>
       <c r="F167" s="1" t="s">
         <v>55</v>
@@ -4973,7 +4973,7 @@
         <v>20</v>
       </c>
       <c r="E172" s="1" t="s">
-        <v>303</v>
+        <v>294</v>
       </c>
       <c r="F172" s="1" t="s">
         <v>55</v>
@@ -4993,7 +4993,7 @@
         <v>24</v>
       </c>
       <c r="E173" s="1" t="s">
-        <v>289</v>
+        <v>280</v>
       </c>
       <c r="F173" s="1" t="s">
         <v>55</v>
@@ -5093,7 +5093,7 @@
         <v>7</v>
       </c>
       <c r="E178" s="1" t="s">
-        <v>304</v>
+        <v>295</v>
       </c>
       <c r="F178" s="1" t="s">
         <v>55</v>
@@ -5161,19 +5161,19 @@
     </row>
     <row r="182" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A182" s="12" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="B182" s="12">
         <v>6</v>
       </c>
       <c r="C182" s="12" t="s">
-        <v>151</v>
+        <v>142</v>
       </c>
       <c r="D182" s="9" t="s">
         <v>22</v>
       </c>
       <c r="E182" s="1" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
       <c r="F182" s="1" t="s">
         <v>55</v>
@@ -5181,19 +5181,19 @@
     </row>
     <row r="183" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A183" s="12" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="B183" s="12">
         <v>6</v>
       </c>
       <c r="C183" s="12" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
       <c r="D183" s="9" t="s">
         <v>22</v>
       </c>
       <c r="E183" s="1" t="s">
-        <v>173</v>
+        <v>164</v>
       </c>
       <c r="F183" s="1" t="s">
         <v>55</v>
@@ -5201,19 +5201,19 @@
     </row>
     <row r="184" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A184" s="12" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="B184" s="12">
         <v>6</v>
       </c>
       <c r="C184" s="12" t="s">
-        <v>193</v>
+        <v>184</v>
       </c>
       <c r="D184" s="9" t="s">
         <v>22</v>
       </c>
       <c r="E184" s="1" t="s">
-        <v>194</v>
+        <v>185</v>
       </c>
       <c r="F184" s="1" t="s">
         <v>55</v>
@@ -5221,19 +5221,19 @@
     </row>
     <row r="185" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A185" s="12" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="B185" s="12">
         <v>6</v>
       </c>
       <c r="C185" s="12" t="s">
-        <v>214</v>
+        <v>205</v>
       </c>
       <c r="D185" s="9" t="s">
         <v>22</v>
       </c>
       <c r="E185" s="1" t="s">
-        <v>215</v>
+        <v>206</v>
       </c>
       <c r="F185" s="1" t="s">
         <v>55</v>
@@ -5241,19 +5241,19 @@
     </row>
     <row r="186" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A186" s="12" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="B186" s="12">
         <v>6</v>
       </c>
       <c r="C186" s="12" t="s">
-        <v>235</v>
+        <v>226</v>
       </c>
       <c r="D186" s="9" t="s">
         <v>22</v>
       </c>
       <c r="E186" s="1" t="s">
-        <v>236</v>
+        <v>227</v>
       </c>
       <c r="F186" s="1" t="s">
         <v>55</v>
@@ -5261,19 +5261,19 @@
     </row>
     <row r="187" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A187" s="12" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="B187" s="12">
         <v>6</v>
       </c>
       <c r="C187" s="12" t="s">
-        <v>256</v>
+        <v>247</v>
       </c>
       <c r="D187" s="9" t="s">
         <v>22</v>
       </c>
       <c r="E187" s="1" t="s">
-        <v>257</v>
+        <v>248</v>
       </c>
       <c r="F187" s="1" t="s">
         <v>55</v>
@@ -5281,19 +5281,19 @@
     </row>
     <row r="188" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A188" s="12" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="B188" s="12">
         <v>6</v>
       </c>
       <c r="C188" s="12" t="s">
-        <v>151</v>
+        <v>142</v>
       </c>
       <c r="D188" s="9" t="s">
         <v>32</v>
       </c>
       <c r="E188" s="1" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="F188" s="1" t="s">
         <v>55</v>
@@ -5301,19 +5301,19 @@
     </row>
     <row r="189" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A189" s="12" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="B189" s="12">
         <v>6</v>
       </c>
       <c r="C189" s="12" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
       <c r="D189" s="9" t="s">
         <v>32</v>
       </c>
       <c r="E189" s="1" t="s">
-        <v>174</v>
+        <v>165</v>
       </c>
       <c r="F189" s="1" t="s">
         <v>55</v>
@@ -5321,19 +5321,19 @@
     </row>
     <row r="190" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A190" s="12" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="B190" s="12">
         <v>6</v>
       </c>
       <c r="C190" s="12" t="s">
-        <v>193</v>
+        <v>184</v>
       </c>
       <c r="D190" s="9" t="s">
         <v>32</v>
       </c>
       <c r="E190" s="1" t="s">
-        <v>195</v>
+        <v>186</v>
       </c>
       <c r="F190" s="1" t="s">
         <v>55</v>
@@ -5341,19 +5341,19 @@
     </row>
     <row r="191" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A191" s="12" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="B191" s="12">
         <v>6</v>
       </c>
       <c r="C191" s="12" t="s">
-        <v>214</v>
+        <v>205</v>
       </c>
       <c r="D191" s="9" t="s">
         <v>32</v>
       </c>
       <c r="E191" s="1" t="s">
-        <v>216</v>
+        <v>207</v>
       </c>
       <c r="F191" s="1" t="s">
         <v>55</v>
@@ -5361,19 +5361,19 @@
     </row>
     <row r="192" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A192" s="12" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="B192" s="12">
         <v>6</v>
       </c>
       <c r="C192" s="12" t="s">
-        <v>235</v>
+        <v>226</v>
       </c>
       <c r="D192" s="9" t="s">
         <v>32</v>
       </c>
       <c r="E192" s="1" t="s">
-        <v>237</v>
+        <v>228</v>
       </c>
       <c r="F192" s="1" t="s">
         <v>55</v>
@@ -5381,19 +5381,19 @@
     </row>
     <row r="193" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A193" s="12" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="B193" s="12">
         <v>6</v>
       </c>
       <c r="C193" s="12" t="s">
-        <v>256</v>
+        <v>247</v>
       </c>
       <c r="D193" s="9" t="s">
         <v>32</v>
       </c>
       <c r="E193" s="1" t="s">
-        <v>258</v>
+        <v>249</v>
       </c>
       <c r="F193" s="1" t="s">
         <v>55</v>
@@ -5401,19 +5401,19 @@
     </row>
     <row r="194" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A194" s="12" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="B194" s="12">
         <v>6</v>
       </c>
       <c r="C194" s="12" t="s">
-        <v>151</v>
+        <v>142</v>
       </c>
       <c r="D194" s="9" t="s">
         <v>23</v>
       </c>
       <c r="E194" s="1" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="F194" s="1" t="s">
         <v>55</v>
@@ -5421,19 +5421,19 @@
     </row>
     <row r="195" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A195" s="12" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="B195" s="12">
         <v>6</v>
       </c>
       <c r="C195" s="12" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
       <c r="D195" s="9" t="s">
         <v>23</v>
       </c>
       <c r="E195" s="1" t="s">
-        <v>175</v>
+        <v>166</v>
       </c>
       <c r="F195" s="1" t="s">
         <v>55</v>
@@ -5441,19 +5441,19 @@
     </row>
     <row r="196" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A196" s="12" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="B196" s="12">
         <v>6</v>
       </c>
       <c r="C196" s="12" t="s">
-        <v>193</v>
+        <v>184</v>
       </c>
       <c r="D196" s="9" t="s">
         <v>23</v>
       </c>
       <c r="E196" s="1" t="s">
-        <v>196</v>
+        <v>187</v>
       </c>
       <c r="F196" s="1" t="s">
         <v>55</v>
@@ -5461,19 +5461,19 @@
     </row>
     <row r="197" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A197" s="12" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="B197" s="12">
         <v>6</v>
       </c>
       <c r="C197" s="12" t="s">
-        <v>214</v>
+        <v>205</v>
       </c>
       <c r="D197" s="9" t="s">
         <v>23</v>
       </c>
       <c r="E197" s="1" t="s">
-        <v>217</v>
+        <v>208</v>
       </c>
       <c r="F197" s="1" t="s">
         <v>55</v>
@@ -5481,19 +5481,19 @@
     </row>
     <row r="198" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A198" s="12" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="B198" s="12">
         <v>6</v>
       </c>
       <c r="C198" s="12" t="s">
-        <v>235</v>
+        <v>226</v>
       </c>
       <c r="D198" s="9" t="s">
         <v>23</v>
       </c>
       <c r="E198" s="1" t="s">
-        <v>238</v>
+        <v>229</v>
       </c>
       <c r="F198" s="1" t="s">
         <v>55</v>
@@ -5501,19 +5501,19 @@
     </row>
     <row r="199" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A199" s="12" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="B199" s="12">
         <v>6</v>
       </c>
       <c r="C199" s="12" t="s">
-        <v>256</v>
+        <v>247</v>
       </c>
       <c r="D199" s="9" t="s">
         <v>23</v>
       </c>
       <c r="E199" s="1" t="s">
-        <v>259</v>
+        <v>250</v>
       </c>
       <c r="F199" s="1" t="s">
         <v>55</v>
@@ -5521,19 +5521,19 @@
     </row>
     <row r="200" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A200" s="12" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="B200" s="12">
         <v>6</v>
       </c>
       <c r="C200" s="12" t="s">
-        <v>151</v>
+        <v>142</v>
       </c>
       <c r="D200" s="9" t="s">
         <v>12</v>
       </c>
       <c r="E200" s="1" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="F200" s="1" t="s">
         <v>55</v>
@@ -5541,19 +5541,19 @@
     </row>
     <row r="201" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A201" s="12" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="B201" s="12">
         <v>6</v>
       </c>
       <c r="C201" s="12" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
       <c r="D201" s="9" t="s">
         <v>12</v>
       </c>
       <c r="E201" s="1" t="s">
-        <v>176</v>
+        <v>167</v>
       </c>
       <c r="F201" s="1" t="s">
         <v>55</v>
@@ -5561,19 +5561,19 @@
     </row>
     <row r="202" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A202" s="12" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="B202" s="12">
         <v>6</v>
       </c>
       <c r="C202" s="12" t="s">
-        <v>193</v>
+        <v>184</v>
       </c>
       <c r="D202" s="9" t="s">
         <v>12</v>
       </c>
       <c r="E202" s="1" t="s">
-        <v>197</v>
+        <v>188</v>
       </c>
       <c r="F202" s="1" t="s">
         <v>55</v>
@@ -5581,19 +5581,19 @@
     </row>
     <row r="203" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A203" s="12" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="B203" s="12">
         <v>6</v>
       </c>
       <c r="C203" s="12" t="s">
-        <v>214</v>
+        <v>205</v>
       </c>
       <c r="D203" s="9" t="s">
         <v>12</v>
       </c>
       <c r="E203" s="1" t="s">
-        <v>218</v>
+        <v>209</v>
       </c>
       <c r="F203" s="1" t="s">
         <v>55</v>
@@ -5601,19 +5601,19 @@
     </row>
     <row r="204" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A204" s="12" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="B204" s="12">
         <v>6</v>
       </c>
       <c r="C204" s="12" t="s">
-        <v>235</v>
+        <v>226</v>
       </c>
       <c r="D204" s="9" t="s">
         <v>12</v>
       </c>
       <c r="E204" s="1" t="s">
-        <v>239</v>
+        <v>230</v>
       </c>
       <c r="F204" s="1" t="s">
         <v>55</v>
@@ -5621,19 +5621,19 @@
     </row>
     <row r="205" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A205" s="12" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="B205" s="12">
         <v>6</v>
       </c>
       <c r="C205" s="12" t="s">
-        <v>256</v>
+        <v>247</v>
       </c>
       <c r="D205" s="9" t="s">
         <v>12</v>
       </c>
       <c r="E205" s="1" t="s">
-        <v>260</v>
+        <v>251</v>
       </c>
       <c r="F205" s="1" t="s">
         <v>55</v>
@@ -5641,19 +5641,19 @@
     </row>
     <row r="206" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A206" s="12" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="B206" s="12">
         <v>6</v>
       </c>
       <c r="C206" s="12" t="s">
-        <v>151</v>
+        <v>142</v>
       </c>
       <c r="D206" s="9" t="s">
         <v>33</v>
       </c>
       <c r="E206" s="1" t="s">
-        <v>156</v>
+        <v>147</v>
       </c>
       <c r="F206" s="1" t="s">
         <v>55</v>
@@ -5661,19 +5661,19 @@
     </row>
     <row r="207" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A207" s="12" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="B207" s="12">
         <v>6</v>
       </c>
       <c r="C207" s="12" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
       <c r="D207" s="9" t="s">
         <v>33</v>
       </c>
       <c r="E207" s="1" t="s">
-        <v>177</v>
+        <v>168</v>
       </c>
       <c r="F207" s="1" t="s">
         <v>55</v>
@@ -5681,19 +5681,19 @@
     </row>
     <row r="208" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A208" s="12" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="B208" s="12">
         <v>6</v>
       </c>
       <c r="C208" s="12" t="s">
-        <v>193</v>
+        <v>184</v>
       </c>
       <c r="D208" s="9" t="s">
         <v>33</v>
       </c>
       <c r="E208" s="1" t="s">
-        <v>198</v>
+        <v>189</v>
       </c>
       <c r="F208" s="1" t="s">
         <v>55</v>
@@ -5701,19 +5701,19 @@
     </row>
     <row r="209" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A209" s="12" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="B209" s="12">
         <v>6</v>
       </c>
       <c r="C209" s="12" t="s">
-        <v>214</v>
+        <v>205</v>
       </c>
       <c r="D209" s="9" t="s">
         <v>33</v>
       </c>
       <c r="E209" s="1" t="s">
-        <v>219</v>
+        <v>210</v>
       </c>
       <c r="F209" s="1" t="s">
         <v>55</v>
@@ -5721,19 +5721,19 @@
     </row>
     <row r="210" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A210" s="12" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="B210" s="12">
         <v>6</v>
       </c>
       <c r="C210" s="12" t="s">
-        <v>235</v>
+        <v>226</v>
       </c>
       <c r="D210" s="9" t="s">
         <v>33</v>
       </c>
       <c r="E210" s="1" t="s">
-        <v>240</v>
+        <v>231</v>
       </c>
       <c r="F210" s="1" t="s">
         <v>55</v>
@@ -5741,19 +5741,19 @@
     </row>
     <row r="211" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A211" s="12" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="B211" s="12">
         <v>6</v>
       </c>
       <c r="C211" s="12" t="s">
-        <v>256</v>
+        <v>247</v>
       </c>
       <c r="D211" s="9" t="s">
         <v>33</v>
       </c>
       <c r="E211" s="1" t="s">
-        <v>261</v>
+        <v>252</v>
       </c>
       <c r="F211" s="1" t="s">
         <v>55</v>
@@ -5761,19 +5761,19 @@
     </row>
     <row r="212" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A212" s="12" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="B212" s="12">
         <v>6</v>
       </c>
       <c r="C212" s="12" t="s">
-        <v>151</v>
+        <v>142</v>
       </c>
       <c r="D212" s="9" t="s">
         <v>25</v>
       </c>
       <c r="E212" s="1" t="s">
-        <v>157</v>
+        <v>148</v>
       </c>
       <c r="F212" s="1" t="s">
         <v>55</v>
@@ -5781,19 +5781,19 @@
     </row>
     <row r="213" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A213" s="12" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="B213" s="12">
         <v>6</v>
       </c>
       <c r="C213" s="12" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
       <c r="D213" s="9" t="s">
         <v>25</v>
       </c>
       <c r="E213" s="1" t="s">
-        <v>178</v>
+        <v>169</v>
       </c>
       <c r="F213" s="1" t="s">
         <v>55</v>
@@ -5801,19 +5801,19 @@
     </row>
     <row r="214" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A214" s="12" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="B214" s="12">
         <v>6</v>
       </c>
       <c r="C214" s="12" t="s">
-        <v>193</v>
+        <v>184</v>
       </c>
       <c r="D214" s="9" t="s">
         <v>25</v>
       </c>
       <c r="E214" s="1" t="s">
-        <v>199</v>
+        <v>190</v>
       </c>
       <c r="F214" s="1" t="s">
         <v>55</v>
@@ -5821,19 +5821,19 @@
     </row>
     <row r="215" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A215" s="12" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="B215" s="12">
         <v>6</v>
       </c>
       <c r="C215" s="12" t="s">
-        <v>214</v>
+        <v>205</v>
       </c>
       <c r="D215" s="9" t="s">
         <v>25</v>
       </c>
       <c r="E215" s="1" t="s">
-        <v>220</v>
+        <v>211</v>
       </c>
       <c r="F215" s="1" t="s">
         <v>55</v>
@@ -5841,19 +5841,19 @@
     </row>
     <row r="216" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A216" s="12" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="B216" s="12">
         <v>6</v>
       </c>
       <c r="C216" s="12" t="s">
-        <v>235</v>
+        <v>226</v>
       </c>
       <c r="D216" s="9" t="s">
         <v>25</v>
       </c>
       <c r="E216" s="1" t="s">
-        <v>241</v>
+        <v>232</v>
       </c>
       <c r="F216" s="1" t="s">
         <v>55</v>
@@ -5861,19 +5861,19 @@
     </row>
     <row r="217" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A217" s="12" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="B217" s="12">
         <v>6</v>
       </c>
       <c r="C217" s="12" t="s">
-        <v>256</v>
+        <v>247</v>
       </c>
       <c r="D217" s="9" t="s">
         <v>25</v>
       </c>
       <c r="E217" s="1" t="s">
-        <v>262</v>
+        <v>253</v>
       </c>
       <c r="F217" s="1" t="s">
         <v>55</v>
@@ -5881,19 +5881,19 @@
     </row>
     <row r="218" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A218" s="12" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="B218" s="12">
         <v>6</v>
       </c>
       <c r="C218" s="12" t="s">
-        <v>151</v>
+        <v>142</v>
       </c>
       <c r="D218" s="9" t="s">
         <v>28</v>
       </c>
       <c r="E218" s="1" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="F218" s="1" t="s">
         <v>55</v>
@@ -5901,19 +5901,19 @@
     </row>
     <row r="219" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A219" s="12" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="B219" s="12">
         <v>6</v>
       </c>
       <c r="C219" s="12" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
       <c r="D219" s="9" t="s">
         <v>28</v>
       </c>
       <c r="E219" s="1" t="s">
-        <v>179</v>
+        <v>170</v>
       </c>
       <c r="F219" s="1" t="s">
         <v>55</v>
@@ -5921,19 +5921,19 @@
     </row>
     <row r="220" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A220" s="12" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="B220" s="12">
         <v>6</v>
       </c>
       <c r="C220" s="12" t="s">
-        <v>193</v>
+        <v>184</v>
       </c>
       <c r="D220" s="9" t="s">
         <v>28</v>
       </c>
       <c r="E220" s="1" t="s">
-        <v>200</v>
+        <v>191</v>
       </c>
       <c r="F220" s="1" t="s">
         <v>55</v>
@@ -5941,19 +5941,19 @@
     </row>
     <row r="221" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A221" s="12" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="B221" s="12">
         <v>6</v>
       </c>
       <c r="C221" s="12" t="s">
-        <v>214</v>
+        <v>205</v>
       </c>
       <c r="D221" s="9" t="s">
         <v>28</v>
       </c>
       <c r="E221" s="1" t="s">
-        <v>221</v>
+        <v>212</v>
       </c>
       <c r="F221" s="1" t="s">
         <v>55</v>
@@ -5961,19 +5961,19 @@
     </row>
     <row r="222" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A222" s="12" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="B222" s="12">
         <v>6</v>
       </c>
       <c r="C222" s="12" t="s">
-        <v>235</v>
+        <v>226</v>
       </c>
       <c r="D222" s="9" t="s">
         <v>28</v>
       </c>
       <c r="E222" s="1" t="s">
-        <v>242</v>
+        <v>233</v>
       </c>
       <c r="F222" s="1" t="s">
         <v>55</v>
@@ -5981,19 +5981,19 @@
     </row>
     <row r="223" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A223" s="12" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="B223" s="12">
         <v>6</v>
       </c>
       <c r="C223" s="12" t="s">
-        <v>256</v>
+        <v>247</v>
       </c>
       <c r="D223" s="9" t="s">
         <v>28</v>
       </c>
       <c r="E223" s="1" t="s">
-        <v>263</v>
+        <v>254</v>
       </c>
       <c r="F223" s="1" t="s">
         <v>55</v>
@@ -6001,19 +6001,19 @@
     </row>
     <row r="224" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A224" s="12" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="B224" s="12">
         <v>6</v>
       </c>
       <c r="C224" s="12" t="s">
-        <v>151</v>
+        <v>142</v>
       </c>
       <c r="D224" s="9" t="s">
         <v>13</v>
       </c>
       <c r="E224" s="1" t="s">
-        <v>159</v>
+        <v>150</v>
       </c>
       <c r="F224" s="1" t="s">
         <v>55</v>
@@ -6021,19 +6021,19 @@
     </row>
     <row r="225" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A225" s="12" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="B225" s="12">
         <v>6</v>
       </c>
       <c r="C225" s="12" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
       <c r="D225" s="9" t="s">
         <v>13</v>
       </c>
       <c r="E225" s="1" t="s">
-        <v>180</v>
+        <v>171</v>
       </c>
       <c r="F225" s="1" t="s">
         <v>55</v>
@@ -6041,19 +6041,19 @@
     </row>
     <row r="226" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A226" s="12" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="B226" s="12">
         <v>6</v>
       </c>
       <c r="C226" s="12" t="s">
-        <v>193</v>
+        <v>184</v>
       </c>
       <c r="D226" s="9" t="s">
         <v>13</v>
       </c>
       <c r="E226" s="1" t="s">
-        <v>201</v>
+        <v>192</v>
       </c>
       <c r="F226" s="1" t="s">
         <v>55</v>
@@ -6061,19 +6061,19 @@
     </row>
     <row r="227" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A227" s="12" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="B227" s="12">
         <v>6</v>
       </c>
       <c r="C227" s="12" t="s">
-        <v>214</v>
+        <v>205</v>
       </c>
       <c r="D227" s="9" t="s">
         <v>13</v>
       </c>
       <c r="E227" s="1" t="s">
-        <v>222</v>
+        <v>213</v>
       </c>
       <c r="F227" s="1" t="s">
         <v>55</v>
@@ -6081,19 +6081,19 @@
     </row>
     <row r="228" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A228" s="12" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="B228" s="12">
         <v>6</v>
       </c>
       <c r="C228" s="12" t="s">
-        <v>235</v>
+        <v>226</v>
       </c>
       <c r="D228" s="9" t="s">
         <v>13</v>
       </c>
       <c r="E228" s="1" t="s">
-        <v>243</v>
+        <v>234</v>
       </c>
       <c r="F228" s="1" t="s">
         <v>55</v>
@@ -6101,19 +6101,19 @@
     </row>
     <row r="229" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A229" s="12" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="B229" s="12">
         <v>6</v>
       </c>
       <c r="C229" s="12" t="s">
-        <v>256</v>
+        <v>247</v>
       </c>
       <c r="D229" s="9" t="s">
         <v>13</v>
       </c>
       <c r="E229" s="1" t="s">
-        <v>264</v>
+        <v>255</v>
       </c>
       <c r="F229" s="1" t="s">
         <v>55</v>
@@ -6121,19 +6121,19 @@
     </row>
     <row r="230" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A230" s="12" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="B230" s="12">
         <v>6</v>
       </c>
       <c r="C230" s="12" t="s">
-        <v>151</v>
+        <v>142</v>
       </c>
       <c r="D230" s="9" t="s">
         <v>26</v>
       </c>
       <c r="E230" s="1" t="s">
-        <v>160</v>
+        <v>151</v>
       </c>
       <c r="F230" s="1" t="s">
         <v>55</v>
@@ -6141,19 +6141,19 @@
     </row>
     <row r="231" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A231" s="12" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="B231" s="12">
         <v>6</v>
       </c>
       <c r="C231" s="12" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
       <c r="D231" s="9" t="s">
         <v>26</v>
       </c>
       <c r="E231" s="1" t="s">
-        <v>181</v>
+        <v>172</v>
       </c>
       <c r="F231" s="1" t="s">
         <v>55</v>
@@ -6161,19 +6161,19 @@
     </row>
     <row r="232" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A232" s="12" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="B232" s="12">
         <v>6</v>
       </c>
       <c r="C232" s="12" t="s">
-        <v>193</v>
+        <v>184</v>
       </c>
       <c r="D232" s="9" t="s">
         <v>26</v>
       </c>
       <c r="E232" s="1" t="s">
-        <v>202</v>
+        <v>193</v>
       </c>
       <c r="F232" s="1" t="s">
         <v>55</v>
@@ -6181,19 +6181,19 @@
     </row>
     <row r="233" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A233" s="12" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="B233" s="12">
         <v>6</v>
       </c>
       <c r="C233" s="12" t="s">
-        <v>214</v>
+        <v>205</v>
       </c>
       <c r="D233" s="9" t="s">
         <v>26</v>
       </c>
       <c r="E233" s="1" t="s">
-        <v>223</v>
+        <v>214</v>
       </c>
       <c r="F233" s="1" t="s">
         <v>55</v>
@@ -6201,19 +6201,19 @@
     </row>
     <row r="234" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A234" s="12" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="B234" s="12">
         <v>6</v>
       </c>
       <c r="C234" s="12" t="s">
-        <v>235</v>
+        <v>226</v>
       </c>
       <c r="D234" s="9" t="s">
         <v>26</v>
       </c>
       <c r="E234" s="1" t="s">
-        <v>244</v>
+        <v>235</v>
       </c>
       <c r="F234" s="1" t="s">
         <v>55</v>
@@ -6221,19 +6221,19 @@
     </row>
     <row r="235" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A235" s="12" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="B235" s="12">
         <v>6</v>
       </c>
       <c r="C235" s="12" t="s">
-        <v>256</v>
+        <v>247</v>
       </c>
       <c r="D235" s="9" t="s">
         <v>26</v>
       </c>
       <c r="E235" s="1" t="s">
-        <v>265</v>
+        <v>256</v>
       </c>
       <c r="F235" s="1" t="s">
         <v>55</v>
@@ -6241,19 +6241,19 @@
     </row>
     <row r="236" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A236" s="12" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="B236" s="12">
         <v>6</v>
       </c>
       <c r="C236" s="12" t="s">
-        <v>151</v>
+        <v>142</v>
       </c>
       <c r="D236" s="9" t="s">
         <v>14</v>
       </c>
       <c r="E236" s="1" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="F236" s="1" t="s">
         <v>55</v>
@@ -6261,19 +6261,19 @@
     </row>
     <row r="237" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A237" s="12" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="B237" s="12">
         <v>6</v>
       </c>
       <c r="C237" s="12" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
       <c r="D237" s="9" t="s">
         <v>14</v>
       </c>
       <c r="E237" s="1" t="s">
-        <v>182</v>
+        <v>173</v>
       </c>
       <c r="F237" s="1" t="s">
         <v>55</v>
@@ -6281,19 +6281,19 @@
     </row>
     <row r="238" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A238" s="12" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="B238" s="12">
         <v>6</v>
       </c>
       <c r="C238" s="12" t="s">
-        <v>193</v>
+        <v>184</v>
       </c>
       <c r="D238" s="9" t="s">
         <v>14</v>
       </c>
       <c r="E238" s="1" t="s">
-        <v>203</v>
+        <v>194</v>
       </c>
       <c r="F238" s="1" t="s">
         <v>55</v>
@@ -6301,19 +6301,19 @@
     </row>
     <row r="239" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A239" s="12" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="B239" s="12">
         <v>6</v>
       </c>
       <c r="C239" s="12" t="s">
-        <v>214</v>
+        <v>205</v>
       </c>
       <c r="D239" s="9" t="s">
         <v>14</v>
       </c>
       <c r="E239" s="1" t="s">
-        <v>224</v>
+        <v>215</v>
       </c>
       <c r="F239" s="1" t="s">
         <v>55</v>
@@ -6321,19 +6321,19 @@
     </row>
     <row r="240" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A240" s="12" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="B240" s="12">
         <v>6</v>
       </c>
       <c r="C240" s="12" t="s">
-        <v>235</v>
+        <v>226</v>
       </c>
       <c r="D240" s="9" t="s">
         <v>14</v>
       </c>
       <c r="E240" s="1" t="s">
-        <v>245</v>
+        <v>236</v>
       </c>
       <c r="F240" s="1" t="s">
         <v>55</v>
@@ -6341,19 +6341,19 @@
     </row>
     <row r="241" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A241" s="12" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="B241" s="12">
         <v>6</v>
       </c>
       <c r="C241" s="12" t="s">
-        <v>256</v>
+        <v>247</v>
       </c>
       <c r="D241" s="9" t="s">
         <v>14</v>
       </c>
       <c r="E241" s="1" t="s">
-        <v>266</v>
+        <v>257</v>
       </c>
       <c r="F241" s="1" t="s">
         <v>55</v>
@@ -6361,19 +6361,19 @@
     </row>
     <row r="242" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A242" s="12" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="B242" s="12">
         <v>6</v>
       </c>
       <c r="C242" s="12" t="s">
-        <v>151</v>
+        <v>142</v>
       </c>
       <c r="D242" s="9" t="s">
         <v>30</v>
       </c>
       <c r="E242" s="1" t="s">
-        <v>162</v>
+        <v>153</v>
       </c>
       <c r="F242" s="1" t="s">
         <v>55</v>
@@ -6381,19 +6381,19 @@
     </row>
     <row r="243" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A243" s="12" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="B243" s="12">
         <v>6</v>
       </c>
       <c r="C243" s="12" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
       <c r="D243" s="9" t="s">
         <v>30</v>
       </c>
       <c r="E243" s="1" t="s">
-        <v>183</v>
+        <v>174</v>
       </c>
       <c r="F243" s="1" t="s">
         <v>55</v>
@@ -6401,19 +6401,19 @@
     </row>
     <row r="244" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A244" s="12" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="B244" s="12">
         <v>6</v>
       </c>
       <c r="C244" s="12" t="s">
-        <v>193</v>
+        <v>184</v>
       </c>
       <c r="D244" s="9" t="s">
         <v>30</v>
       </c>
       <c r="E244" s="1" t="s">
-        <v>204</v>
+        <v>195</v>
       </c>
       <c r="F244" s="1" t="s">
         <v>55</v>
@@ -6421,19 +6421,19 @@
     </row>
     <row r="245" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A245" s="12" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="B245" s="12">
         <v>6</v>
       </c>
       <c r="C245" s="12" t="s">
-        <v>214</v>
+        <v>205</v>
       </c>
       <c r="D245" s="9" t="s">
         <v>30</v>
       </c>
       <c r="E245" s="1" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="F245" s="1" t="s">
         <v>55</v>
@@ -6441,19 +6441,19 @@
     </row>
     <row r="246" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A246" s="12" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="B246" s="12">
         <v>6</v>
       </c>
       <c r="C246" s="12" t="s">
-        <v>235</v>
+        <v>226</v>
       </c>
       <c r="D246" s="9" t="s">
         <v>30</v>
       </c>
       <c r="E246" s="1" t="s">
-        <v>246</v>
+        <v>237</v>
       </c>
       <c r="F246" s="1" t="s">
         <v>55</v>
@@ -6461,19 +6461,19 @@
     </row>
     <row r="247" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A247" s="12" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="B247" s="12">
         <v>6</v>
       </c>
       <c r="C247" s="12" t="s">
-        <v>256</v>
+        <v>247</v>
       </c>
       <c r="D247" s="9" t="s">
         <v>30</v>
       </c>
       <c r="E247" s="1" t="s">
-        <v>267</v>
+        <v>258</v>
       </c>
       <c r="F247" s="1" t="s">
         <v>55</v>
@@ -6481,19 +6481,19 @@
     </row>
     <row r="248" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A248" s="12" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="B248" s="12">
         <v>6</v>
       </c>
       <c r="C248" s="12" t="s">
-        <v>151</v>
+        <v>142</v>
       </c>
       <c r="D248" s="9" t="s">
         <v>15</v>
       </c>
       <c r="E248" s="1" t="s">
-        <v>163</v>
+        <v>154</v>
       </c>
       <c r="F248" s="1" t="s">
         <v>55</v>
@@ -6501,19 +6501,19 @@
     </row>
     <row r="249" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A249" s="12" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="B249" s="12">
         <v>6</v>
       </c>
       <c r="C249" s="12" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
       <c r="D249" s="9" t="s">
         <v>15</v>
       </c>
       <c r="E249" s="1" t="s">
-        <v>184</v>
+        <v>175</v>
       </c>
       <c r="F249" s="1" t="s">
         <v>55</v>
@@ -6521,19 +6521,19 @@
     </row>
     <row r="250" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A250" s="12" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="B250" s="12">
         <v>6</v>
       </c>
       <c r="C250" s="12" t="s">
-        <v>193</v>
+        <v>184</v>
       </c>
       <c r="D250" s="9" t="s">
         <v>15</v>
       </c>
       <c r="E250" s="1" t="s">
-        <v>205</v>
+        <v>196</v>
       </c>
       <c r="F250" s="1" t="s">
         <v>55</v>
@@ -6541,19 +6541,19 @@
     </row>
     <row r="251" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A251" s="12" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="B251" s="12">
         <v>6</v>
       </c>
       <c r="C251" s="12" t="s">
-        <v>214</v>
+        <v>205</v>
       </c>
       <c r="D251" s="9" t="s">
         <v>15</v>
       </c>
       <c r="E251" s="1" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
       <c r="F251" s="1" t="s">
         <v>55</v>
@@ -6561,19 +6561,19 @@
     </row>
     <row r="252" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A252" s="12" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="B252" s="12">
         <v>6</v>
       </c>
       <c r="C252" s="12" t="s">
-        <v>235</v>
+        <v>226</v>
       </c>
       <c r="D252" s="9" t="s">
         <v>15</v>
       </c>
       <c r="E252" s="1" t="s">
-        <v>247</v>
+        <v>238</v>
       </c>
       <c r="F252" s="1" t="s">
         <v>55</v>
@@ -6581,19 +6581,19 @@
     </row>
     <row r="253" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A253" s="12" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="B253" s="12">
         <v>6</v>
       </c>
       <c r="C253" s="12" t="s">
-        <v>256</v>
+        <v>247</v>
       </c>
       <c r="D253" s="9" t="s">
         <v>15</v>
       </c>
       <c r="E253" s="1" t="s">
-        <v>268</v>
+        <v>259</v>
       </c>
       <c r="F253" s="1" t="s">
         <v>55</v>
@@ -6601,19 +6601,19 @@
     </row>
     <row r="254" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A254" s="12" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="B254" s="12">
         <v>6</v>
       </c>
       <c r="C254" s="12" t="s">
-        <v>151</v>
+        <v>142</v>
       </c>
       <c r="D254" s="9" t="s">
         <v>16</v>
       </c>
       <c r="E254" s="1" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="F254" s="1" t="s">
         <v>55</v>
@@ -6621,19 +6621,19 @@
     </row>
     <row r="255" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A255" s="12" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="B255" s="12">
         <v>6</v>
       </c>
       <c r="C255" s="12" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
       <c r="D255" s="9" t="s">
         <v>16</v>
       </c>
       <c r="E255" s="1" t="s">
-        <v>185</v>
+        <v>176</v>
       </c>
       <c r="F255" s="1" t="s">
         <v>55</v>
@@ -6641,19 +6641,19 @@
     </row>
     <row r="256" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A256" s="12" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="B256" s="12">
         <v>6</v>
       </c>
       <c r="C256" s="12" t="s">
-        <v>193</v>
+        <v>184</v>
       </c>
       <c r="D256" s="9" t="s">
         <v>16</v>
       </c>
       <c r="E256" s="1" t="s">
-        <v>206</v>
+        <v>197</v>
       </c>
       <c r="F256" s="1" t="s">
         <v>55</v>
@@ -6661,19 +6661,19 @@
     </row>
     <row r="257" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A257" s="12" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="B257" s="12">
         <v>6</v>
       </c>
       <c r="C257" s="12" t="s">
-        <v>214</v>
+        <v>205</v>
       </c>
       <c r="D257" s="9" t="s">
         <v>16</v>
       </c>
       <c r="E257" s="1" t="s">
-        <v>227</v>
+        <v>218</v>
       </c>
       <c r="F257" s="1" t="s">
         <v>55</v>
@@ -6681,19 +6681,19 @@
     </row>
     <row r="258" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A258" s="12" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="B258" s="12">
         <v>6</v>
       </c>
       <c r="C258" s="12" t="s">
-        <v>235</v>
+        <v>226</v>
       </c>
       <c r="D258" s="9" t="s">
         <v>16</v>
       </c>
       <c r="E258" s="1" t="s">
-        <v>248</v>
+        <v>239</v>
       </c>
       <c r="F258" s="1" t="s">
         <v>55</v>
@@ -6701,19 +6701,19 @@
     </row>
     <row r="259" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A259" s="12" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="B259" s="12">
         <v>6</v>
       </c>
       <c r="C259" s="12" t="s">
-        <v>256</v>
+        <v>247</v>
       </c>
       <c r="D259" s="9" t="s">
         <v>16</v>
       </c>
       <c r="E259" s="1" t="s">
-        <v>269</v>
+        <v>260</v>
       </c>
       <c r="F259" s="1" t="s">
         <v>55</v>
@@ -6721,19 +6721,19 @@
     </row>
     <row r="260" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A260" s="12" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="B260" s="12">
         <v>6</v>
       </c>
       <c r="C260" s="12" t="s">
-        <v>151</v>
+        <v>142</v>
       </c>
       <c r="D260" s="9" t="s">
         <v>17</v>
       </c>
       <c r="E260" s="1" t="s">
-        <v>165</v>
+        <v>156</v>
       </c>
       <c r="F260" s="1" t="s">
         <v>55</v>
@@ -6741,19 +6741,19 @@
     </row>
     <row r="261" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A261" s="12" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="B261" s="12">
         <v>6</v>
       </c>
       <c r="C261" s="12" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
       <c r="D261" s="9" t="s">
         <v>17</v>
       </c>
       <c r="E261" s="1" t="s">
-        <v>186</v>
+        <v>177</v>
       </c>
       <c r="F261" s="1" t="s">
         <v>55</v>
@@ -6761,19 +6761,19 @@
     </row>
     <row r="262" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A262" s="12" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="B262" s="12">
         <v>6</v>
       </c>
       <c r="C262" s="12" t="s">
-        <v>193</v>
+        <v>184</v>
       </c>
       <c r="D262" s="9" t="s">
         <v>17</v>
       </c>
       <c r="E262" s="1" t="s">
-        <v>207</v>
+        <v>198</v>
       </c>
       <c r="F262" s="1" t="s">
         <v>55</v>
@@ -6781,19 +6781,19 @@
     </row>
     <row r="263" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A263" s="12" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="B263" s="12">
         <v>6</v>
       </c>
       <c r="C263" s="12" t="s">
-        <v>214</v>
+        <v>205</v>
       </c>
       <c r="D263" s="9" t="s">
         <v>17</v>
       </c>
       <c r="E263" s="1" t="s">
-        <v>228</v>
+        <v>219</v>
       </c>
       <c r="F263" s="1" t="s">
         <v>55</v>
@@ -6801,19 +6801,19 @@
     </row>
     <row r="264" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A264" s="12" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="B264" s="12">
         <v>6</v>
       </c>
       <c r="C264" s="12" t="s">
-        <v>235</v>
+        <v>226</v>
       </c>
       <c r="D264" s="9" t="s">
         <v>17</v>
       </c>
       <c r="E264" s="1" t="s">
-        <v>249</v>
+        <v>240</v>
       </c>
       <c r="F264" s="1" t="s">
         <v>55</v>
@@ -6821,19 +6821,19 @@
     </row>
     <row r="265" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A265" s="12" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="B265" s="12">
         <v>6</v>
       </c>
       <c r="C265" s="12" t="s">
-        <v>256</v>
+        <v>247</v>
       </c>
       <c r="D265" s="9" t="s">
         <v>17</v>
       </c>
       <c r="E265" s="1" t="s">
-        <v>270</v>
+        <v>261</v>
       </c>
       <c r="F265" s="1" t="s">
         <v>55</v>
@@ -6841,19 +6841,19 @@
     </row>
     <row r="266" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A266" s="12" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="B266" s="12">
         <v>6</v>
       </c>
       <c r="C266" s="12" t="s">
-        <v>151</v>
+        <v>142</v>
       </c>
       <c r="D266" s="9" t="s">
         <v>29</v>
       </c>
       <c r="E266" s="1" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
       <c r="F266" s="1" t="s">
         <v>55</v>
@@ -6861,19 +6861,19 @@
     </row>
     <row r="267" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A267" s="12" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="B267" s="12">
         <v>6</v>
       </c>
       <c r="C267" s="12" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
       <c r="D267" s="9" t="s">
         <v>29</v>
       </c>
       <c r="E267" s="1" t="s">
-        <v>187</v>
+        <v>178</v>
       </c>
       <c r="F267" s="1" t="s">
         <v>55</v>
@@ -6881,19 +6881,19 @@
     </row>
     <row r="268" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A268" s="12" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="B268" s="12">
         <v>6</v>
       </c>
       <c r="C268" s="12" t="s">
-        <v>193</v>
+        <v>184</v>
       </c>
       <c r="D268" s="9" t="s">
         <v>29</v>
       </c>
       <c r="E268" s="1" t="s">
-        <v>208</v>
+        <v>199</v>
       </c>
       <c r="F268" s="1" t="s">
         <v>55</v>
@@ -6901,19 +6901,19 @@
     </row>
     <row r="269" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A269" s="12" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="B269" s="12">
         <v>6</v>
       </c>
       <c r="C269" s="12" t="s">
-        <v>214</v>
+        <v>205</v>
       </c>
       <c r="D269" s="9" t="s">
         <v>29</v>
       </c>
       <c r="E269" s="1" t="s">
-        <v>229</v>
+        <v>220</v>
       </c>
       <c r="F269" s="1" t="s">
         <v>55</v>
@@ -6921,19 +6921,19 @@
     </row>
     <row r="270" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A270" s="12" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="B270" s="12">
         <v>6</v>
       </c>
       <c r="C270" s="12" t="s">
-        <v>235</v>
+        <v>226</v>
       </c>
       <c r="D270" s="9" t="s">
         <v>29</v>
       </c>
       <c r="E270" s="1" t="s">
-        <v>250</v>
+        <v>241</v>
       </c>
       <c r="F270" s="1" t="s">
         <v>55</v>
@@ -6941,19 +6941,19 @@
     </row>
     <row r="271" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A271" s="12" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="B271" s="12">
         <v>6</v>
       </c>
       <c r="C271" s="12" t="s">
-        <v>256</v>
+        <v>247</v>
       </c>
       <c r="D271" s="9" t="s">
         <v>29</v>
       </c>
       <c r="E271" s="1" t="s">
-        <v>271</v>
+        <v>262</v>
       </c>
       <c r="F271" s="1" t="s">
         <v>55</v>
@@ -6961,19 +6961,19 @@
     </row>
     <row r="272" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A272" s="12" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="B272" s="12">
         <v>6</v>
       </c>
       <c r="C272" s="12" t="s">
-        <v>151</v>
+        <v>142</v>
       </c>
       <c r="D272" s="9" t="s">
         <v>18</v>
       </c>
       <c r="E272" s="1" t="s">
-        <v>167</v>
+        <v>158</v>
       </c>
       <c r="F272" s="1" t="s">
         <v>55</v>
@@ -6981,19 +6981,19 @@
     </row>
     <row r="273" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A273" s="12" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="B273" s="12">
         <v>6</v>
       </c>
       <c r="C273" s="12" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
       <c r="D273" s="9" t="s">
         <v>18</v>
       </c>
       <c r="E273" s="1" t="s">
-        <v>188</v>
+        <v>179</v>
       </c>
       <c r="F273" s="1" t="s">
         <v>55</v>
@@ -7001,19 +7001,19 @@
     </row>
     <row r="274" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A274" s="12" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="B274" s="12">
         <v>6</v>
       </c>
       <c r="C274" s="12" t="s">
-        <v>193</v>
+        <v>184</v>
       </c>
       <c r="D274" s="9" t="s">
         <v>18</v>
       </c>
       <c r="E274" s="1" t="s">
-        <v>209</v>
+        <v>200</v>
       </c>
       <c r="F274" s="1" t="s">
         <v>55</v>
@@ -7021,19 +7021,19 @@
     </row>
     <row r="275" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A275" s="12" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="B275" s="12">
         <v>6</v>
       </c>
       <c r="C275" s="12" t="s">
-        <v>214</v>
+        <v>205</v>
       </c>
       <c r="D275" s="9" t="s">
         <v>18</v>
       </c>
       <c r="E275" s="1" t="s">
-        <v>230</v>
+        <v>221</v>
       </c>
       <c r="F275" s="1" t="s">
         <v>55</v>
@@ -7041,19 +7041,19 @@
     </row>
     <row r="276" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A276" s="12" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="B276" s="12">
         <v>6</v>
       </c>
       <c r="C276" s="12" t="s">
-        <v>235</v>
+        <v>226</v>
       </c>
       <c r="D276" s="9" t="s">
         <v>18</v>
       </c>
       <c r="E276" s="1" t="s">
-        <v>251</v>
+        <v>242</v>
       </c>
       <c r="F276" s="1" t="s">
         <v>55</v>
@@ -7061,19 +7061,19 @@
     </row>
     <row r="277" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A277" s="12" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="B277" s="12">
         <v>6</v>
       </c>
       <c r="C277" s="12" t="s">
-        <v>256</v>
+        <v>247</v>
       </c>
       <c r="D277" s="9" t="s">
         <v>18</v>
       </c>
       <c r="E277" s="1" t="s">
-        <v>272</v>
+        <v>263</v>
       </c>
       <c r="F277" s="1" t="s">
         <v>55</v>
@@ -7081,19 +7081,19 @@
     </row>
     <row r="278" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A278" s="12" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="B278" s="12">
         <v>6</v>
       </c>
       <c r="C278" s="12" t="s">
-        <v>151</v>
+        <v>142</v>
       </c>
       <c r="D278" s="9" t="s">
         <v>20</v>
       </c>
       <c r="E278" s="1" t="s">
-        <v>168</v>
+        <v>159</v>
       </c>
       <c r="F278" s="1" t="s">
         <v>55</v>
@@ -7101,19 +7101,19 @@
     </row>
     <row r="279" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A279" s="12" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="B279" s="12">
         <v>6</v>
       </c>
       <c r="C279" s="12" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
       <c r="D279" s="9" t="s">
         <v>20</v>
       </c>
       <c r="E279" s="1" t="s">
-        <v>189</v>
+        <v>180</v>
       </c>
       <c r="F279" s="1" t="s">
         <v>55</v>
@@ -7121,19 +7121,19 @@
     </row>
     <row r="280" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A280" s="12" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="B280" s="12">
         <v>6</v>
       </c>
       <c r="C280" s="12" t="s">
-        <v>193</v>
+        <v>184</v>
       </c>
       <c r="D280" s="9" t="s">
         <v>20</v>
       </c>
       <c r="E280" s="1" t="s">
-        <v>210</v>
+        <v>201</v>
       </c>
       <c r="F280" s="1" t="s">
         <v>55</v>
@@ -7141,19 +7141,19 @@
     </row>
     <row r="281" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A281" s="12" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="B281" s="12">
         <v>6</v>
       </c>
       <c r="C281" s="12" t="s">
-        <v>214</v>
+        <v>205</v>
       </c>
       <c r="D281" s="9" t="s">
         <v>20</v>
       </c>
       <c r="E281" s="1" t="s">
-        <v>231</v>
+        <v>222</v>
       </c>
       <c r="F281" s="1" t="s">
         <v>55</v>
@@ -7161,19 +7161,19 @@
     </row>
     <row r="282" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A282" s="12" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="B282" s="12">
         <v>6</v>
       </c>
       <c r="C282" s="12" t="s">
-        <v>235</v>
+        <v>226</v>
       </c>
       <c r="D282" s="9" t="s">
         <v>20</v>
       </c>
       <c r="E282" s="1" t="s">
-        <v>252</v>
+        <v>243</v>
       </c>
       <c r="F282" s="1" t="s">
         <v>55</v>
@@ -7181,19 +7181,19 @@
     </row>
     <row r="283" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A283" s="12" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="B283" s="12">
         <v>6</v>
       </c>
       <c r="C283" s="12" t="s">
-        <v>256</v>
+        <v>247</v>
       </c>
       <c r="D283" s="9" t="s">
         <v>20</v>
       </c>
       <c r="E283" s="1" t="s">
-        <v>273</v>
+        <v>264</v>
       </c>
       <c r="F283" s="1" t="s">
         <v>55</v>
@@ -7201,19 +7201,19 @@
     </row>
     <row r="284" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A284" s="12" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="B284" s="12">
         <v>6</v>
       </c>
       <c r="C284" s="12" t="s">
-        <v>151</v>
+        <v>142</v>
       </c>
       <c r="D284" s="9" t="s">
         <v>24</v>
       </c>
       <c r="E284" s="1" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
       <c r="F284" s="1" t="s">
         <v>55</v>
@@ -7221,19 +7221,19 @@
     </row>
     <row r="285" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A285" s="12" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="B285" s="12">
         <v>6</v>
       </c>
       <c r="C285" s="12" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
       <c r="D285" s="9" t="s">
         <v>24</v>
       </c>
       <c r="E285" s="1" t="s">
-        <v>190</v>
+        <v>181</v>
       </c>
       <c r="F285" s="1" t="s">
         <v>55</v>
@@ -7241,19 +7241,19 @@
     </row>
     <row r="286" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A286" s="12" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="B286" s="12">
         <v>6</v>
       </c>
       <c r="C286" s="12" t="s">
-        <v>193</v>
+        <v>184</v>
       </c>
       <c r="D286" s="9" t="s">
         <v>24</v>
       </c>
       <c r="E286" s="1" t="s">
-        <v>211</v>
+        <v>202</v>
       </c>
       <c r="F286" s="1" t="s">
         <v>55</v>
@@ -7261,19 +7261,19 @@
     </row>
     <row r="287" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A287" s="12" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="B287" s="12">
         <v>6</v>
       </c>
       <c r="C287" s="12" t="s">
-        <v>214</v>
+        <v>205</v>
       </c>
       <c r="D287" s="9" t="s">
         <v>24</v>
       </c>
       <c r="E287" s="1" t="s">
-        <v>232</v>
+        <v>223</v>
       </c>
       <c r="F287" s="1" t="s">
         <v>55</v>
@@ -7281,19 +7281,19 @@
     </row>
     <row r="288" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A288" s="12" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="B288" s="12">
         <v>6</v>
       </c>
       <c r="C288" s="12" t="s">
-        <v>235</v>
+        <v>226</v>
       </c>
       <c r="D288" s="9" t="s">
         <v>24</v>
       </c>
       <c r="E288" s="1" t="s">
-        <v>253</v>
+        <v>244</v>
       </c>
       <c r="F288" s="1" t="s">
         <v>55</v>
@@ -7301,19 +7301,19 @@
     </row>
     <row r="289" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A289" s="12" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="B289" s="12">
         <v>6</v>
       </c>
       <c r="C289" s="12" t="s">
-        <v>256</v>
+        <v>247</v>
       </c>
       <c r="D289" s="9" t="s">
         <v>24</v>
       </c>
       <c r="E289" s="1" t="s">
-        <v>274</v>
+        <v>265</v>
       </c>
       <c r="F289" s="1" t="s">
         <v>55</v>
@@ -7321,19 +7321,19 @@
     </row>
     <row r="290" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A290" s="12" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="B290" s="12">
         <v>6</v>
       </c>
       <c r="C290" s="12" t="s">
-        <v>151</v>
+        <v>142</v>
       </c>
       <c r="D290" s="9" t="s">
         <v>7</v>
       </c>
       <c r="E290" s="1" t="s">
-        <v>170</v>
+        <v>161</v>
       </c>
       <c r="F290" s="1" t="s">
         <v>55</v>
@@ -7341,19 +7341,19 @@
     </row>
     <row r="291" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A291" s="12" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="B291" s="12">
         <v>6</v>
       </c>
       <c r="C291" s="12" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
       <c r="D291" s="9" t="s">
         <v>7</v>
       </c>
       <c r="E291" s="1" t="s">
-        <v>191</v>
+        <v>182</v>
       </c>
       <c r="F291" s="1" t="s">
         <v>55</v>
@@ -7361,19 +7361,19 @@
     </row>
     <row r="292" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A292" s="12" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="B292" s="12">
         <v>6</v>
       </c>
       <c r="C292" s="12" t="s">
-        <v>193</v>
+        <v>184</v>
       </c>
       <c r="D292" s="9" t="s">
         <v>7</v>
       </c>
       <c r="E292" s="1" t="s">
-        <v>212</v>
+        <v>203</v>
       </c>
       <c r="F292" s="1" t="s">
         <v>55</v>
@@ -7381,19 +7381,19 @@
     </row>
     <row r="293" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A293" s="12" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="B293" s="12">
         <v>6</v>
       </c>
       <c r="C293" s="12" t="s">
-        <v>214</v>
+        <v>205</v>
       </c>
       <c r="D293" s="9" t="s">
         <v>7</v>
       </c>
       <c r="E293" s="1" t="s">
-        <v>233</v>
+        <v>224</v>
       </c>
       <c r="F293" s="1" t="s">
         <v>55</v>
@@ -7401,19 +7401,19 @@
     </row>
     <row r="294" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A294" s="12" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="B294" s="12">
         <v>6</v>
       </c>
       <c r="C294" s="12" t="s">
-        <v>235</v>
+        <v>226</v>
       </c>
       <c r="D294" s="9" t="s">
         <v>7</v>
       </c>
       <c r="E294" s="1" t="s">
-        <v>254</v>
+        <v>245</v>
       </c>
       <c r="F294" s="1" t="s">
         <v>55</v>
@@ -7421,19 +7421,19 @@
     </row>
     <row r="295" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A295" s="12" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="B295" s="12">
         <v>6</v>
       </c>
       <c r="C295" s="12" t="s">
-        <v>256</v>
+        <v>247</v>
       </c>
       <c r="D295" s="9" t="s">
         <v>7</v>
       </c>
       <c r="E295" s="1" t="s">
-        <v>275</v>
+        <v>266</v>
       </c>
       <c r="F295" s="1" t="s">
         <v>55</v>
@@ -7441,19 +7441,19 @@
     </row>
     <row r="296" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A296" s="12" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="B296" s="12">
         <v>6</v>
       </c>
       <c r="C296" s="12" t="s">
-        <v>151</v>
+        <v>142</v>
       </c>
       <c r="D296" s="9" t="s">
         <v>9</v>
       </c>
       <c r="E296" s="1" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
       <c r="F296" s="1" t="s">
         <v>55</v>
@@ -7461,19 +7461,19 @@
     </row>
     <row r="297" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A297" s="12" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="B297" s="12">
         <v>6</v>
       </c>
       <c r="C297" s="12" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
       <c r="D297" s="9" t="s">
         <v>9</v>
       </c>
       <c r="E297" s="1" t="s">
-        <v>192</v>
+        <v>183</v>
       </c>
       <c r="F297" s="1" t="s">
         <v>55</v>
@@ -7481,19 +7481,19 @@
     </row>
     <row r="298" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A298" s="12" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="B298" s="12">
         <v>6</v>
       </c>
       <c r="C298" s="12" t="s">
-        <v>193</v>
+        <v>184</v>
       </c>
       <c r="D298" s="9" t="s">
         <v>9</v>
       </c>
       <c r="E298" s="1" t="s">
-        <v>213</v>
+        <v>204</v>
       </c>
       <c r="F298" s="1" t="s">
         <v>55</v>
@@ -7501,19 +7501,19 @@
     </row>
     <row r="299" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A299" s="12" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="B299" s="12">
         <v>6</v>
       </c>
       <c r="C299" s="12" t="s">
-        <v>214</v>
+        <v>205</v>
       </c>
       <c r="D299" s="9" t="s">
         <v>9</v>
       </c>
       <c r="E299" s="1" t="s">
-        <v>234</v>
+        <v>225</v>
       </c>
       <c r="F299" s="1" t="s">
         <v>55</v>
@@ -7521,19 +7521,19 @@
     </row>
     <row r="300" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A300" s="12" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="B300" s="12">
         <v>6</v>
       </c>
       <c r="C300" s="12" t="s">
-        <v>235</v>
+        <v>226</v>
       </c>
       <c r="D300" s="9" t="s">
         <v>9</v>
       </c>
       <c r="E300" s="1" t="s">
-        <v>255</v>
+        <v>246</v>
       </c>
       <c r="F300" s="1" t="s">
         <v>55</v>
@@ -7541,19 +7541,19 @@
     </row>
     <row r="301" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A301" s="12" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="B301" s="12">
         <v>6</v>
       </c>
       <c r="C301" s="12" t="s">
-        <v>256</v>
+        <v>247</v>
       </c>
       <c r="D301" s="9" t="s">
         <v>9</v>
       </c>
       <c r="E301" s="1" t="s">
-        <v>276</v>
+        <v>267</v>
       </c>
       <c r="F301" s="1" t="s">
         <v>55</v>

</xml_diff>

<commit_message>
Diversify US related to "Finance & Marketing" domain
</commit_message>
<xml_diff>
--- a/refair-server/datasets/few shot dataset/FSDataset.xlsx
+++ b/refair-server/datasets/few shot dataset/FSDataset.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\morel\Desktop\Refair\ReFair-App\refair-server\datasets\few shot dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97058292-C55F-48FC-8EB5-79540C9FA813}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA9E0681-AFC1-4B9E-BC32-359C80B205A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{80773445-FB61-4F04-A882-1600FD96C55A}"/>
+    <workbookView xWindow="5760" yWindow="0" windowWidth="17280" windowHeight="8880" xr2:uid="{80773445-FB61-4F04-A882-1600FD96C55A}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -368,63 +368,24 @@
     <t>As a financial institution, I want to apply adversarial learning techniques to detect and mitigate fraudulent transactions in real-time, so that I can protect our customers' financial assets more effectively.</t>
   </si>
   <si>
-    <t>As a financial institution, I want to utilize CNNs to analyze time-series financial data and predict short-term market trends with higher accuracy, enabling us to optimize our investment strategies.</t>
-  </si>
-  <si>
     <t>As a financial institution, I want to integrate a conversational agent into our mobile banking app to guide users through complex financial processes such as loan applications and investment portfolio management, simplifying the user experience and increasing adoption rates.</t>
   </si>
   <si>
-    <t>As a financial analyst, I want to develop a decision tree model to predict stock price movements based on historical market data and economic indicators, assisting investors in making informed trading decisions.</t>
-  </si>
-  <si>
-    <t>As a financial institution, I want to use document classification algorithms to automatically categorize and prioritize incoming financial reports and statements, enabling faster decision-making and compliance monitoring.</t>
-  </si>
-  <si>
-    <t>As a financial institution, I want to implement entity extraction models to automatically identify and extract key financial entities (e.g., company names, stock symbols, monetary amounts) from news articles and financial reports, enhancing our market analysis and investment strategies.</t>
-  </si>
-  <si>
-    <t>As a financial institution, I want to employ feature selection techniques to identify the most relevant financial indicators (such as volatility, liquidity ratios) from a large dataset for predicting stock prices, improving the accuracy of our investment models.</t>
-  </si>
-  <si>
     <t>As a financial institution, I want to address imbalanced datasets in fraud detection by employing ensemble learning techniques like AdaBoost to enhance the detection of fraudulent transactions while minimizing false alarms.</t>
   </si>
   <si>
     <t>As a financial institution, I want to implement keyword extraction algorithms to analyze customer reviews and identify recurring themes and concerns related to our financial products, enabling us to prioritize areas for improvement.</t>
   </si>
   <si>
-    <t>As a financial analyst, I want to implement KNN algorithms to classify stocks based on historical trading patterns and market indicators, helping investors identify similar stocks for portfolio diversification strategies.</t>
-  </si>
-  <si>
-    <t>As a financial institution, I want to develop multi-label classification models to categorize financial products based on risk levels, return potential, and investment duration, providing comprehensive recommendations to clients.</t>
-  </si>
-  <si>
     <t>As a financial analyst, I want to build a neural network model to predict stock prices based on historical market data and economic indicators, providing accurate forecasts to guide investment decisions.</t>
   </si>
   <si>
     <t>As a financial institution, I want to develop a random forest-based recommendation system for personalized financial products, suggesting suitable investment options based on customer profiles and financial goals.</t>
   </si>
   <si>
-    <t>As a financial institution, I want to apply semantic similarity algorithms to compare legal documents such as contracts and agreements, ensuring consistency and accuracy in regulatory compliance across different jurisdictions.</t>
-  </si>
-  <si>
-    <t>As a marketer, I want to use sentiment analysis to monitor customer sentiment towards our brand and products on social media platforms, identifying opportunities to enhance customer experience and address negative feedback promptly.</t>
-  </si>
-  <si>
     <t>As a financial institution, I want to deploy speech to text systems for automated transcription of customer service calls and inquiries, improving efficiency in resolving customer issues and enhancing service quality.</t>
   </si>
   <si>
-    <t>As a financial analyst, I want to develop text categorization models to classify research papers and articles into relevant financial topics such as macroeconomics, stock analysis, and industry trends, supporting comprehensive market analysis.</t>
-  </si>
-  <si>
-    <t>As a marketer, I want to use unsupervised clustering techniques to group social media followers based on engagement behaviors and interests, optimizing social media marketing campaigns to increase brand awareness and customer engagement.</t>
-  </si>
-  <si>
-    <t>As a financial analyst, I want to develop voice recognition systems to transcribe and analyze financial podcasts and interviews with industry experts, extracting key insights and market predictions for investors.</t>
-  </si>
-  <si>
-    <t>As a marketer, I want to apply word embedding techniques to analyze customer reviews and social media comments about our products, identifying key product features and sentiments that influence consumer preferences and purchasing decisions.</t>
-  </si>
-  <si>
     <t>Economics</t>
   </si>
   <si>
@@ -1077,6 +1038,45 @@
   </si>
   <si>
     <t>As an economic consultant, I seek to use word embedding techniques to analyze economic policy documents and identify clusters of related policy initiatives and their potential impacts on economic outcomes.</t>
+  </si>
+  <si>
+    <t>As a financial planner, I want to implement CNN architectures to analyze customer financial data and recommend personalized investment portfolios based on risk tolerance and market conditions, optimizing returns for our clients.</t>
+  </si>
+  <si>
+    <t>As a financial planner, I want to implement decision tree algorithms to recommend personalized investment strategies based on client financial goals, risk tolerance, and market conditions, optimizing long-term portfolio growth.</t>
+  </si>
+  <si>
+    <t>As an investment banker, I want a document classification system to categorize news articles and financial reports based on market sectors and trends, facilitating timely insights into industry developments and potential investment opportunities.</t>
+  </si>
+  <si>
+    <t>As a financial data analyst, I want to develop an entity extraction model to automatically identify and extract key financial entities (e.g., company names, stock tickers, financial metrics) from unstructured text data such as news articles and earnings reports.</t>
+  </si>
+  <si>
+    <t>As a financial planner, I want to employ feature selection algorithms to identify influential financial planning parameters (e.g., income level, risk tolerance) from client profiles, enabling personalized and effective financial advice.</t>
+  </si>
+  <si>
+    <t>As a market analyst, I want to apply k-nearest neighbor techniques to identify comparable companies in terms of market capitalization and revenue size, facilitating benchmarking and competitive analysis in the financial services industry.</t>
+  </si>
+  <si>
+    <t>As a marketing strategist, I want to build a multi-label classification system to categorize customer preferences across different product categories (e.g., banking services, investment products), enabling personalized marketing campaigns tailored to each customer's interests.</t>
+  </si>
+  <si>
+    <t>As a market researcher, I want to apply semantic similarity models to analyze customer feedback across various social media platforms, identifying common themes and sentiments about our financial products to improve customer satisfaction.</t>
+  </si>
+  <si>
+    <t>As a marketing strategist, I want to conduct sentiment analysis on customer reviews of our products to understand customer preferences and sentiments, enabling us to tailor marketing campaigns effectively.</t>
+  </si>
+  <si>
+    <t>As a financial advisor, I want to categorize client emails and inquiries into topics such as retirement planning, investment advice, and tax optimization using text categorization, enabling personalized and timely client responses.</t>
+  </si>
+  <si>
+    <t>As a portfolio manager, I want to cluster stocks into groups based on their historical price movements and volatility patterns using unsupervised clustering techniques, assisting in portfolio diversification and risk management.</t>
+  </si>
+  <si>
+    <t>As a financial advisor, I want to use voice recognition technology to transcribe client meetings accurately, allowing me to focus on discussions and provide personalized financial advice without missing critical details.</t>
+  </si>
+  <si>
+    <t>As a financial planner, I want to employ word embedding algorithms to cluster client financial goals and preferences based on their articulated needs and aspirations, facilitating personalized financial planning advice and strategies.</t>
   </si>
 </sst>
 </file>
@@ -1526,8 +1526,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8DF0B04-8323-4309-B759-D1CDDA1FBB0E}">
   <dimension ref="A1:F301"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" topLeftCell="A36" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1587,13 +1587,13 @@
         <v>2</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>129</v>
+        <v>116</v>
       </c>
       <c r="D3" s="9" t="s">
         <v>22</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>130</v>
+        <v>117</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>55</v>
@@ -1613,7 +1613,7 @@
         <v>32</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>110</v>
+        <v>334</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>55</v>
@@ -1627,13 +1627,13 @@
         <v>2</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>129</v>
+        <v>116</v>
       </c>
       <c r="D5" s="9" t="s">
         <v>32</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>131</v>
+        <v>118</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>55</v>
@@ -1653,7 +1653,7 @@
         <v>23</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>55</v>
@@ -1667,13 +1667,13 @@
         <v>2</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>129</v>
+        <v>116</v>
       </c>
       <c r="D7" s="9" t="s">
         <v>23</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>338</v>
+        <v>325</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>55</v>
@@ -1693,7 +1693,7 @@
         <v>12</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>112</v>
+        <v>335</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>55</v>
@@ -1707,13 +1707,13 @@
         <v>2</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>129</v>
+        <v>116</v>
       </c>
       <c r="D9" s="9" t="s">
         <v>12</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>339</v>
+        <v>326</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>55</v>
@@ -1733,7 +1733,7 @@
         <v>33</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>113</v>
+        <v>336</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>55</v>
@@ -1747,13 +1747,13 @@
         <v>2</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>129</v>
+        <v>116</v>
       </c>
       <c r="D11" s="9" t="s">
         <v>33</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>340</v>
+        <v>327</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>55</v>
@@ -1773,7 +1773,7 @@
         <v>25</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>114</v>
+        <v>337</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>55</v>
@@ -1787,13 +1787,13 @@
         <v>2</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>129</v>
+        <v>116</v>
       </c>
       <c r="D13" s="9" t="s">
         <v>25</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>132</v>
+        <v>119</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>55</v>
@@ -1806,14 +1806,14 @@
       <c r="B14" s="10">
         <v>2</v>
       </c>
-      <c r="C14" s="10" t="s">
+      <c r="C14" s="11" t="s">
         <v>108</v>
       </c>
       <c r="D14" s="9" t="s">
         <v>28</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>115</v>
+        <v>338</v>
       </c>
       <c r="F14" s="1" t="s">
         <v>55</v>
@@ -1827,13 +1827,13 @@
         <v>2</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>129</v>
+        <v>116</v>
       </c>
       <c r="D15" s="9" t="s">
         <v>28</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>341</v>
+        <v>328</v>
       </c>
       <c r="F15" s="1" t="s">
         <v>55</v>
@@ -1853,7 +1853,7 @@
         <v>13</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="F16" s="1" t="s">
         <v>55</v>
@@ -1867,13 +1867,13 @@
         <v>2</v>
       </c>
       <c r="C17" s="10" t="s">
-        <v>129</v>
+        <v>116</v>
       </c>
       <c r="D17" s="9" t="s">
         <v>13</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>133</v>
+        <v>120</v>
       </c>
       <c r="F17" s="1" t="s">
         <v>55</v>
@@ -1893,7 +1893,7 @@
         <v>26</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="F18" s="1" t="s">
         <v>55</v>
@@ -1907,13 +1907,13 @@
         <v>2</v>
       </c>
       <c r="C19" s="10" t="s">
-        <v>129</v>
+        <v>116</v>
       </c>
       <c r="D19" s="9" t="s">
         <v>26</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>134</v>
+        <v>121</v>
       </c>
       <c r="F19" s="1" t="s">
         <v>55</v>
@@ -1933,7 +1933,7 @@
         <v>14</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>118</v>
+        <v>339</v>
       </c>
       <c r="F20" s="1" t="s">
         <v>55</v>
@@ -1947,13 +1947,13 @@
         <v>2</v>
       </c>
       <c r="C21" s="10" t="s">
-        <v>129</v>
+        <v>116</v>
       </c>
       <c r="D21" s="9" t="s">
         <v>14</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>342</v>
+        <v>329</v>
       </c>
       <c r="F21" s="1" t="s">
         <v>55</v>
@@ -1973,7 +1973,7 @@
         <v>30</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>119</v>
+        <v>340</v>
       </c>
       <c r="F22" s="1" t="s">
         <v>55</v>
@@ -1987,13 +1987,13 @@
         <v>2</v>
       </c>
       <c r="C23" s="10" t="s">
-        <v>129</v>
+        <v>116</v>
       </c>
       <c r="D23" s="9" t="s">
         <v>30</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>343</v>
+        <v>330</v>
       </c>
       <c r="F23" s="1" t="s">
         <v>55</v>
@@ -2013,7 +2013,7 @@
         <v>15</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="F24" s="1" t="s">
         <v>55</v>
@@ -2027,13 +2027,13 @@
         <v>2</v>
       </c>
       <c r="C25" s="10" t="s">
-        <v>129</v>
+        <v>116</v>
       </c>
       <c r="D25" s="9" t="s">
         <v>15</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>135</v>
+        <v>122</v>
       </c>
       <c r="F25" s="1" t="s">
         <v>55</v>
@@ -2053,7 +2053,7 @@
         <v>16</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="F26" s="1" t="s">
         <v>55</v>
@@ -2067,13 +2067,13 @@
         <v>2</v>
       </c>
       <c r="C27" s="10" t="s">
-        <v>129</v>
+        <v>116</v>
       </c>
       <c r="D27" s="9" t="s">
         <v>16</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>136</v>
+        <v>123</v>
       </c>
       <c r="F27" s="1" t="s">
         <v>55</v>
@@ -2093,7 +2093,7 @@
         <v>17</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>122</v>
+        <v>341</v>
       </c>
       <c r="F28" s="1" t="s">
         <v>55</v>
@@ -2107,13 +2107,13 @@
         <v>2</v>
       </c>
       <c r="C29" s="10" t="s">
-        <v>129</v>
+        <v>116</v>
       </c>
       <c r="D29" s="9" t="s">
         <v>17</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>137</v>
+        <v>124</v>
       </c>
       <c r="F29" s="1" t="s">
         <v>55</v>
@@ -2133,7 +2133,7 @@
         <v>29</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>123</v>
+        <v>342</v>
       </c>
       <c r="F30" s="1" t="s">
         <v>55</v>
@@ -2147,13 +2147,13 @@
         <v>2</v>
       </c>
       <c r="C31" s="10" t="s">
-        <v>129</v>
+        <v>116</v>
       </c>
       <c r="D31" s="9" t="s">
         <v>29</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>138</v>
+        <v>125</v>
       </c>
       <c r="F31" s="1" t="s">
         <v>55</v>
@@ -2173,7 +2173,7 @@
         <v>18</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
       <c r="F32" s="1" t="s">
         <v>55</v>
@@ -2187,13 +2187,13 @@
         <v>2</v>
       </c>
       <c r="C33" s="10" t="s">
-        <v>129</v>
+        <v>116</v>
       </c>
       <c r="D33" s="9" t="s">
         <v>18</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>344</v>
+        <v>331</v>
       </c>
       <c r="F33" s="1" t="s">
         <v>55</v>
@@ -2213,7 +2213,7 @@
         <v>20</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>125</v>
+        <v>343</v>
       </c>
       <c r="F34" s="1" t="s">
         <v>55</v>
@@ -2227,13 +2227,13 @@
         <v>2</v>
       </c>
       <c r="C35" s="10" t="s">
-        <v>129</v>
+        <v>116</v>
       </c>
       <c r="D35" s="9" t="s">
         <v>20</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>139</v>
+        <v>126</v>
       </c>
       <c r="F35" s="1" t="s">
         <v>55</v>
@@ -2253,7 +2253,7 @@
         <v>24</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>126</v>
+        <v>344</v>
       </c>
       <c r="F36" s="1" t="s">
         <v>55</v>
@@ -2267,13 +2267,13 @@
         <v>2</v>
       </c>
       <c r="C37" s="10" t="s">
-        <v>129</v>
+        <v>116</v>
       </c>
       <c r="D37" s="9" t="s">
         <v>24</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>345</v>
+        <v>332</v>
       </c>
       <c r="F37" s="1" t="s">
         <v>55</v>
@@ -2286,14 +2286,14 @@
       <c r="B38" s="10">
         <v>2</v>
       </c>
-      <c r="C38" s="10" t="s">
+      <c r="C38" s="11" t="s">
         <v>108</v>
       </c>
       <c r="D38" s="9" t="s">
         <v>7</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>127</v>
+        <v>345</v>
       </c>
       <c r="F38" s="1" t="s">
         <v>55</v>
@@ -2307,13 +2307,13 @@
         <v>2</v>
       </c>
       <c r="C39" s="10" t="s">
-        <v>129</v>
+        <v>116</v>
       </c>
       <c r="D39" s="9" t="s">
         <v>7</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>140</v>
+        <v>127</v>
       </c>
       <c r="F39" s="1" t="s">
         <v>55</v>
@@ -2333,7 +2333,7 @@
         <v>9</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>128</v>
+        <v>346</v>
       </c>
       <c r="F40" s="1" t="s">
         <v>55</v>
@@ -2347,13 +2347,13 @@
         <v>2</v>
       </c>
       <c r="C41" s="10" t="s">
-        <v>129</v>
+        <v>116</v>
       </c>
       <c r="D41" s="9" t="s">
         <v>9</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>346</v>
+        <v>333</v>
       </c>
       <c r="F41" s="1" t="s">
         <v>55</v>
@@ -2513,7 +2513,7 @@
         <v>12</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>331</v>
+        <v>318</v>
       </c>
       <c r="F49" s="1" t="s">
         <v>55</v>
@@ -2553,7 +2553,7 @@
         <v>33</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>332</v>
+        <v>319</v>
       </c>
       <c r="F51" s="1" t="s">
         <v>55</v>
@@ -2633,7 +2633,7 @@
         <v>28</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>333</v>
+        <v>320</v>
       </c>
       <c r="F55" s="1" t="s">
         <v>55</v>
@@ -2713,7 +2713,7 @@
         <v>26</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>334</v>
+        <v>321</v>
       </c>
       <c r="F59" s="1" t="s">
         <v>55</v>
@@ -2833,7 +2833,7 @@
         <v>15</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>335</v>
+        <v>322</v>
       </c>
       <c r="F65" s="1" t="s">
         <v>55</v>
@@ -2913,7 +2913,7 @@
         <v>17</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>336</v>
+        <v>323</v>
       </c>
       <c r="F69" s="1" t="s">
         <v>55</v>
@@ -3073,7 +3073,7 @@
         <v>24</v>
       </c>
       <c r="E77" s="1" t="s">
-        <v>337</v>
+        <v>324</v>
       </c>
       <c r="F77" s="1" t="s">
         <v>55</v>
@@ -3173,7 +3173,7 @@
         <v>22</v>
       </c>
       <c r="E82" s="1" t="s">
-        <v>314</v>
+        <v>301</v>
       </c>
       <c r="F82" s="1" t="s">
         <v>55</v>
@@ -3193,7 +3193,7 @@
         <v>22</v>
       </c>
       <c r="E83" s="1" t="s">
-        <v>297</v>
+        <v>284</v>
       </c>
       <c r="F83" s="1" t="s">
         <v>55</v>
@@ -3213,7 +3213,7 @@
         <v>32</v>
       </c>
       <c r="E84" s="1" t="s">
-        <v>315</v>
+        <v>302</v>
       </c>
       <c r="F84" s="1" t="s">
         <v>55</v>
@@ -3253,7 +3253,7 @@
         <v>23</v>
       </c>
       <c r="E86" s="1" t="s">
-        <v>316</v>
+        <v>303</v>
       </c>
       <c r="F86" s="1" t="s">
         <v>55</v>
@@ -3273,7 +3273,7 @@
         <v>23</v>
       </c>
       <c r="E87" s="1" t="s">
-        <v>298</v>
+        <v>285</v>
       </c>
       <c r="F87" s="1" t="s">
         <v>55</v>
@@ -3313,7 +3313,7 @@
         <v>12</v>
       </c>
       <c r="E89" s="1" t="s">
-        <v>299</v>
+        <v>286</v>
       </c>
       <c r="F89" s="1" t="s">
         <v>55</v>
@@ -3333,7 +3333,7 @@
         <v>33</v>
       </c>
       <c r="E90" s="1" t="s">
-        <v>317</v>
+        <v>304</v>
       </c>
       <c r="F90" s="1" t="s">
         <v>55</v>
@@ -3353,7 +3353,7 @@
         <v>33</v>
       </c>
       <c r="E91" s="1" t="s">
-        <v>300</v>
+        <v>287</v>
       </c>
       <c r="F91" s="1" t="s">
         <v>55</v>
@@ -3373,7 +3373,7 @@
         <v>25</v>
       </c>
       <c r="E92" s="1" t="s">
-        <v>318</v>
+        <v>305</v>
       </c>
       <c r="F92" s="1" t="s">
         <v>55</v>
@@ -3393,7 +3393,7 @@
         <v>25</v>
       </c>
       <c r="E93" s="1" t="s">
-        <v>301</v>
+        <v>288</v>
       </c>
       <c r="F93" s="1" t="s">
         <v>55</v>
@@ -3453,7 +3453,7 @@
         <v>13</v>
       </c>
       <c r="E96" s="1" t="s">
-        <v>319</v>
+        <v>306</v>
       </c>
       <c r="F96" s="1" t="s">
         <v>55</v>
@@ -3473,7 +3473,7 @@
         <v>13</v>
       </c>
       <c r="E97" s="1" t="s">
-        <v>302</v>
+        <v>289</v>
       </c>
       <c r="F97" s="1" t="s">
         <v>55</v>
@@ -3493,7 +3493,7 @@
         <v>26</v>
       </c>
       <c r="E98" s="1" t="s">
-        <v>320</v>
+        <v>307</v>
       </c>
       <c r="F98" s="1" t="s">
         <v>55</v>
@@ -3533,7 +3533,7 @@
         <v>14</v>
       </c>
       <c r="E100" s="1" t="s">
-        <v>322</v>
+        <v>309</v>
       </c>
       <c r="F100" s="1" t="s">
         <v>55</v>
@@ -3553,7 +3553,7 @@
         <v>14</v>
       </c>
       <c r="E101" s="1" t="s">
-        <v>303</v>
+        <v>290</v>
       </c>
       <c r="F101" s="1" t="s">
         <v>55</v>
@@ -3573,7 +3573,7 @@
         <v>30</v>
       </c>
       <c r="E102" s="1" t="s">
-        <v>321</v>
+        <v>308</v>
       </c>
       <c r="F102" s="1" t="s">
         <v>55</v>
@@ -3593,7 +3593,7 @@
         <v>30</v>
       </c>
       <c r="E103" s="1" t="s">
-        <v>304</v>
+        <v>291</v>
       </c>
       <c r="F103" s="1" t="s">
         <v>55</v>
@@ -3613,7 +3613,7 @@
         <v>15</v>
       </c>
       <c r="E104" s="1" t="s">
-        <v>323</v>
+        <v>310</v>
       </c>
       <c r="F104" s="1" t="s">
         <v>55</v>
@@ -3633,7 +3633,7 @@
         <v>15</v>
       </c>
       <c r="E105" s="1" t="s">
-        <v>305</v>
+        <v>292</v>
       </c>
       <c r="F105" s="1" t="s">
         <v>55</v>
@@ -3653,7 +3653,7 @@
         <v>16</v>
       </c>
       <c r="E106" s="1" t="s">
-        <v>324</v>
+        <v>311</v>
       </c>
       <c r="F106" s="1" t="s">
         <v>55</v>
@@ -3673,7 +3673,7 @@
         <v>16</v>
       </c>
       <c r="E107" s="1" t="s">
-        <v>306</v>
+        <v>293</v>
       </c>
       <c r="F107" s="1" t="s">
         <v>55</v>
@@ -3693,7 +3693,7 @@
         <v>17</v>
       </c>
       <c r="E108" s="1" t="s">
-        <v>325</v>
+        <v>312</v>
       </c>
       <c r="F108" s="1" t="s">
         <v>55</v>
@@ -3713,7 +3713,7 @@
         <v>17</v>
       </c>
       <c r="E109" s="1" t="s">
-        <v>307</v>
+        <v>294</v>
       </c>
       <c r="F109" s="1" t="s">
         <v>55</v>
@@ -3733,7 +3733,7 @@
         <v>29</v>
       </c>
       <c r="E110" s="1" t="s">
-        <v>326</v>
+        <v>313</v>
       </c>
       <c r="F110" s="1" t="s">
         <v>55</v>
@@ -3753,7 +3753,7 @@
         <v>29</v>
       </c>
       <c r="E111" s="1" t="s">
-        <v>308</v>
+        <v>295</v>
       </c>
       <c r="F111" s="1" t="s">
         <v>55</v>
@@ -3773,7 +3773,7 @@
         <v>18</v>
       </c>
       <c r="E112" s="1" t="s">
-        <v>327</v>
+        <v>314</v>
       </c>
       <c r="F112" s="1" t="s">
         <v>55</v>
@@ -3793,7 +3793,7 @@
         <v>18</v>
       </c>
       <c r="E113" s="1" t="s">
-        <v>309</v>
+        <v>296</v>
       </c>
       <c r="F113" s="1" t="s">
         <v>55</v>
@@ -3833,7 +3833,7 @@
         <v>20</v>
       </c>
       <c r="E115" s="6" t="s">
-        <v>310</v>
+        <v>297</v>
       </c>
       <c r="F115" s="1" t="s">
         <v>55</v>
@@ -3853,7 +3853,7 @@
         <v>24</v>
       </c>
       <c r="E116" s="1" t="s">
-        <v>328</v>
+        <v>315</v>
       </c>
       <c r="F116" s="1" t="s">
         <v>55</v>
@@ -3873,7 +3873,7 @@
         <v>24</v>
       </c>
       <c r="E117" s="1" t="s">
-        <v>311</v>
+        <v>298</v>
       </c>
       <c r="F117" s="1" t="s">
         <v>55</v>
@@ -3893,7 +3893,7 @@
         <v>7</v>
       </c>
       <c r="E118" s="1" t="s">
-        <v>329</v>
+        <v>316</v>
       </c>
       <c r="F118" s="1" t="s">
         <v>55</v>
@@ -3913,7 +3913,7 @@
         <v>7</v>
       </c>
       <c r="E119" s="1" t="s">
-        <v>312</v>
+        <v>299</v>
       </c>
       <c r="F119" s="1" t="s">
         <v>55</v>
@@ -3933,7 +3933,7 @@
         <v>9</v>
       </c>
       <c r="E120" s="1" t="s">
-        <v>330</v>
+        <v>317</v>
       </c>
       <c r="F120" s="1" t="s">
         <v>55</v>
@@ -3953,7 +3953,7 @@
         <v>9</v>
       </c>
       <c r="E121" s="1" t="s">
-        <v>313</v>
+        <v>300</v>
       </c>
       <c r="F121" s="1" t="s">
         <v>55</v>
@@ -4013,7 +4013,7 @@
         <v>22</v>
       </c>
       <c r="E124" s="1" t="s">
-        <v>281</v>
+        <v>268</v>
       </c>
       <c r="F124" s="1" t="s">
         <v>55</v>
@@ -4033,7 +4033,7 @@
         <v>32</v>
       </c>
       <c r="E125" s="6" t="s">
-        <v>268</v>
+        <v>255</v>
       </c>
       <c r="F125" s="1" t="s">
         <v>55</v>
@@ -4073,7 +4073,7 @@
         <v>32</v>
       </c>
       <c r="E127" s="1" t="s">
-        <v>282</v>
+        <v>269</v>
       </c>
       <c r="F127" s="1" t="s">
         <v>55</v>
@@ -4093,7 +4093,7 @@
         <v>23</v>
       </c>
       <c r="E128" s="1" t="s">
-        <v>269</v>
+        <v>256</v>
       </c>
       <c r="F128" s="1" t="s">
         <v>55</v>
@@ -4133,7 +4133,7 @@
         <v>23</v>
       </c>
       <c r="E130" s="1" t="s">
-        <v>283</v>
+        <v>270</v>
       </c>
       <c r="F130" s="1" t="s">
         <v>55</v>
@@ -4193,7 +4193,7 @@
         <v>12</v>
       </c>
       <c r="E133" s="6" t="s">
-        <v>284</v>
+        <v>271</v>
       </c>
       <c r="F133" s="1" t="s">
         <v>55</v>
@@ -4213,7 +4213,7 @@
         <v>33</v>
       </c>
       <c r="E134" s="1" t="s">
-        <v>270</v>
+        <v>257</v>
       </c>
       <c r="F134" s="1" t="s">
         <v>55</v>
@@ -4253,7 +4253,7 @@
         <v>33</v>
       </c>
       <c r="E136" s="1" t="s">
-        <v>285</v>
+        <v>272</v>
       </c>
       <c r="F136" s="1" t="s">
         <v>55</v>
@@ -4273,7 +4273,7 @@
         <v>25</v>
       </c>
       <c r="E137" s="1" t="s">
-        <v>271</v>
+        <v>258</v>
       </c>
       <c r="F137" s="1" t="s">
         <v>55</v>
@@ -4313,7 +4313,7 @@
         <v>25</v>
       </c>
       <c r="E139" s="1" t="s">
-        <v>286</v>
+        <v>273</v>
       </c>
       <c r="F139" s="1" t="s">
         <v>55</v>
@@ -4373,7 +4373,7 @@
         <v>28</v>
       </c>
       <c r="E142" s="1" t="s">
-        <v>287</v>
+        <v>274</v>
       </c>
       <c r="F142" s="1" t="s">
         <v>55</v>
@@ -4393,7 +4393,7 @@
         <v>13</v>
       </c>
       <c r="E143" s="6" t="s">
-        <v>272</v>
+        <v>259</v>
       </c>
       <c r="F143" s="1" t="s">
         <v>55</v>
@@ -4433,7 +4433,7 @@
         <v>13</v>
       </c>
       <c r="E145" s="1" t="s">
-        <v>288</v>
+        <v>275</v>
       </c>
       <c r="F145" s="1" t="s">
         <v>55</v>
@@ -4493,7 +4493,7 @@
         <v>26</v>
       </c>
       <c r="E148" s="1" t="s">
-        <v>289</v>
+        <v>276</v>
       </c>
       <c r="F148" s="1" t="s">
         <v>55</v>
@@ -4513,7 +4513,7 @@
         <v>14</v>
       </c>
       <c r="E149" s="1" t="s">
-        <v>274</v>
+        <v>261</v>
       </c>
       <c r="F149" s="1" t="s">
         <v>55</v>
@@ -4533,7 +4533,7 @@
         <v>14</v>
       </c>
       <c r="E150" s="1" t="s">
-        <v>296</v>
+        <v>283</v>
       </c>
       <c r="F150" s="1" t="s">
         <v>55</v>
@@ -4553,7 +4553,7 @@
         <v>14</v>
       </c>
       <c r="E151" s="1" t="s">
-        <v>290</v>
+        <v>277</v>
       </c>
       <c r="F151" s="1" t="s">
         <v>55</v>
@@ -4573,7 +4573,7 @@
         <v>30</v>
       </c>
       <c r="E152" s="1" t="s">
-        <v>273</v>
+        <v>260</v>
       </c>
       <c r="F152" s="1" t="s">
         <v>55</v>
@@ -4613,7 +4613,7 @@
         <v>30</v>
       </c>
       <c r="E154" s="1" t="s">
-        <v>291</v>
+        <v>278</v>
       </c>
       <c r="F154" s="1" t="s">
         <v>55</v>
@@ -4633,7 +4633,7 @@
         <v>15</v>
       </c>
       <c r="E155" s="1" t="s">
-        <v>275</v>
+        <v>262</v>
       </c>
       <c r="F155" s="1" t="s">
         <v>55</v>
@@ -4673,7 +4673,7 @@
         <v>15</v>
       </c>
       <c r="E157" s="1" t="s">
-        <v>292</v>
+        <v>279</v>
       </c>
       <c r="F157" s="1" t="s">
         <v>55</v>
@@ -4693,7 +4693,7 @@
         <v>16</v>
       </c>
       <c r="E158" s="1" t="s">
-        <v>276</v>
+        <v>263</v>
       </c>
       <c r="F158" s="1" t="s">
         <v>55</v>
@@ -4753,7 +4753,7 @@
         <v>17</v>
       </c>
       <c r="E161" s="1" t="s">
-        <v>278</v>
+        <v>265</v>
       </c>
       <c r="F161" s="1" t="s">
         <v>55</v>
@@ -4813,7 +4813,7 @@
         <v>29</v>
       </c>
       <c r="E164" s="1" t="s">
-        <v>277</v>
+        <v>264</v>
       </c>
       <c r="F164" s="1" t="s">
         <v>55</v>
@@ -4853,7 +4853,7 @@
         <v>29</v>
       </c>
       <c r="E166" s="1" t="s">
-        <v>293</v>
+        <v>280</v>
       </c>
       <c r="F166" s="1" t="s">
         <v>55</v>
@@ -4873,7 +4873,7 @@
         <v>18</v>
       </c>
       <c r="E167" s="1" t="s">
-        <v>279</v>
+        <v>266</v>
       </c>
       <c r="F167" s="1" t="s">
         <v>55</v>
@@ -4973,7 +4973,7 @@
         <v>20</v>
       </c>
       <c r="E172" s="1" t="s">
-        <v>294</v>
+        <v>281</v>
       </c>
       <c r="F172" s="1" t="s">
         <v>55</v>
@@ -4993,7 +4993,7 @@
         <v>24</v>
       </c>
       <c r="E173" s="1" t="s">
-        <v>280</v>
+        <v>267</v>
       </c>
       <c r="F173" s="1" t="s">
         <v>55</v>
@@ -5093,7 +5093,7 @@
         <v>7</v>
       </c>
       <c r="E178" s="1" t="s">
-        <v>295</v>
+        <v>282</v>
       </c>
       <c r="F178" s="1" t="s">
         <v>55</v>
@@ -5161,19 +5161,19 @@
     </row>
     <row r="182" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A182" s="12" t="s">
-        <v>141</v>
+        <v>128</v>
       </c>
       <c r="B182" s="12">
         <v>6</v>
       </c>
       <c r="C182" s="12" t="s">
-        <v>142</v>
+        <v>129</v>
       </c>
       <c r="D182" s="9" t="s">
         <v>22</v>
       </c>
       <c r="E182" s="1" t="s">
-        <v>143</v>
+        <v>130</v>
       </c>
       <c r="F182" s="1" t="s">
         <v>55</v>
@@ -5181,19 +5181,19 @@
     </row>
     <row r="183" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A183" s="12" t="s">
-        <v>141</v>
+        <v>128</v>
       </c>
       <c r="B183" s="12">
         <v>6</v>
       </c>
       <c r="C183" s="12" t="s">
-        <v>163</v>
+        <v>150</v>
       </c>
       <c r="D183" s="9" t="s">
         <v>22</v>
       </c>
       <c r="E183" s="1" t="s">
-        <v>164</v>
+        <v>151</v>
       </c>
       <c r="F183" s="1" t="s">
         <v>55</v>
@@ -5201,19 +5201,19 @@
     </row>
     <row r="184" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A184" s="12" t="s">
-        <v>141</v>
+        <v>128</v>
       </c>
       <c r="B184" s="12">
         <v>6</v>
       </c>
       <c r="C184" s="12" t="s">
-        <v>184</v>
+        <v>171</v>
       </c>
       <c r="D184" s="9" t="s">
         <v>22</v>
       </c>
       <c r="E184" s="1" t="s">
-        <v>185</v>
+        <v>172</v>
       </c>
       <c r="F184" s="1" t="s">
         <v>55</v>
@@ -5221,19 +5221,19 @@
     </row>
     <row r="185" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A185" s="12" t="s">
-        <v>141</v>
+        <v>128</v>
       </c>
       <c r="B185" s="12">
         <v>6</v>
       </c>
       <c r="C185" s="12" t="s">
-        <v>205</v>
+        <v>192</v>
       </c>
       <c r="D185" s="9" t="s">
         <v>22</v>
       </c>
       <c r="E185" s="1" t="s">
-        <v>206</v>
+        <v>193</v>
       </c>
       <c r="F185" s="1" t="s">
         <v>55</v>
@@ -5241,19 +5241,19 @@
     </row>
     <row r="186" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A186" s="12" t="s">
-        <v>141</v>
+        <v>128</v>
       </c>
       <c r="B186" s="12">
         <v>6</v>
       </c>
       <c r="C186" s="12" t="s">
-        <v>226</v>
+        <v>213</v>
       </c>
       <c r="D186" s="9" t="s">
         <v>22</v>
       </c>
       <c r="E186" s="1" t="s">
-        <v>227</v>
+        <v>214</v>
       </c>
       <c r="F186" s="1" t="s">
         <v>55</v>
@@ -5261,19 +5261,19 @@
     </row>
     <row r="187" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A187" s="12" t="s">
-        <v>141</v>
+        <v>128</v>
       </c>
       <c r="B187" s="12">
         <v>6</v>
       </c>
       <c r="C187" s="12" t="s">
-        <v>247</v>
+        <v>234</v>
       </c>
       <c r="D187" s="9" t="s">
         <v>22</v>
       </c>
       <c r="E187" s="1" t="s">
-        <v>248</v>
+        <v>235</v>
       </c>
       <c r="F187" s="1" t="s">
         <v>55</v>
@@ -5281,19 +5281,19 @@
     </row>
     <row r="188" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A188" s="12" t="s">
-        <v>141</v>
+        <v>128</v>
       </c>
       <c r="B188" s="12">
         <v>6</v>
       </c>
       <c r="C188" s="12" t="s">
-        <v>142</v>
+        <v>129</v>
       </c>
       <c r="D188" s="9" t="s">
         <v>32</v>
       </c>
       <c r="E188" s="1" t="s">
-        <v>144</v>
+        <v>131</v>
       </c>
       <c r="F188" s="1" t="s">
         <v>55</v>
@@ -5301,19 +5301,19 @@
     </row>
     <row r="189" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A189" s="12" t="s">
-        <v>141</v>
+        <v>128</v>
       </c>
       <c r="B189" s="12">
         <v>6</v>
       </c>
       <c r="C189" s="12" t="s">
-        <v>163</v>
+        <v>150</v>
       </c>
       <c r="D189" s="9" t="s">
         <v>32</v>
       </c>
       <c r="E189" s="1" t="s">
-        <v>165</v>
+        <v>152</v>
       </c>
       <c r="F189" s="1" t="s">
         <v>55</v>
@@ -5321,19 +5321,19 @@
     </row>
     <row r="190" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A190" s="12" t="s">
-        <v>141</v>
+        <v>128</v>
       </c>
       <c r="B190" s="12">
         <v>6</v>
       </c>
       <c r="C190" s="12" t="s">
-        <v>184</v>
+        <v>171</v>
       </c>
       <c r="D190" s="9" t="s">
         <v>32</v>
       </c>
       <c r="E190" s="1" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
       <c r="F190" s="1" t="s">
         <v>55</v>
@@ -5341,19 +5341,19 @@
     </row>
     <row r="191" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A191" s="12" t="s">
-        <v>141</v>
+        <v>128</v>
       </c>
       <c r="B191" s="12">
         <v>6</v>
       </c>
       <c r="C191" s="12" t="s">
-        <v>205</v>
+        <v>192</v>
       </c>
       <c r="D191" s="9" t="s">
         <v>32</v>
       </c>
       <c r="E191" s="1" t="s">
-        <v>207</v>
+        <v>194</v>
       </c>
       <c r="F191" s="1" t="s">
         <v>55</v>
@@ -5361,19 +5361,19 @@
     </row>
     <row r="192" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A192" s="12" t="s">
-        <v>141</v>
+        <v>128</v>
       </c>
       <c r="B192" s="12">
         <v>6</v>
       </c>
       <c r="C192" s="12" t="s">
-        <v>226</v>
+        <v>213</v>
       </c>
       <c r="D192" s="9" t="s">
         <v>32</v>
       </c>
       <c r="E192" s="1" t="s">
-        <v>228</v>
+        <v>215</v>
       </c>
       <c r="F192" s="1" t="s">
         <v>55</v>
@@ -5381,19 +5381,19 @@
     </row>
     <row r="193" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A193" s="12" t="s">
-        <v>141</v>
+        <v>128</v>
       </c>
       <c r="B193" s="12">
         <v>6</v>
       </c>
       <c r="C193" s="12" t="s">
-        <v>247</v>
+        <v>234</v>
       </c>
       <c r="D193" s="9" t="s">
         <v>32</v>
       </c>
       <c r="E193" s="1" t="s">
-        <v>249</v>
+        <v>236</v>
       </c>
       <c r="F193" s="1" t="s">
         <v>55</v>
@@ -5401,19 +5401,19 @@
     </row>
     <row r="194" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A194" s="12" t="s">
-        <v>141</v>
+        <v>128</v>
       </c>
       <c r="B194" s="12">
         <v>6</v>
       </c>
       <c r="C194" s="12" t="s">
-        <v>142</v>
+        <v>129</v>
       </c>
       <c r="D194" s="9" t="s">
         <v>23</v>
       </c>
       <c r="E194" s="1" t="s">
-        <v>145</v>
+        <v>132</v>
       </c>
       <c r="F194" s="1" t="s">
         <v>55</v>
@@ -5421,19 +5421,19 @@
     </row>
     <row r="195" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A195" s="12" t="s">
-        <v>141</v>
+        <v>128</v>
       </c>
       <c r="B195" s="12">
         <v>6</v>
       </c>
       <c r="C195" s="12" t="s">
-        <v>163</v>
+        <v>150</v>
       </c>
       <c r="D195" s="9" t="s">
         <v>23</v>
       </c>
       <c r="E195" s="1" t="s">
-        <v>166</v>
+        <v>153</v>
       </c>
       <c r="F195" s="1" t="s">
         <v>55</v>
@@ -5441,19 +5441,19 @@
     </row>
     <row r="196" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A196" s="12" t="s">
-        <v>141</v>
+        <v>128</v>
       </c>
       <c r="B196" s="12">
         <v>6</v>
       </c>
       <c r="C196" s="12" t="s">
-        <v>184</v>
+        <v>171</v>
       </c>
       <c r="D196" s="9" t="s">
         <v>23</v>
       </c>
       <c r="E196" s="1" t="s">
-        <v>187</v>
+        <v>174</v>
       </c>
       <c r="F196" s="1" t="s">
         <v>55</v>
@@ -5461,19 +5461,19 @@
     </row>
     <row r="197" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A197" s="12" t="s">
-        <v>141</v>
+        <v>128</v>
       </c>
       <c r="B197" s="12">
         <v>6</v>
       </c>
       <c r="C197" s="12" t="s">
-        <v>205</v>
+        <v>192</v>
       </c>
       <c r="D197" s="9" t="s">
         <v>23</v>
       </c>
       <c r="E197" s="1" t="s">
-        <v>208</v>
+        <v>195</v>
       </c>
       <c r="F197" s="1" t="s">
         <v>55</v>
@@ -5481,19 +5481,19 @@
     </row>
     <row r="198" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A198" s="12" t="s">
-        <v>141</v>
+        <v>128</v>
       </c>
       <c r="B198" s="12">
         <v>6</v>
       </c>
       <c r="C198" s="12" t="s">
-        <v>226</v>
+        <v>213</v>
       </c>
       <c r="D198" s="9" t="s">
         <v>23</v>
       </c>
       <c r="E198" s="1" t="s">
-        <v>229</v>
+        <v>216</v>
       </c>
       <c r="F198" s="1" t="s">
         <v>55</v>
@@ -5501,19 +5501,19 @@
     </row>
     <row r="199" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A199" s="12" t="s">
-        <v>141</v>
+        <v>128</v>
       </c>
       <c r="B199" s="12">
         <v>6</v>
       </c>
       <c r="C199" s="12" t="s">
-        <v>247</v>
+        <v>234</v>
       </c>
       <c r="D199" s="9" t="s">
         <v>23</v>
       </c>
       <c r="E199" s="1" t="s">
-        <v>250</v>
+        <v>237</v>
       </c>
       <c r="F199" s="1" t="s">
         <v>55</v>
@@ -5521,19 +5521,19 @@
     </row>
     <row r="200" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A200" s="12" t="s">
-        <v>141</v>
+        <v>128</v>
       </c>
       <c r="B200" s="12">
         <v>6</v>
       </c>
       <c r="C200" s="12" t="s">
-        <v>142</v>
+        <v>129</v>
       </c>
       <c r="D200" s="9" t="s">
         <v>12</v>
       </c>
       <c r="E200" s="1" t="s">
-        <v>146</v>
+        <v>133</v>
       </c>
       <c r="F200" s="1" t="s">
         <v>55</v>
@@ -5541,19 +5541,19 @@
     </row>
     <row r="201" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A201" s="12" t="s">
-        <v>141</v>
+        <v>128</v>
       </c>
       <c r="B201" s="12">
         <v>6</v>
       </c>
       <c r="C201" s="12" t="s">
-        <v>163</v>
+        <v>150</v>
       </c>
       <c r="D201" s="9" t="s">
         <v>12</v>
       </c>
       <c r="E201" s="1" t="s">
-        <v>167</v>
+        <v>154</v>
       </c>
       <c r="F201" s="1" t="s">
         <v>55</v>
@@ -5561,19 +5561,19 @@
     </row>
     <row r="202" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A202" s="12" t="s">
-        <v>141</v>
+        <v>128</v>
       </c>
       <c r="B202" s="12">
         <v>6</v>
       </c>
       <c r="C202" s="12" t="s">
-        <v>184</v>
+        <v>171</v>
       </c>
       <c r="D202" s="9" t="s">
         <v>12</v>
       </c>
       <c r="E202" s="1" t="s">
-        <v>188</v>
+        <v>175</v>
       </c>
       <c r="F202" s="1" t="s">
         <v>55</v>
@@ -5581,19 +5581,19 @@
     </row>
     <row r="203" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A203" s="12" t="s">
-        <v>141</v>
+        <v>128</v>
       </c>
       <c r="B203" s="12">
         <v>6</v>
       </c>
       <c r="C203" s="12" t="s">
-        <v>205</v>
+        <v>192</v>
       </c>
       <c r="D203" s="9" t="s">
         <v>12</v>
       </c>
       <c r="E203" s="1" t="s">
-        <v>209</v>
+        <v>196</v>
       </c>
       <c r="F203" s="1" t="s">
         <v>55</v>
@@ -5601,19 +5601,19 @@
     </row>
     <row r="204" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A204" s="12" t="s">
-        <v>141</v>
+        <v>128</v>
       </c>
       <c r="B204" s="12">
         <v>6</v>
       </c>
       <c r="C204" s="12" t="s">
-        <v>226</v>
+        <v>213</v>
       </c>
       <c r="D204" s="9" t="s">
         <v>12</v>
       </c>
       <c r="E204" s="1" t="s">
-        <v>230</v>
+        <v>217</v>
       </c>
       <c r="F204" s="1" t="s">
         <v>55</v>
@@ -5621,19 +5621,19 @@
     </row>
     <row r="205" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A205" s="12" t="s">
-        <v>141</v>
+        <v>128</v>
       </c>
       <c r="B205" s="12">
         <v>6</v>
       </c>
       <c r="C205" s="12" t="s">
-        <v>247</v>
+        <v>234</v>
       </c>
       <c r="D205" s="9" t="s">
         <v>12</v>
       </c>
       <c r="E205" s="1" t="s">
-        <v>251</v>
+        <v>238</v>
       </c>
       <c r="F205" s="1" t="s">
         <v>55</v>
@@ -5641,19 +5641,19 @@
     </row>
     <row r="206" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A206" s="12" t="s">
-        <v>141</v>
+        <v>128</v>
       </c>
       <c r="B206" s="12">
         <v>6</v>
       </c>
       <c r="C206" s="12" t="s">
-        <v>142</v>
+        <v>129</v>
       </c>
       <c r="D206" s="9" t="s">
         <v>33</v>
       </c>
       <c r="E206" s="1" t="s">
-        <v>147</v>
+        <v>134</v>
       </c>
       <c r="F206" s="1" t="s">
         <v>55</v>
@@ -5661,19 +5661,19 @@
     </row>
     <row r="207" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A207" s="12" t="s">
-        <v>141</v>
+        <v>128</v>
       </c>
       <c r="B207" s="12">
         <v>6</v>
       </c>
       <c r="C207" s="12" t="s">
-        <v>163</v>
+        <v>150</v>
       </c>
       <c r="D207" s="9" t="s">
         <v>33</v>
       </c>
       <c r="E207" s="1" t="s">
-        <v>168</v>
+        <v>155</v>
       </c>
       <c r="F207" s="1" t="s">
         <v>55</v>
@@ -5681,19 +5681,19 @@
     </row>
     <row r="208" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A208" s="12" t="s">
-        <v>141</v>
+        <v>128</v>
       </c>
       <c r="B208" s="12">
         <v>6</v>
       </c>
       <c r="C208" s="12" t="s">
-        <v>184</v>
+        <v>171</v>
       </c>
       <c r="D208" s="9" t="s">
         <v>33</v>
       </c>
       <c r="E208" s="1" t="s">
-        <v>189</v>
+        <v>176</v>
       </c>
       <c r="F208" s="1" t="s">
         <v>55</v>
@@ -5701,19 +5701,19 @@
     </row>
     <row r="209" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A209" s="12" t="s">
-        <v>141</v>
+        <v>128</v>
       </c>
       <c r="B209" s="12">
         <v>6</v>
       </c>
       <c r="C209" s="12" t="s">
-        <v>205</v>
+        <v>192</v>
       </c>
       <c r="D209" s="9" t="s">
         <v>33</v>
       </c>
       <c r="E209" s="1" t="s">
-        <v>210</v>
+        <v>197</v>
       </c>
       <c r="F209" s="1" t="s">
         <v>55</v>
@@ -5721,19 +5721,19 @@
     </row>
     <row r="210" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A210" s="12" t="s">
-        <v>141</v>
+        <v>128</v>
       </c>
       <c r="B210" s="12">
         <v>6</v>
       </c>
       <c r="C210" s="12" t="s">
-        <v>226</v>
+        <v>213</v>
       </c>
       <c r="D210" s="9" t="s">
         <v>33</v>
       </c>
       <c r="E210" s="1" t="s">
-        <v>231</v>
+        <v>218</v>
       </c>
       <c r="F210" s="1" t="s">
         <v>55</v>
@@ -5741,19 +5741,19 @@
     </row>
     <row r="211" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A211" s="12" t="s">
-        <v>141</v>
+        <v>128</v>
       </c>
       <c r="B211" s="12">
         <v>6</v>
       </c>
       <c r="C211" s="12" t="s">
-        <v>247</v>
+        <v>234</v>
       </c>
       <c r="D211" s="9" t="s">
         <v>33</v>
       </c>
       <c r="E211" s="1" t="s">
-        <v>252</v>
+        <v>239</v>
       </c>
       <c r="F211" s="1" t="s">
         <v>55</v>
@@ -5761,19 +5761,19 @@
     </row>
     <row r="212" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A212" s="12" t="s">
-        <v>141</v>
+        <v>128</v>
       </c>
       <c r="B212" s="12">
         <v>6</v>
       </c>
       <c r="C212" s="12" t="s">
-        <v>142</v>
+        <v>129</v>
       </c>
       <c r="D212" s="9" t="s">
         <v>25</v>
       </c>
       <c r="E212" s="1" t="s">
-        <v>148</v>
+        <v>135</v>
       </c>
       <c r="F212" s="1" t="s">
         <v>55</v>
@@ -5781,19 +5781,19 @@
     </row>
     <row r="213" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A213" s="12" t="s">
-        <v>141</v>
+        <v>128</v>
       </c>
       <c r="B213" s="12">
         <v>6</v>
       </c>
       <c r="C213" s="12" t="s">
-        <v>163</v>
+        <v>150</v>
       </c>
       <c r="D213" s="9" t="s">
         <v>25</v>
       </c>
       <c r="E213" s="1" t="s">
-        <v>169</v>
+        <v>156</v>
       </c>
       <c r="F213" s="1" t="s">
         <v>55</v>
@@ -5801,19 +5801,19 @@
     </row>
     <row r="214" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A214" s="12" t="s">
-        <v>141</v>
+        <v>128</v>
       </c>
       <c r="B214" s="12">
         <v>6</v>
       </c>
       <c r="C214" s="12" t="s">
-        <v>184</v>
+        <v>171</v>
       </c>
       <c r="D214" s="9" t="s">
         <v>25</v>
       </c>
       <c r="E214" s="1" t="s">
-        <v>190</v>
+        <v>177</v>
       </c>
       <c r="F214" s="1" t="s">
         <v>55</v>
@@ -5821,19 +5821,19 @@
     </row>
     <row r="215" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A215" s="12" t="s">
-        <v>141</v>
+        <v>128</v>
       </c>
       <c r="B215" s="12">
         <v>6</v>
       </c>
       <c r="C215" s="12" t="s">
-        <v>205</v>
+        <v>192</v>
       </c>
       <c r="D215" s="9" t="s">
         <v>25</v>
       </c>
       <c r="E215" s="1" t="s">
-        <v>211</v>
+        <v>198</v>
       </c>
       <c r="F215" s="1" t="s">
         <v>55</v>
@@ -5841,19 +5841,19 @@
     </row>
     <row r="216" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A216" s="12" t="s">
-        <v>141</v>
+        <v>128</v>
       </c>
       <c r="B216" s="12">
         <v>6</v>
       </c>
       <c r="C216" s="12" t="s">
-        <v>226</v>
+        <v>213</v>
       </c>
       <c r="D216" s="9" t="s">
         <v>25</v>
       </c>
       <c r="E216" s="1" t="s">
-        <v>232</v>
+        <v>219</v>
       </c>
       <c r="F216" s="1" t="s">
         <v>55</v>
@@ -5861,19 +5861,19 @@
     </row>
     <row r="217" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A217" s="12" t="s">
-        <v>141</v>
+        <v>128</v>
       </c>
       <c r="B217" s="12">
         <v>6</v>
       </c>
       <c r="C217" s="12" t="s">
-        <v>247</v>
+        <v>234</v>
       </c>
       <c r="D217" s="9" t="s">
         <v>25</v>
       </c>
       <c r="E217" s="1" t="s">
-        <v>253</v>
+        <v>240</v>
       </c>
       <c r="F217" s="1" t="s">
         <v>55</v>
@@ -5881,19 +5881,19 @@
     </row>
     <row r="218" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A218" s="12" t="s">
-        <v>141</v>
+        <v>128</v>
       </c>
       <c r="B218" s="12">
         <v>6</v>
       </c>
       <c r="C218" s="12" t="s">
-        <v>142</v>
+        <v>129</v>
       </c>
       <c r="D218" s="9" t="s">
         <v>28</v>
       </c>
       <c r="E218" s="1" t="s">
-        <v>149</v>
+        <v>136</v>
       </c>
       <c r="F218" s="1" t="s">
         <v>55</v>
@@ -5901,19 +5901,19 @@
     </row>
     <row r="219" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A219" s="12" t="s">
-        <v>141</v>
+        <v>128</v>
       </c>
       <c r="B219" s="12">
         <v>6</v>
       </c>
       <c r="C219" s="12" t="s">
-        <v>163</v>
+        <v>150</v>
       </c>
       <c r="D219" s="9" t="s">
         <v>28</v>
       </c>
       <c r="E219" s="1" t="s">
-        <v>170</v>
+        <v>157</v>
       </c>
       <c r="F219" s="1" t="s">
         <v>55</v>
@@ -5921,19 +5921,19 @@
     </row>
     <row r="220" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A220" s="12" t="s">
-        <v>141</v>
+        <v>128</v>
       </c>
       <c r="B220" s="12">
         <v>6</v>
       </c>
       <c r="C220" s="12" t="s">
-        <v>184</v>
+        <v>171</v>
       </c>
       <c r="D220" s="9" t="s">
         <v>28</v>
       </c>
       <c r="E220" s="1" t="s">
-        <v>191</v>
+        <v>178</v>
       </c>
       <c r="F220" s="1" t="s">
         <v>55</v>
@@ -5941,19 +5941,19 @@
     </row>
     <row r="221" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A221" s="12" t="s">
-        <v>141</v>
+        <v>128</v>
       </c>
       <c r="B221" s="12">
         <v>6</v>
       </c>
       <c r="C221" s="12" t="s">
-        <v>205</v>
+        <v>192</v>
       </c>
       <c r="D221" s="9" t="s">
         <v>28</v>
       </c>
       <c r="E221" s="1" t="s">
-        <v>212</v>
+        <v>199</v>
       </c>
       <c r="F221" s="1" t="s">
         <v>55</v>
@@ -5961,19 +5961,19 @@
     </row>
     <row r="222" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A222" s="12" t="s">
-        <v>141</v>
+        <v>128</v>
       </c>
       <c r="B222" s="12">
         <v>6</v>
       </c>
       <c r="C222" s="12" t="s">
-        <v>226</v>
+        <v>213</v>
       </c>
       <c r="D222" s="9" t="s">
         <v>28</v>
       </c>
       <c r="E222" s="1" t="s">
-        <v>233</v>
+        <v>220</v>
       </c>
       <c r="F222" s="1" t="s">
         <v>55</v>
@@ -5981,19 +5981,19 @@
     </row>
     <row r="223" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A223" s="12" t="s">
-        <v>141</v>
+        <v>128</v>
       </c>
       <c r="B223" s="12">
         <v>6</v>
       </c>
       <c r="C223" s="12" t="s">
-        <v>247</v>
+        <v>234</v>
       </c>
       <c r="D223" s="9" t="s">
         <v>28</v>
       </c>
       <c r="E223" s="1" t="s">
-        <v>254</v>
+        <v>241</v>
       </c>
       <c r="F223" s="1" t="s">
         <v>55</v>
@@ -6001,19 +6001,19 @@
     </row>
     <row r="224" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A224" s="12" t="s">
-        <v>141</v>
+        <v>128</v>
       </c>
       <c r="B224" s="12">
         <v>6</v>
       </c>
       <c r="C224" s="12" t="s">
-        <v>142</v>
+        <v>129</v>
       </c>
       <c r="D224" s="9" t="s">
         <v>13</v>
       </c>
       <c r="E224" s="1" t="s">
-        <v>150</v>
+        <v>137</v>
       </c>
       <c r="F224" s="1" t="s">
         <v>55</v>
@@ -6021,19 +6021,19 @@
     </row>
     <row r="225" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A225" s="12" t="s">
-        <v>141</v>
+        <v>128</v>
       </c>
       <c r="B225" s="12">
         <v>6</v>
       </c>
       <c r="C225" s="12" t="s">
-        <v>163</v>
+        <v>150</v>
       </c>
       <c r="D225" s="9" t="s">
         <v>13</v>
       </c>
       <c r="E225" s="1" t="s">
-        <v>171</v>
+        <v>158</v>
       </c>
       <c r="F225" s="1" t="s">
         <v>55</v>
@@ -6041,19 +6041,19 @@
     </row>
     <row r="226" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A226" s="12" t="s">
-        <v>141</v>
+        <v>128</v>
       </c>
       <c r="B226" s="12">
         <v>6</v>
       </c>
       <c r="C226" s="12" t="s">
-        <v>184</v>
+        <v>171</v>
       </c>
       <c r="D226" s="9" t="s">
         <v>13</v>
       </c>
       <c r="E226" s="1" t="s">
-        <v>192</v>
+        <v>179</v>
       </c>
       <c r="F226" s="1" t="s">
         <v>55</v>
@@ -6061,19 +6061,19 @@
     </row>
     <row r="227" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A227" s="12" t="s">
-        <v>141</v>
+        <v>128</v>
       </c>
       <c r="B227" s="12">
         <v>6</v>
       </c>
       <c r="C227" s="12" t="s">
-        <v>205</v>
+        <v>192</v>
       </c>
       <c r="D227" s="9" t="s">
         <v>13</v>
       </c>
       <c r="E227" s="1" t="s">
-        <v>213</v>
+        <v>200</v>
       </c>
       <c r="F227" s="1" t="s">
         <v>55</v>
@@ -6081,19 +6081,19 @@
     </row>
     <row r="228" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A228" s="12" t="s">
-        <v>141</v>
+        <v>128</v>
       </c>
       <c r="B228" s="12">
         <v>6</v>
       </c>
       <c r="C228" s="12" t="s">
-        <v>226</v>
+        <v>213</v>
       </c>
       <c r="D228" s="9" t="s">
         <v>13</v>
       </c>
       <c r="E228" s="1" t="s">
-        <v>234</v>
+        <v>221</v>
       </c>
       <c r="F228" s="1" t="s">
         <v>55</v>
@@ -6101,19 +6101,19 @@
     </row>
     <row r="229" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A229" s="12" t="s">
-        <v>141</v>
+        <v>128</v>
       </c>
       <c r="B229" s="12">
         <v>6</v>
       </c>
       <c r="C229" s="12" t="s">
-        <v>247</v>
+        <v>234</v>
       </c>
       <c r="D229" s="9" t="s">
         <v>13</v>
       </c>
       <c r="E229" s="1" t="s">
-        <v>255</v>
+        <v>242</v>
       </c>
       <c r="F229" s="1" t="s">
         <v>55</v>
@@ -6121,19 +6121,19 @@
     </row>
     <row r="230" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A230" s="12" t="s">
-        <v>141</v>
+        <v>128</v>
       </c>
       <c r="B230" s="12">
         <v>6</v>
       </c>
       <c r="C230" s="12" t="s">
-        <v>142</v>
+        <v>129</v>
       </c>
       <c r="D230" s="9" t="s">
         <v>26</v>
       </c>
       <c r="E230" s="1" t="s">
-        <v>151</v>
+        <v>138</v>
       </c>
       <c r="F230" s="1" t="s">
         <v>55</v>
@@ -6141,19 +6141,19 @@
     </row>
     <row r="231" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A231" s="12" t="s">
-        <v>141</v>
+        <v>128</v>
       </c>
       <c r="B231" s="12">
         <v>6</v>
       </c>
       <c r="C231" s="12" t="s">
-        <v>163</v>
+        <v>150</v>
       </c>
       <c r="D231" s="9" t="s">
         <v>26</v>
       </c>
       <c r="E231" s="1" t="s">
-        <v>172</v>
+        <v>159</v>
       </c>
       <c r="F231" s="1" t="s">
         <v>55</v>
@@ -6161,19 +6161,19 @@
     </row>
     <row r="232" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A232" s="12" t="s">
-        <v>141</v>
+        <v>128</v>
       </c>
       <c r="B232" s="12">
         <v>6</v>
       </c>
       <c r="C232" s="12" t="s">
-        <v>184</v>
+        <v>171</v>
       </c>
       <c r="D232" s="9" t="s">
         <v>26</v>
       </c>
       <c r="E232" s="1" t="s">
-        <v>193</v>
+        <v>180</v>
       </c>
       <c r="F232" s="1" t="s">
         <v>55</v>
@@ -6181,19 +6181,19 @@
     </row>
     <row r="233" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A233" s="12" t="s">
-        <v>141</v>
+        <v>128</v>
       </c>
       <c r="B233" s="12">
         <v>6</v>
       </c>
       <c r="C233" s="12" t="s">
-        <v>205</v>
+        <v>192</v>
       </c>
       <c r="D233" s="9" t="s">
         <v>26</v>
       </c>
       <c r="E233" s="1" t="s">
-        <v>214</v>
+        <v>201</v>
       </c>
       <c r="F233" s="1" t="s">
         <v>55</v>
@@ -6201,19 +6201,19 @@
     </row>
     <row r="234" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A234" s="12" t="s">
-        <v>141</v>
+        <v>128</v>
       </c>
       <c r="B234" s="12">
         <v>6</v>
       </c>
       <c r="C234" s="12" t="s">
-        <v>226</v>
+        <v>213</v>
       </c>
       <c r="D234" s="9" t="s">
         <v>26</v>
       </c>
       <c r="E234" s="1" t="s">
-        <v>235</v>
+        <v>222</v>
       </c>
       <c r="F234" s="1" t="s">
         <v>55</v>
@@ -6221,19 +6221,19 @@
     </row>
     <row r="235" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A235" s="12" t="s">
-        <v>141</v>
+        <v>128</v>
       </c>
       <c r="B235" s="12">
         <v>6</v>
       </c>
       <c r="C235" s="12" t="s">
-        <v>247</v>
+        <v>234</v>
       </c>
       <c r="D235" s="9" t="s">
         <v>26</v>
       </c>
       <c r="E235" s="1" t="s">
-        <v>256</v>
+        <v>243</v>
       </c>
       <c r="F235" s="1" t="s">
         <v>55</v>
@@ -6241,19 +6241,19 @@
     </row>
     <row r="236" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A236" s="12" t="s">
-        <v>141</v>
+        <v>128</v>
       </c>
       <c r="B236" s="12">
         <v>6</v>
       </c>
       <c r="C236" s="12" t="s">
-        <v>142</v>
+        <v>129</v>
       </c>
       <c r="D236" s="9" t="s">
         <v>14</v>
       </c>
       <c r="E236" s="1" t="s">
-        <v>152</v>
+        <v>139</v>
       </c>
       <c r="F236" s="1" t="s">
         <v>55</v>
@@ -6261,19 +6261,19 @@
     </row>
     <row r="237" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A237" s="12" t="s">
-        <v>141</v>
+        <v>128</v>
       </c>
       <c r="B237" s="12">
         <v>6</v>
       </c>
       <c r="C237" s="12" t="s">
-        <v>163</v>
+        <v>150</v>
       </c>
       <c r="D237" s="9" t="s">
         <v>14</v>
       </c>
       <c r="E237" s="1" t="s">
-        <v>173</v>
+        <v>160</v>
       </c>
       <c r="F237" s="1" t="s">
         <v>55</v>
@@ -6281,19 +6281,19 @@
     </row>
     <row r="238" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A238" s="12" t="s">
-        <v>141</v>
+        <v>128</v>
       </c>
       <c r="B238" s="12">
         <v>6</v>
       </c>
       <c r="C238" s="12" t="s">
-        <v>184</v>
+        <v>171</v>
       </c>
       <c r="D238" s="9" t="s">
         <v>14</v>
       </c>
       <c r="E238" s="1" t="s">
-        <v>194</v>
+        <v>181</v>
       </c>
       <c r="F238" s="1" t="s">
         <v>55</v>
@@ -6301,19 +6301,19 @@
     </row>
     <row r="239" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A239" s="12" t="s">
-        <v>141</v>
+        <v>128</v>
       </c>
       <c r="B239" s="12">
         <v>6</v>
       </c>
       <c r="C239" s="12" t="s">
-        <v>205</v>
+        <v>192</v>
       </c>
       <c r="D239" s="9" t="s">
         <v>14</v>
       </c>
       <c r="E239" s="1" t="s">
-        <v>215</v>
+        <v>202</v>
       </c>
       <c r="F239" s="1" t="s">
         <v>55</v>
@@ -6321,19 +6321,19 @@
     </row>
     <row r="240" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A240" s="12" t="s">
-        <v>141</v>
+        <v>128</v>
       </c>
       <c r="B240" s="12">
         <v>6</v>
       </c>
       <c r="C240" s="12" t="s">
-        <v>226</v>
+        <v>213</v>
       </c>
       <c r="D240" s="9" t="s">
         <v>14</v>
       </c>
       <c r="E240" s="1" t="s">
-        <v>236</v>
+        <v>223</v>
       </c>
       <c r="F240" s="1" t="s">
         <v>55</v>
@@ -6341,19 +6341,19 @@
     </row>
     <row r="241" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A241" s="12" t="s">
-        <v>141</v>
+        <v>128</v>
       </c>
       <c r="B241" s="12">
         <v>6</v>
       </c>
       <c r="C241" s="12" t="s">
-        <v>247</v>
+        <v>234</v>
       </c>
       <c r="D241" s="9" t="s">
         <v>14</v>
       </c>
       <c r="E241" s="1" t="s">
-        <v>257</v>
+        <v>244</v>
       </c>
       <c r="F241" s="1" t="s">
         <v>55</v>
@@ -6361,19 +6361,19 @@
     </row>
     <row r="242" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A242" s="12" t="s">
-        <v>141</v>
+        <v>128</v>
       </c>
       <c r="B242" s="12">
         <v>6</v>
       </c>
       <c r="C242" s="12" t="s">
-        <v>142</v>
+        <v>129</v>
       </c>
       <c r="D242" s="9" t="s">
         <v>30</v>
       </c>
       <c r="E242" s="1" t="s">
-        <v>153</v>
+        <v>140</v>
       </c>
       <c r="F242" s="1" t="s">
         <v>55</v>
@@ -6381,19 +6381,19 @@
     </row>
     <row r="243" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A243" s="12" t="s">
-        <v>141</v>
+        <v>128</v>
       </c>
       <c r="B243" s="12">
         <v>6</v>
       </c>
       <c r="C243" s="12" t="s">
-        <v>163</v>
+        <v>150</v>
       </c>
       <c r="D243" s="9" t="s">
         <v>30</v>
       </c>
       <c r="E243" s="1" t="s">
-        <v>174</v>
+        <v>161</v>
       </c>
       <c r="F243" s="1" t="s">
         <v>55</v>
@@ -6401,19 +6401,19 @@
     </row>
     <row r="244" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A244" s="12" t="s">
-        <v>141</v>
+        <v>128</v>
       </c>
       <c r="B244" s="12">
         <v>6</v>
       </c>
       <c r="C244" s="12" t="s">
-        <v>184</v>
+        <v>171</v>
       </c>
       <c r="D244" s="9" t="s">
         <v>30</v>
       </c>
       <c r="E244" s="1" t="s">
-        <v>195</v>
+        <v>182</v>
       </c>
       <c r="F244" s="1" t="s">
         <v>55</v>
@@ -6421,19 +6421,19 @@
     </row>
     <row r="245" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A245" s="12" t="s">
-        <v>141</v>
+        <v>128</v>
       </c>
       <c r="B245" s="12">
         <v>6</v>
       </c>
       <c r="C245" s="12" t="s">
-        <v>205</v>
+        <v>192</v>
       </c>
       <c r="D245" s="9" t="s">
         <v>30</v>
       </c>
       <c r="E245" s="1" t="s">
-        <v>216</v>
+        <v>203</v>
       </c>
       <c r="F245" s="1" t="s">
         <v>55</v>
@@ -6441,19 +6441,19 @@
     </row>
     <row r="246" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A246" s="12" t="s">
-        <v>141</v>
+        <v>128</v>
       </c>
       <c r="B246" s="12">
         <v>6</v>
       </c>
       <c r="C246" s="12" t="s">
-        <v>226</v>
+        <v>213</v>
       </c>
       <c r="D246" s="9" t="s">
         <v>30</v>
       </c>
       <c r="E246" s="1" t="s">
-        <v>237</v>
+        <v>224</v>
       </c>
       <c r="F246" s="1" t="s">
         <v>55</v>
@@ -6461,19 +6461,19 @@
     </row>
     <row r="247" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A247" s="12" t="s">
-        <v>141</v>
+        <v>128</v>
       </c>
       <c r="B247" s="12">
         <v>6</v>
       </c>
       <c r="C247" s="12" t="s">
-        <v>247</v>
+        <v>234</v>
       </c>
       <c r="D247" s="9" t="s">
         <v>30</v>
       </c>
       <c r="E247" s="1" t="s">
-        <v>258</v>
+        <v>245</v>
       </c>
       <c r="F247" s="1" t="s">
         <v>55</v>
@@ -6481,19 +6481,19 @@
     </row>
     <row r="248" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A248" s="12" t="s">
-        <v>141</v>
+        <v>128</v>
       </c>
       <c r="B248" s="12">
         <v>6</v>
       </c>
       <c r="C248" s="12" t="s">
-        <v>142</v>
+        <v>129</v>
       </c>
       <c r="D248" s="9" t="s">
         <v>15</v>
       </c>
       <c r="E248" s="1" t="s">
-        <v>154</v>
+        <v>141</v>
       </c>
       <c r="F248" s="1" t="s">
         <v>55</v>
@@ -6501,19 +6501,19 @@
     </row>
     <row r="249" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A249" s="12" t="s">
-        <v>141</v>
+        <v>128</v>
       </c>
       <c r="B249" s="12">
         <v>6</v>
       </c>
       <c r="C249" s="12" t="s">
-        <v>163</v>
+        <v>150</v>
       </c>
       <c r="D249" s="9" t="s">
         <v>15</v>
       </c>
       <c r="E249" s="1" t="s">
-        <v>175</v>
+        <v>162</v>
       </c>
       <c r="F249" s="1" t="s">
         <v>55</v>
@@ -6521,19 +6521,19 @@
     </row>
     <row r="250" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A250" s="12" t="s">
-        <v>141</v>
+        <v>128</v>
       </c>
       <c r="B250" s="12">
         <v>6</v>
       </c>
       <c r="C250" s="12" t="s">
-        <v>184</v>
+        <v>171</v>
       </c>
       <c r="D250" s="9" t="s">
         <v>15</v>
       </c>
       <c r="E250" s="1" t="s">
-        <v>196</v>
+        <v>183</v>
       </c>
       <c r="F250" s="1" t="s">
         <v>55</v>
@@ -6541,19 +6541,19 @@
     </row>
     <row r="251" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A251" s="12" t="s">
-        <v>141</v>
+        <v>128</v>
       </c>
       <c r="B251" s="12">
         <v>6</v>
       </c>
       <c r="C251" s="12" t="s">
-        <v>205</v>
+        <v>192</v>
       </c>
       <c r="D251" s="9" t="s">
         <v>15</v>
       </c>
       <c r="E251" s="1" t="s">
-        <v>217</v>
+        <v>204</v>
       </c>
       <c r="F251" s="1" t="s">
         <v>55</v>
@@ -6561,19 +6561,19 @@
     </row>
     <row r="252" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A252" s="12" t="s">
-        <v>141</v>
+        <v>128</v>
       </c>
       <c r="B252" s="12">
         <v>6</v>
       </c>
       <c r="C252" s="12" t="s">
-        <v>226</v>
+        <v>213</v>
       </c>
       <c r="D252" s="9" t="s">
         <v>15</v>
       </c>
       <c r="E252" s="1" t="s">
-        <v>238</v>
+        <v>225</v>
       </c>
       <c r="F252" s="1" t="s">
         <v>55</v>
@@ -6581,19 +6581,19 @@
     </row>
     <row r="253" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A253" s="12" t="s">
-        <v>141</v>
+        <v>128</v>
       </c>
       <c r="B253" s="12">
         <v>6</v>
       </c>
       <c r="C253" s="12" t="s">
-        <v>247</v>
+        <v>234</v>
       </c>
       <c r="D253" s="9" t="s">
         <v>15</v>
       </c>
       <c r="E253" s="1" t="s">
-        <v>259</v>
+        <v>246</v>
       </c>
       <c r="F253" s="1" t="s">
         <v>55</v>
@@ -6601,19 +6601,19 @@
     </row>
     <row r="254" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A254" s="12" t="s">
-        <v>141</v>
+        <v>128</v>
       </c>
       <c r="B254" s="12">
         <v>6</v>
       </c>
       <c r="C254" s="12" t="s">
-        <v>142</v>
+        <v>129</v>
       </c>
       <c r="D254" s="9" t="s">
         <v>16</v>
       </c>
       <c r="E254" s="1" t="s">
-        <v>155</v>
+        <v>142</v>
       </c>
       <c r="F254" s="1" t="s">
         <v>55</v>
@@ -6621,19 +6621,19 @@
     </row>
     <row r="255" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A255" s="12" t="s">
-        <v>141</v>
+        <v>128</v>
       </c>
       <c r="B255" s="12">
         <v>6</v>
       </c>
       <c r="C255" s="12" t="s">
-        <v>163</v>
+        <v>150</v>
       </c>
       <c r="D255" s="9" t="s">
         <v>16</v>
       </c>
       <c r="E255" s="1" t="s">
-        <v>176</v>
+        <v>163</v>
       </c>
       <c r="F255" s="1" t="s">
         <v>55</v>
@@ -6641,19 +6641,19 @@
     </row>
     <row r="256" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A256" s="12" t="s">
-        <v>141</v>
+        <v>128</v>
       </c>
       <c r="B256" s="12">
         <v>6</v>
       </c>
       <c r="C256" s="12" t="s">
-        <v>184</v>
+        <v>171</v>
       </c>
       <c r="D256" s="9" t="s">
         <v>16</v>
       </c>
       <c r="E256" s="1" t="s">
-        <v>197</v>
+        <v>184</v>
       </c>
       <c r="F256" s="1" t="s">
         <v>55</v>
@@ -6661,19 +6661,19 @@
     </row>
     <row r="257" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A257" s="12" t="s">
-        <v>141</v>
+        <v>128</v>
       </c>
       <c r="B257" s="12">
         <v>6</v>
       </c>
       <c r="C257" s="12" t="s">
-        <v>205</v>
+        <v>192</v>
       </c>
       <c r="D257" s="9" t="s">
         <v>16</v>
       </c>
       <c r="E257" s="1" t="s">
-        <v>218</v>
+        <v>205</v>
       </c>
       <c r="F257" s="1" t="s">
         <v>55</v>
@@ -6681,19 +6681,19 @@
     </row>
     <row r="258" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A258" s="12" t="s">
-        <v>141</v>
+        <v>128</v>
       </c>
       <c r="B258" s="12">
         <v>6</v>
       </c>
       <c r="C258" s="12" t="s">
-        <v>226</v>
+        <v>213</v>
       </c>
       <c r="D258" s="9" t="s">
         <v>16</v>
       </c>
       <c r="E258" s="1" t="s">
-        <v>239</v>
+        <v>226</v>
       </c>
       <c r="F258" s="1" t="s">
         <v>55</v>
@@ -6701,19 +6701,19 @@
     </row>
     <row r="259" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A259" s="12" t="s">
-        <v>141</v>
+        <v>128</v>
       </c>
       <c r="B259" s="12">
         <v>6</v>
       </c>
       <c r="C259" s="12" t="s">
-        <v>247</v>
+        <v>234</v>
       </c>
       <c r="D259" s="9" t="s">
         <v>16</v>
       </c>
       <c r="E259" s="1" t="s">
-        <v>260</v>
+        <v>247</v>
       </c>
       <c r="F259" s="1" t="s">
         <v>55</v>
@@ -6721,19 +6721,19 @@
     </row>
     <row r="260" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A260" s="12" t="s">
-        <v>141</v>
+        <v>128</v>
       </c>
       <c r="B260" s="12">
         <v>6</v>
       </c>
       <c r="C260" s="12" t="s">
-        <v>142</v>
+        <v>129</v>
       </c>
       <c r="D260" s="9" t="s">
         <v>17</v>
       </c>
       <c r="E260" s="1" t="s">
-        <v>156</v>
+        <v>143</v>
       </c>
       <c r="F260" s="1" t="s">
         <v>55</v>
@@ -6741,19 +6741,19 @@
     </row>
     <row r="261" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A261" s="12" t="s">
-        <v>141</v>
+        <v>128</v>
       </c>
       <c r="B261" s="12">
         <v>6</v>
       </c>
       <c r="C261" s="12" t="s">
-        <v>163</v>
+        <v>150</v>
       </c>
       <c r="D261" s="9" t="s">
         <v>17</v>
       </c>
       <c r="E261" s="1" t="s">
-        <v>177</v>
+        <v>164</v>
       </c>
       <c r="F261" s="1" t="s">
         <v>55</v>
@@ -6761,19 +6761,19 @@
     </row>
     <row r="262" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A262" s="12" t="s">
-        <v>141</v>
+        <v>128</v>
       </c>
       <c r="B262" s="12">
         <v>6</v>
       </c>
       <c r="C262" s="12" t="s">
-        <v>184</v>
+        <v>171</v>
       </c>
       <c r="D262" s="9" t="s">
         <v>17</v>
       </c>
       <c r="E262" s="1" t="s">
-        <v>198</v>
+        <v>185</v>
       </c>
       <c r="F262" s="1" t="s">
         <v>55</v>
@@ -6781,19 +6781,19 @@
     </row>
     <row r="263" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A263" s="12" t="s">
-        <v>141</v>
+        <v>128</v>
       </c>
       <c r="B263" s="12">
         <v>6</v>
       </c>
       <c r="C263" s="12" t="s">
-        <v>205</v>
+        <v>192</v>
       </c>
       <c r="D263" s="9" t="s">
         <v>17</v>
       </c>
       <c r="E263" s="1" t="s">
-        <v>219</v>
+        <v>206</v>
       </c>
       <c r="F263" s="1" t="s">
         <v>55</v>
@@ -6801,19 +6801,19 @@
     </row>
     <row r="264" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A264" s="12" t="s">
-        <v>141</v>
+        <v>128</v>
       </c>
       <c r="B264" s="12">
         <v>6</v>
       </c>
       <c r="C264" s="12" t="s">
-        <v>226</v>
+        <v>213</v>
       </c>
       <c r="D264" s="9" t="s">
         <v>17</v>
       </c>
       <c r="E264" s="1" t="s">
-        <v>240</v>
+        <v>227</v>
       </c>
       <c r="F264" s="1" t="s">
         <v>55</v>
@@ -6821,19 +6821,19 @@
     </row>
     <row r="265" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A265" s="12" t="s">
-        <v>141</v>
+        <v>128</v>
       </c>
       <c r="B265" s="12">
         <v>6</v>
       </c>
       <c r="C265" s="12" t="s">
-        <v>247</v>
+        <v>234</v>
       </c>
       <c r="D265" s="9" t="s">
         <v>17</v>
       </c>
       <c r="E265" s="1" t="s">
-        <v>261</v>
+        <v>248</v>
       </c>
       <c r="F265" s="1" t="s">
         <v>55</v>
@@ -6841,19 +6841,19 @@
     </row>
     <row r="266" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A266" s="12" t="s">
-        <v>141</v>
+        <v>128</v>
       </c>
       <c r="B266" s="12">
         <v>6</v>
       </c>
       <c r="C266" s="12" t="s">
-        <v>142</v>
+        <v>129</v>
       </c>
       <c r="D266" s="9" t="s">
         <v>29</v>
       </c>
       <c r="E266" s="1" t="s">
-        <v>157</v>
+        <v>144</v>
       </c>
       <c r="F266" s="1" t="s">
         <v>55</v>
@@ -6861,19 +6861,19 @@
     </row>
     <row r="267" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A267" s="12" t="s">
-        <v>141</v>
+        <v>128</v>
       </c>
       <c r="B267" s="12">
         <v>6</v>
       </c>
       <c r="C267" s="12" t="s">
-        <v>163</v>
+        <v>150</v>
       </c>
       <c r="D267" s="9" t="s">
         <v>29</v>
       </c>
       <c r="E267" s="1" t="s">
-        <v>178</v>
+        <v>165</v>
       </c>
       <c r="F267" s="1" t="s">
         <v>55</v>
@@ -6881,19 +6881,19 @@
     </row>
     <row r="268" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A268" s="12" t="s">
-        <v>141</v>
+        <v>128</v>
       </c>
       <c r="B268" s="12">
         <v>6</v>
       </c>
       <c r="C268" s="12" t="s">
-        <v>184</v>
+        <v>171</v>
       </c>
       <c r="D268" s="9" t="s">
         <v>29</v>
       </c>
       <c r="E268" s="1" t="s">
-        <v>199</v>
+        <v>186</v>
       </c>
       <c r="F268" s="1" t="s">
         <v>55</v>
@@ -6901,19 +6901,19 @@
     </row>
     <row r="269" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A269" s="12" t="s">
-        <v>141</v>
+        <v>128</v>
       </c>
       <c r="B269" s="12">
         <v>6</v>
       </c>
       <c r="C269" s="12" t="s">
-        <v>205</v>
+        <v>192</v>
       </c>
       <c r="D269" s="9" t="s">
         <v>29</v>
       </c>
       <c r="E269" s="1" t="s">
-        <v>220</v>
+        <v>207</v>
       </c>
       <c r="F269" s="1" t="s">
         <v>55</v>
@@ -6921,19 +6921,19 @@
     </row>
     <row r="270" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A270" s="12" t="s">
-        <v>141</v>
+        <v>128</v>
       </c>
       <c r="B270" s="12">
         <v>6</v>
       </c>
       <c r="C270" s="12" t="s">
-        <v>226</v>
+        <v>213</v>
       </c>
       <c r="D270" s="9" t="s">
         <v>29</v>
       </c>
       <c r="E270" s="1" t="s">
-        <v>241</v>
+        <v>228</v>
       </c>
       <c r="F270" s="1" t="s">
         <v>55</v>
@@ -6941,19 +6941,19 @@
     </row>
     <row r="271" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A271" s="12" t="s">
-        <v>141</v>
+        <v>128</v>
       </c>
       <c r="B271" s="12">
         <v>6</v>
       </c>
       <c r="C271" s="12" t="s">
-        <v>247</v>
+        <v>234</v>
       </c>
       <c r="D271" s="9" t="s">
         <v>29</v>
       </c>
       <c r="E271" s="1" t="s">
-        <v>262</v>
+        <v>249</v>
       </c>
       <c r="F271" s="1" t="s">
         <v>55</v>
@@ -6961,19 +6961,19 @@
     </row>
     <row r="272" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A272" s="12" t="s">
-        <v>141</v>
+        <v>128</v>
       </c>
       <c r="B272" s="12">
         <v>6</v>
       </c>
       <c r="C272" s="12" t="s">
-        <v>142</v>
+        <v>129</v>
       </c>
       <c r="D272" s="9" t="s">
         <v>18</v>
       </c>
       <c r="E272" s="1" t="s">
-        <v>158</v>
+        <v>145</v>
       </c>
       <c r="F272" s="1" t="s">
         <v>55</v>
@@ -6981,19 +6981,19 @@
     </row>
     <row r="273" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A273" s="12" t="s">
-        <v>141</v>
+        <v>128</v>
       </c>
       <c r="B273" s="12">
         <v>6</v>
       </c>
       <c r="C273" s="12" t="s">
-        <v>163</v>
+        <v>150</v>
       </c>
       <c r="D273" s="9" t="s">
         <v>18</v>
       </c>
       <c r="E273" s="1" t="s">
-        <v>179</v>
+        <v>166</v>
       </c>
       <c r="F273" s="1" t="s">
         <v>55</v>
@@ -7001,19 +7001,19 @@
     </row>
     <row r="274" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A274" s="12" t="s">
-        <v>141</v>
+        <v>128</v>
       </c>
       <c r="B274" s="12">
         <v>6</v>
       </c>
       <c r="C274" s="12" t="s">
-        <v>184</v>
+        <v>171</v>
       </c>
       <c r="D274" s="9" t="s">
         <v>18</v>
       </c>
       <c r="E274" s="1" t="s">
-        <v>200</v>
+        <v>187</v>
       </c>
       <c r="F274" s="1" t="s">
         <v>55</v>
@@ -7021,19 +7021,19 @@
     </row>
     <row r="275" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A275" s="12" t="s">
-        <v>141</v>
+        <v>128</v>
       </c>
       <c r="B275" s="12">
         <v>6</v>
       </c>
       <c r="C275" s="12" t="s">
-        <v>205</v>
+        <v>192</v>
       </c>
       <c r="D275" s="9" t="s">
         <v>18</v>
       </c>
       <c r="E275" s="1" t="s">
-        <v>221</v>
+        <v>208</v>
       </c>
       <c r="F275" s="1" t="s">
         <v>55</v>
@@ -7041,19 +7041,19 @@
     </row>
     <row r="276" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A276" s="12" t="s">
-        <v>141</v>
+        <v>128</v>
       </c>
       <c r="B276" s="12">
         <v>6</v>
       </c>
       <c r="C276" s="12" t="s">
-        <v>226</v>
+        <v>213</v>
       </c>
       <c r="D276" s="9" t="s">
         <v>18</v>
       </c>
       <c r="E276" s="1" t="s">
-        <v>242</v>
+        <v>229</v>
       </c>
       <c r="F276" s="1" t="s">
         <v>55</v>
@@ -7061,19 +7061,19 @@
     </row>
     <row r="277" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A277" s="12" t="s">
-        <v>141</v>
+        <v>128</v>
       </c>
       <c r="B277" s="12">
         <v>6</v>
       </c>
       <c r="C277" s="12" t="s">
-        <v>247</v>
+        <v>234</v>
       </c>
       <c r="D277" s="9" t="s">
         <v>18</v>
       </c>
       <c r="E277" s="1" t="s">
-        <v>263</v>
+        <v>250</v>
       </c>
       <c r="F277" s="1" t="s">
         <v>55</v>
@@ -7081,19 +7081,19 @@
     </row>
     <row r="278" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A278" s="12" t="s">
-        <v>141</v>
+        <v>128</v>
       </c>
       <c r="B278" s="12">
         <v>6</v>
       </c>
       <c r="C278" s="12" t="s">
-        <v>142</v>
+        <v>129</v>
       </c>
       <c r="D278" s="9" t="s">
         <v>20</v>
       </c>
       <c r="E278" s="1" t="s">
-        <v>159</v>
+        <v>146</v>
       </c>
       <c r="F278" s="1" t="s">
         <v>55</v>
@@ -7101,19 +7101,19 @@
     </row>
     <row r="279" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A279" s="12" t="s">
-        <v>141</v>
+        <v>128</v>
       </c>
       <c r="B279" s="12">
         <v>6</v>
       </c>
       <c r="C279" s="12" t="s">
-        <v>163</v>
+        <v>150</v>
       </c>
       <c r="D279" s="9" t="s">
         <v>20</v>
       </c>
       <c r="E279" s="1" t="s">
-        <v>180</v>
+        <v>167</v>
       </c>
       <c r="F279" s="1" t="s">
         <v>55</v>
@@ -7121,19 +7121,19 @@
     </row>
     <row r="280" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A280" s="12" t="s">
-        <v>141</v>
+        <v>128</v>
       </c>
       <c r="B280" s="12">
         <v>6</v>
       </c>
       <c r="C280" s="12" t="s">
-        <v>184</v>
+        <v>171</v>
       </c>
       <c r="D280" s="9" t="s">
         <v>20</v>
       </c>
       <c r="E280" s="1" t="s">
-        <v>201</v>
+        <v>188</v>
       </c>
       <c r="F280" s="1" t="s">
         <v>55</v>
@@ -7141,19 +7141,19 @@
     </row>
     <row r="281" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A281" s="12" t="s">
-        <v>141</v>
+        <v>128</v>
       </c>
       <c r="B281" s="12">
         <v>6</v>
       </c>
       <c r="C281" s="12" t="s">
-        <v>205</v>
+        <v>192</v>
       </c>
       <c r="D281" s="9" t="s">
         <v>20</v>
       </c>
       <c r="E281" s="1" t="s">
-        <v>222</v>
+        <v>209</v>
       </c>
       <c r="F281" s="1" t="s">
         <v>55</v>
@@ -7161,19 +7161,19 @@
     </row>
     <row r="282" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A282" s="12" t="s">
-        <v>141</v>
+        <v>128</v>
       </c>
       <c r="B282" s="12">
         <v>6</v>
       </c>
       <c r="C282" s="12" t="s">
-        <v>226</v>
+        <v>213</v>
       </c>
       <c r="D282" s="9" t="s">
         <v>20</v>
       </c>
       <c r="E282" s="1" t="s">
-        <v>243</v>
+        <v>230</v>
       </c>
       <c r="F282" s="1" t="s">
         <v>55</v>
@@ -7181,19 +7181,19 @@
     </row>
     <row r="283" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A283" s="12" t="s">
-        <v>141</v>
+        <v>128</v>
       </c>
       <c r="B283" s="12">
         <v>6</v>
       </c>
       <c r="C283" s="12" t="s">
-        <v>247</v>
+        <v>234</v>
       </c>
       <c r="D283" s="9" t="s">
         <v>20</v>
       </c>
       <c r="E283" s="1" t="s">
-        <v>264</v>
+        <v>251</v>
       </c>
       <c r="F283" s="1" t="s">
         <v>55</v>
@@ -7201,19 +7201,19 @@
     </row>
     <row r="284" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A284" s="12" t="s">
-        <v>141</v>
+        <v>128</v>
       </c>
       <c r="B284" s="12">
         <v>6</v>
       </c>
       <c r="C284" s="12" t="s">
-        <v>142</v>
+        <v>129</v>
       </c>
       <c r="D284" s="9" t="s">
         <v>24</v>
       </c>
       <c r="E284" s="1" t="s">
-        <v>160</v>
+        <v>147</v>
       </c>
       <c r="F284" s="1" t="s">
         <v>55</v>
@@ -7221,19 +7221,19 @@
     </row>
     <row r="285" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A285" s="12" t="s">
-        <v>141</v>
+        <v>128</v>
       </c>
       <c r="B285" s="12">
         <v>6</v>
       </c>
       <c r="C285" s="12" t="s">
-        <v>163</v>
+        <v>150</v>
       </c>
       <c r="D285" s="9" t="s">
         <v>24</v>
       </c>
       <c r="E285" s="1" t="s">
-        <v>181</v>
+        <v>168</v>
       </c>
       <c r="F285" s="1" t="s">
         <v>55</v>
@@ -7241,19 +7241,19 @@
     </row>
     <row r="286" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A286" s="12" t="s">
-        <v>141</v>
+        <v>128</v>
       </c>
       <c r="B286" s="12">
         <v>6</v>
       </c>
       <c r="C286" s="12" t="s">
-        <v>184</v>
+        <v>171</v>
       </c>
       <c r="D286" s="9" t="s">
         <v>24</v>
       </c>
       <c r="E286" s="1" t="s">
-        <v>202</v>
+        <v>189</v>
       </c>
       <c r="F286" s="1" t="s">
         <v>55</v>
@@ -7261,19 +7261,19 @@
     </row>
     <row r="287" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A287" s="12" t="s">
-        <v>141</v>
+        <v>128</v>
       </c>
       <c r="B287" s="12">
         <v>6</v>
       </c>
       <c r="C287" s="12" t="s">
-        <v>205</v>
+        <v>192</v>
       </c>
       <c r="D287" s="9" t="s">
         <v>24</v>
       </c>
       <c r="E287" s="1" t="s">
-        <v>223</v>
+        <v>210</v>
       </c>
       <c r="F287" s="1" t="s">
         <v>55</v>
@@ -7281,19 +7281,19 @@
     </row>
     <row r="288" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A288" s="12" t="s">
-        <v>141</v>
+        <v>128</v>
       </c>
       <c r="B288" s="12">
         <v>6</v>
       </c>
       <c r="C288" s="12" t="s">
-        <v>226</v>
+        <v>213</v>
       </c>
       <c r="D288" s="9" t="s">
         <v>24</v>
       </c>
       <c r="E288" s="1" t="s">
-        <v>244</v>
+        <v>231</v>
       </c>
       <c r="F288" s="1" t="s">
         <v>55</v>
@@ -7301,19 +7301,19 @@
     </row>
     <row r="289" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A289" s="12" t="s">
-        <v>141</v>
+        <v>128</v>
       </c>
       <c r="B289" s="12">
         <v>6</v>
       </c>
       <c r="C289" s="12" t="s">
-        <v>247</v>
+        <v>234</v>
       </c>
       <c r="D289" s="9" t="s">
         <v>24</v>
       </c>
       <c r="E289" s="1" t="s">
-        <v>265</v>
+        <v>252</v>
       </c>
       <c r="F289" s="1" t="s">
         <v>55</v>
@@ -7321,19 +7321,19 @@
     </row>
     <row r="290" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A290" s="12" t="s">
-        <v>141</v>
+        <v>128</v>
       </c>
       <c r="B290" s="12">
         <v>6</v>
       </c>
       <c r="C290" s="12" t="s">
-        <v>142</v>
+        <v>129</v>
       </c>
       <c r="D290" s="9" t="s">
         <v>7</v>
       </c>
       <c r="E290" s="1" t="s">
-        <v>161</v>
+        <v>148</v>
       </c>
       <c r="F290" s="1" t="s">
         <v>55</v>
@@ -7341,19 +7341,19 @@
     </row>
     <row r="291" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A291" s="12" t="s">
-        <v>141</v>
+        <v>128</v>
       </c>
       <c r="B291" s="12">
         <v>6</v>
       </c>
       <c r="C291" s="12" t="s">
-        <v>163</v>
+        <v>150</v>
       </c>
       <c r="D291" s="9" t="s">
         <v>7</v>
       </c>
       <c r="E291" s="1" t="s">
-        <v>182</v>
+        <v>169</v>
       </c>
       <c r="F291" s="1" t="s">
         <v>55</v>
@@ -7361,19 +7361,19 @@
     </row>
     <row r="292" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A292" s="12" t="s">
-        <v>141</v>
+        <v>128</v>
       </c>
       <c r="B292" s="12">
         <v>6</v>
       </c>
       <c r="C292" s="12" t="s">
-        <v>184</v>
+        <v>171</v>
       </c>
       <c r="D292" s="9" t="s">
         <v>7</v>
       </c>
       <c r="E292" s="1" t="s">
-        <v>203</v>
+        <v>190</v>
       </c>
       <c r="F292" s="1" t="s">
         <v>55</v>
@@ -7381,19 +7381,19 @@
     </row>
     <row r="293" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A293" s="12" t="s">
-        <v>141</v>
+        <v>128</v>
       </c>
       <c r="B293" s="12">
         <v>6</v>
       </c>
       <c r="C293" s="12" t="s">
-        <v>205</v>
+        <v>192</v>
       </c>
       <c r="D293" s="9" t="s">
         <v>7</v>
       </c>
       <c r="E293" s="1" t="s">
-        <v>224</v>
+        <v>211</v>
       </c>
       <c r="F293" s="1" t="s">
         <v>55</v>
@@ -7401,19 +7401,19 @@
     </row>
     <row r="294" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A294" s="12" t="s">
-        <v>141</v>
+        <v>128</v>
       </c>
       <c r="B294" s="12">
         <v>6</v>
       </c>
       <c r="C294" s="12" t="s">
-        <v>226</v>
+        <v>213</v>
       </c>
       <c r="D294" s="9" t="s">
         <v>7</v>
       </c>
       <c r="E294" s="1" t="s">
-        <v>245</v>
+        <v>232</v>
       </c>
       <c r="F294" s="1" t="s">
         <v>55</v>
@@ -7421,19 +7421,19 @@
     </row>
     <row r="295" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A295" s="12" t="s">
-        <v>141</v>
+        <v>128</v>
       </c>
       <c r="B295" s="12">
         <v>6</v>
       </c>
       <c r="C295" s="12" t="s">
-        <v>247</v>
+        <v>234</v>
       </c>
       <c r="D295" s="9" t="s">
         <v>7</v>
       </c>
       <c r="E295" s="1" t="s">
-        <v>266</v>
+        <v>253</v>
       </c>
       <c r="F295" s="1" t="s">
         <v>55</v>
@@ -7441,19 +7441,19 @@
     </row>
     <row r="296" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A296" s="12" t="s">
-        <v>141</v>
+        <v>128</v>
       </c>
       <c r="B296" s="12">
         <v>6</v>
       </c>
       <c r="C296" s="12" t="s">
-        <v>142</v>
+        <v>129</v>
       </c>
       <c r="D296" s="9" t="s">
         <v>9</v>
       </c>
       <c r="E296" s="1" t="s">
-        <v>162</v>
+        <v>149</v>
       </c>
       <c r="F296" s="1" t="s">
         <v>55</v>
@@ -7461,19 +7461,19 @@
     </row>
     <row r="297" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A297" s="12" t="s">
-        <v>141</v>
+        <v>128</v>
       </c>
       <c r="B297" s="12">
         <v>6</v>
       </c>
       <c r="C297" s="12" t="s">
-        <v>163</v>
+        <v>150</v>
       </c>
       <c r="D297" s="9" t="s">
         <v>9</v>
       </c>
       <c r="E297" s="1" t="s">
-        <v>183</v>
+        <v>170</v>
       </c>
       <c r="F297" s="1" t="s">
         <v>55</v>
@@ -7481,19 +7481,19 @@
     </row>
     <row r="298" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A298" s="12" t="s">
-        <v>141</v>
+        <v>128</v>
       </c>
       <c r="B298" s="12">
         <v>6</v>
       </c>
       <c r="C298" s="12" t="s">
-        <v>184</v>
+        <v>171</v>
       </c>
       <c r="D298" s="9" t="s">
         <v>9</v>
       </c>
       <c r="E298" s="1" t="s">
-        <v>204</v>
+        <v>191</v>
       </c>
       <c r="F298" s="1" t="s">
         <v>55</v>
@@ -7501,19 +7501,19 @@
     </row>
     <row r="299" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A299" s="12" t="s">
-        <v>141</v>
+        <v>128</v>
       </c>
       <c r="B299" s="12">
         <v>6</v>
       </c>
       <c r="C299" s="12" t="s">
-        <v>205</v>
+        <v>192</v>
       </c>
       <c r="D299" s="9" t="s">
         <v>9</v>
       </c>
       <c r="E299" s="1" t="s">
-        <v>225</v>
+        <v>212</v>
       </c>
       <c r="F299" s="1" t="s">
         <v>55</v>
@@ -7521,19 +7521,19 @@
     </row>
     <row r="300" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A300" s="12" t="s">
-        <v>141</v>
+        <v>128</v>
       </c>
       <c r="B300" s="12">
         <v>6</v>
       </c>
       <c r="C300" s="12" t="s">
-        <v>226</v>
+        <v>213</v>
       </c>
       <c r="D300" s="9" t="s">
         <v>9</v>
       </c>
       <c r="E300" s="1" t="s">
-        <v>246</v>
+        <v>233</v>
       </c>
       <c r="F300" s="1" t="s">
         <v>55</v>
@@ -7541,19 +7541,19 @@
     </row>
     <row r="301" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A301" s="12" t="s">
-        <v>141</v>
+        <v>128</v>
       </c>
       <c r="B301" s="12">
         <v>6</v>
       </c>
       <c r="C301" s="12" t="s">
-        <v>247</v>
+        <v>234</v>
       </c>
       <c r="D301" s="9" t="s">
         <v>9</v>
       </c>
       <c r="E301" s="1" t="s">
-        <v>267</v>
+        <v>254</v>
       </c>
       <c r="F301" s="1" t="s">
         <v>55</v>

</xml_diff>

<commit_message>
Diversify US related to "Cardiology" domain
</commit_message>
<xml_diff>
--- a/refair-server/datasets/few shot dataset/FSDataset.xlsx
+++ b/refair-server/datasets/few shot dataset/FSDataset.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\morel\Desktop\Refair\ReFair-App\refair-server\datasets\few shot dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA9E0681-AFC1-4B9E-BC32-359C80B205A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18AA64A4-875B-4522-8EDD-9B4AE5BF19D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5760" yWindow="0" windowWidth="17280" windowHeight="8880" xr2:uid="{80773445-FB61-4F04-A882-1600FD96C55A}"/>
+    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{80773445-FB61-4F04-A882-1600FD96C55A}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -431,36 +431,6 @@
     <t>As a cardiologist, I want to apply adversarial learning techniques to detect and mitigate potential adversarial attacks on ECG data classifiers, ensuring the reliability and robustness of heart abnormality diagnoses.</t>
   </si>
   <si>
-    <t>As a cardiologist, I want to explore CNN-based techniques for real-time analysis of wearable device data, such as continuous heart rate monitoring, to detect anomalies and provide timely alerts for patients with underlying cardiac conditions.</t>
-  </si>
-  <si>
-    <t>As a cardiologist, I want to integrate a conversational agent into electronic health records (EHR) systems, enabling patients to easily access and update their medical histories and symptoms, facilitating more efficient and accurate clinical assessments.</t>
-  </si>
-  <si>
-    <t>As a cardiologist, I want to construct decision tree models using patient demographics and medical history to predict the likelihood of adverse cardiac events within the next five years, aiding in early intervention and risk management strategies.</t>
-  </si>
-  <si>
-    <t>As a cardiologist, I want to develop a document classification system to classify electronic health records (EHRs) based on patient symptoms and diagnostic tests, aiding in the identification of patterns and trends in cardiovascular diseases.</t>
-  </si>
-  <si>
-    <t>As a cardiologist, I want to develop an entity extraction system to automatically identify and extract key cardiac parameters (e.g., ejection fraction, QT interval) from clinical notes and reports, enabling faster analysis and decision-making.</t>
-  </si>
-  <si>
-    <t>As a cardiologist, I want to apply feature selection methods to filter out irrelevant or redundant features from ECG data, so that I can enhance the performance of algorithms detecting cardiac arrhythmias.</t>
-  </si>
-  <si>
-    <t>As a cardiologist, I want to use keyword extraction algorithms to extract relevant terms from medical literature and clinical guidelines pertaining to cardiac rehabilitation protocols, aiding in the development of evidence-based treatment plans.</t>
-  </si>
-  <si>
-    <t>As a cardiologist, I want to address class imbalance in datasets used for predicting rare cardiac conditions using machine learning algorithms, ensuring accurate identification and early intervention for patients at higher risk.</t>
-  </si>
-  <si>
-    <t>As a cardiologist, I want to use k-NN models to predict patient-specific responses to different cardiac medications based on similar patient profiles, facilitating personalized treatment plans for heart disease management.</t>
-  </si>
-  <si>
-    <t>As a cardiologist, I want to implement multi-label classification algorithms to classify cardiac imaging studies (e.g., echocardiograms, CT scans) into multiple diagnostic categories (e.g., valve disease, myocardial infarction), aiding in accurate disease characterization.</t>
-  </si>
-  <si>
     <t>As a cardiologist, I want to develop a neural network-based system to predict the progression of heart failure in patients based on dynamic changes in biomarkers and clinical indicators, guiding timely interventions and patient monitoring.</t>
   </si>
   <si>
@@ -470,24 +440,9 @@
     <t>As a cardiologist, I want to develop a semantic similarity model to compare clinical notes and identify similar cases of coronary artery disease, aiding in pattern recognition and treatment planning.</t>
   </si>
   <si>
-    <t>As a cardiologist, I want to implement sentiment analysis on patient feedback from cardiac rehabilitation programs to assess overall patient satisfaction and identify areas for program improvement.</t>
-  </si>
-  <si>
-    <t>As a cardiologist, I want to develop a speech to text system to transcribe cardiology consultations and patient histories accurately, improving documentation efficiency and clinical workflow.</t>
-  </si>
-  <si>
-    <t>As a cardiologist, I want to develop a text categorization model to classify medical literature and research articles on various cardiac conditions (e.g., myocardial infarction, arrhythmias) for easier access and knowledge synthesis.</t>
-  </si>
-  <si>
     <t>As a cardiologist, I want to apply unsupervised clustering algorithms to group patients based on similar risk factor profiles (e.g., smoking history, cholesterol levels), enabling targeted preventive interventions for cardiovascular diseases.</t>
   </si>
   <si>
-    <t>As a cardiologist, I want to develop a voice recognition system to accurately transcribe cardiology consultations and patient histories from audio recordings, improving documentation accuracy and efficiency.</t>
-  </si>
-  <si>
-    <t>As a cardiologist, I want to utilize word embedding techniques to represent clinical terms and medical concepts from cardiology literature, enabling more accurate semantic understanding and retrieval of relevant research findings.</t>
-  </si>
-  <si>
     <t>Dermatology</t>
   </si>
   <si>
@@ -1077,6 +1032,51 @@
   </si>
   <si>
     <t>As a financial planner, I want to employ word embedding algorithms to cluster client financial goals and preferences based on their articulated needs and aspirations, facilitating personalized financial planning advice and strategies.</t>
+  </si>
+  <si>
+    <t>As a cardiovascular surgeon, I want voice recognition capabilities to dictate operative notes during complex procedures, so that I can ensure accurate documentation of surgical techniques and outcomes.</t>
+  </si>
+  <si>
+    <t>As a cardiology educator, I want word embedding models to map out semantic relationships between cardiovascular terms, so that I can create more effective teaching materials and curriculum.</t>
+  </si>
+  <si>
+    <t>As a cardiovascular surgeon, I want to use CNN-based segmentation algorithms to precisely delineate coronary arteries from angiography images, so that I can plan and perform interventions with greater accuracy.</t>
+  </si>
+  <si>
+    <t>As a cardiac nurse, I want a conversational agent to provide patients with post-discharge care instructions and reminders, so that I can ensure they follow their treatment plans and improve recovery outcomes.</t>
+  </si>
+  <si>
+    <t>As a cardiology department head, I want to utilize decision trees to analyze operational data and optimize resource allocation, so that I can improve the efficiency and quality of care provided by my department.</t>
+  </si>
+  <si>
+    <t>As a cardiology department head, I want to employ document classification algorithms to classify procedural guidelines and clinical protocols into different categories (e.g., diagnostic procedures, treatment algorithms), so that I can ensure consistent and standardized practices across the department.</t>
+  </si>
+  <si>
+    <t>As a cardiology clinician, I want to use entity extraction algorithms to identify and extract mentions of cardiac conditions (e.g., heart failure, atrial fibrillation) from patient notes and reports, so that I can prioritize care for patients with complex cardiovascular issues.</t>
+  </si>
+  <si>
+    <t>As a cardiology researcher, I want to use feature selection algorithms to identify the most relevant clinical variables (e.g., age, cholesterol levels, blood pressure) from large datasets of patient records, so that I can build accurate predictive models for cardiovascular risk assessment.</t>
+  </si>
+  <si>
+    <t>As a cardiology researcher, I want to address class imbalance in datasets related to rare cardiac diseases (e.g., myocarditis, pericardial effusion) using oversampling techniques, so that I can build robust predictive models and improve early detection strategies.</t>
+  </si>
+  <si>
+    <t>As a cardiologist, I want to use k-nearest neighbor (k-NN) algorithms to predict patient outcomes based on similar cases with known treatment responses, so that I can personalize treatment plans for my patients.</t>
+  </si>
+  <si>
+    <t>As a cardiology researcher, I want to develop a keyword extraction system to automatically identify key terms related to heart failure from a large corpus of clinical literature, so that I can conduct comprehensive literature reviews efficiently.</t>
+  </si>
+  <si>
+    <t>As a cardiology researcher, I want to develop a multi-label classification model to predict multiple comorbidities (e.g., diabetes, hypertension, obesity) in cardiac patients based on their clinical profiles, so that I can tailor personalized treatment plans.</t>
+  </si>
+  <si>
+    <t>As a cardiac rehabilitation specialist, I want to use sentiment analysis to evaluate patients' emotional responses in their progress notes, so that I can provide tailored support and interventions to improve their rehabilitation experience.</t>
+  </si>
+  <si>
+    <t>As a cardiac rehabilitation specialist, I want to implement speech-to-text technology to record patients' verbal feedback during rehabilitation sessions, so that I can efficiently capture and analyze their progress and concerns.</t>
+  </si>
+  <si>
+    <t>As a cardiology clinic manager, I want to use text categorization to automatically sort incoming emails and messages from patients and other healthcare providers into categories like appointment requests, medication inquiries, and general questions, so that I can streamline communication and improve response times.</t>
   </si>
 </sst>
 </file>
@@ -1526,8 +1526,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8DF0B04-8323-4309-B759-D1CDDA1FBB0E}">
   <dimension ref="A1:F301"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C38" sqref="C38"/>
+    <sheetView tabSelected="1" topLeftCell="C161" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C183" sqref="C183"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1613,7 +1613,7 @@
         <v>32</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>334</v>
+        <v>319</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>55</v>
@@ -1673,7 +1673,7 @@
         <v>23</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>325</v>
+        <v>310</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>55</v>
@@ -1693,7 +1693,7 @@
         <v>12</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>335</v>
+        <v>320</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>55</v>
@@ -1713,7 +1713,7 @@
         <v>12</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>326</v>
+        <v>311</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>55</v>
@@ -1733,7 +1733,7 @@
         <v>33</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>336</v>
+        <v>321</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>55</v>
@@ -1753,7 +1753,7 @@
         <v>33</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>327</v>
+        <v>312</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>55</v>
@@ -1773,7 +1773,7 @@
         <v>25</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>337</v>
+        <v>322</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>55</v>
@@ -1813,7 +1813,7 @@
         <v>28</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>338</v>
+        <v>323</v>
       </c>
       <c r="F14" s="1" t="s">
         <v>55</v>
@@ -1833,7 +1833,7 @@
         <v>28</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>328</v>
+        <v>313</v>
       </c>
       <c r="F15" s="1" t="s">
         <v>55</v>
@@ -1933,7 +1933,7 @@
         <v>14</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>339</v>
+        <v>324</v>
       </c>
       <c r="F20" s="1" t="s">
         <v>55</v>
@@ -1953,7 +1953,7 @@
         <v>14</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>329</v>
+        <v>314</v>
       </c>
       <c r="F21" s="1" t="s">
         <v>55</v>
@@ -1973,7 +1973,7 @@
         <v>30</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>340</v>
+        <v>325</v>
       </c>
       <c r="F22" s="1" t="s">
         <v>55</v>
@@ -1993,7 +1993,7 @@
         <v>30</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>330</v>
+        <v>315</v>
       </c>
       <c r="F23" s="1" t="s">
         <v>55</v>
@@ -2093,7 +2093,7 @@
         <v>17</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>341</v>
+        <v>326</v>
       </c>
       <c r="F28" s="1" t="s">
         <v>55</v>
@@ -2133,7 +2133,7 @@
         <v>29</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>342</v>
+        <v>327</v>
       </c>
       <c r="F30" s="1" t="s">
         <v>55</v>
@@ -2193,7 +2193,7 @@
         <v>18</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>331</v>
+        <v>316</v>
       </c>
       <c r="F33" s="1" t="s">
         <v>55</v>
@@ -2213,7 +2213,7 @@
         <v>20</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>343</v>
+        <v>328</v>
       </c>
       <c r="F34" s="1" t="s">
         <v>55</v>
@@ -2253,7 +2253,7 @@
         <v>24</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>344</v>
+        <v>329</v>
       </c>
       <c r="F36" s="1" t="s">
         <v>55</v>
@@ -2273,7 +2273,7 @@
         <v>24</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>332</v>
+        <v>317</v>
       </c>
       <c r="F37" s="1" t="s">
         <v>55</v>
@@ -2293,7 +2293,7 @@
         <v>7</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>345</v>
+        <v>330</v>
       </c>
       <c r="F38" s="1" t="s">
         <v>55</v>
@@ -2333,7 +2333,7 @@
         <v>9</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>346</v>
+        <v>331</v>
       </c>
       <c r="F40" s="1" t="s">
         <v>55</v>
@@ -2353,7 +2353,7 @@
         <v>9</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>333</v>
+        <v>318</v>
       </c>
       <c r="F41" s="1" t="s">
         <v>55</v>
@@ -2513,7 +2513,7 @@
         <v>12</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>318</v>
+        <v>303</v>
       </c>
       <c r="F49" s="1" t="s">
         <v>55</v>
@@ -2553,7 +2553,7 @@
         <v>33</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>319</v>
+        <v>304</v>
       </c>
       <c r="F51" s="1" t="s">
         <v>55</v>
@@ -2633,7 +2633,7 @@
         <v>28</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>320</v>
+        <v>305</v>
       </c>
       <c r="F55" s="1" t="s">
         <v>55</v>
@@ -2713,7 +2713,7 @@
         <v>26</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>321</v>
+        <v>306</v>
       </c>
       <c r="F59" s="1" t="s">
         <v>55</v>
@@ -2833,7 +2833,7 @@
         <v>15</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>322</v>
+        <v>307</v>
       </c>
       <c r="F65" s="1" t="s">
         <v>55</v>
@@ -2913,7 +2913,7 @@
         <v>17</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>323</v>
+        <v>308</v>
       </c>
       <c r="F69" s="1" t="s">
         <v>55</v>
@@ -3073,7 +3073,7 @@
         <v>24</v>
       </c>
       <c r="E77" s="1" t="s">
-        <v>324</v>
+        <v>309</v>
       </c>
       <c r="F77" s="1" t="s">
         <v>55</v>
@@ -3173,7 +3173,7 @@
         <v>22</v>
       </c>
       <c r="E82" s="1" t="s">
-        <v>301</v>
+        <v>286</v>
       </c>
       <c r="F82" s="1" t="s">
         <v>55</v>
@@ -3193,7 +3193,7 @@
         <v>22</v>
       </c>
       <c r="E83" s="1" t="s">
-        <v>284</v>
+        <v>269</v>
       </c>
       <c r="F83" s="1" t="s">
         <v>55</v>
@@ -3213,7 +3213,7 @@
         <v>32</v>
       </c>
       <c r="E84" s="1" t="s">
-        <v>302</v>
+        <v>287</v>
       </c>
       <c r="F84" s="1" t="s">
         <v>55</v>
@@ -3253,7 +3253,7 @@
         <v>23</v>
       </c>
       <c r="E86" s="1" t="s">
-        <v>303</v>
+        <v>288</v>
       </c>
       <c r="F86" s="1" t="s">
         <v>55</v>
@@ -3273,7 +3273,7 @@
         <v>23</v>
       </c>
       <c r="E87" s="1" t="s">
-        <v>285</v>
+        <v>270</v>
       </c>
       <c r="F87" s="1" t="s">
         <v>55</v>
@@ -3313,7 +3313,7 @@
         <v>12</v>
       </c>
       <c r="E89" s="1" t="s">
-        <v>286</v>
+        <v>271</v>
       </c>
       <c r="F89" s="1" t="s">
         <v>55</v>
@@ -3333,7 +3333,7 @@
         <v>33</v>
       </c>
       <c r="E90" s="1" t="s">
-        <v>304</v>
+        <v>289</v>
       </c>
       <c r="F90" s="1" t="s">
         <v>55</v>
@@ -3353,7 +3353,7 @@
         <v>33</v>
       </c>
       <c r="E91" s="1" t="s">
-        <v>287</v>
+        <v>272</v>
       </c>
       <c r="F91" s="1" t="s">
         <v>55</v>
@@ -3373,7 +3373,7 @@
         <v>25</v>
       </c>
       <c r="E92" s="1" t="s">
-        <v>305</v>
+        <v>290</v>
       </c>
       <c r="F92" s="1" t="s">
         <v>55</v>
@@ -3393,7 +3393,7 @@
         <v>25</v>
       </c>
       <c r="E93" s="1" t="s">
-        <v>288</v>
+        <v>273</v>
       </c>
       <c r="F93" s="1" t="s">
         <v>55</v>
@@ -3453,7 +3453,7 @@
         <v>13</v>
       </c>
       <c r="E96" s="1" t="s">
-        <v>306</v>
+        <v>291</v>
       </c>
       <c r="F96" s="1" t="s">
         <v>55</v>
@@ -3473,7 +3473,7 @@
         <v>13</v>
       </c>
       <c r="E97" s="1" t="s">
-        <v>289</v>
+        <v>274</v>
       </c>
       <c r="F97" s="1" t="s">
         <v>55</v>
@@ -3493,7 +3493,7 @@
         <v>26</v>
       </c>
       <c r="E98" s="1" t="s">
-        <v>307</v>
+        <v>292</v>
       </c>
       <c r="F98" s="1" t="s">
         <v>55</v>
@@ -3533,7 +3533,7 @@
         <v>14</v>
       </c>
       <c r="E100" s="1" t="s">
-        <v>309</v>
+        <v>294</v>
       </c>
       <c r="F100" s="1" t="s">
         <v>55</v>
@@ -3553,7 +3553,7 @@
         <v>14</v>
       </c>
       <c r="E101" s="1" t="s">
-        <v>290</v>
+        <v>275</v>
       </c>
       <c r="F101" s="1" t="s">
         <v>55</v>
@@ -3573,7 +3573,7 @@
         <v>30</v>
       </c>
       <c r="E102" s="1" t="s">
-        <v>308</v>
+        <v>293</v>
       </c>
       <c r="F102" s="1" t="s">
         <v>55</v>
@@ -3593,7 +3593,7 @@
         <v>30</v>
       </c>
       <c r="E103" s="1" t="s">
-        <v>291</v>
+        <v>276</v>
       </c>
       <c r="F103" s="1" t="s">
         <v>55</v>
@@ -3613,7 +3613,7 @@
         <v>15</v>
       </c>
       <c r="E104" s="1" t="s">
-        <v>310</v>
+        <v>295</v>
       </c>
       <c r="F104" s="1" t="s">
         <v>55</v>
@@ -3633,7 +3633,7 @@
         <v>15</v>
       </c>
       <c r="E105" s="1" t="s">
-        <v>292</v>
+        <v>277</v>
       </c>
       <c r="F105" s="1" t="s">
         <v>55</v>
@@ -3653,7 +3653,7 @@
         <v>16</v>
       </c>
       <c r="E106" s="1" t="s">
-        <v>311</v>
+        <v>296</v>
       </c>
       <c r="F106" s="1" t="s">
         <v>55</v>
@@ -3673,7 +3673,7 @@
         <v>16</v>
       </c>
       <c r="E107" s="1" t="s">
-        <v>293</v>
+        <v>278</v>
       </c>
       <c r="F107" s="1" t="s">
         <v>55</v>
@@ -3693,7 +3693,7 @@
         <v>17</v>
       </c>
       <c r="E108" s="1" t="s">
-        <v>312</v>
+        <v>297</v>
       </c>
       <c r="F108" s="1" t="s">
         <v>55</v>
@@ -3713,7 +3713,7 @@
         <v>17</v>
       </c>
       <c r="E109" s="1" t="s">
-        <v>294</v>
+        <v>279</v>
       </c>
       <c r="F109" s="1" t="s">
         <v>55</v>
@@ -3733,7 +3733,7 @@
         <v>29</v>
       </c>
       <c r="E110" s="1" t="s">
-        <v>313</v>
+        <v>298</v>
       </c>
       <c r="F110" s="1" t="s">
         <v>55</v>
@@ -3753,7 +3753,7 @@
         <v>29</v>
       </c>
       <c r="E111" s="1" t="s">
-        <v>295</v>
+        <v>280</v>
       </c>
       <c r="F111" s="1" t="s">
         <v>55</v>
@@ -3773,7 +3773,7 @@
         <v>18</v>
       </c>
       <c r="E112" s="1" t="s">
-        <v>314</v>
+        <v>299</v>
       </c>
       <c r="F112" s="1" t="s">
         <v>55</v>
@@ -3793,7 +3793,7 @@
         <v>18</v>
       </c>
       <c r="E113" s="1" t="s">
-        <v>296</v>
+        <v>281</v>
       </c>
       <c r="F113" s="1" t="s">
         <v>55</v>
@@ -3833,7 +3833,7 @@
         <v>20</v>
       </c>
       <c r="E115" s="6" t="s">
-        <v>297</v>
+        <v>282</v>
       </c>
       <c r="F115" s="1" t="s">
         <v>55</v>
@@ -3853,7 +3853,7 @@
         <v>24</v>
       </c>
       <c r="E116" s="1" t="s">
-        <v>315</v>
+        <v>300</v>
       </c>
       <c r="F116" s="1" t="s">
         <v>55</v>
@@ -3873,7 +3873,7 @@
         <v>24</v>
       </c>
       <c r="E117" s="1" t="s">
-        <v>298</v>
+        <v>283</v>
       </c>
       <c r="F117" s="1" t="s">
         <v>55</v>
@@ -3893,7 +3893,7 @@
         <v>7</v>
       </c>
       <c r="E118" s="1" t="s">
-        <v>316</v>
+        <v>301</v>
       </c>
       <c r="F118" s="1" t="s">
         <v>55</v>
@@ -3913,7 +3913,7 @@
         <v>7</v>
       </c>
       <c r="E119" s="1" t="s">
-        <v>299</v>
+        <v>284</v>
       </c>
       <c r="F119" s="1" t="s">
         <v>55</v>
@@ -3933,7 +3933,7 @@
         <v>9</v>
       </c>
       <c r="E120" s="1" t="s">
-        <v>317</v>
+        <v>302</v>
       </c>
       <c r="F120" s="1" t="s">
         <v>55</v>
@@ -3953,7 +3953,7 @@
         <v>9</v>
       </c>
       <c r="E121" s="1" t="s">
-        <v>300</v>
+        <v>285</v>
       </c>
       <c r="F121" s="1" t="s">
         <v>55</v>
@@ -4013,7 +4013,7 @@
         <v>22</v>
       </c>
       <c r="E124" s="1" t="s">
-        <v>268</v>
+        <v>253</v>
       </c>
       <c r="F124" s="1" t="s">
         <v>55</v>
@@ -4033,7 +4033,7 @@
         <v>32</v>
       </c>
       <c r="E125" s="6" t="s">
-        <v>255</v>
+        <v>240</v>
       </c>
       <c r="F125" s="1" t="s">
         <v>55</v>
@@ -4073,7 +4073,7 @@
         <v>32</v>
       </c>
       <c r="E127" s="1" t="s">
-        <v>269</v>
+        <v>254</v>
       </c>
       <c r="F127" s="1" t="s">
         <v>55</v>
@@ -4093,7 +4093,7 @@
         <v>23</v>
       </c>
       <c r="E128" s="1" t="s">
-        <v>256</v>
+        <v>241</v>
       </c>
       <c r="F128" s="1" t="s">
         <v>55</v>
@@ -4133,7 +4133,7 @@
         <v>23</v>
       </c>
       <c r="E130" s="1" t="s">
-        <v>270</v>
+        <v>255</v>
       </c>
       <c r="F130" s="1" t="s">
         <v>55</v>
@@ -4193,7 +4193,7 @@
         <v>12</v>
       </c>
       <c r="E133" s="6" t="s">
-        <v>271</v>
+        <v>256</v>
       </c>
       <c r="F133" s="1" t="s">
         <v>55</v>
@@ -4213,7 +4213,7 @@
         <v>33</v>
       </c>
       <c r="E134" s="1" t="s">
-        <v>257</v>
+        <v>242</v>
       </c>
       <c r="F134" s="1" t="s">
         <v>55</v>
@@ -4253,7 +4253,7 @@
         <v>33</v>
       </c>
       <c r="E136" s="1" t="s">
-        <v>272</v>
+        <v>257</v>
       </c>
       <c r="F136" s="1" t="s">
         <v>55</v>
@@ -4273,7 +4273,7 @@
         <v>25</v>
       </c>
       <c r="E137" s="1" t="s">
-        <v>258</v>
+        <v>243</v>
       </c>
       <c r="F137" s="1" t="s">
         <v>55</v>
@@ -4313,7 +4313,7 @@
         <v>25</v>
       </c>
       <c r="E139" s="1" t="s">
-        <v>273</v>
+        <v>258</v>
       </c>
       <c r="F139" s="1" t="s">
         <v>55</v>
@@ -4373,7 +4373,7 @@
         <v>28</v>
       </c>
       <c r="E142" s="1" t="s">
-        <v>274</v>
+        <v>259</v>
       </c>
       <c r="F142" s="1" t="s">
         <v>55</v>
@@ -4393,7 +4393,7 @@
         <v>13</v>
       </c>
       <c r="E143" s="6" t="s">
-        <v>259</v>
+        <v>244</v>
       </c>
       <c r="F143" s="1" t="s">
         <v>55</v>
@@ -4433,7 +4433,7 @@
         <v>13</v>
       </c>
       <c r="E145" s="1" t="s">
-        <v>275</v>
+        <v>260</v>
       </c>
       <c r="F145" s="1" t="s">
         <v>55</v>
@@ -4493,7 +4493,7 @@
         <v>26</v>
       </c>
       <c r="E148" s="1" t="s">
-        <v>276</v>
+        <v>261</v>
       </c>
       <c r="F148" s="1" t="s">
         <v>55</v>
@@ -4513,7 +4513,7 @@
         <v>14</v>
       </c>
       <c r="E149" s="1" t="s">
-        <v>261</v>
+        <v>246</v>
       </c>
       <c r="F149" s="1" t="s">
         <v>55</v>
@@ -4533,7 +4533,7 @@
         <v>14</v>
       </c>
       <c r="E150" s="1" t="s">
-        <v>283</v>
+        <v>268</v>
       </c>
       <c r="F150" s="1" t="s">
         <v>55</v>
@@ -4553,7 +4553,7 @@
         <v>14</v>
       </c>
       <c r="E151" s="1" t="s">
-        <v>277</v>
+        <v>262</v>
       </c>
       <c r="F151" s="1" t="s">
         <v>55</v>
@@ -4573,7 +4573,7 @@
         <v>30</v>
       </c>
       <c r="E152" s="1" t="s">
-        <v>260</v>
+        <v>245</v>
       </c>
       <c r="F152" s="1" t="s">
         <v>55</v>
@@ -4613,7 +4613,7 @@
         <v>30</v>
       </c>
       <c r="E154" s="1" t="s">
-        <v>278</v>
+        <v>263</v>
       </c>
       <c r="F154" s="1" t="s">
         <v>55</v>
@@ -4633,7 +4633,7 @@
         <v>15</v>
       </c>
       <c r="E155" s="1" t="s">
-        <v>262</v>
+        <v>247</v>
       </c>
       <c r="F155" s="1" t="s">
         <v>55</v>
@@ -4673,7 +4673,7 @@
         <v>15</v>
       </c>
       <c r="E157" s="1" t="s">
-        <v>279</v>
+        <v>264</v>
       </c>
       <c r="F157" s="1" t="s">
         <v>55</v>
@@ -4693,7 +4693,7 @@
         <v>16</v>
       </c>
       <c r="E158" s="1" t="s">
-        <v>263</v>
+        <v>248</v>
       </c>
       <c r="F158" s="1" t="s">
         <v>55</v>
@@ -4753,7 +4753,7 @@
         <v>17</v>
       </c>
       <c r="E161" s="1" t="s">
-        <v>265</v>
+        <v>250</v>
       </c>
       <c r="F161" s="1" t="s">
         <v>55</v>
@@ -4813,7 +4813,7 @@
         <v>29</v>
       </c>
       <c r="E164" s="1" t="s">
-        <v>264</v>
+        <v>249</v>
       </c>
       <c r="F164" s="1" t="s">
         <v>55</v>
@@ -4853,7 +4853,7 @@
         <v>29</v>
       </c>
       <c r="E166" s="1" t="s">
-        <v>280</v>
+        <v>265</v>
       </c>
       <c r="F166" s="1" t="s">
         <v>55</v>
@@ -4873,7 +4873,7 @@
         <v>18</v>
       </c>
       <c r="E167" s="1" t="s">
-        <v>266</v>
+        <v>251</v>
       </c>
       <c r="F167" s="1" t="s">
         <v>55</v>
@@ -4973,7 +4973,7 @@
         <v>20</v>
       </c>
       <c r="E172" s="1" t="s">
-        <v>281</v>
+        <v>266</v>
       </c>
       <c r="F172" s="1" t="s">
         <v>55</v>
@@ -4993,7 +4993,7 @@
         <v>24</v>
       </c>
       <c r="E173" s="1" t="s">
-        <v>267</v>
+        <v>252</v>
       </c>
       <c r="F173" s="1" t="s">
         <v>55</v>
@@ -5093,7 +5093,7 @@
         <v>7</v>
       </c>
       <c r="E178" s="1" t="s">
-        <v>282</v>
+        <v>267</v>
       </c>
       <c r="F178" s="1" t="s">
         <v>55</v>
@@ -5187,13 +5187,13 @@
         <v>6</v>
       </c>
       <c r="C183" s="12" t="s">
-        <v>150</v>
+        <v>135</v>
       </c>
       <c r="D183" s="9" t="s">
         <v>22</v>
       </c>
       <c r="E183" s="1" t="s">
-        <v>151</v>
+        <v>136</v>
       </c>
       <c r="F183" s="1" t="s">
         <v>55</v>
@@ -5207,13 +5207,13 @@
         <v>6</v>
       </c>
       <c r="C184" s="12" t="s">
-        <v>171</v>
+        <v>156</v>
       </c>
       <c r="D184" s="9" t="s">
         <v>22</v>
       </c>
       <c r="E184" s="1" t="s">
-        <v>172</v>
+        <v>157</v>
       </c>
       <c r="F184" s="1" t="s">
         <v>55</v>
@@ -5227,13 +5227,13 @@
         <v>6</v>
       </c>
       <c r="C185" s="12" t="s">
-        <v>192</v>
+        <v>177</v>
       </c>
       <c r="D185" s="9" t="s">
         <v>22</v>
       </c>
       <c r="E185" s="1" t="s">
-        <v>193</v>
+        <v>178</v>
       </c>
       <c r="F185" s="1" t="s">
         <v>55</v>
@@ -5247,13 +5247,13 @@
         <v>6</v>
       </c>
       <c r="C186" s="12" t="s">
-        <v>213</v>
+        <v>198</v>
       </c>
       <c r="D186" s="9" t="s">
         <v>22</v>
       </c>
       <c r="E186" s="1" t="s">
-        <v>214</v>
+        <v>199</v>
       </c>
       <c r="F186" s="1" t="s">
         <v>55</v>
@@ -5267,13 +5267,13 @@
         <v>6</v>
       </c>
       <c r="C187" s="12" t="s">
-        <v>234</v>
+        <v>219</v>
       </c>
       <c r="D187" s="9" t="s">
         <v>22</v>
       </c>
       <c r="E187" s="1" t="s">
-        <v>235</v>
+        <v>220</v>
       </c>
       <c r="F187" s="1" t="s">
         <v>55</v>
@@ -5293,7 +5293,7 @@
         <v>32</v>
       </c>
       <c r="E188" s="1" t="s">
-        <v>131</v>
+        <v>334</v>
       </c>
       <c r="F188" s="1" t="s">
         <v>55</v>
@@ -5307,13 +5307,13 @@
         <v>6</v>
       </c>
       <c r="C189" s="12" t="s">
-        <v>150</v>
+        <v>135</v>
       </c>
       <c r="D189" s="9" t="s">
         <v>32</v>
       </c>
       <c r="E189" s="1" t="s">
-        <v>152</v>
+        <v>137</v>
       </c>
       <c r="F189" s="1" t="s">
         <v>55</v>
@@ -5327,13 +5327,13 @@
         <v>6</v>
       </c>
       <c r="C190" s="12" t="s">
-        <v>171</v>
+        <v>156</v>
       </c>
       <c r="D190" s="9" t="s">
         <v>32</v>
       </c>
       <c r="E190" s="1" t="s">
-        <v>173</v>
+        <v>158</v>
       </c>
       <c r="F190" s="1" t="s">
         <v>55</v>
@@ -5347,13 +5347,13 @@
         <v>6</v>
       </c>
       <c r="C191" s="12" t="s">
-        <v>192</v>
+        <v>177</v>
       </c>
       <c r="D191" s="9" t="s">
         <v>32</v>
       </c>
       <c r="E191" s="1" t="s">
-        <v>194</v>
+        <v>179</v>
       </c>
       <c r="F191" s="1" t="s">
         <v>55</v>
@@ -5367,13 +5367,13 @@
         <v>6</v>
       </c>
       <c r="C192" s="12" t="s">
-        <v>213</v>
+        <v>198</v>
       </c>
       <c r="D192" s="9" t="s">
         <v>32</v>
       </c>
       <c r="E192" s="1" t="s">
-        <v>215</v>
+        <v>200</v>
       </c>
       <c r="F192" s="1" t="s">
         <v>55</v>
@@ -5387,13 +5387,13 @@
         <v>6</v>
       </c>
       <c r="C193" s="12" t="s">
-        <v>234</v>
+        <v>219</v>
       </c>
       <c r="D193" s="9" t="s">
         <v>32</v>
       </c>
       <c r="E193" s="1" t="s">
-        <v>236</v>
+        <v>221</v>
       </c>
       <c r="F193" s="1" t="s">
         <v>55</v>
@@ -5413,7 +5413,7 @@
         <v>23</v>
       </c>
       <c r="E194" s="1" t="s">
-        <v>132</v>
+        <v>335</v>
       </c>
       <c r="F194" s="1" t="s">
         <v>55</v>
@@ -5427,13 +5427,13 @@
         <v>6</v>
       </c>
       <c r="C195" s="12" t="s">
-        <v>150</v>
+        <v>135</v>
       </c>
       <c r="D195" s="9" t="s">
         <v>23</v>
       </c>
       <c r="E195" s="1" t="s">
-        <v>153</v>
+        <v>138</v>
       </c>
       <c r="F195" s="1" t="s">
         <v>55</v>
@@ -5447,13 +5447,13 @@
         <v>6</v>
       </c>
       <c r="C196" s="12" t="s">
-        <v>171</v>
+        <v>156</v>
       </c>
       <c r="D196" s="9" t="s">
         <v>23</v>
       </c>
       <c r="E196" s="1" t="s">
-        <v>174</v>
+        <v>159</v>
       </c>
       <c r="F196" s="1" t="s">
         <v>55</v>
@@ -5467,13 +5467,13 @@
         <v>6</v>
       </c>
       <c r="C197" s="12" t="s">
-        <v>192</v>
+        <v>177</v>
       </c>
       <c r="D197" s="9" t="s">
         <v>23</v>
       </c>
       <c r="E197" s="1" t="s">
-        <v>195</v>
+        <v>180</v>
       </c>
       <c r="F197" s="1" t="s">
         <v>55</v>
@@ -5487,13 +5487,13 @@
         <v>6</v>
       </c>
       <c r="C198" s="12" t="s">
-        <v>213</v>
+        <v>198</v>
       </c>
       <c r="D198" s="9" t="s">
         <v>23</v>
       </c>
       <c r="E198" s="1" t="s">
-        <v>216</v>
+        <v>201</v>
       </c>
       <c r="F198" s="1" t="s">
         <v>55</v>
@@ -5507,13 +5507,13 @@
         <v>6</v>
       </c>
       <c r="C199" s="12" t="s">
-        <v>234</v>
+        <v>219</v>
       </c>
       <c r="D199" s="9" t="s">
         <v>23</v>
       </c>
       <c r="E199" s="1" t="s">
-        <v>237</v>
+        <v>222</v>
       </c>
       <c r="F199" s="1" t="s">
         <v>55</v>
@@ -5533,7 +5533,7 @@
         <v>12</v>
       </c>
       <c r="E200" s="1" t="s">
-        <v>133</v>
+        <v>336</v>
       </c>
       <c r="F200" s="1" t="s">
         <v>55</v>
@@ -5547,13 +5547,13 @@
         <v>6</v>
       </c>
       <c r="C201" s="12" t="s">
-        <v>150</v>
+        <v>135</v>
       </c>
       <c r="D201" s="9" t="s">
         <v>12</v>
       </c>
       <c r="E201" s="1" t="s">
-        <v>154</v>
+        <v>139</v>
       </c>
       <c r="F201" s="1" t="s">
         <v>55</v>
@@ -5567,13 +5567,13 @@
         <v>6</v>
       </c>
       <c r="C202" s="12" t="s">
-        <v>171</v>
+        <v>156</v>
       </c>
       <c r="D202" s="9" t="s">
         <v>12</v>
       </c>
       <c r="E202" s="1" t="s">
-        <v>175</v>
+        <v>160</v>
       </c>
       <c r="F202" s="1" t="s">
         <v>55</v>
@@ -5587,13 +5587,13 @@
         <v>6</v>
       </c>
       <c r="C203" s="12" t="s">
-        <v>192</v>
+        <v>177</v>
       </c>
       <c r="D203" s="9" t="s">
         <v>12</v>
       </c>
       <c r="E203" s="1" t="s">
-        <v>196</v>
+        <v>181</v>
       </c>
       <c r="F203" s="1" t="s">
         <v>55</v>
@@ -5607,13 +5607,13 @@
         <v>6</v>
       </c>
       <c r="C204" s="12" t="s">
-        <v>213</v>
+        <v>198</v>
       </c>
       <c r="D204" s="9" t="s">
         <v>12</v>
       </c>
       <c r="E204" s="1" t="s">
-        <v>217</v>
+        <v>202</v>
       </c>
       <c r="F204" s="1" t="s">
         <v>55</v>
@@ -5627,13 +5627,13 @@
         <v>6</v>
       </c>
       <c r="C205" s="12" t="s">
-        <v>234</v>
+        <v>219</v>
       </c>
       <c r="D205" s="9" t="s">
         <v>12</v>
       </c>
       <c r="E205" s="1" t="s">
-        <v>238</v>
+        <v>223</v>
       </c>
       <c r="F205" s="1" t="s">
         <v>55</v>
@@ -5653,7 +5653,7 @@
         <v>33</v>
       </c>
       <c r="E206" s="1" t="s">
-        <v>134</v>
+        <v>337</v>
       </c>
       <c r="F206" s="1" t="s">
         <v>55</v>
@@ -5667,13 +5667,13 @@
         <v>6</v>
       </c>
       <c r="C207" s="12" t="s">
-        <v>150</v>
+        <v>135</v>
       </c>
       <c r="D207" s="9" t="s">
         <v>33</v>
       </c>
       <c r="E207" s="1" t="s">
-        <v>155</v>
+        <v>140</v>
       </c>
       <c r="F207" s="1" t="s">
         <v>55</v>
@@ -5687,13 +5687,13 @@
         <v>6</v>
       </c>
       <c r="C208" s="12" t="s">
-        <v>171</v>
+        <v>156</v>
       </c>
       <c r="D208" s="9" t="s">
         <v>33</v>
       </c>
       <c r="E208" s="1" t="s">
-        <v>176</v>
+        <v>161</v>
       </c>
       <c r="F208" s="1" t="s">
         <v>55</v>
@@ -5707,13 +5707,13 @@
         <v>6</v>
       </c>
       <c r="C209" s="12" t="s">
-        <v>192</v>
+        <v>177</v>
       </c>
       <c r="D209" s="9" t="s">
         <v>33</v>
       </c>
       <c r="E209" s="1" t="s">
-        <v>197</v>
+        <v>182</v>
       </c>
       <c r="F209" s="1" t="s">
         <v>55</v>
@@ -5727,13 +5727,13 @@
         <v>6</v>
       </c>
       <c r="C210" s="12" t="s">
-        <v>213</v>
+        <v>198</v>
       </c>
       <c r="D210" s="9" t="s">
         <v>33</v>
       </c>
       <c r="E210" s="1" t="s">
-        <v>218</v>
+        <v>203</v>
       </c>
       <c r="F210" s="1" t="s">
         <v>55</v>
@@ -5747,13 +5747,13 @@
         <v>6</v>
       </c>
       <c r="C211" s="12" t="s">
-        <v>234</v>
+        <v>219</v>
       </c>
       <c r="D211" s="9" t="s">
         <v>33</v>
       </c>
       <c r="E211" s="1" t="s">
-        <v>239</v>
+        <v>224</v>
       </c>
       <c r="F211" s="1" t="s">
         <v>55</v>
@@ -5773,7 +5773,7 @@
         <v>25</v>
       </c>
       <c r="E212" s="1" t="s">
-        <v>135</v>
+        <v>338</v>
       </c>
       <c r="F212" s="1" t="s">
         <v>55</v>
@@ -5787,13 +5787,13 @@
         <v>6</v>
       </c>
       <c r="C213" s="12" t="s">
-        <v>150</v>
+        <v>135</v>
       </c>
       <c r="D213" s="9" t="s">
         <v>25</v>
       </c>
       <c r="E213" s="1" t="s">
-        <v>156</v>
+        <v>141</v>
       </c>
       <c r="F213" s="1" t="s">
         <v>55</v>
@@ -5807,13 +5807,13 @@
         <v>6</v>
       </c>
       <c r="C214" s="12" t="s">
-        <v>171</v>
+        <v>156</v>
       </c>
       <c r="D214" s="9" t="s">
         <v>25</v>
       </c>
       <c r="E214" s="1" t="s">
-        <v>177</v>
+        <v>162</v>
       </c>
       <c r="F214" s="1" t="s">
         <v>55</v>
@@ -5827,13 +5827,13 @@
         <v>6</v>
       </c>
       <c r="C215" s="12" t="s">
-        <v>192</v>
+        <v>177</v>
       </c>
       <c r="D215" s="9" t="s">
         <v>25</v>
       </c>
       <c r="E215" s="1" t="s">
-        <v>198</v>
+        <v>183</v>
       </c>
       <c r="F215" s="1" t="s">
         <v>55</v>
@@ -5847,13 +5847,13 @@
         <v>6</v>
       </c>
       <c r="C216" s="12" t="s">
-        <v>213</v>
+        <v>198</v>
       </c>
       <c r="D216" s="9" t="s">
         <v>25</v>
       </c>
       <c r="E216" s="1" t="s">
-        <v>219</v>
+        <v>204</v>
       </c>
       <c r="F216" s="1" t="s">
         <v>55</v>
@@ -5867,13 +5867,13 @@
         <v>6</v>
       </c>
       <c r="C217" s="12" t="s">
-        <v>234</v>
+        <v>219</v>
       </c>
       <c r="D217" s="9" t="s">
         <v>25</v>
       </c>
       <c r="E217" s="1" t="s">
-        <v>240</v>
+        <v>225</v>
       </c>
       <c r="F217" s="1" t="s">
         <v>55</v>
@@ -5893,7 +5893,7 @@
         <v>28</v>
       </c>
       <c r="E218" s="1" t="s">
-        <v>136</v>
+        <v>339</v>
       </c>
       <c r="F218" s="1" t="s">
         <v>55</v>
@@ -5907,13 +5907,13 @@
         <v>6</v>
       </c>
       <c r="C219" s="12" t="s">
-        <v>150</v>
+        <v>135</v>
       </c>
       <c r="D219" s="9" t="s">
         <v>28</v>
       </c>
       <c r="E219" s="1" t="s">
-        <v>157</v>
+        <v>142</v>
       </c>
       <c r="F219" s="1" t="s">
         <v>55</v>
@@ -5927,13 +5927,13 @@
         <v>6</v>
       </c>
       <c r="C220" s="12" t="s">
-        <v>171</v>
+        <v>156</v>
       </c>
       <c r="D220" s="9" t="s">
         <v>28</v>
       </c>
       <c r="E220" s="1" t="s">
-        <v>178</v>
+        <v>163</v>
       </c>
       <c r="F220" s="1" t="s">
         <v>55</v>
@@ -5947,13 +5947,13 @@
         <v>6</v>
       </c>
       <c r="C221" s="12" t="s">
-        <v>192</v>
+        <v>177</v>
       </c>
       <c r="D221" s="9" t="s">
         <v>28</v>
       </c>
       <c r="E221" s="1" t="s">
-        <v>199</v>
+        <v>184</v>
       </c>
       <c r="F221" s="1" t="s">
         <v>55</v>
@@ -5967,13 +5967,13 @@
         <v>6</v>
       </c>
       <c r="C222" s="12" t="s">
-        <v>213</v>
+        <v>198</v>
       </c>
       <c r="D222" s="9" t="s">
         <v>28</v>
       </c>
       <c r="E222" s="1" t="s">
-        <v>220</v>
+        <v>205</v>
       </c>
       <c r="F222" s="1" t="s">
         <v>55</v>
@@ -5987,19 +5987,19 @@
         <v>6</v>
       </c>
       <c r="C223" s="12" t="s">
-        <v>234</v>
+        <v>219</v>
       </c>
       <c r="D223" s="9" t="s">
         <v>28</v>
       </c>
       <c r="E223" s="1" t="s">
-        <v>241</v>
+        <v>226</v>
       </c>
       <c r="F223" s="1" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="224" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A224" s="12" t="s">
         <v>128</v>
       </c>
@@ -6012,8 +6012,8 @@
       <c r="D224" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="E224" s="1" t="s">
-        <v>137</v>
+      <c r="E224" t="s">
+        <v>340</v>
       </c>
       <c r="F224" s="1" t="s">
         <v>55</v>
@@ -6027,13 +6027,13 @@
         <v>6</v>
       </c>
       <c r="C225" s="12" t="s">
-        <v>150</v>
+        <v>135</v>
       </c>
       <c r="D225" s="9" t="s">
         <v>13</v>
       </c>
       <c r="E225" s="1" t="s">
-        <v>158</v>
+        <v>143</v>
       </c>
       <c r="F225" s="1" t="s">
         <v>55</v>
@@ -6047,13 +6047,13 @@
         <v>6</v>
       </c>
       <c r="C226" s="12" t="s">
-        <v>171</v>
+        <v>156</v>
       </c>
       <c r="D226" s="9" t="s">
         <v>13</v>
       </c>
       <c r="E226" s="1" t="s">
-        <v>179</v>
+        <v>164</v>
       </c>
       <c r="F226" s="1" t="s">
         <v>55</v>
@@ -6067,13 +6067,13 @@
         <v>6</v>
       </c>
       <c r="C227" s="12" t="s">
-        <v>192</v>
+        <v>177</v>
       </c>
       <c r="D227" s="9" t="s">
         <v>13</v>
       </c>
       <c r="E227" s="1" t="s">
-        <v>200</v>
+        <v>185</v>
       </c>
       <c r="F227" s="1" t="s">
         <v>55</v>
@@ -6087,13 +6087,13 @@
         <v>6</v>
       </c>
       <c r="C228" s="12" t="s">
-        <v>213</v>
+        <v>198</v>
       </c>
       <c r="D228" s="9" t="s">
         <v>13</v>
       </c>
       <c r="E228" s="1" t="s">
-        <v>221</v>
+        <v>206</v>
       </c>
       <c r="F228" s="1" t="s">
         <v>55</v>
@@ -6107,13 +6107,13 @@
         <v>6</v>
       </c>
       <c r="C229" s="12" t="s">
-        <v>234</v>
+        <v>219</v>
       </c>
       <c r="D229" s="9" t="s">
         <v>13</v>
       </c>
       <c r="E229" s="1" t="s">
-        <v>242</v>
+        <v>227</v>
       </c>
       <c r="F229" s="1" t="s">
         <v>55</v>
@@ -6133,7 +6133,7 @@
         <v>26</v>
       </c>
       <c r="E230" s="1" t="s">
-        <v>138</v>
+        <v>342</v>
       </c>
       <c r="F230" s="1" t="s">
         <v>55</v>
@@ -6147,13 +6147,13 @@
         <v>6</v>
       </c>
       <c r="C231" s="12" t="s">
-        <v>150</v>
+        <v>135</v>
       </c>
       <c r="D231" s="9" t="s">
         <v>26</v>
       </c>
       <c r="E231" s="1" t="s">
-        <v>159</v>
+        <v>144</v>
       </c>
       <c r="F231" s="1" t="s">
         <v>55</v>
@@ -6167,13 +6167,13 @@
         <v>6</v>
       </c>
       <c r="C232" s="12" t="s">
-        <v>171</v>
+        <v>156</v>
       </c>
       <c r="D232" s="9" t="s">
         <v>26</v>
       </c>
       <c r="E232" s="1" t="s">
-        <v>180</v>
+        <v>165</v>
       </c>
       <c r="F232" s="1" t="s">
         <v>55</v>
@@ -6187,13 +6187,13 @@
         <v>6</v>
       </c>
       <c r="C233" s="12" t="s">
-        <v>192</v>
+        <v>177</v>
       </c>
       <c r="D233" s="9" t="s">
         <v>26</v>
       </c>
       <c r="E233" s="1" t="s">
-        <v>201</v>
+        <v>186</v>
       </c>
       <c r="F233" s="1" t="s">
         <v>55</v>
@@ -6207,13 +6207,13 @@
         <v>6</v>
       </c>
       <c r="C234" s="12" t="s">
-        <v>213</v>
+        <v>198</v>
       </c>
       <c r="D234" s="9" t="s">
         <v>26</v>
       </c>
       <c r="E234" s="1" t="s">
-        <v>222</v>
+        <v>207</v>
       </c>
       <c r="F234" s="1" t="s">
         <v>55</v>
@@ -6227,13 +6227,13 @@
         <v>6</v>
       </c>
       <c r="C235" s="12" t="s">
-        <v>234</v>
+        <v>219</v>
       </c>
       <c r="D235" s="9" t="s">
         <v>26</v>
       </c>
       <c r="E235" s="1" t="s">
-        <v>243</v>
+        <v>228</v>
       </c>
       <c r="F235" s="1" t="s">
         <v>55</v>
@@ -6253,7 +6253,7 @@
         <v>14</v>
       </c>
       <c r="E236" s="1" t="s">
-        <v>139</v>
+        <v>341</v>
       </c>
       <c r="F236" s="1" t="s">
         <v>55</v>
@@ -6267,13 +6267,13 @@
         <v>6</v>
       </c>
       <c r="C237" s="12" t="s">
-        <v>150</v>
+        <v>135</v>
       </c>
       <c r="D237" s="9" t="s">
         <v>14</v>
       </c>
       <c r="E237" s="1" t="s">
-        <v>160</v>
+        <v>145</v>
       </c>
       <c r="F237" s="1" t="s">
         <v>55</v>
@@ -6287,13 +6287,13 @@
         <v>6</v>
       </c>
       <c r="C238" s="12" t="s">
-        <v>171</v>
+        <v>156</v>
       </c>
       <c r="D238" s="9" t="s">
         <v>14</v>
       </c>
       <c r="E238" s="1" t="s">
-        <v>181</v>
+        <v>166</v>
       </c>
       <c r="F238" s="1" t="s">
         <v>55</v>
@@ -6307,13 +6307,13 @@
         <v>6</v>
       </c>
       <c r="C239" s="12" t="s">
-        <v>192</v>
+        <v>177</v>
       </c>
       <c r="D239" s="9" t="s">
         <v>14</v>
       </c>
       <c r="E239" s="1" t="s">
-        <v>202</v>
+        <v>187</v>
       </c>
       <c r="F239" s="1" t="s">
         <v>55</v>
@@ -6327,13 +6327,13 @@
         <v>6</v>
       </c>
       <c r="C240" s="12" t="s">
-        <v>213</v>
+        <v>198</v>
       </c>
       <c r="D240" s="9" t="s">
         <v>14</v>
       </c>
       <c r="E240" s="1" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="F240" s="1" t="s">
         <v>55</v>
@@ -6347,13 +6347,13 @@
         <v>6</v>
       </c>
       <c r="C241" s="12" t="s">
-        <v>234</v>
+        <v>219</v>
       </c>
       <c r="D241" s="9" t="s">
         <v>14</v>
       </c>
       <c r="E241" s="1" t="s">
-        <v>244</v>
+        <v>229</v>
       </c>
       <c r="F241" s="1" t="s">
         <v>55</v>
@@ -6373,7 +6373,7 @@
         <v>30</v>
       </c>
       <c r="E242" s="1" t="s">
-        <v>140</v>
+        <v>343</v>
       </c>
       <c r="F242" s="1" t="s">
         <v>55</v>
@@ -6387,13 +6387,13 @@
         <v>6</v>
       </c>
       <c r="C243" s="12" t="s">
-        <v>150</v>
+        <v>135</v>
       </c>
       <c r="D243" s="9" t="s">
         <v>30</v>
       </c>
       <c r="E243" s="1" t="s">
-        <v>161</v>
+        <v>146</v>
       </c>
       <c r="F243" s="1" t="s">
         <v>55</v>
@@ -6407,13 +6407,13 @@
         <v>6</v>
       </c>
       <c r="C244" s="12" t="s">
-        <v>171</v>
+        <v>156</v>
       </c>
       <c r="D244" s="9" t="s">
         <v>30</v>
       </c>
       <c r="E244" s="1" t="s">
-        <v>182</v>
+        <v>167</v>
       </c>
       <c r="F244" s="1" t="s">
         <v>55</v>
@@ -6427,13 +6427,13 @@
         <v>6</v>
       </c>
       <c r="C245" s="12" t="s">
-        <v>192</v>
+        <v>177</v>
       </c>
       <c r="D245" s="9" t="s">
         <v>30</v>
       </c>
       <c r="E245" s="1" t="s">
-        <v>203</v>
+        <v>188</v>
       </c>
       <c r="F245" s="1" t="s">
         <v>55</v>
@@ -6447,13 +6447,13 @@
         <v>6</v>
       </c>
       <c r="C246" s="12" t="s">
-        <v>213</v>
+        <v>198</v>
       </c>
       <c r="D246" s="9" t="s">
         <v>30</v>
       </c>
       <c r="E246" s="1" t="s">
-        <v>224</v>
+        <v>209</v>
       </c>
       <c r="F246" s="1" t="s">
         <v>55</v>
@@ -6467,13 +6467,13 @@
         <v>6</v>
       </c>
       <c r="C247" s="12" t="s">
-        <v>234</v>
+        <v>219</v>
       </c>
       <c r="D247" s="9" t="s">
         <v>30</v>
       </c>
       <c r="E247" s="1" t="s">
-        <v>245</v>
+        <v>230</v>
       </c>
       <c r="F247" s="1" t="s">
         <v>55</v>
@@ -6493,7 +6493,7 @@
         <v>15</v>
       </c>
       <c r="E248" s="1" t="s">
-        <v>141</v>
+        <v>131</v>
       </c>
       <c r="F248" s="1" t="s">
         <v>55</v>
@@ -6507,13 +6507,13 @@
         <v>6</v>
       </c>
       <c r="C249" s="12" t="s">
-        <v>150</v>
+        <v>135</v>
       </c>
       <c r="D249" s="9" t="s">
         <v>15</v>
       </c>
       <c r="E249" s="1" t="s">
-        <v>162</v>
+        <v>147</v>
       </c>
       <c r="F249" s="1" t="s">
         <v>55</v>
@@ -6527,13 +6527,13 @@
         <v>6</v>
       </c>
       <c r="C250" s="12" t="s">
-        <v>171</v>
+        <v>156</v>
       </c>
       <c r="D250" s="9" t="s">
         <v>15</v>
       </c>
       <c r="E250" s="1" t="s">
-        <v>183</v>
+        <v>168</v>
       </c>
       <c r="F250" s="1" t="s">
         <v>55</v>
@@ -6547,13 +6547,13 @@
         <v>6</v>
       </c>
       <c r="C251" s="12" t="s">
-        <v>192</v>
+        <v>177</v>
       </c>
       <c r="D251" s="9" t="s">
         <v>15</v>
       </c>
       <c r="E251" s="1" t="s">
-        <v>204</v>
+        <v>189</v>
       </c>
       <c r="F251" s="1" t="s">
         <v>55</v>
@@ -6567,13 +6567,13 @@
         <v>6</v>
       </c>
       <c r="C252" s="12" t="s">
-        <v>213</v>
+        <v>198</v>
       </c>
       <c r="D252" s="9" t="s">
         <v>15</v>
       </c>
       <c r="E252" s="1" t="s">
-        <v>225</v>
+        <v>210</v>
       </c>
       <c r="F252" s="1" t="s">
         <v>55</v>
@@ -6587,13 +6587,13 @@
         <v>6</v>
       </c>
       <c r="C253" s="12" t="s">
-        <v>234</v>
+        <v>219</v>
       </c>
       <c r="D253" s="9" t="s">
         <v>15</v>
       </c>
       <c r="E253" s="1" t="s">
-        <v>246</v>
+        <v>231</v>
       </c>
       <c r="F253" s="1" t="s">
         <v>55</v>
@@ -6613,7 +6613,7 @@
         <v>16</v>
       </c>
       <c r="E254" s="1" t="s">
-        <v>142</v>
+        <v>132</v>
       </c>
       <c r="F254" s="1" t="s">
         <v>55</v>
@@ -6627,13 +6627,13 @@
         <v>6</v>
       </c>
       <c r="C255" s="12" t="s">
-        <v>150</v>
+        <v>135</v>
       </c>
       <c r="D255" s="9" t="s">
         <v>16</v>
       </c>
       <c r="E255" s="1" t="s">
-        <v>163</v>
+        <v>148</v>
       </c>
       <c r="F255" s="1" t="s">
         <v>55</v>
@@ -6647,13 +6647,13 @@
         <v>6</v>
       </c>
       <c r="C256" s="12" t="s">
-        <v>171</v>
+        <v>156</v>
       </c>
       <c r="D256" s="9" t="s">
         <v>16</v>
       </c>
       <c r="E256" s="1" t="s">
-        <v>184</v>
+        <v>169</v>
       </c>
       <c r="F256" s="1" t="s">
         <v>55</v>
@@ -6667,13 +6667,13 @@
         <v>6</v>
       </c>
       <c r="C257" s="12" t="s">
-        <v>192</v>
+        <v>177</v>
       </c>
       <c r="D257" s="9" t="s">
         <v>16</v>
       </c>
       <c r="E257" s="1" t="s">
-        <v>205</v>
+        <v>190</v>
       </c>
       <c r="F257" s="1" t="s">
         <v>55</v>
@@ -6687,13 +6687,13 @@
         <v>6</v>
       </c>
       <c r="C258" s="12" t="s">
-        <v>213</v>
+        <v>198</v>
       </c>
       <c r="D258" s="9" t="s">
         <v>16</v>
       </c>
       <c r="E258" s="1" t="s">
-        <v>226</v>
+        <v>211</v>
       </c>
       <c r="F258" s="1" t="s">
         <v>55</v>
@@ -6707,13 +6707,13 @@
         <v>6</v>
       </c>
       <c r="C259" s="12" t="s">
-        <v>234</v>
+        <v>219</v>
       </c>
       <c r="D259" s="9" t="s">
         <v>16</v>
       </c>
       <c r="E259" s="1" t="s">
-        <v>247</v>
+        <v>232</v>
       </c>
       <c r="F259" s="1" t="s">
         <v>55</v>
@@ -6733,7 +6733,7 @@
         <v>17</v>
       </c>
       <c r="E260" s="1" t="s">
-        <v>143</v>
+        <v>133</v>
       </c>
       <c r="F260" s="1" t="s">
         <v>55</v>
@@ -6747,13 +6747,13 @@
         <v>6</v>
       </c>
       <c r="C261" s="12" t="s">
-        <v>150</v>
+        <v>135</v>
       </c>
       <c r="D261" s="9" t="s">
         <v>17</v>
       </c>
       <c r="E261" s="1" t="s">
-        <v>164</v>
+        <v>149</v>
       </c>
       <c r="F261" s="1" t="s">
         <v>55</v>
@@ -6767,13 +6767,13 @@
         <v>6</v>
       </c>
       <c r="C262" s="12" t="s">
-        <v>171</v>
+        <v>156</v>
       </c>
       <c r="D262" s="9" t="s">
         <v>17</v>
       </c>
       <c r="E262" s="1" t="s">
-        <v>185</v>
+        <v>170</v>
       </c>
       <c r="F262" s="1" t="s">
         <v>55</v>
@@ -6787,13 +6787,13 @@
         <v>6</v>
       </c>
       <c r="C263" s="12" t="s">
-        <v>192</v>
+        <v>177</v>
       </c>
       <c r="D263" s="9" t="s">
         <v>17</v>
       </c>
       <c r="E263" s="1" t="s">
-        <v>206</v>
+        <v>191</v>
       </c>
       <c r="F263" s="1" t="s">
         <v>55</v>
@@ -6807,13 +6807,13 @@
         <v>6</v>
       </c>
       <c r="C264" s="12" t="s">
-        <v>213</v>
+        <v>198</v>
       </c>
       <c r="D264" s="9" t="s">
         <v>17</v>
       </c>
       <c r="E264" s="1" t="s">
-        <v>227</v>
+        <v>212</v>
       </c>
       <c r="F264" s="1" t="s">
         <v>55</v>
@@ -6827,13 +6827,13 @@
         <v>6</v>
       </c>
       <c r="C265" s="12" t="s">
-        <v>234</v>
+        <v>219</v>
       </c>
       <c r="D265" s="9" t="s">
         <v>17</v>
       </c>
       <c r="E265" s="1" t="s">
-        <v>248</v>
+        <v>233</v>
       </c>
       <c r="F265" s="1" t="s">
         <v>55</v>
@@ -6853,7 +6853,7 @@
         <v>29</v>
       </c>
       <c r="E266" s="1" t="s">
-        <v>144</v>
+        <v>344</v>
       </c>
       <c r="F266" s="1" t="s">
         <v>55</v>
@@ -6867,13 +6867,13 @@
         <v>6</v>
       </c>
       <c r="C267" s="12" t="s">
-        <v>150</v>
+        <v>135</v>
       </c>
       <c r="D267" s="9" t="s">
         <v>29</v>
       </c>
       <c r="E267" s="1" t="s">
-        <v>165</v>
+        <v>150</v>
       </c>
       <c r="F267" s="1" t="s">
         <v>55</v>
@@ -6887,13 +6887,13 @@
         <v>6</v>
       </c>
       <c r="C268" s="12" t="s">
-        <v>171</v>
+        <v>156</v>
       </c>
       <c r="D268" s="9" t="s">
         <v>29</v>
       </c>
       <c r="E268" s="1" t="s">
-        <v>186</v>
+        <v>171</v>
       </c>
       <c r="F268" s="1" t="s">
         <v>55</v>
@@ -6907,13 +6907,13 @@
         <v>6</v>
       </c>
       <c r="C269" s="12" t="s">
-        <v>192</v>
+        <v>177</v>
       </c>
       <c r="D269" s="9" t="s">
         <v>29</v>
       </c>
       <c r="E269" s="1" t="s">
-        <v>207</v>
+        <v>192</v>
       </c>
       <c r="F269" s="1" t="s">
         <v>55</v>
@@ -6927,13 +6927,13 @@
         <v>6</v>
       </c>
       <c r="C270" s="12" t="s">
-        <v>213</v>
+        <v>198</v>
       </c>
       <c r="D270" s="9" t="s">
         <v>29</v>
       </c>
       <c r="E270" s="1" t="s">
-        <v>228</v>
+        <v>213</v>
       </c>
       <c r="F270" s="1" t="s">
         <v>55</v>
@@ -6947,13 +6947,13 @@
         <v>6</v>
       </c>
       <c r="C271" s="12" t="s">
-        <v>234</v>
+        <v>219</v>
       </c>
       <c r="D271" s="9" t="s">
         <v>29</v>
       </c>
       <c r="E271" s="1" t="s">
-        <v>249</v>
+        <v>234</v>
       </c>
       <c r="F271" s="1" t="s">
         <v>55</v>
@@ -6973,7 +6973,7 @@
         <v>18</v>
       </c>
       <c r="E272" s="1" t="s">
-        <v>145</v>
+        <v>345</v>
       </c>
       <c r="F272" s="1" t="s">
         <v>55</v>
@@ -6987,13 +6987,13 @@
         <v>6</v>
       </c>
       <c r="C273" s="12" t="s">
-        <v>150</v>
+        <v>135</v>
       </c>
       <c r="D273" s="9" t="s">
         <v>18</v>
       </c>
       <c r="E273" s="1" t="s">
-        <v>166</v>
+        <v>151</v>
       </c>
       <c r="F273" s="1" t="s">
         <v>55</v>
@@ -7007,13 +7007,13 @@
         <v>6</v>
       </c>
       <c r="C274" s="12" t="s">
-        <v>171</v>
+        <v>156</v>
       </c>
       <c r="D274" s="9" t="s">
         <v>18</v>
       </c>
       <c r="E274" s="1" t="s">
-        <v>187</v>
+        <v>172</v>
       </c>
       <c r="F274" s="1" t="s">
         <v>55</v>
@@ -7027,13 +7027,13 @@
         <v>6</v>
       </c>
       <c r="C275" s="12" t="s">
-        <v>192</v>
+        <v>177</v>
       </c>
       <c r="D275" s="9" t="s">
         <v>18</v>
       </c>
       <c r="E275" s="1" t="s">
-        <v>208</v>
+        <v>193</v>
       </c>
       <c r="F275" s="1" t="s">
         <v>55</v>
@@ -7047,13 +7047,13 @@
         <v>6</v>
       </c>
       <c r="C276" s="12" t="s">
-        <v>213</v>
+        <v>198</v>
       </c>
       <c r="D276" s="9" t="s">
         <v>18</v>
       </c>
       <c r="E276" s="1" t="s">
-        <v>229</v>
+        <v>214</v>
       </c>
       <c r="F276" s="1" t="s">
         <v>55</v>
@@ -7067,13 +7067,13 @@
         <v>6</v>
       </c>
       <c r="C277" s="12" t="s">
-        <v>234</v>
+        <v>219</v>
       </c>
       <c r="D277" s="9" t="s">
         <v>18</v>
       </c>
       <c r="E277" s="1" t="s">
-        <v>250</v>
+        <v>235</v>
       </c>
       <c r="F277" s="1" t="s">
         <v>55</v>
@@ -7093,7 +7093,7 @@
         <v>20</v>
       </c>
       <c r="E278" s="1" t="s">
-        <v>146</v>
+        <v>346</v>
       </c>
       <c r="F278" s="1" t="s">
         <v>55</v>
@@ -7107,13 +7107,13 @@
         <v>6</v>
       </c>
       <c r="C279" s="12" t="s">
-        <v>150</v>
+        <v>135</v>
       </c>
       <c r="D279" s="9" t="s">
         <v>20</v>
       </c>
       <c r="E279" s="1" t="s">
-        <v>167</v>
+        <v>152</v>
       </c>
       <c r="F279" s="1" t="s">
         <v>55</v>
@@ -7127,13 +7127,13 @@
         <v>6</v>
       </c>
       <c r="C280" s="12" t="s">
-        <v>171</v>
+        <v>156</v>
       </c>
       <c r="D280" s="9" t="s">
         <v>20</v>
       </c>
       <c r="E280" s="1" t="s">
-        <v>188</v>
+        <v>173</v>
       </c>
       <c r="F280" s="1" t="s">
         <v>55</v>
@@ -7147,13 +7147,13 @@
         <v>6</v>
       </c>
       <c r="C281" s="12" t="s">
-        <v>192</v>
+        <v>177</v>
       </c>
       <c r="D281" s="9" t="s">
         <v>20</v>
       </c>
       <c r="E281" s="1" t="s">
-        <v>209</v>
+        <v>194</v>
       </c>
       <c r="F281" s="1" t="s">
         <v>55</v>
@@ -7167,13 +7167,13 @@
         <v>6</v>
       </c>
       <c r="C282" s="12" t="s">
-        <v>213</v>
+        <v>198</v>
       </c>
       <c r="D282" s="9" t="s">
         <v>20</v>
       </c>
       <c r="E282" s="1" t="s">
-        <v>230</v>
+        <v>215</v>
       </c>
       <c r="F282" s="1" t="s">
         <v>55</v>
@@ -7187,13 +7187,13 @@
         <v>6</v>
       </c>
       <c r="C283" s="12" t="s">
-        <v>234</v>
+        <v>219</v>
       </c>
       <c r="D283" s="9" t="s">
         <v>20</v>
       </c>
       <c r="E283" s="1" t="s">
-        <v>251</v>
+        <v>236</v>
       </c>
       <c r="F283" s="1" t="s">
         <v>55</v>
@@ -7213,7 +7213,7 @@
         <v>24</v>
       </c>
       <c r="E284" s="1" t="s">
-        <v>147</v>
+        <v>134</v>
       </c>
       <c r="F284" s="1" t="s">
         <v>55</v>
@@ -7227,13 +7227,13 @@
         <v>6</v>
       </c>
       <c r="C285" s="12" t="s">
-        <v>150</v>
+        <v>135</v>
       </c>
       <c r="D285" s="9" t="s">
         <v>24</v>
       </c>
       <c r="E285" s="1" t="s">
-        <v>168</v>
+        <v>153</v>
       </c>
       <c r="F285" s="1" t="s">
         <v>55</v>
@@ -7247,13 +7247,13 @@
         <v>6</v>
       </c>
       <c r="C286" s="12" t="s">
-        <v>171</v>
+        <v>156</v>
       </c>
       <c r="D286" s="9" t="s">
         <v>24</v>
       </c>
       <c r="E286" s="1" t="s">
-        <v>189</v>
+        <v>174</v>
       </c>
       <c r="F286" s="1" t="s">
         <v>55</v>
@@ -7267,13 +7267,13 @@
         <v>6</v>
       </c>
       <c r="C287" s="12" t="s">
-        <v>192</v>
+        <v>177</v>
       </c>
       <c r="D287" s="9" t="s">
         <v>24</v>
       </c>
       <c r="E287" s="1" t="s">
-        <v>210</v>
+        <v>195</v>
       </c>
       <c r="F287" s="1" t="s">
         <v>55</v>
@@ -7287,13 +7287,13 @@
         <v>6</v>
       </c>
       <c r="C288" s="12" t="s">
-        <v>213</v>
+        <v>198</v>
       </c>
       <c r="D288" s="9" t="s">
         <v>24</v>
       </c>
       <c r="E288" s="1" t="s">
-        <v>231</v>
+        <v>216</v>
       </c>
       <c r="F288" s="1" t="s">
         <v>55</v>
@@ -7307,13 +7307,13 @@
         <v>6</v>
       </c>
       <c r="C289" s="12" t="s">
-        <v>234</v>
+        <v>219</v>
       </c>
       <c r="D289" s="9" t="s">
         <v>24</v>
       </c>
       <c r="E289" s="1" t="s">
-        <v>252</v>
+        <v>237</v>
       </c>
       <c r="F289" s="1" t="s">
         <v>55</v>
@@ -7333,7 +7333,7 @@
         <v>7</v>
       </c>
       <c r="E290" s="1" t="s">
-        <v>148</v>
+        <v>332</v>
       </c>
       <c r="F290" s="1" t="s">
         <v>55</v>
@@ -7347,13 +7347,13 @@
         <v>6</v>
       </c>
       <c r="C291" s="12" t="s">
-        <v>150</v>
+        <v>135</v>
       </c>
       <c r="D291" s="9" t="s">
         <v>7</v>
       </c>
       <c r="E291" s="1" t="s">
-        <v>169</v>
+        <v>154</v>
       </c>
       <c r="F291" s="1" t="s">
         <v>55</v>
@@ -7367,13 +7367,13 @@
         <v>6</v>
       </c>
       <c r="C292" s="12" t="s">
-        <v>171</v>
+        <v>156</v>
       </c>
       <c r="D292" s="9" t="s">
         <v>7</v>
       </c>
       <c r="E292" s="1" t="s">
-        <v>190</v>
+        <v>175</v>
       </c>
       <c r="F292" s="1" t="s">
         <v>55</v>
@@ -7387,13 +7387,13 @@
         <v>6</v>
       </c>
       <c r="C293" s="12" t="s">
-        <v>192</v>
+        <v>177</v>
       </c>
       <c r="D293" s="9" t="s">
         <v>7</v>
       </c>
       <c r="E293" s="1" t="s">
-        <v>211</v>
+        <v>196</v>
       </c>
       <c r="F293" s="1" t="s">
         <v>55</v>
@@ -7407,13 +7407,13 @@
         <v>6</v>
       </c>
       <c r="C294" s="12" t="s">
-        <v>213</v>
+        <v>198</v>
       </c>
       <c r="D294" s="9" t="s">
         <v>7</v>
       </c>
       <c r="E294" s="1" t="s">
-        <v>232</v>
+        <v>217</v>
       </c>
       <c r="F294" s="1" t="s">
         <v>55</v>
@@ -7427,13 +7427,13 @@
         <v>6</v>
       </c>
       <c r="C295" s="12" t="s">
-        <v>234</v>
+        <v>219</v>
       </c>
       <c r="D295" s="9" t="s">
         <v>7</v>
       </c>
       <c r="E295" s="1" t="s">
-        <v>253</v>
+        <v>238</v>
       </c>
       <c r="F295" s="1" t="s">
         <v>55</v>
@@ -7453,7 +7453,7 @@
         <v>9</v>
       </c>
       <c r="E296" s="1" t="s">
-        <v>149</v>
+        <v>333</v>
       </c>
       <c r="F296" s="1" t="s">
         <v>55</v>
@@ -7467,13 +7467,13 @@
         <v>6</v>
       </c>
       <c r="C297" s="12" t="s">
-        <v>150</v>
+        <v>135</v>
       </c>
       <c r="D297" s="9" t="s">
         <v>9</v>
       </c>
       <c r="E297" s="1" t="s">
-        <v>170</v>
+        <v>155</v>
       </c>
       <c r="F297" s="1" t="s">
         <v>55</v>
@@ -7487,13 +7487,13 @@
         <v>6</v>
       </c>
       <c r="C298" s="12" t="s">
-        <v>171</v>
+        <v>156</v>
       </c>
       <c r="D298" s="9" t="s">
         <v>9</v>
       </c>
       <c r="E298" s="1" t="s">
-        <v>191</v>
+        <v>176</v>
       </c>
       <c r="F298" s="1" t="s">
         <v>55</v>
@@ -7507,13 +7507,13 @@
         <v>6</v>
       </c>
       <c r="C299" s="12" t="s">
-        <v>192</v>
+        <v>177</v>
       </c>
       <c r="D299" s="9" t="s">
         <v>9</v>
       </c>
       <c r="E299" s="1" t="s">
-        <v>212</v>
+        <v>197</v>
       </c>
       <c r="F299" s="1" t="s">
         <v>55</v>
@@ -7527,13 +7527,13 @@
         <v>6</v>
       </c>
       <c r="C300" s="12" t="s">
-        <v>213</v>
+        <v>198</v>
       </c>
       <c r="D300" s="9" t="s">
         <v>9</v>
       </c>
       <c r="E300" s="1" t="s">
-        <v>233</v>
+        <v>218</v>
       </c>
       <c r="F300" s="1" t="s">
         <v>55</v>
@@ -7547,13 +7547,13 @@
         <v>6</v>
       </c>
       <c r="C301" s="12" t="s">
-        <v>234</v>
+        <v>219</v>
       </c>
       <c r="D301" s="9" t="s">
         <v>9</v>
       </c>
       <c r="E301" s="1" t="s">
-        <v>254</v>
+        <v>239</v>
       </c>
       <c r="F301" s="1" t="s">
         <v>55</v>

</xml_diff>

<commit_message>
Diversify US related to "Medicine & Health"  macro domain
</commit_message>
<xml_diff>
--- a/refair-server/datasets/few shot dataset/FSDataset.xlsx
+++ b/refair-server/datasets/few shot dataset/FSDataset.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\morel\Desktop\Refair\ReFair-App\refair-server\datasets\few shot dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18AA64A4-875B-4522-8EDD-9B4AE5BF19D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C6647F8-BD0F-4B29-87BA-5D109868EBD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{80773445-FB61-4F04-A882-1600FD96C55A}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{80773445-FB61-4F04-A882-1600FD96C55A}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -446,27 +446,15 @@
     <t>Dermatology</t>
   </si>
   <si>
-    <t>As a dermatologist, I want to apply adversarial learning techniques to detect and mitigate potential attacks on dermatological image recognition models, ensuring robustness and reliability in automated diagnosis systems.</t>
-  </si>
-  <si>
     <t>As a dermatologist, I want to train a CNN model on a large dataset of dermatological images to accurately classify skin lesions into different diagnostic categories, improving diagnostic precision and reducing misdiagnosis rates.</t>
   </si>
   <si>
     <t>As a dermatologist, I want to implement a conversational agent that can provide personalized skincare recommendations based on patient preferences, skin type, and specific dermatological concerns.</t>
   </si>
   <si>
-    <t>As a dermatologist, I want to utilize decision tree analysis to identify key risk factors for developing common dermatological conditions such as acne or eczema, enabling proactive preventive measures and patient education.</t>
-  </si>
-  <si>
-    <t>As a dermatologist, I want to develop a document classification model to automatically categorize research papers and clinical studies related to dermatological diseases, facilitating easier access to relevant literature for evidence-based practice.</t>
-  </si>
-  <si>
     <t>As a dermatologist, I want to develop an entity extraction system to automatically identify and extract key information from dermatological patient records, such as symptoms, diagnoses, and treatment histories, to assist in comprehensive patient management.</t>
   </si>
   <si>
-    <t>As a dermatologist, I want to perform feature selection on dermatological image data to identify the most discriminative features that contribute to accurate classification of skin lesions, enhancing diagnostic precision.</t>
-  </si>
-  <si>
     <t>As a dermatologist, I want to address class imbalance in dermatological datasets when developing AI models to detect rare skin conditions with limited training examples, ensuring robust and reliable diagnostic capabilities.</t>
   </si>
   <si>
@@ -488,9 +476,6 @@
     <t>As a dermatologist, I want to implement semantic similarity algorithms to analyze dermatological research papers and identify relevant studies based on shared concepts and findings, facilitating literature review and evidence synthesis.</t>
   </si>
   <si>
-    <t>As a dermatologist, I want to develop a sentiment analysis model to analyze social media posts and reviews related to skincare products, identifying sentiments and trends among consumers to inform product recommendations.</t>
-  </si>
-  <si>
     <t>As a dermatologist, I want to develop a speech-to-text system to transcribe verbal descriptions of skin conditions provided by patients during consultations, facilitating accurate documentation and diagnosis.</t>
   </si>
   <si>
@@ -500,75 +485,36 @@
     <t>As a dermatologist, I want to apply unsupervised clustering algorithms to group dermatological patient profiles based on similar symptoms and disease progression patterns, enabling personalized treatment plans for patient clusters.</t>
   </si>
   <si>
-    <t>As a dermatologist, I want to implement voice recognition technology to capture patient-reported symptoms and medical histories accurately during dermatological consultations, enhancing data quality and clinical decision-making.</t>
-  </si>
-  <si>
     <t>As a dermatologist, I want to develop word embedding models to capture semantic relationships between dermatological terms (e.g., skin conditions, treatment modalities) from medical literature, enhancing knowledge discovery and research.</t>
   </si>
   <si>
     <t>Endocrinology</t>
   </si>
   <si>
-    <t>As an endocrinologist, I want to apply adversarial learning techniques to identify and mitigate potential vulnerabilities in hormone imbalance prediction models, ensuring robustness against adversarial attacks.</t>
-  </si>
-  <si>
     <t>As an endocrinologist, I want to utilize CNN architectures to classify histopathological images of endocrine tumors, aiding in accurate diagnosis and personalized treatment planning for patients.</t>
   </si>
   <si>
-    <t>As an endocrinologist, I want to develop a conversational agent powered by natural language processing to interact with patients, providing personalized guidance on managing diabetes through diet and lifestyle recommendations.</t>
-  </si>
-  <si>
-    <t>As an endocrinologist, I want to use a decision tree algorithm to predict the risk of developing type 2 diabetes based on patient demographics, lifestyle factors, and genetic predispositions, enabling early intervention strategies.</t>
-  </si>
-  <si>
-    <t>As an endocrinologist, I want to develop a document classification system to automatically categorize patient medical records based on hormone profile data, streamlining the retrieval of information for treatment planning and research purposes.</t>
-  </si>
-  <si>
     <t>As an endocrinologist, I want to implement entity extraction techniques to extract relevant hormone biomarkers from patient laboratory reports, enabling comprehensive analysis and monitoring of hormone levels over time.</t>
   </si>
   <si>
-    <t>As an endocrinologist, I want to use feature selection algorithms to prioritize genetic markers linked to thyroid cancer susceptibility in familial studies, facilitating targeted screening and early detection strategies.</t>
-  </si>
-  <si>
     <t>As an endocrinologist, I want to address class imbalance in datasets related to rare endocrine disorders such as acromegaly, by applying oversampling techniques to ensure robust model training and accurate diagnosis.</t>
   </si>
   <si>
-    <t>As an endocrinologist, I want to develop a keyword extraction system to automatically identify relevant terms from clinical notes and research articles related to hypothyroidism, facilitating comprehensive literature review and evidence synthesis.</t>
-  </si>
-  <si>
     <t>As an endocrinologist, I want to implement k-Nearest Neighbor (k-NN) algorithms to predict insulin resistance in diabetic patients based on similar patient profiles, facilitating personalized treatment plans and monitoring strategies.</t>
   </si>
   <si>
-    <t>As an endocrinologist, I want to implement multi-label classification algorithms to classify patients with adrenal gland disorders into multiple categories (e.g., Cushing's syndrome, adrenal insufficiency), facilitating accurate diagnosis and tailored management approaches.</t>
-  </si>
-  <si>
     <t>As an endocrinologist, I want to develop a neural network model to predict the risk of gestational diabetes mellitus based on maternal health data, enabling early interventions and personalized prenatal care plans.</t>
   </si>
   <si>
     <t>As an endocrinologist, I want to use random forest models to classify patients with different subtypes of diabetes (e.g., type 1, type 2, gestational) based on clinical data and genetic predispositions, guiding tailored management strategies.</t>
   </si>
   <si>
-    <t>As an endocrinologist, I want to use semantic similarity techniques to match patient symptoms with known disease patterns in rare endocrine disorders, supporting early detection and personalized treatment approaches.</t>
-  </si>
-  <si>
     <t>As an endocrinologist, I want to conduct sentiment analysis on social media posts related to weight management strategies in diabetes care, understanding patient attitudes towards dietary recommendations and lifestyle changes.</t>
   </si>
   <si>
-    <t>As an endocrinologist, I want to use speech to text capabilities to convert endocrine conference recordings into text format, enabling easy access to discussions on recent research findings and clinical case studies.</t>
-  </si>
-  <si>
-    <t>As an endocrinologist, I want to use text categorization techniques to classify patient electronic health records based on different types of hormonal disorders (e.g., adrenal gland disorders, pituitary gland disorders), enabling efficient retrieval and analysis of relevant patient data.</t>
-  </si>
-  <si>
-    <t>As an endocrinologist, I want to use unsupervised clustering techniques to cluster symptoms reported by patients with polycystic ovary syndrome (PCOS), identifying common symptom patterns and guiding individualized management plans.</t>
-  </si>
-  <si>
     <t>As an endocrinologist, I want to implement voice recognition technology to transcribe patient conversations during consultations about diabetes management, improving documentation accuracy and workflow efficiency.</t>
   </si>
   <si>
-    <t>As an endocrinologist, I want to use word embedding techniques to analyze similarities and relationships between medical terms in research literature on insulin resistance, aiding in the discovery of novel associations and mechanisms.</t>
-  </si>
-  <si>
     <t>Health</t>
   </si>
   <si>
@@ -578,18 +524,9 @@
     <t>As a healthcare provider, I want to integrate CNN models into wearable health devices to monitor real-time physiological signals, enabling continuous health monitoring and early detection of cardiac abnormalities or respiratory distress.</t>
   </si>
   <si>
-    <t>As a healthcare administrator, I want to develop a multilingual conversational agent using machine learning algorithms to assist international patients in navigating healthcare services, including appointment scheduling, insurance inquiries, and medical translation services.</t>
-  </si>
-  <si>
     <t>As a healthcare administrator, I want to utilize decision tree models to optimize hospital bed allocation based on patient admission criteria, ensuring efficient resource management and reducing emergency room overcrowding during peak periods.</t>
   </si>
   <si>
-    <t>As a healthcare administrator, I want to implement document classification algorithms to categorize and prioritize incoming medical reports (e.g., radiology, pathology) based on urgency and clinical significance, facilitating timely review and decision-making by healthcare professionals.</t>
-  </si>
-  <si>
-    <t>As a healthcare provider, I want to deploy machine learning models for entity extraction in clinical trials documentation, to automatically extract and categorize information on study protocols, participant demographics, and treatment outcomes, facilitating efficient research data management and analysis.</t>
-  </si>
-  <si>
     <t>As a healthcare provider, I want to utilize feature selection techniques in machine learning models to extract meaningful patterns from wearable device data (e.g., heart rate variability, activity levels) for early detection and management of chronic conditions like hypertension and diabetes.</t>
   </si>
   <si>
@@ -635,24 +572,15 @@
     <t>Medicine</t>
   </si>
   <si>
-    <t>As a medical researcher, I want to apply adversarial learning techniques to analyze medical imaging data, so that I can identify and mitigate potential vulnerabilities and ensure the robustness of diagnostic models against adversarial attacks.</t>
-  </si>
-  <si>
     <t>As a medical researcher, I want to apply CNNs to analyze EEG data and identify patterns indicative of neurological disorders, so that I can assist in early diagnosis and intervention strategies for patients with conditions like epilepsy or Alzheimer's disease.</t>
   </si>
   <si>
-    <t>As a medical researcher, I want to deploy a conversational agent for medical students to practice clinical case simulations and receive feedback on diagnostic reasoning and treatment planning, so that I can enhance medical training and competency development.</t>
-  </si>
-  <si>
     <t>As a medical researcher, I want to utilize decision tree models to analyze patient satisfaction survey data and identify key factors influencing patient experience, so that I can implement quality improvement initiatives to enhance overall patient care and satisfaction.</t>
   </si>
   <si>
     <t>As a medical researcher, I want to use document classification algorithms to categorize medical research papers based on disease types and treatment outcomes, so that I can quickly access relevant literature for evidence-based medicine.</t>
   </si>
   <si>
-    <t>As a medical researcher, I want to develop entity extraction models to automatically identify and extract key medical entities (e.g., diseases, medications, symptoms) from clinical notes and patient records, so that I can build comprehensive patient profiles for personalized treatment planning.</t>
-  </si>
-  <si>
     <t>As a medical researcher, I want to use feature selection algorithms to identify clinical variables (e.g., patient demographics, comorbidities) that significantly impact treatment response in cancer patients, so that I can personalize treatment plans and improve patient outcomes.</t>
   </si>
   <si>
@@ -701,12 +629,6 @@
     <t>As a nephrologist, I want to employ adversarial learning techniques to detect and mitigate adversarial attacks on medical imaging data used for diagnosing kidney diseases, ensuring the reliability and integrity of diagnostic systems.</t>
   </si>
   <si>
-    <t>As a nephrologist, I want to utilize CNN models to predict the risk of acute kidney injury (AKI) in hospitalized patients based on a combination of clinical data and imaging findings, facilitating early intervention and patient management.</t>
-  </si>
-  <si>
-    <t>As a nephrologist, I want to deploy a conversational agent that can provide patients with personalized information about kidney disease management, including diet recommendations and lifestyle changes, to improve patient adherence and outcomes.</t>
-  </si>
-  <si>
     <t>As a nephrologist, I want to utilize a decision tree model to classify patients into different stages of chronic kidney disease based on their clinical parameters, facilitating targeted interventions and personalized treatment plans.</t>
   </si>
   <si>
@@ -725,9 +647,6 @@
     <t>As a nephrologist, I want to employ keyword extraction methods to analyze patient feedback forms and surveys related to kidney disease management, extracting recurring themes and patient-reported outcomes to inform quality improvement initiatives in nephrology care.</t>
   </si>
   <si>
-    <t>As a nephrologist, I want to use k-Nearest Neighbor (k-NN) algorithms to predict the risk of acute kidney injury (AKI) in hospitalized patients based on similarities to previous AKI cases with similar clinical profiles, enabling early intervention strategies.</t>
-  </si>
-  <si>
     <t>As a nephrologist, I want to utilize multi-label classification techniques to classify renal biopsy results into multiple histopathological categories (e.g., glomerulonephritis, tubulointerstitial diseases), supporting precise diagnosis and treatment recommendations.</t>
   </si>
   <si>
@@ -740,24 +659,15 @@
     <t>As a nephrologist, I want to develop semantic similarity algorithms to compare and categorize nephrology research articles based on shared concepts and biomedical terms, facilitating systematic literature reviews and knowledge synthesis.</t>
   </si>
   <si>
-    <t>As a nephrologist, I want to develop a sentiment analysis model to analyze social media discussions and patient forums related to kidney transplantation experiences, to gauge patient emotions and concerns post-surgery.</t>
-  </si>
-  <si>
     <t>As a nephrologist, I want to use speech to text algorithms to transcribe patient-doctor interactions during clinic visits, to streamline documentation processes and ensure comprehensive recording of medical histories and treatment plans.</t>
   </si>
   <si>
-    <t>As a nephrologist, I want to develop a text categorization system to classify nephrology research articles into categories such as chronic kidney disease epidemiology, renal replacement therapies, and nephrotoxicity studies, facilitating literature review and research synthesis.</t>
-  </si>
-  <si>
     <t>As a nephrologist, I want to apply unsupervised clustering algorithms to group patients based on similar clinical profiles and treatment responses, enabling personalized medicine approaches in nephrology care.</t>
   </si>
   <si>
     <t>As a nephrologist, I want to use voice recognition algorithms to transcribe patient-doctor interactions during nephrology clinic visits, ensuring accurate capture of medical histories, treatment discussions, and patient concerns.</t>
   </si>
   <si>
-    <t>As a nephrologist, I want to deploy word embedding models to support automated summarization of nephrology research articles and clinical trials, extracting key concepts and findings to aid in evidence-based decision-making and research synthesis.</t>
-  </si>
-  <si>
     <t>As a digital archivist, I want to use CNNs to automatically classify scanned book covers into genres and categories, making it easier for users to browse and discover books in our digital library collection.</t>
   </si>
   <si>
@@ -1077,6 +987,96 @@
   </si>
   <si>
     <t>As a cardiology clinic manager, I want to use text categorization to automatically sort incoming emails and messages from patients and other healthcare providers into categories like appointment requests, medication inquiries, and general questions, so that I can streamline communication and improve response times.</t>
+  </si>
+  <si>
+    <t>As a dermatology clinic manager, I want to explore adversarial learning techniques to detect and counteract potential adversarial inputs that could compromise the privacy and security of patient data handled by our automated diagnostic systems.</t>
+  </si>
+  <si>
+    <t>As a dermatology clinic manager, I want to implement a decision tree algorithm that analyzes patient intake forms and clinical data to prioritize appointments, ensuring that patients with urgent dermatological conditions receive prompt attention and care.</t>
+  </si>
+  <si>
+    <t>As a dermatology clinic administrator, I want to utilize document classification algorithms to organize patient medical records by skin condition categories (e.g., eczema, psoriasis, melanoma) for efficient retrieval and comprehensive patient history analysis during consultations.</t>
+  </si>
+  <si>
+    <t>As a skincare researcher, I want to use feature selection algorithms to analyze genetic and environmental factors that contribute to acne severity, helping to prioritize biomarkers and relevant features for personalized treatment strategies in dermatology.</t>
+  </si>
+  <si>
+    <t>As a skincare marketing strategist, I want to employ sentiment analysis techniques to monitor social media sentiment around skincare trends and influencers, identifying emerging consumer preferences and sentiment shifts that could influence marketing campaigns and product development strategies.</t>
+  </si>
+  <si>
+    <t>As a skincare researcher, I want to utilize voice recognition software to transcribe and analyze qualitative interviews with dermatology patients about their skincare routines, preferences, and treatment experiences, extracting valuable insights for consumer behavior studies and product development strategies.</t>
+  </si>
+  <si>
+    <t>As a clinical endocrinologist, I want to utilize text categorization to classify patient notes and lab reports related to diabetes management, so that I can streamline the process of patient care and ensure timely adjustments to treatment plans.</t>
+  </si>
+  <si>
+    <t>As a researcher in endocrinology, I want to apply adversarial learning techniques to enhance the robustness of predictive models for insulin sensitivity prediction, so that I can provide more accurate assessments for diabetic patients across diverse demographics.</t>
+  </si>
+  <si>
+    <t>As an endocrinology department administrator, I want to implement a conversational agent across our clinic's website and mobile apps to provide patients with real-time answers to common questions about hormone therapies, appointment scheduling, and clinic services, enhancing patient engagement and satisfaction.</t>
+  </si>
+  <si>
+    <t>As a pediatric endocrinologist, I want to develop a decision tree algorithm to assist in diagnosing growth hormone deficiency in children, incorporating clinical symptoms, genetic markers, and growth charts to guide treatment decisions and optimize patient outcomes.</t>
+  </si>
+  <si>
+    <t>As an endocrinology department administrator, I want to implement a document classification model to automatically sort patient medical records based on specific endocrine conditions (e.g., hypothyroidism, Cushing's syndrome), enabling faster access to relevant patient information during consultations and follow-up visits.</t>
+  </si>
+  <si>
+    <t>As an endocrinologist specializing in thyroid disorders, I want to use feature selection algorithms to identify the most informative imaging features (e.g., nodule size, echogenicity, vascularity) from thyroid ultrasound scans, aiding in the differentiation between benign and malignant thyroid nodules.</t>
+  </si>
+  <si>
+    <t>As an endocrinology clinic administrator, I want to implement a keyword extraction model to automatically extract relevant terms (e.g., symptoms, medications) from patient intake forms and medical histories, enabling clinicians to quickly assess patient conditions during consultations.</t>
+  </si>
+  <si>
+    <t>As an endocrinology researcher, I want to develop a multi-label classification system to predict the risk of metabolic syndrome components (e.g., hypertension, dyslipidemia, central obesity) based on patient demographics, lifestyle factors, and biochemical markers, guiding preventive interventions and patient counseling.</t>
+  </si>
+  <si>
+    <t>As an endocrinology researcher, I want to develop a semantic similarity model to compare and correlate clinical notes from patient EHRs, identifying patterns and associations between symptoms, treatments, and disease progression in thyroid disorders.</t>
+  </si>
+  <si>
+    <t>As a researcher studying voice disorders in thyroid patients, I want to develop a speech to text application that accurately transcribes and analyzes voice recordings to detect subtle changes in speech patterns indicative of vocal cord dysfunction or nodules.</t>
+  </si>
+  <si>
+    <t>As an endocrinology clinic director, I want to employ unsupervised clustering methods to analyze patient demographic data and identify clusters of patients with similar patterns of hormone disorders (e.g., polycystic ovary syndrome, adrenal insufficiency), to optimize clinic workflows and resource allocation.</t>
+  </si>
+  <si>
+    <t>As an endocrinology educator, I want to develop word embeddings from textbooks and medical literature on pituitary disorders to create interactive learning tools that visualize and explore relationships between key concepts and clinical scenarios.</t>
+  </si>
+  <si>
+    <t>As a hospital administrator, I want to implement a conversational agent for appointment scheduling and patient reminders, utilizing natural language processing to handle patient inquiries efficiently and reduce administrative workload.</t>
+  </si>
+  <si>
+    <t>As a healthcare compliance officer, I want to deploy document classification models to classify patient records according to privacy sensitivity levels, ensuring compliance with data protection regulations such as HIPAA.</t>
+  </si>
+  <si>
+    <t>As a healthcare data analyst, I want to implement entity extraction algorithms to identify and extract medication names, dosages, and administration frequencies from electronic health records, facilitating medication reconciliation and adverse event monitoring.</t>
+  </si>
+  <si>
+    <t>As a medical researcher studying cancer diagnostics, I want to use adversarial learning techniques to detect and mitigate potential vulnerabilities in my deep learning models, so that I can ensure the reliability of automated tumor detection systems in clinical settings.</t>
+  </si>
+  <si>
+    <t>As a medical receptionist, I want to implement a conversational agent that can understand and respond to patient inquiries about clinic hours, services offered, and insurance coverage, so that we can provide accurate information to patients promptly.</t>
+  </si>
+  <si>
+    <t>As a clinical data analyst, I want to develop an entity extraction system to automatically identify and extract key clinical parameters (e.g., blood pressure, cholesterol levels) from unstructured patient notes, so that I can perform comprehensive population health analytics.</t>
+  </si>
+  <si>
+    <t>As a radiologist specializing in nephrology, I want to integrate CNN-based image classification models to differentiate between various types of renal tumors based on imaging features, assisting in accurate and timely diagnoses for my patients.</t>
+  </si>
+  <si>
+    <t>As a nephrology clinic manager, I want to utilize a conversational agent with machine learning algorithms to conduct preliminary assessments of symptoms reported by patients, assisting in prioritizing appointments and optimizing clinic workflow.</t>
+  </si>
+  <si>
+    <t>As a medical researcher studying renal genetics, I want to employ k-NN classification to identify genetic variants associated with familial nephropathies, facilitating genotype-phenotype correlations and advancing our understanding of inherited kidney diseases.</t>
+  </si>
+  <si>
+    <t>As a nephrology clinic administrator, I want to use sentiment analysis on patient surveys and feedback forms to assess caregiver attitudes and satisfaction with pediatric nephrology services, guiding quality improvement initiatives.</t>
+  </si>
+  <si>
+    <t>As a nephrology researcher, I want to use text categorization algorithms to classify nephrology conference abstracts into thematic categories such as acute kidney injury (AKI), chronic kidney disease (CKD), and renal replacement therapies, facilitating conference organization and academic collaboration.</t>
+  </si>
+  <si>
+    <t>As a nephrologist, I want to utilize word embedding techniques to analyze and categorize patient feedback from nephrology surveys and social media posts, identifying common themes and sentiments related to healthcare experiences.</t>
   </si>
 </sst>
 </file>
@@ -1526,8 +1526,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8DF0B04-8323-4309-B759-D1CDDA1FBB0E}">
   <dimension ref="A1:F301"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C161" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C183" sqref="C183"/>
+    <sheetView tabSelected="1" topLeftCell="C289" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C301" sqref="C301"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1613,7 +1613,7 @@
         <v>32</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>319</v>
+        <v>289</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>55</v>
@@ -1673,7 +1673,7 @@
         <v>23</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>310</v>
+        <v>280</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>55</v>
@@ -1693,7 +1693,7 @@
         <v>12</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>320</v>
+        <v>290</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>55</v>
@@ -1713,7 +1713,7 @@
         <v>12</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>311</v>
+        <v>281</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>55</v>
@@ -1733,7 +1733,7 @@
         <v>33</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>321</v>
+        <v>291</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>55</v>
@@ -1753,7 +1753,7 @@
         <v>33</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>312</v>
+        <v>282</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>55</v>
@@ -1773,7 +1773,7 @@
         <v>25</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>322</v>
+        <v>292</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>55</v>
@@ -1813,7 +1813,7 @@
         <v>28</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>323</v>
+        <v>293</v>
       </c>
       <c r="F14" s="1" t="s">
         <v>55</v>
@@ -1833,7 +1833,7 @@
         <v>28</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>313</v>
+        <v>283</v>
       </c>
       <c r="F15" s="1" t="s">
         <v>55</v>
@@ -1933,7 +1933,7 @@
         <v>14</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>324</v>
+        <v>294</v>
       </c>
       <c r="F20" s="1" t="s">
         <v>55</v>
@@ -1953,7 +1953,7 @@
         <v>14</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>314</v>
+        <v>284</v>
       </c>
       <c r="F21" s="1" t="s">
         <v>55</v>
@@ -1973,7 +1973,7 @@
         <v>30</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>325</v>
+        <v>295</v>
       </c>
       <c r="F22" s="1" t="s">
         <v>55</v>
@@ -1993,7 +1993,7 @@
         <v>30</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>315</v>
+        <v>285</v>
       </c>
       <c r="F23" s="1" t="s">
         <v>55</v>
@@ -2093,7 +2093,7 @@
         <v>17</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>326</v>
+        <v>296</v>
       </c>
       <c r="F28" s="1" t="s">
         <v>55</v>
@@ -2133,7 +2133,7 @@
         <v>29</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>327</v>
+        <v>297</v>
       </c>
       <c r="F30" s="1" t="s">
         <v>55</v>
@@ -2193,7 +2193,7 @@
         <v>18</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>316</v>
+        <v>286</v>
       </c>
       <c r="F33" s="1" t="s">
         <v>55</v>
@@ -2213,7 +2213,7 @@
         <v>20</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>328</v>
+        <v>298</v>
       </c>
       <c r="F34" s="1" t="s">
         <v>55</v>
@@ -2253,7 +2253,7 @@
         <v>24</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>329</v>
+        <v>299</v>
       </c>
       <c r="F36" s="1" t="s">
         <v>55</v>
@@ -2273,7 +2273,7 @@
         <v>24</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>317</v>
+        <v>287</v>
       </c>
       <c r="F37" s="1" t="s">
         <v>55</v>
@@ -2293,7 +2293,7 @@
         <v>7</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>330</v>
+        <v>300</v>
       </c>
       <c r="F38" s="1" t="s">
         <v>55</v>
@@ -2333,7 +2333,7 @@
         <v>9</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>331</v>
+        <v>301</v>
       </c>
       <c r="F40" s="1" t="s">
         <v>55</v>
@@ -2353,7 +2353,7 @@
         <v>9</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>318</v>
+        <v>288</v>
       </c>
       <c r="F41" s="1" t="s">
         <v>55</v>
@@ -2513,7 +2513,7 @@
         <v>12</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>303</v>
+        <v>273</v>
       </c>
       <c r="F49" s="1" t="s">
         <v>55</v>
@@ -2553,7 +2553,7 @@
         <v>33</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>304</v>
+        <v>274</v>
       </c>
       <c r="F51" s="1" t="s">
         <v>55</v>
@@ -2633,7 +2633,7 @@
         <v>28</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>305</v>
+        <v>275</v>
       </c>
       <c r="F55" s="1" t="s">
         <v>55</v>
@@ -2713,7 +2713,7 @@
         <v>26</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>306</v>
+        <v>276</v>
       </c>
       <c r="F59" s="1" t="s">
         <v>55</v>
@@ -2833,7 +2833,7 @@
         <v>15</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>307</v>
+        <v>277</v>
       </c>
       <c r="F65" s="1" t="s">
         <v>55</v>
@@ -2913,7 +2913,7 @@
         <v>17</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>308</v>
+        <v>278</v>
       </c>
       <c r="F69" s="1" t="s">
         <v>55</v>
@@ -3073,7 +3073,7 @@
         <v>24</v>
       </c>
       <c r="E77" s="1" t="s">
-        <v>309</v>
+        <v>279</v>
       </c>
       <c r="F77" s="1" t="s">
         <v>55</v>
@@ -3173,7 +3173,7 @@
         <v>22</v>
       </c>
       <c r="E82" s="1" t="s">
-        <v>286</v>
+        <v>256</v>
       </c>
       <c r="F82" s="1" t="s">
         <v>55</v>
@@ -3193,7 +3193,7 @@
         <v>22</v>
       </c>
       <c r="E83" s="1" t="s">
-        <v>269</v>
+        <v>239</v>
       </c>
       <c r="F83" s="1" t="s">
         <v>55</v>
@@ -3213,7 +3213,7 @@
         <v>32</v>
       </c>
       <c r="E84" s="1" t="s">
-        <v>287</v>
+        <v>257</v>
       </c>
       <c r="F84" s="1" t="s">
         <v>55</v>
@@ -3253,7 +3253,7 @@
         <v>23</v>
       </c>
       <c r="E86" s="1" t="s">
-        <v>288</v>
+        <v>258</v>
       </c>
       <c r="F86" s="1" t="s">
         <v>55</v>
@@ -3273,7 +3273,7 @@
         <v>23</v>
       </c>
       <c r="E87" s="1" t="s">
-        <v>270</v>
+        <v>240</v>
       </c>
       <c r="F87" s="1" t="s">
         <v>55</v>
@@ -3313,7 +3313,7 @@
         <v>12</v>
       </c>
       <c r="E89" s="1" t="s">
-        <v>271</v>
+        <v>241</v>
       </c>
       <c r="F89" s="1" t="s">
         <v>55</v>
@@ -3333,7 +3333,7 @@
         <v>33</v>
       </c>
       <c r="E90" s="1" t="s">
-        <v>289</v>
+        <v>259</v>
       </c>
       <c r="F90" s="1" t="s">
         <v>55</v>
@@ -3353,7 +3353,7 @@
         <v>33</v>
       </c>
       <c r="E91" s="1" t="s">
-        <v>272</v>
+        <v>242</v>
       </c>
       <c r="F91" s="1" t="s">
         <v>55</v>
@@ -3373,7 +3373,7 @@
         <v>25</v>
       </c>
       <c r="E92" s="1" t="s">
-        <v>290</v>
+        <v>260</v>
       </c>
       <c r="F92" s="1" t="s">
         <v>55</v>
@@ -3393,7 +3393,7 @@
         <v>25</v>
       </c>
       <c r="E93" s="1" t="s">
-        <v>273</v>
+        <v>243</v>
       </c>
       <c r="F93" s="1" t="s">
         <v>55</v>
@@ -3453,7 +3453,7 @@
         <v>13</v>
       </c>
       <c r="E96" s="1" t="s">
-        <v>291</v>
+        <v>261</v>
       </c>
       <c r="F96" s="1" t="s">
         <v>55</v>
@@ -3473,7 +3473,7 @@
         <v>13</v>
       </c>
       <c r="E97" s="1" t="s">
-        <v>274</v>
+        <v>244</v>
       </c>
       <c r="F97" s="1" t="s">
         <v>55</v>
@@ -3493,7 +3493,7 @@
         <v>26</v>
       </c>
       <c r="E98" s="1" t="s">
-        <v>292</v>
+        <v>262</v>
       </c>
       <c r="F98" s="1" t="s">
         <v>55</v>
@@ -3533,7 +3533,7 @@
         <v>14</v>
       </c>
       <c r="E100" s="1" t="s">
-        <v>294</v>
+        <v>264</v>
       </c>
       <c r="F100" s="1" t="s">
         <v>55</v>
@@ -3553,7 +3553,7 @@
         <v>14</v>
       </c>
       <c r="E101" s="1" t="s">
-        <v>275</v>
+        <v>245</v>
       </c>
       <c r="F101" s="1" t="s">
         <v>55</v>
@@ -3573,7 +3573,7 @@
         <v>30</v>
       </c>
       <c r="E102" s="1" t="s">
-        <v>293</v>
+        <v>263</v>
       </c>
       <c r="F102" s="1" t="s">
         <v>55</v>
@@ -3593,7 +3593,7 @@
         <v>30</v>
       </c>
       <c r="E103" s="1" t="s">
-        <v>276</v>
+        <v>246</v>
       </c>
       <c r="F103" s="1" t="s">
         <v>55</v>
@@ -3613,7 +3613,7 @@
         <v>15</v>
       </c>
       <c r="E104" s="1" t="s">
-        <v>295</v>
+        <v>265</v>
       </c>
       <c r="F104" s="1" t="s">
         <v>55</v>
@@ -3633,7 +3633,7 @@
         <v>15</v>
       </c>
       <c r="E105" s="1" t="s">
-        <v>277</v>
+        <v>247</v>
       </c>
       <c r="F105" s="1" t="s">
         <v>55</v>
@@ -3653,7 +3653,7 @@
         <v>16</v>
       </c>
       <c r="E106" s="1" t="s">
-        <v>296</v>
+        <v>266</v>
       </c>
       <c r="F106" s="1" t="s">
         <v>55</v>
@@ -3673,7 +3673,7 @@
         <v>16</v>
       </c>
       <c r="E107" s="1" t="s">
-        <v>278</v>
+        <v>248</v>
       </c>
       <c r="F107" s="1" t="s">
         <v>55</v>
@@ -3693,7 +3693,7 @@
         <v>17</v>
       </c>
       <c r="E108" s="1" t="s">
-        <v>297</v>
+        <v>267</v>
       </c>
       <c r="F108" s="1" t="s">
         <v>55</v>
@@ -3713,7 +3713,7 @@
         <v>17</v>
       </c>
       <c r="E109" s="1" t="s">
-        <v>279</v>
+        <v>249</v>
       </c>
       <c r="F109" s="1" t="s">
         <v>55</v>
@@ -3733,7 +3733,7 @@
         <v>29</v>
       </c>
       <c r="E110" s="1" t="s">
-        <v>298</v>
+        <v>268</v>
       </c>
       <c r="F110" s="1" t="s">
         <v>55</v>
@@ -3753,7 +3753,7 @@
         <v>29</v>
       </c>
       <c r="E111" s="1" t="s">
-        <v>280</v>
+        <v>250</v>
       </c>
       <c r="F111" s="1" t="s">
         <v>55</v>
@@ -3773,7 +3773,7 @@
         <v>18</v>
       </c>
       <c r="E112" s="1" t="s">
-        <v>299</v>
+        <v>269</v>
       </c>
       <c r="F112" s="1" t="s">
         <v>55</v>
@@ -3793,7 +3793,7 @@
         <v>18</v>
       </c>
       <c r="E113" s="1" t="s">
-        <v>281</v>
+        <v>251</v>
       </c>
       <c r="F113" s="1" t="s">
         <v>55</v>
@@ -3833,7 +3833,7 @@
         <v>20</v>
       </c>
       <c r="E115" s="6" t="s">
-        <v>282</v>
+        <v>252</v>
       </c>
       <c r="F115" s="1" t="s">
         <v>55</v>
@@ -3853,7 +3853,7 @@
         <v>24</v>
       </c>
       <c r="E116" s="1" t="s">
-        <v>300</v>
+        <v>270</v>
       </c>
       <c r="F116" s="1" t="s">
         <v>55</v>
@@ -3873,7 +3873,7 @@
         <v>24</v>
       </c>
       <c r="E117" s="1" t="s">
-        <v>283</v>
+        <v>253</v>
       </c>
       <c r="F117" s="1" t="s">
         <v>55</v>
@@ -3893,7 +3893,7 @@
         <v>7</v>
       </c>
       <c r="E118" s="1" t="s">
-        <v>301</v>
+        <v>271</v>
       </c>
       <c r="F118" s="1" t="s">
         <v>55</v>
@@ -3913,7 +3913,7 @@
         <v>7</v>
       </c>
       <c r="E119" s="1" t="s">
-        <v>284</v>
+        <v>254</v>
       </c>
       <c r="F119" s="1" t="s">
         <v>55</v>
@@ -3933,7 +3933,7 @@
         <v>9</v>
       </c>
       <c r="E120" s="1" t="s">
-        <v>302</v>
+        <v>272</v>
       </c>
       <c r="F120" s="1" t="s">
         <v>55</v>
@@ -3953,7 +3953,7 @@
         <v>9</v>
       </c>
       <c r="E121" s="1" t="s">
-        <v>285</v>
+        <v>255</v>
       </c>
       <c r="F121" s="1" t="s">
         <v>55</v>
@@ -4013,7 +4013,7 @@
         <v>22</v>
       </c>
       <c r="E124" s="1" t="s">
-        <v>253</v>
+        <v>223</v>
       </c>
       <c r="F124" s="1" t="s">
         <v>55</v>
@@ -4033,7 +4033,7 @@
         <v>32</v>
       </c>
       <c r="E125" s="6" t="s">
-        <v>240</v>
+        <v>210</v>
       </c>
       <c r="F125" s="1" t="s">
         <v>55</v>
@@ -4073,7 +4073,7 @@
         <v>32</v>
       </c>
       <c r="E127" s="1" t="s">
-        <v>254</v>
+        <v>224</v>
       </c>
       <c r="F127" s="1" t="s">
         <v>55</v>
@@ -4093,7 +4093,7 @@
         <v>23</v>
       </c>
       <c r="E128" s="1" t="s">
-        <v>241</v>
+        <v>211</v>
       </c>
       <c r="F128" s="1" t="s">
         <v>55</v>
@@ -4133,7 +4133,7 @@
         <v>23</v>
       </c>
       <c r="E130" s="1" t="s">
-        <v>255</v>
+        <v>225</v>
       </c>
       <c r="F130" s="1" t="s">
         <v>55</v>
@@ -4193,7 +4193,7 @@
         <v>12</v>
       </c>
       <c r="E133" s="6" t="s">
-        <v>256</v>
+        <v>226</v>
       </c>
       <c r="F133" s="1" t="s">
         <v>55</v>
@@ -4213,7 +4213,7 @@
         <v>33</v>
       </c>
       <c r="E134" s="1" t="s">
-        <v>242</v>
+        <v>212</v>
       </c>
       <c r="F134" s="1" t="s">
         <v>55</v>
@@ -4253,7 +4253,7 @@
         <v>33</v>
       </c>
       <c r="E136" s="1" t="s">
-        <v>257</v>
+        <v>227</v>
       </c>
       <c r="F136" s="1" t="s">
         <v>55</v>
@@ -4273,7 +4273,7 @@
         <v>25</v>
       </c>
       <c r="E137" s="1" t="s">
-        <v>243</v>
+        <v>213</v>
       </c>
       <c r="F137" s="1" t="s">
         <v>55</v>
@@ -4313,7 +4313,7 @@
         <v>25</v>
       </c>
       <c r="E139" s="1" t="s">
-        <v>258</v>
+        <v>228</v>
       </c>
       <c r="F139" s="1" t="s">
         <v>55</v>
@@ -4373,7 +4373,7 @@
         <v>28</v>
       </c>
       <c r="E142" s="1" t="s">
-        <v>259</v>
+        <v>229</v>
       </c>
       <c r="F142" s="1" t="s">
         <v>55</v>
@@ -4393,7 +4393,7 @@
         <v>13</v>
       </c>
       <c r="E143" s="6" t="s">
-        <v>244</v>
+        <v>214</v>
       </c>
       <c r="F143" s="1" t="s">
         <v>55</v>
@@ -4433,7 +4433,7 @@
         <v>13</v>
       </c>
       <c r="E145" s="1" t="s">
-        <v>260</v>
+        <v>230</v>
       </c>
       <c r="F145" s="1" t="s">
         <v>55</v>
@@ -4493,7 +4493,7 @@
         <v>26</v>
       </c>
       <c r="E148" s="1" t="s">
-        <v>261</v>
+        <v>231</v>
       </c>
       <c r="F148" s="1" t="s">
         <v>55</v>
@@ -4513,7 +4513,7 @@
         <v>14</v>
       </c>
       <c r="E149" s="1" t="s">
-        <v>246</v>
+        <v>216</v>
       </c>
       <c r="F149" s="1" t="s">
         <v>55</v>
@@ -4533,7 +4533,7 @@
         <v>14</v>
       </c>
       <c r="E150" s="1" t="s">
-        <v>268</v>
+        <v>238</v>
       </c>
       <c r="F150" s="1" t="s">
         <v>55</v>
@@ -4553,7 +4553,7 @@
         <v>14</v>
       </c>
       <c r="E151" s="1" t="s">
-        <v>262</v>
+        <v>232</v>
       </c>
       <c r="F151" s="1" t="s">
         <v>55</v>
@@ -4573,7 +4573,7 @@
         <v>30</v>
       </c>
       <c r="E152" s="1" t="s">
-        <v>245</v>
+        <v>215</v>
       </c>
       <c r="F152" s="1" t="s">
         <v>55</v>
@@ -4613,7 +4613,7 @@
         <v>30</v>
       </c>
       <c r="E154" s="1" t="s">
-        <v>263</v>
+        <v>233</v>
       </c>
       <c r="F154" s="1" t="s">
         <v>55</v>
@@ -4633,7 +4633,7 @@
         <v>15</v>
       </c>
       <c r="E155" s="1" t="s">
-        <v>247</v>
+        <v>217</v>
       </c>
       <c r="F155" s="1" t="s">
         <v>55</v>
@@ -4673,7 +4673,7 @@
         <v>15</v>
       </c>
       <c r="E157" s="1" t="s">
-        <v>264</v>
+        <v>234</v>
       </c>
       <c r="F157" s="1" t="s">
         <v>55</v>
@@ -4693,7 +4693,7 @@
         <v>16</v>
       </c>
       <c r="E158" s="1" t="s">
-        <v>248</v>
+        <v>218</v>
       </c>
       <c r="F158" s="1" t="s">
         <v>55</v>
@@ -4753,7 +4753,7 @@
         <v>17</v>
       </c>
       <c r="E161" s="1" t="s">
-        <v>250</v>
+        <v>220</v>
       </c>
       <c r="F161" s="1" t="s">
         <v>55</v>
@@ -4813,7 +4813,7 @@
         <v>29</v>
       </c>
       <c r="E164" s="1" t="s">
-        <v>249</v>
+        <v>219</v>
       </c>
       <c r="F164" s="1" t="s">
         <v>55</v>
@@ -4853,7 +4853,7 @@
         <v>29</v>
       </c>
       <c r="E166" s="1" t="s">
-        <v>265</v>
+        <v>235</v>
       </c>
       <c r="F166" s="1" t="s">
         <v>55</v>
@@ -4873,7 +4873,7 @@
         <v>18</v>
       </c>
       <c r="E167" s="1" t="s">
-        <v>251</v>
+        <v>221</v>
       </c>
       <c r="F167" s="1" t="s">
         <v>55</v>
@@ -4973,7 +4973,7 @@
         <v>20</v>
       </c>
       <c r="E172" s="1" t="s">
-        <v>266</v>
+        <v>236</v>
       </c>
       <c r="F172" s="1" t="s">
         <v>55</v>
@@ -4993,7 +4993,7 @@
         <v>24</v>
       </c>
       <c r="E173" s="1" t="s">
-        <v>252</v>
+        <v>222</v>
       </c>
       <c r="F173" s="1" t="s">
         <v>55</v>
@@ -5093,7 +5093,7 @@
         <v>7</v>
       </c>
       <c r="E178" s="1" t="s">
-        <v>267</v>
+        <v>237</v>
       </c>
       <c r="F178" s="1" t="s">
         <v>55</v>
@@ -5193,7 +5193,7 @@
         <v>22</v>
       </c>
       <c r="E183" s="1" t="s">
-        <v>136</v>
+        <v>317</v>
       </c>
       <c r="F183" s="1" t="s">
         <v>55</v>
@@ -5207,13 +5207,13 @@
         <v>6</v>
       </c>
       <c r="C184" s="12" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="D184" s="9" t="s">
         <v>22</v>
       </c>
       <c r="E184" s="1" t="s">
-        <v>157</v>
+        <v>324</v>
       </c>
       <c r="F184" s="1" t="s">
         <v>55</v>
@@ -5227,13 +5227,13 @@
         <v>6</v>
       </c>
       <c r="C185" s="12" t="s">
-        <v>177</v>
+        <v>159</v>
       </c>
       <c r="D185" s="9" t="s">
         <v>22</v>
       </c>
       <c r="E185" s="1" t="s">
-        <v>178</v>
+        <v>160</v>
       </c>
       <c r="F185" s="1" t="s">
         <v>55</v>
@@ -5247,13 +5247,13 @@
         <v>6</v>
       </c>
       <c r="C186" s="12" t="s">
-        <v>198</v>
+        <v>177</v>
       </c>
       <c r="D186" s="9" t="s">
         <v>22</v>
       </c>
       <c r="E186" s="1" t="s">
-        <v>199</v>
+        <v>338</v>
       </c>
       <c r="F186" s="1" t="s">
         <v>55</v>
@@ -5267,13 +5267,13 @@
         <v>6</v>
       </c>
       <c r="C187" s="12" t="s">
-        <v>219</v>
+        <v>195</v>
       </c>
       <c r="D187" s="9" t="s">
         <v>22</v>
       </c>
       <c r="E187" s="1" t="s">
-        <v>220</v>
+        <v>196</v>
       </c>
       <c r="F187" s="1" t="s">
         <v>55</v>
@@ -5293,7 +5293,7 @@
         <v>32</v>
       </c>
       <c r="E188" s="1" t="s">
-        <v>334</v>
+        <v>304</v>
       </c>
       <c r="F188" s="1" t="s">
         <v>55</v>
@@ -5313,7 +5313,7 @@
         <v>32</v>
       </c>
       <c r="E189" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F189" s="1" t="s">
         <v>55</v>
@@ -5327,13 +5327,13 @@
         <v>6</v>
       </c>
       <c r="C190" s="12" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="D190" s="9" t="s">
         <v>32</v>
       </c>
       <c r="E190" s="1" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="F190" s="1" t="s">
         <v>55</v>
@@ -5347,13 +5347,13 @@
         <v>6</v>
       </c>
       <c r="C191" s="12" t="s">
-        <v>177</v>
+        <v>159</v>
       </c>
       <c r="D191" s="9" t="s">
         <v>32</v>
       </c>
       <c r="E191" s="1" t="s">
-        <v>179</v>
+        <v>161</v>
       </c>
       <c r="F191" s="1" t="s">
         <v>55</v>
@@ -5367,13 +5367,13 @@
         <v>6</v>
       </c>
       <c r="C192" s="12" t="s">
-        <v>198</v>
+        <v>177</v>
       </c>
       <c r="D192" s="9" t="s">
         <v>32</v>
       </c>
       <c r="E192" s="1" t="s">
-        <v>200</v>
+        <v>178</v>
       </c>
       <c r="F192" s="1" t="s">
         <v>55</v>
@@ -5387,13 +5387,13 @@
         <v>6</v>
       </c>
       <c r="C193" s="12" t="s">
-        <v>219</v>
+        <v>195</v>
       </c>
       <c r="D193" s="9" t="s">
         <v>32</v>
       </c>
       <c r="E193" s="1" t="s">
-        <v>221</v>
+        <v>341</v>
       </c>
       <c r="F193" s="1" t="s">
         <v>55</v>
@@ -5413,7 +5413,7 @@
         <v>23</v>
       </c>
       <c r="E194" s="1" t="s">
-        <v>335</v>
+        <v>305</v>
       </c>
       <c r="F194" s="1" t="s">
         <v>55</v>
@@ -5433,7 +5433,7 @@
         <v>23</v>
       </c>
       <c r="E195" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F195" s="1" t="s">
         <v>55</v>
@@ -5447,13 +5447,13 @@
         <v>6</v>
       </c>
       <c r="C196" s="12" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="D196" s="9" t="s">
         <v>23</v>
       </c>
       <c r="E196" s="1" t="s">
-        <v>159</v>
+        <v>325</v>
       </c>
       <c r="F196" s="1" t="s">
         <v>55</v>
@@ -5467,13 +5467,13 @@
         <v>6</v>
       </c>
       <c r="C197" s="12" t="s">
-        <v>177</v>
+        <v>159</v>
       </c>
       <c r="D197" s="9" t="s">
         <v>23</v>
       </c>
       <c r="E197" s="1" t="s">
-        <v>180</v>
+        <v>335</v>
       </c>
       <c r="F197" s="1" t="s">
         <v>55</v>
@@ -5487,13 +5487,13 @@
         <v>6</v>
       </c>
       <c r="C198" s="12" t="s">
-        <v>198</v>
+        <v>177</v>
       </c>
       <c r="D198" s="9" t="s">
         <v>23</v>
       </c>
       <c r="E198" s="1" t="s">
-        <v>201</v>
+        <v>339</v>
       </c>
       <c r="F198" s="1" t="s">
         <v>55</v>
@@ -5507,13 +5507,13 @@
         <v>6</v>
       </c>
       <c r="C199" s="12" t="s">
-        <v>219</v>
+        <v>195</v>
       </c>
       <c r="D199" s="9" t="s">
         <v>23</v>
       </c>
       <c r="E199" s="1" t="s">
-        <v>222</v>
+        <v>342</v>
       </c>
       <c r="F199" s="1" t="s">
         <v>55</v>
@@ -5533,7 +5533,7 @@
         <v>12</v>
       </c>
       <c r="E200" s="1" t="s">
-        <v>336</v>
+        <v>306</v>
       </c>
       <c r="F200" s="1" t="s">
         <v>55</v>
@@ -5553,7 +5553,7 @@
         <v>12</v>
       </c>
       <c r="E201" s="1" t="s">
-        <v>139</v>
+        <v>318</v>
       </c>
       <c r="F201" s="1" t="s">
         <v>55</v>
@@ -5567,13 +5567,13 @@
         <v>6</v>
       </c>
       <c r="C202" s="12" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="D202" s="9" t="s">
         <v>12</v>
       </c>
       <c r="E202" s="1" t="s">
-        <v>160</v>
+        <v>326</v>
       </c>
       <c r="F202" s="1" t="s">
         <v>55</v>
@@ -5587,13 +5587,13 @@
         <v>6</v>
       </c>
       <c r="C203" s="12" t="s">
-        <v>177</v>
+        <v>159</v>
       </c>
       <c r="D203" s="9" t="s">
         <v>12</v>
       </c>
       <c r="E203" s="1" t="s">
-        <v>181</v>
+        <v>162</v>
       </c>
       <c r="F203" s="1" t="s">
         <v>55</v>
@@ -5607,13 +5607,13 @@
         <v>6</v>
       </c>
       <c r="C204" s="12" t="s">
-        <v>198</v>
+        <v>177</v>
       </c>
       <c r="D204" s="9" t="s">
         <v>12</v>
       </c>
       <c r="E204" s="1" t="s">
-        <v>202</v>
+        <v>179</v>
       </c>
       <c r="F204" s="1" t="s">
         <v>55</v>
@@ -5627,13 +5627,13 @@
         <v>6</v>
       </c>
       <c r="C205" s="12" t="s">
-        <v>219</v>
+        <v>195</v>
       </c>
       <c r="D205" s="9" t="s">
         <v>12</v>
       </c>
       <c r="E205" s="1" t="s">
-        <v>223</v>
+        <v>197</v>
       </c>
       <c r="F205" s="1" t="s">
         <v>55</v>
@@ -5653,7 +5653,7 @@
         <v>33</v>
       </c>
       <c r="E206" s="1" t="s">
-        <v>337</v>
+        <v>307</v>
       </c>
       <c r="F206" s="1" t="s">
         <v>55</v>
@@ -5673,7 +5673,7 @@
         <v>33</v>
       </c>
       <c r="E207" s="1" t="s">
-        <v>140</v>
+        <v>319</v>
       </c>
       <c r="F207" s="1" t="s">
         <v>55</v>
@@ -5687,13 +5687,13 @@
         <v>6</v>
       </c>
       <c r="C208" s="12" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="D208" s="9" t="s">
         <v>33</v>
       </c>
       <c r="E208" s="1" t="s">
-        <v>161</v>
+        <v>327</v>
       </c>
       <c r="F208" s="1" t="s">
         <v>55</v>
@@ -5707,13 +5707,13 @@
         <v>6</v>
       </c>
       <c r="C209" s="12" t="s">
-        <v>177</v>
+        <v>159</v>
       </c>
       <c r="D209" s="9" t="s">
         <v>33</v>
       </c>
       <c r="E209" s="1" t="s">
-        <v>182</v>
+        <v>336</v>
       </c>
       <c r="F209" s="1" t="s">
         <v>55</v>
@@ -5727,13 +5727,13 @@
         <v>6</v>
       </c>
       <c r="C210" s="12" t="s">
-        <v>198</v>
+        <v>177</v>
       </c>
       <c r="D210" s="9" t="s">
         <v>33</v>
       </c>
       <c r="E210" s="1" t="s">
-        <v>203</v>
+        <v>180</v>
       </c>
       <c r="F210" s="1" t="s">
         <v>55</v>
@@ -5747,13 +5747,13 @@
         <v>6</v>
       </c>
       <c r="C211" s="12" t="s">
-        <v>219</v>
+        <v>195</v>
       </c>
       <c r="D211" s="9" t="s">
         <v>33</v>
       </c>
       <c r="E211" s="1" t="s">
-        <v>224</v>
+        <v>198</v>
       </c>
       <c r="F211" s="1" t="s">
         <v>55</v>
@@ -5773,7 +5773,7 @@
         <v>25</v>
       </c>
       <c r="E212" s="1" t="s">
-        <v>338</v>
+        <v>308</v>
       </c>
       <c r="F212" s="1" t="s">
         <v>55</v>
@@ -5793,7 +5793,7 @@
         <v>25</v>
       </c>
       <c r="E213" s="1" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="F213" s="1" t="s">
         <v>55</v>
@@ -5807,13 +5807,13 @@
         <v>6</v>
       </c>
       <c r="C214" s="12" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="D214" s="9" t="s">
         <v>25</v>
       </c>
       <c r="E214" s="1" t="s">
-        <v>162</v>
+        <v>152</v>
       </c>
       <c r="F214" s="1" t="s">
         <v>55</v>
@@ -5827,13 +5827,13 @@
         <v>6</v>
       </c>
       <c r="C215" s="12" t="s">
-        <v>177</v>
+        <v>159</v>
       </c>
       <c r="D215" s="9" t="s">
         <v>25</v>
       </c>
       <c r="E215" s="1" t="s">
-        <v>183</v>
+        <v>337</v>
       </c>
       <c r="F215" s="1" t="s">
         <v>55</v>
@@ -5847,13 +5847,13 @@
         <v>6</v>
       </c>
       <c r="C216" s="12" t="s">
-        <v>198</v>
+        <v>177</v>
       </c>
       <c r="D216" s="9" t="s">
         <v>25</v>
       </c>
       <c r="E216" s="1" t="s">
-        <v>204</v>
+        <v>340</v>
       </c>
       <c r="F216" s="1" t="s">
         <v>55</v>
@@ -5867,13 +5867,13 @@
         <v>6</v>
       </c>
       <c r="C217" s="12" t="s">
-        <v>219</v>
+        <v>195</v>
       </c>
       <c r="D217" s="9" t="s">
         <v>25</v>
       </c>
       <c r="E217" s="1" t="s">
-        <v>225</v>
+        <v>199</v>
       </c>
       <c r="F217" s="1" t="s">
         <v>55</v>
@@ -5893,7 +5893,7 @@
         <v>28</v>
       </c>
       <c r="E218" s="1" t="s">
-        <v>339</v>
+        <v>309</v>
       </c>
       <c r="F218" s="1" t="s">
         <v>55</v>
@@ -5913,7 +5913,7 @@
         <v>28</v>
       </c>
       <c r="E219" s="1" t="s">
-        <v>142</v>
+        <v>320</v>
       </c>
       <c r="F219" s="1" t="s">
         <v>55</v>
@@ -5927,13 +5927,13 @@
         <v>6</v>
       </c>
       <c r="C220" s="12" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="D220" s="9" t="s">
         <v>28</v>
       </c>
       <c r="E220" s="1" t="s">
-        <v>163</v>
+        <v>328</v>
       </c>
       <c r="F220" s="1" t="s">
         <v>55</v>
@@ -5947,13 +5947,13 @@
         <v>6</v>
       </c>
       <c r="C221" s="12" t="s">
-        <v>177</v>
+        <v>159</v>
       </c>
       <c r="D221" s="9" t="s">
         <v>28</v>
       </c>
       <c r="E221" s="1" t="s">
-        <v>184</v>
+        <v>163</v>
       </c>
       <c r="F221" s="1" t="s">
         <v>55</v>
@@ -5967,13 +5967,13 @@
         <v>6</v>
       </c>
       <c r="C222" s="12" t="s">
-        <v>198</v>
+        <v>177</v>
       </c>
       <c r="D222" s="9" t="s">
         <v>28</v>
       </c>
       <c r="E222" s="1" t="s">
-        <v>205</v>
+        <v>181</v>
       </c>
       <c r="F222" s="1" t="s">
         <v>55</v>
@@ -5987,13 +5987,13 @@
         <v>6</v>
       </c>
       <c r="C223" s="12" t="s">
-        <v>219</v>
+        <v>195</v>
       </c>
       <c r="D223" s="9" t="s">
         <v>28</v>
       </c>
       <c r="E223" s="1" t="s">
-        <v>226</v>
+        <v>200</v>
       </c>
       <c r="F223" s="1" t="s">
         <v>55</v>
@@ -6013,7 +6013,7 @@
         <v>13</v>
       </c>
       <c r="E224" t="s">
-        <v>340</v>
+        <v>310</v>
       </c>
       <c r="F224" s="1" t="s">
         <v>55</v>
@@ -6033,7 +6033,7 @@
         <v>13</v>
       </c>
       <c r="E225" s="1" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="F225" s="1" t="s">
         <v>55</v>
@@ -6047,13 +6047,13 @@
         <v>6</v>
       </c>
       <c r="C226" s="12" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="D226" s="9" t="s">
         <v>13</v>
       </c>
       <c r="E226" s="1" t="s">
-        <v>164</v>
+        <v>153</v>
       </c>
       <c r="F226" s="1" t="s">
         <v>55</v>
@@ -6067,13 +6067,13 @@
         <v>6</v>
       </c>
       <c r="C227" s="12" t="s">
-        <v>177</v>
+        <v>159</v>
       </c>
       <c r="D227" s="9" t="s">
         <v>13</v>
       </c>
       <c r="E227" s="1" t="s">
-        <v>185</v>
+        <v>164</v>
       </c>
       <c r="F227" s="1" t="s">
         <v>55</v>
@@ -6087,13 +6087,13 @@
         <v>6</v>
       </c>
       <c r="C228" s="12" t="s">
-        <v>198</v>
+        <v>177</v>
       </c>
       <c r="D228" s="9" t="s">
         <v>13</v>
       </c>
       <c r="E228" s="1" t="s">
-        <v>206</v>
+        <v>182</v>
       </c>
       <c r="F228" s="1" t="s">
         <v>55</v>
@@ -6107,13 +6107,13 @@
         <v>6</v>
       </c>
       <c r="C229" s="12" t="s">
-        <v>219</v>
+        <v>195</v>
       </c>
       <c r="D229" s="9" t="s">
         <v>13</v>
       </c>
       <c r="E229" s="1" t="s">
-        <v>227</v>
+        <v>201</v>
       </c>
       <c r="F229" s="1" t="s">
         <v>55</v>
@@ -6133,7 +6133,7 @@
         <v>26</v>
       </c>
       <c r="E230" s="1" t="s">
-        <v>342</v>
+        <v>312</v>
       </c>
       <c r="F230" s="1" t="s">
         <v>55</v>
@@ -6153,7 +6153,7 @@
         <v>26</v>
       </c>
       <c r="E231" s="1" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="F231" s="1" t="s">
         <v>55</v>
@@ -6167,13 +6167,13 @@
         <v>6</v>
       </c>
       <c r="C232" s="12" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="D232" s="9" t="s">
         <v>26</v>
       </c>
       <c r="E232" s="1" t="s">
-        <v>165</v>
+        <v>329</v>
       </c>
       <c r="F232" s="1" t="s">
         <v>55</v>
@@ -6187,13 +6187,13 @@
         <v>6</v>
       </c>
       <c r="C233" s="12" t="s">
-        <v>177</v>
+        <v>159</v>
       </c>
       <c r="D233" s="9" t="s">
         <v>26</v>
       </c>
       <c r="E233" s="1" t="s">
-        <v>186</v>
+        <v>165</v>
       </c>
       <c r="F233" s="1" t="s">
         <v>55</v>
@@ -6207,13 +6207,13 @@
         <v>6</v>
       </c>
       <c r="C234" s="12" t="s">
-        <v>198</v>
+        <v>177</v>
       </c>
       <c r="D234" s="9" t="s">
         <v>26</v>
       </c>
       <c r="E234" s="1" t="s">
-        <v>207</v>
+        <v>183</v>
       </c>
       <c r="F234" s="1" t="s">
         <v>55</v>
@@ -6227,13 +6227,13 @@
         <v>6</v>
       </c>
       <c r="C235" s="12" t="s">
-        <v>219</v>
+        <v>195</v>
       </c>
       <c r="D235" s="9" t="s">
         <v>26</v>
       </c>
       <c r="E235" s="1" t="s">
-        <v>228</v>
+        <v>202</v>
       </c>
       <c r="F235" s="1" t="s">
         <v>55</v>
@@ -6253,7 +6253,7 @@
         <v>14</v>
       </c>
       <c r="E236" s="1" t="s">
-        <v>341</v>
+        <v>311</v>
       </c>
       <c r="F236" s="1" t="s">
         <v>55</v>
@@ -6273,7 +6273,7 @@
         <v>14</v>
       </c>
       <c r="E237" s="1" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="F237" s="1" t="s">
         <v>55</v>
@@ -6287,13 +6287,13 @@
         <v>6</v>
       </c>
       <c r="C238" s="12" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="D238" s="9" t="s">
         <v>14</v>
       </c>
       <c r="E238" s="1" t="s">
-        <v>166</v>
+        <v>154</v>
       </c>
       <c r="F238" s="1" t="s">
         <v>55</v>
@@ -6307,13 +6307,13 @@
         <v>6</v>
       </c>
       <c r="C239" s="12" t="s">
-        <v>177</v>
+        <v>159</v>
       </c>
       <c r="D239" s="9" t="s">
         <v>14</v>
       </c>
       <c r="E239" s="1" t="s">
-        <v>187</v>
+        <v>166</v>
       </c>
       <c r="F239" s="1" t="s">
         <v>55</v>
@@ -6327,13 +6327,13 @@
         <v>6</v>
       </c>
       <c r="C240" s="12" t="s">
-        <v>198</v>
+        <v>177</v>
       </c>
       <c r="D240" s="9" t="s">
         <v>14</v>
       </c>
       <c r="E240" s="1" t="s">
-        <v>208</v>
+        <v>184</v>
       </c>
       <c r="F240" s="1" t="s">
         <v>55</v>
@@ -6347,13 +6347,13 @@
         <v>6</v>
       </c>
       <c r="C241" s="12" t="s">
-        <v>219</v>
+        <v>195</v>
       </c>
       <c r="D241" s="9" t="s">
         <v>14</v>
       </c>
       <c r="E241" s="1" t="s">
-        <v>229</v>
+        <v>343</v>
       </c>
       <c r="F241" s="1" t="s">
         <v>55</v>
@@ -6373,7 +6373,7 @@
         <v>30</v>
       </c>
       <c r="E242" s="1" t="s">
-        <v>343</v>
+        <v>313</v>
       </c>
       <c r="F242" s="1" t="s">
         <v>55</v>
@@ -6393,7 +6393,7 @@
         <v>30</v>
       </c>
       <c r="E243" s="1" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="F243" s="1" t="s">
         <v>55</v>
@@ -6407,13 +6407,13 @@
         <v>6</v>
       </c>
       <c r="C244" s="12" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="D244" s="9" t="s">
         <v>30</v>
       </c>
       <c r="E244" s="1" t="s">
-        <v>167</v>
+        <v>330</v>
       </c>
       <c r="F244" s="1" t="s">
         <v>55</v>
@@ -6427,13 +6427,13 @@
         <v>6</v>
       </c>
       <c r="C245" s="12" t="s">
-        <v>177</v>
+        <v>159</v>
       </c>
       <c r="D245" s="9" t="s">
         <v>30</v>
       </c>
       <c r="E245" s="1" t="s">
-        <v>188</v>
+        <v>167</v>
       </c>
       <c r="F245" s="1" t="s">
         <v>55</v>
@@ -6447,13 +6447,13 @@
         <v>6</v>
       </c>
       <c r="C246" s="12" t="s">
-        <v>198</v>
+        <v>177</v>
       </c>
       <c r="D246" s="9" t="s">
         <v>30</v>
       </c>
       <c r="E246" s="1" t="s">
-        <v>209</v>
+        <v>185</v>
       </c>
       <c r="F246" s="1" t="s">
         <v>55</v>
@@ -6467,13 +6467,13 @@
         <v>6</v>
       </c>
       <c r="C247" s="12" t="s">
-        <v>219</v>
+        <v>195</v>
       </c>
       <c r="D247" s="9" t="s">
         <v>30</v>
       </c>
       <c r="E247" s="1" t="s">
-        <v>230</v>
+        <v>203</v>
       </c>
       <c r="F247" s="1" t="s">
         <v>55</v>
@@ -6513,7 +6513,7 @@
         <v>15</v>
       </c>
       <c r="E249" s="1" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="F249" s="1" t="s">
         <v>55</v>
@@ -6527,13 +6527,13 @@
         <v>6</v>
       </c>
       <c r="C250" s="12" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="D250" s="9" t="s">
         <v>15</v>
       </c>
       <c r="E250" s="1" t="s">
-        <v>168</v>
+        <v>155</v>
       </c>
       <c r="F250" s="1" t="s">
         <v>55</v>
@@ -6547,13 +6547,13 @@
         <v>6</v>
       </c>
       <c r="C251" s="12" t="s">
-        <v>177</v>
+        <v>159</v>
       </c>
       <c r="D251" s="9" t="s">
         <v>15</v>
       </c>
       <c r="E251" s="1" t="s">
-        <v>189</v>
+        <v>168</v>
       </c>
       <c r="F251" s="1" t="s">
         <v>55</v>
@@ -6567,13 +6567,13 @@
         <v>6</v>
       </c>
       <c r="C252" s="12" t="s">
-        <v>198</v>
+        <v>177</v>
       </c>
       <c r="D252" s="9" t="s">
         <v>15</v>
       </c>
       <c r="E252" s="1" t="s">
-        <v>210</v>
+        <v>186</v>
       </c>
       <c r="F252" s="1" t="s">
         <v>55</v>
@@ -6587,13 +6587,13 @@
         <v>6</v>
       </c>
       <c r="C253" s="12" t="s">
-        <v>219</v>
+        <v>195</v>
       </c>
       <c r="D253" s="9" t="s">
         <v>15</v>
       </c>
       <c r="E253" s="1" t="s">
-        <v>231</v>
+        <v>204</v>
       </c>
       <c r="F253" s="1" t="s">
         <v>55</v>
@@ -6633,7 +6633,7 @@
         <v>16</v>
       </c>
       <c r="E255" s="1" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="F255" s="1" t="s">
         <v>55</v>
@@ -6647,13 +6647,13 @@
         <v>6</v>
       </c>
       <c r="C256" s="12" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="D256" s="9" t="s">
         <v>16</v>
       </c>
       <c r="E256" s="1" t="s">
-        <v>169</v>
+        <v>156</v>
       </c>
       <c r="F256" s="1" t="s">
         <v>55</v>
@@ -6667,13 +6667,13 @@
         <v>6</v>
       </c>
       <c r="C257" s="12" t="s">
-        <v>177</v>
+        <v>159</v>
       </c>
       <c r="D257" s="9" t="s">
         <v>16</v>
       </c>
       <c r="E257" s="1" t="s">
-        <v>190</v>
+        <v>169</v>
       </c>
       <c r="F257" s="1" t="s">
         <v>55</v>
@@ -6687,13 +6687,13 @@
         <v>6</v>
       </c>
       <c r="C258" s="12" t="s">
-        <v>198</v>
+        <v>177</v>
       </c>
       <c r="D258" s="9" t="s">
         <v>16</v>
       </c>
       <c r="E258" s="1" t="s">
-        <v>211</v>
+        <v>187</v>
       </c>
       <c r="F258" s="1" t="s">
         <v>55</v>
@@ -6707,13 +6707,13 @@
         <v>6</v>
       </c>
       <c r="C259" s="12" t="s">
-        <v>219</v>
+        <v>195</v>
       </c>
       <c r="D259" s="9" t="s">
         <v>16</v>
       </c>
       <c r="E259" s="1" t="s">
-        <v>232</v>
+        <v>205</v>
       </c>
       <c r="F259" s="1" t="s">
         <v>55</v>
@@ -6753,7 +6753,7 @@
         <v>17</v>
       </c>
       <c r="E261" s="1" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="F261" s="1" t="s">
         <v>55</v>
@@ -6767,13 +6767,13 @@
         <v>6</v>
       </c>
       <c r="C262" s="12" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="D262" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="E262" s="1" t="s">
-        <v>170</v>
+      <c r="E262" s="6" t="s">
+        <v>331</v>
       </c>
       <c r="F262" s="1" t="s">
         <v>55</v>
@@ -6787,13 +6787,13 @@
         <v>6</v>
       </c>
       <c r="C263" s="12" t="s">
-        <v>177</v>
+        <v>159</v>
       </c>
       <c r="D263" s="9" t="s">
         <v>17</v>
       </c>
       <c r="E263" s="1" t="s">
-        <v>191</v>
+        <v>170</v>
       </c>
       <c r="F263" s="1" t="s">
         <v>55</v>
@@ -6807,13 +6807,13 @@
         <v>6</v>
       </c>
       <c r="C264" s="12" t="s">
-        <v>198</v>
+        <v>177</v>
       </c>
       <c r="D264" s="9" t="s">
         <v>17</v>
       </c>
       <c r="E264" s="1" t="s">
-        <v>212</v>
+        <v>188</v>
       </c>
       <c r="F264" s="1" t="s">
         <v>55</v>
@@ -6827,13 +6827,13 @@
         <v>6</v>
       </c>
       <c r="C265" s="12" t="s">
-        <v>219</v>
+        <v>195</v>
       </c>
       <c r="D265" s="9" t="s">
         <v>17</v>
       </c>
       <c r="E265" s="1" t="s">
-        <v>233</v>
+        <v>206</v>
       </c>
       <c r="F265" s="1" t="s">
         <v>55</v>
@@ -6853,7 +6853,7 @@
         <v>29</v>
       </c>
       <c r="E266" s="1" t="s">
-        <v>344</v>
+        <v>314</v>
       </c>
       <c r="F266" s="1" t="s">
         <v>55</v>
@@ -6873,7 +6873,7 @@
         <v>29</v>
       </c>
       <c r="E267" s="1" t="s">
-        <v>150</v>
+        <v>321</v>
       </c>
       <c r="F267" s="1" t="s">
         <v>55</v>
@@ -6887,13 +6887,13 @@
         <v>6</v>
       </c>
       <c r="C268" s="12" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="D268" s="9" t="s">
         <v>29</v>
       </c>
       <c r="E268" s="1" t="s">
-        <v>171</v>
+        <v>157</v>
       </c>
       <c r="F268" s="1" t="s">
         <v>55</v>
@@ -6907,13 +6907,13 @@
         <v>6</v>
       </c>
       <c r="C269" s="12" t="s">
-        <v>177</v>
+        <v>159</v>
       </c>
       <c r="D269" s="9" t="s">
         <v>29</v>
       </c>
       <c r="E269" s="1" t="s">
-        <v>192</v>
+        <v>171</v>
       </c>
       <c r="F269" s="1" t="s">
         <v>55</v>
@@ -6927,13 +6927,13 @@
         <v>6</v>
       </c>
       <c r="C270" s="12" t="s">
-        <v>198</v>
+        <v>177</v>
       </c>
       <c r="D270" s="9" t="s">
         <v>29</v>
       </c>
       <c r="E270" s="1" t="s">
-        <v>213</v>
+        <v>189</v>
       </c>
       <c r="F270" s="1" t="s">
         <v>55</v>
@@ -6947,13 +6947,13 @@
         <v>6</v>
       </c>
       <c r="C271" s="12" t="s">
-        <v>219</v>
+        <v>195</v>
       </c>
       <c r="D271" s="9" t="s">
         <v>29</v>
       </c>
       <c r="E271" s="1" t="s">
-        <v>234</v>
+        <v>344</v>
       </c>
       <c r="F271" s="1" t="s">
         <v>55</v>
@@ -6973,7 +6973,7 @@
         <v>18</v>
       </c>
       <c r="E272" s="1" t="s">
-        <v>345</v>
+        <v>315</v>
       </c>
       <c r="F272" s="1" t="s">
         <v>55</v>
@@ -6993,7 +6993,7 @@
         <v>18</v>
       </c>
       <c r="E273" s="1" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="F273" s="1" t="s">
         <v>55</v>
@@ -7007,13 +7007,13 @@
         <v>6</v>
       </c>
       <c r="C274" s="12" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="D274" s="9" t="s">
         <v>18</v>
       </c>
       <c r="E274" s="1" t="s">
-        <v>172</v>
+        <v>332</v>
       </c>
       <c r="F274" s="1" t="s">
         <v>55</v>
@@ -7027,13 +7027,13 @@
         <v>6</v>
       </c>
       <c r="C275" s="12" t="s">
-        <v>177</v>
+        <v>159</v>
       </c>
       <c r="D275" s="9" t="s">
         <v>18</v>
       </c>
       <c r="E275" s="1" t="s">
-        <v>193</v>
+        <v>172</v>
       </c>
       <c r="F275" s="1" t="s">
         <v>55</v>
@@ -7047,13 +7047,13 @@
         <v>6</v>
       </c>
       <c r="C276" s="12" t="s">
-        <v>198</v>
+        <v>177</v>
       </c>
       <c r="D276" s="9" t="s">
         <v>18</v>
       </c>
       <c r="E276" s="1" t="s">
-        <v>214</v>
+        <v>190</v>
       </c>
       <c r="F276" s="1" t="s">
         <v>55</v>
@@ -7067,13 +7067,13 @@
         <v>6</v>
       </c>
       <c r="C277" s="12" t="s">
-        <v>219</v>
+        <v>195</v>
       </c>
       <c r="D277" s="9" t="s">
         <v>18</v>
       </c>
       <c r="E277" s="1" t="s">
-        <v>235</v>
+        <v>207</v>
       </c>
       <c r="F277" s="1" t="s">
         <v>55</v>
@@ -7093,7 +7093,7 @@
         <v>20</v>
       </c>
       <c r="E278" s="1" t="s">
-        <v>346</v>
+        <v>316</v>
       </c>
       <c r="F278" s="1" t="s">
         <v>55</v>
@@ -7113,7 +7113,7 @@
         <v>20</v>
       </c>
       <c r="E279" s="1" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="F279" s="1" t="s">
         <v>55</v>
@@ -7127,13 +7127,13 @@
         <v>6</v>
       </c>
       <c r="C280" s="12" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="D280" s="9" t="s">
         <v>20</v>
       </c>
       <c r="E280" s="1" t="s">
-        <v>173</v>
+        <v>323</v>
       </c>
       <c r="F280" s="1" t="s">
         <v>55</v>
@@ -7147,13 +7147,13 @@
         <v>6</v>
       </c>
       <c r="C281" s="12" t="s">
-        <v>177</v>
+        <v>159</v>
       </c>
       <c r="D281" s="9" t="s">
         <v>20</v>
       </c>
       <c r="E281" s="1" t="s">
-        <v>194</v>
+        <v>173</v>
       </c>
       <c r="F281" s="1" t="s">
         <v>55</v>
@@ -7167,13 +7167,13 @@
         <v>6</v>
       </c>
       <c r="C282" s="12" t="s">
-        <v>198</v>
+        <v>177</v>
       </c>
       <c r="D282" s="9" t="s">
         <v>20</v>
       </c>
       <c r="E282" s="1" t="s">
-        <v>215</v>
+        <v>191</v>
       </c>
       <c r="F282" s="1" t="s">
         <v>55</v>
@@ -7187,13 +7187,13 @@
         <v>6</v>
       </c>
       <c r="C283" s="12" t="s">
-        <v>219</v>
+        <v>195</v>
       </c>
       <c r="D283" s="9" t="s">
         <v>20</v>
       </c>
       <c r="E283" s="1" t="s">
-        <v>236</v>
+        <v>345</v>
       </c>
       <c r="F283" s="1" t="s">
         <v>55</v>
@@ -7233,7 +7233,7 @@
         <v>24</v>
       </c>
       <c r="E285" s="1" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="F285" s="1" t="s">
         <v>55</v>
@@ -7247,13 +7247,13 @@
         <v>6</v>
       </c>
       <c r="C286" s="12" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="D286" s="9" t="s">
         <v>24</v>
       </c>
       <c r="E286" s="1" t="s">
-        <v>174</v>
+        <v>333</v>
       </c>
       <c r="F286" s="1" t="s">
         <v>55</v>
@@ -7267,13 +7267,13 @@
         <v>6</v>
       </c>
       <c r="C287" s="12" t="s">
-        <v>177</v>
+        <v>159</v>
       </c>
       <c r="D287" s="9" t="s">
         <v>24</v>
       </c>
       <c r="E287" s="1" t="s">
-        <v>195</v>
+        <v>174</v>
       </c>
       <c r="F287" s="1" t="s">
         <v>55</v>
@@ -7287,13 +7287,13 @@
         <v>6</v>
       </c>
       <c r="C288" s="12" t="s">
-        <v>198</v>
+        <v>177</v>
       </c>
       <c r="D288" s="9" t="s">
         <v>24</v>
       </c>
       <c r="E288" s="1" t="s">
-        <v>216</v>
+        <v>192</v>
       </c>
       <c r="F288" s="1" t="s">
         <v>55</v>
@@ -7307,13 +7307,13 @@
         <v>6</v>
       </c>
       <c r="C289" s="12" t="s">
-        <v>219</v>
+        <v>195</v>
       </c>
       <c r="D289" s="9" t="s">
         <v>24</v>
       </c>
       <c r="E289" s="1" t="s">
-        <v>237</v>
+        <v>208</v>
       </c>
       <c r="F289" s="1" t="s">
         <v>55</v>
@@ -7333,7 +7333,7 @@
         <v>7</v>
       </c>
       <c r="E290" s="1" t="s">
-        <v>332</v>
+        <v>302</v>
       </c>
       <c r="F290" s="1" t="s">
         <v>55</v>
@@ -7353,7 +7353,7 @@
         <v>7</v>
       </c>
       <c r="E291" s="1" t="s">
-        <v>154</v>
+        <v>322</v>
       </c>
       <c r="F291" s="1" t="s">
         <v>55</v>
@@ -7367,13 +7367,13 @@
         <v>6</v>
       </c>
       <c r="C292" s="12" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="D292" s="9" t="s">
         <v>7</v>
       </c>
       <c r="E292" s="1" t="s">
-        <v>175</v>
+        <v>158</v>
       </c>
       <c r="F292" s="1" t="s">
         <v>55</v>
@@ -7387,13 +7387,13 @@
         <v>6</v>
       </c>
       <c r="C293" s="12" t="s">
-        <v>177</v>
+        <v>159</v>
       </c>
       <c r="D293" s="9" t="s">
         <v>7</v>
       </c>
       <c r="E293" s="1" t="s">
-        <v>196</v>
+        <v>175</v>
       </c>
       <c r="F293" s="1" t="s">
         <v>55</v>
@@ -7407,13 +7407,13 @@
         <v>6</v>
       </c>
       <c r="C294" s="12" t="s">
-        <v>198</v>
+        <v>177</v>
       </c>
       <c r="D294" s="9" t="s">
         <v>7</v>
       </c>
       <c r="E294" s="1" t="s">
-        <v>217</v>
+        <v>193</v>
       </c>
       <c r="F294" s="1" t="s">
         <v>55</v>
@@ -7427,13 +7427,13 @@
         <v>6</v>
       </c>
       <c r="C295" s="12" t="s">
-        <v>219</v>
+        <v>195</v>
       </c>
       <c r="D295" s="9" t="s">
         <v>7</v>
       </c>
       <c r="E295" s="1" t="s">
-        <v>238</v>
+        <v>209</v>
       </c>
       <c r="F295" s="1" t="s">
         <v>55</v>
@@ -7453,7 +7453,7 @@
         <v>9</v>
       </c>
       <c r="E296" s="1" t="s">
-        <v>333</v>
+        <v>303</v>
       </c>
       <c r="F296" s="1" t="s">
         <v>55</v>
@@ -7473,7 +7473,7 @@
         <v>9</v>
       </c>
       <c r="E297" s="1" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="F297" s="1" t="s">
         <v>55</v>
@@ -7487,13 +7487,13 @@
         <v>6</v>
       </c>
       <c r="C298" s="12" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="D298" s="9" t="s">
         <v>9</v>
       </c>
       <c r="E298" s="1" t="s">
-        <v>176</v>
+        <v>334</v>
       </c>
       <c r="F298" s="1" t="s">
         <v>55</v>
@@ -7507,13 +7507,13 @@
         <v>6</v>
       </c>
       <c r="C299" s="12" t="s">
-        <v>177</v>
+        <v>159</v>
       </c>
       <c r="D299" s="9" t="s">
         <v>9</v>
       </c>
       <c r="E299" s="1" t="s">
-        <v>197</v>
+        <v>176</v>
       </c>
       <c r="F299" s="1" t="s">
         <v>55</v>
@@ -7527,13 +7527,13 @@
         <v>6</v>
       </c>
       <c r="C300" s="12" t="s">
-        <v>198</v>
+        <v>177</v>
       </c>
       <c r="D300" s="9" t="s">
         <v>9</v>
       </c>
       <c r="E300" s="1" t="s">
-        <v>218</v>
+        <v>194</v>
       </c>
       <c r="F300" s="1" t="s">
         <v>55</v>
@@ -7547,13 +7547,13 @@
         <v>6</v>
       </c>
       <c r="C301" s="12" t="s">
-        <v>219</v>
+        <v>195</v>
       </c>
       <c r="D301" s="9" t="s">
         <v>9</v>
       </c>
       <c r="E301" s="1" t="s">
-        <v>239</v>
+        <v>346</v>
       </c>
       <c r="F301" s="1" t="s">
         <v>55</v>

</xml_diff>

<commit_message>
Diversify US related to "Pediatrics" and "Pharmacology" domain
</commit_message>
<xml_diff>
--- a/refair-server/datasets/few shot dataset/FSDataset.xlsx
+++ b/refair-server/datasets/few shot dataset/FSDataset.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\morel\Desktop\Refair\ReFair-App\refair-server\datasets\few shot dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C6647F8-BD0F-4B29-87BA-5D109868EBD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4ED0D1B-06BB-4C99-836D-27ACAC3DEAE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{80773445-FB61-4F04-A882-1600FD96C55A}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1506" uniqueCount="347">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1706" uniqueCount="389">
   <si>
     <t>Domain cluster</t>
   </si>
@@ -944,146 +944,272 @@
     <t>As a financial planner, I want to employ word embedding algorithms to cluster client financial goals and preferences based on their articulated needs and aspirations, facilitating personalized financial planning advice and strategies.</t>
   </si>
   <si>
-    <t>As a cardiovascular surgeon, I want voice recognition capabilities to dictate operative notes during complex procedures, so that I can ensure accurate documentation of surgical techniques and outcomes.</t>
-  </si>
-  <si>
-    <t>As a cardiology educator, I want word embedding models to map out semantic relationships between cardiovascular terms, so that I can create more effective teaching materials and curriculum.</t>
-  </si>
-  <si>
-    <t>As a cardiovascular surgeon, I want to use CNN-based segmentation algorithms to precisely delineate coronary arteries from angiography images, so that I can plan and perform interventions with greater accuracy.</t>
-  </si>
-  <si>
-    <t>As a cardiac nurse, I want a conversational agent to provide patients with post-discharge care instructions and reminders, so that I can ensure they follow their treatment plans and improve recovery outcomes.</t>
-  </si>
-  <si>
-    <t>As a cardiology department head, I want to utilize decision trees to analyze operational data and optimize resource allocation, so that I can improve the efficiency and quality of care provided by my department.</t>
-  </si>
-  <si>
-    <t>As a cardiology department head, I want to employ document classification algorithms to classify procedural guidelines and clinical protocols into different categories (e.g., diagnostic procedures, treatment algorithms), so that I can ensure consistent and standardized practices across the department.</t>
-  </si>
-  <si>
-    <t>As a cardiology clinician, I want to use entity extraction algorithms to identify and extract mentions of cardiac conditions (e.g., heart failure, atrial fibrillation) from patient notes and reports, so that I can prioritize care for patients with complex cardiovascular issues.</t>
-  </si>
-  <si>
-    <t>As a cardiology researcher, I want to use feature selection algorithms to identify the most relevant clinical variables (e.g., age, cholesterol levels, blood pressure) from large datasets of patient records, so that I can build accurate predictive models for cardiovascular risk assessment.</t>
-  </si>
-  <si>
-    <t>As a cardiology researcher, I want to address class imbalance in datasets related to rare cardiac diseases (e.g., myocarditis, pericardial effusion) using oversampling techniques, so that I can build robust predictive models and improve early detection strategies.</t>
-  </si>
-  <si>
-    <t>As a cardiologist, I want to use k-nearest neighbor (k-NN) algorithms to predict patient outcomes based on similar cases with known treatment responses, so that I can personalize treatment plans for my patients.</t>
-  </si>
-  <si>
-    <t>As a cardiology researcher, I want to develop a keyword extraction system to automatically identify key terms related to heart failure from a large corpus of clinical literature, so that I can conduct comprehensive literature reviews efficiently.</t>
-  </si>
-  <si>
-    <t>As a cardiology researcher, I want to develop a multi-label classification model to predict multiple comorbidities (e.g., diabetes, hypertension, obesity) in cardiac patients based on their clinical profiles, so that I can tailor personalized treatment plans.</t>
-  </si>
-  <si>
-    <t>As a cardiac rehabilitation specialist, I want to use sentiment analysis to evaluate patients' emotional responses in their progress notes, so that I can provide tailored support and interventions to improve their rehabilitation experience.</t>
-  </si>
-  <si>
-    <t>As a cardiac rehabilitation specialist, I want to implement speech-to-text technology to record patients' verbal feedback during rehabilitation sessions, so that I can efficiently capture and analyze their progress and concerns.</t>
-  </si>
-  <si>
-    <t>As a cardiology clinic manager, I want to use text categorization to automatically sort incoming emails and messages from patients and other healthcare providers into categories like appointment requests, medication inquiries, and general questions, so that I can streamline communication and improve response times.</t>
-  </si>
-  <si>
-    <t>As a dermatology clinic manager, I want to explore adversarial learning techniques to detect and counteract potential adversarial inputs that could compromise the privacy and security of patient data handled by our automated diagnostic systems.</t>
-  </si>
-  <si>
-    <t>As a dermatology clinic manager, I want to implement a decision tree algorithm that analyzes patient intake forms and clinical data to prioritize appointments, ensuring that patients with urgent dermatological conditions receive prompt attention and care.</t>
-  </si>
-  <si>
-    <t>As a dermatology clinic administrator, I want to utilize document classification algorithms to organize patient medical records by skin condition categories (e.g., eczema, psoriasis, melanoma) for efficient retrieval and comprehensive patient history analysis during consultations.</t>
-  </si>
-  <si>
-    <t>As a skincare researcher, I want to use feature selection algorithms to analyze genetic and environmental factors that contribute to acne severity, helping to prioritize biomarkers and relevant features for personalized treatment strategies in dermatology.</t>
-  </si>
-  <si>
-    <t>As a skincare marketing strategist, I want to employ sentiment analysis techniques to monitor social media sentiment around skincare trends and influencers, identifying emerging consumer preferences and sentiment shifts that could influence marketing campaigns and product development strategies.</t>
-  </si>
-  <si>
-    <t>As a skincare researcher, I want to utilize voice recognition software to transcribe and analyze qualitative interviews with dermatology patients about their skincare routines, preferences, and treatment experiences, extracting valuable insights for consumer behavior studies and product development strategies.</t>
-  </si>
-  <si>
-    <t>As a clinical endocrinologist, I want to utilize text categorization to classify patient notes and lab reports related to diabetes management, so that I can streamline the process of patient care and ensure timely adjustments to treatment plans.</t>
-  </si>
-  <si>
-    <t>As a researcher in endocrinology, I want to apply adversarial learning techniques to enhance the robustness of predictive models for insulin sensitivity prediction, so that I can provide more accurate assessments for diabetic patients across diverse demographics.</t>
-  </si>
-  <si>
-    <t>As an endocrinology department administrator, I want to implement a conversational agent across our clinic's website and mobile apps to provide patients with real-time answers to common questions about hormone therapies, appointment scheduling, and clinic services, enhancing patient engagement and satisfaction.</t>
-  </si>
-  <si>
-    <t>As a pediatric endocrinologist, I want to develop a decision tree algorithm to assist in diagnosing growth hormone deficiency in children, incorporating clinical symptoms, genetic markers, and growth charts to guide treatment decisions and optimize patient outcomes.</t>
-  </si>
-  <si>
-    <t>As an endocrinology department administrator, I want to implement a document classification model to automatically sort patient medical records based on specific endocrine conditions (e.g., hypothyroidism, Cushing's syndrome), enabling faster access to relevant patient information during consultations and follow-up visits.</t>
-  </si>
-  <si>
-    <t>As an endocrinologist specializing in thyroid disorders, I want to use feature selection algorithms to identify the most informative imaging features (e.g., nodule size, echogenicity, vascularity) from thyroid ultrasound scans, aiding in the differentiation between benign and malignant thyroid nodules.</t>
-  </si>
-  <si>
-    <t>As an endocrinology clinic administrator, I want to implement a keyword extraction model to automatically extract relevant terms (e.g., symptoms, medications) from patient intake forms and medical histories, enabling clinicians to quickly assess patient conditions during consultations.</t>
-  </si>
-  <si>
-    <t>As an endocrinology researcher, I want to develop a multi-label classification system to predict the risk of metabolic syndrome components (e.g., hypertension, dyslipidemia, central obesity) based on patient demographics, lifestyle factors, and biochemical markers, guiding preventive interventions and patient counseling.</t>
-  </si>
-  <si>
-    <t>As an endocrinology researcher, I want to develop a semantic similarity model to compare and correlate clinical notes from patient EHRs, identifying patterns and associations between symptoms, treatments, and disease progression in thyroid disorders.</t>
-  </si>
-  <si>
-    <t>As a researcher studying voice disorders in thyroid patients, I want to develop a speech to text application that accurately transcribes and analyzes voice recordings to detect subtle changes in speech patterns indicative of vocal cord dysfunction or nodules.</t>
-  </si>
-  <si>
-    <t>As an endocrinology clinic director, I want to employ unsupervised clustering methods to analyze patient demographic data and identify clusters of patients with similar patterns of hormone disorders (e.g., polycystic ovary syndrome, adrenal insufficiency), to optimize clinic workflows and resource allocation.</t>
-  </si>
-  <si>
-    <t>As an endocrinology educator, I want to develop word embeddings from textbooks and medical literature on pituitary disorders to create interactive learning tools that visualize and explore relationships between key concepts and clinical scenarios.</t>
-  </si>
-  <si>
-    <t>As a hospital administrator, I want to implement a conversational agent for appointment scheduling and patient reminders, utilizing natural language processing to handle patient inquiries efficiently and reduce administrative workload.</t>
-  </si>
-  <si>
-    <t>As a healthcare compliance officer, I want to deploy document classification models to classify patient records according to privacy sensitivity levels, ensuring compliance with data protection regulations such as HIPAA.</t>
-  </si>
-  <si>
-    <t>As a healthcare data analyst, I want to implement entity extraction algorithms to identify and extract medication names, dosages, and administration frequencies from electronic health records, facilitating medication reconciliation and adverse event monitoring.</t>
-  </si>
-  <si>
-    <t>As a medical researcher studying cancer diagnostics, I want to use adversarial learning techniques to detect and mitigate potential vulnerabilities in my deep learning models, so that I can ensure the reliability of automated tumor detection systems in clinical settings.</t>
-  </si>
-  <si>
-    <t>As a medical receptionist, I want to implement a conversational agent that can understand and respond to patient inquiries about clinic hours, services offered, and insurance coverage, so that we can provide accurate information to patients promptly.</t>
-  </si>
-  <si>
-    <t>As a clinical data analyst, I want to develop an entity extraction system to automatically identify and extract key clinical parameters (e.g., blood pressure, cholesterol levels) from unstructured patient notes, so that I can perform comprehensive population health analytics.</t>
-  </si>
-  <si>
-    <t>As a radiologist specializing in nephrology, I want to integrate CNN-based image classification models to differentiate between various types of renal tumors based on imaging features, assisting in accurate and timely diagnoses for my patients.</t>
-  </si>
-  <si>
-    <t>As a nephrology clinic manager, I want to utilize a conversational agent with machine learning algorithms to conduct preliminary assessments of symptoms reported by patients, assisting in prioritizing appointments and optimizing clinic workflow.</t>
-  </si>
-  <si>
-    <t>As a medical researcher studying renal genetics, I want to employ k-NN classification to identify genetic variants associated with familial nephropathies, facilitating genotype-phenotype correlations and advancing our understanding of inherited kidney diseases.</t>
-  </si>
-  <si>
-    <t>As a nephrology clinic administrator, I want to use sentiment analysis on patient surveys and feedback forms to assess caregiver attitudes and satisfaction with pediatric nephrology services, guiding quality improvement initiatives.</t>
-  </si>
-  <si>
-    <t>As a nephrology researcher, I want to use text categorization algorithms to classify nephrology conference abstracts into thematic categories such as acute kidney injury (AKI), chronic kidney disease (CKD), and renal replacement therapies, facilitating conference organization and academic collaboration.</t>
-  </si>
-  <si>
-    <t>As a nephrologist, I want to utilize word embedding techniques to analyze and categorize patient feedback from nephrology surveys and social media posts, identifying common themes and sentiments related to healthcare experiences.</t>
+    <t>As a dermatologist, I want to apply adversarial learning techniques to detect and mitigate potential attacks on dermatological image recognition models, ensuring robustness and reliability in automated diagnosis systems.</t>
+  </si>
+  <si>
+    <t>As an endocrinologist, I want to apply adversarial learning techniques to identify and mitigate potential vulnerabilities in hormone imbalance prediction models, ensuring robustness against adversarial attacks.</t>
+  </si>
+  <si>
+    <t>As a medical researcher, I want to apply adversarial learning techniques to analyze medical imaging data, so that I can identify and mitigate potential vulnerabilities and ensure the robustness of diagnostic models against adversarial attacks.</t>
+  </si>
+  <si>
+    <t>Pediatrics</t>
+  </si>
+  <si>
+    <t>As a pediatric clinical trial coordinator, I want to employ adversarial learning to detect and mitigate potential data poisoning attacks on clinical trial data, ensuring the integrity and reliability of experimental outcomes in pediatric drug trials.</t>
+  </si>
+  <si>
+    <t>Pharmacology</t>
+  </si>
+  <si>
+    <t>As a pharmaceutical data scientist, I want to leverage adversarial learning to improve the privacy and security of patient data in clinical trials, safeguarding sensitive information while maintaining the integrity of our research outcomes.</t>
+  </si>
+  <si>
+    <t>As a cardiologist, I want to explore CNN-based techniques for real-time analysis of wearable device data, such as continuous heart rate monitoring, to detect anomalies and provide timely alerts for patients with underlying cardiac conditions.</t>
+  </si>
+  <si>
+    <t>As a nephrologist, I want to utilize CNN models to predict the risk of acute kidney injury (AKI) in hospitalized patients based on a combination of clinical data and imaging findings, facilitating early intervention and patient management.</t>
+  </si>
+  <si>
+    <t>As a neonatologist, I want to develop CNN-based algorithms to automatically detect early signs of neonatal diseases from medical imaging scans, facilitating timely interventions and improving survival rates among premature infants.</t>
+  </si>
+  <si>
+    <t>As a pharmaceutical scientist, I want to apply CNNs to analyze medical imaging data such as MRI and CT scans to detect subtle changes indicative of drug-induced organ toxicity, improving safety assessments in preclinical studies.</t>
+  </si>
+  <si>
+    <t>As a cardiologist, I want to integrate a conversational agent into electronic health records (EHR) systems, enabling patients to easily access and update their medical histories and symptoms, facilitating more efficient and accurate clinical assessments.</t>
+  </si>
+  <si>
+    <t>As an endocrinologist, I want to develop a conversational agent powered by natural language processing to interact with patients, providing personalized guidance on managing diabetes through diet and lifestyle recommendations.</t>
+  </si>
+  <si>
+    <t>As a healthcare administrator, I want to develop a multilingual conversational agent using machine learning algorithms to assist international patients in navigating healthcare services, including appointment scheduling, insurance inquiries, and medical translation services.</t>
+  </si>
+  <si>
+    <t>As a medical researcher, I want to deploy a conversational agent for medical students to practice clinical case simulations and receive feedback on diagnostic reasoning and treatment planning, so that I can enhance medical training and competency development.</t>
+  </si>
+  <si>
+    <t>As a nephrologist, I want to deploy a conversational agent that can provide patients with personalized information about kidney disease management, including diet recommendations and lifestyle changes, to improve patient adherence and outcomes.</t>
+  </si>
+  <si>
+    <t>As a pediatrician, I want to develop a conversational agent using natural language processing to provide parents with accurate information about childhood illnesses and developmental milestones, ensuring they can make informed decisions about their child's health.</t>
+  </si>
+  <si>
+    <t>As a pharmaceutical researcher, I want to create a conversational agent using semantic parsing techniques to interpret and respond to inquiries about drug interactions and potential side effects, enhancing patient safety and medication adherence.</t>
+  </si>
+  <si>
+    <t>As a cardiologist, I want to construct decision tree models using patient demographics and medical history to predict the likelihood of adverse cardiac events within the next five years, aiding in early intervention and risk management strategies.</t>
+  </si>
+  <si>
+    <t>As a dermatologist, I want to utilize decision tree analysis to identify key risk factors for developing common dermatological conditions such as acne or eczema, enabling proactive preventive measures and patient education.</t>
+  </si>
+  <si>
+    <t>As an endocrinologist, I want to use a decision tree algorithm to predict the risk of developing type 2 diabetes based on patient demographics, lifestyle factors, and genetic predispositions, enabling early intervention strategies.</t>
+  </si>
+  <si>
+    <t>As a pediatric immunologist, I want to develop decision tree-based algorithms to personalize vaccination schedules for children based on individual health profiles, ensuring optimal protection against infectious diseases while minimizing adverse reactions.</t>
+  </si>
+  <si>
+    <t>As a pharmacologist, I want to build a decision tree model to classify patients into different risk groups for developing antibiotic resistance based on their medical history and microbiological data, aiding in personalized treatment plans.</t>
+  </si>
+  <si>
+    <t>As a cardiologist, I want to develop a document classification system to classify electronic health records (EHRs) based on patient symptoms and diagnostic tests, aiding in the identification of patterns and trends in cardiovascular diseases.</t>
+  </si>
+  <si>
+    <t>As a dermatologist, I want to develop a document classification model to automatically categorize research papers and clinical studies related to dermatological diseases, facilitating easier access to relevant literature for evidence-based practice.</t>
+  </si>
+  <si>
+    <t>As an endocrinologist, I want to develop a document classification system to automatically categorize patient medical records based on hormone profile data, streamlining the retrieval of information for treatment planning and research purposes.</t>
+  </si>
+  <si>
+    <t>As a healthcare administrator, I want to implement document classification algorithms to categorize and prioritize incoming medical reports (e.g., radiology, pathology) based on urgency and clinical significance, facilitating timely review and decision-making by healthcare professionals.</t>
+  </si>
+  <si>
+    <t>As a pediatric hospital administrator, I want to implement document classification using natural language processing to automatically categorize and tag electronic health records (EHRs) of pediatric patients, improving data retrieval efficiency and compliance with medical record standards.</t>
+  </si>
+  <si>
+    <t>As a pharmacologist, I want to employ document classification techniques to automatically categorize research papers and clinical trial reports based on drug efficacy, enabling quicker access to relevant studies for evidence-based decision-making.</t>
+  </si>
+  <si>
+    <t>As a cardiologist, I want to develop an entity extraction system to automatically identify and extract key cardiac parameters (e.g., ejection fraction, QT interval) from clinical notes and reports, enabling faster analysis and decision-making.</t>
+  </si>
+  <si>
+    <t>As a healthcare provider, I want to deploy machine learning models for entity extraction in clinical trials documentation, to automatically extract and categorize information on study protocols, participant demographics, and treatment outcomes, facilitating efficient research data management and analysis.</t>
+  </si>
+  <si>
+    <t>As a medical researcher, I want to develop entity extraction models to automatically identify and extract key medical entities (e.g., diseases, medications, symptoms) from clinical notes and patient records, so that I can build comprehensive patient profiles for personalized treatment planning.</t>
+  </si>
+  <si>
+    <t>As a pediatric pharmacist, I want to develop entity extraction models to identify and extract drug names, dosages, and interactions mentioned in pediatric patient medication records, ensuring safe and effective medication management for young patients.</t>
+  </si>
+  <si>
+    <t>As a researcher in pharmacology, I want to utilize entity extraction algorithms to extract molecular entities and their interactions from biomedical literature, aiding in the discovery of novel drug targets and therapeutic mechanisms.</t>
+  </si>
+  <si>
+    <t>As a cardiologist, I want to apply feature selection methods to filter out irrelevant or redundant features from ECG data, so that I can enhance the performance of algorithms detecting cardiac arrhythmias.</t>
+  </si>
+  <si>
+    <t>As a dermatologist, I want to perform feature selection on dermatological image data to identify the most discriminative features that contribute to accurate classification of skin lesions, enhancing diagnostic precision.</t>
+  </si>
+  <si>
+    <t>As an endocrinologist, I want to use feature selection algorithms to prioritize genetic markers linked to thyroid cancer susceptibility in familial studies, facilitating targeted screening and early detection strategies.</t>
+  </si>
+  <si>
+    <t>As a pediatric pulmonologist, I want to use feature selection techniques to identify the most significant clinical and environmental factors influencing asthma severity and treatment response in children, facilitating personalized asthma management plans for each patient.</t>
+  </si>
+  <si>
+    <t>As a pharmaceutical researcher, I want to use feature selection algorithms to identify molecular descriptors that correlate with drug efficacy and safety profiles, aiding in the prioritization of lead compounds for further preclinical testing.</t>
+  </si>
+  <si>
+    <t>As a cardiologist, I want to use keyword extraction algorithms to extract relevant terms from medical literature and clinical guidelines pertaining to cardiac rehabilitation protocols, aiding in the development of evidence-based treatment plans.</t>
+  </si>
+  <si>
+    <t>As a pediatric geneticist, I want to address the challenge of imbalanced datasets in genomic studies by developing algorithms that can accurately detect and classify rare genetic disorders in children, enabling early diagnosis and personalized treatment planning.</t>
+  </si>
+  <si>
+    <t>As a pharmacologist, I want to address class imbalance in adverse event datasets using techniques like oversampling and ensemble learning, to improve the detection and reporting of rare but serious drug side effects during clinical trials.</t>
+  </si>
+  <si>
+    <t>As a cardiologist, I want to address class imbalance in datasets used for predicting rare cardiac conditions using machine learning algorithms, ensuring accurate identification and early intervention for patients at higher risk.</t>
+  </si>
+  <si>
+    <t>As an endocrinologist, I want to develop a keyword extraction system to automatically identify relevant terms from clinical notes and research articles related to hypothyroidism, facilitating comprehensive literature review and evidence synthesis.</t>
+  </si>
+  <si>
+    <t>As a pediatric pharmacist, I want to employ keyword extraction methods to analyze prescription notes and identify key medications, dosages, and associated instructions for pediatric patients, ensuring accurate medication management and patient safety.</t>
+  </si>
+  <si>
+    <t>As a pharmacologist, I want to develop a keyword extraction system to automatically identify key drug interactions mentioned in medical literature and pharmacovigilance reports, aiding in the compilation of comprehensive drug safety profiles.</t>
+  </si>
+  <si>
+    <t>As a cardiologist, I want to use k-NN models to predict patient-specific responses to different cardiac medications based on similar patient profiles, facilitating personalized treatment plans for heart disease management.</t>
+  </si>
+  <si>
+    <t>As a nephrologist, I want to use k-Nearest Neighbor (k-NN) algorithms to predict the risk of acute kidney injury (AKI) in hospitalized patients based on similarities to previous AKI cases with similar clinical profiles, enabling early intervention strategies.</t>
+  </si>
+  <si>
+    <t>As a pediatric pulmonologist, I want to implement a k-NN classifier to predict asthma severity levels in pediatric patients based on similar historical cases, guiding treatment decisions and improving asthma control strategies.</t>
+  </si>
+  <si>
+    <t>As a pharmaceutical researcher, I want to use k-nearest neighbor classification to predict patient responses to novel drug therapies based on similarities to known patient cohorts with similar genetic backgrounds and disease profiles.</t>
+  </si>
+  <si>
+    <t>As a cardiologist, I want to implement multi-label classification algorithms to classify cardiac imaging studies (e.g., echocardiograms, CT scans) into multiple diagnostic categories (e.g., valve disease, myocardial infarction), aiding in accurate disease characterization.</t>
+  </si>
+  <si>
+    <t>As an endocrinologist, I want to implement multi-label classification algorithms to classify patients with adrenal gland disorders into multiple categories (e.g., Cushing's syndrome, adrenal insufficiency), facilitating accurate diagnosis and tailored management approaches.</t>
+  </si>
+  <si>
+    <t>As a pediatric nutritionist, I want to implement a multi-label classification system to assess and classify pediatric patients' nutritional needs based on their dietary habits, medical conditions, and growth patterns, optimizing personalized nutrition plans.</t>
+  </si>
+  <si>
+    <t>As a pharmaceutical researcher, I want to implement multi-label classification algorithms to classify drugs into multiple therapeutic categories simultaneously, enabling comprehensive drug profiling and comparison studies.</t>
+  </si>
+  <si>
+    <t>As a pediatric cardiologist, I want to develop a neural network model to accurately predict cardiac anomalies in pediatric patients based on medical imaging data, enabling early detection and intervention for congenital heart conditions.</t>
+  </si>
+  <si>
+    <t>As a pharmaceutical researcher, I want to use neural networks to analyze high-dimensional molecular data and identify novel biomarkers associated with drug response variability across diverse patient populations.</t>
+  </si>
+  <si>
+    <t>As a pediatric pulmonologist, I want to develop a random forest model to predict the likelihood of asthma exacerbations in pediatric patients based on various clinical and environmental factors, guiding proactive management strategies and reducing hospitalizations.</t>
+  </si>
+  <si>
+    <t>As a pharmacologist, I want to build a random forest model to predict drug-drug interactions based on molecular features and patient-specific factors extracted from electronic health records (EHRs).</t>
+  </si>
+  <si>
+    <t>As an endocrinologist, I want to use semantic similarity techniques to match patient symptoms with known disease patterns in rare endocrine disorders, supporting early detection and personalized treatment approaches.</t>
+  </si>
+  <si>
+    <t>As a pediatrician, I want to use semantic similarity techniques to match reported symptoms from pediatric patients to a database of medical knowledge, aiding in accurate diagnosis and treatment recommendations.</t>
+  </si>
+  <si>
+    <t>As a pharmaceutical researcher, I want to use semantic similarity techniques to analyze biomedical literature and identify relationships between molecular pathways and disease mechanisms relevant to cardiovascular disorders.</t>
+  </si>
+  <si>
+    <t>As a cardiologist, I want to implement sentiment analysis on patient feedback from cardiac rehabilitation programs to assess overall patient satisfaction and identify areas for program improvement.</t>
+  </si>
+  <si>
+    <t>As a dermatologist, I want to develop a sentiment analysis model to analyze social media posts and reviews related to skincare products, identifying sentiments and trends among consumers to inform product recommendations.</t>
+  </si>
+  <si>
+    <t>As a nephrologist, I want to develop a sentiment analysis model to analyze social media discussions and patient forums related to kidney transplantation experiences, to gauge patient emotions and concerns post-surgery.</t>
+  </si>
+  <si>
+    <t>As a pediatric hospital administrator, I want to perform sentiment analysis on feedback and reviews provided by parents about pediatric healthcare services, identifying areas of satisfaction and areas needing improvement to enhance patient experience.</t>
+  </si>
+  <si>
+    <t>As a pharmaceutical researcher, I want to apply sentiment analysis techniques to analyze feedback from clinical trial participants regarding the tolerability and efficacy of a new heart disease treatment, aiding in drug development decisions.</t>
+  </si>
+  <si>
+    <t>As a cardiologist, I want to develop a speech to text system to transcribe cardiology consultations and patient histories accurately, improving documentation efficiency and clinical workflow.</t>
+  </si>
+  <si>
+    <t>As an endocrinologist, I want to use speech to text capabilities to convert endocrine conference recordings into text format, enabling easy access to discussions on recent research findings and clinical case studies.</t>
+  </si>
+  <si>
+    <t>As a pediatric speech therapist, I want to use speech-to-text systems to transcribe speech and language therapy sessions for pediatric patients, aiding in progress tracking, treatment planning, and communication with caregivers.</t>
+  </si>
+  <si>
+    <t>As a pharmaceutical researcher, I want to convert recorded interviews with key opinion leaders in cardiology into text format using speech to text technology, enabling detailed analysis of insights into emerging therapies and treatment guidelines.</t>
+  </si>
+  <si>
+    <t>As a cardiologist, I want to develop a text categorization model to classify medical literature and research articles on various cardiac conditions (e.g., myocardial infarction, arrhythmias) for easier access and knowledge synthesis.</t>
+  </si>
+  <si>
+    <t>As an endocrinologist, I want to use text categorization techniques to classify patient electronic health records based on different types of hormonal disorders (e.g., adrenal gland disorders, pituitary gland disorders), enabling efficient retrieval and analysis of relevant patient data.</t>
+  </si>
+  <si>
+    <t>As a nephrologist, I want to develop a text categorization system to classify nephrology research articles into categories such as chronic kidney disease epidemiology, renal replacement therapies, and nephrotoxicity studies, facilitating literature review and research synthesis.</t>
+  </si>
+  <si>
+    <t>As a pediatric researcher, I want to develop a text categorization system to classify research articles related to pediatric diseases and treatments into relevant categories (e.g., epidemiology, treatment outcomes), facilitating efficient literature review and research synthesis.</t>
+  </si>
+  <si>
+    <t>As a pharmacologist, I want to use text categorization to classify research articles into categories such as drug efficacy, adverse effects, and pharmacokinetics, so that I can quickly access relevant literature for my studies.</t>
+  </si>
+  <si>
+    <t>As an endocrinologist, I want to use unsupervised clustering techniques to cluster symptoms reported by patients with polycystic ovary syndrome (PCOS), identifying common symptom patterns and guiding individualized management plans.</t>
+  </si>
+  <si>
+    <t>As a pediatric geneticist, I want to use unsupervised clustering techniques to group and cluster pediatric genetic profiles based on similarities in genetic mutations and variations, aiding in the identification of novel genetic associations and disease pathways.</t>
+  </si>
+  <si>
+    <t>As a pharmacologist, I want to apply unsupervised clustering to group patient demographic data based on medical history, genetic markers, and lifestyle factors, so that I can identify subpopulations for personalized medicine approaches.</t>
+  </si>
+  <si>
+    <t>As a cardiologist, I want to develop a voice recognition system to accurately transcribe cardiology consultations and patient histories from audio recordings, improving documentation accuracy and efficiency.</t>
+  </si>
+  <si>
+    <t>As a dermatologist, I want to implement voice recognition technology to capture patient-reported symptoms and medical histories accurately during dermatological consultations, enhancing data quality and clinical decision-making.</t>
+  </si>
+  <si>
+    <t>As a pediatric surgeon, I want to use voice recognition systems to dictate operative and procedure notes during pediatric surgeries, ensuring timely and accurate documentation of surgical details for medical records.</t>
+  </si>
+  <si>
+    <t>As a clinical pharmacist, I want to implement voice recognition technology to transcribe patient consultations accurately, so that I can efficiently document medication histories and adherence behaviors.</t>
+  </si>
+  <si>
+    <t>As a cardiologist, I want to utilize word embedding techniques to represent clinical terms and medical concepts from cardiology literature, enabling more accurate semantic understanding and retrieval of relevant research findings.</t>
+  </si>
+  <si>
+    <t>As an endocrinologist, I want to use word embedding techniques to analyze similarities and relationships between medical terms in research literature on insulin resistance, aiding in the discovery of novel associations and mechanisms.</t>
+  </si>
+  <si>
+    <t>As a nephrologist, I want to deploy word embedding models to support automated summarization of nephrology research articles and clinical trials, extracting key concepts and findings to aid in evidence-based decision-making and research synthesis.</t>
+  </si>
+  <si>
+    <t>As a pediatric researcher, I want to utilize word embedding techniques to analyze medical texts related to pediatric diseases and treatments, extracting semantic similarities and patterns to uncover novel insights and research directions.</t>
+  </si>
+  <si>
+    <t>As a drug safety analyst, I want to utilize word embedding to map adverse event descriptions to vector spaces, facilitating automated signal detection and identification of potential safety issues associated with specific drug classes.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1115,6 +1241,11 @@
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="7">
@@ -1167,7 +1298,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1190,6 +1321,16 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -1524,10 +1665,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8DF0B04-8323-4309-B759-D1CDDA1FBB0E}">
-  <dimension ref="A1:F301"/>
+  <dimension ref="A1:F341"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C289" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C301" sqref="C301"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -5163,16 +5304,16 @@
       <c r="A182" s="12" t="s">
         <v>128</v>
       </c>
-      <c r="B182" s="12">
-        <v>6</v>
-      </c>
-      <c r="C182" s="12" t="s">
+      <c r="B182" s="14">
+        <v>6</v>
+      </c>
+      <c r="C182" s="14" t="s">
         <v>129</v>
       </c>
       <c r="D182" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="E182" s="1" t="s">
+      <c r="E182" s="15" t="s">
         <v>130</v>
       </c>
       <c r="F182" s="1" t="s">
@@ -5192,47 +5333,47 @@
       <c r="D183" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="E183" s="1" t="s">
-        <v>317</v>
+      <c r="E183" s="15" t="s">
+        <v>302</v>
       </c>
       <c r="F183" s="1" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="184" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A184" s="12" t="s">
-        <v>128</v>
-      </c>
-      <c r="B184" s="12">
-        <v>6</v>
-      </c>
-      <c r="C184" s="12" t="s">
+      <c r="A184" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="B184" s="14">
+        <v>6</v>
+      </c>
+      <c r="C184" s="14" t="s">
         <v>150</v>
       </c>
       <c r="D184" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="E184" s="1" t="s">
-        <v>324</v>
+      <c r="E184" s="15" t="s">
+        <v>303</v>
       </c>
       <c r="F184" s="1" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="185" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A185" s="12" t="s">
-        <v>128</v>
-      </c>
-      <c r="B185" s="12">
-        <v>6</v>
-      </c>
-      <c r="C185" s="12" t="s">
+      <c r="A185" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="B185" s="14">
+        <v>6</v>
+      </c>
+      <c r="C185" s="14" t="s">
         <v>159</v>
       </c>
       <c r="D185" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="E185" s="1" t="s">
+      <c r="E185" s="15" t="s">
         <v>160</v>
       </c>
       <c r="F185" s="1" t="s">
@@ -5240,20 +5381,20 @@
       </c>
     </row>
     <row r="186" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A186" s="12" t="s">
-        <v>128</v>
-      </c>
-      <c r="B186" s="12">
-        <v>6</v>
-      </c>
-      <c r="C186" s="12" t="s">
+      <c r="A186" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="B186" s="14">
+        <v>6</v>
+      </c>
+      <c r="C186" s="14" t="s">
         <v>177</v>
       </c>
       <c r="D186" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="E186" s="1" t="s">
-        <v>338</v>
+      <c r="E186" s="15" t="s">
+        <v>304</v>
       </c>
       <c r="F186" s="1" t="s">
         <v>55</v>
@@ -5272,7 +5413,7 @@
       <c r="D187" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="E187" s="1" t="s">
+      <c r="E187" s="15" t="s">
         <v>196</v>
       </c>
       <c r="F187" s="1" t="s">
@@ -5280,60 +5421,60 @@
       </c>
     </row>
     <row r="188" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A188" s="12" t="s">
-        <v>128</v>
-      </c>
-      <c r="B188" s="12">
-        <v>6</v>
-      </c>
-      <c r="C188" s="12" t="s">
+      <c r="A188" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="B188" s="14">
+        <v>6</v>
+      </c>
+      <c r="C188" s="14" t="s">
+        <v>305</v>
+      </c>
+      <c r="D188" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="E188" s="15" t="s">
+        <v>306</v>
+      </c>
+      <c r="F188" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="189" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A189" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="B189" s="14">
+        <v>6</v>
+      </c>
+      <c r="C189" s="14" t="s">
+        <v>307</v>
+      </c>
+      <c r="D189" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="E189" s="15" t="s">
+        <v>308</v>
+      </c>
+      <c r="F189" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="190" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A190" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="B190" s="14">
+        <v>6</v>
+      </c>
+      <c r="C190" s="14" t="s">
         <v>129</v>
-      </c>
-      <c r="D188" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="E188" s="1" t="s">
-        <v>304</v>
-      </c>
-      <c r="F188" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="189" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A189" s="12" t="s">
-        <v>128</v>
-      </c>
-      <c r="B189" s="12">
-        <v>6</v>
-      </c>
-      <c r="C189" s="12" t="s">
-        <v>135</v>
-      </c>
-      <c r="D189" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="E189" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="F189" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="190" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A190" s="12" t="s">
-        <v>128</v>
-      </c>
-      <c r="B190" s="12">
-        <v>6</v>
-      </c>
-      <c r="C190" s="12" t="s">
-        <v>150</v>
       </c>
       <c r="D190" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="E190" s="1" t="s">
-        <v>151</v>
+      <c r="E190" s="15" t="s">
+        <v>309</v>
       </c>
       <c r="F190" s="1" t="s">
         <v>55</v>
@@ -5347,73 +5488,73 @@
         <v>6</v>
       </c>
       <c r="C191" s="12" t="s">
-        <v>159</v>
+        <v>135</v>
       </c>
       <c r="D191" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="E191" s="1" t="s">
-        <v>161</v>
+      <c r="E191" s="15" t="s">
+        <v>136</v>
       </c>
       <c r="F191" s="1" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="192" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A192" s="12" t="s">
-        <v>128</v>
-      </c>
-      <c r="B192" s="12">
-        <v>6</v>
-      </c>
-      <c r="C192" s="12" t="s">
-        <v>177</v>
+      <c r="A192" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="B192" s="14">
+        <v>6</v>
+      </c>
+      <c r="C192" s="14" t="s">
+        <v>150</v>
       </c>
       <c r="D192" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="E192" s="1" t="s">
-        <v>178</v>
+      <c r="E192" s="15" t="s">
+        <v>151</v>
       </c>
       <c r="F192" s="1" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="193" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A193" s="12" t="s">
-        <v>128</v>
-      </c>
-      <c r="B193" s="12">
-        <v>6</v>
-      </c>
-      <c r="C193" s="12" t="s">
-        <v>195</v>
+      <c r="A193" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="B193" s="14">
+        <v>6</v>
+      </c>
+      <c r="C193" s="14" t="s">
+        <v>159</v>
       </c>
       <c r="D193" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="E193" s="1" t="s">
-        <v>341</v>
+      <c r="E193" s="15" t="s">
+        <v>161</v>
       </c>
       <c r="F193" s="1" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="194" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A194" s="12" t="s">
-        <v>128</v>
-      </c>
-      <c r="B194" s="12">
-        <v>6</v>
-      </c>
-      <c r="C194" s="12" t="s">
-        <v>129</v>
+      <c r="A194" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="B194" s="14">
+        <v>6</v>
+      </c>
+      <c r="C194" s="14" t="s">
+        <v>177</v>
       </c>
       <c r="D194" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="E194" s="1" t="s">
-        <v>305</v>
+        <v>32</v>
+      </c>
+      <c r="E194" s="15" t="s">
+        <v>178</v>
       </c>
       <c r="F194" s="1" t="s">
         <v>55</v>
@@ -5427,73 +5568,73 @@
         <v>6</v>
       </c>
       <c r="C195" s="12" t="s">
-        <v>135</v>
+        <v>195</v>
       </c>
       <c r="D195" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="E195" s="1" t="s">
-        <v>137</v>
+        <v>32</v>
+      </c>
+      <c r="E195" s="15" t="s">
+        <v>310</v>
       </c>
       <c r="F195" s="1" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="196" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A196" s="12" t="s">
-        <v>128</v>
-      </c>
-      <c r="B196" s="12">
-        <v>6</v>
-      </c>
-      <c r="C196" s="12" t="s">
-        <v>150</v>
+      <c r="A196" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="B196" s="14">
+        <v>6</v>
+      </c>
+      <c r="C196" s="14" t="s">
+        <v>305</v>
       </c>
       <c r="D196" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="E196" s="1" t="s">
-        <v>325</v>
+        <v>32</v>
+      </c>
+      <c r="E196" s="15" t="s">
+        <v>311</v>
       </c>
       <c r="F196" s="1" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="197" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A197" s="12" t="s">
-        <v>128</v>
-      </c>
-      <c r="B197" s="12">
-        <v>6</v>
-      </c>
-      <c r="C197" s="12" t="s">
-        <v>159</v>
+      <c r="A197" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="B197" s="14">
+        <v>6</v>
+      </c>
+      <c r="C197" s="14" t="s">
+        <v>307</v>
       </c>
       <c r="D197" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="E197" s="1" t="s">
-        <v>335</v>
+        <v>32</v>
+      </c>
+      <c r="E197" s="15" t="s">
+        <v>312</v>
       </c>
       <c r="F197" s="1" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="198" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A198" s="12" t="s">
-        <v>128</v>
-      </c>
-      <c r="B198" s="12">
-        <v>6</v>
-      </c>
-      <c r="C198" s="12" t="s">
-        <v>177</v>
+      <c r="A198" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="B198" s="14">
+        <v>6</v>
+      </c>
+      <c r="C198" s="14" t="s">
+        <v>129</v>
       </c>
       <c r="D198" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="E198" s="1" t="s">
-        <v>339</v>
+      <c r="E198" s="15" t="s">
+        <v>313</v>
       </c>
       <c r="F198" s="1" t="s">
         <v>55</v>
@@ -5507,73 +5648,73 @@
         <v>6</v>
       </c>
       <c r="C199" s="12" t="s">
-        <v>195</v>
+        <v>135</v>
       </c>
       <c r="D199" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="E199" s="1" t="s">
-        <v>342</v>
+      <c r="E199" s="15" t="s">
+        <v>137</v>
       </c>
       <c r="F199" s="1" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="200" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A200" s="12" t="s">
-        <v>128</v>
-      </c>
-      <c r="B200" s="12">
-        <v>6</v>
-      </c>
-      <c r="C200" s="12" t="s">
-        <v>129</v>
+      <c r="A200" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="B200" s="14">
+        <v>6</v>
+      </c>
+      <c r="C200" s="14" t="s">
+        <v>150</v>
       </c>
       <c r="D200" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="E200" s="1" t="s">
-        <v>306</v>
+        <v>23</v>
+      </c>
+      <c r="E200" s="15" t="s">
+        <v>314</v>
       </c>
       <c r="F200" s="1" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="201" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A201" s="12" t="s">
-        <v>128</v>
-      </c>
-      <c r="B201" s="12">
-        <v>6</v>
-      </c>
-      <c r="C201" s="12" t="s">
-        <v>135</v>
+      <c r="A201" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="B201" s="14">
+        <v>6</v>
+      </c>
+      <c r="C201" s="14" t="s">
+        <v>159</v>
       </c>
       <c r="D201" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="E201" s="1" t="s">
-        <v>318</v>
+        <v>23</v>
+      </c>
+      <c r="E201" s="15" t="s">
+        <v>315</v>
       </c>
       <c r="F201" s="1" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="202" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A202" s="12" t="s">
-        <v>128</v>
-      </c>
-      <c r="B202" s="12">
-        <v>6</v>
-      </c>
-      <c r="C202" s="12" t="s">
-        <v>150</v>
+      <c r="A202" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="B202" s="14">
+        <v>6</v>
+      </c>
+      <c r="C202" s="14" t="s">
+        <v>177</v>
       </c>
       <c r="D202" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="E202" s="1" t="s">
-        <v>326</v>
+        <v>23</v>
+      </c>
+      <c r="E202" s="15" t="s">
+        <v>316</v>
       </c>
       <c r="F202" s="1" t="s">
         <v>55</v>
@@ -5587,73 +5728,73 @@
         <v>6</v>
       </c>
       <c r="C203" s="12" t="s">
-        <v>159</v>
+        <v>195</v>
       </c>
       <c r="D203" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="E203" s="15" t="s">
+        <v>317</v>
+      </c>
+      <c r="F203" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="204" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A204" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="B204" s="14">
+        <v>6</v>
+      </c>
+      <c r="C204" s="14" t="s">
+        <v>305</v>
+      </c>
+      <c r="D204" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="E204" s="15" t="s">
+        <v>318</v>
+      </c>
+      <c r="F204" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="205" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A205" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="B205" s="14">
+        <v>6</v>
+      </c>
+      <c r="C205" s="14" t="s">
+        <v>307</v>
+      </c>
+      <c r="D205" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="E205" s="15" t="s">
+        <v>319</v>
+      </c>
+      <c r="F205" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="206" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A206" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="B206" s="14">
+        <v>6</v>
+      </c>
+      <c r="C206" s="14" t="s">
+        <v>129</v>
+      </c>
+      <c r="D206" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="E203" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="F203" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="204" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A204" s="12" t="s">
-        <v>128</v>
-      </c>
-      <c r="B204" s="12">
-        <v>6</v>
-      </c>
-      <c r="C204" s="12" t="s">
-        <v>177</v>
-      </c>
-      <c r="D204" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="E204" s="1" t="s">
-        <v>179</v>
-      </c>
-      <c r="F204" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="205" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A205" s="12" t="s">
-        <v>128</v>
-      </c>
-      <c r="B205" s="12">
-        <v>6</v>
-      </c>
-      <c r="C205" s="12" t="s">
-        <v>195</v>
-      </c>
-      <c r="D205" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="E205" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="F205" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="206" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A206" s="12" t="s">
-        <v>128</v>
-      </c>
-      <c r="B206" s="12">
-        <v>6</v>
-      </c>
-      <c r="C206" s="12" t="s">
-        <v>129</v>
-      </c>
-      <c r="D206" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="E206" s="1" t="s">
-        <v>307</v>
+      <c r="E206" s="15" t="s">
+        <v>320</v>
       </c>
       <c r="F206" s="1" t="s">
         <v>55</v>
@@ -5670,70 +5811,70 @@
         <v>135</v>
       </c>
       <c r="D207" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="E207" s="1" t="s">
-        <v>319</v>
+        <v>12</v>
+      </c>
+      <c r="E207" s="15" t="s">
+        <v>321</v>
       </c>
       <c r="F207" s="1" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="208" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A208" s="12" t="s">
-        <v>128</v>
-      </c>
-      <c r="B208" s="12">
-        <v>6</v>
-      </c>
-      <c r="C208" s="12" t="s">
+      <c r="A208" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="B208" s="14">
+        <v>6</v>
+      </c>
+      <c r="C208" s="14" t="s">
         <v>150</v>
       </c>
       <c r="D208" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="E208" s="1" t="s">
-        <v>327</v>
+        <v>12</v>
+      </c>
+      <c r="E208" s="15" t="s">
+        <v>322</v>
       </c>
       <c r="F208" s="1" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="209" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A209" s="12" t="s">
-        <v>128</v>
-      </c>
-      <c r="B209" s="12">
-        <v>6</v>
-      </c>
-      <c r="C209" s="12" t="s">
+      <c r="A209" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="B209" s="14">
+        <v>6</v>
+      </c>
+      <c r="C209" s="14" t="s">
         <v>159</v>
       </c>
       <c r="D209" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="E209" s="1" t="s">
-        <v>336</v>
+        <v>12</v>
+      </c>
+      <c r="E209" s="15" t="s">
+        <v>162</v>
       </c>
       <c r="F209" s="1" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="210" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A210" s="12" t="s">
-        <v>128</v>
-      </c>
-      <c r="B210" s="12">
-        <v>6</v>
-      </c>
-      <c r="C210" s="12" t="s">
+      <c r="A210" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="B210" s="14">
+        <v>6</v>
+      </c>
+      <c r="C210" s="14" t="s">
         <v>177</v>
       </c>
       <c r="D210" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="E210" s="1" t="s">
-        <v>180</v>
+        <v>12</v>
+      </c>
+      <c r="E210" s="15" t="s">
+        <v>179</v>
       </c>
       <c r="F210" s="1" t="s">
         <v>55</v>
@@ -5750,70 +5891,70 @@
         <v>195</v>
       </c>
       <c r="D211" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="E211" s="15" t="s">
+        <v>197</v>
+      </c>
+      <c r="F211" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="212" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A212" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="B212" s="14">
+        <v>6</v>
+      </c>
+      <c r="C212" s="14" t="s">
+        <v>305</v>
+      </c>
+      <c r="D212" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="E212" s="15" t="s">
+        <v>323</v>
+      </c>
+      <c r="F212" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="213" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A213" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="B213" s="14">
+        <v>6</v>
+      </c>
+      <c r="C213" s="14" t="s">
+        <v>307</v>
+      </c>
+      <c r="D213" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="E213" s="15" t="s">
+        <v>324</v>
+      </c>
+      <c r="F213" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="214" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A214" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="B214" s="14">
+        <v>6</v>
+      </c>
+      <c r="C214" s="14" t="s">
+        <v>129</v>
+      </c>
+      <c r="D214" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="E211" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="F211" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="212" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A212" s="12" t="s">
-        <v>128</v>
-      </c>
-      <c r="B212" s="12">
-        <v>6</v>
-      </c>
-      <c r="C212" s="12" t="s">
-        <v>129</v>
-      </c>
-      <c r="D212" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="E212" s="1" t="s">
-        <v>308</v>
-      </c>
-      <c r="F212" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="213" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A213" s="12" t="s">
-        <v>128</v>
-      </c>
-      <c r="B213" s="12">
-        <v>6</v>
-      </c>
-      <c r="C213" s="12" t="s">
-        <v>135</v>
-      </c>
-      <c r="D213" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="E213" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="F213" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="214" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A214" s="12" t="s">
-        <v>128</v>
-      </c>
-      <c r="B214" s="12">
-        <v>6</v>
-      </c>
-      <c r="C214" s="12" t="s">
-        <v>150</v>
-      </c>
-      <c r="D214" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="E214" s="1" t="s">
-        <v>152</v>
+      <c r="E214" s="15" t="s">
+        <v>325</v>
       </c>
       <c r="F214" s="1" t="s">
         <v>55</v>
@@ -5827,73 +5968,73 @@
         <v>6</v>
       </c>
       <c r="C215" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="D215" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="E215" s="15" t="s">
+        <v>326</v>
+      </c>
+      <c r="F215" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="216" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A216" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="B216" s="14">
+        <v>6</v>
+      </c>
+      <c r="C216" s="14" t="s">
+        <v>150</v>
+      </c>
+      <c r="D216" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="E216" s="15" t="s">
+        <v>327</v>
+      </c>
+      <c r="F216" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="217" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A217" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="B217" s="14">
+        <v>6</v>
+      </c>
+      <c r="C217" s="14" t="s">
         <v>159</v>
       </c>
-      <c r="D215" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="E215" s="1" t="s">
-        <v>337</v>
-      </c>
-      <c r="F215" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="216" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A216" s="12" t="s">
-        <v>128</v>
-      </c>
-      <c r="B216" s="12">
-        <v>6</v>
-      </c>
-      <c r="C216" s="12" t="s">
+      <c r="D217" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="E217" s="15" t="s">
+        <v>328</v>
+      </c>
+      <c r="F217" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="218" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A218" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="B218" s="14">
+        <v>6</v>
+      </c>
+      <c r="C218" s="14" t="s">
         <v>177</v>
       </c>
-      <c r="D216" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="E216" s="1" t="s">
-        <v>340</v>
-      </c>
-      <c r="F216" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="217" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A217" s="12" t="s">
-        <v>128</v>
-      </c>
-      <c r="B217" s="12">
-        <v>6</v>
-      </c>
-      <c r="C217" s="12" t="s">
-        <v>195</v>
-      </c>
-      <c r="D217" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="E217" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="F217" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="218" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A218" s="12" t="s">
-        <v>128</v>
-      </c>
-      <c r="B218" s="12">
-        <v>6</v>
-      </c>
-      <c r="C218" s="12" t="s">
-        <v>129</v>
-      </c>
       <c r="D218" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="E218" s="1" t="s">
-        <v>309</v>
+        <v>33</v>
+      </c>
+      <c r="E218" s="15" t="s">
+        <v>180</v>
       </c>
       <c r="F218" s="1" t="s">
         <v>55</v>
@@ -5907,73 +6048,73 @@
         <v>6</v>
       </c>
       <c r="C219" s="12" t="s">
-        <v>135</v>
+        <v>195</v>
       </c>
       <c r="D219" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="E219" s="1" t="s">
-        <v>320</v>
+        <v>33</v>
+      </c>
+      <c r="E219" s="15" t="s">
+        <v>198</v>
       </c>
       <c r="F219" s="1" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="220" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A220" s="12" t="s">
-        <v>128</v>
-      </c>
-      <c r="B220" s="12">
-        <v>6</v>
-      </c>
-      <c r="C220" s="12" t="s">
-        <v>150</v>
+      <c r="A220" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="B220" s="14">
+        <v>6</v>
+      </c>
+      <c r="C220" s="14" t="s">
+        <v>305</v>
       </c>
       <c r="D220" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="E220" s="1" t="s">
-        <v>328</v>
+        <v>33</v>
+      </c>
+      <c r="E220" s="15" t="s">
+        <v>329</v>
       </c>
       <c r="F220" s="1" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="221" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A221" s="12" t="s">
-        <v>128</v>
-      </c>
-      <c r="B221" s="12">
-        <v>6</v>
-      </c>
-      <c r="C221" s="12" t="s">
-        <v>159</v>
+      <c r="A221" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="B221" s="14">
+        <v>6</v>
+      </c>
+      <c r="C221" s="14" t="s">
+        <v>307</v>
       </c>
       <c r="D221" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="E221" s="1" t="s">
-        <v>163</v>
+        <v>33</v>
+      </c>
+      <c r="E221" s="15" t="s">
+        <v>330</v>
       </c>
       <c r="F221" s="1" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="222" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A222" s="12" t="s">
-        <v>128</v>
-      </c>
-      <c r="B222" s="12">
-        <v>6</v>
-      </c>
-      <c r="C222" s="12" t="s">
-        <v>177</v>
+      <c r="A222" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="B222" s="14">
+        <v>6</v>
+      </c>
+      <c r="C222" s="14" t="s">
+        <v>129</v>
       </c>
       <c r="D222" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="E222" s="1" t="s">
-        <v>181</v>
+        <v>25</v>
+      </c>
+      <c r="E222" s="15" t="s">
+        <v>331</v>
       </c>
       <c r="F222" s="1" t="s">
         <v>55</v>
@@ -5987,73 +6128,73 @@
         <v>6</v>
       </c>
       <c r="C223" s="12" t="s">
-        <v>195</v>
+        <v>135</v>
       </c>
       <c r="D223" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="E223" s="1" t="s">
-        <v>200</v>
+        <v>25</v>
+      </c>
+      <c r="E223" s="15" t="s">
+        <v>138</v>
       </c>
       <c r="F223" s="1" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="224" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A224" s="12" t="s">
-        <v>128</v>
-      </c>
-      <c r="B224" s="12">
-        <v>6</v>
-      </c>
-      <c r="C224" s="12" t="s">
-        <v>129</v>
+    <row r="224" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A224" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="B224" s="14">
+        <v>6</v>
+      </c>
+      <c r="C224" s="14" t="s">
+        <v>150</v>
       </c>
       <c r="D224" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="E224" t="s">
-        <v>310</v>
+        <v>25</v>
+      </c>
+      <c r="E224" s="15" t="s">
+        <v>152</v>
       </c>
       <c r="F224" s="1" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="225" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A225" s="12" t="s">
-        <v>128</v>
-      </c>
-      <c r="B225" s="12">
-        <v>6</v>
-      </c>
-      <c r="C225" s="12" t="s">
-        <v>135</v>
+      <c r="A225" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="B225" s="14">
+        <v>6</v>
+      </c>
+      <c r="C225" s="14" t="s">
+        <v>159</v>
       </c>
       <c r="D225" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="E225" s="1" t="s">
-        <v>139</v>
+        <v>25</v>
+      </c>
+      <c r="E225" s="15" t="s">
+        <v>332</v>
       </c>
       <c r="F225" s="1" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="226" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A226" s="12" t="s">
-        <v>128</v>
-      </c>
-      <c r="B226" s="12">
-        <v>6</v>
-      </c>
-      <c r="C226" s="12" t="s">
-        <v>150</v>
+      <c r="A226" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="B226" s="14">
+        <v>6</v>
+      </c>
+      <c r="C226" s="14" t="s">
+        <v>177</v>
       </c>
       <c r="D226" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="E226" s="1" t="s">
-        <v>153</v>
+        <v>25</v>
+      </c>
+      <c r="E226" s="15" t="s">
+        <v>333</v>
       </c>
       <c r="F226" s="1" t="s">
         <v>55</v>
@@ -6067,73 +6208,73 @@
         <v>6</v>
       </c>
       <c r="C227" s="12" t="s">
-        <v>159</v>
+        <v>195</v>
       </c>
       <c r="D227" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="E227" s="1" t="s">
-        <v>164</v>
+        <v>25</v>
+      </c>
+      <c r="E227" s="15" t="s">
+        <v>199</v>
       </c>
       <c r="F227" s="1" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="228" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A228" s="12" t="s">
-        <v>128</v>
-      </c>
-      <c r="B228" s="12">
-        <v>6</v>
-      </c>
-      <c r="C228" s="12" t="s">
-        <v>177</v>
+      <c r="A228" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="B228" s="14">
+        <v>6</v>
+      </c>
+      <c r="C228" s="14" t="s">
+        <v>305</v>
       </c>
       <c r="D228" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="E228" s="1" t="s">
-        <v>182</v>
+        <v>25</v>
+      </c>
+      <c r="E228" s="15" t="s">
+        <v>334</v>
       </c>
       <c r="F228" s="1" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="229" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A229" s="12" t="s">
-        <v>128</v>
-      </c>
-      <c r="B229" s="12">
-        <v>6</v>
-      </c>
-      <c r="C229" s="12" t="s">
-        <v>195</v>
+      <c r="A229" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="B229" s="14">
+        <v>6</v>
+      </c>
+      <c r="C229" s="14" t="s">
+        <v>307</v>
       </c>
       <c r="D229" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="E229" s="1" t="s">
-        <v>201</v>
+        <v>25</v>
+      </c>
+      <c r="E229" s="15" t="s">
+        <v>335</v>
       </c>
       <c r="F229" s="1" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="230" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A230" s="12" t="s">
-        <v>128</v>
-      </c>
-      <c r="B230" s="12">
-        <v>6</v>
-      </c>
-      <c r="C230" s="12" t="s">
+      <c r="A230" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="B230" s="14">
+        <v>6</v>
+      </c>
+      <c r="C230" s="14" t="s">
         <v>129</v>
       </c>
       <c r="D230" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="E230" s="1" t="s">
-        <v>312</v>
+        <v>28</v>
+      </c>
+      <c r="E230" s="15" t="s">
+        <v>336</v>
       </c>
       <c r="F230" s="1" t="s">
         <v>55</v>
@@ -6150,70 +6291,70 @@
         <v>135</v>
       </c>
       <c r="D231" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="E231" s="1" t="s">
-        <v>140</v>
+        <v>28</v>
+      </c>
+      <c r="E231" s="15" t="s">
+        <v>337</v>
       </c>
       <c r="F231" s="1" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="232" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A232" s="12" t="s">
-        <v>128</v>
-      </c>
-      <c r="B232" s="12">
-        <v>6</v>
-      </c>
-      <c r="C232" s="12" t="s">
+      <c r="A232" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="B232" s="14">
+        <v>6</v>
+      </c>
+      <c r="C232" s="14" t="s">
         <v>150</v>
       </c>
       <c r="D232" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="E232" s="1" t="s">
-        <v>329</v>
+        <v>28</v>
+      </c>
+      <c r="E232" s="15" t="s">
+        <v>338</v>
       </c>
       <c r="F232" s="1" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="233" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A233" s="12" t="s">
-        <v>128</v>
-      </c>
-      <c r="B233" s="12">
-        <v>6</v>
-      </c>
-      <c r="C233" s="12" t="s">
+      <c r="A233" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="B233" s="14">
+        <v>6</v>
+      </c>
+      <c r="C233" s="14" t="s">
         <v>159</v>
       </c>
       <c r="D233" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="E233" s="1" t="s">
-        <v>165</v>
+        <v>28</v>
+      </c>
+      <c r="E233" s="15" t="s">
+        <v>163</v>
       </c>
       <c r="F233" s="1" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="234" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A234" s="12" t="s">
-        <v>128</v>
-      </c>
-      <c r="B234" s="12">
-        <v>6</v>
-      </c>
-      <c r="C234" s="12" t="s">
+      <c r="A234" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="B234" s="14">
+        <v>6</v>
+      </c>
+      <c r="C234" s="14" t="s">
         <v>177</v>
       </c>
       <c r="D234" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="E234" s="1" t="s">
-        <v>183</v>
+        <v>28</v>
+      </c>
+      <c r="E234" s="15" t="s">
+        <v>181</v>
       </c>
       <c r="F234" s="1" t="s">
         <v>55</v>
@@ -6230,70 +6371,70 @@
         <v>195</v>
       </c>
       <c r="D235" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="E235" s="1" t="s">
-        <v>202</v>
+        <v>28</v>
+      </c>
+      <c r="E235" s="15" t="s">
+        <v>200</v>
       </c>
       <c r="F235" s="1" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="236" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A236" s="12" t="s">
-        <v>128</v>
-      </c>
-      <c r="B236" s="12">
-        <v>6</v>
-      </c>
-      <c r="C236" s="12" t="s">
+      <c r="A236" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="B236" s="14">
+        <v>6</v>
+      </c>
+      <c r="C236" s="14" t="s">
+        <v>305</v>
+      </c>
+      <c r="D236" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="E236" s="16" t="s">
+        <v>339</v>
+      </c>
+      <c r="F236" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="237" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A237" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="B237" s="14">
+        <v>6</v>
+      </c>
+      <c r="C237" s="14" t="s">
+        <v>307</v>
+      </c>
+      <c r="D237" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="E237" s="15" t="s">
+        <v>340</v>
+      </c>
+      <c r="F237" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="238" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A238" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="B238" s="14">
+        <v>6</v>
+      </c>
+      <c r="C238" s="14" t="s">
         <v>129</v>
       </c>
-      <c r="D236" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="E236" s="1" t="s">
-        <v>311</v>
-      </c>
-      <c r="F236" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="237" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A237" s="12" t="s">
-        <v>128</v>
-      </c>
-      <c r="B237" s="12">
-        <v>6</v>
-      </c>
-      <c r="C237" s="12" t="s">
-        <v>135</v>
-      </c>
-      <c r="D237" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="E237" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="F237" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="238" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A238" s="12" t="s">
-        <v>128</v>
-      </c>
-      <c r="B238" s="12">
-        <v>6</v>
-      </c>
-      <c r="C238" s="12" t="s">
-        <v>150</v>
-      </c>
       <c r="D238" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="E238" s="1" t="s">
-        <v>154</v>
+        <v>13</v>
+      </c>
+      <c r="E238" s="15" t="s">
+        <v>341</v>
       </c>
       <c r="F238" s="1" t="s">
         <v>55</v>
@@ -6307,73 +6448,73 @@
         <v>6</v>
       </c>
       <c r="C239" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="D239" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="E239" s="15" t="s">
+        <v>139</v>
+      </c>
+      <c r="F239" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="240" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A240" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="B240" s="14">
+        <v>6</v>
+      </c>
+      <c r="C240" s="14" t="s">
+        <v>150</v>
+      </c>
+      <c r="D240" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="E240" s="15" t="s">
+        <v>153</v>
+      </c>
+      <c r="F240" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="241" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A241" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="B241" s="14">
+        <v>6</v>
+      </c>
+      <c r="C241" s="14" t="s">
         <v>159</v>
       </c>
-      <c r="D239" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="E239" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="F239" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="240" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A240" s="12" t="s">
-        <v>128</v>
-      </c>
-      <c r="B240" s="12">
-        <v>6</v>
-      </c>
-      <c r="C240" s="12" t="s">
+      <c r="D241" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="E241" s="15" t="s">
+        <v>164</v>
+      </c>
+      <c r="F241" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="242" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A242" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="B242" s="14">
+        <v>6</v>
+      </c>
+      <c r="C242" s="14" t="s">
         <v>177</v>
       </c>
-      <c r="D240" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="E240" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="F240" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="241" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A241" s="12" t="s">
-        <v>128</v>
-      </c>
-      <c r="B241" s="12">
-        <v>6</v>
-      </c>
-      <c r="C241" s="12" t="s">
-        <v>195</v>
-      </c>
-      <c r="D241" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="E241" s="1" t="s">
-        <v>343</v>
-      </c>
-      <c r="F241" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="242" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A242" s="12" t="s">
-        <v>128</v>
-      </c>
-      <c r="B242" s="12">
-        <v>6</v>
-      </c>
-      <c r="C242" s="12" t="s">
-        <v>129</v>
-      </c>
       <c r="D242" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="E242" s="1" t="s">
-        <v>313</v>
+        <v>13</v>
+      </c>
+      <c r="E242" s="15" t="s">
+        <v>182</v>
       </c>
       <c r="F242" s="1" t="s">
         <v>55</v>
@@ -6387,73 +6528,73 @@
         <v>6</v>
       </c>
       <c r="C243" s="12" t="s">
-        <v>135</v>
+        <v>195</v>
       </c>
       <c r="D243" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="E243" s="1" t="s">
-        <v>142</v>
+        <v>13</v>
+      </c>
+      <c r="E243" s="15" t="s">
+        <v>201</v>
       </c>
       <c r="F243" s="1" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="244" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A244" s="12" t="s">
-        <v>128</v>
-      </c>
-      <c r="B244" s="12">
-        <v>6</v>
-      </c>
-      <c r="C244" s="12" t="s">
-        <v>150</v>
+      <c r="A244" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="B244" s="14">
+        <v>6</v>
+      </c>
+      <c r="C244" s="14" t="s">
+        <v>305</v>
       </c>
       <c r="D244" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="E244" s="1" t="s">
-        <v>330</v>
+        <v>13</v>
+      </c>
+      <c r="E244" s="15" t="s">
+        <v>342</v>
       </c>
       <c r="F244" s="1" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="245" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A245" s="12" t="s">
-        <v>128</v>
-      </c>
-      <c r="B245" s="12">
-        <v>6</v>
-      </c>
-      <c r="C245" s="12" t="s">
-        <v>159</v>
+      <c r="A245" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="B245" s="14">
+        <v>6</v>
+      </c>
+      <c r="C245" s="14" t="s">
+        <v>307</v>
       </c>
       <c r="D245" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="E245" s="1" t="s">
-        <v>167</v>
+        <v>13</v>
+      </c>
+      <c r="E245" s="15" t="s">
+        <v>343</v>
       </c>
       <c r="F245" s="1" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="246" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A246" s="12" t="s">
-        <v>128</v>
-      </c>
-      <c r="B246" s="12">
-        <v>6</v>
-      </c>
-      <c r="C246" s="12" t="s">
-        <v>177</v>
+      <c r="A246" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="B246" s="14">
+        <v>6</v>
+      </c>
+      <c r="C246" s="14" t="s">
+        <v>129</v>
       </c>
       <c r="D246" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="E246" s="1" t="s">
-        <v>185</v>
+        <v>26</v>
+      </c>
+      <c r="E246" s="15" t="s">
+        <v>344</v>
       </c>
       <c r="F246" s="1" t="s">
         <v>55</v>
@@ -6467,73 +6608,73 @@
         <v>6</v>
       </c>
       <c r="C247" s="12" t="s">
-        <v>195</v>
+        <v>135</v>
       </c>
       <c r="D247" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="E247" s="1" t="s">
-        <v>203</v>
+        <v>26</v>
+      </c>
+      <c r="E247" s="15" t="s">
+        <v>140</v>
       </c>
       <c r="F247" s="1" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="248" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A248" s="12" t="s">
-        <v>128</v>
-      </c>
-      <c r="B248" s="12">
-        <v>6</v>
-      </c>
-      <c r="C248" s="12" t="s">
-        <v>129</v>
+      <c r="A248" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="B248" s="14">
+        <v>6</v>
+      </c>
+      <c r="C248" s="14" t="s">
+        <v>150</v>
       </c>
       <c r="D248" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="E248" s="1" t="s">
-        <v>131</v>
+        <v>26</v>
+      </c>
+      <c r="E248" s="15" t="s">
+        <v>345</v>
       </c>
       <c r="F248" s="1" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="249" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A249" s="12" t="s">
-        <v>128</v>
-      </c>
-      <c r="B249" s="12">
-        <v>6</v>
-      </c>
-      <c r="C249" s="12" t="s">
-        <v>135</v>
+      <c r="A249" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="B249" s="14">
+        <v>6</v>
+      </c>
+      <c r="C249" s="14" t="s">
+        <v>159</v>
       </c>
       <c r="D249" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="E249" s="1" t="s">
-        <v>143</v>
+        <v>26</v>
+      </c>
+      <c r="E249" s="15" t="s">
+        <v>165</v>
       </c>
       <c r="F249" s="1" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="250" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A250" s="12" t="s">
-        <v>128</v>
-      </c>
-      <c r="B250" s="12">
-        <v>6</v>
-      </c>
-      <c r="C250" s="12" t="s">
-        <v>150</v>
+      <c r="A250" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="B250" s="14">
+        <v>6</v>
+      </c>
+      <c r="C250" s="14" t="s">
+        <v>177</v>
       </c>
       <c r="D250" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="E250" s="1" t="s">
-        <v>155</v>
+        <v>26</v>
+      </c>
+      <c r="E250" s="15" t="s">
+        <v>183</v>
       </c>
       <c r="F250" s="1" t="s">
         <v>55</v>
@@ -6547,73 +6688,73 @@
         <v>6</v>
       </c>
       <c r="C251" s="12" t="s">
-        <v>159</v>
+        <v>195</v>
       </c>
       <c r="D251" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="E251" s="1" t="s">
-        <v>168</v>
+        <v>26</v>
+      </c>
+      <c r="E251" s="15" t="s">
+        <v>202</v>
       </c>
       <c r="F251" s="1" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="252" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A252" s="12" t="s">
-        <v>128</v>
-      </c>
-      <c r="B252" s="12">
-        <v>6</v>
-      </c>
-      <c r="C252" s="12" t="s">
-        <v>177</v>
+      <c r="A252" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="B252" s="14">
+        <v>6</v>
+      </c>
+      <c r="C252" s="14" t="s">
+        <v>305</v>
       </c>
       <c r="D252" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="E252" s="1" t="s">
-        <v>186</v>
+        <v>26</v>
+      </c>
+      <c r="E252" s="15" t="s">
+        <v>346</v>
       </c>
       <c r="F252" s="1" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="253" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A253" s="12" t="s">
-        <v>128</v>
-      </c>
-      <c r="B253" s="12">
-        <v>6</v>
-      </c>
-      <c r="C253" s="12" t="s">
-        <v>195</v>
+      <c r="A253" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="B253" s="14">
+        <v>6</v>
+      </c>
+      <c r="C253" s="14" t="s">
+        <v>307</v>
       </c>
       <c r="D253" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="E253" s="1" t="s">
-        <v>204</v>
+        <v>26</v>
+      </c>
+      <c r="E253" s="15" t="s">
+        <v>347</v>
       </c>
       <c r="F253" s="1" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="254" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A254" s="12" t="s">
-        <v>128</v>
-      </c>
-      <c r="B254" s="12">
-        <v>6</v>
-      </c>
-      <c r="C254" s="12" t="s">
+      <c r="A254" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="B254" s="14">
+        <v>6</v>
+      </c>
+      <c r="C254" s="14" t="s">
         <v>129</v>
       </c>
       <c r="D254" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="E254" s="1" t="s">
-        <v>132</v>
+        <v>14</v>
+      </c>
+      <c r="E254" s="15" t="s">
+        <v>348</v>
       </c>
       <c r="F254" s="1" t="s">
         <v>55</v>
@@ -6630,70 +6771,70 @@
         <v>135</v>
       </c>
       <c r="D255" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="E255" s="1" t="s">
-        <v>144</v>
+        <v>14</v>
+      </c>
+      <c r="E255" s="15" t="s">
+        <v>141</v>
       </c>
       <c r="F255" s="1" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="256" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A256" s="12" t="s">
-        <v>128</v>
-      </c>
-      <c r="B256" s="12">
-        <v>6</v>
-      </c>
-      <c r="C256" s="12" t="s">
+      <c r="A256" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="B256" s="14">
+        <v>6</v>
+      </c>
+      <c r="C256" s="14" t="s">
         <v>150</v>
       </c>
       <c r="D256" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="E256" s="1" t="s">
-        <v>156</v>
+        <v>14</v>
+      </c>
+      <c r="E256" s="15" t="s">
+        <v>154</v>
       </c>
       <c r="F256" s="1" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="257" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A257" s="12" t="s">
-        <v>128</v>
-      </c>
-      <c r="B257" s="12">
-        <v>6</v>
-      </c>
-      <c r="C257" s="12" t="s">
+      <c r="A257" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="B257" s="14">
+        <v>6</v>
+      </c>
+      <c r="C257" s="14" t="s">
         <v>159</v>
       </c>
       <c r="D257" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="E257" s="1" t="s">
-        <v>169</v>
+        <v>14</v>
+      </c>
+      <c r="E257" s="15" t="s">
+        <v>166</v>
       </c>
       <c r="F257" s="1" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="258" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A258" s="12" t="s">
-        <v>128</v>
-      </c>
-      <c r="B258" s="12">
-        <v>6</v>
-      </c>
-      <c r="C258" s="12" t="s">
+      <c r="A258" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="B258" s="14">
+        <v>6</v>
+      </c>
+      <c r="C258" s="14" t="s">
         <v>177</v>
       </c>
       <c r="D258" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="E258" s="1" t="s">
-        <v>187</v>
+        <v>14</v>
+      </c>
+      <c r="E258" s="15" t="s">
+        <v>184</v>
       </c>
       <c r="F258" s="1" t="s">
         <v>55</v>
@@ -6710,70 +6851,70 @@
         <v>195</v>
       </c>
       <c r="D259" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="E259" s="1" t="s">
-        <v>205</v>
+        <v>14</v>
+      </c>
+      <c r="E259" s="15" t="s">
+        <v>349</v>
       </c>
       <c r="F259" s="1" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="260" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A260" s="12" t="s">
-        <v>128</v>
-      </c>
-      <c r="B260" s="12">
-        <v>6</v>
-      </c>
-      <c r="C260" s="12" t="s">
+      <c r="A260" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="B260" s="14">
+        <v>6</v>
+      </c>
+      <c r="C260" s="14" t="s">
+        <v>305</v>
+      </c>
+      <c r="D260" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="E260" s="15" t="s">
+        <v>350</v>
+      </c>
+      <c r="F260" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="261" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A261" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="B261" s="14">
+        <v>6</v>
+      </c>
+      <c r="C261" s="14" t="s">
+        <v>307</v>
+      </c>
+      <c r="D261" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="E261" s="15" t="s">
+        <v>351</v>
+      </c>
+      <c r="F261" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="262" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A262" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="B262" s="14">
+        <v>6</v>
+      </c>
+      <c r="C262" s="14" t="s">
         <v>129</v>
       </c>
-      <c r="D260" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="E260" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="F260" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="261" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A261" s="12" t="s">
-        <v>128</v>
-      </c>
-      <c r="B261" s="12">
-        <v>6</v>
-      </c>
-      <c r="C261" s="12" t="s">
-        <v>135</v>
-      </c>
-      <c r="D261" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="E261" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="F261" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="262" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A262" s="12" t="s">
-        <v>128</v>
-      </c>
-      <c r="B262" s="12">
-        <v>6</v>
-      </c>
-      <c r="C262" s="12" t="s">
-        <v>150</v>
-      </c>
       <c r="D262" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="E262" s="6" t="s">
-        <v>331</v>
+        <v>30</v>
+      </c>
+      <c r="E262" s="15" t="s">
+        <v>352</v>
       </c>
       <c r="F262" s="1" t="s">
         <v>55</v>
@@ -6787,73 +6928,73 @@
         <v>6</v>
       </c>
       <c r="C263" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="D263" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="E263" s="15" t="s">
+        <v>142</v>
+      </c>
+      <c r="F263" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="264" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A264" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="B264" s="14">
+        <v>6</v>
+      </c>
+      <c r="C264" s="14" t="s">
+        <v>150</v>
+      </c>
+      <c r="D264" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="E264" s="15" t="s">
+        <v>353</v>
+      </c>
+      <c r="F264" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="265" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A265" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="B265" s="14">
+        <v>6</v>
+      </c>
+      <c r="C265" s="14" t="s">
         <v>159</v>
       </c>
-      <c r="D263" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="E263" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="F263" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="264" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A264" s="12" t="s">
-        <v>128</v>
-      </c>
-      <c r="B264" s="12">
-        <v>6</v>
-      </c>
-      <c r="C264" s="12" t="s">
+      <c r="D265" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="E265" s="15" t="s">
+        <v>167</v>
+      </c>
+      <c r="F265" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="266" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A266" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="B266" s="14">
+        <v>6</v>
+      </c>
+      <c r="C266" s="14" t="s">
         <v>177</v>
       </c>
-      <c r="D264" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="E264" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="F264" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="265" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A265" s="12" t="s">
-        <v>128</v>
-      </c>
-      <c r="B265" s="12">
-        <v>6</v>
-      </c>
-      <c r="C265" s="12" t="s">
-        <v>195</v>
-      </c>
-      <c r="D265" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="E265" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="F265" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="266" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A266" s="12" t="s">
-        <v>128</v>
-      </c>
-      <c r="B266" s="12">
-        <v>6</v>
-      </c>
-      <c r="C266" s="12" t="s">
-        <v>129</v>
-      </c>
       <c r="D266" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="E266" s="1" t="s">
-        <v>314</v>
+        <v>30</v>
+      </c>
+      <c r="E266" s="15" t="s">
+        <v>185</v>
       </c>
       <c r="F266" s="1" t="s">
         <v>55</v>
@@ -6867,73 +7008,73 @@
         <v>6</v>
       </c>
       <c r="C267" s="12" t="s">
-        <v>135</v>
+        <v>195</v>
       </c>
       <c r="D267" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="E267" s="1" t="s">
-        <v>321</v>
+        <v>30</v>
+      </c>
+      <c r="E267" s="15" t="s">
+        <v>203</v>
       </c>
       <c r="F267" s="1" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="268" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A268" s="12" t="s">
-        <v>128</v>
-      </c>
-      <c r="B268" s="12">
-        <v>6</v>
-      </c>
-      <c r="C268" s="12" t="s">
-        <v>150</v>
+      <c r="A268" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="B268" s="14">
+        <v>6</v>
+      </c>
+      <c r="C268" s="14" t="s">
+        <v>305</v>
       </c>
       <c r="D268" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="E268" s="1" t="s">
-        <v>157</v>
+        <v>30</v>
+      </c>
+      <c r="E268" s="15" t="s">
+        <v>354</v>
       </c>
       <c r="F268" s="1" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="269" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A269" s="12" t="s">
-        <v>128</v>
-      </c>
-      <c r="B269" s="12">
-        <v>6</v>
-      </c>
-      <c r="C269" s="12" t="s">
-        <v>159</v>
+      <c r="A269" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="B269" s="14">
+        <v>6</v>
+      </c>
+      <c r="C269" s="14" t="s">
+        <v>307</v>
       </c>
       <c r="D269" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="E269" s="1" t="s">
-        <v>171</v>
+        <v>30</v>
+      </c>
+      <c r="E269" s="15" t="s">
+        <v>355</v>
       </c>
       <c r="F269" s="1" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="270" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A270" s="12" t="s">
-        <v>128</v>
-      </c>
-      <c r="B270" s="12">
-        <v>6</v>
-      </c>
-      <c r="C270" s="12" t="s">
-        <v>177</v>
+      <c r="A270" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="B270" s="14">
+        <v>6</v>
+      </c>
+      <c r="C270" s="14" t="s">
+        <v>129</v>
       </c>
       <c r="D270" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="E270" s="1" t="s">
-        <v>189</v>
+        <v>15</v>
+      </c>
+      <c r="E270" s="15" t="s">
+        <v>131</v>
       </c>
       <c r="F270" s="1" t="s">
         <v>55</v>
@@ -6947,73 +7088,73 @@
         <v>6</v>
       </c>
       <c r="C271" s="12" t="s">
-        <v>195</v>
+        <v>135</v>
       </c>
       <c r="D271" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="E271" s="1" t="s">
-        <v>344</v>
+        <v>15</v>
+      </c>
+      <c r="E271" s="15" t="s">
+        <v>143</v>
       </c>
       <c r="F271" s="1" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="272" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A272" s="12" t="s">
-        <v>128</v>
-      </c>
-      <c r="B272" s="12">
-        <v>6</v>
-      </c>
-      <c r="C272" s="12" t="s">
-        <v>129</v>
+      <c r="A272" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="B272" s="14">
+        <v>6</v>
+      </c>
+      <c r="C272" s="14" t="s">
+        <v>150</v>
       </c>
       <c r="D272" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="E272" s="1" t="s">
-        <v>315</v>
+        <v>15</v>
+      </c>
+      <c r="E272" s="15" t="s">
+        <v>155</v>
       </c>
       <c r="F272" s="1" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="273" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A273" s="12" t="s">
-        <v>128</v>
-      </c>
-      <c r="B273" s="12">
-        <v>6</v>
-      </c>
-      <c r="C273" s="12" t="s">
-        <v>135</v>
+      <c r="A273" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="B273" s="14">
+        <v>6</v>
+      </c>
+      <c r="C273" s="14" t="s">
+        <v>159</v>
       </c>
       <c r="D273" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="E273" s="1" t="s">
-        <v>146</v>
+        <v>15</v>
+      </c>
+      <c r="E273" s="15" t="s">
+        <v>168</v>
       </c>
       <c r="F273" s="1" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="274" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A274" s="12" t="s">
-        <v>128</v>
-      </c>
-      <c r="B274" s="12">
-        <v>6</v>
-      </c>
-      <c r="C274" s="12" t="s">
-        <v>150</v>
+      <c r="A274" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="B274" s="14">
+        <v>6</v>
+      </c>
+      <c r="C274" s="14" t="s">
+        <v>177</v>
       </c>
       <c r="D274" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="E274" s="1" t="s">
-        <v>332</v>
+        <v>15</v>
+      </c>
+      <c r="E274" s="15" t="s">
+        <v>186</v>
       </c>
       <c r="F274" s="1" t="s">
         <v>55</v>
@@ -7027,73 +7168,73 @@
         <v>6</v>
       </c>
       <c r="C275" s="12" t="s">
-        <v>159</v>
+        <v>195</v>
       </c>
       <c r="D275" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="E275" s="1" t="s">
-        <v>172</v>
+        <v>15</v>
+      </c>
+      <c r="E275" s="15" t="s">
+        <v>204</v>
       </c>
       <c r="F275" s="1" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="276" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A276" s="12" t="s">
-        <v>128</v>
-      </c>
-      <c r="B276" s="12">
-        <v>6</v>
-      </c>
-      <c r="C276" s="12" t="s">
-        <v>177</v>
+      <c r="A276" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="B276" s="14">
+        <v>6</v>
+      </c>
+      <c r="C276" s="14" t="s">
+        <v>305</v>
       </c>
       <c r="D276" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="E276" s="1" t="s">
-        <v>190</v>
+        <v>15</v>
+      </c>
+      <c r="E276" s="15" t="s">
+        <v>356</v>
       </c>
       <c r="F276" s="1" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="277" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A277" s="12" t="s">
-        <v>128</v>
-      </c>
-      <c r="B277" s="12">
-        <v>6</v>
-      </c>
-      <c r="C277" s="12" t="s">
-        <v>195</v>
+      <c r="A277" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="B277" s="14">
+        <v>6</v>
+      </c>
+      <c r="C277" s="14" t="s">
+        <v>307</v>
       </c>
       <c r="D277" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="E277" s="1" t="s">
-        <v>207</v>
+        <v>15</v>
+      </c>
+      <c r="E277" s="15" t="s">
+        <v>357</v>
       </c>
       <c r="F277" s="1" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="278" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A278" s="12" t="s">
-        <v>128</v>
-      </c>
-      <c r="B278" s="12">
-        <v>6</v>
-      </c>
-      <c r="C278" s="12" t="s">
+      <c r="A278" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="B278" s="14">
+        <v>6</v>
+      </c>
+      <c r="C278" s="14" t="s">
         <v>129</v>
       </c>
       <c r="D278" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="E278" s="1" t="s">
-        <v>316</v>
+        <v>16</v>
+      </c>
+      <c r="E278" s="15" t="s">
+        <v>132</v>
       </c>
       <c r="F278" s="1" t="s">
         <v>55</v>
@@ -7110,70 +7251,70 @@
         <v>135</v>
       </c>
       <c r="D279" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="E279" s="1" t="s">
-        <v>147</v>
+        <v>16</v>
+      </c>
+      <c r="E279" s="15" t="s">
+        <v>144</v>
       </c>
       <c r="F279" s="1" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="280" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A280" s="12" t="s">
-        <v>128</v>
-      </c>
-      <c r="B280" s="12">
-        <v>6</v>
-      </c>
-      <c r="C280" s="12" t="s">
+      <c r="A280" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="B280" s="14">
+        <v>6</v>
+      </c>
+      <c r="C280" s="14" t="s">
         <v>150</v>
       </c>
       <c r="D280" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="E280" s="1" t="s">
-        <v>323</v>
+        <v>16</v>
+      </c>
+      <c r="E280" s="15" t="s">
+        <v>156</v>
       </c>
       <c r="F280" s="1" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="281" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A281" s="12" t="s">
-        <v>128</v>
-      </c>
-      <c r="B281" s="12">
-        <v>6</v>
-      </c>
-      <c r="C281" s="12" t="s">
+      <c r="A281" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="B281" s="14">
+        <v>6</v>
+      </c>
+      <c r="C281" s="14" t="s">
         <v>159</v>
       </c>
       <c r="D281" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="E281" s="1" t="s">
-        <v>173</v>
+        <v>16</v>
+      </c>
+      <c r="E281" s="15" t="s">
+        <v>169</v>
       </c>
       <c r="F281" s="1" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="282" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A282" s="12" t="s">
-        <v>128</v>
-      </c>
-      <c r="B282" s="12">
-        <v>6</v>
-      </c>
-      <c r="C282" s="12" t="s">
+      <c r="A282" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="B282" s="14">
+        <v>6</v>
+      </c>
+      <c r="C282" s="14" t="s">
         <v>177</v>
       </c>
       <c r="D282" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="E282" s="1" t="s">
-        <v>191</v>
+        <v>16</v>
+      </c>
+      <c r="E282" s="15" t="s">
+        <v>187</v>
       </c>
       <c r="F282" s="1" t="s">
         <v>55</v>
@@ -7190,70 +7331,70 @@
         <v>195</v>
       </c>
       <c r="D283" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="E283" s="1" t="s">
-        <v>345</v>
+        <v>16</v>
+      </c>
+      <c r="E283" s="15" t="s">
+        <v>205</v>
       </c>
       <c r="F283" s="1" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="284" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A284" s="12" t="s">
-        <v>128</v>
-      </c>
-      <c r="B284" s="12">
-        <v>6</v>
-      </c>
-      <c r="C284" s="12" t="s">
+      <c r="A284" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="B284" s="14">
+        <v>6</v>
+      </c>
+      <c r="C284" s="14" t="s">
+        <v>305</v>
+      </c>
+      <c r="D284" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="E284" s="15" t="s">
+        <v>358</v>
+      </c>
+      <c r="F284" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="285" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A285" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="B285" s="14">
+        <v>6</v>
+      </c>
+      <c r="C285" s="14" t="s">
+        <v>307</v>
+      </c>
+      <c r="D285" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="E285" s="15" t="s">
+        <v>359</v>
+      </c>
+      <c r="F285" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="286" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A286" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="B286" s="14">
+        <v>6</v>
+      </c>
+      <c r="C286" s="14" t="s">
         <v>129</v>
       </c>
-      <c r="D284" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="E284" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="F284" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="285" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A285" s="12" t="s">
-        <v>128</v>
-      </c>
-      <c r="B285" s="12">
-        <v>6</v>
-      </c>
-      <c r="C285" s="12" t="s">
-        <v>135</v>
-      </c>
-      <c r="D285" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="E285" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="F285" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="286" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A286" s="12" t="s">
-        <v>128</v>
-      </c>
-      <c r="B286" s="12">
-        <v>6</v>
-      </c>
-      <c r="C286" s="12" t="s">
-        <v>150</v>
-      </c>
       <c r="D286" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="E286" s="1" t="s">
-        <v>333</v>
+        <v>17</v>
+      </c>
+      <c r="E286" s="15" t="s">
+        <v>133</v>
       </c>
       <c r="F286" s="1" t="s">
         <v>55</v>
@@ -7267,73 +7408,73 @@
         <v>6</v>
       </c>
       <c r="C287" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="D287" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="E287" s="15" t="s">
+        <v>145</v>
+      </c>
+      <c r="F287" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="288" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A288" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="B288" s="14">
+        <v>6</v>
+      </c>
+      <c r="C288" s="14" t="s">
+        <v>150</v>
+      </c>
+      <c r="D288" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="E288" s="15" t="s">
+        <v>360</v>
+      </c>
+      <c r="F288" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="289" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A289" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="B289" s="14">
+        <v>6</v>
+      </c>
+      <c r="C289" s="14" t="s">
         <v>159</v>
       </c>
-      <c r="D287" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="E287" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="F287" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="288" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A288" s="12" t="s">
-        <v>128</v>
-      </c>
-      <c r="B288" s="12">
-        <v>6</v>
-      </c>
-      <c r="C288" s="12" t="s">
+      <c r="D289" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="E289" s="15" t="s">
+        <v>170</v>
+      </c>
+      <c r="F289" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="290" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A290" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="B290" s="14">
+        <v>6</v>
+      </c>
+      <c r="C290" s="14" t="s">
         <v>177</v>
       </c>
-      <c r="D288" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="E288" s="1" t="s">
-        <v>192</v>
-      </c>
-      <c r="F288" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="289" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A289" s="12" t="s">
-        <v>128</v>
-      </c>
-      <c r="B289" s="12">
-        <v>6</v>
-      </c>
-      <c r="C289" s="12" t="s">
-        <v>195</v>
-      </c>
-      <c r="D289" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="E289" s="1" t="s">
-        <v>208</v>
-      </c>
-      <c r="F289" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="290" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A290" s="12" t="s">
-        <v>128</v>
-      </c>
-      <c r="B290" s="12">
-        <v>6</v>
-      </c>
-      <c r="C290" s="12" t="s">
-        <v>129</v>
-      </c>
       <c r="D290" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="E290" s="1" t="s">
-        <v>302</v>
+        <v>17</v>
+      </c>
+      <c r="E290" s="15" t="s">
+        <v>188</v>
       </c>
       <c r="F290" s="1" t="s">
         <v>55</v>
@@ -7347,73 +7488,73 @@
         <v>6</v>
       </c>
       <c r="C291" s="12" t="s">
-        <v>135</v>
+        <v>195</v>
       </c>
       <c r="D291" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="E291" s="1" t="s">
-        <v>322</v>
+        <v>17</v>
+      </c>
+      <c r="E291" s="15" t="s">
+        <v>206</v>
       </c>
       <c r="F291" s="1" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="292" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A292" s="12" t="s">
-        <v>128</v>
-      </c>
-      <c r="B292" s="12">
-        <v>6</v>
-      </c>
-      <c r="C292" s="12" t="s">
-        <v>150</v>
+      <c r="A292" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="B292" s="14">
+        <v>6</v>
+      </c>
+      <c r="C292" s="14" t="s">
+        <v>305</v>
       </c>
       <c r="D292" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="E292" s="1" t="s">
-        <v>158</v>
+        <v>17</v>
+      </c>
+      <c r="E292" s="17" t="s">
+        <v>361</v>
       </c>
       <c r="F292" s="1" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="293" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A293" s="12" t="s">
-        <v>128</v>
-      </c>
-      <c r="B293" s="12">
-        <v>6</v>
-      </c>
-      <c r="C293" s="12" t="s">
-        <v>159</v>
+      <c r="A293" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="B293" s="14">
+        <v>6</v>
+      </c>
+      <c r="C293" s="14" t="s">
+        <v>307</v>
       </c>
       <c r="D293" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="E293" s="1" t="s">
-        <v>175</v>
+        <v>17</v>
+      </c>
+      <c r="E293" s="15" t="s">
+        <v>362</v>
       </c>
       <c r="F293" s="1" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="294" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A294" s="12" t="s">
-        <v>128</v>
-      </c>
-      <c r="B294" s="12">
-        <v>6</v>
-      </c>
-      <c r="C294" s="12" t="s">
-        <v>177</v>
+      <c r="A294" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="B294" s="14">
+        <v>6</v>
+      </c>
+      <c r="C294" s="14" t="s">
+        <v>129</v>
       </c>
       <c r="D294" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="E294" s="1" t="s">
-        <v>193</v>
+        <v>29</v>
+      </c>
+      <c r="E294" s="15" t="s">
+        <v>363</v>
       </c>
       <c r="F294" s="1" t="s">
         <v>55</v>
@@ -7427,73 +7568,73 @@
         <v>6</v>
       </c>
       <c r="C295" s="12" t="s">
-        <v>195</v>
+        <v>135</v>
       </c>
       <c r="D295" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="E295" s="1" t="s">
-        <v>209</v>
+        <v>29</v>
+      </c>
+      <c r="E295" s="15" t="s">
+        <v>364</v>
       </c>
       <c r="F295" s="1" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="296" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A296" s="12" t="s">
-        <v>128</v>
-      </c>
-      <c r="B296" s="12">
-        <v>6</v>
-      </c>
-      <c r="C296" s="12" t="s">
-        <v>129</v>
+      <c r="A296" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="B296" s="14">
+        <v>6</v>
+      </c>
+      <c r="C296" s="14" t="s">
+        <v>150</v>
       </c>
       <c r="D296" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E296" s="1" t="s">
-        <v>303</v>
+        <v>29</v>
+      </c>
+      <c r="E296" s="15" t="s">
+        <v>157</v>
       </c>
       <c r="F296" s="1" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="297" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A297" s="12" t="s">
-        <v>128</v>
-      </c>
-      <c r="B297" s="12">
-        <v>6</v>
-      </c>
-      <c r="C297" s="12" t="s">
-        <v>135</v>
+      <c r="A297" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="B297" s="14">
+        <v>6</v>
+      </c>
+      <c r="C297" s="14" t="s">
+        <v>159</v>
       </c>
       <c r="D297" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E297" s="1" t="s">
-        <v>149</v>
+        <v>29</v>
+      </c>
+      <c r="E297" s="15" t="s">
+        <v>171</v>
       </c>
       <c r="F297" s="1" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="298" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A298" s="12" t="s">
-        <v>128</v>
-      </c>
-      <c r="B298" s="12">
-        <v>6</v>
-      </c>
-      <c r="C298" s="12" t="s">
-        <v>150</v>
+      <c r="A298" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="B298" s="14">
+        <v>6</v>
+      </c>
+      <c r="C298" s="14" t="s">
+        <v>177</v>
       </c>
       <c r="D298" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E298" s="1" t="s">
-        <v>334</v>
+        <v>29</v>
+      </c>
+      <c r="E298" s="15" t="s">
+        <v>189</v>
       </c>
       <c r="F298" s="1" t="s">
         <v>55</v>
@@ -7507,55 +7648,855 @@
         <v>6</v>
       </c>
       <c r="C299" s="12" t="s">
+        <v>195</v>
+      </c>
+      <c r="D299" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="E299" s="15" t="s">
+        <v>365</v>
+      </c>
+      <c r="F299" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="300" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A300" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="B300" s="14">
+        <v>6</v>
+      </c>
+      <c r="C300" s="14" t="s">
+        <v>305</v>
+      </c>
+      <c r="D300" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="E300" s="15" t="s">
+        <v>366</v>
+      </c>
+      <c r="F300" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="301" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A301" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="B301" s="14">
+        <v>6</v>
+      </c>
+      <c r="C301" s="14" t="s">
+        <v>307</v>
+      </c>
+      <c r="D301" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="E301" s="15" t="s">
+        <v>367</v>
+      </c>
+      <c r="F301" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="302" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A302" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="B302" s="14">
+        <v>6</v>
+      </c>
+      <c r="C302" s="14" t="s">
+        <v>129</v>
+      </c>
+      <c r="D302" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="E302" s="15" t="s">
+        <v>368</v>
+      </c>
+      <c r="F302" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="303" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A303" s="12" t="s">
+        <v>128</v>
+      </c>
+      <c r="B303" s="12">
+        <v>6</v>
+      </c>
+      <c r="C303" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="D303" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="E303" s="15" t="s">
+        <v>146</v>
+      </c>
+      <c r="F303" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="304" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A304" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="B304" s="14">
+        <v>6</v>
+      </c>
+      <c r="C304" s="14" t="s">
+        <v>150</v>
+      </c>
+      <c r="D304" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="E304" s="15" t="s">
+        <v>369</v>
+      </c>
+      <c r="F304" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="305" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A305" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="B305" s="14">
+        <v>6</v>
+      </c>
+      <c r="C305" s="14" t="s">
         <v>159</v>
       </c>
-      <c r="D299" s="9" t="s">
+      <c r="D305" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="E305" s="15" t="s">
+        <v>172</v>
+      </c>
+      <c r="F305" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="306" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A306" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="B306" s="14">
+        <v>6</v>
+      </c>
+      <c r="C306" s="14" t="s">
+        <v>177</v>
+      </c>
+      <c r="D306" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="E306" s="15" t="s">
+        <v>190</v>
+      </c>
+      <c r="F306" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="307" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A307" s="12" t="s">
+        <v>128</v>
+      </c>
+      <c r="B307" s="12">
+        <v>6</v>
+      </c>
+      <c r="C307" s="12" t="s">
+        <v>195</v>
+      </c>
+      <c r="D307" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="E307" s="15" t="s">
+        <v>207</v>
+      </c>
+      <c r="F307" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="308" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A308" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="B308" s="14">
+        <v>6</v>
+      </c>
+      <c r="C308" s="14" t="s">
+        <v>305</v>
+      </c>
+      <c r="D308" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="E308" s="15" t="s">
+        <v>370</v>
+      </c>
+      <c r="F308" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="309" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A309" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="B309" s="14">
+        <v>6</v>
+      </c>
+      <c r="C309" s="14" t="s">
+        <v>307</v>
+      </c>
+      <c r="D309" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="E309" s="15" t="s">
+        <v>371</v>
+      </c>
+      <c r="F309" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="310" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A310" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="B310" s="14">
+        <v>6</v>
+      </c>
+      <c r="C310" s="14" t="s">
+        <v>129</v>
+      </c>
+      <c r="D310" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="E310" s="15" t="s">
+        <v>372</v>
+      </c>
+      <c r="F310" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="311" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A311" s="12" t="s">
+        <v>128</v>
+      </c>
+      <c r="B311" s="12">
+        <v>6</v>
+      </c>
+      <c r="C311" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="D311" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="E311" s="15" t="s">
+        <v>147</v>
+      </c>
+      <c r="F311" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="312" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A312" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="B312" s="14">
+        <v>6</v>
+      </c>
+      <c r="C312" s="14" t="s">
+        <v>150</v>
+      </c>
+      <c r="D312" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="E312" s="15" t="s">
+        <v>373</v>
+      </c>
+      <c r="F312" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="313" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A313" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="B313" s="14">
+        <v>6</v>
+      </c>
+      <c r="C313" s="14" t="s">
+        <v>159</v>
+      </c>
+      <c r="D313" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="E313" s="15" t="s">
+        <v>173</v>
+      </c>
+      <c r="F313" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="314" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A314" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="B314" s="14">
+        <v>6</v>
+      </c>
+      <c r="C314" s="14" t="s">
+        <v>177</v>
+      </c>
+      <c r="D314" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="E314" s="15" t="s">
+        <v>191</v>
+      </c>
+      <c r="F314" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="315" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A315" s="12" t="s">
+        <v>128</v>
+      </c>
+      <c r="B315" s="12">
+        <v>6</v>
+      </c>
+      <c r="C315" s="12" t="s">
+        <v>195</v>
+      </c>
+      <c r="D315" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="E315" s="15" t="s">
+        <v>374</v>
+      </c>
+      <c r="F315" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="316" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A316" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="B316" s="14">
+        <v>6</v>
+      </c>
+      <c r="C316" s="14" t="s">
+        <v>305</v>
+      </c>
+      <c r="D316" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="E316" s="15" t="s">
+        <v>375</v>
+      </c>
+      <c r="F316" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="317" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A317" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="B317" s="14">
+        <v>6</v>
+      </c>
+      <c r="C317" s="14" t="s">
+        <v>307</v>
+      </c>
+      <c r="D317" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="E317" s="15" t="s">
+        <v>376</v>
+      </c>
+      <c r="F317" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="318" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A318" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="B318" s="14">
+        <v>6</v>
+      </c>
+      <c r="C318" s="12" t="s">
+        <v>129</v>
+      </c>
+      <c r="D318" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="E318" s="15" t="s">
+        <v>134</v>
+      </c>
+      <c r="F318" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="319" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A319" s="12" t="s">
+        <v>128</v>
+      </c>
+      <c r="B319" s="12">
+        <v>6</v>
+      </c>
+      <c r="C319" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="D319" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="E319" s="15" t="s">
+        <v>148</v>
+      </c>
+      <c r="F319" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="320" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A320" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="B320" s="14">
+        <v>6</v>
+      </c>
+      <c r="C320" s="14" t="s">
+        <v>150</v>
+      </c>
+      <c r="D320" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="E320" s="15" t="s">
+        <v>377</v>
+      </c>
+      <c r="F320" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="321" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A321" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="B321" s="14">
+        <v>6</v>
+      </c>
+      <c r="C321" s="14" t="s">
+        <v>159</v>
+      </c>
+      <c r="D321" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="E321" s="15" t="s">
+        <v>174</v>
+      </c>
+      <c r="F321" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="322" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A322" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="B322" s="14">
+        <v>6</v>
+      </c>
+      <c r="C322" s="14" t="s">
+        <v>177</v>
+      </c>
+      <c r="D322" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="E322" s="15" t="s">
+        <v>192</v>
+      </c>
+      <c r="F322" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="323" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A323" s="12" t="s">
+        <v>128</v>
+      </c>
+      <c r="B323" s="12">
+        <v>6</v>
+      </c>
+      <c r="C323" s="12" t="s">
+        <v>195</v>
+      </c>
+      <c r="D323" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="E323" s="15" t="s">
+        <v>208</v>
+      </c>
+      <c r="F323" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="324" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A324" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="B324" s="14">
+        <v>6</v>
+      </c>
+      <c r="C324" s="14" t="s">
+        <v>305</v>
+      </c>
+      <c r="D324" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="E324" s="15" t="s">
+        <v>378</v>
+      </c>
+      <c r="F324" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="325" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A325" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="B325" s="14">
+        <v>6</v>
+      </c>
+      <c r="C325" s="14" t="s">
+        <v>307</v>
+      </c>
+      <c r="D325" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="E325" s="15" t="s">
+        <v>379</v>
+      </c>
+      <c r="F325" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="326" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A326" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="B326" s="14">
+        <v>6</v>
+      </c>
+      <c r="C326" s="14" t="s">
+        <v>129</v>
+      </c>
+      <c r="D326" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="E326" s="15" t="s">
+        <v>380</v>
+      </c>
+      <c r="F326" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="327" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A327" s="12" t="s">
+        <v>128</v>
+      </c>
+      <c r="B327" s="12">
+        <v>6</v>
+      </c>
+      <c r="C327" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="D327" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="E327" s="15" t="s">
+        <v>381</v>
+      </c>
+      <c r="F327" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="328" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A328" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="B328" s="14">
+        <v>6</v>
+      </c>
+      <c r="C328" s="14" t="s">
+        <v>150</v>
+      </c>
+      <c r="D328" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="E328" s="15" t="s">
+        <v>158</v>
+      </c>
+      <c r="F328" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="329" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A329" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="B329" s="14">
+        <v>6</v>
+      </c>
+      <c r="C329" s="14" t="s">
+        <v>159</v>
+      </c>
+      <c r="D329" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="E329" s="15" t="s">
+        <v>175</v>
+      </c>
+      <c r="F329" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="330" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A330" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="B330" s="14">
+        <v>6</v>
+      </c>
+      <c r="C330" s="14" t="s">
+        <v>177</v>
+      </c>
+      <c r="D330" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="E330" s="15" t="s">
+        <v>193</v>
+      </c>
+      <c r="F330" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="331" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A331" s="12" t="s">
+        <v>128</v>
+      </c>
+      <c r="B331" s="12">
+        <v>6</v>
+      </c>
+      <c r="C331" s="12" t="s">
+        <v>195</v>
+      </c>
+      <c r="D331" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="E331" s="15" t="s">
+        <v>209</v>
+      </c>
+      <c r="F331" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="332" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A332" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="B332" s="14">
+        <v>6</v>
+      </c>
+      <c r="C332" s="14" t="s">
+        <v>305</v>
+      </c>
+      <c r="D332" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="E332" s="15" t="s">
+        <v>382</v>
+      </c>
+      <c r="F332" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="333" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A333" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="B333" s="14">
+        <v>6</v>
+      </c>
+      <c r="C333" s="14" t="s">
+        <v>307</v>
+      </c>
+      <c r="D333" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="E333" s="15" t="s">
+        <v>383</v>
+      </c>
+      <c r="F333" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="334" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A334" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="B334" s="14">
+        <v>6</v>
+      </c>
+      <c r="C334" s="14" t="s">
+        <v>129</v>
+      </c>
+      <c r="D334" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="E299" s="1" t="s">
+      <c r="E334" s="15" t="s">
+        <v>384</v>
+      </c>
+      <c r="F334" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="335" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A335" s="12" t="s">
+        <v>128</v>
+      </c>
+      <c r="B335" s="12">
+        <v>6</v>
+      </c>
+      <c r="C335" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="D335" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E335" s="15" t="s">
+        <v>149</v>
+      </c>
+      <c r="F335" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="336" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A336" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="B336" s="14">
+        <v>6</v>
+      </c>
+      <c r="C336" s="14" t="s">
+        <v>150</v>
+      </c>
+      <c r="D336" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E336" s="15" t="s">
+        <v>385</v>
+      </c>
+      <c r="F336" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="337" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A337" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="B337" s="14">
+        <v>6</v>
+      </c>
+      <c r="C337" s="14" t="s">
+        <v>159</v>
+      </c>
+      <c r="D337" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E337" s="15" t="s">
         <v>176</v>
       </c>
-      <c r="F299" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="300" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A300" s="12" t="s">
-        <v>128</v>
-      </c>
-      <c r="B300" s="12">
-        <v>6</v>
-      </c>
-      <c r="C300" s="12" t="s">
+      <c r="F337" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="338" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A338" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="B338" s="14">
+        <v>6</v>
+      </c>
+      <c r="C338" s="12" t="s">
         <v>177</v>
       </c>
-      <c r="D300" s="9" t="s">
+      <c r="D338" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="E300" s="1" t="s">
+      <c r="E338" s="15" t="s">
         <v>194</v>
       </c>
-      <c r="F300" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="301" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A301" s="12" t="s">
-        <v>128</v>
-      </c>
-      <c r="B301" s="12">
-        <v>6</v>
-      </c>
-      <c r="C301" s="12" t="s">
+      <c r="F338" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="339" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A339" s="12" t="s">
+        <v>128</v>
+      </c>
+      <c r="B339" s="12">
+        <v>6</v>
+      </c>
+      <c r="C339" s="12" t="s">
         <v>195</v>
       </c>
-      <c r="D301" s="9" t="s">
+      <c r="D339" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="E301" s="1" t="s">
-        <v>346</v>
-      </c>
-      <c r="F301" s="1" t="s">
+      <c r="E339" s="15" t="s">
+        <v>386</v>
+      </c>
+      <c r="F339" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="340" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A340" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="B340" s="14">
+        <v>6</v>
+      </c>
+      <c r="C340" s="14" t="s">
+        <v>305</v>
+      </c>
+      <c r="D340" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E340" s="15" t="s">
+        <v>387</v>
+      </c>
+      <c r="F340" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="341" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A341" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="B341" s="14">
+        <v>6</v>
+      </c>
+      <c r="C341" s="14" t="s">
+        <v>307</v>
+      </c>
+      <c r="D341" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E341" s="15" t="s">
+        <v>388</v>
+      </c>
+      <c r="F341" s="1" t="s">
         <v>55</v>
       </c>
     </row>

</xml_diff>